<commit_message>
update script for finding WGS data
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/Education/MichiganStateUniversity/Josephs_Lab_Projects/tajimasDacrossSpecies/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="11_F25DC773A252ABDACC104837A95C598C5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A5212DE-2050-4172-B96D-57B23734B773}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="11_F25DC773A252ABDACC104837A95C598C5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FDB8A2A-7700-4573-BDBC-5E566FB1AC20}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="139">
   <si>
     <t>Species</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Arabidopsis thaliana</t>
   </si>
   <si>
-    <t>Bracypodium distachyon</t>
-  </si>
-  <si>
     <t>Triticum aestivum</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>SRP155312</t>
   </si>
   <si>
-    <t>Cotton</t>
-  </si>
-  <si>
     <t>SRP115740</t>
   </si>
   <si>
@@ -244,19 +238,229 @@
   </si>
   <si>
     <t>Medicago truncatula</t>
+  </si>
+  <si>
+    <t>Cinnamomum kanehirae</t>
+  </si>
+  <si>
+    <t>Nymphaea colorata</t>
+  </si>
+  <si>
+    <t>Aquilegia coerulea</t>
+  </si>
+  <si>
+    <t>Amaranthus hypochondriacus</t>
+  </si>
+  <si>
+    <t>Beta vulgaris</t>
+  </si>
+  <si>
+    <t>Chenopodium quinoa</t>
+  </si>
+  <si>
+    <t>Kalanchoe fedtschenkoi </t>
+  </si>
+  <si>
+    <t>Spinacia oleracea </t>
+  </si>
+  <si>
+    <t>Daucus carota</t>
+  </si>
+  <si>
+    <t>Helianthus annuus </t>
+  </si>
+  <si>
+    <t>Lactuca sativa</t>
+  </si>
+  <si>
+    <t>Olea europaea</t>
+  </si>
+  <si>
+    <t>Solanum tuberosum</t>
+  </si>
+  <si>
+    <t>Vaccinium darrowii </t>
+  </si>
+  <si>
+    <t>Eucalyptus grandis</t>
+  </si>
+  <si>
+    <t>Arachis hypogaea</t>
+  </si>
+  <si>
+    <t>Betula platyphylla</t>
+  </si>
+  <si>
+    <t>Cicer arietinum </t>
+  </si>
+  <si>
+    <t>Cucumis sativus</t>
+  </si>
+  <si>
+    <t>Fragaria vesca</t>
+  </si>
+  <si>
+    <t>Fragaria x ananassa</t>
+  </si>
+  <si>
+    <t>Glycine soja</t>
+  </si>
+  <si>
+    <t>Lens culinaris</t>
+  </si>
+  <si>
+    <t>Lens ervoides</t>
+  </si>
+  <si>
+    <t>Lotus japonicus</t>
+  </si>
+  <si>
+    <t>Lupinus albus</t>
+  </si>
+  <si>
+    <t>Phaseolus acutifolius</t>
+  </si>
+  <si>
+    <t>Prunus persica</t>
+  </si>
+  <si>
+    <t>Trifolium pratense</t>
+  </si>
+  <si>
+    <t>Carya illinoinensis</t>
+  </si>
+  <si>
+    <t>Vigna unguiculata</t>
+  </si>
+  <si>
+    <t>Corymbia citriodora</t>
+  </si>
+  <si>
+    <t>Linum usitatissimum</t>
+  </si>
+  <si>
+    <t>Manihot esculenta</t>
+  </si>
+  <si>
+    <t>Ricinus communis</t>
+  </si>
+  <si>
+    <t>Salix purpurea</t>
+  </si>
+  <si>
+    <t>Carica papaya</t>
+  </si>
+  <si>
+    <t>Theobroma cacao</t>
+  </si>
+  <si>
+    <t>Boechera stricta</t>
+  </si>
+  <si>
+    <t>Eutrema salsugineum</t>
+  </si>
+  <si>
+    <t>Schrenkiella parvula</t>
+  </si>
+  <si>
+    <t>Brassica oleracea capitata</t>
+  </si>
+  <si>
+    <t>Brassica rapa</t>
+  </si>
+  <si>
+    <t>Gossypium barbadense</t>
+  </si>
+  <si>
+    <t>Gossypium darwinii</t>
+  </si>
+  <si>
+    <t>Gossypium hirsutum </t>
+  </si>
+  <si>
+    <t>Gossypium mustelinum</t>
+  </si>
+  <si>
+    <t>Gossypium raimondii</t>
+  </si>
+  <si>
+    <t>Gossypium tomentosum</t>
+  </si>
+  <si>
+    <t>Citrus clementina</t>
+  </si>
+  <si>
+    <t>Citrus sinensis</t>
+  </si>
+  <si>
+    <t>Poncirus trifoliata</t>
+  </si>
+  <si>
+    <t>Ananas comosus</t>
+  </si>
+  <si>
+    <t>Asparagus officinalis </t>
+  </si>
+  <si>
+    <t>Dioscorea alata</t>
+  </si>
+  <si>
+    <t>Musa acuminata</t>
+  </si>
+  <si>
+    <t>Spirodela polyrhiza</t>
+  </si>
+  <si>
+    <t>Zostera marina </t>
+  </si>
+  <si>
+    <t>Oropetium thomaeum</t>
+  </si>
+  <si>
+    <t>Brachypodium hybridum</t>
+  </si>
+  <si>
+    <t>Brachypodium stacei</t>
+  </si>
+  <si>
+    <t>Brachypodium distachyon</t>
+  </si>
+  <si>
+    <t>Miscanthus sinensis </t>
+  </si>
+  <si>
+    <t>Panicum virgatum</t>
+  </si>
+  <si>
+    <t>Setaria italica </t>
+  </si>
+  <si>
+    <t>Setaria viridis</t>
+  </si>
+  <si>
+    <t>Panicum hallii</t>
+  </si>
+  <si>
+    <t>PRJNA399050</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -279,8 +483,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,15 +766,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="42.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
   </cols>
@@ -585,332 +790,670 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>51</v>
+      </c>
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" t="s">
         <v>55</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B79" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>18</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C86" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>32</v>
+      </c>
+      <c r="B88" t="s">
+        <v>35</v>
+      </c>
+      <c r="C88" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>28</v>
+      </c>
+      <c r="B92" t="s">
+        <v>66</v>
+      </c>
+      <c r="C92" t="s">
+        <v>67</v>
+      </c>
+      <c r="D92" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>33</v>
       </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" t="s">
-        <v>69</v>
-      </c>
-      <c r="D28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>10</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C98" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>10</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C99" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>10</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C100" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>10</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C101" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>9</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C102" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>9</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C103" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>9</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C104" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>9</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C105" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>72</v>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C38">
-    <sortCondition ref="A2:A38"/>
-    <sortCondition ref="C2:C38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D106">
+    <sortCondition ref="A2:A106"/>
+    <sortCondition ref="C2:C106"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added Panicum halli to snakemake input
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/Education/MichiganStateUniversity/Josephs_Lab_Projects/tajimasDacrossSpecies/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\4260834_2_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="777" documentId="11_F25DC773A252ABDACC104837A95C598C5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5165D49C-CBCE-4E3A-AEC2-6A96A83394CE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="299">
   <si>
     <t>Species</t>
   </si>
@@ -809,9 +809,6 @@
     <t>Potentially a lot more data for this species, but I can't find the raw data on the SRA</t>
   </si>
   <si>
-    <t>Includes 3 subspecies</t>
-  </si>
-  <si>
     <t>Could potentially find more data in SRA?</t>
   </si>
   <si>
@@ -894,6 +891,48 @@
   </si>
   <si>
     <t>WGS; I found 38 accessions in the SRA, but only 36 are mentioned in the publication</t>
+  </si>
+  <si>
+    <t>Found 537 in SRA based on the project numbers given in the publication</t>
+  </si>
+  <si>
+    <t>doi: 10.3390/ijms21186700</t>
+  </si>
+  <si>
+    <t>PRJNA605320</t>
+  </si>
+  <si>
+    <t>A smaller number of accessions compared to other studies, but I can clearly identify them in the SRA, 55 accessions mentioned in publications but there are 56 in the SRA</t>
+  </si>
+  <si>
+    <t>PRJNA681974 </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2022.03.24.485586</t>
+  </si>
+  <si>
+    <t>doi:10.1038/nbt.3096</t>
+  </si>
+  <si>
+    <t>PRJNA257011 </t>
+  </si>
+  <si>
+    <t>PRJNA552939</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.molp.2020.01.014</t>
+  </si>
+  <si>
+    <t>279 accessions</t>
+  </si>
+  <si>
+    <t>Following the methods in this paper, I should get 2214 Glycine accessions. This paper published new sequences for 1674 accessions, the rest were previously published. However, this paper includes some Glycine soja accessions, which I will need to separate out. Maybe I can use these accessions? The paper says there should only be 1,993 glycine max accessions, but I'm seeing 2193 across all three studies...</t>
+  </si>
+  <si>
+    <t>302 accessions in study, but only 240 are Glycine max</t>
+  </si>
+  <si>
+    <t>Includes 3 subspecies. Paper mentions 187 accessions, but I only found 185. There are some non-public accessions in this group too. I only got 85 unique samples though… Also there's some pacbio data in here</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="G126" sqref="G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,10 +1357,10 @@
         <v>212</v>
       </c>
       <c r="F1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" t="s">
         <v>260</v>
-      </c>
-      <c r="G1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1342,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1374,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1406,7 +1445,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1428,7 +1467,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>21</v>
@@ -1441,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1519,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1533,7 +1572,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>105</v>
       </c>
@@ -1543,12 +1582,17 @@
       <c r="C16" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="8" t="s">
+        <v>285</v>
+      </c>
       <c r="E16" s="11">
         <v>467</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1565,85 +1609,80 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="E18" s="11">
+        <v>56</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>263</v>
-      </c>
-      <c r="E18" s="11">
-        <v>107</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>154</v>
-      </c>
+      <c r="D19" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" t="s">
-        <v>136</v>
+        <v>126</v>
+      </c>
+      <c r="B20" t="s">
+        <v>153</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>108</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>156</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E22" s="11">
-        <v>119</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>159</v>
@@ -1655,105 +1694,117 @@
         <v>160</v>
       </c>
       <c r="E23" s="11">
+        <v>119</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" s="11">
         <v>199</v>
       </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>109</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>157</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D25" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E26" s="11">
         <v>40</v>
       </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="7" t="s">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="E28" s="11">
+      <c r="D29" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="E29" s="11">
         <v>52</v>
       </c>
-      <c r="F28" s="3">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C29" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>137</v>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
         <v>136</v>
@@ -1762,100 +1813,100 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="E31" s="11">
-        <v>296</v>
-      </c>
-      <c r="F31" s="3">
-        <v>1</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>262</v>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E32" s="11">
+        <v>296</v>
+      </c>
+      <c r="F32" s="3">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D33" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="E33" s="11">
+        <v>3171</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="E32" s="11">
-        <v>3171</v>
-      </c>
-      <c r="F32" s="3">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" t="s">
-        <v>136</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="E34" s="11">
+      <c r="E35" s="11">
         <v>337</v>
       </c>
-      <c r="F34" s="3">
-        <v>1</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35" t="s">
-        <v>136</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>137</v>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
         <v>136</v>
@@ -1866,7 +1917,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
         <v>136</v>
@@ -1875,41 +1926,38 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E39" s="11">
         <v>115</v>
       </c>
-      <c r="F38" s="3">
-        <v>1</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" t="s">
-        <v>177</v>
-      </c>
-      <c r="C39" t="s">
-        <v>178</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>145</v>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1920,7 +1968,7 @@
         <v>177</v>
       </c>
       <c r="C40" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>145</v>
@@ -1928,43 +1976,46 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>177</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>176</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>121</v>
-      </c>
-      <c r="B42" t="s">
-        <v>182</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>121</v>
+      </c>
+      <c r="B43" t="s">
+        <v>182</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
         <v>136</v>
@@ -1975,7 +2026,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="C45" t="s">
         <v>136</v>
@@ -1986,7 +2037,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
         <v>136</v>
@@ -1997,7 +2048,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
         <v>136</v>
@@ -2006,125 +2057,134 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B49" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E49" s="11">
+        <v>1674</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E50" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E51" s="11">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C52" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>258</v>
-      </c>
-      <c r="E48" s="11">
-        <v>438</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="D52" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="E52" s="16"/>
+    </row>
+    <row r="53" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B53" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C53" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="11">
+      <c r="D53" s="8"/>
+      <c r="E53" s="11">
         <v>185</v>
       </c>
-      <c r="F49" s="3">
-        <v>1</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="F53" s="3">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="11">
+      <c r="D54" s="8"/>
+      <c r="E54" s="11">
         <v>336</v>
       </c>
-      <c r="F50" s="3">
-        <v>1</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>111</v>
-      </c>
-      <c r="C51" t="s">
-        <v>136</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="11">
-        <v>1081</v>
-      </c>
-      <c r="F52" s="3">
-        <v>1</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" t="s">
-        <v>136</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>137</v>
+      <c r="F54" s="3">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C55" t="s">
         <v>136</v>
@@ -2133,55 +2193,52 @@
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>137</v>
+    <row r="56" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="11">
+        <v>1081</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>25</v>
-      </c>
-      <c r="B57" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" t="s">
-        <v>37</v>
+        <v>112</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D58" s="8"/>
-      <c r="E58" s="11">
-        <v>300</v>
-      </c>
-      <c r="F58" s="3">
-        <v>1</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>262</v>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
         <v>136</v>
@@ -2190,376 +2247,355 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>270</v>
-      </c>
-      <c r="E60" s="11">
-        <v>131</v>
-      </c>
-      <c r="F60" s="3">
-        <v>1</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>262</v>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>115</v>
+      </c>
+      <c r="C60" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="C61" t="s">
-        <v>192</v>
+        <v>37</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" t="s">
-        <v>194</v>
-      </c>
-      <c r="C62" t="s">
-        <v>195</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>145</v>
+    <row r="62" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D62" s="8"/>
+      <c r="E62" s="11">
+        <v>300</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>99</v>
-      </c>
-      <c r="B63" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>28</v>
-      </c>
-      <c r="C64" t="s">
-        <v>136</v>
-      </c>
-      <c r="D64" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="E65" s="11">
-        <v>136</v>
-      </c>
-      <c r="F65" s="3">
-        <v>1</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>262</v>
+    <row r="64" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="E64" s="11">
+        <v>131</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" t="s">
+        <v>192</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>90</v>
+      </c>
+      <c r="B66" t="s">
+        <v>194</v>
       </c>
       <c r="C66" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="E67" s="11">
-        <v>44</v>
-      </c>
-      <c r="F67" s="3">
-        <v>1</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>262</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" t="s">
+        <v>136</v>
+      </c>
+      <c r="C67" t="s">
+        <v>197</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="C68" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E69" s="11">
+        <v>136</v>
+      </c>
+      <c r="F69" s="3">
+        <v>1</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C68" t="s">
+      <c r="B71" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="E71" s="11">
+        <v>44</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>100</v>
+      </c>
+      <c r="C72" t="s">
         <v>201</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D72" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    <row r="73" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B73" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E73" s="3">
+        <v>39</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="D74" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E69" s="3">
-        <v>39</v>
-      </c>
-      <c r="F69" s="3">
-        <v>1</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
+      <c r="E74" s="16"/>
+    </row>
+    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>67</v>
       </c>
-      <c r="B70" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="E70" s="16"/>
-    </row>
-    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="B75" t="s">
         <v>185</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C75" t="s">
         <v>196</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D75" s="7" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D72" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="E72" s="11">
-        <v>38</v>
-      </c>
-      <c r="F72" s="3">
-        <v>1</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>129</v>
-      </c>
-      <c r="C73" t="s">
-        <v>136</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>122</v>
-      </c>
-      <c r="C74" t="s">
-        <v>136</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>69</v>
-      </c>
-      <c r="C75" t="s">
-        <v>136</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>207</v>
+        <v>20</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>206</v>
+        <v>248</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E76" s="11">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F76" s="3">
         <v>1</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C77" t="s">
-        <v>205</v>
+        <v>136</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>125</v>
-      </c>
-      <c r="B78" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C78" t="s">
         <v>136</v>
       </c>
       <c r="D78" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>69</v>
+      </c>
+      <c r="C79" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="E79" s="12">
-        <v>3024</v>
-      </c>
-      <c r="F79" s="3">
-        <v>1</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>47</v>
+        <v>206</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="E80" s="11">
-        <f>94+78+15</f>
-        <v>187</v>
+        <v>52</v>
       </c>
       <c r="F80" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="E81" s="11">
-        <v>747</v>
-      </c>
-      <c r="F81" s="3">
-        <v>1</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>262</v>
+      <c r="G80" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" t="s">
+        <v>136</v>
+      </c>
+      <c r="C81" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>125</v>
+      </c>
+      <c r="B82" t="s">
+        <v>136</v>
       </c>
       <c r="C82" t="s">
         <v>136</v>
@@ -2568,581 +2604,617 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>42</v>
+        <v>208</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D83" s="8"/>
-      <c r="E83" s="11">
-        <v>683</v>
+        <v>4</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E83" s="12">
+        <v>3024</v>
       </c>
       <c r="F83" s="3">
         <v>1</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>118</v>
-      </c>
-      <c r="C84" t="s">
-        <v>136</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>137</v>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E84" s="11">
+        <v>85</v>
+      </c>
+      <c r="F84" s="3">
+        <v>1</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>51</v>
+        <v>130</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>57</v>
+        <v>211</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>56</v>
+        <v>210</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="E85" s="11">
-        <v>52</v>
+        <v>747</v>
       </c>
       <c r="F85" s="3">
         <v>1</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>51</v>
-      </c>
-      <c r="B86" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="C86" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>51</v>
-      </c>
-      <c r="B87" t="s">
-        <v>57</v>
-      </c>
-      <c r="C87" t="s">
-        <v>56</v>
+        <v>136</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" s="8"/>
+      <c r="E87" s="11">
+        <v>683</v>
+      </c>
+      <c r="F87" s="3">
+        <v>1</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>118</v>
+      </c>
+      <c r="C88" t="s">
+        <v>136</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C88" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="B89" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="E89" s="11">
+        <v>52</v>
+      </c>
+      <c r="F89" s="3">
+        <v>1</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>51</v>
       </c>
-      <c r="B89" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="E90" s="11">
-        <v>428</v>
-      </c>
-      <c r="F90" s="3">
-        <v>1</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>262</v>
+      <c r="B90" t="s">
+        <v>54</v>
+      </c>
+      <c r="C90" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>101</v>
+        <v>51</v>
+      </c>
+      <c r="B91" t="s">
+        <v>57</v>
       </c>
       <c r="C91" t="s">
-        <v>136</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>137</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="C92" t="s">
-        <v>136</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>137</v>
+        <v>55</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>107</v>
-      </c>
-      <c r="C93" t="s">
-        <v>136</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>137</v>
+        <v>51</v>
+      </c>
+      <c r="B93" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="94" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E94" s="11">
-        <v>909</v>
+        <v>428</v>
       </c>
       <c r="F94" s="3">
         <v>1</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="E95" s="11">
-        <v>38</v>
-      </c>
-      <c r="F95" s="3">
-        <v>1</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>101</v>
+      </c>
+      <c r="C95" t="s">
+        <v>136</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="C96" t="s">
-        <v>17</v>
+        <v>136</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="C97" t="s">
-        <v>220</v>
+        <v>136</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>160</v>
+        <v>280</v>
       </c>
       <c r="E98" s="11">
-        <v>360</v>
+        <v>909</v>
       </c>
       <c r="F98" s="3">
         <v>1</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>79</v>
-      </c>
-      <c r="C99" t="s">
-        <v>224</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>225</v>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E99" s="11">
+        <v>38</v>
+      </c>
+      <c r="F99" s="3">
+        <v>1</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>31</v>
-      </c>
-      <c r="B100" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C100" t="s">
-        <v>33</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>145</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>31</v>
-      </c>
-      <c r="B101" t="s">
-        <v>227</v>
+        <v>18</v>
       </c>
       <c r="C101" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>228</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>160</v>
       </c>
       <c r="E102" s="11">
-        <v>400</v>
+        <v>360</v>
       </c>
       <c r="F102" s="3">
         <v>1</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="E103" s="11">
-        <v>296</v>
-      </c>
-      <c r="F103" s="3">
-        <v>1</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="D104" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="E104" s="11">
-        <v>36</v>
-      </c>
-      <c r="F104" s="3">
-        <v>1</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>79</v>
+      </c>
+      <c r="C103" t="s">
+        <v>224</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" t="s">
+        <v>34</v>
+      </c>
+      <c r="C104" t="s">
+        <v>33</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>31</v>
+      </c>
+      <c r="B105" t="s">
+        <v>227</v>
       </c>
       <c r="C105" t="s">
-        <v>136</v>
+        <v>226</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>27</v>
-      </c>
-      <c r="B106" t="s">
-        <v>64</v>
-      </c>
-      <c r="C106" t="s">
-        <v>65</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>95</v>
-      </c>
-      <c r="D107" s="7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>23</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>236</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E106" s="11">
+        <v>400</v>
+      </c>
+      <c r="F106" s="3">
+        <v>1</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E107" s="11">
+        <v>296</v>
+      </c>
+      <c r="F107" s="3">
+        <v>1</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E108" s="11">
+        <v>36</v>
+      </c>
+      <c r="F108" s="3">
+        <v>1</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="C109" t="s">
-        <v>237</v>
+        <v>136</v>
       </c>
       <c r="D109" s="7" t="s">
-        <v>238</v>
+        <v>137</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>80</v>
+        <v>27</v>
+      </c>
+      <c r="B110" t="s">
+        <v>64</v>
       </c>
       <c r="C110" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>97</v>
-      </c>
-      <c r="C111" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>137</v>
+        <v>235</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>10</v>
-      </c>
-      <c r="C112" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E113" s="11">
-        <v>117</v>
-      </c>
-      <c r="F113" s="3">
-        <v>1</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>262</v>
+        <v>23</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>32</v>
+      </c>
+      <c r="C113" t="s">
+        <v>237</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="C114" t="s">
-        <v>13</v>
+        <v>136</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>97</v>
+      </c>
+      <c r="C115" t="s">
+        <v>136</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>10</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C116" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B117" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="E117" s="11">
+        <v>117</v>
+      </c>
+      <c r="F117" s="3">
+        <v>1</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+    <row r="120" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C116" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="8"/>
-      <c r="E116" s="11">
+      <c r="D120" s="8"/>
+      <c r="E120" s="11">
         <v>1218</v>
       </c>
-      <c r="F116" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+      <c r="F120" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D117" s="8"/>
-      <c r="E117" s="11"/>
-    </row>
-    <row r="118" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+      <c r="D121" s="8"/>
+      <c r="E121" s="11"/>
+    </row>
+    <row r="122" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C122" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D118" s="8"/>
-      <c r="E118" s="11"/>
-    </row>
-    <row r="119" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+      <c r="D122" s="8"/>
+      <c r="E122" s="11"/>
+    </row>
+    <row r="123" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C123" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D119" s="8"/>
-      <c r="E119" s="11"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>124</v>
-      </c>
-      <c r="C120" t="s">
-        <v>239</v>
-      </c>
-      <c r="D120" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>161</v>
-      </c>
-      <c r="B121" t="s">
-        <v>163</v>
-      </c>
-      <c r="C121" t="s">
-        <v>162</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>165</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C122" t="s">
-        <v>167</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>169</v>
-      </c>
-      <c r="B123" t="s">
-        <v>168</v>
-      </c>
-      <c r="D123" s="7" t="s">
-        <v>164</v>
-      </c>
+      <c r="D123" s="8"/>
+      <c r="E123" s="11"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>246</v>
-      </c>
-      <c r="B124" t="s">
-        <v>247</v>
+        <v>124</v>
+      </c>
+      <c r="C124" t="s">
+        <v>239</v>
       </c>
       <c r="D124" s="7" t="s">
-        <v>164</v>
+        <v>238</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>268</v>
+        <v>161</v>
+      </c>
+      <c r="B125" t="s">
+        <v>163</v>
+      </c>
+      <c r="C125" t="s">
+        <v>162</v>
       </c>
       <c r="D125" s="7" t="s">
         <v>164</v>
@@ -3150,7 +3222,13 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>269</v>
+        <v>165</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C126" t="s">
+        <v>167</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>164</v>
@@ -3158,45 +3236,84 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>39</v>
-      </c>
-      <c r="C127" t="s">
-        <v>40</v>
+        <v>169</v>
+      </c>
+      <c r="B127" t="s">
+        <v>168</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E128" s="13">
-        <f>SUM(E2:E123)</f>
-        <v>18101</v>
-      </c>
-      <c r="F128" s="5" t="s">
+      <c r="A128" t="s">
+        <v>246</v>
+      </c>
+      <c r="B128" t="s">
+        <v>247</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>267</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>268</v>
+      </c>
+      <c r="D130" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>39</v>
+      </c>
+      <c r="C131" t="s">
+        <v>40</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E132" s="13">
+        <f>SUM(E2:E127)</f>
+        <v>19703</v>
+      </c>
+      <c r="F132" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="129" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E129" s="13">
-        <f>SUM(F2:F123)</f>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E133" s="13">
+        <f>SUM(F2:F127)</f>
         <v>40</v>
       </c>
-      <c r="F129" s="5" t="s">
+      <c r="F133" s="5" t="s">
         <v>241</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D120">
-    <sortCondition ref="A2:A120"/>
-    <sortCondition ref="C2:C120"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D124">
+    <sortCondition ref="A2:A124"/>
+    <sortCondition ref="C2:C124"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B122" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
-    <hyperlink ref="B32" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
-    <hyperlink ref="B67" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
-    <hyperlink ref="B28" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
+    <hyperlink ref="B126" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B33" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
+    <hyperlink ref="B71" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
+    <hyperlink ref="B29" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
+    <hyperlink ref="B18" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Zea mays to workflow input
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\4260834_2_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/66962_2_13/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{426CDD82-63B8-4424-9885-81CE2250AC06}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="302">
   <si>
     <t>Species</t>
   </si>
@@ -933,6 +933,15 @@
   </si>
   <si>
     <t>Includes 3 subspecies. Paper mentions 187 accessions, but I only found 185. There are some non-public accessions in this group too. I only got 85 unique samples though… Also there's some pacbio data in here</t>
+  </si>
+  <si>
+    <t>doi: 10.1093/gigascience/gix134</t>
+  </si>
+  <si>
+    <t>Paper lists 1218 taxa across all four studies</t>
+  </si>
+  <si>
+    <t>I could not find data linked to this study in the SRA</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1018,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1034,13 +1043,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1326,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="G126" sqref="G126"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,20 +1634,19 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="E19" s="16"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -2125,20 +2126,19 @@
         <v>279</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" t="s">
         <v>47</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="E52" s="16"/>
     </row>
     <row r="53" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
@@ -2471,20 +2471,19 @@
         <v>261</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="s">
+    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>67</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" t="s">
         <v>203</v>
       </c>
-      <c r="C74" s="14" t="s">
+      <c r="C74" t="s">
         <v>254</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D74" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="E74" s="16"/>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -3154,25 +3153,35 @@
       <c r="A120" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B120" s="3" t="s">
+        <v>299</v>
+      </c>
       <c r="C120" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D120" s="8"/>
+      <c r="D120" s="8" t="s">
+        <v>300</v>
+      </c>
       <c r="E120" s="11">
-        <v>1218</v>
+        <v>33</v>
       </c>
       <c r="F120" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G120" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D121" s="8"/>
+      <c r="D121" s="8" t="s">
+        <v>301</v>
+      </c>
       <c r="E121" s="11"/>
     </row>
     <row r="122" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3183,7 +3192,9 @@
         <v>5</v>
       </c>
       <c r="D122" s="8"/>
-      <c r="E122" s="11"/>
+      <c r="E122" s="11">
+        <v>277</v>
+      </c>
     </row>
     <row r="123" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
@@ -3193,7 +3204,9 @@
         <v>8</v>
       </c>
       <c r="D123" s="8"/>
-      <c r="E123" s="11"/>
+      <c r="E123" s="11">
+        <v>599</v>
+      </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -3286,7 +3299,7 @@
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E132" s="13">
         <f>SUM(E2:E127)</f>
-        <v>19703</v>
+        <v>19394</v>
       </c>
       <c r="F132" s="5" t="s">
         <v>215</v>

</xml_diff>

<commit_message>
call degenotate in conda env
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/66962_2_13/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/395010_2_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{426CDD82-63B8-4424-9885-81CE2250AC06}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{648528EA-2A51-46A0-AC9E-65190091873F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="304">
   <si>
     <t>Species</t>
   </si>
@@ -942,6 +942,12 @@
   </si>
   <si>
     <t>I could not find data linked to this study in the SRA</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41467-022-35368-1</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41588-020-00722-w</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1044,6 +1050,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1326,23 +1335,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G133"/>
+  <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="42.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.26171875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.26171875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="35.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1365,7 +1372,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -1386,7 +1393,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1397,7 +1404,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>119</v>
       </c>
@@ -1418,7 +1425,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -1429,7 +1436,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1450,263 +1457,258 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="11">
+        <v>142</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>245</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="11">
+      <c r="D9" s="8"/>
+      <c r="E9" s="11">
         <v>1135</v>
       </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
         <v>120</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E15" s="11">
         <v>597</v>
       </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
         <v>83</v>
       </c>
-      <c r="C15" t="s">
-        <v>136</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="C16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E17" s="11">
         <v>467</v>
       </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>105</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>151</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>150</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D18" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:7" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E19" s="11">
         <v>56</v>
       </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
         <v>128</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D20" s="7" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
         <v>126</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>153</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
         <v>127</v>
       </c>
-      <c r="C21" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="C22" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
         <v>108</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>156</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E23" s="11">
-        <v>119</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>159</v>
@@ -1718,105 +1720,117 @@
         <v>160</v>
       </c>
       <c r="E24" s="11">
+        <v>119</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="11">
         <v>199</v>
       </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
         <v>109</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>157</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D26" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E27" s="11">
         <v>40</v>
       </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>59</v>
-      </c>
-      <c r="C27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>60</v>
       </c>
       <c r="C28" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="7" t="s">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E30" s="11">
         <v>52</v>
       </c>
-      <c r="F29" s="3">
-        <v>1</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
         <v>103</v>
-      </c>
-      <c r="C30" t="s">
-        <v>136</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>96</v>
       </c>
       <c r="C31" t="s">
         <v>136</v>
@@ -1825,100 +1839,100 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="E32" s="11">
+      <c r="E33" s="11">
         <v>296</v>
       </c>
-      <c r="F32" s="3">
-        <v>1</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E34" s="11">
         <v>3171</v>
       </c>
-      <c r="F33" s="3">
-        <v>1</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
         <v>68</v>
       </c>
-      <c r="C34" t="s">
-        <v>136</v>
-      </c>
-      <c r="D34" s="7" t="s">
+      <c r="C35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E36" s="11">
         <v>337</v>
       </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
         <v>116</v>
-      </c>
-      <c r="C36" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>117</v>
       </c>
       <c r="C37" t="s">
         <v>136</v>
@@ -1927,9 +1941,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
         <v>136</v>
@@ -1938,44 +1952,41 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D40" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E40" s="11">
         <v>115</v>
       </c>
-      <c r="F39" s="3">
-        <v>1</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" t="s">
-        <v>177</v>
-      </c>
-      <c r="C40" t="s">
-        <v>178</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -1983,51 +1994,54 @@
         <v>177</v>
       </c>
       <c r="C41" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
         <v>76</v>
       </c>
-      <c r="C42" t="s">
-        <v>136</v>
-      </c>
-      <c r="D42" s="7" t="s">
+      <c r="C43" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
         <v>121</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>182</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>181</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D44" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
         <v>29</v>
-      </c>
-      <c r="C44" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>81</v>
       </c>
       <c r="C45" t="s">
         <v>136</v>
@@ -2036,9 +2050,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
         <v>136</v>
@@ -2047,9 +2061,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
         <v>136</v>
@@ -2058,9 +2072,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" t="s">
         <v>136</v>
@@ -2069,176 +2083,176 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="E49" s="11">
-        <v>1674</v>
-      </c>
-      <c r="F49" s="3">
-        <v>1</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E50" s="11">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1674</v>
+      </c>
+      <c r="F50" s="3">
+        <v>1</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E51" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D52" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="E51" s="11">
+      <c r="E52" s="11">
         <v>279</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
         <v>45</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>46</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>47</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D53" s="7" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+    <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B54" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C54" s="9" t="s">
         <v>184</v>
-      </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="11">
-        <v>185</v>
-      </c>
-      <c r="F53" s="3">
-        <v>1</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="11">
+        <v>185</v>
+      </c>
+      <c r="F54" s="3">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="11">
         <v>336</v>
       </c>
-      <c r="F54" s="3">
-        <v>1</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
         <v>111</v>
       </c>
-      <c r="C55" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="7" t="s">
+      <c r="C56" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="57" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B57" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="11">
+      <c r="D57" s="8"/>
+      <c r="E57" s="11">
         <v>1081</v>
       </c>
-      <c r="F56" s="3">
-        <v>1</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D58" s="7" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
         <v>113</v>
-      </c>
-      <c r="C58" t="s">
-        <v>136</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>114</v>
       </c>
       <c r="C59" t="s">
         <v>136</v>
@@ -2247,9 +2261,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C60" t="s">
         <v>136</v>
@@ -2258,284 +2272,284 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" t="s">
+        <v>136</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
         <v>25</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>38</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>37</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D62" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+    <row r="63" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="11">
+      <c r="D63" s="8"/>
+      <c r="E63" s="11">
         <v>300</v>
       </c>
-      <c r="F62" s="3">
-        <v>1</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="F63" s="3">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
         <v>74</v>
       </c>
-      <c r="C63" t="s">
-        <v>136</v>
-      </c>
-      <c r="D63" s="7" t="s">
+      <c r="C64" t="s">
+        <v>136</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+    <row r="65" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B65" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D65" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="E64" s="11">
+      <c r="E65" s="11">
         <v>131</v>
       </c>
-      <c r="F64" s="3">
-        <v>1</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
         <v>89</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>193</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>192</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>90</v>
-      </c>
-      <c r="B66" t="s">
-        <v>194</v>
-      </c>
-      <c r="C66" t="s">
-        <v>195</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
+        <v>90</v>
+      </c>
+      <c r="B67" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s">
+        <v>195</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
         <v>99</v>
       </c>
-      <c r="B67" t="s">
-        <v>136</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B68" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" t="s">
         <v>197</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D68" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
         <v>28</v>
       </c>
-      <c r="C68" t="s">
-        <v>136</v>
-      </c>
-      <c r="D68" s="7" t="s">
+      <c r="C69" t="s">
+        <v>136</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+    <row r="70" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B70" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D69" s="8" t="s">
+      <c r="D70" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="E69" s="11">
-        <v>136</v>
-      </c>
-      <c r="F69" s="3">
-        <v>1</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="E70" s="11">
+        <v>136</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
         <v>92</v>
       </c>
-      <c r="C70" t="s">
-        <v>136</v>
-      </c>
-      <c r="D70" s="7" t="s">
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:7" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+    <row r="72" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B72" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D71" s="8" t="s">
+      <c r="D72" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="E71" s="11">
+      <c r="E72" s="11">
         <v>44</v>
       </c>
-      <c r="F71" s="3">
-        <v>1</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="F72" s="3">
+        <v>1</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
         <v>100</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>201</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D73" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+    <row r="74" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B74" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D73" s="8" t="s">
+      <c r="D74" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E73" s="3">
+      <c r="E74" s="3">
         <v>39</v>
       </c>
-      <c r="F73" s="3">
-        <v>1</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" t="s">
-        <v>203</v>
-      </c>
-      <c r="C74" t="s">
-        <v>254</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F74" s="3">
+        <v>1</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>67</v>
       </c>
       <c r="B75" t="s">
+        <v>203</v>
+      </c>
+      <c r="C75" t="s">
+        <v>254</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" t="s">
         <v>185</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>196</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D76" s="7" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="76" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+    <row r="77" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B77" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D76" s="8" t="s">
+      <c r="D77" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="E76" s="11">
+      <c r="E77" s="11">
         <v>38</v>
       </c>
-      <c r="F76" s="3">
-        <v>1</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="F77" s="3">
+        <v>1</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
         <v>129</v>
-      </c>
-      <c r="C77" t="s">
-        <v>136</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>122</v>
       </c>
       <c r="C78" t="s">
         <v>136</v>
@@ -2544,275 +2558,275 @@
         <v>204</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
         <v>69</v>
       </c>
-      <c r="C79" t="s">
-        <v>136</v>
-      </c>
-      <c r="D79" s="7" t="s">
+      <c r="C80" t="s">
+        <v>136</v>
+      </c>
+      <c r="D80" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+    <row r="81" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C81" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D81" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="E80" s="11">
+      <c r="E81" s="11">
         <v>52</v>
       </c>
-      <c r="F80" s="3">
-        <v>1</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="F81" s="3">
+        <v>1</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
         <v>78</v>
       </c>
-      <c r="B81" t="s">
-        <v>136</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="B82" t="s">
+        <v>136</v>
+      </c>
+      <c r="C82" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
         <v>125</v>
       </c>
-      <c r="B82" t="s">
-        <v>136</v>
-      </c>
-      <c r="C82" t="s">
-        <v>136</v>
-      </c>
-      <c r="D82" s="7" t="s">
+      <c r="B83" t="s">
+        <v>136</v>
+      </c>
+      <c r="C83" t="s">
+        <v>136</v>
+      </c>
+      <c r="D83" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+    <row r="84" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D83" s="8" t="s">
+      <c r="D84" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="E83" s="12">
+      <c r="E84" s="12">
         <v>3024</v>
       </c>
-      <c r="F83" s="3">
-        <v>1</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="F84" s="3">
+        <v>1</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D84" s="8" t="s">
+      <c r="D85" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="E84" s="11">
+      <c r="E85" s="11">
         <v>85</v>
       </c>
-      <c r="F84" s="3">
-        <v>1</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+      <c r="F85" s="3">
+        <v>1</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D85" s="8" t="s">
+      <c r="D86" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="E85" s="11">
+      <c r="E86" s="11">
         <v>747</v>
       </c>
-      <c r="F85" s="3">
-        <v>1</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="F86" s="3">
+        <v>1</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
         <v>93</v>
       </c>
-      <c r="C86" t="s">
-        <v>136</v>
-      </c>
-      <c r="D86" s="7" t="s">
+      <c r="C87" t="s">
+        <v>136</v>
+      </c>
+      <c r="D87" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+    <row r="88" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D87" s="8"/>
-      <c r="E87" s="11">
+      <c r="D88" s="8"/>
+      <c r="E88" s="11">
         <v>683</v>
       </c>
-      <c r="F87" s="3">
-        <v>1</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="F88" s="3">
+        <v>1</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
         <v>118</v>
       </c>
-      <c r="C88" t="s">
-        <v>136</v>
-      </c>
-      <c r="D88" s="7" t="s">
+      <c r="C89" t="s">
+        <v>136</v>
+      </c>
+      <c r="D89" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+    <row r="90" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D89" s="8" t="s">
+      <c r="D90" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="E89" s="11">
+      <c r="E90" s="11">
         <v>52</v>
       </c>
-      <c r="F89" s="3">
-        <v>1</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>51</v>
-      </c>
-      <c r="B90" t="s">
-        <v>54</v>
-      </c>
-      <c r="C90" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F90" s="3">
+        <v>1</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>51</v>
       </c>
       <c r="B91" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C91" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>51</v>
       </c>
+      <c r="B92" t="s">
+        <v>57</v>
+      </c>
       <c r="C92" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>51</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>51</v>
+      </c>
+      <c r="B94" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+    <row r="95" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="B95" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D94" s="8" t="s">
+      <c r="D95" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="E94" s="11">
+      <c r="E95" s="11">
         <v>428</v>
       </c>
-      <c r="F94" s="3">
-        <v>1</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="F95" s="3">
+        <v>1</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="s">
         <v>101</v>
-      </c>
-      <c r="C95" t="s">
-        <v>136</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>102</v>
       </c>
       <c r="C96" t="s">
         <v>136</v>
@@ -2821,9 +2835,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C97" t="s">
         <v>136</v>
@@ -2832,268 +2846,273 @@
         <v>137</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>107</v>
+      </c>
+      <c r="C98" t="s">
+        <v>136</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="B99" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="C99" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D98" s="8" t="s">
+      <c r="D99" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="E98" s="11">
+      <c r="E99" s="11">
         <v>909</v>
       </c>
-      <c r="F98" s="3">
-        <v>1</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
+      <c r="F99" s="3">
+        <v>1</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B99" s="3" t="s">
+      <c r="B100" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C99" s="3" t="s">
+      <c r="C100" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D99" s="8" t="s">
+      <c r="D100" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="E99" s="11">
+      <c r="E100" s="11">
         <v>38</v>
       </c>
-      <c r="F99" s="3">
-        <v>1</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>18</v>
-      </c>
-      <c r="C100" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F100" s="3">
+        <v>1</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>18</v>
       </c>
       <c r="C101" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" t="s">
+        <v>18</v>
+      </c>
+      <c r="C102" t="s">
         <v>220</v>
       </c>
-      <c r="D101" s="7" t="s">
+      <c r="D102" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+    <row r="103" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="B103" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="C103" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D102" s="8" t="s">
+      <c r="D103" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E102" s="11">
+      <c r="E103" s="11">
         <v>360</v>
       </c>
-      <c r="F102" s="3">
-        <v>1</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="F103" s="3">
+        <v>1</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" t="s">
         <v>79</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>224</v>
       </c>
-      <c r="D103" s="7" t="s">
+      <c r="D104" s="7" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>31</v>
-      </c>
-      <c r="B104" t="s">
-        <v>34</v>
-      </c>
-      <c r="C104" t="s">
-        <v>33</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>31</v>
       </c>
       <c r="B105" t="s">
+        <v>34</v>
+      </c>
+      <c r="C105" t="s">
+        <v>33</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" t="s">
+        <v>31</v>
+      </c>
+      <c r="B106" t="s">
         <v>227</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>226</v>
       </c>
-      <c r="D105" s="7" t="s">
+      <c r="D106" s="7" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+    <row r="107" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="C107" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D106" s="8" t="s">
+      <c r="D107" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E106" s="11">
+      <c r="E107" s="11">
         <v>400</v>
       </c>
-      <c r="F106" s="3">
-        <v>1</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+      <c r="F107" s="3">
+        <v>1</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="B108" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="D107" s="8" t="s">
+      <c r="D108" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="E107" s="11">
+      <c r="E108" s="11">
         <v>296</v>
       </c>
-      <c r="F107" s="3">
-        <v>1</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+      <c r="F108" s="3">
+        <v>1</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="D108" s="8" t="s">
+      <c r="D109" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="E108" s="11">
+      <c r="E109" s="11">
         <v>36</v>
       </c>
-      <c r="F108" s="3">
-        <v>1</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="F109" s="3">
+        <v>1</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="s">
         <v>104</v>
       </c>
-      <c r="C109" t="s">
-        <v>136</v>
-      </c>
-      <c r="D109" s="7" t="s">
+      <c r="C110" t="s">
+        <v>136</v>
+      </c>
+      <c r="D110" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" t="s">
         <v>27</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>64</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>65</v>
       </c>
-      <c r="D110" s="7" t="s">
+      <c r="D111" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="s">
         <v>95</v>
       </c>
-      <c r="D111" s="7" t="s">
+      <c r="D112" s="7" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="113" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="D113" s="14" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="E113" s="13"/>
+    </row>
+    <row r="114" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C113" t="s">
+      <c r="B114" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C114" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="D113" s="7" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="D114" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E114" s="13"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" t="s">
         <v>80</v>
-      </c>
-      <c r="C114" t="s">
-        <v>136</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>97</v>
       </c>
       <c r="C115" t="s">
         <v>136</v>
@@ -3102,229 +3121,240 @@
         <v>137</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
+        <v>97</v>
+      </c>
+      <c r="C116" t="s">
+        <v>136</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" t="s">
         <v>10</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C117" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+    <row r="118" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="3" t="s">
+      <c r="B118" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="C117" s="3" t="s">
+      <c r="C118" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D117" s="8" t="s">
+      <c r="D118" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="E117" s="11">
+      <c r="E118" s="11">
         <v>117</v>
       </c>
-      <c r="F117" s="3">
-        <v>1</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>10</v>
-      </c>
-      <c r="C118" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F118" s="3">
+        <v>1</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>10</v>
       </c>
       <c r="C119" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>300</v>
-      </c>
-      <c r="E120" s="11">
-        <v>33</v>
-      </c>
-      <c r="F120" s="3">
-        <v>1</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B121" s="3" t="s">
+        <v>299</v>
+      </c>
       <c r="C121" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="E121" s="11"/>
-    </row>
-    <row r="122" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="E121" s="11">
+        <v>33</v>
+      </c>
+      <c r="F121" s="3">
+        <v>1</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D122" s="8"/>
-      <c r="E122" s="11">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="D122" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="E122" s="11"/>
+    </row>
+    <row r="123" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D123" s="8"/>
       <c r="E123" s="11">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D124" s="8"/>
+      <c r="E124" s="11">
         <v>599</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" t="s">
         <v>124</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C125" t="s">
         <v>239</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="D125" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" t="s">
         <v>161</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>163</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C126" t="s">
         <v>162</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>165</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C126" t="s">
-        <v>167</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>169</v>
-      </c>
-      <c r="B127" t="s">
-        <v>168</v>
+        <v>165</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C127" t="s">
+        <v>167</v>
       </c>
       <c r="D127" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>246</v>
+        <v>169</v>
       </c>
       <c r="B128" t="s">
-        <v>247</v>
+        <v>168</v>
       </c>
       <c r="D128" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>267</v>
+        <v>246</v>
+      </c>
+      <c r="B129" t="s">
+        <v>247</v>
       </c>
       <c r="D129" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>39</v>
-      </c>
-      <c r="C131" t="s">
-        <v>40</v>
+        <v>268</v>
       </c>
       <c r="D131" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E132" s="13">
-        <f>SUM(E2:E127)</f>
-        <v>19394</v>
-      </c>
-      <c r="F132" s="5" t="s">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" t="s">
+        <v>39</v>
+      </c>
+      <c r="C132" t="s">
+        <v>40</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E133" s="13">
+        <f>SUM(E2:E128)</f>
+        <v>19536</v>
+      </c>
+      <c r="F133" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E133" s="13">
-        <f>SUM(F2:F127)</f>
-        <v>40</v>
-      </c>
-      <c r="F133" s="5" t="s">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E134" s="13">
+        <f>SUM(F2:F128)</f>
+        <v>41</v>
+      </c>
+      <c r="F134" s="5" t="s">
         <v>241</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D124">
-    <sortCondition ref="A2:A124"/>
-    <sortCondition ref="C2:C124"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D125">
+    <sortCondition ref="A2:A125"/>
+    <sortCondition ref="C2:C125"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B126" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
-    <hyperlink ref="B33" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
-    <hyperlink ref="B71" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
-    <hyperlink ref="B29" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
-    <hyperlink ref="B18" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
+    <hyperlink ref="B127" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B34" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
+    <hyperlink ref="B72" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
+    <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
+    <hyperlink ref="B19" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
add triticum aestivum to workflow input
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/395010_2_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/1181128_2_8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{648528EA-2A51-46A0-AC9E-65190091873F}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEC694DE-D7C9-42F1-81E8-C3ADB98656A4}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2922" yWindow="114" windowWidth="20118" windowHeight="12846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="306">
   <si>
     <t>Species</t>
   </si>
@@ -948,6 +948,12 @@
   </si>
   <si>
     <t>https://doi.org/10.1038/s41588-020-00722-w</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41588-022-01189-7</t>
+  </si>
+  <si>
+    <t>PRJEB48988 (WGS) and PRJEB48738 (WGS)</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1030,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1051,8 +1057,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1337,7 +1347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -3086,29 +3098,43 @@
         <v>235</v>
       </c>
     </row>
-    <row r="113" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="5" t="s">
+    <row r="113" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D113" s="14" t="s">
+      <c r="B113" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D113" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="E113" s="13"/>
-    </row>
-    <row r="114" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="5" t="s">
+      <c r="E113" s="11">
+        <v>786</v>
+      </c>
+      <c r="F113" s="3">
+        <v>1</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="C114" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="D114" s="14" t="s">
+      <c r="D114" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="E114" s="13"/>
+      <c r="E114" s="16"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
@@ -3329,7 +3355,7 @@
     <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E133" s="13">
         <f>SUM(E2:E128)</f>
-        <v>19536</v>
+        <v>20322</v>
       </c>
       <c r="F133" s="5" t="s">
         <v>215</v>
@@ -3338,7 +3364,7 @@
     <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="E134" s="13">
         <f>SUM(F2:F128)</f>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F134" s="5" t="s">
         <v>241</v>

</xml_diff>

<commit_message>
add ploidy option to gatk haplotype caller, samples.tsv
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/1181128_2_8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/1181128_2_9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEC694DE-D7C9-42F1-81E8-C3ADB98656A4}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E490A58-4C96-4B65-AC1C-0143E4C37EB5}"/>
   <bookViews>
     <workbookView xWindow="2922" yWindow="114" windowWidth="20118" windowHeight="12846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,9 +671,6 @@
     <t>PRJNA622568</t>
   </si>
   <si>
-    <t>doi: 10.1371/journal.pbio.3001681</t>
-  </si>
-  <si>
     <t>Sample size</t>
   </si>
   <si>
@@ -836,9 +833,6 @@
     <t>3171 genomes are from this species, but publication mentions 3366</t>
   </si>
   <si>
-    <t>Publication mentions 414 genomes, but only 402 are on the SRA and only 337 genomes are of the relevant species</t>
-  </si>
-  <si>
     <t>Vanilla planifolia</t>
   </si>
   <si>
@@ -954,6 +948,12 @@
   </si>
   <si>
     <t>PRJEB48988 (WGS) and PRJEB48738 (WGS)</t>
+  </si>
+  <si>
+    <t>Not on phytozome; Publication mentions 414 genomes, but only 402 are on the SRA and only 337 genomes are of the relevant species</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41586-020-03127-1; doi: 10.1371/journal.pbio.3001681</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1030,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1055,13 +1055,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1347,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1375,13 +1368,13 @@
         <v>66</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" t="s">
         <v>259</v>
-      </c>
-      <c r="G1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1402,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1434,7 +1427,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1466,7 +1459,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1474,7 +1467,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="11">
@@ -1484,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1492,13 +1485,13 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1506,7 +1499,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -1519,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1582,13 +1575,13 @@
         <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E15" s="11">
         <v>597</v>
@@ -1597,7 +1590,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1622,7 +1615,7 @@
         <v>170</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E17" s="11">
         <v>467</v>
@@ -1631,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1653,13 +1646,13 @@
         <v>128</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>288</v>
       </c>
       <c r="E19" s="11">
         <v>56</v>
@@ -1668,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1682,7 +1675,7 @@
         <v>62</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1738,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1761,7 +1754,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1780,7 +1773,7 @@
         <v>59</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>61</v>
@@ -1795,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1822,13 +1815,13 @@
         <v>50</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E30" s="11">
         <v>52</v>
@@ -1837,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1873,7 +1866,7 @@
         <v>172</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E33" s="11">
         <v>296</v>
@@ -1882,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1896,7 +1889,7 @@
         <v>175</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E34" s="11">
         <v>3171</v>
@@ -1905,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1930,7 +1923,7 @@
         <v>43</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>266</v>
+        <v>304</v>
       </c>
       <c r="E36" s="11">
         <v>337</v>
@@ -1939,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1995,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2111,13 +2104,13 @@
         <v>45</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E50" s="11">
         <v>1674</v>
@@ -2126,7 +2119,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2134,13 +2127,13 @@
         <v>45</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E51" s="11">
         <v>240</v>
@@ -2151,13 +2144,13 @@
         <v>45</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>293</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>295</v>
       </c>
       <c r="E52" s="11">
         <v>279</v>
@@ -2174,7 +2167,7 @@
         <v>47</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2195,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2216,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2235,10 +2228,10 @@
         <v>112</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="11">
@@ -2248,7 +2241,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2259,7 +2252,7 @@
         <v>134</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2327,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2352,7 +2345,7 @@
         <v>190</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E65" s="11">
         <v>131</v>
@@ -2361,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2428,7 +2421,7 @@
         <v>199</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E70" s="11">
         <v>136</v>
@@ -2437,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2456,13 +2449,13 @@
         <v>100</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>202</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E72" s="11">
         <v>44</v>
@@ -2471,7 +2464,7 @@
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2490,10 +2483,10 @@
         <v>67</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>160</v>
@@ -2505,7 +2498,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2516,10 +2509,10 @@
         <v>203</v>
       </c>
       <c r="C75" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2533,7 +2526,7 @@
         <v>196</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="77" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2544,10 +2537,10 @@
         <v>20</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E77" s="11">
         <v>38</v>
@@ -2556,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2603,7 +2596,7 @@
         <v>206</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E81" s="11">
         <v>52</v>
@@ -2612,7 +2605,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2651,7 +2644,7 @@
         <v>4</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E84" s="12">
         <v>3024</v>
@@ -2660,7 +2653,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:7" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -2674,7 +2667,7 @@
         <v>47</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E85" s="11">
         <v>85</v>
@@ -2683,21 +2676,21 @@
         <v>1</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>211</v>
+      <c r="B86" s="6" t="s">
+        <v>305</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>210</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E86" s="11">
         <v>747</v>
@@ -2706,7 +2699,7 @@
         <v>1</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2738,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2763,7 +2756,7 @@
         <v>56</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E90" s="11">
         <v>52</v>
@@ -2772,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2818,13 +2811,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E95" s="11">
         <v>428</v>
@@ -2833,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2874,13 +2867,13 @@
         <v>131</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E99" s="11">
         <v>909</v>
@@ -2889,7 +2882,7 @@
         <v>1</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2897,13 +2890,13 @@
         <v>132</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E100" s="11">
         <v>38</v>
@@ -2912,7 +2905,7 @@
         <v>1</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2928,7 +2921,7 @@
         <v>18</v>
       </c>
       <c r="C102" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>145</v>
@@ -2939,10 +2932,10 @@
         <v>18</v>
       </c>
       <c r="B103" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="D103" s="8" t="s">
         <v>160</v>
@@ -2954,7 +2947,7 @@
         <v>1</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2962,10 +2955,10 @@
         <v>79</v>
       </c>
       <c r="C104" t="s">
+        <v>223</v>
+      </c>
+      <c r="D104" s="7" t="s">
         <v>224</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2987,13 +2980,13 @@
         <v>31</v>
       </c>
       <c r="B106" t="s">
+        <v>226</v>
+      </c>
+      <c r="C106" t="s">
+        <v>225</v>
+      </c>
+      <c r="D106" s="7" t="s">
         <v>227</v>
-      </c>
-      <c r="C106" t="s">
-        <v>226</v>
-      </c>
-      <c r="D106" s="7" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3001,10 +2994,10 @@
         <v>31</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>229</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>230</v>
       </c>
       <c r="D107" s="8" t="s">
         <v>160</v>
@@ -3016,7 +3009,7 @@
         <v>1</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="108" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3024,13 +3017,13 @@
         <v>75</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D108" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E108" s="11">
         <v>296</v>
@@ -3039,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3047,13 +3040,13 @@
         <v>123</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E109" s="11">
         <v>36</v>
@@ -3062,7 +3055,7 @@
         <v>1</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3095,7 +3088,7 @@
         <v>95</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3103,13 +3096,13 @@
         <v>23</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D113" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E113" s="11">
         <v>786</v>
@@ -3118,23 +3111,22 @@
         <v>1</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" t="s">
         <v>32</v>
       </c>
-      <c r="B114" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="C114" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="D114" s="15" t="s">
+      <c r="B114" t="s">
+        <v>301</v>
+      </c>
+      <c r="C114" t="s">
+        <v>236</v>
+      </c>
+      <c r="D114" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="E114" s="16"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
@@ -3171,13 +3163,13 @@
         <v>10</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E118" s="11">
         <v>117</v>
@@ -3186,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3210,13 +3202,13 @@
         <v>9</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E121" s="11">
         <v>33</v>
@@ -3225,7 +3217,7 @@
         <v>1</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="122" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3236,7 +3228,7 @@
         <v>7</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E122" s="11"/>
     </row>
@@ -3269,10 +3261,10 @@
         <v>124</v>
       </c>
       <c r="C125" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D125" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3316,10 +3308,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
+        <v>245</v>
+      </c>
+      <c r="B129" t="s">
         <v>246</v>
-      </c>
-      <c r="B129" t="s">
-        <v>247</v>
       </c>
       <c r="D129" s="7" t="s">
         <v>164</v>
@@ -3327,7 +3319,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>164</v>
@@ -3335,7 +3327,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D131" s="7" t="s">
         <v>164</v>
@@ -3358,7 +3350,7 @@
         <v>20322</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3367,7 +3359,7 @@
         <v>42</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -3381,8 +3373,9 @@
     <hyperlink ref="B72" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
     <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
     <hyperlink ref="B19" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
+    <hyperlink ref="B86" r:id="rId6" xr:uid="{2677786D-08C7-4346-837D-960E754FAB79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more species to workflow
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/1181128_2_9/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/1181128_2_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E490A58-4C96-4B65-AC1C-0143E4C37EB5}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC17FF5A-CDD5-4C91-86F2-659F2DA424AC}"/>
   <bookViews>
     <workbookView xWindow="2922" yWindow="114" windowWidth="20118" windowHeight="12846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="313">
   <si>
     <t>Species</t>
   </si>
@@ -500,9 +500,6 @@
     <t>https://doi.org/10.1038/s41467-020-17302-5</t>
   </si>
   <si>
-    <t>See Supplemental Data 4 in publication</t>
-  </si>
-  <si>
     <t>PRJNA544934</t>
   </si>
   <si>
@@ -950,10 +947,34 @@
     <t>PRJEB48988 (WGS) and PRJEB48738 (WGS)</t>
   </si>
   <si>
-    <t>Not on phytozome; Publication mentions 414 genomes, but only 402 are on the SRA and only 337 genomes are of the relevant species</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1038/s41586-020-03127-1; doi: 10.1371/journal.pbio.3001681</t>
+  </si>
+  <si>
+    <t>Not on phytozome, but on ensembl; Publication mentions 414 genomes, but only 402 are on the SRA and only 337 genomes are of the relevant species</t>
+  </si>
+  <si>
+    <t>Not on phytozome, but on ensembl</t>
+  </si>
+  <si>
+    <t>PRJNA590636</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpls.2019.01682</t>
+  </si>
+  <si>
+    <t>200 accessions</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/1755-0998.12991</t>
+  </si>
+  <si>
+    <t>PRJNA489364</t>
+  </si>
+  <si>
+    <t>Available on Ensembl</t>
+  </si>
+  <si>
+    <t>See Supplemental Data 4 in publication; generally can't find much data; only includes 9 genotypes</t>
   </si>
 </sst>
 </file>
@@ -1338,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G134"/>
+  <dimension ref="A1:G136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1368,13 +1389,13 @@
         <v>66</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1" t="s">
         <v>258</v>
-      </c>
-      <c r="G1" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1395,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1427,7 +1448,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1459,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1467,7 +1488,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="11">
@@ -1477,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1485,13 +1506,13 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1499,7 +1520,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
@@ -1512,7 +1533,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1575,13 +1596,13 @@
         <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E15" s="11">
         <v>597</v>
@@ -1590,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1609,13 +1630,13 @@
         <v>105</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E17" s="11">
         <v>467</v>
@@ -1624,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1646,13 +1667,13 @@
         <v>128</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="E19" s="11">
         <v>56</v>
@@ -1661,7 +1682,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1675,10 +1696,10 @@
         <v>62</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -1686,7 +1707,7 @@
         <v>153</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>154</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1705,10 +1726,10 @@
         <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1716,13 +1737,13 @@
         <v>108</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="E24" s="11">
         <v>119</v>
@@ -1731,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1739,13 +1760,13 @@
         <v>109</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>159</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>160</v>
       </c>
       <c r="E25" s="11">
         <v>199</v>
@@ -1754,7 +1775,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1762,7 +1783,7 @@
         <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>145</v>
@@ -1773,13 +1794,13 @@
         <v>59</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E27" s="11">
         <v>40</v>
@@ -1788,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1807,7 +1828,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1815,13 +1836,13 @@
         <v>50</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E30" s="11">
         <v>52</v>
@@ -1830,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1860,13 +1881,13 @@
         <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E33" s="11">
         <v>296</v>
@@ -1875,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1883,13 +1904,13 @@
         <v>84</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E34" s="11">
         <v>3171</v>
@@ -1898,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1932,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1973,13 +1994,13 @@
         <v>85</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E40" s="11">
         <v>115</v>
@@ -1988,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1996,10 +2017,10 @@
         <v>85</v>
       </c>
       <c r="B41" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" t="s">
         <v>177</v>
-      </c>
-      <c r="C41" t="s">
-        <v>178</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>145</v>
@@ -2010,10 +2031,10 @@
         <v>85</v>
       </c>
       <c r="B42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>145</v>
@@ -2035,10 +2056,10 @@
         <v>121</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>145</v>
@@ -2104,13 +2125,13 @@
         <v>45</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E50" s="11">
         <v>1674</v>
@@ -2119,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2127,13 +2148,13 @@
         <v>45</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>290</v>
-      </c>
       <c r="D51" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E51" s="11">
         <v>240</v>
@@ -2144,13 +2165,13 @@
         <v>45</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>292</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>293</v>
       </c>
       <c r="E52" s="11">
         <v>279</v>
@@ -2167,7 +2188,7 @@
         <v>47</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2175,10 +2196,10 @@
         <v>88</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>184</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="11">
@@ -2188,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2196,10 +2217,10 @@
         <v>110</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="11">
@@ -2209,7 +2230,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2228,10 +2249,10 @@
         <v>112</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="11">
@@ -2241,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2252,7 +2273,7 @@
         <v>134</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2307,10 +2328,10 @@
         <v>24</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>189</v>
       </c>
       <c r="D63" s="8"/>
       <c r="E63" s="11">
@@ -2320,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2339,13 +2360,13 @@
         <v>77</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E65" s="11">
         <v>131</v>
@@ -2354,7 +2375,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2362,10 +2383,10 @@
         <v>89</v>
       </c>
       <c r="B66" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C66" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>145</v>
@@ -2376,407 +2397,419 @@
         <v>90</v>
       </c>
       <c r="B67" t="s">
+        <v>193</v>
+      </c>
+      <c r="C67" t="s">
         <v>194</v>
-      </c>
-      <c r="C67" t="s">
-        <v>195</v>
       </c>
       <c r="D67" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" t="s">
+    <row r="68" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B68" t="s">
-        <v>136</v>
-      </c>
-      <c r="C68" t="s">
-        <v>197</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>198</v>
+      <c r="B68" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="E68" s="11">
+        <v>200</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" t="s">
+        <v>136</v>
+      </c>
+      <c r="C69" t="s">
+        <v>196</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
         <v>28</v>
       </c>
-      <c r="C69" t="s">
-        <v>136</v>
-      </c>
-      <c r="D69" s="7" t="s">
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="3" t="s">
+    <row r="71" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B71" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D71" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="E71" s="11">
+        <v>136</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" t="s">
+        <v>136</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D73" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E73" s="11">
+        <v>44</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" t="s">
         <v>200</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>268</v>
-      </c>
-      <c r="E70" s="11">
-        <v>136</v>
-      </c>
-      <c r="F70" s="3">
-        <v>1</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" t="s">
-        <v>92</v>
-      </c>
-      <c r="C71" t="s">
-        <v>136</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="D72" s="8" t="s">
+      <c r="D74" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="E72" s="11">
-        <v>44</v>
-      </c>
-      <c r="F72" s="3">
-        <v>1</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" t="s">
-        <v>100</v>
-      </c>
-      <c r="C73" t="s">
-        <v>201</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E74" s="3">
+      <c r="D75" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E75" s="3">
         <v>39</v>
       </c>
-      <c r="F74" s="3">
-        <v>1</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" t="s">
-        <v>203</v>
-      </c>
-      <c r="C75" t="s">
-        <v>253</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F75" s="3">
+        <v>1</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="C76" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" t="s">
+        <v>184</v>
+      </c>
+      <c r="C77" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="E77" s="11">
+      <c r="C78" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E78" s="11">
         <v>38</v>
       </c>
-      <c r="F77" s="3">
-        <v>1</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" t="s">
-        <v>129</v>
-      </c>
-      <c r="C78" t="s">
-        <v>136</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>204</v>
+      <c r="F78" s="3">
+        <v>1</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C79" t="s">
         <v>136</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
+        <v>122</v>
+      </c>
+      <c r="C80" t="s">
+        <v>136</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
         <v>69</v>
       </c>
-      <c r="C80" t="s">
-        <v>136</v>
-      </c>
-      <c r="D80" s="7" t="s">
+      <c r="C81" t="s">
+        <v>136</v>
+      </c>
+      <c r="D81" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="3" t="s">
+    <row r="82" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C81" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D81" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="E81" s="11">
+      <c r="C82" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E82" s="11">
         <v>52</v>
       </c>
-      <c r="F81" s="3">
-        <v>1</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" t="s">
-        <v>78</v>
-      </c>
-      <c r="B82" t="s">
-        <v>136</v>
-      </c>
-      <c r="C82" t="s">
-        <v>205</v>
+      <c r="F82" s="3">
+        <v>1</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
+        <v>78</v>
+      </c>
+      <c r="B83" t="s">
+        <v>136</v>
+      </c>
+      <c r="C83" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
         <v>125</v>
       </c>
-      <c r="B83" t="s">
-        <v>136</v>
-      </c>
-      <c r="C83" t="s">
-        <v>136</v>
-      </c>
-      <c r="D83" s="7" t="s">
+      <c r="B84" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" t="s">
+        <v>136</v>
+      </c>
+      <c r="D84" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="3" t="s">
+    <row r="85" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B85" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="E85" s="12">
+        <v>3024</v>
+      </c>
+      <c r="F85" s="3">
+        <v>1</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C84" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D84" s="8" t="s">
+      <c r="C86" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E86" s="11">
+        <v>85</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D87" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="E84" s="12">
-        <v>3024</v>
-      </c>
-      <c r="F84" s="3">
-        <v>1</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="E85" s="11">
-        <v>85</v>
-      </c>
-      <c r="F85" s="3">
-        <v>1</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="E86" s="11">
+      <c r="E87" s="11">
         <v>747</v>
       </c>
-      <c r="F86" s="3">
-        <v>1</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" t="s">
+      <c r="F87" s="3">
+        <v>1</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="s">
         <v>93</v>
       </c>
-      <c r="C87" t="s">
-        <v>136</v>
-      </c>
-      <c r="D87" s="7" t="s">
+      <c r="C88" t="s">
+        <v>136</v>
+      </c>
+      <c r="D88" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="3" t="s">
+    <row r="89" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D88" s="8"/>
-      <c r="E88" s="11">
+      <c r="D89" s="8"/>
+      <c r="E89" s="11">
         <v>683</v>
       </c>
-      <c r="F88" s="3">
-        <v>1</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" t="s">
+      <c r="F89" s="3">
+        <v>1</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
         <v>118</v>
       </c>
-      <c r="C89" t="s">
-        <v>136</v>
-      </c>
-      <c r="D89" s="7" t="s">
+      <c r="C90" t="s">
+        <v>136</v>
+      </c>
+      <c r="D90" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="3" t="s">
+    <row r="91" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D90" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="E90" s="11">
+      <c r="D91" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="E91" s="11">
         <v>52</v>
       </c>
-      <c r="F90" s="3">
-        <v>1</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" t="s">
-        <v>51</v>
-      </c>
-      <c r="B91" t="s">
-        <v>54</v>
-      </c>
-      <c r="C91" t="s">
-        <v>53</v>
+      <c r="F91" s="3">
+        <v>1</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2784,65 +2817,65 @@
         <v>51</v>
       </c>
       <c r="B92" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C92" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>51</v>
       </c>
+      <c r="B93" t="s">
+        <v>57</v>
+      </c>
       <c r="C93" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>51</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>51</v>
+      </c>
+      <c r="B95" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="3" t="s">
+    <row r="96" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C95" s="3" t="s">
+      <c r="B96" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="D95" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="E95" s="11">
+      <c r="C96" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E96" s="11">
         <v>428</v>
       </c>
-      <c r="F95" s="3">
-        <v>1</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" t="s">
-        <v>101</v>
-      </c>
-      <c r="C96" t="s">
-        <v>136</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>137</v>
+      <c r="F96" s="3">
+        <v>1</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C97" t="s">
         <v>136</v>
@@ -2853,7 +2886,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C98" t="s">
         <v>136</v>
@@ -2862,58 +2895,61 @@
         <v>137</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="E99" s="11">
-        <v>909</v>
-      </c>
-      <c r="F99" s="3">
-        <v>1</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>260</v>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" t="s">
+        <v>107</v>
+      </c>
+      <c r="C99" t="s">
+        <v>136</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="E100" s="11">
+        <v>909</v>
+      </c>
+      <c r="F100" s="3">
+        <v>1</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B100" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C100" s="3" t="s">
+      <c r="B101" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="D100" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="E100" s="11">
+      <c r="C101" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="E101" s="11">
         <v>38</v>
       </c>
-      <c r="F100" s="3">
-        <v>1</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" t="s">
-        <v>18</v>
-      </c>
-      <c r="C101" t="s">
-        <v>17</v>
+      <c r="F101" s="3">
+        <v>1</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2921,58 +2957,52 @@
         <v>18</v>
       </c>
       <c r="C102" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>18</v>
+      </c>
+      <c r="C103" t="s">
+        <v>218</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D102" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B103" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C103" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D103" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E103" s="11">
+      <c r="D104" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E104" s="11">
         <v>360</v>
       </c>
-      <c r="F103" s="3">
-        <v>1</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" t="s">
-        <v>79</v>
-      </c>
-      <c r="C104" t="s">
-        <v>223</v>
-      </c>
-      <c r="D104" s="7" t="s">
-        <v>224</v>
+      <c r="F104" s="3">
+        <v>1</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>31</v>
-      </c>
-      <c r="B105" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="C105" t="s">
-        <v>33</v>
+        <v>222</v>
       </c>
       <c r="D105" s="7" t="s">
-        <v>145</v>
+        <v>223</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2980,168 +3010,180 @@
         <v>31</v>
       </c>
       <c r="B106" t="s">
+        <v>34</v>
+      </c>
+      <c r="C106" t="s">
+        <v>33</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" t="s">
+        <v>31</v>
+      </c>
+      <c r="B107" t="s">
+        <v>225</v>
+      </c>
+      <c r="C107" t="s">
+        <v>224</v>
+      </c>
+      <c r="D107" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="C106" t="s">
-        <v>225</v>
-      </c>
-      <c r="D106" s="7" t="s">
+    </row>
+    <row r="108" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B107" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="E107" s="11">
+      <c r="D108" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E108" s="11">
         <v>400</v>
       </c>
-      <c r="F107" s="3">
-        <v>1</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="E108" s="11">
-        <v>296</v>
-      </c>
       <c r="F108" s="3">
         <v>1</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="109" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="E109" s="11">
+        <v>296</v>
+      </c>
+      <c r="F109" s="3">
+        <v>1</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B109" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C109" s="3" t="s">
+      <c r="B110" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D109" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="E109" s="11">
+      <c r="C110" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E110" s="11">
         <v>36</v>
       </c>
-      <c r="F109" s="3">
-        <v>1</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" t="s">
-        <v>104</v>
-      </c>
-      <c r="C110" t="s">
-        <v>136</v>
-      </c>
-      <c r="D110" s="7" t="s">
-        <v>137</v>
+      <c r="F110" s="3">
+        <v>1</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>27</v>
-      </c>
-      <c r="B111" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="C111" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
+        <v>27</v>
+      </c>
+      <c r="B112" t="s">
+        <v>64</v>
+      </c>
+      <c r="C112" t="s">
+        <v>65</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
         <v>95</v>
       </c>
-      <c r="D112" s="7" t="s">
+      <c r="D113" s="7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D114" s="8" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="D113" s="8" t="s">
+      <c r="E114" s="11">
+        <v>786</v>
+      </c>
+      <c r="F114" s="3">
+        <v>1</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E113" s="11">
-        <v>786</v>
-      </c>
-      <c r="F113" s="3">
-        <v>1</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" t="s">
-        <v>32</v>
-      </c>
-      <c r="B114" t="s">
-        <v>301</v>
-      </c>
-      <c r="C114" t="s">
-        <v>236</v>
-      </c>
-      <c r="D114" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" t="s">
-        <v>80</v>
-      </c>
-      <c r="C115" t="s">
-        <v>136</v>
-      </c>
-      <c r="D115" s="7" t="s">
-        <v>137</v>
+      <c r="D115" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="E115" s="11">
+        <v>114</v>
+      </c>
+      <c r="F115" s="3">
+        <v>1</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C116" t="s">
         <v>136</v>
@@ -3152,41 +3194,44 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
+        <v>97</v>
+      </c>
+      <c r="C117" t="s">
+        <v>136</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" t="s">
         <v>10</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C118" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="3" t="s">
+    <row r="119" spans="1:7" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B118" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C118" s="3" t="s">
+      <c r="B119" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D118" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="E118" s="11">
+      <c r="D119" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="E119" s="11">
         <v>117</v>
       </c>
-      <c r="F118" s="3">
-        <v>1</v>
-      </c>
-      <c r="G118" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" t="s">
-        <v>10</v>
-      </c>
-      <c r="C119" t="s">
-        <v>13</v>
+      <c r="F119" s="3">
+        <v>1</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3194,186 +3239,217 @@
         <v>10</v>
       </c>
       <c r="C120" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D121" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="E121" s="11">
-        <v>33</v>
-      </c>
-      <c r="F121" s="3">
-        <v>1</v>
-      </c>
-      <c r="G121" s="3" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="122" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B122" s="3" t="s">
+        <v>296</v>
+      </c>
       <c r="C122" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="E122" s="11"/>
+        <v>297</v>
+      </c>
+      <c r="E122" s="11">
+        <v>33</v>
+      </c>
+      <c r="F122" s="3">
+        <v>1</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="123" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D123" s="8"/>
-      <c r="E123" s="11">
-        <v>277</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D123" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="E123" s="11"/>
     </row>
     <row r="124" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D124" s="8"/>
       <c r="E124" s="11">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" s="8"/>
+      <c r="E125" s="11">
         <v>599</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" t="s">
-        <v>124</v>
-      </c>
-      <c r="C125" t="s">
-        <v>238</v>
-      </c>
-      <c r="D125" s="7" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>161</v>
-      </c>
-      <c r="B126" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
       <c r="C126" t="s">
-        <v>162</v>
+        <v>237</v>
       </c>
       <c r="D126" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" t="s">
-        <v>165</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C127" t="s">
-        <v>167</v>
-      </c>
-      <c r="D127" s="7" t="s">
-        <v>164</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D127" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="E127" s="11">
+        <v>306</v>
+      </c>
+      <c r="F127" s="3">
+        <v>1</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B128" t="s">
-        <v>168</v>
+        <v>162</v>
+      </c>
+      <c r="C128" t="s">
+        <v>161</v>
       </c>
       <c r="D128" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>245</v>
-      </c>
-      <c r="B129" t="s">
-        <v>246</v>
+        <v>164</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C129" t="s">
+        <v>166</v>
       </c>
       <c r="D129" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>265</v>
+        <v>168</v>
+      </c>
+      <c r="B130" t="s">
+        <v>167</v>
       </c>
       <c r="D130" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>266</v>
+        <v>244</v>
+      </c>
+      <c r="B131" t="s">
+        <v>245</v>
       </c>
       <c r="D131" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
+        <v>264</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" t="s">
+        <v>265</v>
+      </c>
+      <c r="D133" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" t="s">
         <v>39</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C134" t="s">
         <v>40</v>
       </c>
-      <c r="D132" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E133" s="13">
-        <f>SUM(E2:E128)</f>
-        <v>20322</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E134" s="13">
-        <f>SUM(F2:F128)</f>
-        <v>42</v>
-      </c>
-      <c r="F134" s="5" t="s">
-        <v>240</v>
+      <c r="D134" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E135" s="13">
+        <f>SUM(E2:E130)</f>
+        <v>20942</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="E136" s="13">
+        <f>SUM(F2:F130)</f>
+        <v>45</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D125">
-    <sortCondition ref="A2:A125"/>
-    <sortCondition ref="C2:C125"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D126">
+    <sortCondition ref="A2:A126"/>
+    <sortCondition ref="C2:C126"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B127" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B129" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
     <hyperlink ref="B34" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
-    <hyperlink ref="B72" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
+    <hyperlink ref="B73" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
     <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
     <hyperlink ref="B19" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
-    <hyperlink ref="B86" r:id="rId6" xr:uid="{2677786D-08C7-4346-837D-960E754FAB79}"/>
+    <hyperlink ref="B87" r:id="rId6" xr:uid="{2677786D-08C7-4346-837D-960E754FAB79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
add cannabis and rye
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{223FC408-33A9-4519-AFE5-3E0850D95F17}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF692185-FACC-4AAA-9031-B905214276EE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="335">
   <si>
     <t>Species</t>
   </si>
@@ -1014,6 +1014,33 @@
   </si>
   <si>
     <t>https://doi.org/10.1016/j.molp.2018.11.007</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.13436</t>
+  </si>
+  <si>
+    <t>PRJEB6215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostly found GBS data, but there may be WGS data for about 10 lines </t>
+  </si>
+  <si>
+    <t>Camelina sativa</t>
+  </si>
+  <si>
+    <t>Found RAD-Seq data, but not WGS</t>
+  </si>
+  <si>
+    <t>Cannabis sativa</t>
+  </si>
+  <si>
+    <t>PRJNA866500</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/g3journal/jkac209</t>
+  </si>
+  <si>
+    <t>Lots more GBS and RAD-seq data</t>
   </si>
 </sst>
 </file>
@@ -1398,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H141"/>
+  <dimension ref="A1:H143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F142" sqref="F142"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3483,42 +3510,78 @@
         <v>259</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="133" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
         <v>313</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E133" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="F133" s="11">
+        <v>10</v>
+      </c>
+      <c r="G133" s="3">
+        <v>1</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>164</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C134" t="s">
-        <v>166</v>
+        <v>329</v>
+      </c>
+      <c r="D134" t="s">
+        <v>323</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>168</v>
-      </c>
-      <c r="B135" t="s">
-        <v>167</v>
-      </c>
-      <c r="E135" s="7" t="s">
-        <v>163</v>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E135" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F135" s="11">
+        <v>135</v>
+      </c>
+      <c r="G135" s="3">
+        <v>1</v>
+      </c>
+      <c r="H135" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>244</v>
-      </c>
-      <c r="B136" t="s">
-        <v>245</v>
+        <v>164</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C136" t="s">
+        <v>166</v>
       </c>
       <c r="E136" s="7" t="s">
         <v>163</v>
@@ -3526,7 +3589,10 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>264</v>
+        <v>168</v>
+      </c>
+      <c r="B137" t="s">
+        <v>167</v>
       </c>
       <c r="E137" s="7" t="s">
         <v>163</v>
@@ -3534,7 +3600,10 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>265</v>
+        <v>244</v>
+      </c>
+      <c r="B138" t="s">
+        <v>245</v>
       </c>
       <c r="E138" s="7" t="s">
         <v>163</v>
@@ -3542,30 +3611,46 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>39</v>
-      </c>
-      <c r="C139" t="s">
-        <v>40</v>
+        <v>264</v>
       </c>
       <c r="E139" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F140" s="13">
-        <f>SUM(F2:F135)</f>
-        <v>22734</v>
-      </c>
-      <c r="G140" s="5" t="s">
+      <c r="A140" t="s">
+        <v>265</v>
+      </c>
+      <c r="E140" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>39</v>
+      </c>
+      <c r="C141" t="s">
+        <v>40</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F142" s="13">
+        <f>SUM(F2:F137)</f>
+        <v>22879</v>
+      </c>
+      <c r="G142" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F141" s="13">
-        <f>SUM(G2:G135)</f>
-        <v>48</v>
-      </c>
-      <c r="G141" s="5" t="s">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F143" s="13">
+        <f>SUM(G2:G137)</f>
+        <v>50</v>
+      </c>
+      <c r="G143" s="5" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3575,7 +3660,7 @@
     <sortCondition ref="C2:C126"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B134" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B136" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
     <hyperlink ref="B34" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
     <hyperlink ref="B73" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
     <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>

</xml_diff>

<commit_message>
add coffea, cucumis melo
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF692185-FACC-4AAA-9031-B905214276EE}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="13_ncr:1_{F5DFC21C-F620-48EC-BA16-3E8E7C14D37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7591A721-C38F-4D11-BA73-A3E3319A37DD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="353">
   <si>
     <t>Species</t>
   </si>
@@ -1041,6 +1041,60 @@
   </si>
   <si>
     <t>Lots more GBS and RAD-seq data</t>
+  </si>
+  <si>
+    <t>Capsicum annuum</t>
+  </si>
+  <si>
+    <t>GBS data for 10000 accessions</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/dnares/dsac052</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRJDB14137 </t>
+  </si>
+  <si>
+    <t>Chara braunii</t>
+  </si>
+  <si>
+    <t>Chlamydomonas reinhardtii</t>
+  </si>
+  <si>
+    <t>Not sure if I should include single-cell plants?</t>
+  </si>
+  <si>
+    <t>Chondrus crispus</t>
+  </si>
+  <si>
+    <t>couldn't find WGS data in SRA</t>
+  </si>
+  <si>
+    <t>couldn't find anything in SRA; though didn't Corbett-Detig include this in their study?</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11103-020-00974-4</t>
+  </si>
+  <si>
+    <t>Coffea canephora</t>
+  </si>
+  <si>
+    <t>PRJNA505204</t>
+  </si>
+  <si>
+    <t>More GBS data in SRA</t>
+  </si>
+  <si>
+    <t>Corchorus capsularis</t>
+  </si>
+  <si>
+    <t>Corylus avellana</t>
+  </si>
+  <si>
+    <t>RAD-seq and GBS data, WGS data only looks at chloroplast? See PRJNA693261</t>
+  </si>
+  <si>
+    <t>WGS data for maybe 3 genomes?</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1142,6 +1196,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1425,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H143"/>
+  <dimension ref="A1:H152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144:XFD144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2026,7 +2087,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>116</v>
       </c>
@@ -2034,7 +2095,7 @@
         <v>136</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>137</v>
+        <v>344</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -3573,84 +3634,197 @@
         <v>259</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="136" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E136" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="F136" s="11">
+        <v>7</v>
+      </c>
+      <c r="G136" s="3">
+        <v>1</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="D137" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="E137" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F137" s="16"/>
+    </row>
+    <row r="138" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="E138" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="F138" s="16"/>
+    </row>
+    <row r="139" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="E139" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="F139" s="16"/>
+    </row>
+    <row r="140" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E140" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="F140" s="11">
+        <v>34</v>
+      </c>
+      <c r="G140" s="3">
+        <v>1</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="E141" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F141" s="16"/>
+    </row>
+    <row r="142" spans="1:8" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A142" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="E142" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="F142" s="16"/>
+    </row>
+    <row r="143" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E143" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="F143" s="16"/>
+    </row>
+    <row r="144" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E144" s="15"/>
+      <c r="F144" s="16"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>164</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B145" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C145" t="s">
         <v>166</v>
       </c>
-      <c r="E136" s="7" t="s">
+      <c r="E145" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>168</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B146" t="s">
         <v>167</v>
       </c>
-      <c r="E137" s="7" t="s">
+      <c r="E146" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>244</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B147" t="s">
         <v>245</v>
       </c>
-      <c r="E138" s="7" t="s">
+      <c r="E147" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>264</v>
       </c>
-      <c r="E139" s="7" t="s">
+      <c r="E148" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>265</v>
       </c>
-      <c r="E140" s="7" t="s">
+      <c r="E149" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>39</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C150" t="s">
         <v>40</v>
       </c>
-      <c r="E141" s="7" t="s">
+      <c r="E150" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F142" s="13">
-        <f>SUM(F2:F137)</f>
-        <v>22879</v>
-      </c>
-      <c r="G142" s="5" t="s">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F151" s="13">
+        <f>SUM(F2:F146)</f>
+        <v>22920</v>
+      </c>
+      <c r="G151" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F143" s="13">
-        <f>SUM(G2:G137)</f>
-        <v>50</v>
-      </c>
-      <c r="G143" s="5" t="s">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F152" s="13">
+        <f>SUM(G2:G146)</f>
+        <v>52</v>
+      </c>
+      <c r="G152" s="5" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3660,7 +3834,7 @@
     <sortCondition ref="C2:C126"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B136" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B145" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
     <hyperlink ref="B34" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
     <hyperlink ref="B73" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
     <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>

</xml_diff>

<commit_message>
add Juglans regia, Lupinus angustifolius, Oryza barthii
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198290_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE602FAE-5492-4711-839D-042A1F5CDEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{88011C5E-FC03-4010-96B4-9DF5C02F9AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{723F50A0-402E-4C20-8B43-2664BB9AAC77}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="387">
   <si>
     <t>Species</t>
   </si>
@@ -1137,6 +1137,66 @@
   </si>
   <si>
     <t>Eragrostis tef</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpls.2021.647599</t>
+  </si>
+  <si>
+    <t>Ficus carica</t>
+  </si>
+  <si>
+    <t>More RAD-seq data in SRA</t>
+  </si>
+  <si>
+    <t>Galdieria sulphuraria</t>
+  </si>
+  <si>
+    <t>Ipomoea triloba</t>
+  </si>
+  <si>
+    <t>can't find WGS data in SRA</t>
+  </si>
+  <si>
+    <t>Juglans regia</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s13059-021-02517-6</t>
+  </si>
+  <si>
+    <t>PRJNA721107</t>
+  </si>
+  <si>
+    <t>Leersia perrieri</t>
+  </si>
+  <si>
+    <t>Lolium perenne</t>
+  </si>
+  <si>
+    <t>Lupinus angustifolius</t>
+  </si>
+  <si>
+    <t>PRJNA797109</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.15885</t>
+  </si>
+  <si>
+    <t>Marchantia polymorpha</t>
+  </si>
+  <si>
+    <t>Nicotiana attenuata</t>
+  </si>
+  <si>
+    <t>Oryza barthii</t>
+  </si>
+  <si>
+    <t>PRJDB4702</t>
+  </si>
+  <si>
+    <t>can't find publication that generated the data, though other papers have used the data before</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.15516</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1273,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1246,6 +1306,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1528,10 +1591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H159"/>
+  <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3803,29 +3866,27 @@
         <v>259</v>
       </c>
     </row>
-    <row r="145" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14" t="s">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>356</v>
       </c>
-      <c r="D145" s="14" t="s">
+      <c r="D145" t="s">
         <v>323</v>
       </c>
-      <c r="E145" s="15" t="s">
+      <c r="E145" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="F145" s="16"/>
-    </row>
-    <row r="146" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14" t="s">
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>358</v>
       </c>
-      <c r="D146" s="14" t="s">
+      <c r="D146" t="s">
         <v>323</v>
       </c>
-      <c r="E146" s="15" t="s">
+      <c r="E146" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="F146" s="16"/>
     </row>
     <row r="147" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
@@ -3851,132 +3912,283 @@
         <v>259</v>
       </c>
     </row>
-    <row r="148" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14" t="s">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>362</v>
       </c>
-      <c r="D148" s="14" t="s">
+      <c r="D148" t="s">
         <v>323</v>
       </c>
-      <c r="E148" s="15" t="s">
+      <c r="E148" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="F148" s="16"/>
-    </row>
-    <row r="149" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="14" t="s">
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>364</v>
       </c>
-      <c r="D149" s="14" t="s">
+      <c r="D149" t="s">
         <v>323</v>
       </c>
-      <c r="E149" s="15" t="s">
+      <c r="E149" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="F149" s="16"/>
-    </row>
-    <row r="150" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14" t="s">
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>365</v>
       </c>
-      <c r="D150" s="14" t="s">
+      <c r="D150" t="s">
         <v>323</v>
       </c>
-      <c r="E150" s="15" t="s">
+      <c r="E150" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="F150" s="16"/>
-    </row>
-    <row r="151" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14" t="s">
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>366</v>
       </c>
-      <c r="D151" s="14" t="s">
+      <c r="D151" t="s">
         <v>323</v>
       </c>
-      <c r="E151" s="15" t="s">
+      <c r="E151" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="F151" s="16"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>164</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C152" t="s">
-        <v>166</v>
-      </c>
-      <c r="E152" s="7" t="s">
-        <v>163</v>
+    </row>
+    <row r="152" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E152" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="F152" s="11">
+        <v>14</v>
+      </c>
+      <c r="G152" s="3">
+        <v>1</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>168</v>
-      </c>
-      <c r="B153" t="s">
-        <v>167</v>
+        <v>370</v>
       </c>
       <c r="E153" s="7" t="s">
-        <v>163</v>
+        <v>357</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>371</v>
+      </c>
+      <c r="E154" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E155" s="8"/>
+      <c r="F155" s="11">
+        <v>550</v>
+      </c>
+      <c r="G155" s="3">
+        <v>1</v>
+      </c>
+      <c r="H155" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="D156" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="E156" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="F156" s="16"/>
+    </row>
+    <row r="157" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="D157" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="E157" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="F157" s="16"/>
+    </row>
+    <row r="158" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E158" s="8"/>
+      <c r="F158" s="11">
+        <v>55</v>
+      </c>
+      <c r="G158" s="3">
+        <v>1</v>
+      </c>
+      <c r="H158" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="E159" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="F159" s="16"/>
+    </row>
+    <row r="160" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="E160" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="F160" s="16"/>
+    </row>
+    <row r="161" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D161" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="E161" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="F161" s="13">
+        <v>21</v>
+      </c>
+      <c r="G161" s="5">
+        <v>1</v>
+      </c>
+      <c r="H161" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>164</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C162" t="s">
+        <v>166</v>
+      </c>
+      <c r="E162" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>168</v>
+      </c>
+      <c r="B163" t="s">
+        <v>167</v>
+      </c>
+      <c r="E163" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>244</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B164" t="s">
         <v>245</v>
       </c>
-      <c r="E154" s="7" t="s">
+      <c r="E164" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>264</v>
       </c>
-      <c r="E155" s="7" t="s">
+      <c r="E165" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>265</v>
       </c>
-      <c r="E156" s="7" t="s">
+      <c r="E166" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>39</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C167" t="s">
         <v>40</v>
       </c>
-      <c r="E157" s="7" t="s">
+      <c r="E167" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F158" s="13">
-        <f>SUM(F2:F153)</f>
-        <v>24266</v>
-      </c>
-      <c r="G158" s="5" t="s">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F168" s="13">
+        <f>SUM(F2:F163)</f>
+        <v>24906</v>
+      </c>
+      <c r="G168" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F159" s="13">
-        <f>SUM(G2:G153)</f>
-        <v>54</v>
-      </c>
-      <c r="G159" s="5" t="s">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F169" s="13">
+        <f>SUM(G2:G163)</f>
+        <v>58</v>
+      </c>
+      <c r="G169" s="5" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3986,7 +4198,7 @@
     <sortCondition ref="C2:C126"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B152" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B162" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
     <hyperlink ref="B34" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
     <hyperlink ref="B73" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
     <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>

</xml_diff>

<commit_message>
add more oryza species
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{88011C5E-FC03-4010-96B4-9DF5C02F9AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7A35059-55F9-4301-9987-CA55E8039937}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{88011C5E-FC03-4010-96B4-9DF5C02F9AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77C94E9A-4487-4CAD-A08A-386424647F49}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1170" yWindow="15" windowWidth="14385" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="401">
   <si>
     <t>Species</t>
   </si>
@@ -1233,6 +1233,12 @@
   </si>
   <si>
     <t>Oryza meridionalis</t>
+  </si>
+  <si>
+    <t>Oryza nivara</t>
+  </si>
+  <si>
+    <t>there might be WGS data, SRA metadata was hard to decipher</t>
   </si>
 </sst>
 </file>
@@ -1627,10 +1633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H175"/>
+  <dimension ref="A1:H176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="F168" sqref="F168"/>
+      <selection activeCell="E169" sqref="E169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4272,26 +4278,27 @@
         <v>259</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>164</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C168" t="s">
-        <v>166</v>
-      </c>
-      <c r="E168" s="7" t="s">
-        <v>163</v>
-      </c>
+    <row r="168" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="D168" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="E168" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="F168" s="17"/>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>168</v>
-      </c>
-      <c r="B169" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C169" t="s">
+        <v>166</v>
       </c>
       <c r="E169" s="7" t="s">
         <v>163</v>
@@ -4299,10 +4306,10 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>244</v>
+        <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>245</v>
+        <v>167</v>
       </c>
       <c r="E170" s="7" t="s">
         <v>163</v>
@@ -4310,7 +4317,10 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>264</v>
+        <v>244</v>
+      </c>
+      <c r="B171" t="s">
+        <v>245</v>
       </c>
       <c r="E171" s="7" t="s">
         <v>163</v>
@@ -4318,7 +4328,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E172" s="7" t="s">
         <v>163</v>
@@ -4326,30 +4336,38 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>39</v>
-      </c>
-      <c r="C173" t="s">
-        <v>40</v>
+        <v>265</v>
       </c>
       <c r="E173" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F174" s="13">
-        <f>SUM(F2:F169)</f>
-        <v>25208</v>
-      </c>
-      <c r="G174" s="5" t="s">
-        <v>213</v>
+      <c r="A174" t="s">
+        <v>39</v>
+      </c>
+      <c r="C174" t="s">
+        <v>40</v>
+      </c>
+      <c r="E174" s="7" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F175" s="13">
-        <f>SUM(G2:G169)</f>
+        <f>SUM(F2:F170)</f>
+        <v>25208</v>
+      </c>
+      <c r="G175" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F176" s="13">
+        <f>SUM(G2:G170)</f>
         <v>63</v>
       </c>
-      <c r="G175" s="5" t="s">
+      <c r="G176" s="5" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4359,7 +4377,7 @@
     <sortCondition ref="C2:C126"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B168" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B169" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
     <hyperlink ref="B34" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
     <hyperlink ref="B73" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
     <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>

</xml_diff>

<commit_message>
add remaining ensembl species
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_9/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{88011C5E-FC03-4010-96B4-9DF5C02F9AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77C94E9A-4487-4CAD-A08A-386424647F49}"/>
+  <xr:revisionPtr revIDLastSave="263" documentId="13_ncr:1_{88011C5E-FC03-4010-96B4-9DF5C02F9AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B5310D7-526B-4DD0-A6C0-B3BE7AB16FC0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="454">
   <si>
     <t>Species</t>
   </si>
@@ -1239,6 +1239,165 @@
   </si>
   <si>
     <t>there might be WGS data, SRA metadata was hard to decipher</t>
+  </si>
+  <si>
+    <t>Oryza punctata</t>
+  </si>
+  <si>
+    <t>PRJDB4620</t>
+  </si>
+  <si>
+    <t>can't find publication, SRA says 8 accessions were sequenced, but I found 10 samples</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/nature11532</t>
+  </si>
+  <si>
+    <t>Oryza rufipogon</t>
+  </si>
+  <si>
+    <t>PRJEB2829</t>
+  </si>
+  <si>
+    <t>Paper claims 446 accessions, but I only found 445</t>
+  </si>
+  <si>
+    <t>Ostreococcus lucimarinus</t>
+  </si>
+  <si>
+    <t>Papaver somniferum</t>
+  </si>
+  <si>
+    <t>Only GBS data, but not WGS data</t>
+  </si>
+  <si>
+    <t>Physcomitrium patens</t>
+  </si>
+  <si>
+    <t>Not sure I want to include moss</t>
+  </si>
+  <si>
+    <t>Pistacia vera</t>
+  </si>
+  <si>
+    <t>Pisum sativum</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41588-019-0480-1</t>
+  </si>
+  <si>
+    <t>Lots more GBS data, but mostly for RILS. I want data from natural populations, not RILs, might be more data in PRJNA509279, again I can't find data for the same number of accessions listed in the paper, also studies rarely give SRA run numbers - only bioproject numbers</t>
+  </si>
+  <si>
+    <t>Prunus avium</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093%2Fhr%2Fuhac233</t>
+  </si>
+  <si>
+    <t>PRJNA813711</t>
+  </si>
+  <si>
+    <t>235+64=299, all accessions in paper accounted for</t>
+  </si>
+  <si>
+    <t>Prunus dulcis</t>
+  </si>
+  <si>
+    <t>PRJNA339570</t>
+  </si>
+  <si>
+    <t>Can't find publication, but this data was used in one preprint</t>
+  </si>
+  <si>
+    <t>PRJNA729978</t>
+  </si>
+  <si>
+    <t>Quercus lobata</t>
+  </si>
+  <si>
+    <t>can't find publication, but data is a part of a genome project, found 160 samples - not 125 like SRA claims</t>
+  </si>
+  <si>
+    <t>Quercus suber</t>
+  </si>
+  <si>
+    <t>Rosa chinensis</t>
+  </si>
+  <si>
+    <t>Saccharum spontaneum</t>
+  </si>
+  <si>
+    <t>WGS for 9 cultivars in 9 different bioprojects, can't find publication</t>
+  </si>
+  <si>
+    <t>Selaginella moellendorffii</t>
+  </si>
+  <si>
+    <t>not sure if I want to include this</t>
+  </si>
+  <si>
+    <t>Sesamum indicum</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/ncomms9609</t>
+  </si>
+  <si>
+    <t>PRJEB8078</t>
+  </si>
+  <si>
+    <t>Publication includes 715 genomes, but some of these are from another species</t>
+  </si>
+  <si>
+    <t>Triticum dicoccoides</t>
+  </si>
+  <si>
+    <t>found exome capture data, and GBS data, but no WGS data</t>
+  </si>
+  <si>
+    <t>Triticum spelta</t>
+  </si>
+  <si>
+    <t>PRJNA918327</t>
+  </si>
+  <si>
+    <t>This has some data, but I can't find the publication</t>
+  </si>
+  <si>
+    <t>Triticum urartu</t>
+  </si>
+  <si>
+    <t>Vigna angularis</t>
+  </si>
+  <si>
+    <t>PRJNA885164</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389%2Ffpls.2022.1043784</t>
+  </si>
+  <si>
+    <t>Vigna radiata</t>
+  </si>
+  <si>
+    <t>PRJNA889224</t>
+  </si>
+  <si>
+    <t>uploaded Oct 2022, so I can't find publication yet…</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1101/2022.08.22.504811</t>
+  </si>
+  <si>
+    <t>This is a preprint that links to several datasets, could be useful</t>
+  </si>
+  <si>
+    <t>SRP077082</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.13404</t>
+  </si>
+  <si>
+    <t>I can probably find more data, but it hasn't been peer-reviewed</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1344,13 +1503,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1633,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H176"/>
+  <dimension ref="A1:H199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="E169" sqref="E169"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3448,6 +3600,9 @@
       <c r="C115" s="3" t="s">
         <v>235</v>
       </c>
+      <c r="D115" s="3" t="s">
+        <v>323</v>
+      </c>
       <c r="E115" s="8" t="s">
         <v>305</v>
       </c>
@@ -4147,23 +4302,22 @@
         <v>259</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="15" t="s">
+    <row r="162" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>383</v>
       </c>
-      <c r="B162" s="15" t="s">
+      <c r="B162" t="s">
         <v>385</v>
       </c>
-      <c r="C162" s="15" t="s">
+      <c r="C162" t="s">
         <v>384</v>
       </c>
-      <c r="D162" s="15" t="s">
+      <c r="D162" t="s">
         <v>323</v>
       </c>
-      <c r="E162" s="16" t="s">
+      <c r="E162" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="F162" s="17"/>
     </row>
     <row r="163" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
@@ -4278,96 +4432,418 @@
         <v>259</v>
       </c>
     </row>
-    <row r="168" spans="1:8" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="15" t="s">
+    <row r="168" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>399</v>
       </c>
-      <c r="D168" s="15" t="s">
+      <c r="D168" t="s">
         <v>323</v>
       </c>
-      <c r="E168" s="16" t="s">
+      <c r="E168" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="F168" s="17"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>164</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C169" t="s">
-        <v>166</v>
-      </c>
-      <c r="E169" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>168</v>
-      </c>
-      <c r="B170" t="s">
-        <v>167</v>
-      </c>
-      <c r="E170" s="7" t="s">
-        <v>163</v>
+    </row>
+    <row r="169" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C169" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="E169" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="F169" s="13">
+        <v>10</v>
+      </c>
+      <c r="G169" s="5">
+        <v>1</v>
+      </c>
+      <c r="H169" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E170" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="F170" s="11">
+        <v>445</v>
+      </c>
+      <c r="G170" s="3">
+        <v>1</v>
+      </c>
+      <c r="H170" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>244</v>
-      </c>
-      <c r="B171" t="s">
-        <v>245</v>
+        <v>408</v>
       </c>
       <c r="E171" s="7" t="s">
-        <v>163</v>
+        <v>357</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>264</v>
+        <v>409</v>
       </c>
       <c r="E172" s="7" t="s">
-        <v>163</v>
+        <v>410</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>265</v>
+        <v>411</v>
       </c>
       <c r="E173" s="7" t="s">
-        <v>163</v>
+        <v>412</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>413</v>
+      </c>
+      <c r="E174" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E175" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="F175" s="11">
+        <v>27</v>
+      </c>
+      <c r="G175" s="3">
+        <v>1</v>
+      </c>
+      <c r="H175" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E176" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="F176" s="11">
+        <v>299</v>
+      </c>
+      <c r="G176" s="3">
+        <v>1</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>421</v>
+      </c>
+      <c r="C177" t="s">
+        <v>422</v>
+      </c>
+      <c r="E177" s="7" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E178" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="F178" s="11">
+        <v>160</v>
+      </c>
+      <c r="G178" s="3">
+        <v>1</v>
+      </c>
+      <c r="H178" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>427</v>
+      </c>
+      <c r="E179" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>428</v>
+      </c>
+      <c r="E180" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>429</v>
+      </c>
+      <c r="E181" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>431</v>
+      </c>
+      <c r="E182" s="7" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="E183" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="F183" s="11">
+        <v>705</v>
+      </c>
+      <c r="G183" s="3">
+        <v>1</v>
+      </c>
+      <c r="H183" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>437</v>
+      </c>
+      <c r="E184" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>439</v>
+      </c>
+      <c r="C185" t="s">
+        <v>440</v>
+      </c>
+      <c r="E185" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>442</v>
+      </c>
+      <c r="E186" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>443</v>
+      </c>
+      <c r="E187" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E188" s="8"/>
+      <c r="F188" s="11">
+        <v>558</v>
+      </c>
+      <c r="G188" s="3">
+        <v>1</v>
+      </c>
+      <c r="H188" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>97</v>
+      </c>
+      <c r="C189" t="s">
+        <v>447</v>
+      </c>
+      <c r="E189" s="7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>97</v>
+      </c>
+      <c r="B190" t="s">
+        <v>449</v>
+      </c>
+      <c r="E190" s="7" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="E191" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="F191" s="11">
+        <v>37</v>
+      </c>
+      <c r="G191" s="3">
+        <v>1</v>
+      </c>
+      <c r="H191" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>164</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C192" t="s">
+        <v>166</v>
+      </c>
+      <c r="E192" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>168</v>
+      </c>
+      <c r="B193" t="s">
+        <v>167</v>
+      </c>
+      <c r="E193" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>244</v>
+      </c>
+      <c r="B194" t="s">
+        <v>245</v>
+      </c>
+      <c r="E194" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>264</v>
+      </c>
+      <c r="E195" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>265</v>
+      </c>
+      <c r="E196" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
         <v>39</v>
       </c>
-      <c r="C174" t="s">
+      <c r="C197" t="s">
         <v>40</v>
       </c>
-      <c r="E174" s="7" t="s">
+      <c r="E197" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F175" s="13">
-        <f>SUM(F2:F170)</f>
-        <v>25208</v>
-      </c>
-      <c r="G175" s="5" t="s">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F198" s="13">
+        <f>SUM(F2:F193)</f>
+        <v>27449</v>
+      </c>
+      <c r="G198" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F176" s="13">
-        <f>SUM(G2:G170)</f>
-        <v>63</v>
-      </c>
-      <c r="G176" s="5" t="s">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F199" s="13">
+        <f>SUM(G2:G193)</f>
+        <v>71</v>
+      </c>
+      <c r="G199" s="5" t="s">
         <v>239</v>
       </c>
     </row>
@@ -4377,7 +4853,7 @@
     <sortCondition ref="C2:C126"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B169" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B192" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
     <hyperlink ref="B34" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
     <hyperlink ref="B73" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
     <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>

</xml_diff>

<commit_message>
increase mem for downloads
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/263534_2_11/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198194_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="13_ncr:1_{88011C5E-FC03-4010-96B4-9DF5C02F9AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B5310D7-526B-4DD0-A6C0-B3BE7AB16FC0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207FC0D1-FC45-47DB-B61C-3A29A9DF7698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="459">
   <si>
     <t>Species</t>
   </si>
@@ -1398,6 +1398,21 @@
   </si>
   <si>
     <t>I can probably find more data, but it hasn't been peer-reviewed</t>
+  </si>
+  <si>
+    <t>Phytozome</t>
+  </si>
+  <si>
+    <t>Generation time</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>a few years</t>
+  </si>
+  <si>
+    <t>2 years</t>
   </si>
 </sst>
 </file>
@@ -1785,23 +1800,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H199"/>
+  <dimension ref="A1:I199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E190" sqref="E190"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
-    <col min="3" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="42.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="3" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1814,20 +1829,23 @@
       <c r="D1" t="s">
         <v>322</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" t="s">
+        <v>455</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>257</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -1837,29 +1855,35 @@
       <c r="C2" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="11">
+      <c r="D2" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="11">
         <v>48</v>
       </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>136</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>119</v>
       </c>
@@ -1869,29 +1893,35 @@
       <c r="C4" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="11">
+      <c r="D4" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="11">
         <v>87</v>
       </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="3">
+        <v>1</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>136</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1901,36 +1931,48 @@
       <c r="C6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="11">
+      <c r="D6" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="11">
         <v>56</v>
       </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="11">
+      <c r="D7" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="11">
         <v>142</v>
       </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1940,11 +1982,11 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1954,73 +1996,79 @@
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="11">
+      <c r="D9" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="11">
         <v>1135</v>
       </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
       <c r="C10" t="s">
         <v>143</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
       <c r="C11" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
       <c r="C12" t="s">
         <v>144</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>82</v>
       </c>
       <c r="C13" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>120</v>
       </c>
       <c r="C14" t="s">
         <v>147</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
@@ -2030,31 +2078,34 @@
       <c r="C15" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="D15" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="F15" s="11">
+      <c r="G15" s="11">
         <v>597</v>
       </c>
-      <c r="G15" s="3">
-        <v>1</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>83</v>
       </c>
       <c r="C16" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>105</v>
       </c>
@@ -2064,21 +2115,24 @@
       <c r="C17" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="F17" s="11">
+      <c r="G17" s="11">
         <v>467</v>
       </c>
-      <c r="G17" s="3">
-        <v>1</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -2088,11 +2142,11 @@
       <c r="C18" t="s">
         <v>150</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>128</v>
       </c>
@@ -2102,20 +2156,23 @@
       <c r="C19" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="D19" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="F19" s="11">
+      <c r="G19" s="11">
         <v>56</v>
       </c>
-      <c r="G19" s="3">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>128</v>
       </c>
@@ -2125,33 +2182,33 @@
       <c r="C20" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>126</v>
       </c>
       <c r="B21" t="s">
         <v>153</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>127</v>
       </c>
       <c r="C22" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -2162,7 +2219,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>108</v>
       </c>
@@ -2172,20 +2229,23 @@
       <c r="C24" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F24" s="11">
+      <c r="G24" s="11">
         <v>119</v>
       </c>
-      <c r="G24" s="3">
-        <v>1</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="3">
+        <v>1</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>109</v>
       </c>
@@ -2195,31 +2255,34 @@
       <c r="C25" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="D25" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F25" s="11">
+      <c r="G25" s="11">
         <v>199</v>
       </c>
-      <c r="G25" s="3">
-        <v>1</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="3">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>109</v>
       </c>
       <c r="C26" t="s">
         <v>156</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>59</v>
       </c>
@@ -2229,20 +2292,23 @@
       <c r="C27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F27" s="11">
+      <c r="G27" s="11">
         <v>40</v>
       </c>
-      <c r="G27" s="3">
-        <v>1</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="3">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -2250,18 +2316,18 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>60</v>
       </c>
       <c r="C29" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>50</v>
       </c>
@@ -2271,42 +2337,45 @@
       <c r="C30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="D30" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="F30" s="11">
+      <c r="G30" s="11">
         <v>52</v>
       </c>
-      <c r="G30" s="3">
-        <v>1</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="3">
+        <v>1</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>103</v>
       </c>
       <c r="C31" t="s">
         <v>136</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>96</v>
       </c>
       <c r="C32" t="s">
         <v>136</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>73</v>
       </c>
@@ -2316,20 +2385,23 @@
       <c r="C33" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="D33" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="F33" s="11">
+      <c r="G33" s="11">
         <v>296</v>
       </c>
-      <c r="G33" s="3">
-        <v>1</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
@@ -2339,31 +2411,34 @@
       <c r="C34" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="D34" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="F34" s="11">
+      <c r="G34" s="11">
         <v>3171</v>
       </c>
-      <c r="G34" s="3">
-        <v>1</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>68</v>
       </c>
       <c r="C35" t="s">
         <v>136</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>48</v>
       </c>
@@ -2373,53 +2448,53 @@
       <c r="C36" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="F36" s="11">
+      <c r="G36" s="11">
         <v>337</v>
       </c>
-      <c r="G36" s="3">
-        <v>1</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H36" s="3">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>116</v>
       </c>
       <c r="C37" t="s">
         <v>136</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>117</v>
       </c>
       <c r="C38" t="s">
         <v>136</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>98</v>
       </c>
       <c r="C39" t="s">
         <v>136</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>85</v>
       </c>
@@ -2429,20 +2504,20 @@
       <c r="C40" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F40" s="11">
+      <c r="G40" s="11">
         <v>115</v>
       </c>
-      <c r="G40" s="3">
-        <v>1</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -2452,11 +2527,11 @@
       <c r="C41" t="s">
         <v>177</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -2466,22 +2541,22 @@
       <c r="C42" t="s">
         <v>175</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>76</v>
       </c>
       <c r="C43" t="s">
         <v>136</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>121</v>
       </c>
@@ -2491,66 +2566,66 @@
       <c r="C44" t="s">
         <v>180</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>29</v>
       </c>
       <c r="C45" t="s">
         <v>136</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>81</v>
       </c>
       <c r="C46" t="s">
         <v>136</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="F46" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
       <c r="C47" t="s">
         <v>136</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
       <c r="C48" t="s">
         <v>136</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="F48" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>87</v>
       </c>
       <c r="C49" t="s">
         <v>136</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>45</v>
       </c>
@@ -2560,20 +2635,20 @@
       <c r="C50" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="F50" s="8" t="s">
         <v>293</v>
       </c>
-      <c r="F50" s="11">
+      <c r="G50" s="11">
         <v>1674</v>
       </c>
-      <c r="G50" s="3">
-        <v>1</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H50" s="3">
+        <v>1</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>45</v>
       </c>
@@ -2583,14 +2658,14 @@
       <c r="C51" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="F51" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="F51" s="11">
+      <c r="G51" s="11">
         <v>240</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>45</v>
       </c>
@@ -2600,14 +2675,14 @@
       <c r="C52" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="F52" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="F52" s="11">
+      <c r="G52" s="11">
         <v>279</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -2617,11 +2692,11 @@
       <c r="C53" t="s">
         <v>47</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="F53" s="7" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>88</v>
       </c>
@@ -2631,19 +2706,24 @@
       <c r="C54" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="D54" s="9"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="11">
+      <c r="D54" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="F54" s="8"/>
+      <c r="G54" s="11">
         <v>185</v>
       </c>
-      <c r="G54" s="3">
-        <v>1</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>110</v>
       </c>
@@ -2653,29 +2733,29 @@
       <c r="C55" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E55" s="8"/>
-      <c r="F55" s="11">
+      <c r="F55" s="8"/>
+      <c r="G55" s="11">
         <v>336</v>
       </c>
-      <c r="G55" s="3">
-        <v>1</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H55" s="3">
+        <v>1</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>111</v>
       </c>
       <c r="C56" t="s">
         <v>136</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="F56" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>112</v>
       </c>
@@ -2685,18 +2765,18 @@
       <c r="C57" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="E57" s="8"/>
-      <c r="F57" s="11">
+      <c r="F57" s="8"/>
+      <c r="G57" s="11">
         <v>1081</v>
       </c>
-      <c r="G57" s="3">
-        <v>1</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H57" s="3">
+        <v>1</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -2704,44 +2784,45 @@
         <v>134</v>
       </c>
       <c r="D58" s="2"/>
-      <c r="E58" s="7" t="s">
+      <c r="E58" s="2"/>
+      <c r="F58" s="7" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>113</v>
       </c>
       <c r="C59" t="s">
         <v>136</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="F59" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>114</v>
       </c>
       <c r="C60" t="s">
         <v>136</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="F60" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>115</v>
       </c>
       <c r="C61" t="s">
         <v>136</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="F61" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>25</v>
       </c>
@@ -2751,11 +2832,11 @@
       <c r="C62" t="s">
         <v>37</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="F62" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>24</v>
       </c>
@@ -2765,29 +2846,29 @@
       <c r="C63" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E63" s="8"/>
-      <c r="F63" s="11">
+      <c r="F63" s="8"/>
+      <c r="G63" s="11">
         <v>300</v>
       </c>
-      <c r="G63" s="3">
-        <v>1</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H63" s="3">
+        <v>1</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>74</v>
       </c>
       <c r="C64" t="s">
         <v>136</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="F64" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>77</v>
       </c>
@@ -2797,20 +2878,20 @@
       <c r="C65" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="F65" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="F65" s="11">
+      <c r="G65" s="11">
         <v>131</v>
       </c>
-      <c r="G65" s="3">
-        <v>1</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="3">
+        <v>1</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>89</v>
       </c>
@@ -2820,11 +2901,11 @@
       <c r="C66" t="s">
         <v>191</v>
       </c>
-      <c r="E66" s="7" t="s">
+      <c r="F66" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -2834,11 +2915,11 @@
       <c r="C67" t="s">
         <v>194</v>
       </c>
-      <c r="E67" s="7" t="s">
+      <c r="F67" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>99</v>
       </c>
@@ -2848,20 +2929,20 @@
       <c r="C68" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="F68" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="F68" s="11">
+      <c r="G68" s="11">
         <v>200</v>
       </c>
-      <c r="G68" s="3">
-        <v>1</v>
-      </c>
-      <c r="H68" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H68" s="3">
+        <v>1</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>99</v>
       </c>
@@ -2871,22 +2952,22 @@
       <c r="C69" t="s">
         <v>196</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="F69" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>28</v>
       </c>
       <c r="C70" t="s">
         <v>136</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="F70" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>91</v>
       </c>
@@ -2896,31 +2977,31 @@
       <c r="C71" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="F71" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="F71" s="11">
+      <c r="G71" s="11">
         <v>136</v>
       </c>
-      <c r="G71" s="3">
-        <v>1</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H71" s="3">
+        <v>1</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>92</v>
       </c>
       <c r="C72" t="s">
         <v>136</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="F72" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>100</v>
       </c>
@@ -2930,31 +3011,31 @@
       <c r="C73" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="F73" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="F73" s="11">
+      <c r="G73" s="11">
         <v>44</v>
       </c>
-      <c r="G73" s="3">
-        <v>1</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H73" s="3">
+        <v>1</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>100</v>
       </c>
       <c r="C74" t="s">
         <v>200</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="F74" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>67</v>
       </c>
@@ -2964,20 +3045,20 @@
       <c r="C75" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="F75" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F75" s="3">
+      <c r="G75" s="3">
         <v>39</v>
       </c>
-      <c r="G75" s="3">
-        <v>1</v>
-      </c>
-      <c r="H75" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H75" s="3">
+        <v>1</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -2987,11 +3068,11 @@
       <c r="C76" t="s">
         <v>252</v>
       </c>
-      <c r="E76" s="7" t="s">
+      <c r="F76" s="7" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>67</v>
       </c>
@@ -3001,11 +3082,11 @@
       <c r="C77" t="s">
         <v>195</v>
       </c>
-      <c r="E77" s="7" t="s">
+      <c r="F77" s="7" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>19</v>
       </c>
@@ -3015,53 +3096,53 @@
       <c r="C78" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="E78" s="8" t="s">
+      <c r="F78" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="F78" s="11">
+      <c r="G78" s="11">
         <v>38</v>
       </c>
-      <c r="G78" s="3">
-        <v>1</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H78" s="3">
+        <v>1</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>129</v>
       </c>
       <c r="C79" t="s">
         <v>136</v>
       </c>
-      <c r="E79" s="7" t="s">
+      <c r="F79" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>122</v>
       </c>
       <c r="C80" t="s">
         <v>136</v>
       </c>
-      <c r="E80" s="7" t="s">
+      <c r="F80" s="7" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>69</v>
       </c>
       <c r="C81" t="s">
         <v>136</v>
       </c>
-      <c r="E81" s="7" t="s">
+      <c r="F81" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>78</v>
       </c>
@@ -3071,20 +3152,20 @@
       <c r="C82" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E82" s="8" t="s">
+      <c r="F82" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="F82" s="11">
+      <c r="G82" s="11">
         <v>52</v>
       </c>
-      <c r="G82" s="3">
-        <v>1</v>
-      </c>
-      <c r="H82" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H82" s="3">
+        <v>1</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>78</v>
       </c>
@@ -3095,7 +3176,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>125</v>
       </c>
@@ -3105,11 +3186,11 @@
       <c r="C84" t="s">
         <v>136</v>
       </c>
-      <c r="E84" s="7" t="s">
+      <c r="F84" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
@@ -3119,20 +3200,20 @@
       <c r="C85" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E85" s="8" t="s">
+      <c r="F85" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="F85" s="12">
+      <c r="G85" s="12">
         <v>3024</v>
       </c>
-      <c r="G85" s="3">
-        <v>1</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="H85" s="3">
+        <v>1</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>133</v>
       </c>
@@ -3142,20 +3223,20 @@
       <c r="C86" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E86" s="8" t="s">
+      <c r="F86" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="F86" s="11">
+      <c r="G86" s="11">
         <v>85</v>
       </c>
-      <c r="G86" s="3">
-        <v>1</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H86" s="3">
+        <v>1</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>130</v>
       </c>
@@ -3165,31 +3246,31 @@
       <c r="C87" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="F87" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="F87" s="11">
+      <c r="G87" s="11">
         <v>747</v>
       </c>
-      <c r="G87" s="3">
-        <v>1</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="3">
+        <v>1</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>93</v>
       </c>
       <c r="C88" t="s">
         <v>136</v>
       </c>
-      <c r="E88" s="7" t="s">
+      <c r="F88" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>49</v>
       </c>
@@ -3199,29 +3280,29 @@
       <c r="C89" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E89" s="8"/>
-      <c r="F89" s="11">
+      <c r="F89" s="8"/>
+      <c r="G89" s="11">
         <v>683</v>
       </c>
-      <c r="G89" s="3">
-        <v>1</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="3">
+        <v>1</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>118</v>
       </c>
       <c r="C90" t="s">
         <v>136</v>
       </c>
-      <c r="E90" s="7" t="s">
+      <c r="F90" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="91" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>51</v>
       </c>
@@ -3231,20 +3312,20 @@
       <c r="C91" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="F91" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="F91" s="11">
+      <c r="G91" s="11">
         <v>52</v>
       </c>
-      <c r="G91" s="3">
-        <v>1</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="3">
+        <v>1</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>51</v>
       </c>
@@ -3255,7 +3336,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>51</v>
       </c>
@@ -3266,7 +3347,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>51</v>
       </c>
@@ -3274,7 +3355,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>51</v>
       </c>
@@ -3282,7 +3363,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="96" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>94</v>
       </c>
@@ -3292,53 +3373,53 @@
       <c r="C96" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E96" s="8" t="s">
+      <c r="F96" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="F96" s="11">
+      <c r="G96" s="11">
         <v>428</v>
       </c>
-      <c r="G96" s="3">
-        <v>1</v>
-      </c>
-      <c r="H96" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H96" s="3">
+        <v>1</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>101</v>
       </c>
       <c r="C97" t="s">
         <v>136</v>
       </c>
-      <c r="E97" s="7" t="s">
+      <c r="F97" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>102</v>
       </c>
       <c r="C98" t="s">
         <v>136</v>
       </c>
-      <c r="E98" s="7" t="s">
+      <c r="F98" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>107</v>
       </c>
       <c r="C99" t="s">
         <v>136</v>
       </c>
-      <c r="E99" s="7" t="s">
+      <c r="F99" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>131</v>
       </c>
@@ -3348,20 +3429,20 @@
       <c r="C100" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="E100" s="8" t="s">
+      <c r="F100" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="F100" s="11">
+      <c r="G100" s="11">
         <v>909</v>
       </c>
-      <c r="G100" s="3">
-        <v>1</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H100" s="3">
+        <v>1</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>132</v>
       </c>
@@ -3371,20 +3452,20 @@
       <c r="C101" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="F101" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="F101" s="11">
+      <c r="G101" s="11">
         <v>38</v>
       </c>
-      <c r="G101" s="3">
-        <v>1</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H101" s="3">
+        <v>1</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>18</v>
       </c>
@@ -3392,18 +3473,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>18</v>
       </c>
       <c r="C103" t="s">
         <v>218</v>
       </c>
-      <c r="E103" s="7" t="s">
+      <c r="F103" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="104" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>18</v>
       </c>
@@ -3413,31 +3494,31 @@
       <c r="C104" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E104" s="8" t="s">
+      <c r="F104" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F104" s="11">
+      <c r="G104" s="11">
         <v>360</v>
       </c>
-      <c r="G104" s="3">
-        <v>1</v>
-      </c>
-      <c r="H104" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H104" s="3">
+        <v>1</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>79</v>
       </c>
       <c r="C105" t="s">
         <v>222</v>
       </c>
-      <c r="E105" s="7" t="s">
+      <c r="F105" s="7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>31</v>
       </c>
@@ -3447,11 +3528,11 @@
       <c r="C106" t="s">
         <v>33</v>
       </c>
-      <c r="E106" s="7" t="s">
+      <c r="F106" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>31</v>
       </c>
@@ -3461,11 +3542,11 @@
       <c r="C107" t="s">
         <v>224</v>
       </c>
-      <c r="E107" s="7" t="s">
+      <c r="F107" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>31</v>
       </c>
@@ -3475,20 +3556,20 @@
       <c r="C108" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E108" s="8" t="s">
+      <c r="F108" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="F108" s="11">
+      <c r="G108" s="11">
         <v>400</v>
       </c>
-      <c r="G108" s="3">
-        <v>1</v>
-      </c>
-      <c r="H108" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H108" s="3">
+        <v>1</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>75</v>
       </c>
@@ -3498,20 +3579,20 @@
       <c r="C109" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="E109" s="8" t="s">
+      <c r="F109" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="F109" s="11">
+      <c r="G109" s="11">
         <v>296</v>
       </c>
-      <c r="G109" s="3">
-        <v>1</v>
-      </c>
-      <c r="H109" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H109" s="3">
+        <v>1</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>123</v>
       </c>
@@ -3521,31 +3602,31 @@
       <c r="C110" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="E110" s="8" t="s">
+      <c r="F110" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="F110" s="11">
+      <c r="G110" s="11">
         <v>36</v>
       </c>
-      <c r="G110" s="3">
-        <v>1</v>
-      </c>
-      <c r="H110" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H110" s="3">
+        <v>1</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>104</v>
       </c>
       <c r="C111" t="s">
         <v>136</v>
       </c>
-      <c r="E111" s="7" t="s">
+      <c r="F111" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>27</v>
       </c>
@@ -3555,19 +3636,19 @@
       <c r="C112" t="s">
         <v>65</v>
       </c>
-      <c r="E112" s="7" t="s">
+      <c r="F112" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>95</v>
       </c>
-      <c r="E113" s="7" t="s">
+      <c r="F113" s="7" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="114" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>23</v>
       </c>
@@ -3577,20 +3658,20 @@
       <c r="C114" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E114" s="8" t="s">
+      <c r="F114" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="F114" s="11">
+      <c r="G114" s="11">
         <v>786</v>
       </c>
-      <c r="G114" s="3">
-        <v>1</v>
-      </c>
-      <c r="H114" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H114" s="3">
+        <v>1</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>32</v>
       </c>
@@ -3603,42 +3684,42 @@
       <c r="D115" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E115" s="8" t="s">
+      <c r="F115" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="F115" s="11">
+      <c r="G115" s="11">
         <v>114</v>
       </c>
-      <c r="G115" s="3">
-        <v>1</v>
-      </c>
-      <c r="H115" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H115" s="3">
+        <v>1</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>80</v>
       </c>
       <c r="C116" t="s">
         <v>136</v>
       </c>
-      <c r="E116" s="7" t="s">
+      <c r="F116" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>97</v>
       </c>
       <c r="C117" t="s">
         <v>136</v>
       </c>
-      <c r="E117" s="7" t="s">
+      <c r="F117" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>10</v>
       </c>
@@ -3646,7 +3727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>10</v>
       </c>
@@ -3656,20 +3737,20 @@
       <c r="C119" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E119" s="8" t="s">
+      <c r="F119" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F119" s="11">
+      <c r="G119" s="11">
         <v>117</v>
       </c>
-      <c r="G119" s="3">
-        <v>1</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H119" s="3">
+        <v>1</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>10</v>
       </c>
@@ -3677,7 +3758,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -3685,7 +3766,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>9</v>
       </c>
@@ -3695,67 +3776,67 @@
       <c r="C122" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E122" s="8" t="s">
+      <c r="F122" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="F122" s="11">
+      <c r="G122" s="11">
         <v>33</v>
       </c>
-      <c r="G122" s="3">
-        <v>1</v>
-      </c>
-      <c r="H122" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H122" s="3">
+        <v>1</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E123" s="8" t="s">
+      <c r="F123" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="F123" s="11"/>
-    </row>
-    <row r="124" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G123" s="11"/>
+    </row>
+    <row r="124" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E124" s="8"/>
-      <c r="F124" s="11">
+      <c r="F124" s="8"/>
+      <c r="G124" s="11">
         <v>277</v>
       </c>
     </row>
-    <row r="125" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E125" s="8"/>
-      <c r="F125" s="11">
+      <c r="F125" s="8"/>
+      <c r="G125" s="11">
         <v>599</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
       <c r="C126" t="s">
         <v>237</v>
       </c>
-      <c r="E126" s="7" t="s">
+      <c r="F126" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="127" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>160</v>
       </c>
@@ -3768,18 +3849,18 @@
       <c r="D127" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E127" s="8"/>
-      <c r="F127" s="11">
+      <c r="F127" s="8"/>
+      <c r="G127" s="11">
         <v>306</v>
       </c>
-      <c r="G127" s="3">
-        <v>1</v>
-      </c>
-      <c r="H127" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H127" s="3">
+        <v>1</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>160</v>
       </c>
@@ -3789,19 +3870,19 @@
       <c r="C128" t="s">
         <v>161</v>
       </c>
-      <c r="E128" s="7" t="s">
+      <c r="F128" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>312</v>
       </c>
-      <c r="E129" s="7" t="s">
+      <c r="F129" s="7" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="130" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>315</v>
       </c>
@@ -3814,18 +3895,18 @@
       <c r="D130" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E130" s="8"/>
-      <c r="F130" s="11">
+      <c r="F130" s="8"/>
+      <c r="G130" s="11">
         <v>306</v>
       </c>
-      <c r="G130" s="3">
-        <v>1</v>
-      </c>
-      <c r="H130" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="131" spans="1:8" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H130" s="3">
+        <v>1</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>318</v>
       </c>
@@ -3838,18 +3919,18 @@
       <c r="D131" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E131" s="8"/>
-      <c r="F131" s="11">
+      <c r="F131" s="8"/>
+      <c r="G131" s="11">
         <v>479</v>
       </c>
-      <c r="G131" s="3">
-        <v>1</v>
-      </c>
-      <c r="H131" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H131" s="3">
+        <v>1</v>
+      </c>
+      <c r="I131" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>319</v>
       </c>
@@ -3862,18 +3943,18 @@
       <c r="D132" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E132" s="8"/>
-      <c r="F132" s="11">
+      <c r="F132" s="8"/>
+      <c r="G132" s="11">
         <v>1007</v>
       </c>
-      <c r="G132" s="3">
-        <v>1</v>
-      </c>
-      <c r="H132" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H132" s="3">
+        <v>1</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>313</v>
       </c>
@@ -3886,31 +3967,31 @@
       <c r="D133" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E133" s="8" t="s">
+      <c r="F133" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="F133" s="11">
+      <c r="G133" s="11">
         <v>10</v>
       </c>
-      <c r="G133" s="3">
-        <v>1</v>
-      </c>
-      <c r="H133" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H133" s="3">
+        <v>1</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>329</v>
       </c>
       <c r="D134" t="s">
         <v>323</v>
       </c>
-      <c r="E134" s="7" t="s">
+      <c r="F134" s="7" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="135" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>331</v>
       </c>
@@ -3923,20 +4004,20 @@
       <c r="D135" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E135" s="8" t="s">
+      <c r="F135" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="F135" s="11">
+      <c r="G135" s="11">
         <v>135</v>
       </c>
-      <c r="G135" s="3">
-        <v>1</v>
-      </c>
-      <c r="H135" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="136" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H135" s="3">
+        <v>1</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>335</v>
       </c>
@@ -3949,47 +4030,47 @@
       <c r="D136" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E136" s="8" t="s">
+      <c r="F136" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="F136" s="11">
+      <c r="G136" s="11">
         <v>7</v>
       </c>
-      <c r="G136" s="3">
-        <v>1</v>
-      </c>
-      <c r="H136" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H136" s="3">
+        <v>1</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>339</v>
       </c>
       <c r="D137" t="s">
         <v>323</v>
       </c>
-      <c r="E137" s="7" t="s">
+      <c r="F137" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>340</v>
       </c>
-      <c r="E138" s="7" t="s">
+      <c r="F138" s="7" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>342</v>
       </c>
-      <c r="E139" s="7" t="s">
+      <c r="F139" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>346</v>
       </c>
@@ -4002,44 +4083,44 @@
       <c r="D140" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E140" s="8" t="s">
+      <c r="F140" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="F140" s="11">
+      <c r="G140" s="11">
         <v>34</v>
       </c>
-      <c r="G140" s="3">
-        <v>1</v>
-      </c>
-      <c r="H140" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H140" s="3">
+        <v>1</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>349</v>
       </c>
-      <c r="E141" s="7" t="s">
+      <c r="F141" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>350</v>
       </c>
-      <c r="E142" s="7" t="s">
+      <c r="F142" s="7" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>98</v>
       </c>
-      <c r="E143" s="7" t="s">
+      <c r="F143" s="7" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="144" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>353</v>
       </c>
@@ -4052,40 +4133,40 @@
       <c r="D144" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E144" s="8"/>
-      <c r="F144" s="11">
+      <c r="F144" s="8"/>
+      <c r="G144" s="11">
         <v>1175</v>
       </c>
-      <c r="G144" s="3">
-        <v>1</v>
-      </c>
-      <c r="H144" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H144" s="3">
+        <v>1</v>
+      </c>
+      <c r="I144" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>356</v>
       </c>
       <c r="D145" t="s">
         <v>323</v>
       </c>
-      <c r="E145" s="7" t="s">
+      <c r="F145" s="7" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>358</v>
       </c>
       <c r="D146" t="s">
         <v>323</v>
       </c>
-      <c r="E146" s="7" t="s">
+      <c r="F146" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="147" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>361</v>
       </c>
@@ -4098,62 +4179,62 @@
       <c r="D147" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E147" s="8"/>
-      <c r="F147" s="11">
+      <c r="F147" s="8"/>
+      <c r="G147" s="11">
         <v>171</v>
       </c>
-      <c r="G147" s="3">
-        <v>1</v>
-      </c>
-      <c r="H147" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H147" s="3">
+        <v>1</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>362</v>
       </c>
       <c r="D148" t="s">
         <v>323</v>
       </c>
-      <c r="E148" s="7" t="s">
+      <c r="F148" s="7" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>364</v>
       </c>
       <c r="D149" t="s">
         <v>323</v>
       </c>
-      <c r="E149" s="7" t="s">
+      <c r="F149" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>365</v>
       </c>
       <c r="D150" t="s">
         <v>323</v>
       </c>
-      <c r="E150" s="7" t="s">
+      <c r="F150" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>366</v>
       </c>
       <c r="D151" t="s">
         <v>323</v>
       </c>
-      <c r="E151" s="7" t="s">
+      <c r="F151" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="152" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>368</v>
       </c>
@@ -4163,36 +4244,36 @@
       <c r="D152" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E152" s="8" t="s">
+      <c r="F152" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="F152" s="11">
+      <c r="G152" s="11">
         <v>14</v>
       </c>
-      <c r="G152" s="3">
-        <v>1</v>
-      </c>
-      <c r="H152" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H152" s="3">
+        <v>1</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>370</v>
       </c>
-      <c r="E153" s="7" t="s">
+      <c r="F153" s="7" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>371</v>
       </c>
-      <c r="E154" s="7" t="s">
+      <c r="F154" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="155" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>373</v>
       </c>
@@ -4205,40 +4286,40 @@
       <c r="D155" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E155" s="8"/>
-      <c r="F155" s="11">
+      <c r="F155" s="8"/>
+      <c r="G155" s="11">
         <v>550</v>
       </c>
-      <c r="G155" s="3">
-        <v>1</v>
-      </c>
-      <c r="H155" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H155" s="3">
+        <v>1</v>
+      </c>
+      <c r="I155" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>376</v>
       </c>
       <c r="D156" t="s">
         <v>323</v>
       </c>
-      <c r="E156" s="7" t="s">
+      <c r="F156" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>377</v>
       </c>
       <c r="D157" t="s">
         <v>323</v>
       </c>
-      <c r="E157" s="7" t="s">
+      <c r="F157" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="158" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>378</v>
       </c>
@@ -4251,34 +4332,34 @@
       <c r="D158" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E158" s="8"/>
-      <c r="F158" s="11">
+      <c r="F158" s="8"/>
+      <c r="G158" s="11">
         <v>55</v>
       </c>
-      <c r="G158" s="3">
-        <v>1</v>
-      </c>
-      <c r="H158" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H158" s="3">
+        <v>1</v>
+      </c>
+      <c r="I158" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>381</v>
       </c>
-      <c r="E159" s="7" t="s">
+      <c r="F159" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>382</v>
       </c>
-      <c r="E160" s="7" t="s">
+      <c r="F160" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="161" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>383</v>
       </c>
@@ -4291,18 +4372,18 @@
       <c r="D161" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E161" s="8"/>
-      <c r="F161" s="11">
+      <c r="F161" s="8"/>
+      <c r="G161" s="11">
         <v>86</v>
       </c>
-      <c r="G161" s="3">
-        <v>1</v>
-      </c>
-      <c r="H161" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H161" s="3">
+        <v>1</v>
+      </c>
+      <c r="I161" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>383</v>
       </c>
@@ -4315,11 +4396,11 @@
       <c r="D162" t="s">
         <v>323</v>
       </c>
-      <c r="E162" s="7" t="s">
+      <c r="F162" s="7" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="163" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>387</v>
       </c>
@@ -4329,20 +4410,20 @@
       <c r="D163" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="E163" s="14" t="s">
+      <c r="F163" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="F163" s="13">
+      <c r="G163" s="13">
         <v>16</v>
       </c>
-      <c r="G163" s="5">
-        <v>1</v>
-      </c>
-      <c r="H163" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H163" s="5">
+        <v>1</v>
+      </c>
+      <c r="I163" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>390</v>
       </c>
@@ -4352,18 +4433,18 @@
       <c r="C164" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="E164" s="8"/>
-      <c r="F164" s="11">
+      <c r="F164" s="8"/>
+      <c r="G164" s="11">
         <v>163</v>
       </c>
-      <c r="G164" s="3">
-        <v>1</v>
-      </c>
-      <c r="H164" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H164" s="3">
+        <v>1</v>
+      </c>
+      <c r="I164" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>394</v>
       </c>
@@ -4373,20 +4454,20 @@
       <c r="D165" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="E165" s="14" t="s">
+      <c r="F165" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="F165" s="13">
+      <c r="G165" s="13">
         <v>21</v>
       </c>
-      <c r="G165" s="5">
-        <v>1</v>
-      </c>
-      <c r="H165" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H165" s="5">
+        <v>1</v>
+      </c>
+      <c r="I165" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>395</v>
       </c>
@@ -4396,20 +4477,20 @@
       <c r="D166" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="E166" s="14" t="s">
+      <c r="F166" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="F166" s="13">
+      <c r="G166" s="13">
         <v>18</v>
       </c>
-      <c r="G166" s="5">
-        <v>1</v>
-      </c>
-      <c r="H166" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H166" s="5">
+        <v>1</v>
+      </c>
+      <c r="I166" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>398</v>
       </c>
@@ -4419,31 +4500,31 @@
       <c r="D167" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="E167" s="14" t="s">
+      <c r="F167" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="F167" s="13">
+      <c r="G167" s="13">
         <v>19</v>
       </c>
-      <c r="G167" s="5">
-        <v>1</v>
-      </c>
-      <c r="H167" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H167" s="5">
+        <v>1</v>
+      </c>
+      <c r="I167" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>399</v>
       </c>
       <c r="D168" t="s">
         <v>323</v>
       </c>
-      <c r="E168" s="7" t="s">
+      <c r="F168" s="7" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="169" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>401</v>
       </c>
@@ -4453,20 +4534,20 @@
       <c r="D169" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="E169" s="14" t="s">
+      <c r="F169" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="F169" s="13">
+      <c r="G169" s="13">
         <v>10</v>
       </c>
-      <c r="G169" s="5">
-        <v>1</v>
-      </c>
-      <c r="H169" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H169" s="5">
+        <v>1</v>
+      </c>
+      <c r="I169" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
         <v>405</v>
       </c>
@@ -4479,52 +4560,52 @@
       <c r="D170" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E170" s="8" t="s">
+      <c r="F170" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="F170" s="11">
+      <c r="G170" s="11">
         <v>445</v>
       </c>
-      <c r="G170" s="3">
-        <v>1</v>
-      </c>
-      <c r="H170" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H170" s="3">
+        <v>1</v>
+      </c>
+      <c r="I170" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>408</v>
       </c>
-      <c r="E171" s="7" t="s">
+      <c r="F171" s="7" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>409</v>
       </c>
-      <c r="E172" s="7" t="s">
+      <c r="F172" s="7" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>411</v>
       </c>
-      <c r="E173" s="7" t="s">
+      <c r="F173" s="7" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>413</v>
       </c>
-      <c r="E174" s="7" t="s">
+      <c r="F174" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="175" spans="1:8" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
         <v>414</v>
       </c>
@@ -4534,20 +4615,20 @@
       <c r="D175" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E175" s="8" t="s">
+      <c r="F175" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="F175" s="11">
+      <c r="G175" s="11">
         <v>27</v>
       </c>
-      <c r="G175" s="3">
-        <v>1</v>
-      </c>
-      <c r="H175" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="H175" s="3">
+        <v>1</v>
+      </c>
+      <c r="I175" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>417</v>
       </c>
@@ -4560,31 +4641,31 @@
       <c r="D176" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E176" s="8" t="s">
+      <c r="F176" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="F176" s="11">
+      <c r="G176" s="11">
         <v>299</v>
       </c>
-      <c r="G176" s="3">
-        <v>1</v>
-      </c>
-      <c r="H176" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="177" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H176" s="3">
+        <v>1</v>
+      </c>
+      <c r="I176" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>421</v>
       </c>
       <c r="C177" t="s">
         <v>422</v>
       </c>
-      <c r="E177" s="7" t="s">
+      <c r="F177" s="7" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="178" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
         <v>425</v>
       </c>
@@ -4594,52 +4675,52 @@
       <c r="D178" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E178" s="8" t="s">
+      <c r="F178" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="F178" s="11">
+      <c r="G178" s="11">
         <v>160</v>
       </c>
-      <c r="G178" s="3">
-        <v>1</v>
-      </c>
-      <c r="H178" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H178" s="3">
+        <v>1</v>
+      </c>
+      <c r="I178" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>427</v>
       </c>
-      <c r="E179" s="7" t="s">
+      <c r="F179" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>428</v>
       </c>
-      <c r="E180" s="7" t="s">
+      <c r="F180" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>429</v>
       </c>
-      <c r="E181" s="7" t="s">
+      <c r="F181" s="7" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>431</v>
       </c>
-      <c r="E182" s="7" t="s">
+      <c r="F182" s="7" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="183" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
         <v>433</v>
       </c>
@@ -4652,55 +4733,55 @@
       <c r="D183" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E183" s="8" t="s">
+      <c r="F183" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="F183" s="11">
+      <c r="G183" s="11">
         <v>705</v>
       </c>
-      <c r="G183" s="3">
-        <v>1</v>
-      </c>
-      <c r="H183" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="184" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H183" s="3">
+        <v>1</v>
+      </c>
+      <c r="I183" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>437</v>
       </c>
-      <c r="E184" s="7" t="s">
+      <c r="F184" s="7" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>439</v>
       </c>
       <c r="C185" t="s">
         <v>440</v>
       </c>
-      <c r="E185" s="7" t="s">
+      <c r="F185" s="7" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>442</v>
       </c>
-      <c r="E186" s="7" t="s">
+      <c r="F186" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>443</v>
       </c>
-      <c r="E187" s="7" t="s">
+      <c r="F187" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="188" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
         <v>446</v>
       </c>
@@ -4710,40 +4791,40 @@
       <c r="C188" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="E188" s="8"/>
-      <c r="F188" s="11">
+      <c r="F188" s="8"/>
+      <c r="G188" s="11">
         <v>558</v>
       </c>
-      <c r="G188" s="3">
-        <v>1</v>
-      </c>
-      <c r="H188" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="189" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H188" s="3">
+        <v>1</v>
+      </c>
+      <c r="I188" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>97</v>
       </c>
       <c r="C189" t="s">
         <v>447</v>
       </c>
-      <c r="E189" s="7" t="s">
+      <c r="F189" s="7" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>97</v>
       </c>
       <c r="B190" t="s">
         <v>449</v>
       </c>
-      <c r="E190" s="7" t="s">
+      <c r="F190" s="7" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="191" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
         <v>97</v>
       </c>
@@ -4753,20 +4834,20 @@
       <c r="C191" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="E191" s="8" t="s">
+      <c r="F191" s="8" t="s">
         <v>453</v>
       </c>
-      <c r="F191" s="11">
+      <c r="G191" s="11">
         <v>37</v>
       </c>
-      <c r="G191" s="3">
-        <v>1</v>
-      </c>
-      <c r="H191" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H191" s="3">
+        <v>1</v>
+      </c>
+      <c r="I191" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>164</v>
       </c>
@@ -4776,79 +4857,79 @@
       <c r="C192" t="s">
         <v>166</v>
       </c>
-      <c r="E192" s="7" t="s">
+      <c r="F192" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>168</v>
       </c>
       <c r="B193" t="s">
         <v>167</v>
       </c>
-      <c r="E193" s="7" t="s">
+      <c r="F193" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>244</v>
       </c>
       <c r="B194" t="s">
         <v>245</v>
       </c>
-      <c r="E194" s="7" t="s">
+      <c r="F194" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>264</v>
       </c>
-      <c r="E195" s="7" t="s">
+      <c r="F195" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>265</v>
       </c>
-      <c r="E196" s="7" t="s">
+      <c r="F196" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>39</v>
       </c>
       <c r="C197" t="s">
         <v>40</v>
       </c>
-      <c r="E197" s="7" t="s">
+      <c r="F197" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F198" s="13">
-        <f>SUM(F2:F193)</f>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G198" s="13">
+        <f>SUM(G2:G193)</f>
         <v>27449</v>
       </c>
-      <c r="G198" s="5" t="s">
+      <c r="H198" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F199" s="13">
-        <f>SUM(G2:G193)</f>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G199" s="13">
+        <f>SUM(H2:H193)</f>
         <v>71</v>
       </c>
-      <c r="G199" s="5" t="s">
+      <c r="H199" s="5" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E126">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F126">
     <sortCondition ref="A2:A126"/>
     <sortCondition ref="C2:C126"/>
   </sortState>

</xml_diff>

<commit_message>
add potential species to look at
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198194_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198222_2_11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207FC0D1-FC45-47DB-B61C-3A29A9DF7698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7BA10F-1B90-4949-A4F4-8D15989727E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="461">
   <si>
     <t>Species</t>
   </si>
@@ -1413,6 +1413,12 @@
   </si>
   <si>
     <t>2 years</t>
+  </si>
+  <si>
+    <t>Amaranthus tuberculatus</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.1900870116</t>
   </si>
 </sst>
 </file>
@@ -1800,10 +1806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I199"/>
+  <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,88 +1878,77 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F4" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="11">
+      <c r="F5" s="8"/>
+      <c r="G5" s="11">
         <v>87</v>
       </c>
-      <c r="H4" s="3">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>70</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>136</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="11">
-        <v>56</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>299</v>
+        <v>36</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>454</v>
@@ -1963,65 +1958,78 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="11">
+        <v>56</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="11">
         <v>142</v>
       </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>243</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F9" s="7" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="11">
+      <c r="F10" s="8"/>
+      <c r="G10" s="11">
         <v>1135</v>
       </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" t="s">
-        <v>143</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>142</v>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2029,7 +2037,7 @@
         <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>142</v>
@@ -2040,10 +2048,10 @@
         <v>82</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2051,7 +2059,7 @@
         <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>145</v>
@@ -2059,195 +2067,180 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>120</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>147</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F15" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="G15" s="11">
+      <c r="G16" s="11">
         <v>597</v>
       </c>
-      <c r="H15" s="3">
-        <v>1</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="H16" s="3">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>83</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>136</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>454</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="8" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G18" s="11">
         <v>467</v>
       </c>
-      <c r="H17" s="3">
-        <v>1</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>105</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>151</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B20" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="G19" s="11">
+      <c r="G20" s="11">
         <v>56</v>
       </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>128</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>63</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>126</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>153</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F22" s="7" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" t="s">
-        <v>136</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>108</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>155</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="G24" s="11">
-        <v>119</v>
-      </c>
-      <c r="H24" s="3">
-        <v>1</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>158</v>
@@ -2262,111 +2255,126 @@
         <v>159</v>
       </c>
       <c r="G25" s="11">
+        <v>119</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" s="11">
         <v>199</v>
       </c>
-      <c r="H25" s="3">
-        <v>1</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="H26" s="3">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>109</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>156</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G28" s="11">
         <v>40</v>
       </c>
-      <c r="H27" s="3">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" t="s">
-        <v>58</v>
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
         <v>58</v>
       </c>
-      <c r="F29" s="7" t="s">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F31" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G31" s="11">
         <v>52</v>
       </c>
-      <c r="H30" s="3">
-        <v>1</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>137</v>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C32" t="s">
         <v>136</v>
@@ -2375,117 +2383,117 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="G33" s="11">
-        <v>296</v>
-      </c>
-      <c r="H33" s="3">
-        <v>1</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>259</v>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>173</v>
+        <v>73</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>454</v>
       </c>
       <c r="F34" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="G34" s="11">
+        <v>296</v>
+      </c>
+      <c r="H34" s="3">
+        <v>1</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G35" s="11">
         <v>3171</v>
       </c>
-      <c r="H34" s="3">
-        <v>1</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>68</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>136</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F36" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G37" s="11">
         <v>337</v>
       </c>
-      <c r="H36" s="3">
-        <v>1</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="H37" s="3">
+        <v>1</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>116</v>
-      </c>
-      <c r="C37" t="s">
-        <v>136</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>117</v>
       </c>
       <c r="C38" t="s">
         <v>136</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>137</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
         <v>136</v>
@@ -2494,41 +2502,38 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G41" s="11">
         <v>115</v>
       </c>
-      <c r="H40" s="3">
-        <v>1</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" t="s">
-        <v>176</v>
-      </c>
-      <c r="C41" t="s">
-        <v>177</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>145</v>
+      <c r="H41" s="3">
+        <v>1</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2539,7 +2544,7 @@
         <v>176</v>
       </c>
       <c r="C42" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F42" s="7" t="s">
         <v>145</v>
@@ -2547,43 +2552,46 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>176</v>
       </c>
       <c r="C43" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" t="s">
-        <v>181</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>121</v>
+      </c>
+      <c r="B45" t="s">
+        <v>181</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>180</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
         <v>136</v>
@@ -2594,7 +2602,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="C47" t="s">
         <v>136</v>
@@ -2605,7 +2613,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
         <v>136</v>
@@ -2616,7 +2624,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
         <v>136</v>
@@ -2625,184 +2633,184 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="G50" s="11">
-        <v>1674</v>
-      </c>
-      <c r="H50" s="3">
-        <v>1</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G51" s="11">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1674</v>
+      </c>
+      <c r="H51" s="3">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="G52" s="11">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F53" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G53" s="11">
         <v>279</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>45</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>46</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>47</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F54" s="7" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>454</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>456</v>
-      </c>
-      <c r="F54" s="8"/>
-      <c r="G54" s="11">
-        <v>185</v>
-      </c>
-      <c r="H54" s="3">
-        <v>1</v>
-      </c>
-      <c r="I54" s="3" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>456</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="11">
+        <v>185</v>
+      </c>
+      <c r="H55" s="3">
+        <v>1</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F56" s="8"/>
+      <c r="G56" s="11">
         <v>336</v>
       </c>
-      <c r="H55" s="3">
-        <v>1</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="H56" s="3">
+        <v>1</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>111</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>136</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="F57" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+    <row r="58" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F57" s="8"/>
-      <c r="G57" s="11">
+      <c r="F58" s="8"/>
+      <c r="G58" s="11">
         <v>1081</v>
       </c>
-      <c r="H57" s="3">
-        <v>1</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="7" t="s">
-        <v>251</v>
+      <c r="H58" s="3">
+        <v>1</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>113</v>
-      </c>
-      <c r="C59" t="s">
-        <v>136</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
       <c r="F59" s="7" t="s">
-        <v>137</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C60" t="s">
         <v>136</v>
@@ -2813,7 +2821,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C61" t="s">
         <v>136</v>
@@ -2824,305 +2832,305 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62" t="s">
+        <v>136</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>25</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>38</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>37</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F63" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+    <row r="64" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B64" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="F63" s="8"/>
-      <c r="G63" s="11">
+      <c r="F64" s="8"/>
+      <c r="G64" s="11">
         <v>300</v>
       </c>
-      <c r="H63" s="3">
-        <v>1</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="H64" s="3">
+        <v>1</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>74</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>136</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F65" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+    <row r="66" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B66" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="F65" s="8" t="s">
+      <c r="F66" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="G65" s="11">
+      <c r="G66" s="11">
         <v>131</v>
       </c>
-      <c r="H65" s="3">
-        <v>1</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>89</v>
-      </c>
-      <c r="B66" t="s">
-        <v>192</v>
-      </c>
-      <c r="C66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>145</v>
+      <c r="H66" s="3">
+        <v>1</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B67" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C67" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F67" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>90</v>
+      </c>
+      <c r="B68" t="s">
+        <v>193</v>
+      </c>
+      <c r="C68" t="s">
+        <v>194</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B69" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F69" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="G68" s="11">
+      <c r="G69" s="11">
         <v>200</v>
       </c>
-      <c r="H68" s="3">
-        <v>1</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>99</v>
-      </c>
-      <c r="B69" t="s">
-        <v>136</v>
-      </c>
-      <c r="C69" t="s">
-        <v>196</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>197</v>
+      <c r="H69" s="3">
+        <v>1</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" t="s">
+        <v>196</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>28</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>136</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+    <row r="72" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B72" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="F72" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="G71" s="11">
+      <c r="G72" s="11">
         <v>136</v>
       </c>
-      <c r="H71" s="3">
-        <v>1</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="H72" s="3">
+        <v>1</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>92</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>136</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F73" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+    <row r="74" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B74" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F74" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="G73" s="11">
+      <c r="G74" s="11">
         <v>44</v>
       </c>
-      <c r="H73" s="3">
-        <v>1</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="H74" s="3">
+        <v>1</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>100</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>200</v>
       </c>
-      <c r="F74" s="7" t="s">
+      <c r="F75" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+    <row r="76" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="F75" s="8" t="s">
+      <c r="F76" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="G75" s="3">
+      <c r="G76" s="3">
         <v>39</v>
       </c>
-      <c r="H75" s="3">
-        <v>1</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>67</v>
-      </c>
-      <c r="B76" t="s">
-        <v>202</v>
-      </c>
-      <c r="C76" t="s">
-        <v>252</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="H76" s="3">
+        <v>1</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>67</v>
       </c>
       <c r="B77" t="s">
+        <v>202</v>
+      </c>
+      <c r="C77" t="s">
+        <v>252</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" t="s">
         <v>184</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>195</v>
       </c>
-      <c r="F77" s="7" t="s">
+      <c r="F78" s="7" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="78" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+    <row r="79" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="F78" s="8" t="s">
+      <c r="F79" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="G78" s="11">
+      <c r="G79" s="11">
         <v>38</v>
       </c>
-      <c r="H78" s="3">
-        <v>1</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>129</v>
-      </c>
-      <c r="C79" t="s">
-        <v>136</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>203</v>
+      <c r="H79" s="3">
+        <v>1</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C80" t="s">
         <v>136</v>
@@ -3133,207 +3141,207 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>122</v>
       </c>
       <c r="C81" t="s">
         <v>136</v>
       </c>
       <c r="F81" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>69</v>
+      </c>
+      <c r="C82" t="s">
+        <v>136</v>
+      </c>
+      <c r="F82" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="82" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+    <row r="83" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="F82" s="8" t="s">
+      <c r="F83" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="G82" s="11">
+      <c r="G83" s="11">
         <v>52</v>
       </c>
-      <c r="H82" s="3">
-        <v>1</v>
-      </c>
-      <c r="I82" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>78</v>
-      </c>
-      <c r="B83" t="s">
-        <v>136</v>
-      </c>
-      <c r="C83" t="s">
-        <v>204</v>
+      <c r="H83" s="3">
+        <v>1</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
       <c r="B84" t="s">
         <v>136</v>
       </c>
       <c r="C84" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>125</v>
+      </c>
+      <c r="B85" t="s">
         <v>136</v>
       </c>
-      <c r="F84" s="7" t="s">
+      <c r="C85" t="s">
+        <v>136</v>
+      </c>
+      <c r="F85" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="85" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+    <row r="86" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F85" s="8" t="s">
+      <c r="F86" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="G85" s="12">
+      <c r="G86" s="12">
         <v>3024</v>
       </c>
-      <c r="H85" s="3">
-        <v>1</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="H86" s="3">
+        <v>1</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F86" s="8" t="s">
+      <c r="F87" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="G86" s="11">
+      <c r="G87" s="11">
         <v>85</v>
       </c>
-      <c r="H86" s="3">
-        <v>1</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="H87" s="3">
+        <v>1</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B88" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="F87" s="8" t="s">
+      <c r="F88" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="G87" s="11">
+      <c r="G88" s="11">
         <v>747</v>
       </c>
-      <c r="H87" s="3">
-        <v>1</v>
-      </c>
-      <c r="I87" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="H88" s="3">
+        <v>1</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>93</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>136</v>
       </c>
-      <c r="F88" s="7" t="s">
+      <c r="F89" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+    <row r="90" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F89" s="8"/>
-      <c r="G89" s="11">
+      <c r="F90" s="8"/>
+      <c r="G90" s="11">
         <v>683</v>
       </c>
-      <c r="H89" s="3">
-        <v>1</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="H90" s="3">
+        <v>1</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>118</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" t="s">
         <v>136</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="F91" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="91" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+    <row r="92" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C92" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F91" s="8" t="s">
+      <c r="F92" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="G91" s="11">
+      <c r="G92" s="11">
         <v>52</v>
       </c>
-      <c r="H91" s="3">
-        <v>1</v>
-      </c>
-      <c r="I91" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>51</v>
-      </c>
-      <c r="B92" t="s">
-        <v>54</v>
-      </c>
-      <c r="C92" t="s">
-        <v>53</v>
+      <c r="H92" s="3">
+        <v>1</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3341,65 +3349,65 @@
         <v>51</v>
       </c>
       <c r="B93" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C93" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>51</v>
       </c>
+      <c r="B94" t="s">
+        <v>57</v>
+      </c>
       <c r="C94" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>51</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>51</v>
+      </c>
+      <c r="B96" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="96" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+    <row r="97" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B97" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="C97" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="F96" s="8" t="s">
+      <c r="F97" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="G96" s="11">
+      <c r="G97" s="11">
         <v>428</v>
       </c>
-      <c r="H96" s="3">
-        <v>1</v>
-      </c>
-      <c r="I96" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>101</v>
-      </c>
-      <c r="C97" t="s">
-        <v>136</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>137</v>
+      <c r="H97" s="3">
+        <v>1</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C98" t="s">
         <v>136</v>
@@ -3410,7 +3418,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C99" t="s">
         <v>136</v>
@@ -3419,58 +3427,61 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="F100" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="G100" s="11">
-        <v>909</v>
-      </c>
-      <c r="H100" s="3">
-        <v>1</v>
-      </c>
-      <c r="I100" s="3" t="s">
-        <v>259</v>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>107</v>
+      </c>
+      <c r="C100" t="s">
+        <v>136</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F101" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="G101" s="11">
+        <v>909</v>
+      </c>
+      <c r="H101" s="3">
+        <v>1</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B101" s="3" t="s">
+      <c r="B102" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F101" s="8" t="s">
+      <c r="F102" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="G101" s="11">
+      <c r="G102" s="11">
         <v>38</v>
       </c>
-      <c r="H101" s="3">
-        <v>1</v>
-      </c>
-      <c r="I101" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>18</v>
-      </c>
-      <c r="C102" t="s">
-        <v>17</v>
+      <c r="H102" s="3">
+        <v>1</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -3478,58 +3489,52 @@
         <v>18</v>
       </c>
       <c r="C103" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>18</v>
+      </c>
+      <c r="C104" t="s">
         <v>218</v>
       </c>
-      <c r="F103" s="7" t="s">
+      <c r="F104" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="104" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+    <row r="105" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="B105" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C104" s="3" t="s">
+      <c r="C105" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F104" s="8" t="s">
+      <c r="F105" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="G104" s="11">
+      <c r="G105" s="11">
         <v>360</v>
       </c>
-      <c r="H104" s="3">
-        <v>1</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>79</v>
-      </c>
-      <c r="C105" t="s">
-        <v>222</v>
-      </c>
-      <c r="F105" s="7" t="s">
-        <v>223</v>
+      <c r="H105" s="3">
+        <v>1</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>31</v>
-      </c>
-      <c r="B106" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="C106" t="s">
-        <v>33</v>
+        <v>222</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>145</v>
+        <v>223</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -3537,53 +3542,44 @@
         <v>31</v>
       </c>
       <c r="B107" t="s">
+        <v>34</v>
+      </c>
+      <c r="C107" t="s">
+        <v>33</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>31</v>
+      </c>
+      <c r="B108" t="s">
         <v>225</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C108" t="s">
         <v>224</v>
       </c>
-      <c r="F107" s="7" t="s">
+      <c r="F108" s="7" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="108" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+    <row r="109" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B109" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="C109" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F108" s="8" t="s">
+      <c r="F109" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="G108" s="11">
+      <c r="G109" s="11">
         <v>400</v>
-      </c>
-      <c r="H108" s="3">
-        <v>1</v>
-      </c>
-      <c r="I108" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="F109" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="G109" s="11">
-        <v>296</v>
       </c>
       <c r="H109" s="3">
         <v>1</v>
@@ -3594,123 +3590,135 @@
     </row>
     <row r="110" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="F110" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="G110" s="11">
+        <v>296</v>
+      </c>
+      <c r="H110" s="3">
+        <v>1</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B111" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="F110" s="8" t="s">
+      <c r="F111" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="G110" s="11">
+      <c r="G111" s="11">
         <v>36</v>
       </c>
-      <c r="H110" s="3">
-        <v>1</v>
-      </c>
-      <c r="I110" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>104</v>
-      </c>
-      <c r="C111" t="s">
-        <v>136</v>
-      </c>
-      <c r="F111" s="7" t="s">
-        <v>137</v>
+      <c r="H111" s="3">
+        <v>1</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>27</v>
-      </c>
-      <c r="B112" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="C112" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>27</v>
+      </c>
+      <c r="B113" t="s">
+        <v>64</v>
+      </c>
+      <c r="C113" t="s">
+        <v>65</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>95</v>
       </c>
-      <c r="F113" s="7" t="s">
+      <c r="F114" s="7" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B114" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="G114" s="11">
-        <v>786</v>
-      </c>
-      <c r="H114" s="3">
-        <v>1</v>
-      </c>
-      <c r="I114" s="3" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="F115" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G115" s="11">
+        <v>786</v>
+      </c>
+      <c r="H115" s="3">
+        <v>1</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B115" s="3" t="s">
+      <c r="B116" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C116" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="D116" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F115" s="8" t="s">
+      <c r="F116" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="G115" s="11">
+      <c r="G116" s="11">
         <v>114</v>
       </c>
-      <c r="H115" s="3">
-        <v>1</v>
-      </c>
-      <c r="I115" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>80</v>
-      </c>
-      <c r="C116" t="s">
-        <v>136</v>
-      </c>
-      <c r="F116" s="7" t="s">
-        <v>137</v>
+      <c r="H116" s="3">
+        <v>1</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="C117" t="s">
         <v>136</v>
@@ -3721,41 +3729,44 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>97</v>
+      </c>
+      <c r="C118" t="s">
+        <v>136</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>10</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+    <row r="120" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B120" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C120" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F119" s="8" t="s">
+      <c r="F120" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="G119" s="11">
+      <c r="G120" s="11">
         <v>117</v>
       </c>
-      <c r="H119" s="3">
-        <v>1</v>
-      </c>
-      <c r="I119" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>10</v>
-      </c>
-      <c r="C120" t="s">
-        <v>13</v>
+      <c r="H120" s="3">
+        <v>1</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -3763,165 +3774,149 @@
         <v>10</v>
       </c>
       <c r="C121" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>10</v>
+      </c>
+      <c r="C122" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F122" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="G122" s="11">
-        <v>33</v>
-      </c>
-      <c r="H122" s="3">
-        <v>1</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B123" s="3" t="s">
+        <v>296</v>
+      </c>
       <c r="C123" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F123" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="G123" s="11"/>
-    </row>
-    <row r="124" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="G123" s="11">
+        <v>33</v>
+      </c>
+      <c r="H123" s="3">
+        <v>1</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F124" s="8"/>
-      <c r="G124" s="11">
-        <v>277</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F124" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="G124" s="11"/>
     </row>
     <row r="125" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F125" s="8"/>
       <c r="G125" s="11">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" s="8"/>
+      <c r="G126" s="11">
         <v>599</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>124</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C127" t="s">
         <v>237</v>
       </c>
-      <c r="F126" s="7" t="s">
+      <c r="F127" s="7" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="127" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
+    <row r="128" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B128" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C128" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="D127" s="3" t="s">
+      <c r="D128" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F127" s="8"/>
-      <c r="G127" s="11">
+      <c r="F128" s="8"/>
+      <c r="G128" s="11">
         <v>306</v>
       </c>
-      <c r="H127" s="3">
-        <v>1</v>
-      </c>
-      <c r="I127" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="H128" s="3">
+        <v>1</v>
+      </c>
+      <c r="I128" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>160</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>162</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C129" t="s">
         <v>161</v>
       </c>
-      <c r="F128" s="7" t="s">
+      <c r="F129" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>312</v>
       </c>
-      <c r="F129" s="7" t="s">
+      <c r="F130" s="7" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="130" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
+    <row r="131" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B131" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C131" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F130" s="8"/>
-      <c r="G130" s="11">
-        <v>306</v>
-      </c>
-      <c r="H130" s="3">
-        <v>1</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>321</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>323</v>
       </c>
       <c r="F131" s="8"/>
       <c r="G131" s="11">
-        <v>479</v>
+        <v>306</v>
       </c>
       <c r="H131" s="3">
         <v>1</v>
@@ -3932,20 +3927,20 @@
     </row>
     <row r="132" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>323</v>
       </c>
       <c r="F132" s="8"/>
       <c r="G132" s="11">
-        <v>1007</v>
+        <v>479</v>
       </c>
       <c r="H132" s="3">
         <v>1</v>
@@ -3954,267 +3949,280 @@
         <v>259</v>
       </c>
     </row>
-    <row r="133" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F133" s="8" t="s">
+      <c r="F133" s="8"/>
+      <c r="G133" s="11">
+        <v>1007</v>
+      </c>
+      <c r="H133" s="3">
+        <v>1</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F134" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="G133" s="11">
+      <c r="G134" s="11">
         <v>10</v>
       </c>
-      <c r="H133" s="3">
-        <v>1</v>
-      </c>
-      <c r="I133" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="H134" s="3">
+        <v>1</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>329</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D135" t="s">
         <v>323</v>
       </c>
-      <c r="F134" s="7" t="s">
+      <c r="F135" s="7" t="s">
         <v>330</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F135" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="G135" s="11">
-        <v>135</v>
-      </c>
-      <c r="H135" s="3">
-        <v>1</v>
-      </c>
-      <c r="I135" s="3" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="136" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>323</v>
       </c>
       <c r="F136" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="G136" s="11">
+        <v>135</v>
+      </c>
+      <c r="H136" s="3">
+        <v>1</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F137" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="G136" s="11">
+      <c r="G137" s="11">
         <v>7</v>
       </c>
-      <c r="H136" s="3">
-        <v>1</v>
-      </c>
-      <c r="I136" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>339</v>
-      </c>
-      <c r="D137" t="s">
-        <v>323</v>
-      </c>
-      <c r="F137" s="7" t="s">
-        <v>137</v>
+      <c r="H137" s="3">
+        <v>1</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>340</v>
+        <v>339</v>
+      </c>
+      <c r="D138" t="s">
+        <v>323</v>
       </c>
       <c r="F138" s="7" t="s">
-        <v>341</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>340</v>
+      </c>
+      <c r="F139" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>342</v>
       </c>
-      <c r="F139" s="7" t="s">
+      <c r="F140" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="140" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
+    <row r="141" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B140" s="3" t="s">
+      <c r="B141" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="C140" s="3" t="s">
+      <c r="C141" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="D140" s="3" t="s">
+      <c r="D141" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F140" s="8" t="s">
+      <c r="F141" s="8" t="s">
         <v>348</v>
       </c>
-      <c r="G140" s="11">
+      <c r="G141" s="11">
         <v>34</v>
       </c>
-      <c r="H140" s="3">
-        <v>1</v>
-      </c>
-      <c r="I140" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="H141" s="3">
+        <v>1</v>
+      </c>
+      <c r="I141" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>349</v>
       </c>
-      <c r="F141" s="7" t="s">
+      <c r="F142" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>350</v>
       </c>
-      <c r="F142" s="7" t="s">
+      <c r="F143" s="7" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>98</v>
       </c>
-      <c r="F143" s="7" t="s">
+      <c r="F144" s="7" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="144" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
+    <row r="145" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B145" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="C144" s="3" t="s">
+      <c r="C145" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D145" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F144" s="8"/>
-      <c r="G144" s="11">
+      <c r="F145" s="8"/>
+      <c r="G145" s="11">
         <v>1175</v>
       </c>
-      <c r="H144" s="3">
-        <v>1</v>
-      </c>
-      <c r="I144" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>356</v>
-      </c>
-      <c r="D145" t="s">
-        <v>323</v>
-      </c>
-      <c r="F145" s="7" t="s">
-        <v>357</v>
+      <c r="H145" s="3">
+        <v>1</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D146" t="s">
         <v>323</v>
       </c>
       <c r="F146" s="7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>358</v>
+      </c>
+      <c r="D147" t="s">
+        <v>323</v>
+      </c>
+      <c r="F147" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="147" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
+    <row r="148" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B148" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="C147" s="3" t="s">
+      <c r="C148" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D147" s="3" t="s">
+      <c r="D148" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F147" s="8"/>
-      <c r="G147" s="11">
+      <c r="F148" s="8"/>
+      <c r="G148" s="11">
         <v>171</v>
       </c>
-      <c r="H147" s="3">
-        <v>1</v>
-      </c>
-      <c r="I147" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>362</v>
-      </c>
-      <c r="D148" t="s">
-        <v>323</v>
-      </c>
-      <c r="F148" s="7" t="s">
-        <v>363</v>
+      <c r="H148" s="3">
+        <v>1</v>
+      </c>
+      <c r="I148" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D149" t="s">
         <v>323</v>
       </c>
       <c r="F149" s="7" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D150" t="s">
         <v>323</v>
@@ -4225,7 +4233,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D151" t="s">
         <v>323</v>
@@ -4234,83 +4242,83 @@
         <v>343</v>
       </c>
     </row>
-    <row r="152" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="s">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>366</v>
+      </c>
+      <c r="D152" t="s">
+        <v>323</v>
+      </c>
+      <c r="F152" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="B152" s="3" t="s">
+      <c r="B153" s="3" t="s">
         <v>367</v>
       </c>
-      <c r="D152" s="3" t="s">
+      <c r="D153" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F152" s="8" t="s">
+      <c r="F153" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="G152" s="11">
+      <c r="G153" s="11">
         <v>14</v>
       </c>
-      <c r="H152" s="3">
-        <v>1</v>
-      </c>
-      <c r="I152" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>370</v>
-      </c>
-      <c r="F153" s="7" t="s">
-        <v>357</v>
+      <c r="H153" s="3">
+        <v>1</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>370</v>
+      </c>
+      <c r="F154" s="7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>371</v>
       </c>
-      <c r="F154" s="7" t="s">
+      <c r="F155" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="155" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="3" t="s">
+    <row r="156" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B156" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="C155" s="3" t="s">
+      <c r="C156" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D156" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F155" s="8"/>
-      <c r="G155" s="11">
+      <c r="F156" s="8"/>
+      <c r="G156" s="11">
         <v>550</v>
       </c>
-      <c r="H155" s="3">
-        <v>1</v>
-      </c>
-      <c r="I155" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>376</v>
-      </c>
-      <c r="D156" t="s">
-        <v>323</v>
-      </c>
-      <c r="F156" s="7" t="s">
-        <v>372</v>
+      <c r="H156" s="3">
+        <v>1</v>
+      </c>
+      <c r="I156" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D157" t="s">
         <v>323</v>
@@ -4319,160 +4327,148 @@
         <v>372</v>
       </c>
     </row>
-    <row r="158" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>377</v>
+      </c>
+      <c r="D158" t="s">
+        <v>323</v>
+      </c>
+      <c r="F158" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="B158" s="3" t="s">
+      <c r="B159" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="C159" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="D159" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F158" s="8"/>
-      <c r="G158" s="11">
+      <c r="F159" s="8"/>
+      <c r="G159" s="11">
         <v>55</v>
       </c>
-      <c r="H158" s="3">
-        <v>1</v>
-      </c>
-      <c r="I158" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>381</v>
-      </c>
-      <c r="F159" s="7" t="s">
-        <v>372</v>
+      <c r="H159" s="3">
+        <v>1</v>
+      </c>
+      <c r="I159" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F160" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="161" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>382</v>
+      </c>
+      <c r="F161" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="B161" s="3" t="s">
+      <c r="B162" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="C161" s="3" t="s">
+      <c r="C162" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D161" s="3" t="s">
+      <c r="D162" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F161" s="8"/>
-      <c r="G161" s="11">
+      <c r="F162" s="8"/>
+      <c r="G162" s="11">
         <v>86</v>
       </c>
-      <c r="H161" s="3">
-        <v>1</v>
-      </c>
-      <c r="I161" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="H162" s="3">
+        <v>1</v>
+      </c>
+      <c r="I162" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>383</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B163" t="s">
         <v>385</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C163" t="s">
         <v>384</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D163" t="s">
         <v>323</v>
       </c>
-      <c r="F162" s="7" t="s">
+      <c r="F163" s="7" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="163" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
+    <row r="164" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="C163" s="5" t="s">
+      <c r="C164" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="D163" s="5" t="s">
+      <c r="D164" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="F163" s="14" t="s">
+      <c r="F164" s="14" t="s">
         <v>388</v>
       </c>
-      <c r="G163" s="13">
+      <c r="G164" s="13">
         <v>16</v>
       </c>
-      <c r="H163" s="5">
-        <v>1</v>
-      </c>
-      <c r="I163" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="3" t="s">
+      <c r="H164" s="5">
+        <v>1</v>
+      </c>
+      <c r="I164" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="B165" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="C164" s="3" t="s">
+      <c r="C165" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="F164" s="8"/>
-      <c r="G164" s="11">
+      <c r="F165" s="8"/>
+      <c r="G165" s="11">
         <v>163</v>
       </c>
-      <c r="H164" s="3">
-        <v>1</v>
-      </c>
-      <c r="I164" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="C165" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D165" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="F165" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="G165" s="13">
-        <v>21</v>
-      </c>
-      <c r="H165" s="5">
-        <v>1</v>
-      </c>
-      <c r="I165" s="5" t="s">
+      <c r="H165" s="3">
+        <v>1</v>
+      </c>
+      <c r="I165" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="166" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>323</v>
@@ -4481,7 +4477,7 @@
         <v>236</v>
       </c>
       <c r="G166" s="13">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H166" s="5">
         <v>1</v>
@@ -4492,10 +4488,10 @@
     </row>
     <row r="167" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D167" s="5" t="s">
         <v>323</v>
@@ -4504,369 +4500,381 @@
         <v>236</v>
       </c>
       <c r="G167" s="13">
+        <v>18</v>
+      </c>
+      <c r="H167" s="5">
+        <v>1</v>
+      </c>
+      <c r="I167" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C168" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="F168" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="G168" s="13">
         <v>19</v>
       </c>
-      <c r="H167" s="5">
-        <v>1</v>
-      </c>
-      <c r="I167" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="H168" s="5">
+        <v>1</v>
+      </c>
+      <c r="I168" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>399</v>
       </c>
-      <c r="D168" t="s">
+      <c r="D169" t="s">
         <v>323</v>
       </c>
-      <c r="F168" s="7" t="s">
+      <c r="F169" s="7" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="169" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
+    <row r="170" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="C169" s="5" t="s">
+      <c r="C170" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="D169" s="5" t="s">
+      <c r="D170" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="F169" s="14" t="s">
+      <c r="F170" s="14" t="s">
         <v>403</v>
       </c>
-      <c r="G169" s="13">
+      <c r="G170" s="13">
         <v>10</v>
       </c>
-      <c r="H169" s="5">
-        <v>1</v>
-      </c>
-      <c r="I169" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="3" t="s">
+      <c r="H170" s="5">
+        <v>1</v>
+      </c>
+      <c r="I170" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="B170" s="3" t="s">
+      <c r="B171" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="C170" s="3" t="s">
+      <c r="C171" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="D170" s="3" t="s">
+      <c r="D171" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F170" s="8" t="s">
+      <c r="F171" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="G170" s="11">
+      <c r="G171" s="11">
         <v>445</v>
       </c>
-      <c r="H170" s="3">
-        <v>1</v>
-      </c>
-      <c r="I170" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>408</v>
-      </c>
-      <c r="F171" s="7" t="s">
-        <v>357</v>
+      <c r="H171" s="3">
+        <v>1</v>
+      </c>
+      <c r="I171" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F172" s="7" t="s">
-        <v>410</v>
+        <v>357</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F173" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>411</v>
+      </c>
+      <c r="F174" s="7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>413</v>
       </c>
-      <c r="F174" s="7" t="s">
+      <c r="F175" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="175" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A175" s="3" t="s">
+    <row r="176" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="B175" s="3" t="s">
+      <c r="B176" s="3" t="s">
         <v>415</v>
-      </c>
-      <c r="D175" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F175" s="8" t="s">
-        <v>416</v>
-      </c>
-      <c r="G175" s="11">
-        <v>27</v>
-      </c>
-      <c r="H175" s="3">
-        <v>1</v>
-      </c>
-      <c r="I175" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>419</v>
       </c>
       <c r="D176" s="3" t="s">
         <v>323</v>
       </c>
       <c r="F176" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="G176" s="11">
+        <v>27</v>
+      </c>
+      <c r="H176" s="3">
+        <v>1</v>
+      </c>
+      <c r="I176" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F177" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="G176" s="11">
+      <c r="G177" s="11">
         <v>299</v>
       </c>
-      <c r="H176" s="3">
-        <v>1</v>
-      </c>
-      <c r="I176" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="H177" s="3">
+        <v>1</v>
+      </c>
+      <c r="I177" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>421</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C178" t="s">
         <v>422</v>
       </c>
-      <c r="F177" s="7" t="s">
+      <c r="F178" s="7" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="178" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A178" s="3" t="s">
+    <row r="179" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="C178" s="3" t="s">
+      <c r="C179" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="D178" s="3" t="s">
+      <c r="D179" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F178" s="8" t="s">
+      <c r="F179" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="G178" s="11">
+      <c r="G179" s="11">
         <v>160</v>
       </c>
-      <c r="H178" s="3">
-        <v>1</v>
-      </c>
-      <c r="I178" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>427</v>
-      </c>
-      <c r="F179" s="7" t="s">
-        <v>343</v>
+      <c r="H179" s="3">
+        <v>1</v>
+      </c>
+      <c r="I179" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F180" s="7" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>428</v>
+      </c>
+      <c r="F181" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>429</v>
       </c>
-      <c r="F181" s="7" t="s">
+      <c r="F182" s="7" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>431</v>
       </c>
-      <c r="F182" s="7" t="s">
+      <c r="F183" s="7" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="183" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A183" s="3" t="s">
+    <row r="184" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="B183" s="3" t="s">
+      <c r="B184" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="C183" s="3" t="s">
+      <c r="C184" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="D183" s="3" t="s">
+      <c r="D184" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F183" s="8" t="s">
+      <c r="F184" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="G183" s="11">
+      <c r="G184" s="11">
         <v>705</v>
       </c>
-      <c r="H183" s="3">
-        <v>1</v>
-      </c>
-      <c r="I183" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>437</v>
-      </c>
-      <c r="F184" s="7" t="s">
-        <v>438</v>
+      <c r="H184" s="3">
+        <v>1</v>
+      </c>
+      <c r="I184" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>437</v>
+      </c>
+      <c r="F185" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>439</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C186" t="s">
         <v>440</v>
       </c>
-      <c r="F185" s="7" t="s">
+      <c r="F186" s="7" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>442</v>
-      </c>
-      <c r="F186" s="7" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F187" s="7" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="188" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="3" t="s">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>443</v>
+      </c>
+      <c r="F188" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="B188" s="3" t="s">
+      <c r="B189" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="C188" s="3" t="s">
+      <c r="C189" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="F188" s="8"/>
-      <c r="G188" s="11">
+      <c r="F189" s="8"/>
+      <c r="G189" s="11">
         <v>558</v>
       </c>
-      <c r="H188" s="3">
-        <v>1</v>
-      </c>
-      <c r="I188" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>97</v>
-      </c>
-      <c r="C189" t="s">
-        <v>447</v>
-      </c>
-      <c r="F189" s="7" t="s">
-        <v>448</v>
+      <c r="H189" s="3">
+        <v>1</v>
+      </c>
+      <c r="I189" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>97</v>
       </c>
-      <c r="B190" t="s">
+      <c r="C190" t="s">
+        <v>447</v>
+      </c>
+      <c r="F190" s="7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>97</v>
+      </c>
+      <c r="B191" t="s">
         <v>449</v>
       </c>
-      <c r="F190" s="7" t="s">
+      <c r="F191" s="7" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="191" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" s="3" t="s">
+    <row r="192" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B191" s="3" t="s">
+      <c r="B192" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="C191" s="3" t="s">
+      <c r="C192" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="F191" s="8" t="s">
+      <c r="F192" s="8" t="s">
         <v>453</v>
       </c>
-      <c r="G191" s="11">
+      <c r="G192" s="11">
         <v>37</v>
       </c>
-      <c r="H191" s="3">
-        <v>1</v>
-      </c>
-      <c r="I191" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>164</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C192" t="s">
-        <v>166</v>
-      </c>
-      <c r="F192" s="7" t="s">
-        <v>163</v>
+      <c r="H192" s="3">
+        <v>1</v>
+      </c>
+      <c r="I192" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>168</v>
-      </c>
-      <c r="B193" t="s">
-        <v>167</v>
+        <v>164</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C193" t="s">
+        <v>166</v>
       </c>
       <c r="F193" s="7" t="s">
         <v>163</v>
@@ -4874,10 +4882,10 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>244</v>
+        <v>168</v>
       </c>
       <c r="B194" t="s">
-        <v>245</v>
+        <v>167</v>
       </c>
       <c r="F194" s="7" t="s">
         <v>163</v>
@@ -4885,7 +4893,10 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>264</v>
+        <v>244</v>
+      </c>
+      <c r="B195" t="s">
+        <v>245</v>
       </c>
       <c r="F195" s="7" t="s">
         <v>163</v>
@@ -4893,7 +4904,7 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F196" s="7" t="s">
         <v>163</v>
@@ -4901,45 +4912,53 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>39</v>
-      </c>
-      <c r="C197" t="s">
-        <v>40</v>
+        <v>265</v>
       </c>
       <c r="F197" s="7" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G198" s="13">
-        <f>SUM(G2:G193)</f>
-        <v>27449</v>
-      </c>
-      <c r="H198" s="5" t="s">
-        <v>213</v>
+      <c r="A198" t="s">
+        <v>39</v>
+      </c>
+      <c r="C198" t="s">
+        <v>40</v>
+      </c>
+      <c r="F198" s="7" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G199" s="13">
-        <f>SUM(H2:H193)</f>
+        <f>SUM(G2:G194)</f>
+        <v>27449</v>
+      </c>
+      <c r="H199" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G200" s="13">
+        <f>SUM(H2:H194)</f>
         <v>71</v>
       </c>
-      <c r="H199" s="5" t="s">
+      <c r="H200" s="5" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F126">
-    <sortCondition ref="A2:A126"/>
-    <sortCondition ref="C2:C126"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F127">
+    <sortCondition ref="A2:A127"/>
+    <sortCondition ref="C2:C127"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B192" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
-    <hyperlink ref="B34" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
-    <hyperlink ref="B73" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
-    <hyperlink ref="B30" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
-    <hyperlink ref="B19" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
-    <hyperlink ref="B87" r:id="rId6" xr:uid="{2677786D-08C7-4346-837D-960E754FAB79}"/>
+    <hyperlink ref="B193" r:id="rId1" xr:uid="{86A33A3B-22B9-43A2-8CE0-011267E52D14}"/>
+    <hyperlink ref="B35" r:id="rId2" xr:uid="{FB209BDA-41BD-45F8-A916-8086AFD4E4D1}"/>
+    <hyperlink ref="B74" r:id="rId3" xr:uid="{698A0B63-529A-4336-92B6-5976A23AAC8F}"/>
+    <hyperlink ref="B31" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
+    <hyperlink ref="B20" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
+    <hyperlink ref="B88" r:id="rId6" xr:uid="{2677786D-08C7-4346-837D-960E754FAB79}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
change PE to SE
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198222_2_11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198222_2_12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7BA10F-1B90-4949-A4F4-8D15989727E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA340547-04E1-4C6E-BF91-52CD53F565A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="462">
   <si>
     <t>Species</t>
   </si>
@@ -1419,6 +1419,9 @@
   </si>
   <si>
     <t>https://doi.org/10.1073/pnas.1900870116</t>
+  </si>
+  <si>
+    <t>Doesn't look like a divergence time between A. tuberculatus and A. hypochondriacus is known… It's less than 9 million years because that is when the genus according to timetree.org</t>
   </si>
 </sst>
 </file>
@@ -1809,7 +1812,7 @@
   <dimension ref="A1:I200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1878,7 +1881,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>459</v>
       </c>
@@ -1888,7 +1891,9 @@
       <c r="D3" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="14" t="s">
+        <v>461</v>
+      </c>
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add date palm, list of NCBI species
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198222_2_12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\1771458_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA340547-04E1-4C6E-BF91-52CD53F565A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC19667-8114-4598-AE0C-92806505D2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Included species" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="579">
   <si>
     <t>Species</t>
   </si>
@@ -677,9 +678,6 @@
     <t>doi: 10.1186/s13059-019-1648-9</t>
   </si>
   <si>
-    <t>Total number of sequenced individuals</t>
-  </si>
-  <si>
     <t xml:space="preserve">PRJEB1234 </t>
   </si>
   <si>
@@ -755,9 +753,6 @@
     <t>https://doi.org/10.1038/s41467-021-27487-y</t>
   </si>
   <si>
-    <t>Total number of species</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1038/s41467-022-29676-9</t>
   </si>
   <si>
@@ -1422,12 +1417,372 @@
   </si>
   <si>
     <t>Doesn't look like a divergence time between A. tuberculatus and A. hypochondriacus is known… It's less than 9 million years because that is when the genus according to timetree.org</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41467-019-12604-9</t>
+  </si>
+  <si>
+    <t>PRJNA505141</t>
+  </si>
+  <si>
+    <t>NCBI</t>
+  </si>
+  <si>
+    <t>Abrus precatorius</t>
+  </si>
+  <si>
+    <t>Actinidia rufa</t>
+  </si>
+  <si>
+    <t>Adiantum capillus-veneris</t>
+  </si>
+  <si>
+    <t>Adiantum nelumboides</t>
+  </si>
+  <si>
+    <t>Arabidopsis suecica</t>
+  </si>
+  <si>
+    <t>Arabis nemorensis</t>
+  </si>
+  <si>
+    <t>Arachis duranensis</t>
+  </si>
+  <si>
+    <t>Arachis ipaensis</t>
+  </si>
+  <si>
+    <t>Aristolochia fimbriata</t>
+  </si>
+  <si>
+    <t>Bauhinia variegata</t>
+  </si>
+  <si>
+    <t>Benincasa hispida</t>
+  </si>
+  <si>
+    <t>Brassica carinata</t>
+  </si>
+  <si>
+    <t>Buddleja alternifolia</t>
+  </si>
+  <si>
+    <t>Cajanus cajan</t>
+  </si>
+  <si>
+    <t>Camellia sinensis</t>
+  </si>
+  <si>
+    <t>Carex littledalei</t>
+  </si>
+  <si>
+    <t>Castanea mollissima</t>
+  </si>
+  <si>
+    <t>Ceratodon purpureus</t>
+  </si>
+  <si>
+    <t>Ceratopteris richardii</t>
+  </si>
+  <si>
+    <t>Coffea arabica</t>
+  </si>
+  <si>
+    <t>Coffea eugenioides</t>
+  </si>
+  <si>
+    <t>Coptis chinensis</t>
+  </si>
+  <si>
+    <t>Cucurbita argyrosperma</t>
+  </si>
+  <si>
+    <t>Cucurbita maxima</t>
+  </si>
+  <si>
+    <t>Cucurbita moschata</t>
+  </si>
+  <si>
+    <t>Cucurbita pepo</t>
+  </si>
+  <si>
+    <t>Cuscuta campestris</t>
+  </si>
+  <si>
+    <t>Cuscuta epithymum</t>
+  </si>
+  <si>
+    <t>Cuscuta europaea</t>
+  </si>
+  <si>
+    <t>Dendrobium chrysotoxum</t>
+  </si>
+  <si>
+    <t>Dendrobium nobile</t>
+  </si>
+  <si>
+    <t>Dioscorea cayenensis</t>
+  </si>
+  <si>
+    <t>Diospyros lotus</t>
+  </si>
+  <si>
+    <t>Durio zibethinus</t>
+  </si>
+  <si>
+    <t>Elaeis guineensis</t>
+  </si>
+  <si>
+    <t>Eleusine coracana</t>
+  </si>
+  <si>
+    <t>Ensete ventricosum</t>
+  </si>
+  <si>
+    <t>Erigeron canadensis</t>
+  </si>
+  <si>
+    <t>Genlisea aurea</t>
+  </si>
+  <si>
+    <t>Gossypium anomalum</t>
+  </si>
+  <si>
+    <t>Gossypium arboreum</t>
+  </si>
+  <si>
+    <t>Gossypium aridum</t>
+  </si>
+  <si>
+    <t>Gossypium armourianum</t>
+  </si>
+  <si>
+    <t>Gossypium davidsonii</t>
+  </si>
+  <si>
+    <t>Gossypium gossypioides</t>
+  </si>
+  <si>
+    <t>Gossypium harknessii</t>
+  </si>
+  <si>
+    <t>Gossypium klotzschianum</t>
+  </si>
+  <si>
+    <t>Gossypium laxum</t>
+  </si>
+  <si>
+    <t>Gossypium lobatum</t>
+  </si>
+  <si>
+    <t>Gossypium schwendimanii</t>
+  </si>
+  <si>
+    <t>Gossypium stocksii</t>
+  </si>
+  <si>
+    <t>Gossypium trilobum</t>
+  </si>
+  <si>
+    <t>Heliosperma pusillum</t>
+  </si>
+  <si>
+    <t>Herrania umbratica</t>
+  </si>
+  <si>
+    <t>Hevea brasiliensis</t>
+  </si>
+  <si>
+    <t>Impatiens glandulifera</t>
+  </si>
+  <si>
+    <t>Jatropha curcas</t>
+  </si>
+  <si>
+    <t>Kingdonia uniflora</t>
+  </si>
+  <si>
+    <t>Lithospermum erythrorhizon</t>
+  </si>
+  <si>
+    <t>Lolium rigidum</t>
+  </si>
+  <si>
+    <t>Macadamia integrifolia</t>
+  </si>
+  <si>
+    <t>Malus domestica</t>
+  </si>
+  <si>
+    <t>Malus sylvestris</t>
+  </si>
+  <si>
+    <t>Mangifera indica</t>
+  </si>
+  <si>
+    <t>Marchantia paleacea</t>
+  </si>
+  <si>
+    <t>Melastoma candidum</t>
+  </si>
+  <si>
+    <t>Microthlaspi erraticum</t>
+  </si>
+  <si>
+    <t>Miscanthus lutarioriparius</t>
+  </si>
+  <si>
+    <t>Momordica charantia</t>
+  </si>
+  <si>
+    <t>Morus notabilis</t>
+  </si>
+  <si>
+    <t>Musa troglodytarum</t>
+  </si>
+  <si>
+    <t>Nelumbo nucifera</t>
+  </si>
+  <si>
+    <t>Nymphaea thermarum</t>
+  </si>
+  <si>
+    <t>Papaver armeniacum</t>
+  </si>
+  <si>
+    <t>Papaver atlanticum</t>
+  </si>
+  <si>
+    <t>Papaver bracteatum</t>
+  </si>
+  <si>
+    <t>Papaver californicum</t>
+  </si>
+  <si>
+    <t>Paulownia fortunei</t>
+  </si>
+  <si>
+    <t>Perilla frutescens</t>
+  </si>
+  <si>
+    <t>Phtheirospermum japonicum</t>
+  </si>
+  <si>
+    <t>Populus deltoides</t>
+  </si>
+  <si>
+    <t>Populus tomentosa</t>
+  </si>
+  <si>
+    <t>Potentilla anserina</t>
+  </si>
+  <si>
+    <t>Prosopis alba</t>
+  </si>
+  <si>
+    <t>Prunus armeniaca</t>
+  </si>
+  <si>
+    <t>Psidium guajava</t>
+  </si>
+  <si>
+    <t>Punica granatum</t>
+  </si>
+  <si>
+    <t>Quercus robur</t>
+  </si>
+  <si>
+    <t>Rhodamnia argentea</t>
+  </si>
+  <si>
+    <t>Rhododendron griersonianum</t>
+  </si>
+  <si>
+    <t>Rhododendron simsii</t>
+  </si>
+  <si>
+    <t>Salix dunnii</t>
+  </si>
+  <si>
+    <t>Salix suchowensis</t>
+  </si>
+  <si>
+    <t>Salvia hispanica</t>
+  </si>
+  <si>
+    <t>Salvia splendens</t>
+  </si>
+  <si>
+    <t>Senna tora</t>
+  </si>
+  <si>
+    <t>Shorea leprosula</t>
+  </si>
+  <si>
+    <t>Sinapis alba</t>
+  </si>
+  <si>
+    <t>Solanum commersonii</t>
+  </si>
+  <si>
+    <t>Solanum pennellii</t>
+  </si>
+  <si>
+    <t>Solanum stenotomum</t>
+  </si>
+  <si>
+    <t>Spirodela intermedia</t>
+  </si>
+  <si>
+    <t>Striga hermonthica</t>
+  </si>
+  <si>
+    <t>Tarenaya hassleriana</t>
+  </si>
+  <si>
+    <t>Taxus chinensis</t>
+  </si>
+  <si>
+    <t>Telopea speciosissima</t>
+  </si>
+  <si>
+    <t>Tetracentron sinense</t>
+  </si>
+  <si>
+    <t>Thalictrum thalictroides</t>
+  </si>
+  <si>
+    <t>Thlaspi arvense</t>
+  </si>
+  <si>
+    <t>Tripterygium wilfordii</t>
+  </si>
+  <si>
+    <t>Vigna umbellata</t>
+  </si>
+  <si>
+    <t>Vitis riparia</t>
+  </si>
+  <si>
+    <t>Xanthoceras sorbifolium</t>
+  </si>
+  <si>
+    <t>Zingiber officinale</t>
+  </si>
+  <si>
+    <t>Zizania palustris</t>
+  </si>
+  <si>
+    <t>Ziziphus jujuba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="&quot;''&quot;@&quot;''&quot;\,"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1498,7 +1853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1528,6 +1883,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1809,10 +2165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I200"/>
+  <dimension ref="A1:I317"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B210" sqref="B210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,10 +2192,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>66</v>
@@ -1848,10 +2204,10 @@
         <v>210</v>
       </c>
       <c r="H1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1865,10 +2221,10 @@
         <v>135</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>454</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="11">
@@ -1878,21 +2234,21 @@
         <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>459</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>461</v>
       </c>
       <c r="G3" s="13"/>
     </row>
@@ -1918,10 +2274,10 @@
         <v>138</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="11">
@@ -1931,7 +2287,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1956,10 +2312,10 @@
         <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="11">
@@ -1969,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1977,13 +2333,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="11">
@@ -1993,7 +2349,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2001,13 +2357,13 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2015,16 +2371,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="11">
@@ -2034,7 +2390,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2097,16 +2453,16 @@
         <v>72</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>149</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G16" s="11">
         <v>597</v>
@@ -2115,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2140,11 +2496,11 @@
         <v>169</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G18" s="11">
         <v>467</v>
@@ -2153,7 +2509,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2175,16 +2531,16 @@
         <v>128</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>454</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>285</v>
       </c>
       <c r="G20" s="11">
         <v>56</v>
@@ -2193,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -2207,7 +2563,7 @@
         <v>62</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -2218,7 +2574,7 @@
         <v>153</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2254,7 +2610,7 @@
         <v>157</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>159</v>
@@ -2266,7 +2622,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2280,7 +2636,7 @@
         <v>157</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>159</v>
@@ -2292,7 +2648,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2311,13 +2667,13 @@
         <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>159</v>
@@ -2329,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2356,16 +2712,16 @@
         <v>50</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G31" s="11">
         <v>52</v>
@@ -2374,7 +2730,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2410,10 +2766,10 @@
         <v>171</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G34" s="11">
         <v>296</v>
@@ -2422,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2436,10 +2792,10 @@
         <v>174</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G35" s="11">
         <v>3171</v>
@@ -2448,7 +2804,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2473,7 +2829,7 @@
         <v>43</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G37" s="11">
         <v>337</v>
@@ -2482,7 +2838,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -2493,7 +2849,7 @@
         <v>136</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2538,7 +2894,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2654,13 +3010,13 @@
         <v>45</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G51" s="11">
         <v>1674</v>
@@ -2669,7 +3025,7 @@
         <v>1</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -2677,13 +3033,13 @@
         <v>45</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G52" s="11">
         <v>240</v>
@@ -2694,13 +3050,13 @@
         <v>45</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="F53" s="8" t="s">
         <v>290</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>292</v>
       </c>
       <c r="G53" s="11">
         <v>279</v>
@@ -2717,7 +3073,7 @@
         <v>47</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2731,10 +3087,10 @@
         <v>183</v>
       </c>
       <c r="D55" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="E55" s="9" t="s">
         <v>454</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>456</v>
       </c>
       <c r="F55" s="8"/>
       <c r="G55" s="11">
@@ -2744,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2765,7 +3121,7 @@
         <v>1</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2784,10 +3140,10 @@
         <v>112</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F58" s="8"/>
       <c r="G58" s="11">
@@ -2797,7 +3153,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2810,7 +3166,7 @@
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2878,7 +3234,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2903,7 +3259,7 @@
         <v>189</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G66" s="11">
         <v>131</v>
@@ -2912,7 +3268,7 @@
         <v>1</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -2948,13 +3304,13 @@
         <v>99</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C69" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="F69" s="8" t="s">
         <v>306</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>308</v>
       </c>
       <c r="G69" s="11">
         <v>200</v>
@@ -2963,7 +3319,7 @@
         <v>1</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3002,7 +3358,7 @@
         <v>198</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G72" s="11">
         <v>136</v>
@@ -3011,7 +3367,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3030,13 +3386,13 @@
         <v>100</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>201</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G74" s="11">
         <v>44</v>
@@ -3045,7 +3401,7 @@
         <v>1</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3064,10 +3420,10 @@
         <v>67</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F76" s="8" t="s">
         <v>159</v>
@@ -3079,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -3090,10 +3446,10 @@
         <v>202</v>
       </c>
       <c r="C77" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3107,7 +3463,7 @@
         <v>195</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3118,10 +3474,10 @@
         <v>20</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G79" s="11">
         <v>38</v>
@@ -3130,7 +3486,7 @@
         <v>1</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3177,7 +3533,7 @@
         <v>205</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G83" s="11">
         <v>52</v>
@@ -3186,7 +3542,7 @@
         <v>1</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3225,7 +3581,7 @@
         <v>4</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G86" s="12">
         <v>3024</v>
@@ -3234,7 +3590,7 @@
         <v>1</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="87" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -3248,7 +3604,7 @@
         <v>47</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G87" s="11">
         <v>85</v>
@@ -3257,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3265,13 +3621,13 @@
         <v>130</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>209</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G88" s="11">
         <v>747</v>
@@ -3280,7 +3636,7 @@
         <v>1</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
@@ -3312,7 +3668,7 @@
         <v>1</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3337,7 +3693,7 @@
         <v>56</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G92" s="11">
         <v>52</v>
@@ -3346,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3398,7 +3754,7 @@
         <v>211</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G97" s="11">
         <v>428</v>
@@ -3407,7 +3763,7 @@
         <v>1</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -3448,13 +3804,13 @@
         <v>131</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F101" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G101" s="11">
         <v>909</v>
@@ -3463,7 +3819,7 @@
         <v>1</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="102" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3471,13 +3827,13 @@
         <v>132</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F102" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G102" s="11">
         <v>38</v>
@@ -3486,7 +3842,7 @@
         <v>1</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -3502,7 +3858,7 @@
         <v>18</v>
       </c>
       <c r="C104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F104" s="7" t="s">
         <v>145</v>
@@ -3513,10 +3869,10 @@
         <v>18</v>
       </c>
       <c r="B105" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>220</v>
       </c>
       <c r="F105" s="8" t="s">
         <v>159</v>
@@ -3528,7 +3884,7 @@
         <v>1</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -3536,10 +3892,10 @@
         <v>79</v>
       </c>
       <c r="C106" t="s">
+        <v>221</v>
+      </c>
+      <c r="F106" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="F106" s="7" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -3561,13 +3917,13 @@
         <v>31</v>
       </c>
       <c r="B108" t="s">
+        <v>224</v>
+      </c>
+      <c r="C108" t="s">
+        <v>223</v>
+      </c>
+      <c r="F108" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="C108" t="s">
-        <v>224</v>
-      </c>
-      <c r="F108" s="7" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="109" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3575,10 +3931,10 @@
         <v>31</v>
       </c>
       <c r="B109" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>227</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="F109" s="8" t="s">
         <v>159</v>
@@ -3590,7 +3946,7 @@
         <v>1</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="110" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3598,13 +3954,13 @@
         <v>75</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G110" s="11">
         <v>296</v>
@@ -3613,7 +3969,7 @@
         <v>1</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="111" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3621,13 +3977,13 @@
         <v>123</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F111" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G111" s="11">
         <v>36</v>
@@ -3636,7 +3992,7 @@
         <v>1</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -3669,7 +4025,7 @@
         <v>95</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="115" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3677,13 +4033,13 @@
         <v>23</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G115" s="11">
         <v>786</v>
@@ -3692,7 +4048,7 @@
         <v>1</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="116" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3700,16 +4056,16 @@
         <v>32</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G116" s="11">
         <v>114</v>
@@ -3718,7 +4074,7 @@
         <v>1</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -3756,13 +4112,13 @@
         <v>10</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F120" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="G120" s="11">
         <v>117</v>
@@ -3771,7 +4127,7 @@
         <v>1</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -3795,13 +4151,13 @@
         <v>9</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F123" s="8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G123" s="11">
         <v>33</v>
@@ -3810,7 +4166,7 @@
         <v>1</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="124" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3821,7 +4177,7 @@
         <v>7</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G124" s="11"/>
     </row>
@@ -3854,10 +4210,10 @@
         <v>124</v>
       </c>
       <c r="C127" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F127" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="128" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3865,13 +4221,13 @@
         <v>160</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F128" s="8"/>
       <c r="G128" s="11">
@@ -3881,7 +4237,7 @@
         <v>1</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -3900,24 +4256,24 @@
     </row>
     <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>310</v>
+      </c>
+      <c r="F130" s="7" t="s">
         <v>312</v>
-      </c>
-      <c r="F130" s="7" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="131" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C131" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="B131" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>317</v>
-      </c>
       <c r="D131" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F131" s="8"/>
       <c r="G131" s="11">
@@ -3927,21 +4283,21 @@
         <v>1</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="132" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B132" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B132" s="3" t="s">
-        <v>320</v>
-      </c>
       <c r="C132" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D132" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>323</v>
       </c>
       <c r="F132" s="8"/>
       <c r="G132" s="11">
@@ -3951,21 +4307,21 @@
         <v>1</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="133" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F133" s="8"/>
       <c r="G133" s="11">
@@ -3975,24 +4331,24 @@
         <v>1</v>
       </c>
       <c r="I133" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B134" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F134" s="8" t="s">
         <v>326</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F134" s="8" t="s">
-        <v>328</v>
       </c>
       <c r="G134" s="11">
         <v>10</v>
@@ -4001,35 +4357,35 @@
         <v>1</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D135" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="136" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B136" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="B136" s="3" t="s">
-        <v>333</v>
-      </c>
       <c r="C136" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F136" s="8" t="s">
         <v>332</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F136" s="8" t="s">
-        <v>334</v>
       </c>
       <c r="G136" s="11">
         <v>135</v>
@@ -4038,24 +4394,24 @@
         <v>1</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="137" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B137" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="B137" s="3" t="s">
-        <v>337</v>
-      </c>
       <c r="C137" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G137" s="11">
         <v>7</v>
@@ -4064,15 +4420,15 @@
         <v>1</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D138" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F138" s="7" t="s">
         <v>137</v>
@@ -4080,35 +4436,35 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F139" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="141" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F141" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F141" s="8" t="s">
-        <v>348</v>
       </c>
       <c r="G141" s="11">
         <v>34</v>
@@ -4117,12 +4473,12 @@
         <v>1</v>
       </c>
       <c r="I141" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F142" s="7" t="s">
         <v>137</v>
@@ -4130,10 +4486,10 @@
     </row>
     <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F143" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -4141,21 +4497,21 @@
         <v>98</v>
       </c>
       <c r="F144" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="145" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="B145" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>355</v>
-      </c>
       <c r="D145" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F145" s="8"/>
       <c r="G145" s="11">
@@ -4165,43 +4521,43 @@
         <v>1</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D146" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F146" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D147" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F147" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="148" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F148" s="8"/>
       <c r="G148" s="11">
@@ -4211,65 +4567,65 @@
         <v>1</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D149" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F149" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D150" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F150" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D151" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F151" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D152" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F152" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="153" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B153" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F153" s="8" t="s">
         <v>367</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F153" s="8" t="s">
-        <v>369</v>
       </c>
       <c r="G153" s="11">
         <v>14</v>
@@ -4278,37 +4634,37 @@
         <v>1</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F154" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F155" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="156" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C156" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="B156" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>375</v>
-      </c>
       <c r="D156" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F156" s="8"/>
       <c r="G156" s="11">
@@ -4318,43 +4674,43 @@
         <v>1</v>
       </c>
       <c r="I156" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D157" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F157" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D158" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F158" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="159" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B159" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="B159" s="3" t="s">
-        <v>380</v>
-      </c>
       <c r="C159" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F159" s="8"/>
       <c r="G159" s="11">
@@ -4364,37 +4720,37 @@
         <v>1</v>
       </c>
       <c r="I159" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F160" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F161" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="162" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F162" s="8"/>
       <c r="G162" s="11">
@@ -4404,38 +4760,38 @@
         <v>1</v>
       </c>
       <c r="I162" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>381</v>
+      </c>
+      <c r="B163" t="s">
         <v>383</v>
       </c>
-      <c r="B163" t="s">
-        <v>385</v>
-      </c>
       <c r="C163" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D163" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F163" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="164" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C164" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D164" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="F164" s="14" t="s">
         <v>386</v>
-      </c>
-      <c r="D164" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="F164" s="14" t="s">
-        <v>388</v>
       </c>
       <c r="G164" s="13">
         <v>16</v>
@@ -4444,18 +4800,18 @@
         <v>1</v>
       </c>
       <c r="I164" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="165" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C165" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>392</v>
       </c>
       <c r="F165" s="8"/>
       <c r="G165" s="11">
@@ -4465,21 +4821,21 @@
         <v>1</v>
       </c>
       <c r="I165" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="166" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F166" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G166" s="13">
         <v>21</v>
@@ -4488,21 +4844,21 @@
         <v>1</v>
       </c>
       <c r="I166" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="167" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C167" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D167" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F167" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G167" s="13">
         <v>18</v>
@@ -4511,21 +4867,21 @@
         <v>1</v>
       </c>
       <c r="I167" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="168" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F168" s="14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G168" s="13">
         <v>19</v>
@@ -4534,32 +4890,32 @@
         <v>1</v>
       </c>
       <c r="I168" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D169" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F169" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="170" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="F170" s="14" t="s">
         <v>401</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="D170" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="F170" s="14" t="s">
-        <v>403</v>
       </c>
       <c r="G170" s="13">
         <v>10</v>
@@ -4568,24 +4924,24 @@
         <v>1</v>
       </c>
       <c r="I170" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F171" s="8" t="s">
         <v>405</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="D171" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F171" s="8" t="s">
-        <v>407</v>
       </c>
       <c r="G171" s="11">
         <v>445</v>
@@ -4594,53 +4950,53 @@
         <v>1</v>
       </c>
       <c r="I171" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F172" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F173" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F174" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F175" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="176" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F176" s="8" t="s">
         <v>414</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="D176" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F176" s="8" t="s">
-        <v>416</v>
       </c>
       <c r="G176" s="11">
         <v>27</v>
@@ -4649,24 +5005,24 @@
         <v>1</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="177" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C177" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="B177" s="3" t="s">
+      <c r="D177" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F177" s="8" t="s">
         <v>418</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D177" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F177" s="8" t="s">
-        <v>420</v>
       </c>
       <c r="G177" s="11">
         <v>299</v>
@@ -4675,32 +5031,32 @@
         <v>1</v>
       </c>
       <c r="I177" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>419</v>
+      </c>
+      <c r="C178" t="s">
+        <v>420</v>
+      </c>
+      <c r="F178" s="7" t="s">
         <v>421</v>
-      </c>
-      <c r="C178" t="s">
-        <v>422</v>
-      </c>
-      <c r="F178" s="7" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="179" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C179" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F179" s="8" t="s">
         <v>424</v>
-      </c>
-      <c r="D179" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F179" s="8" t="s">
-        <v>426</v>
       </c>
       <c r="G179" s="11">
         <v>160</v>
@@ -4709,56 +5065,56 @@
         <v>1</v>
       </c>
       <c r="I179" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F180" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F181" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F182" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F183" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="184" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C184" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="B184" s="3" t="s">
+      <c r="D184" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F184" s="8" t="s">
         <v>434</v>
-      </c>
-      <c r="C184" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="D184" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F184" s="8" t="s">
-        <v>436</v>
       </c>
       <c r="G184" s="11">
         <v>705</v>
@@ -4767,53 +5123,53 @@
         <v>1</v>
       </c>
       <c r="I184" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F185" s="7" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
+        <v>437</v>
+      </c>
+      <c r="C186" t="s">
+        <v>438</v>
+      </c>
+      <c r="F186" s="7" t="s">
         <v>439</v>
-      </c>
-      <c r="C186" t="s">
-        <v>440</v>
-      </c>
-      <c r="F186" s="7" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F187" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F188" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="189" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F189" s="8"/>
       <c r="G189" s="11">
@@ -4823,7 +5179,7 @@
         <v>1</v>
       </c>
       <c r="I189" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4831,10 +5187,10 @@
         <v>97</v>
       </c>
       <c r="C190" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F190" s="7" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4842,10 +5198,10 @@
         <v>97</v>
       </c>
       <c r="B191" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F191" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="192" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4853,13 +5209,13 @@
         <v>97</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C192" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F192" s="8" t="s">
         <v>451</v>
-      </c>
-      <c r="F192" s="8" t="s">
-        <v>453</v>
       </c>
       <c r="G192" s="11">
         <v>37</v>
@@ -4868,10 +5224,10 @@
         <v>1</v>
       </c>
       <c r="I192" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>164</v>
       </c>
@@ -4885,7 +5241,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>168</v>
       </c>
@@ -4896,60 +5252,1007 @@
         <v>163</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>244</v>
-      </c>
-      <c r="B195" t="s">
-        <v>245</v>
-      </c>
-      <c r="F195" s="7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F195" s="8"/>
+      <c r="G195" s="11">
+        <v>157</v>
+      </c>
+      <c r="H195" s="3">
+        <v>1</v>
+      </c>
+      <c r="I195" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>264</v>
+        <v>242</v>
+      </c>
+      <c r="B196" t="s">
+        <v>243</v>
       </c>
       <c r="F196" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F197" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>39</v>
-      </c>
-      <c r="C198" t="s">
-        <v>40</v>
+        <v>263</v>
       </c>
       <c r="F198" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G199" s="13">
-        <f>SUM(G2:G194)</f>
-        <v>27449</v>
-      </c>
-      <c r="H199" s="5" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G200" s="13">
-        <f>SUM(H2:H194)</f>
-        <v>71</v>
-      </c>
-      <c r="H200" s="5" t="s">
-        <v>239</v>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>39</v>
+      </c>
+      <c r="C199" t="s">
+        <v>40</v>
+      </c>
+      <c r="F199" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>463</v>
+      </c>
+      <c r="D200" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>464</v>
+      </c>
+      <c r="D201" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>465</v>
+      </c>
+      <c r="D202" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>466</v>
+      </c>
+      <c r="D203" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>467</v>
+      </c>
+      <c r="D204" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>468</v>
+      </c>
+      <c r="D205" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>469</v>
+      </c>
+      <c r="D206" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>470</v>
+      </c>
+      <c r="D207" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>471</v>
+      </c>
+      <c r="D208" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>472</v>
+      </c>
+      <c r="D209" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>473</v>
+      </c>
+      <c r="D210" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>474</v>
+      </c>
+      <c r="D211" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>475</v>
+      </c>
+      <c r="D212" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>476</v>
+      </c>
+      <c r="D213" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>477</v>
+      </c>
+      <c r="D214" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>478</v>
+      </c>
+      <c r="D215" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>479</v>
+      </c>
+      <c r="D216" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>480</v>
+      </c>
+      <c r="D217" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>481</v>
+      </c>
+      <c r="D218" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>482</v>
+      </c>
+      <c r="D219" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>483</v>
+      </c>
+      <c r="D220" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>484</v>
+      </c>
+      <c r="D221" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>485</v>
+      </c>
+      <c r="D222" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>486</v>
+      </c>
+      <c r="D223" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>487</v>
+      </c>
+      <c r="D224" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>488</v>
+      </c>
+      <c r="D225" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>489</v>
+      </c>
+      <c r="D226" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>490</v>
+      </c>
+      <c r="D227" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>491</v>
+      </c>
+      <c r="D228" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>492</v>
+      </c>
+      <c r="D229" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>493</v>
+      </c>
+      <c r="D230" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>494</v>
+      </c>
+      <c r="D231" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>495</v>
+      </c>
+      <c r="D232" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>496</v>
+      </c>
+      <c r="D233" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>497</v>
+      </c>
+      <c r="D234" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>498</v>
+      </c>
+      <c r="D235" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>499</v>
+      </c>
+      <c r="D236" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>500</v>
+      </c>
+      <c r="D237" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>501</v>
+      </c>
+      <c r="D238" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>502</v>
+      </c>
+      <c r="D239" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>503</v>
+      </c>
+      <c r="D240" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>504</v>
+      </c>
+      <c r="D241" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>505</v>
+      </c>
+      <c r="D242" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>506</v>
+      </c>
+      <c r="D243" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>507</v>
+      </c>
+      <c r="D244" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>508</v>
+      </c>
+      <c r="D245" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>509</v>
+      </c>
+      <c r="D246" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>510</v>
+      </c>
+      <c r="D247" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>511</v>
+      </c>
+      <c r="D248" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>512</v>
+      </c>
+      <c r="D249" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>513</v>
+      </c>
+      <c r="D250" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>514</v>
+      </c>
+      <c r="D251" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>515</v>
+      </c>
+      <c r="D252" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>516</v>
+      </c>
+      <c r="D253" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>517</v>
+      </c>
+      <c r="D254" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>518</v>
+      </c>
+      <c r="D255" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>519</v>
+      </c>
+      <c r="D256" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>520</v>
+      </c>
+      <c r="D257" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>521</v>
+      </c>
+      <c r="D258" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>522</v>
+      </c>
+      <c r="D259" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>523</v>
+      </c>
+      <c r="D260" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>524</v>
+      </c>
+      <c r="D261" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>525</v>
+      </c>
+      <c r="D262" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>526</v>
+      </c>
+      <c r="D263" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>527</v>
+      </c>
+      <c r="D264" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>528</v>
+      </c>
+      <c r="D265" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>529</v>
+      </c>
+      <c r="D266" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>530</v>
+      </c>
+      <c r="D267" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>531</v>
+      </c>
+      <c r="D268" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>532</v>
+      </c>
+      <c r="D269" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>533</v>
+      </c>
+      <c r="D270" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>534</v>
+      </c>
+      <c r="D271" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>535</v>
+      </c>
+      <c r="D272" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>536</v>
+      </c>
+      <c r="D273" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>537</v>
+      </c>
+      <c r="D274" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>538</v>
+      </c>
+      <c r="D275" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>539</v>
+      </c>
+      <c r="D276" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>540</v>
+      </c>
+      <c r="D277" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>541</v>
+      </c>
+      <c r="D278" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>542</v>
+      </c>
+      <c r="D279" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>543</v>
+      </c>
+      <c r="D280" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>544</v>
+      </c>
+      <c r="D281" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>545</v>
+      </c>
+      <c r="D282" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>546</v>
+      </c>
+      <c r="D283" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>547</v>
+      </c>
+      <c r="D284" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>548</v>
+      </c>
+      <c r="D285" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>549</v>
+      </c>
+      <c r="D286" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>550</v>
+      </c>
+      <c r="D287" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>551</v>
+      </c>
+      <c r="D288" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>552</v>
+      </c>
+      <c r="D289" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>553</v>
+      </c>
+      <c r="D290" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>554</v>
+      </c>
+      <c r="D291" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>555</v>
+      </c>
+      <c r="D292" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>556</v>
+      </c>
+      <c r="D293" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>557</v>
+      </c>
+      <c r="D294" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>558</v>
+      </c>
+      <c r="D295" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>559</v>
+      </c>
+      <c r="D296" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>560</v>
+      </c>
+      <c r="D297" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>561</v>
+      </c>
+      <c r="D298" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>562</v>
+      </c>
+      <c r="D299" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>563</v>
+      </c>
+      <c r="D300" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>564</v>
+      </c>
+      <c r="D301" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>565</v>
+      </c>
+      <c r="D302" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>566</v>
+      </c>
+      <c r="D303" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>567</v>
+      </c>
+      <c r="D304" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>568</v>
+      </c>
+      <c r="D305" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>569</v>
+      </c>
+      <c r="D306" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>570</v>
+      </c>
+      <c r="D307" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>571</v>
+      </c>
+      <c r="D308" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>572</v>
+      </c>
+      <c r="D309" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>262</v>
+      </c>
+      <c r="D310" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>573</v>
+      </c>
+      <c r="D311" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>574</v>
+      </c>
+      <c r="D312" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>575</v>
+      </c>
+      <c r="D313" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>576</v>
+      </c>
+      <c r="D314" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>577</v>
+      </c>
+      <c r="D315" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>578</v>
+      </c>
+      <c r="D316" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D317" t="s">
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -4968,4 +6271,813 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA0D188-8CB9-4E9E-A4CF-6AB440175DE3}">
+  <dimension ref="A1:A158"/>
+  <sheetViews>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A56" sqref="A1:A158"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="15" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="15" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="15" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="15" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="15" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="15" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="15" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="15" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="15" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="15" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="15" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="15" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="15" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="15" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="15" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="15" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="15" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="15" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="15" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="15" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="15" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="15" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="15" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="15" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="15" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="15" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="15" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="15" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="15" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="15" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="15" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="15" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="15" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="15" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="15" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="15" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="15" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="15" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="15" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="15" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="15" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="15" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="15" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="15" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="15" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
quickly scan NCBI species for available datasets
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\1771458_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/525510_2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC19667-8114-4598-AE0C-92806505D2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{21C4D0B7-59BC-47B8-AA0A-8F4F599772A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4897AA6F-08FB-4F1F-8A35-A95848072406}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="613">
   <si>
     <t>Species</t>
   </si>
@@ -1774,6 +1774,108 @@
   </si>
   <si>
     <t>Ziziphus jujuba</t>
+  </si>
+  <si>
+    <t>RAD-seq data, but no WGS data in SRA</t>
+  </si>
+  <si>
+    <t>PRJNA309929</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/molbev/msw299</t>
+  </si>
+  <si>
+    <t>PRJEB39992</t>
+  </si>
+  <si>
+    <t>Maybe works, not sure if WGS</t>
+  </si>
+  <si>
+    <t>PRJNA525866</t>
+  </si>
+  <si>
+    <t>Maybe works</t>
+  </si>
+  <si>
+    <t>found only 1 WGS sample</t>
+  </si>
+  <si>
+    <t>PRJNA576075</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41467-019-13185-3</t>
+  </si>
+  <si>
+    <t>PRJNA577174</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/nph.17637</t>
+  </si>
+  <si>
+    <t>A lot of data, need to look at more closely</t>
+  </si>
+  <si>
+    <t>PRJNA506619</t>
+  </si>
+  <si>
+    <t>Maybe some data, need to look at more closely</t>
+  </si>
+  <si>
+    <t>PRJNA485527</t>
+  </si>
+  <si>
+    <t>PRJNA797700</t>
+  </si>
+  <si>
+    <t>don't think there's data, might need to confirm</t>
+  </si>
+  <si>
+    <t>PRJNA515691</t>
+  </si>
+  <si>
+    <t>RAD-seq data, but no WGS</t>
+  </si>
+  <si>
+    <t>PRJEB58004</t>
+  </si>
+  <si>
+    <t>PRJNA909356</t>
+  </si>
+  <si>
+    <t>PRJNA322175</t>
+  </si>
+  <si>
+    <t>maybe works</t>
+  </si>
+  <si>
+    <t>maybe some data</t>
+  </si>
+  <si>
+    <t>PRJNA565883</t>
+  </si>
+  <si>
+    <t>PRJNA659608</t>
+  </si>
+  <si>
+    <t>maybe the same as brassica napus?</t>
+  </si>
+  <si>
+    <t>PRJNA801489</t>
+  </si>
+  <si>
+    <t>I think I found some data, but its not public</t>
+  </si>
+  <si>
+    <t>PRJNA625382</t>
+  </si>
+  <si>
+    <t>PRJNA439007</t>
+  </si>
+  <si>
+    <t>GBS data, but no WGS data</t>
+  </si>
+  <si>
+    <t>PRJNA803965</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1883,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="&quot;''&quot;@&quot;''&quot;\,"/>
+    <numFmt numFmtId="164" formatCode="&quot;''&quot;@&quot;''&quot;\,"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1883,7 +1985,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2165,10 +2267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I317"/>
+  <dimension ref="A1:I316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B210" sqref="B210"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5321,6 +5423,9 @@
       <c r="D200" t="s">
         <v>462</v>
       </c>
+      <c r="F200" s="7" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
@@ -5329,6 +5434,9 @@
       <c r="D201" t="s">
         <v>462</v>
       </c>
+      <c r="F201" s="7" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
@@ -5337,6 +5445,9 @@
       <c r="D202" t="s">
         <v>462</v>
       </c>
+      <c r="F202" s="7" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
@@ -5345,11 +5456,20 @@
       <c r="D203" t="s">
         <v>462</v>
       </c>
+      <c r="F203" s="7" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>467</v>
       </c>
+      <c r="B204" t="s">
+        <v>581</v>
+      </c>
+      <c r="C204" t="s">
+        <v>580</v>
+      </c>
       <c r="D204" t="s">
         <v>462</v>
       </c>
@@ -5358,24 +5478,42 @@
       <c r="A205" t="s">
         <v>468</v>
       </c>
+      <c r="C205" t="s">
+        <v>582</v>
+      </c>
       <c r="D205" t="s">
         <v>462</v>
+      </c>
+      <c r="F205" s="7" t="s">
+        <v>583</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>469</v>
       </c>
+      <c r="C206" t="s">
+        <v>584</v>
+      </c>
       <c r="D206" t="s">
         <v>462</v>
+      </c>
+      <c r="F206" s="7" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>470</v>
       </c>
+      <c r="C207" t="s">
+        <v>584</v>
+      </c>
       <c r="D207" t="s">
         <v>462</v>
+      </c>
+      <c r="F207" s="7" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -5385,874 +5523,1238 @@
       <c r="D208" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F208" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>472</v>
       </c>
       <c r="D209" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F209" s="7" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>473</v>
       </c>
+      <c r="B210" t="s">
+        <v>588</v>
+      </c>
+      <c r="C210" t="s">
+        <v>587</v>
+      </c>
       <c r="D210" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>474</v>
       </c>
       <c r="D211" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F211" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>475</v>
       </c>
+      <c r="B212" t="s">
+        <v>590</v>
+      </c>
+      <c r="C212" t="s">
+        <v>589</v>
+      </c>
       <c r="D212" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>476</v>
       </c>
       <c r="D213" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F213" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>477</v>
       </c>
       <c r="D214" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F214" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>478</v>
       </c>
       <c r="D215" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F215" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>479</v>
       </c>
       <c r="D216" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F216" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>480</v>
       </c>
       <c r="D217" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F217" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>481</v>
       </c>
+      <c r="C218" t="s">
+        <v>592</v>
+      </c>
       <c r="D218" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F218" s="7" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>482</v>
       </c>
       <c r="D219" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F219" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>483</v>
       </c>
       <c r="D220" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F220" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>484</v>
       </c>
       <c r="D221" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F221" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>485</v>
       </c>
+      <c r="C222" t="s">
+        <v>594</v>
+      </c>
       <c r="D222" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F222" s="7" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>486</v>
       </c>
+      <c r="C223" t="s">
+        <v>595</v>
+      </c>
       <c r="D223" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F223" s="7" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>487</v>
       </c>
       <c r="D224" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F224" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>488</v>
       </c>
       <c r="D225" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F225" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>489</v>
       </c>
       <c r="D226" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F226" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>490</v>
       </c>
       <c r="D227" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F227" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>491</v>
       </c>
       <c r="D228" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F228" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>492</v>
       </c>
       <c r="D229" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F229" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>493</v>
       </c>
       <c r="D230" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F230" s="7" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>494</v>
       </c>
+      <c r="C231" t="s">
+        <v>597</v>
+      </c>
       <c r="D231" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F231" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>495</v>
       </c>
       <c r="D232" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F232" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>496</v>
       </c>
       <c r="D233" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F233" s="7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>497</v>
       </c>
       <c r="D234" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F234" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>498</v>
       </c>
       <c r="D235" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F235" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>499</v>
       </c>
+      <c r="C236" t="s">
+        <v>599</v>
+      </c>
       <c r="D236" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F236" s="7" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>500</v>
       </c>
       <c r="D237" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F237" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>501</v>
       </c>
       <c r="D238" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F238" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>502</v>
       </c>
       <c r="D239" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F239" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>503</v>
       </c>
       <c r="D240" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F240" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>504</v>
       </c>
       <c r="D241" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F241" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>505</v>
       </c>
       <c r="D242" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F242" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>506</v>
       </c>
       <c r="D243" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F243" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>507</v>
       </c>
       <c r="D244" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F244" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>508</v>
       </c>
       <c r="D245" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F245" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>509</v>
       </c>
       <c r="D246" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F246" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>510</v>
       </c>
       <c r="D247" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F247" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>511</v>
       </c>
       <c r="D248" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F248" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>512</v>
       </c>
       <c r="D249" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F249" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>513</v>
       </c>
       <c r="D250" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F250" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>514</v>
       </c>
       <c r="D251" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F251" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>515</v>
       </c>
       <c r="D252" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F252" s="7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>516</v>
       </c>
       <c r="D253" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F253" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>517</v>
       </c>
       <c r="D254" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F254" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>518</v>
       </c>
       <c r="D255" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F255" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>519</v>
       </c>
       <c r="D256" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F256" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>520</v>
       </c>
       <c r="D257" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F257" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>521</v>
       </c>
       <c r="D258" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F258" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>522</v>
       </c>
       <c r="D259" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F259" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>523</v>
       </c>
+      <c r="C260" t="s">
+        <v>600</v>
+      </c>
       <c r="D260" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>524</v>
       </c>
       <c r="D261" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F261" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>525</v>
       </c>
+      <c r="C262" t="s">
+        <v>601</v>
+      </c>
       <c r="D262" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F262" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>526</v>
       </c>
       <c r="D263" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F263" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>527</v>
       </c>
       <c r="D264" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F264" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>528</v>
       </c>
       <c r="D265" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F265" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>529</v>
       </c>
       <c r="D266" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F266" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>530</v>
       </c>
       <c r="D267" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F267" s="7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>531</v>
       </c>
       <c r="D268" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F268" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>532</v>
       </c>
       <c r="D269" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F269" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>533</v>
       </c>
       <c r="D270" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F270" s="7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>534</v>
       </c>
       <c r="D271" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F271" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>535</v>
       </c>
       <c r="D272" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F272" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>536</v>
       </c>
       <c r="D273" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F273" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>537</v>
       </c>
       <c r="D274" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F274" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>538</v>
       </c>
       <c r="D275" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F275" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>539</v>
       </c>
       <c r="D276" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F276" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>540</v>
       </c>
       <c r="D277" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F277" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>541</v>
       </c>
       <c r="D278" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F278" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>542</v>
       </c>
       <c r="D279" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F279" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>543</v>
       </c>
       <c r="D280" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F280" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>544</v>
       </c>
       <c r="D281" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F281" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>545</v>
       </c>
       <c r="D282" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F282" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>546</v>
       </c>
       <c r="D283" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F283" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>547</v>
       </c>
       <c r="D284" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F284" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>548</v>
       </c>
+      <c r="C285" t="s">
+        <v>604</v>
+      </c>
       <c r="D285" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F285" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>549</v>
       </c>
       <c r="D286" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F286" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>550</v>
       </c>
       <c r="D287" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F287" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>551</v>
       </c>
       <c r="D288" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F288" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>552</v>
       </c>
+      <c r="C289" t="s">
+        <v>605</v>
+      </c>
       <c r="D289" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F289" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>553</v>
       </c>
       <c r="D290" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F290" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>554</v>
       </c>
       <c r="D291" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F291" s="7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>555</v>
       </c>
       <c r="D292" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F292" s="7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>556</v>
       </c>
       <c r="D293" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F293" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>557</v>
       </c>
       <c r="D294" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F294" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>558</v>
       </c>
       <c r="D295" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F295" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>559</v>
       </c>
       <c r="D296" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F296" s="7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>560</v>
       </c>
       <c r="D297" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F297" s="7" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>561</v>
       </c>
       <c r="D298" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F298" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>562</v>
       </c>
       <c r="D299" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F299" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>563</v>
       </c>
       <c r="D300" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F300" s="7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>564</v>
       </c>
       <c r="D301" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F301" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>565</v>
       </c>
+      <c r="C302" t="s">
+        <v>607</v>
+      </c>
       <c r="D302" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F302" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>566</v>
       </c>
       <c r="D303" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F303" s="7" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>567</v>
       </c>
       <c r="D304" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F304" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>568</v>
       </c>
       <c r="D305" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F305" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>569</v>
       </c>
+      <c r="C306" t="s">
+        <v>609</v>
+      </c>
       <c r="D306" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F306" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>570</v>
       </c>
+      <c r="C307" t="s">
+        <v>610</v>
+      </c>
       <c r="D307" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F307" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>571</v>
       </c>
       <c r="D308" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F308" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>572</v>
       </c>
       <c r="D309" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F309" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>262</v>
       </c>
       <c r="D310" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F310" s="7" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>573</v>
       </c>
+      <c r="C311" t="s">
+        <v>612</v>
+      </c>
       <c r="D311" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F311" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>574</v>
       </c>
       <c r="D312" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F312" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>575</v>
       </c>
       <c r="D313" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F313" s="7" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>576</v>
       </c>
       <c r="D314" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F314" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>577</v>
       </c>
       <c r="D315" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F315" s="7" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>578</v>
       </c>
       <c r="D316" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D317" t="s">
-        <v>462</v>
+      <c r="F316" s="7" t="s">
+        <v>591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add read metadata for NCBI species
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/525510_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\7931372_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{21C4D0B7-59BC-47B8-AA0A-8F4F599772A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4897AA6F-08FB-4F1F-8A35-A95848072406}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645F8A15-B977-43BD-965E-0F11E2676A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="620">
   <si>
     <t>Species</t>
   </si>
@@ -1876,6 +1876,27 @@
   </si>
   <si>
     <t>PRJNA803965</t>
+  </si>
+  <si>
+    <t>I can't find a source because it looks like the data was published only recently</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41467-017-00336-7</t>
+  </si>
+  <si>
+    <t>I think this is GBS data, not WGS</t>
+  </si>
+  <si>
+    <t>WGS data from QTL study, so data comes from F2 population, not a natural population. Thus, data is not relevant to my study</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.16086</t>
+  </si>
+  <si>
+    <t>Maybe some data, need to look at more closely, also includes Musa acuminata, only contains one sample of Ensete ventricosum, but about 48 samples of Musa acuminata!</t>
+  </si>
+  <si>
+    <t>no WGS data on SRA, only GBS and RAD-seq, but while searching SRA for wild banana reads later I found some Musa acuminata data!</t>
   </si>
 </sst>
 </file>
@@ -2269,8 +2290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I316"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="C200" sqref="C200"/>
+    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
+      <selection activeCell="F321" sqref="F321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3602,15 +3623,27 @@
         <v>203</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C81" t="s">
-        <v>136</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>203</v>
+      <c r="B81" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>619</v>
+      </c>
+      <c r="G81" s="11">
+        <v>48</v>
+      </c>
+      <c r="H81" s="3">
+        <v>1</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -5460,18 +5493,28 @@
         <v>370</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
+    <row r="204" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C204" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="D204" t="s">
-        <v>462</v>
+      <c r="D204" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F204" s="8"/>
+      <c r="G204" s="11">
+        <v>12</v>
+      </c>
+      <c r="H204" s="3">
+        <v>1</v>
+      </c>
+      <c r="I204" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -5527,7 +5570,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>472</v>
       </c>
@@ -5538,21 +5581,31 @@
         <v>586</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
+    <row r="210" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C210" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="D210" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D210" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F210" s="8"/>
+      <c r="G210" s="11">
+        <v>146</v>
+      </c>
+      <c r="H210" s="3">
+        <v>1</v>
+      </c>
+      <c r="I210" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>474</v>
       </c>
@@ -5563,21 +5616,31 @@
         <v>370</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
+    <row r="212" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="B212" t="s">
+      <c r="B212" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C212" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="D212" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D212" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F212" s="8"/>
+      <c r="G212" s="11">
+        <v>97</v>
+      </c>
+      <c r="H212" s="3">
+        <v>1</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>476</v>
       </c>
@@ -5588,7 +5651,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>477</v>
       </c>
@@ -5599,7 +5662,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>478</v>
       </c>
@@ -5610,7 +5673,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>479</v>
       </c>
@@ -5621,7 +5684,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>480</v>
       </c>
@@ -5632,7 +5695,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>481</v>
       </c>
@@ -5646,7 +5709,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>482</v>
       </c>
@@ -5657,7 +5720,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>483</v>
       </c>
@@ -5668,7 +5731,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>484</v>
       </c>
@@ -5679,7 +5742,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>485</v>
       </c>
@@ -5690,10 +5753,10 @@
         <v>462</v>
       </c>
       <c r="F222" s="7" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>486</v>
       </c>
@@ -5704,10 +5767,10 @@
         <v>462</v>
       </c>
       <c r="F223" s="7" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>487</v>
       </c>
@@ -5842,10 +5905,13 @@
         <v>593</v>
       </c>
     </row>
-    <row r="236" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>499</v>
       </c>
+      <c r="B236" t="s">
+        <v>617</v>
+      </c>
       <c r="C236" t="s">
         <v>599</v>
       </c>
@@ -5853,7 +5919,7 @@
         <v>462</v>
       </c>
       <c r="F236" s="7" t="s">
-        <v>593</v>
+        <v>618</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -6076,7 +6142,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>520</v>
       </c>
@@ -6087,7 +6153,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>521</v>
       </c>
@@ -6098,7 +6164,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>522</v>
       </c>
@@ -6109,18 +6175,31 @@
         <v>370</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
+    <row r="260" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="C260" t="s">
+      <c r="B260" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="C260" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="D260" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D260" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F260" s="8"/>
+      <c r="G260" s="11">
+        <v>208</v>
+      </c>
+      <c r="H260" s="3">
+        <v>1</v>
+      </c>
+      <c r="I260" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>524</v>
       </c>
@@ -6131,21 +6210,33 @@
         <v>591</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A262" t="s">
+    <row r="262" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="C262" t="s">
+      <c r="B262" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="C262" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="D262" t="s">
-        <v>462</v>
-      </c>
-      <c r="F262" s="7" t="s">
+      <c r="D262" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F262" s="8" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G262" s="11">
+        <v>10</v>
+      </c>
+      <c r="H262" s="3">
+        <v>1</v>
+      </c>
+      <c r="I262" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>526</v>
       </c>
@@ -6156,7 +6247,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>527</v>
       </c>
@@ -6167,7 +6258,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>528</v>
       </c>
@@ -6178,7 +6269,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>529</v>
       </c>
@@ -6189,7 +6280,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>530</v>
       </c>
@@ -6200,7 +6291,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>531</v>
       </c>
@@ -6211,7 +6302,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>532</v>
       </c>
@@ -6222,7 +6313,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>533</v>
       </c>
@@ -6233,7 +6324,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>534</v>
       </c>
@@ -6244,7 +6335,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>535</v>
       </c>

</xml_diff>

<commit_message>
add last batch of NCBI species
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\5965364_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\5047028_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A78DE89-4149-4B4B-962E-CFE9E0D28C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A474588-0505-4388-A0D1-133B13DCBE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="683">
   <si>
     <t>Species</t>
   </si>
@@ -1122,9 +1122,6 @@
     <t>Dioscorea rotundata</t>
   </si>
   <si>
-    <t>Maybe WGS data for 3 genotypes</t>
-  </si>
-  <si>
     <t>Echinochloa crus-galli</t>
   </si>
   <si>
@@ -1939,6 +1936,156 @@
   </si>
   <si>
     <t>https://doi.org/10.1038/s41467-020-17111-w</t>
+  </si>
+  <si>
+    <t>A lot of data, need to look at more closely. There's some WGS data from JGI, but its new and separated by bioprojects. This is also a moss species</t>
+  </si>
+  <si>
+    <t>I don't think this dataset looks at nuclear DNA</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s12870-022-03449-4</t>
+  </si>
+  <si>
+    <t>PRJNA790687</t>
+  </si>
+  <si>
+    <t>Maybe some data, need to look at more closely. Some WGS data, but not enough</t>
+  </si>
+  <si>
+    <t>A lot of data, need to look at more closely. I don't think there's enough WGS data</t>
+  </si>
+  <si>
+    <t>PRJNA523120</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41438-019-0176-9</t>
+  </si>
+  <si>
+    <t>Maybe some data, need to look at more closely. No WGS data after all</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1126/sciadv.aaw1947</t>
+  </si>
+  <si>
+    <t>Maybe WGS data for 3 genotypes. Actually, I found some data while looking for data on D. cayanensis</t>
+  </si>
+  <si>
+    <t>Maybe some data, need to look at more closely. This is the same species as D. rotundata</t>
+  </si>
+  <si>
+    <t>PRJDB11628</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.gpb.2022.11.002</t>
+  </si>
+  <si>
+    <t>PRJNA610152</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41588-018-0116-x</t>
+  </si>
+  <si>
+    <t>PRJNA349094</t>
+  </si>
+  <si>
+    <t>A lot of data, need to look at more closely. Found GBS data, but no WGS</t>
+  </si>
+  <si>
+    <t>A lot of data, need to look at more closely. Didn't find WGS data</t>
+  </si>
+  <si>
+    <t>maybe works, also includes malus domestica</t>
+  </si>
+  <si>
+    <t>PRJNA487154</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s13059-020-01959-8</t>
+  </si>
+  <si>
+    <t>PRJEB24033</t>
+  </si>
+  <si>
+    <t>A lot of data, need to look at more closely. There could be more if I look at some other studies</t>
+  </si>
+  <si>
+    <t>maybe some data. No WGS data</t>
+  </si>
+  <si>
+    <t>PRJNA357653</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s12864-019-6376-8</t>
+  </si>
+  <si>
+    <t>A lot of data, need to look at more closely. No WGS data</t>
+  </si>
+  <si>
+    <t>PRJNA628142</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41467-020-19559-2</t>
+  </si>
+  <si>
+    <t>PRJEB40984</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41467-021-24283-6</t>
+  </si>
+  <si>
+    <t>maybe works… still not sure</t>
+  </si>
+  <si>
+    <t>PRJEB30573</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/f12121683</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.15399</t>
+  </si>
+  <si>
+    <t>PRJEB46635</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/pbi.13775</t>
+  </si>
+  <si>
+    <t>PRJNA790469</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/f13020338</t>
+  </si>
+  <si>
+    <t>PRJNA560664</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41438-020-0312-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2022.02.01.478712 </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s13059-020-02198-7</t>
+  </si>
+  <si>
+    <t>maybe works. Not enough WGS data</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41467-022-33515-2</t>
+  </si>
+  <si>
+    <t>PRJNA671733</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/1755-0998.13362</t>
+  </si>
+  <si>
+    <t>PRJNA394943</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41586-022-04822-x</t>
   </si>
 </sst>
 </file>
@@ -2332,8 +2479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A216" workbookViewId="0">
-      <selection activeCell="B222" sqref="B222"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,7 +2507,7 @@
         <v>320</v>
       </c>
       <c r="E1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>66</v>
@@ -2386,10 +2533,10 @@
         <v>135</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="11">
@@ -2404,16 +2551,16 @@
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>458</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>459</v>
       </c>
       <c r="G3" s="13"/>
     </row>
@@ -2439,10 +2586,10 @@
         <v>138</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="11">
@@ -2477,10 +2624,10 @@
         <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="11">
@@ -2501,10 +2648,10 @@
         <v>297</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="11">
@@ -2542,10 +2689,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="11">
@@ -2563,13 +2710,13 @@
         <v>82</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>624</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>625</v>
       </c>
       <c r="G11" s="11">
         <v>171</v>
@@ -2647,7 +2794,7 @@
         <v>149</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>239</v>
@@ -2684,7 +2831,7 @@
         <v>169</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="8" t="s">
@@ -2725,7 +2872,7 @@
         <v>282</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>283</v>
@@ -2798,7 +2945,7 @@
         <v>157</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>159</v>
@@ -2824,7 +2971,7 @@
         <v>157</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>159</v>
@@ -2861,7 +3008,7 @@
         <v>61</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>159</v>
@@ -2906,7 +3053,7 @@
         <v>58</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>259</v>
@@ -2954,7 +3101,7 @@
         <v>171</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>260</v>
@@ -2980,7 +3127,7 @@
         <v>174</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>261</v>
@@ -3275,10 +3422,10 @@
         <v>183</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F56" s="8"/>
       <c r="G56" s="11">
@@ -3693,13 +3840,13 @@
         <v>122</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G82" s="11">
         <v>48</v>
@@ -4092,10 +4239,10 @@
         <v>18</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="F107" s="14" t="s">
         <v>620</v>
-      </c>
-      <c r="F107" s="14" t="s">
-        <v>621</v>
       </c>
       <c r="G107" s="13"/>
     </row>
@@ -4782,20 +4929,35 @@
         <v>257</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="151" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="D151" t="s">
+      <c r="B151" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="D151" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="F151" s="7" t="s">
-        <v>361</v>
+      <c r="F151" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="G151" s="11">
+        <v>86</v>
+      </c>
+      <c r="H151" s="3">
+        <v>1</v>
+      </c>
+      <c r="I151" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D152" t="s">
         <v>321</v>
@@ -4806,7 +4968,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D153" t="s">
         <v>321</v>
@@ -4817,7 +4979,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D154" t="s">
         <v>321</v>
@@ -4828,16 +4990,16 @@
     </row>
     <row r="155" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>321</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G155" s="11">
         <v>14</v>
@@ -4851,7 +5013,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F156" s="7" t="s">
         <v>355</v>
@@ -4859,21 +5021,21 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
+        <v>368</v>
+      </c>
+      <c r="F157" s="7" t="s">
         <v>369</v>
-      </c>
-      <c r="F157" s="7" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="158" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B158" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="B158" s="3" t="s">
+      <c r="C158" s="3" t="s">
         <v>372</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>373</v>
       </c>
       <c r="D158" s="3" t="s">
         <v>321</v>
@@ -4891,35 +5053,35 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D159" t="s">
         <v>321</v>
       </c>
       <c r="F159" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D160" t="s">
         <v>321</v>
       </c>
       <c r="F160" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="161" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>376</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>377</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>321</v>
@@ -4937,29 +5099,29 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F162" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F163" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="164" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>321</v>
@@ -4977,33 +5139,33 @@
     </row>
     <row r="165" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>380</v>
+      </c>
+      <c r="B165" t="s">
+        <v>382</v>
+      </c>
+      <c r="C165" t="s">
         <v>381</v>
-      </c>
-      <c r="B165" t="s">
-        <v>383</v>
-      </c>
-      <c r="C165" t="s">
-        <v>382</v>
       </c>
       <c r="D165" t="s">
         <v>321</v>
       </c>
       <c r="F165" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="166" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C166" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D166" s="5" t="s">
         <v>321</v>
       </c>
       <c r="F166" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G166" s="13">
         <v>16</v>
@@ -5017,13 +5179,13 @@
     </row>
     <row r="167" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F167" s="8"/>
       <c r="G167" s="11">
@@ -5038,10 +5200,10 @@
     </row>
     <row r="168" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C168" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D168" s="5" t="s">
         <v>321</v>
@@ -5061,10 +5223,10 @@
     </row>
     <row r="169" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C169" s="5" t="s">
         <v>393</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>394</v>
       </c>
       <c r="D169" s="5" t="s">
         <v>321</v>
@@ -5084,10 +5246,10 @@
     </row>
     <row r="170" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C170" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D170" s="5" t="s">
         <v>321</v>
@@ -5107,27 +5269,27 @@
     </row>
     <row r="171" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D171" t="s">
         <v>321</v>
       </c>
       <c r="F171" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="172" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C172" s="5" t="s">
         <v>399</v>
-      </c>
-      <c r="C172" s="5" t="s">
-        <v>400</v>
       </c>
       <c r="D172" s="5" t="s">
         <v>321</v>
       </c>
       <c r="F172" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G172" s="13">
         <v>10</v>
@@ -5141,19 +5303,19 @@
     </row>
     <row r="173" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C173" s="3" t="s">
         <v>403</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>404</v>
       </c>
       <c r="D173" s="3" t="s">
         <v>321</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G173" s="11">
         <v>445</v>
@@ -5167,7 +5329,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F174" s="7" t="s">
         <v>355</v>
@@ -5175,23 +5337,23 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>406</v>
+      </c>
+      <c r="F175" s="7" t="s">
         <v>407</v>
-      </c>
-      <c r="F175" s="7" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
+        <v>408</v>
+      </c>
+      <c r="F176" s="7" t="s">
         <v>409</v>
-      </c>
-      <c r="F176" s="7" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F177" s="7" t="s">
         <v>341</v>
@@ -5199,16 +5361,16 @@
     </row>
     <row r="178" spans="1:9" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B178" s="3" t="s">
         <v>412</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>413</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>321</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G178" s="11">
         <v>27</v>
@@ -5222,19 +5384,19 @@
     </row>
     <row r="179" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B179" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="B179" s="3" t="s">
+      <c r="C179" s="3" t="s">
         <v>416</v>
-      </c>
-      <c r="C179" s="3" t="s">
-        <v>417</v>
       </c>
       <c r="D179" s="3" t="s">
         <v>321</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G179" s="11">
         <v>299</v>
@@ -5248,27 +5410,27 @@
     </row>
     <row r="180" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>418</v>
+      </c>
+      <c r="C180" t="s">
         <v>419</v>
       </c>
-      <c r="C180" t="s">
+      <c r="F180" s="7" t="s">
         <v>420</v>
-      </c>
-      <c r="F180" s="7" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="181" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D181" s="3" t="s">
         <v>321</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G181" s="11">
         <v>160</v>
@@ -5282,7 +5444,7 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F182" s="7" t="s">
         <v>341</v>
@@ -5290,7 +5452,7 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F183" s="7" t="s">
         <v>341</v>
@@ -5298,35 +5460,35 @@
     </row>
     <row r="184" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>426</v>
+      </c>
+      <c r="F184" s="7" t="s">
         <v>427</v>
-      </c>
-      <c r="F184" s="7" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
+        <v>428</v>
+      </c>
+      <c r="F185" s="7" t="s">
         <v>429</v>
-      </c>
-      <c r="F185" s="7" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="186" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B186" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="B186" s="3" t="s">
+      <c r="C186" s="3" t="s">
         <v>432</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>433</v>
       </c>
       <c r="D186" s="3" t="s">
         <v>321</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G186" s="11">
         <v>705</v>
@@ -5340,48 +5502,48 @@
     </row>
     <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>434</v>
+      </c>
+      <c r="F187" s="7" t="s">
         <v>435</v>
-      </c>
-      <c r="F187" s="7" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>436</v>
+      </c>
+      <c r="C188" t="s">
         <v>437</v>
       </c>
-      <c r="C188" t="s">
+      <c r="F188" s="7" t="s">
         <v>438</v>
-      </c>
-      <c r="F188" s="7" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F189" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F190" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="191" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F191" s="8"/>
       <c r="G191" s="11">
@@ -5399,10 +5561,10 @@
         <v>97</v>
       </c>
       <c r="C192" t="s">
+        <v>444</v>
+      </c>
+      <c r="F192" s="7" t="s">
         <v>445</v>
-      </c>
-      <c r="F192" s="7" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="193" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -5410,10 +5572,10 @@
         <v>97</v>
       </c>
       <c r="B193" t="s">
+        <v>446</v>
+      </c>
+      <c r="F193" s="7" t="s">
         <v>447</v>
-      </c>
-      <c r="F193" s="7" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="194" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5421,13 +5583,13 @@
         <v>97</v>
       </c>
       <c r="B194" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="F194" s="8" t="s">
         <v>450</v>
-      </c>
-      <c r="C194" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="F194" s="8" t="s">
-        <v>451</v>
       </c>
       <c r="G194" s="11">
         <v>37</v>
@@ -5469,13 +5631,13 @@
         <v>242</v>
       </c>
       <c r="B197" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C197" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="C197" s="3" t="s">
-        <v>461</v>
-      </c>
       <c r="D197" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F197" s="8"/>
       <c r="G197" s="11">
@@ -5528,60 +5690,60 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D202" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F202" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D203" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F203" s="7" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D204" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F204" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D205" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F205" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="206" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F206" s="8"/>
       <c r="G206" s="11">
@@ -5596,37 +5758,37 @@
     </row>
     <row r="207" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C207" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F207" s="8" t="s">
         <v>582</v>
-      </c>
-      <c r="D207" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="F207" s="8" t="s">
-        <v>583</v>
       </c>
       <c r="G207" s="11"/>
     </row>
     <row r="208" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F208" s="8" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="G208" s="11">
         <v>5</v>
@@ -5640,19 +5802,19 @@
     </row>
     <row r="209" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C209" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F209" s="8" t="s">
         <v>584</v>
-      </c>
-      <c r="D209" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="F209" s="8" t="s">
-        <v>585</v>
       </c>
       <c r="G209" s="11">
         <v>3</v>
@@ -5666,38 +5828,38 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D210" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F210" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D211" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F211" s="7" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="212" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F212" s="8"/>
       <c r="G212" s="11">
@@ -5712,27 +5874,27 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D213" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F213" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="214" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F214" s="8"/>
       <c r="G214" s="11">
@@ -5747,19 +5909,19 @@
     </row>
     <row r="215" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F215" s="8" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G215" s="11">
         <v>292</v>
@@ -5773,19 +5935,19 @@
     </row>
     <row r="216" spans="1:9" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B216" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="C216" s="3" t="s">
         <v>629</v>
       </c>
-      <c r="C216" s="3" t="s">
+      <c r="D216" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F216" s="8" t="s">
         <v>630</v>
-      </c>
-      <c r="D216" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="F216" s="8" t="s">
-        <v>631</v>
       </c>
       <c r="G216" s="11">
         <v>127</v>
@@ -5799,30 +5961,30 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D217" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F217" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="218" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F218" s="8" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G218" s="11">
         <v>565</v>
@@ -5834,509 +5996,581 @@
         <v>257</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D219" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F219" s="7" t="s">
-        <v>591</v>
+        <v>633</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
+        <v>480</v>
+      </c>
+      <c r="C220" t="s">
+        <v>591</v>
+      </c>
+      <c r="D220" t="s">
+        <v>461</v>
+      </c>
+      <c r="F220" s="7" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="C220" t="s">
-        <v>592</v>
-      </c>
-      <c r="D220" t="s">
-        <v>462</v>
-      </c>
-      <c r="F220" s="7" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>482</v>
-      </c>
-      <c r="D221" t="s">
-        <v>462</v>
-      </c>
-      <c r="F221" s="7" t="s">
-        <v>591</v>
+      <c r="B221" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F221" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G221" s="11">
+        <v>90</v>
+      </c>
+      <c r="H221" s="3">
+        <v>1</v>
+      </c>
+      <c r="I221" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="222" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D222" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F222" s="7" t="s">
-        <v>593</v>
+        <v>637</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D223" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F223" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>484</v>
+      </c>
+      <c r="C224" t="s">
+        <v>593</v>
+      </c>
+      <c r="D224" t="s">
+        <v>461</v>
+      </c>
+      <c r="F224" s="7" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>485</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C225" t="s">
         <v>594</v>
       </c>
-      <c r="D224" t="s">
-        <v>462</v>
-      </c>
-      <c r="F224" s="7" t="s">
+      <c r="D225" t="s">
+        <v>461</v>
+      </c>
+      <c r="F225" s="7" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="225" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
+    <row r="226" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>486</v>
       </c>
-      <c r="C225" t="s">
+      <c r="D226" t="s">
+        <v>461</v>
+      </c>
+      <c r="F226" s="7" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F227" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G227" s="11">
+        <v>8</v>
+      </c>
+      <c r="H227" s="3">
+        <v>1</v>
+      </c>
+      <c r="I227" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>488</v>
+      </c>
+      <c r="D228" t="s">
+        <v>461</v>
+      </c>
+      <c r="F228" s="7" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>489</v>
+      </c>
+      <c r="D229" t="s">
+        <v>461</v>
+      </c>
+      <c r="F229" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>490</v>
+      </c>
+      <c r="D230" t="s">
+        <v>461</v>
+      </c>
+      <c r="F230" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>491</v>
+      </c>
+      <c r="D231" t="s">
+        <v>461</v>
+      </c>
+      <c r="F231" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>492</v>
+      </c>
+      <c r="D232" t="s">
+        <v>461</v>
+      </c>
+      <c r="F232" s="7" t="s">
         <v>595</v>
       </c>
-      <c r="D225" t="s">
-        <v>462</v>
-      </c>
-      <c r="F225" s="7" t="s">
+    </row>
+    <row r="233" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>493</v>
+      </c>
+      <c r="C233" t="s">
+        <v>596</v>
+      </c>
+      <c r="D233" t="s">
+        <v>461</v>
+      </c>
+      <c r="F233" s="7" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>494</v>
+      </c>
+      <c r="D234" t="s">
+        <v>461</v>
+      </c>
+      <c r="F234" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>495</v>
+      </c>
+      <c r="D235" t="s">
+        <v>461</v>
+      </c>
+      <c r="F235" s="7" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F236" s="8" t="s">
+        <v>592</v>
+      </c>
+      <c r="G236" s="11">
+        <v>72</v>
+      </c>
+      <c r="H236" s="3">
+        <v>1</v>
+      </c>
+      <c r="I236" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F237" s="8" t="s">
+        <v>592</v>
+      </c>
+      <c r="G237" s="11">
+        <v>88</v>
+      </c>
+      <c r="H237" s="3">
+        <v>1</v>
+      </c>
+      <c r="I237" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>498</v>
+      </c>
+      <c r="B238" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>487</v>
-      </c>
-      <c r="D226" t="s">
-        <v>462</v>
-      </c>
-      <c r="F226" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
-        <v>488</v>
-      </c>
-      <c r="D227" t="s">
-        <v>462</v>
-      </c>
-      <c r="F227" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>489</v>
-      </c>
-      <c r="D228" t="s">
-        <v>462</v>
-      </c>
-      <c r="F228" s="7" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>490</v>
-      </c>
-      <c r="D229" t="s">
-        <v>462</v>
-      </c>
-      <c r="F229" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>491</v>
-      </c>
-      <c r="D230" t="s">
-        <v>462</v>
-      </c>
-      <c r="F230" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>492</v>
-      </c>
-      <c r="D231" t="s">
-        <v>462</v>
-      </c>
-      <c r="F231" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>493</v>
-      </c>
-      <c r="D232" t="s">
-        <v>462</v>
-      </c>
-      <c r="F232" s="7" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>494</v>
-      </c>
-      <c r="C233" t="s">
+      <c r="C238" t="s">
+        <v>598</v>
+      </c>
+      <c r="D238" t="s">
+        <v>461</v>
+      </c>
+      <c r="F238" s="7" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>499</v>
+      </c>
+      <c r="D239" t="s">
+        <v>461</v>
+      </c>
+      <c r="F239" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>500</v>
+      </c>
+      <c r="D240" t="s">
+        <v>461</v>
+      </c>
+      <c r="F240" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>501</v>
+      </c>
+      <c r="D241" t="s">
+        <v>461</v>
+      </c>
+      <c r="F241" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F242" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G242" s="11">
+        <v>228</v>
+      </c>
+      <c r="H242" s="3">
+        <v>1</v>
+      </c>
+      <c r="I242" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>503</v>
+      </c>
+      <c r="D243" t="s">
+        <v>461</v>
+      </c>
+      <c r="F243" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>504</v>
+      </c>
+      <c r="D244" t="s">
+        <v>461</v>
+      </c>
+      <c r="F244" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>505</v>
+      </c>
+      <c r="D245" t="s">
+        <v>461</v>
+      </c>
+      <c r="F245" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>506</v>
+      </c>
+      <c r="D246" t="s">
+        <v>461</v>
+      </c>
+      <c r="F246" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>507</v>
+      </c>
+      <c r="D247" t="s">
+        <v>461</v>
+      </c>
+      <c r="F247" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>508</v>
+      </c>
+      <c r="D248" t="s">
+        <v>461</v>
+      </c>
+      <c r="F248" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>509</v>
+      </c>
+      <c r="D249" t="s">
+        <v>461</v>
+      </c>
+      <c r="F249" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>510</v>
+      </c>
+      <c r="D250" t="s">
+        <v>461</v>
+      </c>
+      <c r="F250" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>511</v>
+      </c>
+      <c r="D251" t="s">
+        <v>461</v>
+      </c>
+      <c r="F251" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>512</v>
+      </c>
+      <c r="D252" t="s">
+        <v>461</v>
+      </c>
+      <c r="F252" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>513</v>
+      </c>
+      <c r="D253" t="s">
+        <v>461</v>
+      </c>
+      <c r="F253" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>514</v>
+      </c>
+      <c r="D254" t="s">
+        <v>461</v>
+      </c>
+      <c r="F254" s="7" t="s">
         <v>597</v>
       </c>
-      <c r="D233" t="s">
-        <v>462</v>
-      </c>
-      <c r="F233" s="7" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>495</v>
-      </c>
-      <c r="D234" t="s">
-        <v>462</v>
-      </c>
-      <c r="F234" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>496</v>
-      </c>
-      <c r="D235" t="s">
-        <v>462</v>
-      </c>
-      <c r="F235" s="7" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>497</v>
-      </c>
-      <c r="D236" t="s">
-        <v>462</v>
-      </c>
-      <c r="F236" s="7" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>498</v>
-      </c>
-      <c r="D237" t="s">
-        <v>462</v>
-      </c>
-      <c r="F237" s="7" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>499</v>
-      </c>
-      <c r="B238" t="s">
-        <v>617</v>
-      </c>
-      <c r="C238" t="s">
-        <v>599</v>
-      </c>
-      <c r="D238" t="s">
-        <v>462</v>
-      </c>
-      <c r="F238" s="7" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>500</v>
-      </c>
-      <c r="D239" t="s">
-        <v>462</v>
-      </c>
-      <c r="F239" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>501</v>
-      </c>
-      <c r="D240" t="s">
-        <v>462</v>
-      </c>
-      <c r="F240" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A241" t="s">
-        <v>502</v>
-      </c>
-      <c r="D241" t="s">
-        <v>462</v>
-      </c>
-      <c r="F241" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>503</v>
-      </c>
-      <c r="D242" t="s">
-        <v>462</v>
-      </c>
-      <c r="F242" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>504</v>
-      </c>
-      <c r="D243" t="s">
-        <v>462</v>
-      </c>
-      <c r="F243" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>505</v>
-      </c>
-      <c r="D244" t="s">
-        <v>462</v>
-      </c>
-      <c r="F244" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>506</v>
-      </c>
-      <c r="D245" t="s">
-        <v>462</v>
-      </c>
-      <c r="F245" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>507</v>
-      </c>
-      <c r="D246" t="s">
-        <v>462</v>
-      </c>
-      <c r="F246" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>508</v>
-      </c>
-      <c r="D247" t="s">
-        <v>462</v>
-      </c>
-      <c r="F247" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>509</v>
-      </c>
-      <c r="D248" t="s">
-        <v>462</v>
-      </c>
-      <c r="F248" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>510</v>
-      </c>
-      <c r="D249" t="s">
-        <v>462</v>
-      </c>
-      <c r="F249" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>511</v>
-      </c>
-      <c r="D250" t="s">
-        <v>462</v>
-      </c>
-      <c r="F250" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>512</v>
-      </c>
-      <c r="D251" t="s">
-        <v>462</v>
-      </c>
-      <c r="F251" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>513</v>
-      </c>
-      <c r="D252" t="s">
-        <v>462</v>
-      </c>
-      <c r="F252" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>514</v>
-      </c>
-      <c r="D253" t="s">
-        <v>462</v>
-      </c>
-      <c r="F253" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
         <v>515</v>
       </c>
-      <c r="D254" t="s">
-        <v>462</v>
-      </c>
-      <c r="F254" s="7" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
+      <c r="D255" t="s">
+        <v>461</v>
+      </c>
+      <c r="F255" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>516</v>
       </c>
-      <c r="D255" t="s">
-        <v>462</v>
-      </c>
-      <c r="F255" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>517</v>
-      </c>
       <c r="D256" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F256" s="7" t="s">
-        <v>591</v>
+        <v>650</v>
       </c>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
+        <v>517</v>
+      </c>
+      <c r="D257" t="s">
+        <v>461</v>
+      </c>
+      <c r="F257" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
         <v>518</v>
       </c>
-      <c r="D257" t="s">
-        <v>462</v>
-      </c>
-      <c r="F257" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A258" t="s">
-        <v>519</v>
-      </c>
       <c r="D258" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F258" s="7" t="s">
-        <v>591</v>
+        <v>651</v>
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D259" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F259" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D260" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F260" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D261" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F261" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="262" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D262" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F262" s="8"/>
       <c r="G262" s="11">
@@ -6349,32 +6583,47 @@
         <v>257</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A263" t="s">
-        <v>524</v>
-      </c>
-      <c r="D263" t="s">
-        <v>462</v>
-      </c>
-      <c r="F263" s="7" t="s">
-        <v>591</v>
+    <row r="263" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B263" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D263" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F263" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G263" s="11">
+        <v>86</v>
+      </c>
+      <c r="H263" s="3">
+        <v>1</v>
+      </c>
+      <c r="I263" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="264" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D264" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F264" s="8" t="s">
-        <v>602</v>
+        <v>652</v>
       </c>
       <c r="G264" s="11">
         <v>10</v>
@@ -6386,616 +6635,806 @@
         <v>257</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
-        <v>526</v>
-      </c>
-      <c r="D265" t="s">
-        <v>462</v>
-      </c>
-      <c r="F265" s="7" t="s">
-        <v>591</v>
+    <row r="265" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="D265" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F265" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G265" s="11">
+        <v>49</v>
+      </c>
+      <c r="H265" s="3">
+        <v>1</v>
+      </c>
+      <c r="I265" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D266" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F266" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D267" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F267" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D268" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F268" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
+        <v>529</v>
+      </c>
+      <c r="D269" t="s">
+        <v>461</v>
+      </c>
+      <c r="F269" s="7" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A270" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="D269" t="s">
-        <v>462</v>
-      </c>
-      <c r="F269" s="7" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>531</v>
-      </c>
-      <c r="D270" t="s">
-        <v>462</v>
-      </c>
-      <c r="F270" s="7" t="s">
-        <v>591</v>
+      <c r="C270" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="D270" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F270" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="G270" s="11">
+        <v>181</v>
+      </c>
+      <c r="H270" s="3">
+        <v>1</v>
+      </c>
+      <c r="I270" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D271" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F271" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
+        <v>532</v>
+      </c>
+      <c r="D272" t="s">
+        <v>461</v>
+      </c>
+      <c r="F272" s="7" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="D272" t="s">
-        <v>462</v>
-      </c>
-      <c r="F272" s="7" t="s">
+      <c r="B273" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="D273" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F273" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G273" s="11">
+        <v>67</v>
+      </c>
+      <c r="H273" s="3">
+        <v>1</v>
+      </c>
+      <c r="I273" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>534</v>
+      </c>
+      <c r="D274" t="s">
+        <v>461</v>
+      </c>
+      <c r="F274" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>535</v>
+      </c>
+      <c r="D275" t="s">
+        <v>461</v>
+      </c>
+      <c r="F275" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>536</v>
+      </c>
+      <c r="D276" t="s">
+        <v>461</v>
+      </c>
+      <c r="F276" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>537</v>
+      </c>
+      <c r="D277" t="s">
+        <v>461</v>
+      </c>
+      <c r="F277" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>538</v>
+      </c>
+      <c r="D278" t="s">
+        <v>461</v>
+      </c>
+      <c r="F278" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>539</v>
+      </c>
+      <c r="D279" t="s">
+        <v>461</v>
+      </c>
+      <c r="F279" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>540</v>
+      </c>
+      <c r="D280" t="s">
+        <v>461</v>
+      </c>
+      <c r="F280" s="7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>541</v>
+      </c>
+      <c r="D281" t="s">
+        <v>461</v>
+      </c>
+      <c r="F281" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="C282" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="D282" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F282" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G282" s="11">
+        <v>95</v>
+      </c>
+      <c r="H282" s="3">
+        <v>1</v>
+      </c>
+      <c r="I282" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>543</v>
+      </c>
+      <c r="D283" t="s">
+        <v>461</v>
+      </c>
+      <c r="F283" s="7" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>544</v>
+      </c>
+      <c r="D284" t="s">
+        <v>461</v>
+      </c>
+      <c r="F284" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>545</v>
+      </c>
+      <c r="D285" t="s">
+        <v>461</v>
+      </c>
+      <c r="F285" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B286" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="C286" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F286" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G286" s="11">
+        <v>359</v>
+      </c>
+      <c r="H286" s="3">
+        <v>1</v>
+      </c>
+      <c r="I286" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>547</v>
+      </c>
+      <c r="C287" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A273" t="s">
-        <v>534</v>
-      </c>
-      <c r="D273" t="s">
-        <v>462</v>
-      </c>
-      <c r="F273" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A274" t="s">
-        <v>535</v>
-      </c>
-      <c r="D274" t="s">
-        <v>462</v>
-      </c>
-      <c r="F274" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>536</v>
-      </c>
-      <c r="D275" t="s">
-        <v>462</v>
-      </c>
-      <c r="F275" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>537</v>
-      </c>
-      <c r="D276" t="s">
-        <v>462</v>
-      </c>
-      <c r="F276" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>538</v>
-      </c>
-      <c r="D277" t="s">
-        <v>462</v>
-      </c>
-      <c r="F277" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>539</v>
-      </c>
-      <c r="D278" t="s">
-        <v>462</v>
-      </c>
-      <c r="F278" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>540</v>
-      </c>
-      <c r="D279" t="s">
-        <v>462</v>
-      </c>
-      <c r="F279" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>541</v>
-      </c>
-      <c r="D280" t="s">
-        <v>462</v>
-      </c>
-      <c r="F280" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A281" t="s">
-        <v>542</v>
-      </c>
-      <c r="D281" t="s">
-        <v>462</v>
-      </c>
-      <c r="F281" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A282" t="s">
-        <v>543</v>
-      </c>
-      <c r="D282" t="s">
-        <v>462</v>
-      </c>
-      <c r="F282" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A283" t="s">
-        <v>544</v>
-      </c>
-      <c r="D283" t="s">
-        <v>462</v>
-      </c>
-      <c r="F283" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>545</v>
-      </c>
-      <c r="D284" t="s">
-        <v>462</v>
-      </c>
-      <c r="F284" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>546</v>
-      </c>
-      <c r="D285" t="s">
-        <v>462</v>
-      </c>
-      <c r="F285" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>547</v>
-      </c>
-      <c r="D286" t="s">
-        <v>462</v>
-      </c>
-      <c r="F286" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
+      <c r="D287" t="s">
+        <v>461</v>
+      </c>
+      <c r="F287" s="7" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
         <v>548</v>
       </c>
-      <c r="C287" t="s">
+      <c r="D288" t="s">
+        <v>461</v>
+      </c>
+      <c r="F288" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F289" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G289" s="11">
+        <v>447</v>
+      </c>
+      <c r="H289" s="3">
+        <v>1</v>
+      </c>
+      <c r="I289" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>550</v>
+      </c>
+      <c r="D290" t="s">
+        <v>461</v>
+      </c>
+      <c r="F290" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="B291" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="C291" s="3" t="s">
         <v>604</v>
       </c>
-      <c r="D287" t="s">
-        <v>462</v>
-      </c>
-      <c r="F287" s="7" t="s">
+      <c r="D291" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F291" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="G291" s="11">
+        <v>32</v>
+      </c>
+      <c r="H291" s="3">
+        <v>1</v>
+      </c>
+      <c r="I291" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>552</v>
+      </c>
+      <c r="D292" t="s">
+        <v>461</v>
+      </c>
+      <c r="F292" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B293" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="D293" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F293" s="8" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
-        <v>549</v>
-      </c>
-      <c r="D288" t="s">
-        <v>462</v>
-      </c>
-      <c r="F288" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A289" t="s">
-        <v>550</v>
-      </c>
-      <c r="D289" t="s">
-        <v>462</v>
-      </c>
-      <c r="F289" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A290" t="s">
-        <v>551</v>
-      </c>
-      <c r="D290" t="s">
-        <v>462</v>
-      </c>
-      <c r="F290" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A291" t="s">
-        <v>552</v>
-      </c>
-      <c r="C291" t="s">
+      <c r="G293" s="11"/>
+      <c r="H293" s="3">
+        <v>1</v>
+      </c>
+      <c r="I293" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>554</v>
+      </c>
+      <c r="D294" t="s">
+        <v>461</v>
+      </c>
+      <c r="F294" s="7" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>555</v>
+      </c>
+      <c r="D295" t="s">
+        <v>461</v>
+      </c>
+      <c r="F295" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>556</v>
+      </c>
+      <c r="D296" t="s">
+        <v>461</v>
+      </c>
+      <c r="F296" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>557</v>
+      </c>
+      <c r="D297" t="s">
+        <v>461</v>
+      </c>
+      <c r="F297" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>558</v>
+      </c>
+      <c r="D298" t="s">
+        <v>461</v>
+      </c>
+      <c r="F298" s="7" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>559</v>
+      </c>
+      <c r="D299" t="s">
+        <v>461</v>
+      </c>
+      <c r="F299" s="7" t="s">
         <v>605</v>
       </c>
-      <c r="D291" t="s">
-        <v>462</v>
-      </c>
-      <c r="F291" s="7" t="s">
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>560</v>
+      </c>
+      <c r="D300" t="s">
+        <v>461</v>
+      </c>
+      <c r="F300" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>561</v>
+      </c>
+      <c r="D301" t="s">
+        <v>461</v>
+      </c>
+      <c r="F301" s="7" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="B302" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="C302" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="D302" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F302" s="8" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A292" t="s">
-        <v>553</v>
-      </c>
-      <c r="D292" t="s">
-        <v>462</v>
-      </c>
-      <c r="F292" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A293" t="s">
-        <v>554</v>
-      </c>
-      <c r="D293" t="s">
-        <v>462</v>
-      </c>
-      <c r="F293" s="7" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A294" t="s">
-        <v>555</v>
-      </c>
-      <c r="D294" t="s">
-        <v>462</v>
-      </c>
-      <c r="F294" s="7" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A295" t="s">
-        <v>556</v>
-      </c>
-      <c r="D295" t="s">
-        <v>462</v>
-      </c>
-      <c r="F295" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A296" t="s">
-        <v>557</v>
-      </c>
-      <c r="D296" t="s">
-        <v>462</v>
-      </c>
-      <c r="F296" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A297" t="s">
-        <v>558</v>
-      </c>
-      <c r="D297" t="s">
-        <v>462</v>
-      </c>
-      <c r="F297" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A298" t="s">
-        <v>559</v>
-      </c>
-      <c r="D298" t="s">
-        <v>462</v>
-      </c>
-      <c r="F298" s="7" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>560</v>
-      </c>
-      <c r="D299" t="s">
-        <v>462</v>
-      </c>
-      <c r="F299" s="7" t="s">
+      <c r="G302" s="11"/>
+      <c r="H302" s="3">
+        <v>1</v>
+      </c>
+      <c r="I302" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>563</v>
+      </c>
+      <c r="D303" t="s">
+        <v>461</v>
+      </c>
+      <c r="F303" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="B304" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C304" s="3" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>561</v>
-      </c>
-      <c r="D300" t="s">
-        <v>462</v>
-      </c>
-      <c r="F300" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>562</v>
-      </c>
-      <c r="D301" t="s">
-        <v>462</v>
-      </c>
-      <c r="F301" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A302" t="s">
-        <v>563</v>
-      </c>
-      <c r="D302" t="s">
-        <v>462</v>
-      </c>
-      <c r="F302" s="7" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A303" t="s">
-        <v>564</v>
-      </c>
-      <c r="D303" t="s">
-        <v>462</v>
-      </c>
-      <c r="F303" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A304" t="s">
+      <c r="D304" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F304" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="G304" s="11"/>
+      <c r="H304" s="3">
+        <v>1</v>
+      </c>
+      <c r="I304" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
         <v>565</v>
       </c>
-      <c r="C304" t="s">
+      <c r="D305" t="s">
+        <v>461</v>
+      </c>
+      <c r="F305" s="7" t="s">
         <v>607</v>
       </c>
-      <c r="D304" t="s">
-        <v>462</v>
-      </c>
-      <c r="F304" s="7" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
         <v>566</v>
       </c>
-      <c r="D305" t="s">
-        <v>462</v>
-      </c>
-      <c r="F305" s="7" t="s">
+      <c r="D306" t="s">
+        <v>461</v>
+      </c>
+      <c r="F306" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>567</v>
+      </c>
+      <c r="D307" t="s">
+        <v>461</v>
+      </c>
+      <c r="F307" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="C308" s="3" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A306" t="s">
-        <v>567</v>
-      </c>
-      <c r="D306" t="s">
-        <v>462</v>
-      </c>
-      <c r="F306" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A307" t="s">
-        <v>568</v>
-      </c>
-      <c r="D307" t="s">
-        <v>462</v>
-      </c>
-      <c r="F307" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A308" t="s">
+      <c r="D308" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F308" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="G308" s="11"/>
+      <c r="H308" s="3">
+        <v>1</v>
+      </c>
+      <c r="I308" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
         <v>569</v>
       </c>
-      <c r="C308" t="s">
+      <c r="C309" t="s">
         <v>609</v>
       </c>
-      <c r="D308" t="s">
-        <v>462</v>
-      </c>
-      <c r="F308" s="7" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A309" t="s">
+      <c r="D309" t="s">
+        <v>461</v>
+      </c>
+      <c r="F309" s="7" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="C309" t="s">
-        <v>610</v>
-      </c>
-      <c r="D309" t="s">
-        <v>462</v>
-      </c>
-      <c r="F309" s="7" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A310" t="s">
+      <c r="B310" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="C310" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="D310" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F310" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G310" s="11"/>
+      <c r="H310" s="3">
+        <v>1</v>
+      </c>
+      <c r="I310" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
         <v>571</v>
       </c>
-      <c r="D310" t="s">
-        <v>462</v>
-      </c>
-      <c r="F310" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A311" t="s">
-        <v>572</v>
-      </c>
       <c r="D311" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F311" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>262</v>
       </c>
       <c r="D312" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F312" s="7" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A313" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="C313" s="3" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A313" t="s">
+      <c r="D313" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F313" s="8" t="s">
+        <v>601</v>
+      </c>
+      <c r="G313" s="11"/>
+    </row>
+    <row r="314" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
         <v>573</v>
       </c>
-      <c r="C313" t="s">
-        <v>612</v>
-      </c>
-      <c r="D313" t="s">
-        <v>462</v>
-      </c>
-      <c r="F313" s="7" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A314" t="s">
+      <c r="D314" t="s">
+        <v>461</v>
+      </c>
+      <c r="F314" s="7" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A315" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="D314" t="s">
-        <v>462</v>
-      </c>
-      <c r="F314" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A315" t="s">
+      <c r="B315" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="C315" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="D315" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F315" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G315" s="11">
+        <v>119</v>
+      </c>
+      <c r="H315" s="3">
+        <v>1</v>
+      </c>
+      <c r="I315" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
         <v>575</v>
       </c>
-      <c r="D315" t="s">
-        <v>462</v>
-      </c>
-      <c r="F315" s="7" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A316" t="s">
+      <c r="D316" t="s">
+        <v>461</v>
+      </c>
+      <c r="F316" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
         <v>576</v>
       </c>
-      <c r="D316" t="s">
-        <v>462</v>
-      </c>
-      <c r="F316" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A317" t="s">
+      <c r="D317" t="s">
+        <v>461</v>
+      </c>
+      <c r="F317" s="7" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A318" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="D317" t="s">
-        <v>462</v>
-      </c>
-      <c r="F317" s="7" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A318" t="s">
-        <v>578</v>
-      </c>
-      <c r="D318" t="s">
-        <v>462</v>
-      </c>
-      <c r="F318" s="7" t="s">
-        <v>591</v>
+      <c r="B318" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="C318" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="D318" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F318" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G318" s="11"/>
+      <c r="H318" s="3">
+        <v>1</v>
+      </c>
+      <c r="I318" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -7036,7 +7475,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -7601,197 +8040,197 @@
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="15" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="15" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="15" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update readme and notes
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,17 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\5047028_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67318_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A474588-0505-4388-A0D1-133B13DCBE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C6EC8D-F8D2-4ECA-913B-6487EFD7B16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Included species" sheetId="2" r:id="rId2"/>
+    <sheet name="diversity vs population size" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'diversity vs population size'!$A$1:$B$318</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1372" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="685">
   <si>
     <t>Species</t>
   </si>
@@ -2086,6 +2090,12 @@
   </si>
   <si>
     <t>https://doi.org/10.1038/s41586-022-04822-x</t>
+  </si>
+  <si>
+    <t>Species with genetic diversity estimates</t>
+  </si>
+  <si>
+    <t>Species with population size estimates</t>
   </si>
 </sst>
 </file>
@@ -2479,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="F121" sqref="F121"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7459,8 +7469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA0D188-8CB9-4E9E-A4CF-6AB440175DE3}">
   <dimension ref="A1:A158"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A56" sqref="A1:A158"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8262,4 +8272,596 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F5CC31-DEE7-4BD6-8EEB-669C598FA203}">
+  <dimension ref="A1:B108"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>683</v>
+      </c>
+      <c r="B1" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B7" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B318">
+    <sortCondition ref="A2:A318"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
defined R environment for download-gbif script
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67318_2_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/1377500_2_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C6EC8D-F8D2-4ECA-913B-6487EFD7B16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{42C6EC8D-F8D2-4ECA-913B-6487EFD7B16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{293A5F4A-6E4F-42A1-B169-B3037E2E7578}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
     <sheet name="Included species" sheetId="2" r:id="rId2"/>
     <sheet name="diversity vs population size" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="695">
   <si>
     <t>Species</t>
   </si>
@@ -2096,6 +2096,36 @@
   </si>
   <si>
     <t>Species with population size estimates</t>
+  </si>
+  <si>
+    <t>Solanum melongena</t>
+  </si>
+  <si>
+    <t>Solanum lycopersicoides</t>
+  </si>
+  <si>
+    <t>Solanum pimpinellifolium</t>
+  </si>
+  <si>
+    <t>Iochroma cyaneum</t>
+  </si>
+  <si>
+    <t>Nicotiana benthamiana</t>
+  </si>
+  <si>
+    <t>Nicotiana tabacum</t>
+  </si>
+  <si>
+    <t>Petunia axillaris</t>
+  </si>
+  <si>
+    <t>Petunia inflata</t>
+  </si>
+  <si>
+    <t>Solanum chilense</t>
+  </si>
+  <si>
+    <t>Coffea humblotiana</t>
   </si>
 </sst>
 </file>
@@ -2487,10 +2517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I318"/>
+  <dimension ref="A1:I329"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="A329" sqref="A329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7445,6 +7475,61 @@
       </c>
       <c r="I318" s="3" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -8278,7 +8363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F5CC31-DEE7-4BD6-8EEB-669C598FA203}">
   <dimension ref="A1:B108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add scripts to prepare genomes for workflow
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/1377500_2_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67280_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{42C6EC8D-F8D2-4ECA-913B-6487EFD7B16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{293A5F4A-6E4F-42A1-B169-B3037E2E7578}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC6F109-7AE2-4592-8214-F367871F8CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="699">
   <si>
     <t>Species</t>
   </si>
@@ -2126,6 +2126,18 @@
   </si>
   <si>
     <t>Coffea humblotiana</t>
+  </si>
+  <si>
+    <t>GBIF taxon key</t>
+  </si>
+  <si>
+    <t>Brassica cretica</t>
+  </si>
+  <si>
+    <t>Brassica elongata</t>
+  </si>
+  <si>
+    <t>Arabis planisiliqua</t>
   </si>
 </sst>
 </file>
@@ -2205,7 +2217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2236,6 +2248,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2519,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
-      <selection activeCell="A329" sqref="A329"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,6 +2774,9 @@
       <c r="C11" s="3" t="s">
         <v>622</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F11" s="8" t="s">
         <v>624</v>
       </c>
@@ -3203,6 +3225,9 @@
       <c r="C38" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="D38" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F38" s="8" t="s">
         <v>302</v>
       </c>
@@ -3259,6 +3284,9 @@
       <c r="C42" s="3" t="s">
         <v>178</v>
       </c>
+      <c r="D42" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F42" s="8" t="s">
         <v>159</v>
       </c>
@@ -3390,6 +3418,9 @@
       <c r="C52" s="3" t="s">
         <v>284</v>
       </c>
+      <c r="D52" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F52" s="8" t="s">
         <v>291</v>
       </c>
@@ -3413,6 +3444,9 @@
       <c r="C53" s="3" t="s">
         <v>287</v>
       </c>
+      <c r="D53" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F53" s="8" t="s">
         <v>292</v>
       </c>
@@ -3430,6 +3464,9 @@
       <c r="C54" s="3" t="s">
         <v>288</v>
       </c>
+      <c r="D54" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F54" s="8" t="s">
         <v>290</v>
       </c>
@@ -3488,6 +3525,9 @@
       <c r="C57" s="3" t="s">
         <v>185</v>
       </c>
+      <c r="D57" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F57" s="8"/>
       <c r="G57" s="11">
         <v>336</v>
@@ -3519,6 +3559,9 @@
       </c>
       <c r="C59" s="3" t="s">
         <v>247</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="F59" s="8"/>
       <c r="G59" s="11">
@@ -3601,6 +3644,9 @@
       <c r="C65" s="3" t="s">
         <v>188</v>
       </c>
+      <c r="D65" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F65" s="8"/>
       <c r="G65" s="11">
         <v>300</v>
@@ -3633,6 +3679,9 @@
       <c r="C67" s="3" t="s">
         <v>189</v>
       </c>
+      <c r="D67" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F67" s="8" t="s">
         <v>264</v>
       </c>
@@ -3684,6 +3733,9 @@
       <c r="C70" s="3" t="s">
         <v>304</v>
       </c>
+      <c r="D70" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F70" s="8" t="s">
         <v>306</v>
       </c>
@@ -3732,6 +3784,9 @@
       <c r="C73" s="3" t="s">
         <v>198</v>
       </c>
+      <c r="D73" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F73" s="8" t="s">
         <v>265</v>
       </c>
@@ -3766,6 +3821,9 @@
       <c r="C75" s="3" t="s">
         <v>201</v>
       </c>
+      <c r="D75" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F75" s="8" t="s">
         <v>266</v>
       </c>
@@ -3800,6 +3858,9 @@
       <c r="C77" s="3" t="s">
         <v>267</v>
       </c>
+      <c r="D77" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F77" s="8" t="s">
         <v>159</v>
       </c>
@@ -3851,6 +3912,9 @@
       <c r="C80" s="3" t="s">
         <v>244</v>
       </c>
+      <c r="D80" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F80" s="8" t="s">
         <v>270</v>
       </c>
@@ -3885,6 +3949,9 @@
       <c r="C82" s="3" t="s">
         <v>598</v>
       </c>
+      <c r="D82" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F82" s="8" t="s">
         <v>618</v>
       </c>
@@ -3919,6 +3986,9 @@
       <c r="C84" s="3" t="s">
         <v>205</v>
       </c>
+      <c r="D84" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F84" s="8" t="s">
         <v>271</v>
       </c>
@@ -3967,6 +4037,9 @@
       <c r="C87" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D87" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F87" s="8" t="s">
         <v>272</v>
       </c>
@@ -3990,6 +4063,9 @@
       <c r="C88" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="D88" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F88" s="8" t="s">
         <v>293</v>
       </c>
@@ -4013,6 +4089,9 @@
       <c r="C89" s="3" t="s">
         <v>209</v>
       </c>
+      <c r="D89" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F89" s="8" t="s">
         <v>273</v>
       </c>
@@ -4047,6 +4126,9 @@
       <c r="C91" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="D91" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F91" s="8"/>
       <c r="G91" s="11">
         <v>683</v>
@@ -4079,6 +4161,9 @@
       <c r="C93" s="3" t="s">
         <v>56</v>
       </c>
+      <c r="D93" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F93" s="8" t="s">
         <v>252</v>
       </c>
@@ -4140,6 +4225,9 @@
       <c r="C98" s="3" t="s">
         <v>211</v>
       </c>
+      <c r="D98" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F98" s="8" t="s">
         <v>274</v>
       </c>
@@ -4196,6 +4284,9 @@
       <c r="C102" s="3" t="s">
         <v>213</v>
       </c>
+      <c r="D102" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F102" s="8" t="s">
         <v>275</v>
       </c>
@@ -4219,6 +4310,9 @@
       <c r="C103" s="3" t="s">
         <v>215</v>
       </c>
+      <c r="D103" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F103" s="8" t="s">
         <v>276</v>
       </c>
@@ -4261,6 +4355,9 @@
       <c r="C106" s="3" t="s">
         <v>219</v>
       </c>
+      <c r="D106" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F106" s="8" t="s">
         <v>159</v>
       </c>
@@ -4286,16 +4383,17 @@
       </c>
       <c r="G107" s="13"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="108" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="F108" s="7" t="s">
+      <c r="F108" s="17" t="s">
         <v>222</v>
       </c>
+      <c r="G108" s="18"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -4335,6 +4433,9 @@
       <c r="C111" s="3" t="s">
         <v>227</v>
       </c>
+      <c r="D111" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F111" s="8" t="s">
         <v>159</v>
       </c>
@@ -4358,6 +4459,9 @@
       <c r="C112" s="3" t="s">
         <v>228</v>
       </c>
+      <c r="D112" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F112" s="8" t="s">
         <v>277</v>
       </c>
@@ -4381,6 +4485,9 @@
       <c r="C113" s="3" t="s">
         <v>230</v>
       </c>
+      <c r="D113" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F113" s="8" t="s">
         <v>279</v>
       </c>
@@ -4437,6 +4544,9 @@
       <c r="C117" s="3" t="s">
         <v>300</v>
       </c>
+      <c r="D117" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F117" s="8" t="s">
         <v>233</v>
       </c>
@@ -4516,6 +4626,9 @@
       <c r="C122" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="D122" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F122" s="8" t="s">
         <v>278</v>
       </c>
@@ -4555,6 +4668,9 @@
       <c r="C125" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D125" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F125" s="8" t="s">
         <v>295</v>
       </c>
@@ -4575,6 +4691,9 @@
       <c r="C126" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D126" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F126" s="8" t="s">
         <v>296</v>
       </c>
@@ -4587,6 +4706,9 @@
       <c r="C127" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="D127" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="F127" s="8"/>
       <c r="G127" s="11">
         <v>277</v>
@@ -4598,6 +4720,9 @@
       </c>
       <c r="C128" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="F128" s="8"/>
       <c r="G128" s="11">
@@ -8361,10 +8486,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F5CC31-DEE7-4BD6-8EEB-669C598FA203}">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8373,186 +8498,252 @@
     <col min="2" max="2" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>683</v>
       </c>
       <c r="B1" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>3052450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3052468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>466</v>
       </c>
       <c r="B7" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>3052544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3052436</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9">
+        <v>5375020</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>698</v>
+      </c>
+      <c r="C10">
+        <v>5374933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B16" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>3043392</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17">
+        <v>5290143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>327</v>
+      </c>
+      <c r="C18">
+        <v>9073641</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>697</v>
+      </c>
+      <c r="C19">
+        <v>3042888</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>696</v>
+      </c>
+      <c r="C20">
+        <v>3042837</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21">
+        <v>7903057</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B26" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>5375387</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B27" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>5375425</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>48</v>
       </c>
@@ -8948,5 +9139,6 @@
     <sortCondition ref="A2:A318"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug in cat_replicates
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/394744_2_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\133032_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{4BC6F109-7AE2-4592-8214-F367871F8CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72C23F8C-65A4-4CDE-8B5B-8A5CCA971711}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288CFB60-3D1E-438A-AD79-978746AFC312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1579" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="726">
   <si>
     <t>Species</t>
   </si>
@@ -2186,6 +2186,39 @@
   </si>
   <si>
     <t>Genome Database for Rosaceae</t>
+  </si>
+  <si>
+    <t>Aethionema arabicum</t>
+  </si>
+  <si>
+    <t>Boechera retrofracta</t>
+  </si>
+  <si>
+    <t>Brassica nigra </t>
+  </si>
+  <si>
+    <t>Caradmine hirsuta</t>
+  </si>
+  <si>
+    <t>Crucihimalaya himalaica</t>
+  </si>
+  <si>
+    <t>Descurainia sophia</t>
+  </si>
+  <si>
+    <t>Isatis indigotica</t>
+  </si>
+  <si>
+    <t>Leavenworthia alabamica</t>
+  </si>
+  <si>
+    <t>Raphanus sativus</t>
+  </si>
+  <si>
+    <t>Sisymbrium irio</t>
+  </si>
+  <si>
+    <t>Thellungiella halophila</t>
   </si>
 </sst>
 </file>
@@ -2577,10 +2610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I331"/>
+  <dimension ref="A1:I343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="G322" sqref="G322"/>
+    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
+      <selection activeCell="A342" sqref="A342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7822,12 +7855,111 @@
       </c>
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>715</v>
+      </c>
       <c r="D330" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>716</v>
+      </c>
       <c r="D331" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>473</v>
+      </c>
+      <c r="D332" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>717</v>
+      </c>
+      <c r="D333" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>718</v>
+      </c>
+      <c r="D334" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>719</v>
+      </c>
+      <c r="D335" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>720</v>
+      </c>
+      <c r="D336" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>721</v>
+      </c>
+      <c r="D337" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>722</v>
+      </c>
+      <c r="D338" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>723</v>
+      </c>
+      <c r="D339" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>724</v>
+      </c>
+      <c r="D340" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>725</v>
+      </c>
+      <c r="D341" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>570</v>
+      </c>
+      <c r="D342" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D343" t="s">
         <v>714</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bug in kmc_pe
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\133032_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/394744_2_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288CFB60-3D1E-438A-AD79-978746AFC312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{288CFB60-3D1E-438A-AD79-978746AFC312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F39FCC6D-D1D8-41CB-A824-6A1C93F3125D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="731">
   <si>
     <t>Species</t>
   </si>
@@ -2219,6 +2219,21 @@
   </si>
   <si>
     <t>Thellungiella halophila</t>
+  </si>
+  <si>
+    <t>WGS data for mapping population</t>
+  </si>
+  <si>
+    <t>lots of data, need to look at more closely</t>
+  </si>
+  <si>
+    <t>found data in set for other species</t>
+  </si>
+  <si>
+    <t>PRJNA634208</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038%2Fs41438-020-00385-y</t>
   </si>
 </sst>
 </file>
@@ -2610,10 +2625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I343"/>
+  <dimension ref="A1:I342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
-      <selection activeCell="A342" sqref="A342"/>
+    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="D342" sqref="D342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7861,6 +7876,9 @@
       <c r="D330" t="s">
         <v>713</v>
       </c>
+      <c r="F330" s="7" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
@@ -7869,6 +7887,9 @@
       <c r="D331" t="s">
         <v>713</v>
       </c>
+      <c r="F331" s="7" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
@@ -7877,13 +7898,34 @@
       <c r="D332" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A333" t="s">
+      <c r="F332" s="7" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="3" t="s">
         <v>717</v>
       </c>
-      <c r="D333" t="s">
+      <c r="B333" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C333" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D333" s="3" t="s">
         <v>713</v>
+      </c>
+      <c r="F333" s="8" t="s">
+        <v>728</v>
+      </c>
+      <c r="G333" s="11">
+        <v>7</v>
+      </c>
+      <c r="H333" s="3">
+        <v>1</v>
+      </c>
+      <c r="I333" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.25">
@@ -7893,6 +7935,9 @@
       <c r="D334" t="s">
         <v>713</v>
       </c>
+      <c r="F334" s="7" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
@@ -7901,6 +7946,9 @@
       <c r="D335" t="s">
         <v>713</v>
       </c>
+      <c r="F335" s="7" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
@@ -7909,57 +7957,82 @@
       <c r="D336" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F336" s="7" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>721</v>
       </c>
       <c r="D337" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F337" s="7" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>722</v>
       </c>
       <c r="D338" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
+      <c r="F338" s="7" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="3" t="s">
         <v>723</v>
       </c>
-      <c r="D339" t="s">
+      <c r="B339" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="D339" s="3" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F339" s="8" t="s">
+        <v>727</v>
+      </c>
+      <c r="G339" s="11">
+        <v>179</v>
+      </c>
+      <c r="H339" s="3">
+        <v>1</v>
+      </c>
+      <c r="I339" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>724</v>
       </c>
       <c r="D340" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F340" s="7" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>725</v>
       </c>
       <c r="D341" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
-        <v>570</v>
-      </c>
+      <c r="F341" s="7" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D342" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D343" t="s">
         <v>714</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bugs in pi calculation
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/394744_2_10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/198084_2_11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{288CFB60-3D1E-438A-AD79-978746AFC312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F39FCC6D-D1D8-41CB-A824-6A1C93F3125D}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{288CFB60-3D1E-438A-AD79-978746AFC312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{702FF519-3A50-44B6-98A4-F8C76C83D394}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="732">
   <si>
     <t>Species</t>
   </si>
@@ -2234,6 +2234,9 @@
   </si>
   <si>
     <t>https://doi.org/10.1038%2Fs41438-020-00385-y</t>
+  </si>
+  <si>
+    <t>PLAZA 5.0</t>
   </si>
 </sst>
 </file>
@@ -2625,10 +2628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I342"/>
+  <dimension ref="A1:I343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
-      <selection activeCell="D342" sqref="D342"/>
+    <sheetView tabSelected="1" topLeftCell="A333" workbookViewId="0">
+      <selection activeCell="D333" sqref="D333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8034,6 +8037,11 @@
     <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D342" t="s">
         <v>714</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D343" t="s">
+        <v>731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bugs in kmer unionizing
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/1312106_2_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\66558_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{288CFB60-3D1E-438A-AD79-978746AFC312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA672FB4-6E90-4E30-B727-5803AF69ACE3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6845A9D8-AAB2-4289-A714-5808F1106EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="736">
   <si>
     <t>Species</t>
   </si>
@@ -2237,6 +2237,18 @@
   </si>
   <si>
     <t>Publication only mentions 50 genomes, but SRA dataset has 52, ERR636156 is single end</t>
+  </si>
+  <si>
+    <t>PRJNA207721</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/aob/mcu084</t>
+  </si>
+  <si>
+    <t>PRJNA765476</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpls.2021.748750</t>
   </si>
 </sst>
 </file>
@@ -2631,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I343"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,18 +3444,30 @@
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="D46" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F46" s="7" t="s">
         <v>145</v>
+      </c>
+      <c r="G46" s="10">
+        <v>643</v>
+      </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3713,18 +3737,30 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F64" s="6" t="s">
+      <c r="D64" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F64" s="7" t="s">
         <v>145</v>
+      </c>
+      <c r="G64" s="10">
+        <v>98</v>
+      </c>
+      <c r="H64" s="3">
+        <v>1</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3788,32 +3824,50 @@
         <v>257</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="F68" s="7" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="G68" s="10">
+        <v>176</v>
+      </c>
+      <c r="H68" s="3">
+        <v>1</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="F69" s="6" t="s">
+      <c r="F69" s="7" t="s">
         <v>145</v>
+      </c>
+      <c r="G69" s="10">
+        <v>17</v>
+      </c>
+      <c r="H69" s="3">
+        <v>1</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4021,15 +4075,30 @@
         <v>257</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C81" t="s">
-        <v>136</v>
-      </c>
-      <c r="F81" s="6" t="s">
+      <c r="B81" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F81" s="7" t="s">
         <v>203</v>
+      </c>
+      <c r="G81" s="10">
+        <v>2644</v>
+      </c>
+      <c r="H81" s="3">
+        <v>1</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -4476,16 +4545,17 @@
       </c>
       <c r="G107" s="12"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="108" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="F108" s="6" t="s">
+      <c r="F108" s="13" t="s">
         <v>222</v>
       </c>
+      <c r="G108" s="12"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -4604,26 +4674,56 @@
         <v>137</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="115" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F115" s="6" t="s">
+      <c r="D115" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F115" s="7" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="G115" s="10">
+        <v>768</v>
+      </c>
+      <c r="H115" s="3">
+        <v>1</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="F116" s="6" t="s">
+      <c r="B116" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F116" s="7" t="s">
         <v>232</v>
+      </c>
+      <c r="G116" s="10">
+        <v>672</v>
+      </c>
+      <c r="H116" s="3">
+        <v>1</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
test workflow on 7 species
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/131816_2_10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/131816_3_13/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{6845A9D8-AAB2-4289-A714-5808F1106EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10671482-6DF1-46E1-B9C4-E189FED29D66}"/>
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="A207" sqref="A207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add body size data
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/131816_3_13/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/131816_2_14/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{6845A9D8-AAB2-4289-A714-5808F1106EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10671482-6DF1-46E1-B9C4-E189FED29D66}"/>
@@ -2733,8 +2733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="A207" sqref="A207"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
remove problematic parts of workflow for now
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/131816_2_14/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/1116386_2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{6845A9D8-AAB2-4289-A714-5808F1106EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10671482-6DF1-46E1-B9C4-E189FED29D66}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{6845A9D8-AAB2-4289-A714-5808F1106EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C0B65AB-8D7A-4ECD-8648-864058569A3F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="767">
   <si>
     <t>Species</t>
   </si>
@@ -2339,6 +2339,9 @@
   </si>
   <si>
     <t>Ananas comosus var. microstachys</t>
+  </si>
+  <si>
+    <t>Beta vulgaris subsp. maritima</t>
   </si>
 </sst>
 </file>
@@ -2733,21 +2736,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J344"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="C117" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
     <col min="3" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" customWidth="1"/>
+    <col min="7" max="7" width="42.26171875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.26171875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="35.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2779,7 +2782,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -2811,7 +2814,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4" t="s">
         <v>451</v>
       </c>
@@ -2826,7 +2829,7 @@
       </c>
       <c r="H3" s="12"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2837,7 +2840,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>119</v>
       </c>
@@ -2867,7 +2870,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2908,7 +2911,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2949,7 +2952,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -2979,7 +2982,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4" t="s">
         <v>82</v>
       </c>
@@ -3005,7 +3008,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -3016,7 +3019,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -3027,7 +3030,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -3049,7 +3052,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>72</v>
       </c>
@@ -3073,6 +3076,9 @@
       <c r="D17" s="3" t="s">
         <v>446</v>
       </c>
+      <c r="F17" s="3" t="s">
+        <v>766</v>
+      </c>
       <c r="G17" s="7" t="s">
         <v>239</v>
       </c>
@@ -3086,7 +3092,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -3097,7 +3103,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4" t="s">
         <v>105</v>
       </c>
@@ -3125,7 +3131,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -3139,7 +3145,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
         <v>128</v>
       </c>
@@ -3165,7 +3171,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -3179,7 +3185,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -3190,7 +3196,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -3201,7 +3207,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -3212,7 +3218,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
         <v>108</v>
       </c>
@@ -3238,7 +3244,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
         <v>109</v>
       </c>
@@ -3264,7 +3270,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -3275,7 +3281,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
         <v>59</v>
       </c>
@@ -3301,7 +3307,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -3309,7 +3315,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -3320,7 +3326,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
@@ -3346,7 +3352,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>103</v>
       </c>
@@ -3357,7 +3363,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>96</v>
       </c>
@@ -3368,7 +3374,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="s">
         <v>73</v>
       </c>
@@ -3394,7 +3400,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="s">
         <v>84</v>
       </c>
@@ -3420,7 +3426,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -3431,7 +3437,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3" t="s">
         <v>48</v>
       </c>
@@ -3457,7 +3463,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -3468,7 +3474,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="4" t="s">
         <v>85</v>
       </c>
@@ -3516,7 +3522,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -3530,7 +3536,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -3544,7 +3550,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -3555,7 +3561,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="s">
         <v>121</v>
       </c>
@@ -3581,7 +3587,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -3603,7 +3609,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>106</v>
       </c>
@@ -3614,7 +3620,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -3625,7 +3631,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>87</v>
       </c>
@@ -3636,7 +3642,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="3" customFormat="1" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3" t="s">
         <v>45</v>
       </c>
@@ -3662,7 +3668,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3" t="s">
         <v>45</v>
       </c>
@@ -3682,7 +3688,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3" t="s">
         <v>45</v>
       </c>
@@ -3702,7 +3708,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>45</v>
       </c>
@@ -3716,7 +3722,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3" t="s">
         <v>88</v>
       </c>
@@ -3744,7 +3750,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3" t="s">
         <v>110</v>
       </c>
@@ -3768,7 +3774,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -3779,7 +3785,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
         <v>112</v>
       </c>
@@ -3803,7 +3809,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -3817,7 +3823,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>113</v>
       </c>
@@ -3828,7 +3834,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>114</v>
       </c>
@@ -3839,7 +3845,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
         <v>115</v>
       </c>
@@ -3850,7 +3856,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3" t="s">
         <v>25</v>
       </c>
@@ -3876,7 +3882,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3" t="s">
         <v>24</v>
       </c>
@@ -3900,7 +3906,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -3911,7 +3917,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
         <v>77</v>
       </c>
@@ -3937,7 +3943,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3" t="s">
         <v>89</v>
       </c>
@@ -3960,7 +3966,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3" t="s">
         <v>90</v>
       </c>
@@ -3983,7 +3989,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3" t="s">
         <v>99</v>
       </c>
@@ -4009,7 +4015,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>99</v>
       </c>
@@ -4023,7 +4029,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -4034,7 +4040,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
         <v>91</v>
       </c>
@@ -4060,7 +4066,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>92</v>
       </c>
@@ -4071,7 +4077,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3" t="s">
         <v>100</v>
       </c>
@@ -4097,7 +4103,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>100</v>
       </c>
@@ -4108,7 +4114,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3" t="s">
         <v>67</v>
       </c>
@@ -4134,7 +4140,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>67</v>
       </c>
@@ -4148,7 +4154,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>67</v>
       </c>
@@ -4162,7 +4168,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="3" t="s">
         <v>19</v>
       </c>
@@ -4188,7 +4194,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="3" t="s">
         <v>129</v>
       </c>
@@ -4214,7 +4220,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3" t="s">
         <v>122</v>
       </c>
@@ -4240,7 +4246,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>69</v>
       </c>
@@ -4251,7 +4257,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="3" t="s">
         <v>78</v>
       </c>
@@ -4277,7 +4283,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>78</v>
       </c>
@@ -4288,7 +4294,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>125</v>
       </c>
@@ -4302,7 +4308,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="3" t="s">
         <v>3</v>
       </c>
@@ -4328,7 +4334,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="88" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="3" t="s">
         <v>133</v>
       </c>
@@ -4354,7 +4360,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="3" t="s">
         <v>130</v>
       </c>
@@ -4380,7 +4386,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -4391,7 +4397,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="91" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="3" t="s">
         <v>49</v>
       </c>
@@ -4415,7 +4421,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>118</v>
       </c>
@@ -4426,7 +4432,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="3" t="s">
         <v>51</v>
       </c>
@@ -4452,7 +4458,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>51</v>
       </c>
@@ -4463,7 +4469,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>51</v>
       </c>
@@ -4474,7 +4480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>51</v>
       </c>
@@ -4482,7 +4488,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>51</v>
       </c>
@@ -4490,7 +4496,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="3" t="s">
         <v>94</v>
       </c>
@@ -4516,7 +4522,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -4527,7 +4533,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -4538,7 +4544,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -4549,7 +4555,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="3" t="s">
         <v>131</v>
       </c>
@@ -4575,7 +4581,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="3" t="s">
         <v>132</v>
       </c>
@@ -4601,7 +4607,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
         <v>18</v>
       </c>
@@ -4609,7 +4615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>18</v>
       </c>
@@ -4620,7 +4626,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="106" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="3" t="s">
         <v>18</v>
       </c>
@@ -4646,7 +4652,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="107" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="4" t="s">
         <v>18</v>
       </c>
@@ -4658,7 +4664,7 @@
       </c>
       <c r="H107" s="12"/>
     </row>
-    <row r="108" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="4" t="s">
         <v>79</v>
       </c>
@@ -4670,7 +4676,7 @@
       </c>
       <c r="H108" s="12"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
         <v>31</v>
       </c>
@@ -4684,7 +4690,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>31</v>
       </c>
@@ -4698,7 +4704,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="111" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="4" t="s">
         <v>31</v>
       </c>
@@ -4724,7 +4730,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="112" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="3" t="s">
         <v>75</v>
       </c>
@@ -4750,7 +4756,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="113" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="3" t="s">
         <v>123</v>
       </c>
@@ -4776,7 +4782,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>104</v>
       </c>
@@ -4787,7 +4793,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="115" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="3" t="s">
         <v>27</v>
       </c>
@@ -4813,7 +4819,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="116" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="3" t="s">
         <v>95</v>
       </c>
@@ -4839,7 +4845,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="117" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="3" t="s">
         <v>23</v>
       </c>
@@ -4865,7 +4871,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="118" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="3" t="s">
         <v>32</v>
       </c>
@@ -4891,7 +4897,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>80</v>
       </c>
@@ -4902,7 +4908,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>97</v>
       </c>
@@ -4913,7 +4919,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -4921,7 +4927,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="3" t="s">
         <v>10</v>
       </c>
@@ -4947,7 +4953,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>10</v>
       </c>
@@ -4955,7 +4961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>10</v>
       </c>
@@ -4963,7 +4969,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="3" t="s">
         <v>9</v>
       </c>
@@ -4989,7 +4995,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="126" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="3" t="s">
         <v>9</v>
       </c>
@@ -5004,7 +5010,7 @@
       </c>
       <c r="H126" s="10"/>
     </row>
-    <row r="127" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="3" t="s">
         <v>9</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="128" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="3" t="s">
         <v>9</v>
       </c>
@@ -5034,7 +5040,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>124</v>
       </c>
@@ -5045,7 +5051,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="130" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="3" t="s">
         <v>160</v>
       </c>
@@ -5057,6 +5063,9 @@
       </c>
       <c r="D130" s="3" t="s">
         <v>318</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="G130" s="7"/>
       <c r="H130" s="10">
@@ -5069,7 +5078,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>160</v>
       </c>
@@ -5083,7 +5092,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="132" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="3" t="s">
         <v>308</v>
       </c>
@@ -5112,7 +5121,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="133" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="3" t="s">
         <v>310</v>
       </c>
@@ -5139,7 +5148,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="134" spans="1:10" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="3" t="s">
         <v>313</v>
       </c>
@@ -5163,7 +5172,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="135" spans="1:10" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="3" t="s">
         <v>314</v>
       </c>
@@ -5187,7 +5196,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="136" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="4" t="s">
         <v>309</v>
       </c>
@@ -5213,7 +5222,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="137" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="4" t="s">
         <v>324</v>
       </c>
@@ -5239,7 +5248,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="138" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="4" t="s">
         <v>326</v>
       </c>
@@ -5265,7 +5274,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="139" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="3" t="s">
         <v>330</v>
       </c>
@@ -5288,7 +5297,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
         <v>330</v>
       </c>
@@ -5314,7 +5323,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>333</v>
       </c>
@@ -5325,7 +5334,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
         <v>334</v>
       </c>
@@ -5333,7 +5342,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
         <v>336</v>
       </c>
@@ -5341,7 +5350,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="144" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="4" t="s">
         <v>340</v>
       </c>
@@ -5367,7 +5376,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
         <v>343</v>
       </c>
@@ -5375,7 +5384,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="146" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="3" t="s">
         <v>344</v>
       </c>
@@ -5398,7 +5407,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>98</v>
       </c>
@@ -5406,7 +5415,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="148" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="3" t="s">
         <v>347</v>
       </c>
@@ -5430,7 +5439,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
         <v>350</v>
       </c>
@@ -5441,7 +5450,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
         <v>352</v>
       </c>
@@ -5452,7 +5461,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="151" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="3" t="s">
         <v>355</v>
       </c>
@@ -5476,7 +5485,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="152" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="3" t="s">
         <v>356</v>
       </c>
@@ -5502,7 +5511,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
         <v>357</v>
       </c>
@@ -5513,7 +5522,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
         <v>358</v>
       </c>
@@ -5524,7 +5533,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
         <v>359</v>
       </c>
@@ -5535,7 +5544,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="156" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="4" t="s">
         <v>361</v>
       </c>
@@ -5558,7 +5567,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
         <v>363</v>
       </c>
@@ -5566,7 +5575,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
         <v>364</v>
       </c>
@@ -5574,7 +5583,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="159" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="3" t="s">
         <v>366</v>
       </c>
@@ -5598,7 +5607,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
         <v>369</v>
       </c>
@@ -5609,7 +5618,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
         <v>370</v>
       </c>
@@ -5620,7 +5629,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="162" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="3" t="s">
         <v>371</v>
       </c>
@@ -5644,7 +5653,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
         <v>374</v>
       </c>
@@ -5652,7 +5661,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
         <v>375</v>
       </c>
@@ -5660,7 +5669,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="165" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="3" t="s">
         <v>376</v>
       </c>
@@ -5684,7 +5693,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
         <v>376</v>
       </c>
@@ -5701,7 +5710,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="167" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="4" t="s">
         <v>380</v>
       </c>
@@ -5724,7 +5733,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="168" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="3" t="s">
         <v>383</v>
       </c>
@@ -5745,7 +5754,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="169" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="4" t="s">
         <v>387</v>
       </c>
@@ -5768,7 +5777,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="170" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="4" t="s">
         <v>388</v>
       </c>
@@ -5791,7 +5800,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="171" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="4" t="s">
         <v>391</v>
       </c>
@@ -5814,7 +5823,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
         <v>392</v>
       </c>
@@ -5825,7 +5834,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="173" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="4" t="s">
         <v>394</v>
       </c>
@@ -5848,7 +5857,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="174" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="3" t="s">
         <v>398</v>
       </c>
@@ -5874,7 +5883,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
         <v>401</v>
       </c>
@@ -5882,7 +5891,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="176" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="3" t="s">
         <v>402</v>
       </c>
@@ -5905,7 +5914,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
         <v>404</v>
       </c>
@@ -5913,7 +5922,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
         <v>406</v>
       </c>
@@ -5921,7 +5930,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="179" spans="1:10" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="3" t="s">
         <v>407</v>
       </c>
@@ -5944,7 +5953,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="180" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="3" t="s">
         <v>410</v>
       </c>
@@ -5970,7 +5979,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
         <v>414</v>
       </c>
@@ -5981,7 +5990,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="182" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="3" t="s">
         <v>418</v>
       </c>
@@ -6004,7 +6013,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
         <v>420</v>
       </c>
@@ -6012,7 +6021,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
         <v>421</v>
       </c>
@@ -6020,7 +6029,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
         <v>422</v>
       </c>
@@ -6028,7 +6037,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
         <v>424</v>
       </c>
@@ -6036,7 +6045,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="187" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="3" t="s">
         <v>426</v>
       </c>
@@ -6062,7 +6071,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="188" spans="1:10" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="3" t="s">
         <v>430</v>
       </c>
@@ -6085,7 +6094,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" t="s">
         <v>431</v>
       </c>
@@ -6096,7 +6105,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" t="s">
         <v>434</v>
       </c>
@@ -6104,7 +6113,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" t="s">
         <v>435</v>
       </c>
@@ -6112,7 +6121,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="192" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="3" t="s">
         <v>438</v>
       </c>
@@ -6133,7 +6142,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" t="s">
         <v>97</v>
       </c>
@@ -6144,7 +6153,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" t="s">
         <v>97</v>
       </c>
@@ -6155,7 +6164,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="195" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A195" s="3" t="s">
         <v>97</v>
       </c>
@@ -6178,7 +6187,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A196" t="s">
         <v>164</v>
       </c>
@@ -6192,7 +6201,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A197" t="s">
         <v>168</v>
       </c>
@@ -6203,7 +6212,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="198" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A198" s="3" t="s">
         <v>242</v>
       </c>
@@ -6227,7 +6236,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A199" t="s">
         <v>242</v>
       </c>
@@ -6238,7 +6247,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A200" t="s">
         <v>261</v>
       </c>
@@ -6246,7 +6255,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A201" t="s">
         <v>262</v>
       </c>
@@ -6254,7 +6263,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A202" t="s">
         <v>39</v>
       </c>
@@ -6265,7 +6274,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A203" t="s">
         <v>457</v>
       </c>
@@ -6276,7 +6285,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A204" t="s">
         <v>458</v>
       </c>
@@ -6287,7 +6296,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A205" t="s">
         <v>459</v>
       </c>
@@ -6298,7 +6307,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A206" t="s">
         <v>460</v>
       </c>
@@ -6309,7 +6318,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="207" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A207" s="3" t="s">
         <v>461</v>
       </c>
@@ -6336,7 +6345,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="208" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A208" s="3" t="s">
         <v>462</v>
       </c>
@@ -6354,7 +6363,7 @@
       </c>
       <c r="H208" s="10"/>
     </row>
-    <row r="209" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A209" s="3" t="s">
         <v>463</v>
       </c>
@@ -6380,7 +6389,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="210" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A210" s="3" t="s">
         <v>464</v>
       </c>
@@ -6406,7 +6415,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A211" t="s">
         <v>465</v>
       </c>
@@ -6417,7 +6426,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" t="s">
         <v>466</v>
       </c>
@@ -6428,7 +6437,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="213" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="3" t="s">
         <v>467</v>
       </c>
@@ -6452,7 +6461,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" t="s">
         <v>468</v>
       </c>
@@ -6463,7 +6472,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="215" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="3" t="s">
         <v>469</v>
       </c>
@@ -6487,7 +6496,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="216" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="3" t="s">
         <v>470</v>
       </c>
@@ -6513,7 +6522,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="217" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="3" t="s">
         <v>471</v>
       </c>
@@ -6539,7 +6548,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" t="s">
         <v>472</v>
       </c>
@@ -6550,7 +6559,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="219" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="3" t="s">
         <v>473</v>
       </c>
@@ -6576,7 +6585,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="220" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" t="s">
         <v>474</v>
       </c>
@@ -6587,7 +6596,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" t="s">
         <v>475</v>
       </c>
@@ -6601,7 +6610,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="222" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="3" t="s">
         <v>476</v>
       </c>
@@ -6627,7 +6636,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="223" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" t="s">
         <v>477</v>
       </c>
@@ -6638,7 +6647,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" t="s">
         <v>478</v>
       </c>
@@ -6649,7 +6658,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="225" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="3" t="s">
         <v>479</v>
       </c>
@@ -6675,7 +6684,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="226" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" t="s">
         <v>480</v>
       </c>
@@ -6689,7 +6698,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="227" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" t="s">
         <v>481</v>
       </c>
@@ -6700,7 +6709,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="228" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" s="3" t="s">
         <v>482</v>
       </c>
@@ -6726,7 +6735,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="229" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" t="s">
         <v>483</v>
       </c>
@@ -6737,7 +6746,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" t="s">
         <v>484</v>
       </c>
@@ -6748,7 +6757,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="s">
         <v>485</v>
       </c>
@@ -6759,7 +6768,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" t="s">
         <v>486</v>
       </c>
@@ -6770,7 +6779,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="233" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" t="s">
         <v>487</v>
       </c>
@@ -6781,7 +6790,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="234" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" t="s">
         <v>488</v>
       </c>
@@ -6795,7 +6804,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" t="s">
         <v>489</v>
       </c>
@@ -6806,7 +6815,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="236" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="3" t="s">
         <v>490</v>
       </c>
@@ -6832,7 +6841,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="237" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="3" t="s">
         <v>491</v>
       </c>
@@ -6858,7 +6867,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="238" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="3" t="s">
         <v>492</v>
       </c>
@@ -6881,7 +6890,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="239" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" t="s">
         <v>493</v>
       </c>
@@ -6898,7 +6907,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" t="s">
         <v>494</v>
       </c>
@@ -6909,7 +6918,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" t="s">
         <v>495</v>
       </c>
@@ -6920,7 +6929,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" t="s">
         <v>496</v>
       </c>
@@ -6931,7 +6940,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="243" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="3" t="s">
         <v>497</v>
       </c>
@@ -6957,7 +6966,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" t="s">
         <v>498</v>
       </c>
@@ -6968,7 +6977,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" t="s">
         <v>499</v>
       </c>
@@ -6979,7 +6988,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" t="s">
         <v>500</v>
       </c>
@@ -6990,7 +6999,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" t="s">
         <v>501</v>
       </c>
@@ -7001,7 +7010,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" t="s">
         <v>502</v>
       </c>
@@ -7012,7 +7021,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" t="s">
         <v>503</v>
       </c>
@@ -7023,7 +7032,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" t="s">
         <v>504</v>
       </c>
@@ -7034,7 +7043,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" t="s">
         <v>505</v>
       </c>
@@ -7045,7 +7054,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A252" t="s">
         <v>506</v>
       </c>
@@ -7056,7 +7065,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A253" t="s">
         <v>507</v>
       </c>
@@ -7067,7 +7076,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A254" t="s">
         <v>508</v>
       </c>
@@ -7078,7 +7087,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="255" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A255" s="3" t="s">
         <v>509</v>
       </c>
@@ -7104,7 +7113,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" t="s">
         <v>510</v>
       </c>
@@ -7115,7 +7124,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="257" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" t="s">
         <v>511</v>
       </c>
@@ -7126,7 +7135,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" t="s">
         <v>512</v>
       </c>
@@ -7137,7 +7146,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="259" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" t="s">
         <v>513</v>
       </c>
@@ -7148,7 +7157,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" t="s">
         <v>514</v>
       </c>
@@ -7159,7 +7168,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" t="s">
         <v>515</v>
       </c>
@@ -7170,7 +7179,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A262" t="s">
         <v>516</v>
       </c>
@@ -7181,7 +7190,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="263" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A263" s="3" t="s">
         <v>517</v>
       </c>
@@ -7205,7 +7214,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="264" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A264" s="3" t="s">
         <v>518</v>
       </c>
@@ -7231,7 +7240,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="265" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A265" s="3" t="s">
         <v>519</v>
       </c>
@@ -7257,7 +7266,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="266" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A266" s="3" t="s">
         <v>520</v>
       </c>
@@ -7283,7 +7292,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" t="s">
         <v>521</v>
       </c>
@@ -7294,7 +7303,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" t="s">
         <v>522</v>
       </c>
@@ -7305,7 +7314,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" t="s">
         <v>523</v>
       </c>
@@ -7316,7 +7325,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="270" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A270" t="s">
         <v>524</v>
       </c>
@@ -7330,7 +7339,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="271" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A271" s="3" t="s">
         <v>525</v>
       </c>
@@ -7353,7 +7362,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A272" t="s">
         <v>526</v>
       </c>
@@ -7364,7 +7373,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A273" t="s">
         <v>527</v>
       </c>
@@ -7375,7 +7384,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="274" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A274" s="3" t="s">
         <v>528</v>
       </c>
@@ -7401,7 +7410,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A275" t="s">
         <v>529</v>
       </c>
@@ -7412,7 +7421,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A276" t="s">
         <v>530</v>
       </c>
@@ -7423,7 +7432,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" t="s">
         <v>531</v>
       </c>
@@ -7434,7 +7443,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" t="s">
         <v>532</v>
       </c>
@@ -7445,7 +7454,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" t="s">
         <v>533</v>
       </c>
@@ -7456,7 +7465,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" t="s">
         <v>534</v>
       </c>
@@ -7467,7 +7476,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="281" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" t="s">
         <v>535</v>
       </c>
@@ -7478,7 +7487,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" t="s">
         <v>536</v>
       </c>
@@ -7489,7 +7498,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="283" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="3" t="s">
         <v>537</v>
       </c>
@@ -7515,7 +7524,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="284" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" t="s">
         <v>538</v>
       </c>
@@ -7526,7 +7535,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" t="s">
         <v>539</v>
       </c>
@@ -7537,7 +7546,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" t="s">
         <v>540</v>
       </c>
@@ -7548,7 +7557,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="287" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="3" t="s">
         <v>541</v>
       </c>
@@ -7574,7 +7583,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" t="s">
         <v>542</v>
       </c>
@@ -7588,7 +7597,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" t="s">
         <v>543</v>
       </c>
@@ -7599,7 +7608,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="290" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="3" t="s">
         <v>544</v>
       </c>
@@ -7625,7 +7634,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" t="s">
         <v>545</v>
       </c>
@@ -7636,7 +7645,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="292" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="3" t="s">
         <v>546</v>
       </c>
@@ -7662,7 +7671,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" t="s">
         <v>547</v>
       </c>
@@ -7673,7 +7682,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="294" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="3" t="s">
         <v>548</v>
       </c>
@@ -7697,7 +7706,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" t="s">
         <v>549</v>
       </c>
@@ -7708,7 +7717,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" t="s">
         <v>550</v>
       </c>
@@ -7719,7 +7728,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" t="s">
         <v>551</v>
       </c>
@@ -7730,7 +7739,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" t="s">
         <v>552</v>
       </c>
@@ -7741,7 +7750,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" t="s">
         <v>553</v>
       </c>
@@ -7752,7 +7761,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A300" t="s">
         <v>554</v>
       </c>
@@ -7763,7 +7772,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A301" t="s">
         <v>555</v>
       </c>
@@ -7774,7 +7783,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="302" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" t="s">
         <v>556</v>
       </c>
@@ -7785,7 +7794,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="303" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" s="3" t="s">
         <v>557</v>
       </c>
@@ -7809,7 +7818,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" t="s">
         <v>558</v>
       </c>
@@ -7820,7 +7829,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="305" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" s="3" t="s">
         <v>559</v>
       </c>
@@ -7844,7 +7853,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" t="s">
         <v>560</v>
       </c>
@@ -7855,7 +7864,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" t="s">
         <v>561</v>
       </c>
@@ -7866,7 +7875,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" t="s">
         <v>562</v>
       </c>
@@ -7877,7 +7886,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="309" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" s="3" t="s">
         <v>563</v>
       </c>
@@ -7901,7 +7910,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" t="s">
         <v>564</v>
       </c>
@@ -7915,7 +7924,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="311" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" s="3" t="s">
         <v>565</v>
       </c>
@@ -7939,7 +7948,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" t="s">
         <v>566</v>
       </c>
@@ -7950,7 +7959,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="313" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" s="3" t="s">
         <v>261</v>
       </c>
@@ -7976,7 +7985,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="314" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" s="3" t="s">
         <v>567</v>
       </c>
@@ -7994,7 +8003,7 @@
       </c>
       <c r="H314" s="10"/>
     </row>
-    <row r="315" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" t="s">
         <v>568</v>
       </c>
@@ -8005,7 +8014,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="316" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" s="3" t="s">
         <v>569</v>
       </c>
@@ -8031,7 +8040,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" t="s">
         <v>570</v>
       </c>
@@ -8042,7 +8051,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="318" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" s="3" t="s">
         <v>571</v>
       </c>
@@ -8068,7 +8077,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="319" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" s="3" t="s">
         <v>572</v>
       </c>
@@ -8092,7 +8101,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="320" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" s="3" t="s">
         <v>677</v>
       </c>
@@ -8118,7 +8127,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" t="s">
         <v>678</v>
       </c>
@@ -8129,7 +8138,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="322" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" s="4" t="s">
         <v>679</v>
       </c>
@@ -8155,7 +8164,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" t="s">
         <v>680</v>
       </c>
@@ -8166,7 +8175,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" t="s">
         <v>375</v>
       </c>
@@ -8177,7 +8186,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" t="s">
         <v>681</v>
       </c>
@@ -8188,7 +8197,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="326" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" s="4" t="s">
         <v>682</v>
       </c>
@@ -8214,7 +8223,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" t="s">
         <v>683</v>
       </c>
@@ -8225,7 +8234,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>684</v>
       </c>
@@ -8236,7 +8245,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="329" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" s="3" t="s">
         <v>685</v>
       </c>
@@ -8260,7 +8269,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" t="s">
         <v>686</v>
       </c>
@@ -8271,7 +8280,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" t="s">
         <v>707</v>
       </c>
@@ -8282,7 +8291,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>708</v>
       </c>
@@ -8293,7 +8302,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" t="s">
         <v>468</v>
       </c>
@@ -8304,7 +8313,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="334" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" s="3" t="s">
         <v>709</v>
       </c>
@@ -8330,7 +8339,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" t="s">
         <v>710</v>
       </c>
@@ -8341,7 +8350,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" t="s">
         <v>711</v>
       </c>
@@ -8352,7 +8361,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" t="s">
         <v>712</v>
       </c>
@@ -8363,7 +8372,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" t="s">
         <v>713</v>
       </c>
@@ -8374,7 +8383,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" t="s">
         <v>714</v>
       </c>
@@ -8385,7 +8394,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="340" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" s="3" t="s">
         <v>715</v>
       </c>
@@ -8411,7 +8420,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" t="s">
         <v>716</v>
       </c>
@@ -8422,7 +8431,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>717</v>
       </c>
@@ -8433,12 +8442,12 @@
         <v>695</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D343" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D344" t="s">
         <v>723</v>
       </c>
@@ -8469,797 +8478,797 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="14" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="14" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="14" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="14" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="14" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="14" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="14" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="14" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="14" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="14" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="14" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="14" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="14" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="14" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="14" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="14" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="14" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="14" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="14" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="14" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="14" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="14" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="14" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="14" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="14" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="14" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="14" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="14" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="14" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="14" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="14" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="14" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="14" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="14" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="14" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="14" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="14" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="14" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="14" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="14" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="14" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="14" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="14" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="14" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="14" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="14" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="14" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="14" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="14" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="14" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="14" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="14" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="14" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="14" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="14" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="14" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="14" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="14" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="14" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="14" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="14" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="14" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="14" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="14" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="14" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="14" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="14" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="14" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="14" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="14" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="14" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="14" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="14" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="14" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="14" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="14" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="14" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="14" t="s">
         <v>242</v>
       </c>
@@ -9278,13 +9287,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="38.15625" customWidth="1"/>
+    <col min="2" max="2" width="35.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>675</v>
       </c>
@@ -9295,22 +9304,22 @@
         <v>687</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
@@ -9321,7 +9330,7 @@
         <v>3052450</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -9332,7 +9341,7 @@
         <v>3052468</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>461</v>
       </c>
@@ -9343,7 +9352,7 @@
         <v>3052544</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -9354,7 +9363,7 @@
         <v>3052436</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>160</v>
       </c>
@@ -9365,7 +9374,7 @@
         <v>5375020</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>462</v>
       </c>
@@ -9376,32 +9385,32 @@
         <v>5374933</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>105</v>
       </c>
@@ -9412,7 +9421,7 @@
         <v>3043392</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>128</v>
       </c>
@@ -9423,7 +9432,7 @@
         <v>5290143</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>313</v>
       </c>
@@ -9434,7 +9443,7 @@
         <v>9073641</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>314</v>
       </c>
@@ -9445,7 +9454,7 @@
         <v>3042888</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
         <v>108</v>
       </c>
@@ -9456,7 +9465,7 @@
         <v>3042837</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
         <v>109</v>
       </c>
@@ -9467,27 +9476,27 @@
         <v>7903057</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
         <v>59</v>
       </c>
@@ -9498,7 +9507,7 @@
         <v>5375387</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
@@ -9509,87 +9518,87 @@
         <v>5375425</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3" t="s">
         <v>88</v>
       </c>
@@ -9597,82 +9606,82 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3" t="s">
         <v>19</v>
       </c>
@@ -9680,242 +9689,242 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="4" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="4" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="4" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="4" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="4" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="3" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="3" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="3" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="3" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="3" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="3" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="3" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="3" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="3" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="3" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="3" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="3" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="3" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="3" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="3" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="3" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="3" t="s">
         <v>572</v>
       </c>

</xml_diff>

<commit_message>
refine SNP and k-mer filters
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/1116386_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopcki7fh5/RemoteFiles/1116386_2_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{6845A9D8-AAB2-4289-A714-5808F1106EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C0B65AB-8D7A-4ECD-8648-864058569A3F}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="13_ncr:1_{6845A9D8-AAB2-4289-A714-5808F1106EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A21D7B5-EEF4-4EC8-94C1-AA9EB389DD96}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="770">
   <si>
     <t>Species</t>
   </si>
@@ -2342,6 +2342,15 @@
   </si>
   <si>
     <t>Beta vulgaris subsp. maritima</t>
+  </si>
+  <si>
+    <t>Arachis stenosperma</t>
+  </si>
+  <si>
+    <t>Benincasa pruriens</t>
+  </si>
+  <si>
+    <t>I think B. hispida and B. pruriens could be the same species…</t>
   </si>
 </sst>
 </file>
@@ -2736,8 +2745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C117" workbookViewId="0">
-      <selection activeCell="F131" sqref="F131"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2995,6 +3004,9 @@
       <c r="D11" s="4" t="s">
         <v>446</v>
       </c>
+      <c r="F11" s="4" t="s">
+        <v>767</v>
+      </c>
       <c r="G11" s="13" t="s">
         <v>760</v>
       </c>
@@ -3117,7 +3129,9 @@
         <v>446</v>
       </c>
       <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="F19" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="G19" s="13" t="s">
         <v>724</v>
       </c>
@@ -6358,6 +6372,9 @@
       <c r="D208" s="3" t="s">
         <v>456</v>
       </c>
+      <c r="F208" s="3" t="s">
+        <v>462</v>
+      </c>
       <c r="G208" s="7" t="s">
         <v>576</v>
       </c>
@@ -6437,7 +6454,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="213" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:10" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="3" t="s">
         <v>467</v>
       </c>
@@ -6450,7 +6467,12 @@
       <c r="D213" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="G213" s="7"/>
+      <c r="F213" s="3" t="s">
+        <v>768</v>
+      </c>
+      <c r="G213" s="7" t="s">
+        <v>769</v>
+      </c>
       <c r="H213" s="10">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
remove seqkit stats rule so temp files delete sooner
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\197478_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\133162_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FB87D9-D7BB-413E-9A14-BC8826F0C24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F2541A-E374-44C5-A922-679436B8CC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2754,8 +2754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update input to 9 species with little data
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\133162_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\263300_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F2541A-E374-44C5-A922-679436B8CC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572143A8-F737-4A98-BD46-B5CF2B5EDA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="777">
   <si>
     <t>Species</t>
   </si>
@@ -2360,6 +2360,18 @@
   </si>
   <si>
     <t>Hopping ME.,1994</t>
+  </si>
+  <si>
+    <t>Camelina rumelica; Camelina hispida</t>
+  </si>
+  <si>
+    <t>Nicotiana sylvestris</t>
+  </si>
+  <si>
+    <t>Brassica nigra</t>
+  </si>
+  <si>
+    <t>Ficus erecta</t>
   </si>
 </sst>
 </file>
@@ -2754,8 +2766,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B133" sqref="B133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5274,6 +5288,9 @@
       <c r="D137" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="F137" s="4" t="s">
+        <v>773</v>
+      </c>
       <c r="I137" s="13" t="s">
         <v>325</v>
       </c>
@@ -5593,6 +5610,9 @@
       <c r="D156" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="F156" s="4" t="s">
+        <v>776</v>
+      </c>
       <c r="I156" s="13" t="s">
         <v>362</v>
       </c>
@@ -5883,6 +5903,9 @@
       <c r="D173" s="4" t="s">
         <v>318</v>
       </c>
+      <c r="F173" s="4" t="s">
+        <v>394</v>
+      </c>
       <c r="I173" s="13" t="s">
         <v>396</v>
       </c>
@@ -7854,6 +7877,9 @@
       <c r="D303" s="3" t="s">
         <v>456</v>
       </c>
+      <c r="F303" s="3" t="s">
+        <v>557</v>
+      </c>
       <c r="I303" s="7" t="s">
         <v>596</v>
       </c>
@@ -8257,6 +8283,9 @@
       <c r="D326" s="4" t="s">
         <v>691</v>
       </c>
+      <c r="F326" s="4" t="s">
+        <v>774</v>
+      </c>
       <c r="I326" s="13" t="s">
         <v>702</v>
       </c>
@@ -8372,6 +8401,9 @@
       </c>
       <c r="D334" s="3" t="s">
         <v>705</v>
+      </c>
+      <c r="F334" s="3" t="s">
+        <v>775</v>
       </c>
       <c r="I334" s="7" t="s">
         <v>720</v>

</xml_diff>

<commit_message>
filter out sites with super high depth
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\263300_2_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/722550_2_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0921E56B-32A3-4FCD-A9CD-38BE1A074ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{0921E56B-32A3-4FCD-A9CD-38BE1A074ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F31C0E9-0105-4A55-A389-1A5D3DB17692}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="781">
   <si>
     <t>Species</t>
   </si>
@@ -2372,15 +2372,24 @@
   </si>
   <si>
     <t>Ficus erecta</t>
+  </si>
+  <si>
+    <t>Snakemake output aquired?</t>
+  </si>
+  <si>
+    <t>Cercis canadensis</t>
+  </si>
+  <si>
+    <t>Brachypodium arbuscula</t>
+  </si>
+  <si>
+    <t>Brachypodium sylvaticum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;''&quot;@&quot;''&quot;\,"/>
-  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2451,7 +2460,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2480,7 +2489,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
@@ -2764,12 +2772,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L344"/>
+  <dimension ref="A1:M348"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A156" sqref="A156"/>
+      <selection pane="bottomLeft" activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2780,9 +2788,10 @@
     <col min="9" max="9" width="42.28515625" style="6" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" style="9" customWidth="1"/>
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2819,8 +2828,11 @@
       <c r="L1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -2852,7 +2864,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>451</v>
       </c>
@@ -2867,7 +2879,7 @@
       </c>
       <c r="J3" s="12"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2878,7 +2890,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>119</v>
       </c>
@@ -2908,7 +2920,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -2919,7 +2931,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -2949,7 +2961,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -2976,7 +2988,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2990,7 +3002,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -3020,7 +3032,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>82</v>
       </c>
@@ -3049,7 +3061,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -3060,7 +3072,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -3071,7 +3083,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -3082,7 +3094,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -3093,7 +3105,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -3151,13 +3163,13 @@
       <c r="B19" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="E19" s="15"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="4" t="s">
         <v>105</v>
       </c>
@@ -3373,7 +3385,7 @@
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>246</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -5677,7 +5689,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>370</v>
       </c>
@@ -5688,7 +5700,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="162" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>371</v>
       </c>
@@ -5712,7 +5724,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>374</v>
       </c>
@@ -5720,7 +5732,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>375</v>
       </c>
@@ -5728,7 +5740,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="165" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>376</v>
       </c>
@@ -5752,7 +5764,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>376</v>
       </c>
@@ -5769,7 +5781,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="167" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>380</v>
       </c>
@@ -5792,7 +5804,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="168" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>383</v>
       </c>
@@ -5813,7 +5825,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="169" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>387</v>
       </c>
@@ -5836,7 +5848,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="170" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>388</v>
       </c>
@@ -5859,7 +5871,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="171" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>391</v>
       </c>
@@ -5882,7 +5894,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>392</v>
       </c>
@@ -5893,7 +5905,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="173" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>394</v>
       </c>
@@ -5918,8 +5930,11 @@
       <c r="L173" s="4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="174" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="M173" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
         <v>398</v>
       </c>
@@ -5945,7 +5960,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>401</v>
       </c>
@@ -5953,7 +5968,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="176" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
         <v>402</v>
       </c>
@@ -6204,7 +6219,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>97</v>
       </c>
@@ -6215,7 +6230,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>97</v>
       </c>
@@ -6226,7 +6241,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="195" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
         <v>97</v>
       </c>
@@ -6249,7 +6264,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>164</v>
       </c>
@@ -6263,7 +6278,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>168</v>
       </c>
@@ -6274,7 +6289,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="198" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3" t="s">
         <v>242</v>
       </c>
@@ -6298,7 +6313,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>242</v>
       </c>
@@ -6309,7 +6324,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>261</v>
       </c>
@@ -6317,7 +6332,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>262</v>
       </c>
@@ -6325,7 +6340,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>39</v>
       </c>
@@ -6336,7 +6351,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>457</v>
       </c>
@@ -6347,7 +6362,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>458</v>
       </c>
@@ -6358,7 +6373,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>459</v>
       </c>
@@ -6369,7 +6384,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>460</v>
       </c>
@@ -6380,7 +6395,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="207" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3" t="s">
         <v>461</v>
       </c>
@@ -6406,8 +6421,11 @@
       <c r="L207" s="3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M207" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3" t="s">
         <v>462</v>
       </c>
@@ -6427,8 +6445,11 @@
         <v>576</v>
       </c>
       <c r="J208" s="10"/>
-    </row>
-    <row r="209" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="M208" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>463</v>
       </c>
@@ -6454,7 +6475,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="210" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>464</v>
       </c>
@@ -6479,8 +6500,11 @@
       <c r="L210" s="3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M210" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>465</v>
       </c>
@@ -6491,7 +6515,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>466</v>
       </c>
@@ -6502,7 +6526,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="213" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>467</v>
       </c>
@@ -6531,7 +6555,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>468</v>
       </c>
@@ -6542,7 +6566,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="215" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>469</v>
       </c>
@@ -6566,7 +6590,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="216" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>470</v>
       </c>
@@ -6592,7 +6616,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="217" spans="1:12" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>471</v>
       </c>
@@ -6618,7 +6642,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>472</v>
       </c>
@@ -6629,7 +6653,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="219" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>473</v>
       </c>
@@ -6655,7 +6679,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="220" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>474</v>
       </c>
@@ -6666,7 +6690,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>475</v>
       </c>
@@ -6680,7 +6704,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="222" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>476</v>
       </c>
@@ -6706,7 +6730,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>477</v>
       </c>
@@ -6717,7 +6741,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>478</v>
       </c>
@@ -8521,13 +8545,53 @@
         <v>695</v>
       </c>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D343" t="s">
+    <row r="343" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D343" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I343" s="13"/>
+      <c r="J343" s="12"/>
+    </row>
+    <row r="344" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="D344" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I344" s="13"/>
+      <c r="J344" s="12"/>
+    </row>
+    <row r="345" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="4" t="s">
+        <v>779</v>
+      </c>
+      <c r="D345" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I345" s="13"/>
+      <c r="J345" s="12"/>
+    </row>
+    <row r="346" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="4" t="s">
+        <v>780</v>
+      </c>
+      <c r="D346" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I346" s="13"/>
+      <c r="J346" s="12"/>
+    </row>
+    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D347" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D344" t="s">
+    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D348" t="s">
         <v>723</v>
       </c>
     </row>
@@ -8551,805 +8615,2136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA0D188-8CB9-4E9E-A4CF-6AB440175DE3}">
-  <dimension ref="A1:A158"/>
+  <dimension ref="A1:C268"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B61" s="3">
+        <v>1</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B62" s="4">
+        <v>1</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B63" s="4">
+        <v>1</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B64" s="4">
+        <v>1</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>330</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B70" s="4">
+        <v>1</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B72" s="3">
+        <v>1</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14" t="s">
+    <row r="74" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B74" s="3">
+        <v>1</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B78" s="3">
+        <v>1</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B82" s="4">
+        <v>1</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B85" s="3">
+        <v>1</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B88" s="3">
+        <v>1</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B93" s="4">
+        <v>1</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B95" s="4">
+        <v>1</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B96" s="4">
+        <v>1</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="B97" s="4">
+        <v>1</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B99" s="4">
+        <v>1</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B100" s="3">
+        <v>1</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B102" s="3">
+        <v>1</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B105" s="3">
+        <v>1</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B106" s="3">
+        <v>1</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="B108" s="3">
+        <v>1</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B113" s="3">
+        <v>1</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B114" s="3">
+        <v>1</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B118" s="3">
+        <v>1</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="14" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="14" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="14" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="14" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="14" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="14" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="14" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="14" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="14" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="14" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="14" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="14" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="14" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B121" s="3">
+        <v>1</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B124" s="3">
+        <v>1</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B133" s="3">
+        <v>1</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B135" s="3">
+        <v>1</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B136" s="3">
+        <v>1</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B139" s="3">
+        <v>1</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B141" s="3">
+        <v>1</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B142" s="3">
+        <v>1</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B143" s="3">
+        <v>1</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B145" s="3">
+        <v>1</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B148" s="3">
+        <v>1</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B151" s="3">
+        <v>1</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="B154" s="3">
+        <v>1</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B162" s="3">
+        <v>1</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B163" s="3">
+        <v>1</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B164" s="3">
+        <v>1</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B169" s="3">
+        <v>1</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B181" s="3">
+        <v>1</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="B189" s="3">
+        <v>1</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="B190" s="3">
+        <v>1</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="B191" s="3">
+        <v>1</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="B192" s="3">
+        <v>1</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B197" s="3">
+        <v>1</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="B200" s="3">
+        <v>1</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B209" s="3">
+        <v>1</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="B213" s="3">
+        <v>1</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B216" s="3">
+        <v>1</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B218" s="3">
+        <v>1</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B220" s="3">
+        <v>1</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="B229" s="3">
+        <v>1</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="B231" s="3">
+        <v>1</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="B235" s="3">
+        <v>1</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="B237" s="3">
+        <v>1</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B239" s="3">
+        <v>1</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B242" s="3">
+        <v>1</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="B244" s="3">
+        <v>1</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B245" s="3">
+        <v>1</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="B246" s="3">
+        <v>1</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="B248" s="4">
+        <v>1</v>
+      </c>
+      <c r="C248" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="14" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="14" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="14" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="14" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="14" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="14" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="14" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="14" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="14" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="14" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="14" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="14" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="14" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="14" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="14" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="14" t="s">
-        <v>242</v>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="B252" s="4">
+        <v>1</v>
+      </c>
+      <c r="C252" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B255" s="3">
+        <v>1</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="B260" s="3">
+        <v>1</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="B266" s="3">
+        <v>1</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
count number of variant and invariant sites
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/722550_2_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{0921E56B-32A3-4FCD-A9CD-38BE1A074ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F31C0E9-0105-4A55-A389-1A5D3DB17692}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{0921E56B-32A3-4FCD-A9CD-38BE1A074ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B63024E-BF73-42C1-9E6E-FA564887B6DA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="781">
   <si>
     <t>Species</t>
   </si>
@@ -2774,10 +2774,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M60" sqref="M60"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6449,7 +6449,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="209" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>463</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="210" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
         <v>464</v>
       </c>
@@ -6500,11 +6500,8 @@
       <c r="L210" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="M210" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>465</v>
       </c>
@@ -6515,7 +6512,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>466</v>
       </c>
@@ -6526,7 +6523,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="213" spans="1:13" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A213" s="3" t="s">
         <v>467</v>
       </c>
@@ -6555,7 +6552,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>468</v>
       </c>
@@ -6566,7 +6563,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="215" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3" t="s">
         <v>469</v>
       </c>
@@ -6590,7 +6587,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="216" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
         <v>470</v>
       </c>
@@ -6616,7 +6613,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="217" spans="1:13" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A217" s="3" t="s">
         <v>471</v>
       </c>
@@ -6642,7 +6639,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>472</v>
       </c>
@@ -6653,7 +6650,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="219" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
         <v>473</v>
       </c>
@@ -6679,7 +6676,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>474</v>
       </c>
@@ -6690,7 +6687,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>475</v>
       </c>
@@ -6704,7 +6701,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="222" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3" t="s">
         <v>476</v>
       </c>
@@ -6730,7 +6727,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="223" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>477</v>
       </c>
@@ -6741,7 +6738,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>478</v>
       </c>

</xml_diff>

<commit_message>
remove species with large chromosomes, add more priorities
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\395220_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/3015712_2_7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CDB36F-5F83-46B7-8506-950D16C61435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D8CDB36F-5F83-46B7-8506-950D16C61435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2607EB25-D8CD-482D-ACA7-84003474161E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1966" uniqueCount="791">
   <si>
     <t>Species</t>
   </si>
@@ -2411,6 +2411,9 @@
   </si>
   <si>
     <t>PRJNA476867</t>
+  </si>
+  <si>
+    <t>Chromosomes are &gt; 520 Mb so they can't be indexed. I'll need to split the chromosomes into smaller units before running the pipeline using seqkit split2 or something similar</t>
   </si>
 </sst>
 </file>
@@ -2487,7 +2490,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2519,14 +2522,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2811,10 +2807,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P347"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A325" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A341" sqref="A341"/>
+      <selection pane="bottomLeft" activeCell="P133" sqref="P133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3104,27 +3100,26 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="17" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+    <row r="11" spans="1:16" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" t="s">
         <v>617</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" t="s">
         <v>616</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="6" t="s">
         <v>785</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="N11" s="20">
+      <c r="N11" s="17">
         <v>45009</v>
       </c>
-      <c r="O11" s="17">
+      <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P11" t="s">
         <v>783</v>
       </c>
     </row>
@@ -3248,13 +3243,13 @@
       <c r="B19" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="E19" s="21"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="3" t="s">
         <v>105</v>
       </c>
@@ -5309,6 +5304,9 @@
       <c r="O133" s="3">
         <v>1</v>
       </c>
+      <c r="P133" s="3" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="134" spans="1:16" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
@@ -8699,29 +8697,27 @@
         <v>695</v>
       </c>
     </row>
-    <row r="343" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="17" t="s">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
         <v>777</v>
       </c>
-      <c r="D343" s="17" t="s">
+      <c r="D343" t="s">
         <v>446</v>
       </c>
-      <c r="I343" s="18" t="s">
+      <c r="I343" s="6" t="s">
         <v>787</v>
       </c>
-      <c r="J343" s="19"/>
-    </row>
-    <row r="344" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A344" s="17" t="s">
+    </row>
+    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
         <v>778</v>
       </c>
-      <c r="D344" s="17" t="s">
+      <c r="D344" t="s">
         <v>446</v>
       </c>
-      <c r="I344" s="18" t="s">
+      <c r="I344" s="6" t="s">
         <v>787</v>
       </c>
-      <c r="J344" s="19"/>
     </row>
     <row r="345" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">

</xml_diff>

<commit_message>
update readme, move input to config
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/3015712_2_7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\4524362_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D8CDB36F-5F83-46B7-8506-950D16C61435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2607EB25-D8CD-482D-ACA7-84003474161E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277522D2-54C2-49D0-B96B-0D9BC5AE9FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -2326,9 +2326,6 @@
     <t>Species used of Ne estimation</t>
   </si>
   <si>
-    <t>Actinidia eriantha</t>
-  </si>
-  <si>
     <t>Amaranthus hybridus</t>
   </si>
   <si>
@@ -2414,6 +2411,9 @@
   </si>
   <si>
     <t>Chromosomes are &gt; 520 Mb so they can't be indexed. I'll need to split the chromosomes into smaller units before running the pipeline using seqkit split2 or something similar</t>
+  </si>
+  <si>
+    <t>Actinidia callosa</t>
   </si>
 </sst>
 </file>
@@ -2807,10 +2807,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="P133" sqref="P133"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,10 +2846,10 @@
         <v>760</v>
       </c>
       <c r="G1" t="s">
+        <v>768</v>
+      </c>
+      <c r="H1" t="s">
         <v>769</v>
-      </c>
-      <c r="H1" t="s">
-        <v>770</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>66</v>
@@ -2864,16 +2864,16 @@
         <v>256</v>
       </c>
       <c r="M1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="N1" t="s">
+        <v>779</v>
+      </c>
+      <c r="O1" t="s">
         <v>780</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>781</v>
-      </c>
-      <c r="P1" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2893,10 +2893,10 @@
         <v>448</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>761</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>762</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>763</v>
       </c>
       <c r="J2" s="10">
         <v>48</v>
@@ -2957,7 +2957,7 @@
         <v>449</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="10">
@@ -3111,7 +3111,7 @@
         <v>616</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="N11" s="17">
         <v>45009</v>
@@ -3120,7 +3120,7 @@
         <v>0</v>
       </c>
       <c r="P11" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -3150,7 +3150,7 @@
         <v>82</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>144</v>
@@ -3159,7 +3159,7 @@
         <v>446</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>145</v>
@@ -3196,7 +3196,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>72</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>446</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>239</v>
@@ -3224,8 +3224,14 @@
       <c r="L17" s="3" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N17" s="15">
+        <v>45023</v>
+      </c>
+      <c r="O17" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -3236,7 +3242,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>105</v>
       </c>
@@ -3266,7 +3272,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -3280,7 +3286,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>128</v>
       </c>
@@ -3306,7 +3312,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -3320,7 +3326,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -3331,7 +3337,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>127</v>
       </c>
@@ -3342,7 +3348,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -3353,7 +3359,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>108</v>
       </c>
@@ -3379,7 +3385,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>109</v>
       </c>
@@ -3405,7 +3411,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -3416,7 +3422,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>59</v>
       </c>
@@ -3442,7 +3448,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -3450,7 +3456,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -3461,7 +3467,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
@@ -5216,6 +5222,12 @@
       <c r="L130" s="3" t="s">
         <v>257</v>
       </c>
+      <c r="N130" s="15">
+        <v>45023</v>
+      </c>
+      <c r="O130" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -5245,13 +5257,13 @@
         <v>318</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>761</v>
+        <v>790</v>
       </c>
       <c r="G132" s="3">
         <v>784</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="I132" s="7" t="s">
         <v>730</v>
@@ -5305,7 +5317,7 @@
         <v>1</v>
       </c>
       <c r="P133" s="3" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="134" spans="1:16" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5396,7 +5408,7 @@
         <v>318</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="I137" s="7" t="s">
         <v>325</v>
@@ -5417,7 +5429,7 @@
         <v>0</v>
       </c>
       <c r="P137" s="3" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="138" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5727,7 +5739,7 @@
         <v>318</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="I156" s="13" t="s">
         <v>362</v>
@@ -5751,7 +5763,7 @@
         <v>0</v>
       </c>
       <c r="P156" s="4" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
@@ -6608,6 +6620,12 @@
       <c r="L209" s="3" t="s">
         <v>257</v>
       </c>
+      <c r="N209" s="15">
+        <v>45023</v>
+      </c>
+      <c r="O209" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="210" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3" t="s">
@@ -6680,10 +6698,10 @@
         <v>456</v>
       </c>
       <c r="F213" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="I213" s="7" t="s">
         <v>767</v>
-      </c>
-      <c r="I213" s="7" t="s">
-        <v>768</v>
       </c>
       <c r="J213" s="10">
         <v>146</v>
@@ -6693,6 +6711,12 @@
       </c>
       <c r="L213" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="N213" s="15">
+        <v>45023</v>
+      </c>
+      <c r="O213" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="214" spans="1:15" x14ac:dyDescent="0.25">
@@ -8448,7 +8472,7 @@
         <v>691</v>
       </c>
       <c r="F326" s="4" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="I326" s="13" t="s">
         <v>702</v>
@@ -8472,7 +8496,7 @@
         <v>0</v>
       </c>
       <c r="P326" s="4" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="327" spans="1:16" x14ac:dyDescent="0.25">
@@ -8579,7 +8603,7 @@
         <v>705</v>
       </c>
       <c r="F334" s="3" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I334" s="7" t="s">
         <v>720</v>
@@ -8699,35 +8723,35 @@
     </row>
     <row r="343" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D343" t="s">
         <v>446</v>
       </c>
       <c r="I343" s="6" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="344" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D344" t="s">
         <v>446</v>
       </c>
       <c r="I344" s="6" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="345" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B345" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="C345" s="3" t="s">
         <v>788</v>
-      </c>
-      <c r="C345" s="3" t="s">
-        <v>789</v>
       </c>
       <c r="D345" s="3" t="s">
         <v>446</v>

</xml_diff>

<commit_message>
fix bugs in GBIF range estimation, sort coordinates
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/67010_2_17/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/198256_2_26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{277522D2-54C2-49D0-B96B-0D9BC5AE9FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBDA3857-8383-4288-ADD6-5231CBC9A5E3}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{277522D2-54C2-49D0-B96B-0D9BC5AE9FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B750D218-1F56-4C8C-B3E1-34D099DD23F9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2872" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="794">
   <si>
     <t>Species</t>
   </si>
@@ -2414,6 +2414,15 @@
   </si>
   <si>
     <t>Actinidia callosa</t>
+  </si>
+  <si>
+    <t>Actinidia polygama</t>
+  </si>
+  <si>
+    <t>Arachis prostrata</t>
+  </si>
+  <si>
+    <t>Arachis glabrata</t>
   </si>
 </sst>
 </file>
@@ -2490,7 +2499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2523,13 +2532,6 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2813,10 +2815,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2906,7 +2908,7 @@
       <c r="O2"/>
       <c r="P2"/>
     </row>
-    <row r="3" spans="1:16" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>308</v>
       </c>
@@ -2921,7 +2923,7 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="G3" s="3">
         <v>784</v>
@@ -3103,30 +3105,30 @@
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" t="s">
         <v>451</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" t="s">
         <v>452</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18" t="s">
+      <c r="C10"/>
+      <c r="D10" t="s">
         <v>452</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="19" t="s">
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
+      <c r="J10" s="9"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
     </row>
     <row r="11" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -3540,7 +3542,7 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>765</v>
+        <v>793</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -3655,7 +3657,9 @@
         <v>456</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>792</v>
+      </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="7" t="s">

</xml_diff>

<commit_message>
use newest version of degenotate
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/198256_2_26/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\4393668_2_27\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{277522D2-54C2-49D0-B96B-0D9BC5AE9FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B750D218-1F56-4C8C-B3E1-34D099DD23F9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B3BF0D-B861-4605-83A6-85599501AEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="794">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="796">
   <si>
     <t>Species</t>
   </si>
@@ -2423,6 +2423,12 @@
   </si>
   <si>
     <t>Arachis glabrata</t>
+  </si>
+  <si>
+    <t>Nicotiana glauca</t>
+  </si>
+  <si>
+    <t>Ficus americana</t>
   </si>
 </sst>
 </file>
@@ -2816,9 +2822,9 @@
   <dimension ref="A1:P347"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5884,7 +5890,7 @@
       </c>
       <c r="E125" s="4"/>
       <c r="F125" s="4" t="s">
-        <v>774</v>
+        <v>795</v>
       </c>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
@@ -7610,7 +7616,7 @@
       </c>
       <c r="E206" s="4"/>
       <c r="F206" s="4" t="s">
-        <v>772</v>
+        <v>794</v>
       </c>
       <c r="G206" s="4"/>
       <c r="H206" s="4"/>

</xml_diff>

<commit_message>
remove support for script instead of conda
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\4393668_2_27\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\1836066_2_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B3BF0D-B861-4605-83A6-85599501AEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78136BA1-0FCB-4583-A72D-AC971E95F248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2887" uniqueCount="808">
   <si>
     <t>Species</t>
   </si>
@@ -2429,6 +2429,42 @@
   </si>
   <si>
     <t>Ficus americana</t>
+  </si>
+  <si>
+    <t>Agave tequilana</t>
+  </si>
+  <si>
+    <t>Andropogon gerardi</t>
+  </si>
+  <si>
+    <t>Saccharum officinarum x spontaneum</t>
+  </si>
+  <si>
+    <t>Paper lists 1218 taxa across all four studies, but there is a newer paper from James Schnable that includes more genotypes</t>
+  </si>
+  <si>
+    <t>There's one sample with a massive amount of data and it was holding up the entire pipeline, so I removed this species from batch 3</t>
+  </si>
+  <si>
+    <t>found data in set for other species; can't find genome fasta + gff</t>
+  </si>
+  <si>
+    <t>Coffea mauritiana</t>
+  </si>
+  <si>
+    <t>Dioscorea communis</t>
+  </si>
+  <si>
+    <t>Durio graveolens</t>
+  </si>
+  <si>
+    <t>Elaeis oleifera</t>
+  </si>
+  <si>
+    <t>Eleusine indica</t>
+  </si>
+  <si>
+    <t>Cucurbita palmata</t>
   </si>
 </sst>
 </file>
@@ -2819,17 +2855,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P347"/>
+  <dimension ref="A1:P348"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="59" customWidth="1"/>
     <col min="3" max="8" width="31" customWidth="1"/>
     <col min="9" max="9" width="42.28515625" style="6" customWidth="1"/>
@@ -2837,7 +2873,7 @@
     <col min="11" max="11" width="35.7109375" customWidth="1"/>
     <col min="12" max="12" width="25.140625" customWidth="1"/>
     <col min="13" max="13" width="25.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -3484,43 +3520,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>617</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="7" t="s">
+      <c r="D22" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="I22" s="13" t="s">
         <v>618</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="12">
         <v>5</v>
       </c>
-      <c r="K22" s="3">
-        <v>1</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="M22" s="3"/>
-      <c r="N22" s="15">
+      <c r="K22" s="4">
+        <v>1</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="N22" s="16">
         <v>45023</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22" s="4">
         <v>3</v>
       </c>
-      <c r="P22" s="3"/>
+      <c r="P22" s="4" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -3966,7 +3999,9 @@
         <v>446</v>
       </c>
       <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="7" t="s">
@@ -3982,8 +4017,12 @@
         <v>257</v>
       </c>
       <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
+      <c r="N40" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O40" s="3">
+        <v>4</v>
+      </c>
       <c r="P40" s="3"/>
     </row>
     <row r="41" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -4131,41 +4170,35 @@
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3" t="s">
+      <c r="F48" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="7" t="s">
-        <v>720</v>
-      </c>
-      <c r="J48" s="10">
+      <c r="I48" s="13" t="s">
+        <v>801</v>
+      </c>
+      <c r="J48" s="12">
         <v>7</v>
       </c>
-      <c r="K48" s="3">
-        <v>1</v>
-      </c>
-      <c r="L48" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
+      <c r="K48" s="4">
+        <v>1</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="N48" s="16"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
@@ -4293,6 +4326,12 @@
       <c r="L53" s="3" t="s">
         <v>257</v>
       </c>
+      <c r="N53" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O53" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
@@ -4438,7 +4477,9 @@
         <v>446</v>
       </c>
       <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
+      <c r="F58" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="I58" s="7" t="s">
@@ -4454,8 +4495,12 @@
         <v>257</v>
       </c>
       <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
+      <c r="N58" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O58" s="3">
+        <v>4</v>
+      </c>
       <c r="P58" s="3"/>
     </row>
     <row r="59" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4491,39 +4536,40 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:16" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="13" t="s">
+      <c r="F61" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I61" s="7" t="s">
         <v>725</v>
       </c>
-      <c r="J61" s="12">
+      <c r="J61" s="10">
         <v>52</v>
       </c>
-      <c r="K61" s="4">
-        <v>1</v>
-      </c>
-      <c r="L61" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="M61" s="4"/>
-      <c r="N61" s="4"/>
-      <c r="O61" s="4"/>
-      <c r="P61" s="4"/>
+      <c r="K61" s="3">
+        <v>1</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="N61" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O61" s="3">
+        <v>4</v>
+      </c>
     </row>
     <row r="62" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -4982,6 +5028,9 @@
       <c r="D82" s="3" t="s">
         <v>456</v>
       </c>
+      <c r="F82" s="3" t="s">
+        <v>802</v>
+      </c>
       <c r="I82" s="7" t="s">
         <v>584</v>
       </c>
@@ -4993,6 +5042,12 @@
       </c>
       <c r="L82" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="N82" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O82" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -5356,7 +5411,9 @@
         <v>456</v>
       </c>
       <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
+      <c r="F99" s="3" t="s">
+        <v>807</v>
+      </c>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="7" t="s">
@@ -5372,8 +5429,12 @@
         <v>257</v>
       </c>
       <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
+      <c r="N99" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O99" s="3">
+        <v>4</v>
+      </c>
       <c r="P99" s="3"/>
     </row>
     <row r="100" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -5645,6 +5706,9 @@
       <c r="D112" s="3" t="s">
         <v>318</v>
       </c>
+      <c r="F112" s="3" t="s">
+        <v>803</v>
+      </c>
       <c r="I112" s="7" t="s">
         <v>636</v>
       </c>
@@ -5656,6 +5720,12 @@
       </c>
       <c r="L112" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="N112" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O112" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5706,6 +5776,9 @@
       <c r="D115" s="3" t="s">
         <v>456</v>
       </c>
+      <c r="F115" s="3" t="s">
+        <v>804</v>
+      </c>
       <c r="I115" s="7" t="s">
         <v>591</v>
       </c>
@@ -5717,6 +5790,12 @@
       </c>
       <c r="L115" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="N115" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O115" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -5756,6 +5835,9 @@
       <c r="D117" s="3" t="s">
         <v>456</v>
       </c>
+      <c r="F117" s="3" t="s">
+        <v>805</v>
+      </c>
       <c r="I117" s="7" t="s">
         <v>586</v>
       </c>
@@ -5767,6 +5849,12 @@
       </c>
       <c r="L117" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="N117" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O117" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="1:16" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5779,6 +5867,9 @@
       <c r="D118" s="3" t="s">
         <v>456</v>
       </c>
+      <c r="F118" s="3" t="s">
+        <v>806</v>
+      </c>
       <c r="I118" s="7" t="s">
         <v>586</v>
       </c>
@@ -5790,6 +5881,12 @@
       </c>
       <c r="L118" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="N118" s="15">
+        <v>45036</v>
+      </c>
+      <c r="O118" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:16" ht="60" x14ac:dyDescent="0.25">
@@ -10377,106 +10474,76 @@
       <c r="O337" s="3"/>
       <c r="P337" s="3"/>
     </row>
-    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A338" s="3" t="s">
+    <row r="338" spans="1:16" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A338" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B338" s="3" t="s">
+      <c r="B338" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C338" s="3" t="s">
+      <c r="C338" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D338" s="3" t="s">
+      <c r="D338" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="E338" s="3"/>
-      <c r="F338" s="3"/>
-      <c r="G338" s="3"/>
-      <c r="H338" s="3"/>
-      <c r="I338" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="J338" s="10">
+      <c r="I338" s="13" t="s">
+        <v>799</v>
+      </c>
+      <c r="J338" s="12">
         <v>33</v>
       </c>
-      <c r="K338" s="3">
-        <v>1</v>
-      </c>
-      <c r="L338" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="M338" s="3"/>
-      <c r="N338" s="3"/>
-      <c r="O338" s="3"/>
-      <c r="P338" s="3"/>
-    </row>
-    <row r="339" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A339" s="3" t="s">
+      <c r="K338" s="4">
+        <v>1</v>
+      </c>
+      <c r="L338" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="339" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A339" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B339" s="3"/>
-      <c r="C339" s="3" t="s">
+      <c r="C339" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D339" s="3" t="s">
+      <c r="D339" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="E339" s="3"/>
-      <c r="F339" s="3"/>
-      <c r="G339" s="3"/>
-      <c r="H339" s="3"/>
-      <c r="I339" s="7" t="s">
+      <c r="I339" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="J339" s="10"/>
-      <c r="K339" s="3"/>
-      <c r="L339" s="3"/>
-      <c r="M339" s="3"/>
-      <c r="N339" s="3"/>
-      <c r="O339" s="3"/>
-      <c r="P339" s="3"/>
-    </row>
-    <row r="340" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A340" s="3" t="s">
+      <c r="J339" s="12"/>
+    </row>
+    <row r="340" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C340" s="3" t="s">
+      <c r="C340" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D340" s="3" t="s">
+      <c r="D340" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="I340" s="7"/>
-      <c r="J340" s="10">
+      <c r="I340" s="13"/>
+      <c r="J340" s="12">
         <v>277</v>
       </c>
     </row>
-    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A341" s="3" t="s">
+    <row r="341" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B341" s="3"/>
-      <c r="C341" s="3" t="s">
+      <c r="C341" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D341" s="3" t="s">
+      <c r="D341" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="E341" s="3"/>
-      <c r="F341" s="3"/>
-      <c r="G341" s="3"/>
-      <c r="H341" s="3"/>
-      <c r="I341" s="7"/>
-      <c r="J341" s="10">
+      <c r="I341" s="13"/>
+      <c r="J341" s="12">
         <v>599</v>
       </c>
-      <c r="K341" s="3"/>
-      <c r="L341" s="3"/>
-      <c r="M341" s="3"/>
-      <c r="N341" s="3"/>
-      <c r="O341" s="3"/>
-      <c r="P341" s="3"/>
     </row>
     <row r="342" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
@@ -10579,15 +10646,35 @@
       <c r="O345"/>
       <c r="P345"/>
     </row>
-    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D346" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D347" t="s">
-        <v>723</v>
-      </c>
+    <row r="346" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="4" t="s">
+        <v>796</v>
+      </c>
+      <c r="D346" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I346" s="13"/>
+      <c r="J346" s="12"/>
+    </row>
+    <row r="347" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="4" t="s">
+        <v>797</v>
+      </c>
+      <c r="D347" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I347" s="13"/>
+      <c r="J347" s="12"/>
+    </row>
+    <row r="348" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="4" t="s">
+        <v>798</v>
+      </c>
+      <c r="D348" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="I348" s="13"/>
+      <c r="J348" s="12"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P347">

</xml_diff>

<commit_message>
remove support for not using conda environments
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\1836066_2_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\1181974_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78136BA1-0FCB-4583-A72D-AC971E95F248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7272F1-46D8-4C11-BB34-88E54284EBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2887" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2888" uniqueCount="809">
   <si>
     <t>Species</t>
   </si>
@@ -2465,6 +2465,9 @@
   </si>
   <si>
     <t>Cucurbita palmata</t>
+  </si>
+  <si>
+    <t>Annotation file could not be read properly by degenotate, so I dropped this species from the batch for now. It appears that the annotation file only has gene and CDS sequences. I changed the categories to mRNA and exon, respectively, but then degenotate threw an error: **Error GXF1: Invalid number of IDs found during transcript parent id parsing</t>
   </si>
 </sst>
 </file>
@@ -2857,10 +2860,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P348"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
+      <selection pane="bottomLeft" activeCell="P118" sqref="P118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5857,36 +5860,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:16" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+    <row r="118" spans="1:16" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="C118" s="3" t="s">
+      <c r="C118" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="D118" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="F118" s="3" t="s">
+      <c r="D118" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="F118" s="4" t="s">
         <v>806</v>
       </c>
-      <c r="I118" s="7" t="s">
+      <c r="I118" s="13" t="s">
         <v>586</v>
       </c>
-      <c r="J118" s="10">
+      <c r="J118" s="12">
         <v>88</v>
       </c>
-      <c r="K118" s="3">
-        <v>1</v>
-      </c>
-      <c r="L118" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="N118" s="15">
+      <c r="K118" s="4">
+        <v>1</v>
+      </c>
+      <c r="L118" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="N118" s="16">
         <v>45036</v>
       </c>
-      <c r="O118" s="3">
+      <c r="O118" s="4">
         <v>4</v>
+      </c>
+      <c r="P118" s="4" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="119" spans="1:16" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update readme, add dynamic memory limits and time limits
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67066_2_12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\460340_2_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E28F0B7-678D-4FCF-80A3-E2585E9627AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA4BE7A-93E7-456B-8972-23349D7C7C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2894" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2897" uniqueCount="815">
   <si>
     <t>Species</t>
   </si>
@@ -2483,6 +2483,9 @@
   </si>
   <si>
     <t>https://doi.org/10.1371%2Fjournal.pone.0277537</t>
+  </si>
+  <si>
+    <t>Helianthus maximiliani</t>
   </si>
 </sst>
 </file>
@@ -2875,10 +2878,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R348"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
+      <selection pane="bottomLeft" activeCell="Q172" sqref="Q172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6819,7 +6822,9 @@
         <v>446</v>
       </c>
       <c r="E155" s="3"/>
-      <c r="F155" s="3"/>
+      <c r="F155" s="3" t="s">
+        <v>814</v>
+      </c>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
@@ -6837,8 +6842,12 @@
         <v>257</v>
       </c>
       <c r="O155" s="3"/>
-      <c r="P155" s="3"/>
-      <c r="Q155" s="3"/>
+      <c r="P155" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q155" s="3">
+        <v>5</v>
+      </c>
       <c r="R155" s="3"/>
     </row>
     <row r="156" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -6855,7 +6864,9 @@
         <v>456</v>
       </c>
       <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
+      <c r="F156" s="3" t="s">
+        <v>509</v>
+      </c>
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
@@ -6873,8 +6884,12 @@
         <v>257</v>
       </c>
       <c r="O156" s="3"/>
-      <c r="P156" s="3"/>
-      <c r="Q156" s="3"/>
+      <c r="P156" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q156" s="3">
+        <v>5</v>
+      </c>
       <c r="R156" s="3"/>
     </row>
     <row r="157" spans="1:18" x14ac:dyDescent="0.25">
@@ -7165,7 +7180,9 @@
       </c>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
-      <c r="F172" s="3"/>
+      <c r="F172" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
       <c r="I172" s="3"/>
@@ -7183,8 +7200,12 @@
         <v>257</v>
       </c>
       <c r="O172" s="3"/>
-      <c r="P172" s="3"/>
-      <c r="Q172" s="3"/>
+      <c r="P172" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q172" s="3">
+        <v>5</v>
+      </c>
       <c r="R172" s="3"/>
     </row>
     <row r="173" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
output time in minutes
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\460340_2_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\460340_2_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA4BE7A-93E7-456B-8972-23349D7C7C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCFE36F-21FA-4DBD-935D-CEB1E75B6743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2897" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2910" uniqueCount="825">
   <si>
     <t>Species</t>
   </si>
@@ -2486,6 +2486,36 @@
   </si>
   <si>
     <t>Helianthus maximiliani</t>
+  </si>
+  <si>
+    <t>Lupinus argenteus</t>
+  </si>
+  <si>
+    <t>There are some more common relatives, but they're cultivated as ornamentals</t>
+  </si>
+  <si>
+    <t>Malus sieversii</t>
+  </si>
+  <si>
+    <t>Malus sylvestris is also a wild relative, but I want to use that for it's own genetic data</t>
+  </si>
+  <si>
+    <t>Mangifera foetida</t>
+  </si>
+  <si>
+    <t>Manihot tripartita</t>
+  </si>
+  <si>
+    <t>Medicago lupulina</t>
+  </si>
+  <si>
+    <t>M. truncatula is technically a forage crop in some places</t>
+  </si>
+  <si>
+    <t>Erythranthe moschata</t>
+  </si>
+  <si>
+    <t>M. guttatus is cultivated as a perennial</t>
   </si>
 </sst>
 </file>
@@ -2878,10 +2908,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="Q172" sqref="Q172"/>
+      <selection pane="bottomLeft" activeCell="A185" sqref="A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7155,6 +7185,9 @@
       <c r="C171" s="3" t="s">
         <v>191</v>
       </c>
+      <c r="D171" s="3" t="s">
+        <v>446</v>
+      </c>
       <c r="K171" s="7" t="s">
         <v>145</v>
       </c>
@@ -7178,7 +7211,9 @@
       <c r="C172" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="D172" s="3"/>
+      <c r="D172" s="3" t="s">
+        <v>446</v>
+      </c>
       <c r="E172" s="3"/>
       <c r="F172" s="3" t="s">
         <v>90</v>
@@ -7387,8 +7422,12 @@
         <v>318</v>
       </c>
       <c r="E181" s="3"/>
-      <c r="F181" s="3"/>
-      <c r="G181" s="3"/>
+      <c r="F181" s="3" t="s">
+        <v>815</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>816</v>
+      </c>
       <c r="H181" s="3"/>
       <c r="I181" s="3"/>
       <c r="J181" s="3"/>
@@ -7403,8 +7442,12 @@
         <v>257</v>
       </c>
       <c r="O181" s="3"/>
-      <c r="P181" s="3"/>
-      <c r="Q181" s="3"/>
+      <c r="P181" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q181" s="3">
+        <v>5</v>
+      </c>
       <c r="R181" s="3"/>
     </row>
     <row r="182" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7445,8 +7488,12 @@
         <v>456</v>
       </c>
       <c r="E183" s="3"/>
-      <c r="F183" s="3"/>
-      <c r="G183" s="3"/>
+      <c r="F183" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>818</v>
+      </c>
       <c r="H183" s="3"/>
       <c r="I183" s="3"/>
       <c r="J183" s="3"/>
@@ -7463,8 +7510,12 @@
         <v>257</v>
       </c>
       <c r="O183" s="3"/>
-      <c r="P183" s="3"/>
-      <c r="Q183" s="3"/>
+      <c r="P183" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q183" s="3">
+        <v>5</v>
+      </c>
       <c r="R183" s="3"/>
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.25">
@@ -7481,7 +7532,9 @@
         <v>456</v>
       </c>
       <c r="E184" s="3"/>
-      <c r="F184" s="3"/>
+      <c r="F184" s="3" t="s">
+        <v>519</v>
+      </c>
       <c r="G184" s="3"/>
       <c r="H184" s="3"/>
       <c r="I184" s="3"/>
@@ -7499,8 +7552,12 @@
         <v>257</v>
       </c>
       <c r="O184" s="3"/>
-      <c r="P184" s="3"/>
-      <c r="Q184" s="3"/>
+      <c r="P184" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q184" s="3">
+        <v>5</v>
+      </c>
       <c r="R184" s="3"/>
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.25">
@@ -7517,7 +7574,9 @@
         <v>456</v>
       </c>
       <c r="E185" s="3"/>
-      <c r="F185" s="3"/>
+      <c r="F185" s="3" t="s">
+        <v>819</v>
+      </c>
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
       <c r="I185" s="3"/>
@@ -7535,8 +7594,12 @@
         <v>257</v>
       </c>
       <c r="O185" s="3"/>
-      <c r="P185" s="3"/>
-      <c r="Q185" s="3"/>
+      <c r="P185" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q185" s="3">
+        <v>5</v>
+      </c>
       <c r="R185" s="3"/>
     </row>
     <row r="186" spans="1:18" ht="60" x14ac:dyDescent="0.25">
@@ -7553,7 +7616,9 @@
         <v>446</v>
       </c>
       <c r="E186" s="3"/>
-      <c r="F186" s="3"/>
+      <c r="F186" s="3" t="s">
+        <v>820</v>
+      </c>
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
       <c r="I186" s="3"/>
@@ -7571,8 +7636,12 @@
         <v>257</v>
       </c>
       <c r="O186" s="3"/>
-      <c r="P186" s="3"/>
-      <c r="Q186" s="3"/>
+      <c r="P186" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q186" s="3">
+        <v>5</v>
+      </c>
       <c r="R186" s="3"/>
     </row>
     <row r="187" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -7663,8 +7732,12 @@
         <v>446</v>
       </c>
       <c r="E191" s="3"/>
-      <c r="F191" s="3"/>
-      <c r="G191" s="3"/>
+      <c r="F191" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="G191" s="3" t="s">
+        <v>822</v>
+      </c>
       <c r="H191" s="3"/>
       <c r="I191" s="3"/>
       <c r="J191" s="3"/>
@@ -7681,8 +7754,12 @@
         <v>257</v>
       </c>
       <c r="O191" s="3"/>
-      <c r="P191" s="3"/>
-      <c r="Q191" s="3"/>
+      <c r="P191" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q191" s="3">
+        <v>5</v>
+      </c>
       <c r="R191" s="3"/>
     </row>
     <row r="192" spans="1:18" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -7748,6 +7825,12 @@
       <c r="D195" s="3" t="s">
         <v>446</v>
       </c>
+      <c r="F195" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="G195" s="3" t="s">
+        <v>824</v>
+      </c>
       <c r="K195" s="7" t="s">
         <v>269</v>
       </c>
@@ -7759,6 +7842,12 @@
       </c>
       <c r="N195" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="P195" s="15">
+        <v>45050</v>
+      </c>
+      <c r="Q195" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="1:18" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
move to next batch
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktopco2lop1/RemoteFiles/131836_2_3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67086_2_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{DCCFE36F-21FA-4DBD-935D-CEB1E75B6743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D27BF781-D2F6-4C78-B5A7-0B6BD335AFA8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE15BD-6172-47B0-8B89-D8D833BEF299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2913" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2925" uniqueCount="837">
   <si>
     <t>Species</t>
   </si>
@@ -2522,6 +2522,36 @@
   </si>
   <si>
     <t>Brassica repanda</t>
+  </si>
+  <si>
+    <t>Musa balbisiana</t>
+  </si>
+  <si>
+    <t>Musa velutina has more occurrence records, but balbisiana is one of the progenitors of cultivated banana, and has more occurrences in its native range</t>
+  </si>
+  <si>
+    <t>Nelumbo lutea</t>
+  </si>
+  <si>
+    <t>The native range of N. lutea does not overlap with the native range of N. nucifera, but there were no other plants in this genus with over 20 occurrence records on GBIF</t>
+  </si>
+  <si>
+    <t>Olea paniculata</t>
+  </si>
+  <si>
+    <t>can't find publication, O. glumipatula is a synonym for Oryza rufipogon, so we'll ignore this genome</t>
+  </si>
+  <si>
+    <t>Papaver rhoeas</t>
+  </si>
+  <si>
+    <t>Lathyrus pratensis</t>
+  </si>
+  <si>
+    <t>Pisum sativum is a synonym for Lathyrus oleraceus</t>
+  </si>
+  <si>
+    <t>Has one chromosome longer than 512 Mb, which means that tabix/bai indexes won't work</t>
   </si>
 </sst>
 </file>
@@ -2598,7 +2628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2631,6 +2661,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2915,9 +2946,9 @@
   <dimension ref="A1:R348"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+      <selection pane="bottomLeft" activeCell="A245" sqref="A245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7961,8 +7992,12 @@
         <v>446</v>
       </c>
       <c r="E200" s="3"/>
-      <c r="F200" s="3"/>
-      <c r="G200" s="3"/>
+      <c r="F200" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="G200" s="3" t="s">
+        <v>828</v>
+      </c>
       <c r="H200" s="3"/>
       <c r="I200" s="3"/>
       <c r="J200" s="3"/>
@@ -7979,8 +8014,12 @@
         <v>257</v>
       </c>
       <c r="O200" s="3"/>
-      <c r="P200" s="3"/>
-      <c r="Q200" s="3"/>
+      <c r="P200" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q200" s="3">
+        <v>6</v>
+      </c>
       <c r="R200" s="3"/>
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.25">
@@ -8008,8 +8047,12 @@
         <v>456</v>
       </c>
       <c r="E202" s="3"/>
-      <c r="F202" s="3"/>
-      <c r="G202" s="3"/>
+      <c r="F202" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>830</v>
+      </c>
       <c r="H202" s="3"/>
       <c r="I202" s="3"/>
       <c r="J202" s="3"/>
@@ -8026,8 +8069,12 @@
         <v>257</v>
       </c>
       <c r="O202" s="3"/>
-      <c r="P202" s="3"/>
-      <c r="Q202" s="3"/>
+      <c r="P202" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q202" s="3">
+        <v>6</v>
+      </c>
       <c r="R202" s="3"/>
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.25">
@@ -8224,7 +8271,9 @@
         <v>446</v>
       </c>
       <c r="E211" s="3"/>
-      <c r="F211" s="3"/>
+      <c r="F211" s="3" t="s">
+        <v>831</v>
+      </c>
       <c r="G211" s="3"/>
       <c r="H211" s="3"/>
       <c r="I211" s="3"/>
@@ -8242,8 +8291,12 @@
         <v>257</v>
       </c>
       <c r="O211" s="3"/>
-      <c r="P211" s="3"/>
-      <c r="Q211" s="3"/>
+      <c r="P211" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q211" s="3">
+        <v>6</v>
+      </c>
       <c r="R211" s="3"/>
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.25">
@@ -8315,6 +8368,9 @@
       <c r="D215" s="3" t="s">
         <v>318</v>
       </c>
+      <c r="F215" s="3" t="s">
+        <v>376</v>
+      </c>
       <c r="K215" s="7"/>
       <c r="L215" s="10">
         <v>86</v>
@@ -8325,6 +8381,12 @@
       <c r="N215" s="3" t="s">
         <v>257</v>
       </c>
+      <c r="P215" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q215" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="216" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3" t="s">
@@ -8336,6 +8398,9 @@
       <c r="D216" s="3" t="s">
         <v>318</v>
       </c>
+      <c r="F216" s="3" t="s">
+        <v>380</v>
+      </c>
       <c r="K216" s="7" t="s">
         <v>381</v>
       </c>
@@ -8347,6 +8412,12 @@
       </c>
       <c r="N216" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="P216" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q216" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="217" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -8370,39 +8441,20 @@
         <v>257</v>
       </c>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A218" s="3" t="s">
+    <row r="218" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>387</v>
       </c>
-      <c r="B218" s="3"/>
-      <c r="C218" s="3" t="s">
+      <c r="C218" t="s">
         <v>386</v>
       </c>
-      <c r="D218" s="3" t="s">
+      <c r="D218" t="s">
         <v>318</v>
       </c>
-      <c r="E218" s="3"/>
-      <c r="F218" s="3"/>
-      <c r="G218" s="3"/>
-      <c r="H218" s="3"/>
-      <c r="I218" s="3"/>
-      <c r="J218" s="3"/>
-      <c r="K218" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="L218" s="10">
-        <v>21</v>
-      </c>
-      <c r="M218" s="3">
-        <v>1</v>
-      </c>
-      <c r="N218" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="O218" s="3"/>
-      <c r="P218" s="3"/>
-      <c r="Q218" s="3"/>
-      <c r="R218" s="3"/>
+      <c r="K218" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="P218" s="18"/>
     </row>
     <row r="219" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3" t="s">
@@ -8425,6 +8477,12 @@
       </c>
       <c r="N219" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="P219" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q219" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.25">
@@ -8457,8 +8515,12 @@
         <v>257</v>
       </c>
       <c r="O220" s="3"/>
-      <c r="P220" s="3"/>
-      <c r="Q220" s="3"/>
+      <c r="P220" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q220" s="3">
+        <v>6</v>
+      </c>
       <c r="R220" s="3"/>
     </row>
     <row r="221" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -8617,7 +8679,9 @@
         <v>446</v>
       </c>
       <c r="E226" s="3"/>
-      <c r="F226" s="3"/>
+      <c r="F226" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="G226" s="3"/>
       <c r="H226" s="3"/>
       <c r="I226" s="3"/>
@@ -8635,8 +8699,12 @@
         <v>257</v>
       </c>
       <c r="O226" s="3"/>
-      <c r="P226" s="3"/>
-      <c r="Q226" s="3"/>
+      <c r="P226" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q226" s="3">
+        <v>6</v>
+      </c>
       <c r="R226" s="3"/>
     </row>
     <row r="227" spans="1:18" ht="30" x14ac:dyDescent="0.25">
@@ -8744,9 +8812,13 @@
       <c r="C232" s="3" t="s">
         <v>741</v>
       </c>
-      <c r="D232" s="3"/>
+      <c r="D232" s="3" t="s">
+        <v>318</v>
+      </c>
       <c r="E232" s="3"/>
-      <c r="F232" s="3"/>
+      <c r="F232" s="3" t="s">
+        <v>833</v>
+      </c>
       <c r="G232" s="3"/>
       <c r="H232" s="3"/>
       <c r="I232" s="3"/>
@@ -8764,8 +8836,12 @@
         <v>257</v>
       </c>
       <c r="O232" s="3"/>
-      <c r="P232" s="3"/>
-      <c r="Q232" s="3"/>
+      <c r="P232" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q232" s="3">
+        <v>6</v>
+      </c>
       <c r="R232" s="3"/>
     </row>
     <row r="233" spans="1:18" x14ac:dyDescent="0.25">
@@ -8977,39 +9053,38 @@
         <v>337</v>
       </c>
     </row>
-    <row r="245" spans="1:18" ht="105" x14ac:dyDescent="0.25">
-      <c r="A245" s="3" t="s">
+    <row r="245" spans="1:18" s="4" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A245" s="4" t="s">
         <v>407</v>
       </c>
-      <c r="B245" s="3" t="s">
+      <c r="B245" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="C245" s="3"/>
-      <c r="D245" s="3" t="s">
+      <c r="D245" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="E245" s="3"/>
-      <c r="F245" s="3"/>
-      <c r="G245" s="3"/>
-      <c r="H245" s="3"/>
-      <c r="I245" s="3"/>
-      <c r="J245" s="3"/>
-      <c r="K245" s="7" t="s">
+      <c r="F245" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="G245" s="4" t="s">
+        <v>835</v>
+      </c>
+      <c r="K245" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="L245" s="10">
+      <c r="L245" s="12">
         <v>27</v>
       </c>
-      <c r="M245" s="3">
-        <v>1</v>
-      </c>
-      <c r="N245" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="O245" s="3"/>
-      <c r="P245" s="3"/>
-      <c r="Q245" s="3"/>
-      <c r="R245" s="3"/>
+      <c r="M245" s="4">
+        <v>1</v>
+      </c>
+      <c r="N245" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="P245" s="16"/>
+      <c r="R245" s="4" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
@@ -9054,8 +9129,12 @@
         <v>257</v>
       </c>
       <c r="O247" s="3"/>
-      <c r="P247" s="3"/>
-      <c r="Q247" s="3"/>
+      <c r="P247" s="15">
+        <v>45065</v>
+      </c>
+      <c r="Q247" s="3">
+        <v>6</v>
+      </c>
       <c r="R247" s="3"/>
     </row>
     <row r="248" spans="1:18" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add more taxon keys
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\2622974_2_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\2819968_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B9E6A4-3D2F-4313-87D5-4E079CDB3F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B1415B-FF35-4969-9F67-98839AD1ADCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3024" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="924">
   <si>
     <t>Species</t>
   </si>
@@ -2762,6 +2762,57 @@
   </si>
   <si>
     <t>has one chromosome &gt;520 Mb</t>
+  </si>
+  <si>
+    <t>Restricted to Fort Lauderdale accord</t>
+  </si>
+  <si>
+    <t>Unrestricted!</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0028715</t>
+  </si>
+  <si>
+    <t>There were no other related species in the same genus with enough gbif observations</t>
+  </si>
+  <si>
+    <t>Capsicum annuum var. glabriusculum</t>
+  </si>
+  <si>
+    <t>This species is often wild, although cultivated in china. The occurences on gbif match it's native range anyway</t>
+  </si>
+  <si>
+    <t>After C. mannii there aren't any more species with lots of observations on Gbif in the Coffea genus</t>
+  </si>
+  <si>
+    <t>Coffea mayombensis</t>
+  </si>
+  <si>
+    <t>Cucumis myriocarpus</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.1005338107</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.1005338107 - gives wild progenitors of melon, but these species have almost no gbif observations</t>
+  </si>
+  <si>
+    <t>Cucumis hystrix</t>
+  </si>
+  <si>
+    <t>Dioscorea oryzetorum, Dioscorea inopinata</t>
+  </si>
+  <si>
+    <t>These were the closest related species in timetree</t>
+  </si>
+  <si>
+    <t>Glycine tabacina</t>
+  </si>
+  <si>
+    <t>I want to use G. soja for soja. Glycine tabacina has some occurrences in asia and is in the same genus</t>
+  </si>
+  <si>
+    <t>closest relative in timetree</t>
   </si>
 </sst>
 </file>
@@ -2838,7 +2889,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2876,6 +2927,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3161,10 +3215,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="V171" sqref="V171"/>
+      <selection pane="bottomLeft" activeCell="G140" sqref="G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4999,7 +5053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>326</v>
       </c>
@@ -5013,8 +5067,12 @@
         <v>318</v>
       </c>
       <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="13"/>
+      <c r="F57" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>910</v>
+      </c>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
@@ -5186,7 +5244,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>330</v>
       </c>
@@ -5198,8 +5256,12 @@
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="7"/>
+      <c r="F63" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>909</v>
+      </c>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
@@ -5325,7 +5387,7 @@
       <c r="U67"/>
       <c r="V67"/>
     </row>
-    <row r="68" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>473</v>
       </c>
@@ -5338,7 +5400,12 @@
       <c r="D68" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="G68" s="7"/>
+      <c r="F68" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>912</v>
+      </c>
       <c r="O68" s="7" t="s">
         <v>584</v>
       </c>
@@ -5745,7 +5812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>340</v>
       </c>
@@ -5758,16 +5825,12 @@
       <c r="D83" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
-      <c r="K83" s="4"/>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
-      <c r="N83" s="4"/>
+      <c r="F83" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>913</v>
+      </c>
       <c r="O83" s="13" t="s">
         <v>342</v>
       </c>
@@ -5780,10 +5843,6 @@
       <c r="R83" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="S83" s="4"/>
-      <c r="T83" s="4"/>
-      <c r="U83" s="4"/>
-      <c r="V83" s="4"/>
     </row>
     <row r="84" spans="1:22" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -5974,7 +6033,7 @@
       <c r="U91"/>
       <c r="V91"/>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>347</v>
       </c>
@@ -5988,8 +6047,12 @@
         <v>318</v>
       </c>
       <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="7"/>
+      <c r="F92" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="G92" s="21" t="s">
+        <v>917</v>
+      </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
@@ -6026,8 +6089,12 @@
         <v>446</v>
       </c>
       <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="G93" s="13"/>
+      <c r="F93" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="G93" s="13" t="s">
+        <v>916</v>
+      </c>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
       <c r="J93" s="4"/>
@@ -6458,7 +6525,7 @@
       </c>
       <c r="V109" s="3"/>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>121</v>
       </c>
@@ -6472,8 +6539,12 @@
         <v>446</v>
       </c>
       <c r="E110" s="3"/>
-      <c r="F110" s="3"/>
-      <c r="G110" s="7"/>
+      <c r="F110" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="G110" s="7" t="s">
+        <v>920</v>
+      </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
@@ -7056,7 +7127,12 @@
       <c r="D132" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="G132" s="7"/>
+      <c r="F132" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="G132" s="7" t="s">
+        <v>922</v>
+      </c>
       <c r="O132" s="7" t="s">
         <v>289</v>
       </c>
@@ -7301,7 +7377,12 @@
       <c r="D139" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="G139" s="7"/>
+      <c r="F139" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>923</v>
+      </c>
       <c r="O139" s="7"/>
       <c r="P139" s="10">
         <v>336</v>
@@ -12559,7 +12640,9 @@
         <v>446</v>
       </c>
       <c r="G347" s="13"/>
-      <c r="O347" s="13"/>
+      <c r="O347" s="13" t="s">
+        <v>907</v>
+      </c>
       <c r="P347" s="12"/>
     </row>
     <row r="348" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12570,7 +12653,9 @@
         <v>446</v>
       </c>
       <c r="G348" s="13"/>
-      <c r="O348" s="13"/>
+      <c r="O348" s="13" t="s">
+        <v>907</v>
+      </c>
       <c r="P348" s="12"/>
     </row>
     <row r="349" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12581,7 +12666,9 @@
         <v>446</v>
       </c>
       <c r="G349" s="13"/>
-      <c r="O349" s="13"/>
+      <c r="O349" s="13" t="s">
+        <v>907</v>
+      </c>
       <c r="P349" s="12"/>
     </row>
     <row r="350" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -12592,7 +12679,9 @@
         <v>446</v>
       </c>
       <c r="G350" s="13"/>
-      <c r="O350" s="13"/>
+      <c r="O350" s="13" t="s">
+        <v>908</v>
+      </c>
       <c r="P350" s="12"/>
     </row>
   </sheetData>
@@ -12607,9 +12696,10 @@
     <hyperlink ref="B61" r:id="rId4" xr:uid="{E45E1430-16DD-43DA-A38A-1FD9044C4E4C}"/>
     <hyperlink ref="B40" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
     <hyperlink ref="B228" r:id="rId6" xr:uid="{2677786D-08C7-4346-837D-960E754FAB79}"/>
+    <hyperlink ref="G92" r:id="rId7" xr:uid="{BA568409-981D-4049-9F64-BEB3B33169A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
finish adding taxon keys
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\2819968_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\16516764_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B1415B-FF35-4969-9F67-98839AD1ADCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2111BF43-E624-4F1A-98E5-D23E320AC50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3101" uniqueCount="972">
   <si>
     <t>Species</t>
   </si>
@@ -2813,6 +2813,150 @@
   </si>
   <si>
     <t>closest relative in timetree</t>
+  </si>
+  <si>
+    <t>Gossypium thurberi</t>
+  </si>
+  <si>
+    <t>close relative in timetree with lots of gbif observations, native range also overlaps native range of G. hirsutum</t>
+  </si>
+  <si>
+    <t>Hordeum vulgare subsp. spontaneum</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371%2Fjournal.pone.0160745</t>
+  </si>
+  <si>
+    <t>Juglans mandshurica</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/plphys/kiad394</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/aps3.11349</t>
+  </si>
+  <si>
+    <t>Linum bienne</t>
+  </si>
+  <si>
+    <t>Macadamia ternifolia</t>
+  </si>
+  <si>
+    <t>In the same genus, overlapping native ranges, and has most observations in gbif</t>
+  </si>
+  <si>
+    <t>Miscanthus sacchariflorus</t>
+  </si>
+  <si>
+    <t>has most observations in gbif and native range overlaps with M. sinensis and is not cultivated as far as I can tell</t>
+  </si>
+  <si>
+    <t>Oryza officinalis</t>
+  </si>
+  <si>
+    <t>Close relative in the same genus with native range that overlaps with O. sativa</t>
+  </si>
+  <si>
+    <t>Panicum capillare</t>
+  </si>
+  <si>
+    <t>Has the most gbif observations in genus and is a seemingly non-cultivated wild relative</t>
+  </si>
+  <si>
+    <t>Phaseolus leptostachyus</t>
+  </si>
+  <si>
+    <t>non-cultivated relative with most observations on gbif</t>
+  </si>
+  <si>
+    <t>Prunus leveilleana</t>
+  </si>
+  <si>
+    <t>non-cultivated relative with most gbif observations</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11295-015-0921-7, observations overlap with native range and I can filter out non-native continents</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s13059-014-0415-1</t>
+  </si>
+  <si>
+    <t>Prunus davidiana</t>
+  </si>
+  <si>
+    <t>quercus robur</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/23802359.2021.2011447</t>
+  </si>
+  <si>
+    <t>Secale strictum</t>
+  </si>
+  <si>
+    <t>Sesamum radiatum</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/pdf/10.1002/lipi.19920940705 , has the most observations out of the three wild species in this study</t>
+  </si>
+  <si>
+    <t>Setaria faberi</t>
+  </si>
+  <si>
+    <t>Sorghum halepense</t>
+  </si>
+  <si>
+    <t>in the same genus as S. bicolor and has lots of gbif observations and overlaps with the native range of S. bicolor a little bit</t>
+  </si>
+  <si>
+    <t>Spinacia oleracea subsp. turkestanica</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10722-020-01042-y</t>
+  </si>
+  <si>
+    <t>Thinopyrum junceum</t>
+  </si>
+  <si>
+    <t>close relative with lots of gbif observations and a native range that overlaps the native range of T. intermedium</t>
+  </si>
+  <si>
+    <t>Trifolium medium</t>
+  </si>
+  <si>
+    <t>close relative in timetree with lots of gbif observations and a native range that overlaps the native range of T. pratense</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/srep10763</t>
+  </si>
+  <si>
+    <t>Triticum timopheevii</t>
+  </si>
+  <si>
+    <t>has lots of gbif observations in this genus. Native range is close to native range of T. turgidum</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s12870-016-0847-8</t>
+  </si>
+  <si>
+    <t>Vigna radiata var. sublobata</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/BF00028613</t>
+  </si>
+  <si>
+    <t>Vigna minima</t>
+  </si>
+  <si>
+    <t>Zea mays subsp. parviglumis</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41588-022-01186-w</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.17113%2Fftb.57.01.19.5910</t>
+  </si>
+  <si>
+    <t>Ziziphus jujuba var. spinosa</t>
   </si>
 </sst>
 </file>
@@ -3216,9 +3360,9 @@
   <dimension ref="A1:V350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G140" sqref="G140"/>
+      <selection pane="bottomLeft" activeCell="F345" sqref="F345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7474,7 +7618,7 @@
       <c r="U144"/>
       <c r="V144"/>
     </row>
-    <row r="145" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>112</v>
       </c>
@@ -7488,8 +7632,12 @@
         <v>446</v>
       </c>
       <c r="E145" s="3"/>
-      <c r="F145" s="3"/>
-      <c r="G145" s="7"/>
+      <c r="F145" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="G145" s="7" t="s">
+        <v>925</v>
+      </c>
       <c r="H145" s="3"/>
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
@@ -7814,7 +7962,12 @@
       <c r="D159" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="G159" s="13"/>
+      <c r="F159" s="4" t="s">
+        <v>926</v>
+      </c>
+      <c r="G159" s="13" t="s">
+        <v>927</v>
+      </c>
       <c r="O159" s="13"/>
       <c r="P159" s="12">
         <v>300</v>
@@ -7915,7 +8068,12 @@
       <c r="D165" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="G165" s="7"/>
+      <c r="F165" s="3" t="s">
+        <v>928</v>
+      </c>
+      <c r="G165" s="7" t="s">
+        <v>929</v>
+      </c>
       <c r="O165" s="7"/>
       <c r="P165" s="10">
         <v>550</v>
@@ -8156,7 +8314,12 @@
       <c r="D173" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="G173" s="7"/>
+      <c r="F173" s="3" t="s">
+        <v>931</v>
+      </c>
+      <c r="G173" s="7" t="s">
+        <v>930</v>
+      </c>
       <c r="O173" s="7" t="s">
         <v>304</v>
       </c>
@@ -8385,7 +8548,7 @@
       </c>
       <c r="V181" s="3"/>
     </row>
-    <row r="182" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:22" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
         <v>517</v>
       </c>
@@ -8398,7 +8561,12 @@
       <c r="D182" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="G182" s="7"/>
+      <c r="F182" s="3" t="s">
+        <v>932</v>
+      </c>
+      <c r="G182" s="7" t="s">
+        <v>933</v>
+      </c>
       <c r="O182" s="7"/>
       <c r="P182" s="10">
         <v>208</v>
@@ -8838,7 +9006,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="197" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" s="3" t="s">
         <v>129</v>
       </c>
@@ -8852,8 +9020,12 @@
         <v>446</v>
       </c>
       <c r="E197" s="3"/>
-      <c r="F197" s="3"/>
-      <c r="G197" s="7"/>
+      <c r="F197" s="3" t="s">
+        <v>934</v>
+      </c>
+      <c r="G197" s="7" t="s">
+        <v>935</v>
+      </c>
       <c r="H197" s="3"/>
       <c r="I197" s="3"/>
       <c r="J197" s="3"/>
@@ -9626,7 +9798,9 @@
         <v>318</v>
       </c>
       <c r="E224" s="3"/>
-      <c r="F224" s="3"/>
+      <c r="F224" s="3" t="s">
+        <v>398</v>
+      </c>
       <c r="G224" s="7"/>
       <c r="H224" s="3"/>
       <c r="I224" s="3"/>
@@ -9674,8 +9848,12 @@
         <v>446</v>
       </c>
       <c r="E225" s="3"/>
-      <c r="F225" s="3"/>
-      <c r="G225" s="7"/>
+      <c r="F225" s="3" t="s">
+        <v>936</v>
+      </c>
+      <c r="G225" s="7" t="s">
+        <v>937</v>
+      </c>
       <c r="H225" s="3"/>
       <c r="I225" s="3"/>
       <c r="J225" s="3"/>
@@ -9785,8 +9963,12 @@
         <v>446</v>
       </c>
       <c r="E228" s="3"/>
-      <c r="F228" s="3"/>
-      <c r="G228" s="7"/>
+      <c r="F228" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="G228" s="7" t="s">
+        <v>939</v>
+      </c>
       <c r="H228" s="3"/>
       <c r="I228" s="3"/>
       <c r="J228" s="3"/>
@@ -10006,7 +10188,7 @@
       <c r="U238"/>
       <c r="V238"/>
     </row>
-    <row r="239" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:22" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
         <v>49</v>
       </c>
@@ -10019,7 +10201,12 @@
       <c r="D239" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="G239" s="7"/>
+      <c r="F239" s="3" t="s">
+        <v>940</v>
+      </c>
+      <c r="G239" s="7" t="s">
+        <v>941</v>
+      </c>
       <c r="O239" s="7"/>
       <c r="P239" s="10">
         <v>683</v>
@@ -10375,7 +10562,7 @@
       <c r="U256"/>
       <c r="V256"/>
     </row>
-    <row r="257" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
         <v>541</v>
       </c>
@@ -10389,8 +10576,12 @@
         <v>456</v>
       </c>
       <c r="E257" s="3"/>
-      <c r="F257" s="3"/>
-      <c r="G257" s="7"/>
+      <c r="F257" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="G257" s="7" t="s">
+        <v>943</v>
+      </c>
       <c r="H257" s="3"/>
       <c r="I257" s="3"/>
       <c r="J257" s="3"/>
@@ -10415,7 +10606,7 @@
       <c r="U257" s="3"/>
       <c r="V257" s="3"/>
     </row>
-    <row r="258" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
         <v>410</v>
       </c>
@@ -10429,8 +10620,12 @@
         <v>318</v>
       </c>
       <c r="E258" s="3"/>
-      <c r="F258" s="3"/>
-      <c r="G258" s="7"/>
+      <c r="F258" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="G258" s="21" t="s">
+        <v>944</v>
+      </c>
       <c r="H258" s="3"/>
       <c r="I258" s="3"/>
       <c r="J258" s="3"/>
@@ -10484,8 +10679,12 @@
         <v>446</v>
       </c>
       <c r="E260" s="3"/>
-      <c r="F260" s="3"/>
-      <c r="G260" s="7"/>
+      <c r="F260" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="G260" s="7" t="s">
+        <v>945</v>
+      </c>
       <c r="H260" s="3"/>
       <c r="I260" s="3"/>
       <c r="J260" s="3"/>
@@ -10593,6 +10792,9 @@
       </c>
       <c r="D264" s="3" t="s">
         <v>456</v>
+      </c>
+      <c r="F264" s="3" t="s">
+        <v>947</v>
       </c>
       <c r="G264" s="7"/>
       <c r="O264" s="7" t="s">
@@ -10932,7 +11134,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="279" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:22" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="4" t="s">
         <v>309</v>
       </c>
@@ -10945,16 +11147,12 @@
       <c r="D279" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="E279" s="4"/>
-      <c r="F279" s="4"/>
-      <c r="G279" s="13"/>
-      <c r="H279" s="4"/>
-      <c r="I279" s="4"/>
-      <c r="J279" s="4"/>
-      <c r="K279" s="4"/>
-      <c r="L279" s="4"/>
-      <c r="M279" s="4"/>
-      <c r="N279" s="4"/>
+      <c r="F279" s="4" t="s">
+        <v>949</v>
+      </c>
+      <c r="G279" s="4" t="s">
+        <v>948</v>
+      </c>
       <c r="O279" s="13" t="s">
         <v>323</v>
       </c>
@@ -10967,10 +11165,6 @@
       <c r="R279" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="S279" s="4"/>
-      <c r="T279" s="4"/>
-      <c r="U279" s="4"/>
-      <c r="V279" s="4"/>
     </row>
     <row r="280" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
@@ -10991,7 +11185,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="282" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:22" ht="60" x14ac:dyDescent="0.25">
       <c r="A282" s="3" t="s">
         <v>426</v>
       </c>
@@ -11005,8 +11199,12 @@
         <v>318</v>
       </c>
       <c r="E282" s="3"/>
-      <c r="F282" s="3"/>
-      <c r="G282" s="7"/>
+      <c r="F282" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="G282" s="21" t="s">
+        <v>951</v>
+      </c>
       <c r="H282" s="3"/>
       <c r="I282" s="3"/>
       <c r="J282" s="3"/>
@@ -11045,7 +11243,9 @@
         <v>446</v>
       </c>
       <c r="E283" s="3"/>
-      <c r="F283" s="3"/>
+      <c r="F283" s="3" t="s">
+        <v>952</v>
+      </c>
       <c r="G283" s="7"/>
       <c r="H283" s="3"/>
       <c r="I283" s="3"/>
@@ -11208,6 +11408,9 @@
       </c>
       <c r="D291" s="3" t="s">
         <v>446</v>
+      </c>
+      <c r="F291" s="3" t="s">
+        <v>556</v>
       </c>
       <c r="G291" s="7"/>
       <c r="O291" s="7" t="s">
@@ -11458,7 +11661,7 @@
       <c r="U299" s="4"/>
       <c r="V299" s="4"/>
     </row>
-    <row r="300" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A300" s="4" t="s">
         <v>31</v>
       </c>
@@ -11472,8 +11675,12 @@
         <v>446</v>
       </c>
       <c r="E300" s="4"/>
-      <c r="F300" s="4"/>
-      <c r="G300" s="13"/>
+      <c r="F300" s="4" t="s">
+        <v>953</v>
+      </c>
+      <c r="G300" s="13" t="s">
+        <v>954</v>
+      </c>
       <c r="H300" s="4"/>
       <c r="I300" s="4"/>
       <c r="J300" s="4"/>
@@ -11540,8 +11747,12 @@
         <v>446</v>
       </c>
       <c r="E303" s="3"/>
-      <c r="F303" s="3"/>
-      <c r="G303" s="7"/>
+      <c r="F303" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="G303" s="7" t="s">
+        <v>956</v>
+      </c>
       <c r="H303" s="3"/>
       <c r="I303" s="3"/>
       <c r="J303" s="3"/>
@@ -11800,7 +12011,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="314" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:22" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A314" s="3" t="s">
         <v>27</v>
       </c>
@@ -11813,7 +12024,12 @@
       <c r="D314" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="G314" s="7"/>
+      <c r="F314" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="G314" s="7" t="s">
+        <v>958</v>
+      </c>
       <c r="O314" s="7" t="s">
         <v>142</v>
       </c>
@@ -11840,6 +12056,9 @@
       <c r="D315" s="3" t="s">
         <v>456</v>
       </c>
+      <c r="F315" s="3" t="s">
+        <v>565</v>
+      </c>
       <c r="G315" s="7"/>
       <c r="O315" s="7" t="s">
         <v>584</v>
@@ -11852,7 +12071,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="316" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A316" s="3" t="s">
         <v>95</v>
       </c>
@@ -11866,8 +12085,12 @@
         <v>446</v>
       </c>
       <c r="E316" s="3"/>
-      <c r="F316" s="3"/>
-      <c r="G316" s="7"/>
+      <c r="F316" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="G316" s="7" t="s">
+        <v>960</v>
+      </c>
       <c r="H316" s="3"/>
       <c r="I316" s="3"/>
       <c r="J316" s="3"/>
@@ -11936,7 +12159,9 @@
         <v>446</v>
       </c>
       <c r="E318" s="3"/>
-      <c r="F318" s="3"/>
+      <c r="F318" s="3" t="s">
+        <v>434</v>
+      </c>
       <c r="G318" s="7"/>
       <c r="H318" s="3"/>
       <c r="I318" s="3"/>
@@ -11972,7 +12197,12 @@
       <c r="C319" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="G319" s="13"/>
+      <c r="F319" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="G319" s="13" t="s">
+        <v>961</v>
+      </c>
       <c r="O319" s="13" t="s">
         <v>743</v>
       </c>
@@ -12019,7 +12249,7 @@
       <c r="U320"/>
       <c r="V320"/>
     </row>
-    <row r="321" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:22" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A321" s="4" t="s">
         <v>32</v>
       </c>
@@ -12032,7 +12262,12 @@
       <c r="D321" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="G321" s="13"/>
+      <c r="F321" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="G321" s="13" t="s">
+        <v>963</v>
+      </c>
       <c r="O321" s="13" t="s">
         <v>301</v>
       </c>
@@ -12163,8 +12398,12 @@
       </c>
       <c r="D327" s="3"/>
       <c r="E327" s="3"/>
-      <c r="F327" s="3"/>
-      <c r="G327" s="7"/>
+      <c r="F327" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="G327" s="3" t="s">
+        <v>964</v>
+      </c>
       <c r="H327" s="3"/>
       <c r="I327" s="3"/>
       <c r="J327" s="3"/>
@@ -12201,8 +12440,12 @@
         <v>456</v>
       </c>
       <c r="E328" s="3"/>
-      <c r="F328" s="3"/>
-      <c r="G328" s="7"/>
+      <c r="F328" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="G328" s="3" t="s">
+        <v>966</v>
+      </c>
       <c r="H328" s="3"/>
       <c r="I328" s="3"/>
       <c r="J328" s="3"/>
@@ -12451,7 +12694,12 @@
       <c r="D339" s="4" t="s">
         <v>446</v>
       </c>
-      <c r="G339" s="13"/>
+      <c r="F339" s="13" t="s">
+        <v>968</v>
+      </c>
+      <c r="G339" s="13" t="s">
+        <v>969</v>
+      </c>
       <c r="O339" s="13" t="s">
         <v>798</v>
       </c>
@@ -12538,7 +12786,9 @@
         <v>456</v>
       </c>
       <c r="E344" s="3"/>
-      <c r="F344" s="3"/>
+      <c r="F344" s="3" t="s">
+        <v>571</v>
+      </c>
       <c r="G344" s="7"/>
       <c r="H344" s="3"/>
       <c r="I344" s="3"/>
@@ -12564,7 +12814,7 @@
       <c r="U344" s="3"/>
       <c r="V344" s="3"/>
     </row>
-    <row r="345" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A345" s="3" t="s">
         <v>572</v>
       </c>
@@ -12578,8 +12828,12 @@
         <v>456</v>
       </c>
       <c r="E345" s="3"/>
-      <c r="F345" s="3"/>
-      <c r="G345" s="7"/>
+      <c r="F345" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="G345" s="7" t="s">
+        <v>970</v>
+      </c>
       <c r="H345" s="3"/>
       <c r="I345" s="3"/>
       <c r="J345" s="3"/>
@@ -12697,9 +12951,11 @@
     <hyperlink ref="B40" r:id="rId5" display="https://doi.org/10.3390%2Fijms21186700" xr:uid="{EC67C21D-41B4-4AED-B5CA-A031949BD1CE}"/>
     <hyperlink ref="B228" r:id="rId6" xr:uid="{2677786D-08C7-4346-837D-960E754FAB79}"/>
     <hyperlink ref="G92" r:id="rId7" xr:uid="{BA568409-981D-4049-9F64-BEB3B33169A6}"/>
+    <hyperlink ref="G258" r:id="rId8" xr:uid="{9B248C90-96EE-4A81-A486-9C3F17AAAE42}"/>
+    <hyperlink ref="G282" r:id="rId9" xr:uid="{70EA6D1D-5EF1-4BE0-BD29-78343D9AEAC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add wcvp distribution data
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\16516764_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\3737510_2_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0669C488-0554-4391-8C4E-9A59B609DB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC596C0-F660-41F5-9B71-2C17179E7112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3369,9 +3369,9 @@
   <dimension ref="A1:V350"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A340" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A350" sqref="A350"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add plant height data, remove empty mass data
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\3737510_2_7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\1312258_3_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC596C0-F660-41F5-9B71-2C17179E7112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8BBC85-2613-4052-96E4-ED529DF7D620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3104" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3109" uniqueCount="980">
   <si>
     <t>Species</t>
   </si>
@@ -2966,6 +2966,21 @@
   </si>
   <si>
     <t>https://doi.org/10.1101/2023.04.27.537858</t>
+  </si>
+  <si>
+    <t>Saponaria officinalis v1.1</t>
+  </si>
+  <si>
+    <t>Ehretia anacua AZ 03848 HAP1 v1.1</t>
+  </si>
+  <si>
+    <t>Mimulus nasutus var. SF v2.1</t>
+  </si>
+  <si>
+    <t>Rubus argutus v1.2</t>
+  </si>
+  <si>
+    <t>Rubus ulmifolius v1.1</t>
   </si>
 </sst>
 </file>
@@ -3366,12 +3381,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V350"/>
+  <dimension ref="A1:V355"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6229,48 +6244,42 @@
       <c r="V92" s="3"/>
     </row>
     <row r="93" spans="1:22" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
+      <c r="A93" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C93" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="E93" s="4"/>
-      <c r="F93" s="4" t="s">
+      <c r="F93" s="3" t="s">
         <v>917</v>
       </c>
-      <c r="G93" s="13" t="s">
+      <c r="G93" s="7" t="s">
         <v>915</v>
       </c>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="4"/>
-      <c r="K93" s="4"/>
-      <c r="L93" s="4"/>
-      <c r="M93" s="4"/>
-      <c r="N93" s="4"/>
-      <c r="O93" s="13" t="s">
+      <c r="O93" s="7" t="s">
         <v>758</v>
       </c>
-      <c r="P93" s="12">
+      <c r="P93" s="10">
         <v>115</v>
       </c>
-      <c r="Q93" s="4">
-        <v>1</v>
-      </c>
-      <c r="R93" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="S93" s="4"/>
-      <c r="T93" s="4"/>
-      <c r="U93" s="4"/>
-      <c r="V93" s="4"/>
+      <c r="Q93" s="3">
+        <v>1</v>
+      </c>
+      <c r="R93" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="T93" s="15">
+        <v>45202</v>
+      </c>
+      <c r="U93" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
@@ -7958,7 +7967,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="159" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:22" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>24</v>
       </c>
@@ -10611,8 +10620,12 @@
         <v>257</v>
       </c>
       <c r="S257" s="3"/>
-      <c r="T257" s="3"/>
-      <c r="U257" s="3"/>
+      <c r="T257" s="15">
+        <v>45202</v>
+      </c>
+      <c r="U257" s="3">
+        <v>12</v>
+      </c>
       <c r="V257" s="3"/>
     </row>
     <row r="258" spans="1:22" ht="45" x14ac:dyDescent="0.25">
@@ -11433,6 +11446,12 @@
       </c>
       <c r="R291" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="T291" s="15">
+        <v>45202</v>
+      </c>
+      <c r="U291" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="292" spans="1:22" x14ac:dyDescent="0.25">
@@ -11670,49 +11689,38 @@
       <c r="U299" s="4"/>
       <c r="V299" s="4"/>
     </row>
-    <row r="300" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A300" s="4" t="s">
+    <row r="300" spans="1:22" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B300" s="4" t="s">
+      <c r="B300" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C300" s="4" t="s">
+      <c r="C300" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D300" s="4" t="s">
+      <c r="D300" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="E300" s="4"/>
-      <c r="F300" s="4" t="s">
+      <c r="F300" s="3" t="s">
         <v>952</v>
       </c>
-      <c r="G300" s="13" t="s">
+      <c r="G300" s="7" t="s">
         <v>953</v>
       </c>
-      <c r="H300" s="4"/>
-      <c r="I300" s="4"/>
-      <c r="J300" s="4"/>
-      <c r="K300" s="4"/>
-      <c r="L300" s="4"/>
-      <c r="M300" s="4"/>
-      <c r="N300" s="4"/>
-      <c r="O300" s="13" t="s">
+      <c r="O300" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="P300" s="12">
+      <c r="P300" s="10">
         <v>400</v>
       </c>
-      <c r="Q300" s="4">
-        <v>1</v>
-      </c>
-      <c r="R300" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="S300" s="4"/>
-      <c r="T300" s="4"/>
-      <c r="U300" s="4"/>
-      <c r="V300" s="4"/>
+      <c r="Q300" s="3">
+        <v>1</v>
+      </c>
+      <c r="R300" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="T300" s="15"/>
     </row>
     <row r="301" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
@@ -11782,8 +11790,12 @@
         <v>257</v>
       </c>
       <c r="S303" s="3"/>
-      <c r="T303" s="3"/>
-      <c r="U303" s="3"/>
+      <c r="T303" s="15">
+        <v>45202</v>
+      </c>
+      <c r="U303" s="3">
+        <v>12</v>
+      </c>
       <c r="V303" s="3"/>
     </row>
     <row r="304" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -12959,6 +12971,31 @@
       </c>
       <c r="P350" s="10">
         <v>227</v>
+      </c>
+    </row>
+    <row r="351" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="352" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more genome sizes
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\1312258_3_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\6031870_2_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8BBC85-2613-4052-96E4-ED529DF7D620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEEE715-5A78-44F8-8530-B4E6CAC86A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3109" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3151" uniqueCount="1014">
   <si>
     <t>Species</t>
   </si>
@@ -2981,6 +2981,108 @@
   </si>
   <si>
     <t>Rubus ulmifolius v1.1</t>
+  </si>
+  <si>
+    <t>DNA amount (1 C; pg)</t>
+  </si>
+  <si>
+    <t>Hopping ME.  1994.  Flow cytometric analysis of Actinidia species.  New Zealand Journal of Botany 32: 85-93.</t>
+  </si>
+  <si>
+    <t>Bennett MD, Smith JB. 1991. Nuclear DNA amounts in angiosperms. Philosophical Transactions of the Royal Society of London Series B-Biological Sciences 334: 309-345.</t>
+  </si>
+  <si>
+    <t>Arumuganathan K, Earle ED. 1991. Nuclear DNA content of some important plant species. Plant Molecular Biology Reporter 9: 208-218.</t>
+  </si>
+  <si>
+    <t>Lysák MA, Koch MA, Beaulieu JM, Meister A, Leitch IJ. 2009. The dynamic ups and downs of genome size evolution in Brassicaceae. Molecular Biology and Evolution 26: 85-98.</t>
+  </si>
+  <si>
+    <t>Bennett  et al . Comparisons with Caenorhabditis (~100 Mb) and Drosophila (~ 175 Mb) using flow cytometry show genome size in Arabidopsis to be ~157 Mb and thus ~25 % larger than the Arabidopsis Genome Initiative estimate of ~125 Mb. Ann Bot 91: 547-557.</t>
+  </si>
+  <si>
+    <t>Temsch EM, Greilhuber J. 2001. Genome size in Arachis duranensis: a critical study. Genome 44: 826-830.</t>
+  </si>
+  <si>
+    <t>Temsch EM, Greilhuber J. 2000. Genome size variation in Arachis hypogaea and A. monticola re- evaluated. Genome 43: 449-451.</t>
+  </si>
+  <si>
+    <t>Singh KP, Raina SN, Singh AK. 1996. Variation in chromosomal DNA associated with the evolution of Arachis species. Genome 39, 890-897.</t>
+  </si>
+  <si>
+    <t>Bennett MD,  Smith JB, Heslop-Harrison JS. 1982. Nuclear DNA amounts in angiosperms. Proceedings of the Royal Society of London Series B-Biological Sciences 216: 179-199.</t>
+  </si>
+  <si>
+    <t>Barow M, Meister A. 2003. Endopolyploidy in seed plants is differently correlated to systematics, organ, life strategy and genome size. Plant Cell and Environment 26: 571-584.</t>
+  </si>
+  <si>
+    <t>Catalán P, Müller J, Hasterok R, Jenkins G, Mur LAJ et al. 2012.  Evolution and taxonomic split of the model grass Brachypodium distachyon. Annals of Botany 109: 385-405.</t>
+  </si>
+  <si>
+    <t>Wolny E, Hasterok R. 2009. Comparative cytogenetic analysis of the genomes of the model grass Brachypodium distachyon and its close relatives. Annals of Botany 104: 873-881.</t>
+  </si>
+  <si>
+    <t>Verma SC, Rees H. 1974. Nuclear DNA and evolution of allotetraploid Brassicae. Heredity 33: 61-68.</t>
+  </si>
+  <si>
+    <t>Greilhuber J. 1988.</t>
+  </si>
+  <si>
+    <t>Olszewska MJ, Osiecka R. 1983 Relationship between 2C DNA content, life-cycle, systematic position of DNA endoreplication dynamics in parenchyma nuclei during growth &amp;amp; differentiation of roots in dicot herbaceous sp. Biochem Physiol  Pflanzen 178: 581-599</t>
+  </si>
+  <si>
+    <t>Ingle J,  Timmis JN, Sinclair J. 1975. Relationship between satellite deoxyribonucleic acid, ribosomal ribonucleic acid gene redundancy, and genome size in plants. Plant Physiology 55: 496-501.</t>
+  </si>
+  <si>
+    <t>Bennett MD, Smith JB. 1976. Nuclear DNA amounts in angiosperms. Philosophical Transactions of the Royal Society of London Series B-Biological Sciences 274: 227-274.</t>
+  </si>
+  <si>
+    <t>Hanson L., McMahon KA, Johnson MAT, Bennett MD. 2001. First nuclear DNA C-values for another 25 angiosperm families. Annals of Botany 88: 851-858</t>
+  </si>
+  <si>
+    <t>Sakamoto K, Akiyama Y, Fukui K, Kamada H, Satoh S. 1998. Characterization: genome sizes and morphology of sex chromosomes in Hemp (Cannabis sativa L.). Cytologia 63: 459-464</t>
+  </si>
+  <si>
+    <t>Moscone EA, Baranyi M, Ebert I, Greilhuber J, Ehrendorfer F, Hunziker AT. 2003. Analysis of nuclear DNA content in Capsicum (Solanaceae) by flow cytometry and Feulgen densitometry. Annals of Botany 92: 21-29.</t>
+  </si>
+  <si>
+    <t>Palomino G, Hernandez LT, Torres ED. 2008. Nuclear genome size and chromosome analysis in Chenopodium quinoa and C. berlandieri subsp. nuttalliae. Euphytica 164: 221-230.</t>
+  </si>
+  <si>
+    <t>Kiehn M. 1986. Karyosystematische Untersuchungen und DNA-Messungen an Rubiaceae und ihre Bedeutung für die Systematik dieser Familie. Ph. D. Thesis. Universität Wien.</t>
+  </si>
+  <si>
+    <t>Noirot M, Poncet V, Barre P, Hamon P, Hamon S, De Kochko A. 2003. Genome size variations in diploid African Coffea species. Annals of Botany 92: 709-714.</t>
+  </si>
+  <si>
+    <t>Pustahija F, Brown SC, Bogunic F, Bašic N, Muratovic E, Ollier S, Hidalgo O, Bourge M, Stevanovic V, Sijak-Yakovev S. 2013.  Small genomes dominate in plants growing on serpentine soils in West Balkans, an exhaustive study of 8 habitats covering 308 taxa.</t>
+  </si>
+  <si>
+    <t>Ramachandran C, Narayan RKJ. 1985. Chromosomal DNA variation in Cucumis. Theoretical and Applied Genetics 69: 497-502.</t>
+  </si>
+  <si>
+    <t>Sisko M, Ivancic A, Bohanec B. 2003. Genome size analysis in the genus Cucurbita and its use for determination of interspecific hybrids obtained using the embryo-rescue technique. Plant Science 165: 663-669.</t>
+  </si>
+  <si>
+    <t>Adoukonou-Sagbadja H, Schubert V, Dansi A et al. 2007. Flow cytometric analysis reveals different nuclear DNA contents in cultivated Fonio (Digitaria spp.) and some wild relatives from West-Africa. Pl. Syst. Evol. 267: 163-176.</t>
+  </si>
+  <si>
+    <t>The average of two estimates from: Arumuganathan K, Earle ED. 1991. Nuclear DNA content of some important plant species. Plant Molecular Biology Reporter 9: 208-218. and Dansi A, Saïnou O, Agbangla C, Ahanhanzo C, Brown S, Adoukonou-Sagbadja H. 2005. Ploidy level and nuclear DNA content of some accessions of water yam (Dioscorea alata) collected at Savè, a district of central Benin. Plant Genet. Res. Newslet. 144: 20-23.</t>
+  </si>
+  <si>
+    <t>Obidiegwu JE, Rodriguez E, Ene-obong EE, Loureiro J, Muoneke CO, Santos C, Kolesnikova-Allen M, Asiedu R. 2009. Estimation of the nuclear DNA content in some representative of genus Dioscorea. Scientific Research and Essays 4: 448-452.</t>
+  </si>
+  <si>
+    <t>Camillo J, Leão AP, Alves AA, Formighieri EF, Azevedo ALS, Nunes JD, de Capdeville G, Mattos JKdA, Souza Jr MT. 2014.  Reassessment of the genome size in Elaeis guineensis and Elaeis oleifera, and its interspecific hybrid. Genomics Insights 7: 13-22.</t>
+  </si>
+  <si>
+    <t>Loureiro J, Rodriguez E, Doležel J, Santos C. 2007. Two new nuclear isolation buffers for plant DNA flow cytometry: a test with 37 species. Annals of Botany 100: 875-888.</t>
+  </si>
+  <si>
+    <t>Greilhuber J, Obermayer R. 1997. Genome size and maturity group in Glycine max (soybean). Heredity 78: 547-551.</t>
+  </si>
+  <si>
+    <t>Hammatt N, Blackhall NW, Davey MR. 1991. Variation in the DNA content of Glycine species. 42: 659-665.</t>
   </si>
 </sst>
 </file>
@@ -3383,10 +3485,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V355"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A257" sqref="A257"/>
+      <selection pane="bottomLeft" activeCell="J134" sqref="J134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3430,7 +3532,7 @@
         <v>811</v>
       </c>
       <c r="I1" t="s">
-        <v>767</v>
+        <v>980</v>
       </c>
       <c r="J1" t="s">
         <v>768</v>
@@ -3522,10 +3624,10 @@
       <c r="G3" s="7"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3">
-        <v>784</v>
+        <v>0.8</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>769</v>
+        <v>981</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -3694,8 +3796,12 @@
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>982</v>
+      </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -3806,8 +3912,12 @@
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>983</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -3864,6 +3974,12 @@
         <v>26</v>
       </c>
       <c r="G14" s="7"/>
+      <c r="I14" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>984</v>
+      </c>
       <c r="K14" s="3" t="s">
         <v>869</v>
       </c>
@@ -3923,8 +4039,12 @@
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>984</v>
+      </c>
       <c r="K16" s="3" t="s">
         <v>852</v>
       </c>
@@ -3969,6 +4089,12 @@
         <v>461</v>
       </c>
       <c r="G17" s="7"/>
+      <c r="I17" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>984</v>
+      </c>
       <c r="O17" s="7"/>
       <c r="P17" s="10">
         <v>12</v>
@@ -4010,8 +4136,12 @@
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>985</v>
+      </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -4086,6 +4216,12 @@
         <v>160</v>
       </c>
       <c r="G20" s="13"/>
+      <c r="I20" s="4">
+        <v>0.38</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>984</v>
+      </c>
       <c r="O20" s="13"/>
       <c r="P20" s="12">
         <v>306</v>
@@ -4157,6 +4293,12 @@
         <v>456</v>
       </c>
       <c r="G22" s="13"/>
+      <c r="I22" s="4">
+        <v>1.27</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>986</v>
+      </c>
       <c r="O22" s="13" t="s">
         <v>618</v>
       </c>
@@ -4209,8 +4351,12 @@
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="3">
+        <v>2.87</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>987</v>
+      </c>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -4355,8 +4501,12 @@
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>988</v>
+      </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -4453,6 +4603,12 @@
         <v>765</v>
       </c>
       <c r="G32" s="13"/>
+      <c r="I32" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>989</v>
+      </c>
       <c r="O32" s="13" t="s">
         <v>766</v>
       </c>
@@ -4494,8 +4650,12 @@
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>990</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -4613,8 +4773,12 @@
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="I37" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>984</v>
+      </c>
       <c r="K37" s="3" t="s">
         <v>845</v>
       </c>
@@ -4703,8 +4867,12 @@
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
+      <c r="I40" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>991</v>
+      </c>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -4788,6 +4956,12 @@
         <v>777</v>
       </c>
       <c r="G43" s="13"/>
+      <c r="I43" s="4">
+        <v>0.43</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>992</v>
+      </c>
       <c r="O43" s="13" t="s">
         <v>842</v>
       </c>
@@ -4841,6 +5015,12 @@
         <v>824</v>
       </c>
       <c r="G46" s="7"/>
+      <c r="I46" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>993</v>
+      </c>
       <c r="O46" s="7"/>
       <c r="P46" s="10">
         <v>479</v>
@@ -4871,8 +5051,12 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
+      <c r="I47" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>994</v>
+      </c>
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -4909,6 +5093,12 @@
         <v>772</v>
       </c>
       <c r="G48" s="13"/>
+      <c r="I48" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>993</v>
+      </c>
       <c r="O48" s="13" t="s">
         <v>800</v>
       </c>
@@ -4944,8 +5134,12 @@
         <v>858</v>
       </c>
       <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
+      <c r="I49" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>995</v>
+      </c>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
@@ -5003,8 +5197,12 @@
         <v>860</v>
       </c>
       <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
+      <c r="I51" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>996</v>
+      </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
@@ -5108,6 +5306,12 @@
         <v>875</v>
       </c>
       <c r="G54" s="7"/>
+      <c r="I54" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>997</v>
+      </c>
       <c r="M54" s="3">
         <v>2</v>
       </c>
@@ -5202,6 +5406,12 @@
       <c r="G56" s="7" t="s">
         <v>862</v>
       </c>
+      <c r="I56" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>998</v>
+      </c>
       <c r="O56" s="7" t="s">
         <v>623</v>
       </c>
@@ -5242,8 +5452,12 @@
         <v>909</v>
       </c>
       <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="I57" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>999</v>
+      </c>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
@@ -5367,6 +5581,12 @@
         <v>50</v>
       </c>
       <c r="G61" s="7"/>
+      <c r="I61" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>984</v>
+      </c>
       <c r="O61" s="7" t="s">
         <v>724</v>
       </c>
@@ -5431,8 +5651,12 @@
         <v>908</v>
       </c>
       <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
+      <c r="I63" s="3">
+        <v>3.16</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>1000</v>
+      </c>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
@@ -5689,6 +5913,12 @@
       </c>
       <c r="G73" s="7" t="s">
         <v>876</v>
+      </c>
+      <c r="I73" s="3">
+        <v>1.48</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>1001</v>
       </c>
       <c r="M73" s="3">
         <v>4</v>
@@ -5768,8 +5998,12 @@
       <c r="F76" s="3"/>
       <c r="G76" s="7"/>
       <c r="H76" s="3"/>
-      <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
+      <c r="I76" s="3">
+        <v>1</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>997</v>
+      </c>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
       <c r="M76" s="3"/>
@@ -5961,6 +6195,12 @@
       <c r="G82" s="7" t="s">
         <v>810</v>
       </c>
+      <c r="I82" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>1002</v>
+      </c>
       <c r="O82" s="7" t="s">
         <v>584</v>
       </c>
@@ -5998,6 +6238,12 @@
       </c>
       <c r="G83" s="4" t="s">
         <v>912</v>
+      </c>
+      <c r="I83" s="4">
+        <v>0.72</v>
+      </c>
+      <c r="J83" s="4" t="s">
+        <v>1003</v>
       </c>
       <c r="O83" s="13" t="s">
         <v>342</v>
@@ -6108,6 +6354,12 @@
       <c r="G88" s="7" t="s">
         <v>881</v>
       </c>
+      <c r="I88" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>1004</v>
+      </c>
       <c r="M88" s="3">
         <v>2</v>
       </c>
@@ -6222,8 +6474,12 @@
         <v>916</v>
       </c>
       <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
+      <c r="I92" s="3">
+        <v>1</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>996</v>
+      </c>
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
       <c r="M92" s="3"/>
@@ -6262,6 +6518,12 @@
       <c r="G93" s="7" t="s">
         <v>915</v>
       </c>
+      <c r="I93" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>1005</v>
+      </c>
       <c r="O93" s="7" t="s">
         <v>758</v>
       </c>
@@ -6330,8 +6592,12 @@
         <v>746</v>
       </c>
       <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
+      <c r="I96" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>1006</v>
+      </c>
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
       <c r="M96" s="3"/>
@@ -6420,8 +6686,12 @@
       </c>
       <c r="G99" s="7"/>
       <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
+      <c r="I99" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="J99" s="3" t="s">
+        <v>983</v>
+      </c>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
       <c r="M99" s="3"/>
@@ -6662,8 +6932,12 @@
         <v>864</v>
       </c>
       <c r="H109" s="3"/>
-      <c r="I109" s="3"/>
-      <c r="J109" s="3"/>
+      <c r="I109" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="J109" s="3" t="s">
+        <v>1007</v>
+      </c>
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
       <c r="M109" s="3"/>
@@ -6708,8 +6982,12 @@
         <v>919</v>
       </c>
       <c r="H110" s="3"/>
-      <c r="I110" s="3"/>
-      <c r="J110" s="3"/>
+      <c r="I110" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>1008</v>
+      </c>
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
       <c r="M110" s="3"/>
@@ -6783,6 +7061,12 @@
       <c r="H112" s="3" t="s">
         <v>812</v>
       </c>
+      <c r="I112" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>1009</v>
+      </c>
       <c r="O112" s="7" t="s">
         <v>636</v>
       </c>
@@ -6926,6 +7210,12 @@
         <v>803</v>
       </c>
       <c r="G117" s="7"/>
+      <c r="I117" s="3">
+        <v>2.16</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>1010</v>
+      </c>
       <c r="O117" s="7" t="s">
         <v>586</v>
       </c>
@@ -6959,6 +7249,12 @@
         <v>804</v>
       </c>
       <c r="G118" s="13"/>
+      <c r="I118" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="J118" s="4" t="s">
+        <v>997</v>
+      </c>
       <c r="O118" s="13" t="s">
         <v>586</v>
       </c>
@@ -7089,8 +7385,12 @@
       </c>
       <c r="G125" s="13"/>
       <c r="H125" s="4"/>
-      <c r="I125" s="4"/>
-      <c r="J125" s="4"/>
+      <c r="I125" s="4">
+        <v>0.37</v>
+      </c>
+      <c r="J125" s="4" t="s">
+        <v>1011</v>
+      </c>
       <c r="K125" s="4"/>
       <c r="L125" s="4"/>
       <c r="M125" s="4"/>
@@ -7233,6 +7533,12 @@
         <v>446</v>
       </c>
       <c r="G130" s="7"/>
+      <c r="I130" s="3">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>1012</v>
+      </c>
       <c r="O130" s="7" t="s">
         <v>290</v>
       </c>
@@ -7361,8 +7667,12 @@
       </c>
       <c r="G134" s="19"/>
       <c r="H134" s="8"/>
-      <c r="I134" s="8"/>
-      <c r="J134" s="8"/>
+      <c r="I134" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J134" s="8" t="s">
+        <v>1013</v>
+      </c>
       <c r="K134" s="8"/>
       <c r="L134" s="8"/>
       <c r="M134" s="8"/>

</xml_diff>

<commit_message>
add genome size and mating info
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67100_2_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/132102_2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD57AC0C-C9C2-49CC-9A9B-865AD4069F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{BD57AC0C-C9C2-49CC-9A9B-865AD4069F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9584345-A0A4-48E7-86D0-C6014439D9DB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="1164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3483" uniqueCount="1192">
   <si>
     <t>Species</t>
   </si>
@@ -3533,6 +3533,90 @@
   </si>
   <si>
     <t>https://doi.org/10.1007/s00299-005-0017-1</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/14620316.2015.1108542</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1105/tpc.112.100115</t>
+  </si>
+  <si>
+    <t>mixed</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1439-0523.1991.tb00544.x - but with some small amout of outcrossing, 10-11 %</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.17660/ActaHortic.2009.822.6 ; https://doi.org/10.17660/ActaHortic.1993.334.4</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1601-5223.2004.01833.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1073/pnas.0406970101</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.scienta.2007.03.019 - I think this species might be outcrossing because it experiences a lot of heterosis</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/ece3.1061</t>
+  </si>
+  <si>
+    <t>PMID: 11743099</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1017/S0021859600037801 - 19-79 % outcrossing</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1023/A:1003637814963</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/978-94-009-1207-6_6</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0065-2113(08)60831-7</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s12870-021-02909-7 - no seeds produced when self-pollinated</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/BF00936107 ; https://doi.org/10.2135/cropsci1995.0011183X003500040008x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.4141/cjps2011-182</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371%2Fjournal.pone.0151424 - self-incompatible ; https://doi.org/10.1080/14620316.2007.11512298</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389%2Ffpls.2020.00718</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.flora.2022.152206</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pgen.1003754</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.21273/HORTSCI.19.4.580 ; https://doi.org/10.1023/A:1025075118200</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/g3journal/jkab325</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10722-014-0193-3#citeas</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/ng.2669 - comes from assembly size, couldn't find flow cytometry data</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/gigascience/giz112 - estimated from k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/ng.2470 - based on k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/ng.3972 - estimated from k-mers</t>
   </si>
 </sst>
 </file>
@@ -3936,9 +4020,9 @@
   <dimension ref="A1:W356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A335" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A356" sqref="A356"/>
+      <selection pane="bottomLeft" activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4084,8 +4168,12 @@
       <c r="K3" s="3" t="s">
         <v>981</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="L3" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>1164</v>
+      </c>
       <c r="N3" s="3">
         <v>2</v>
       </c>
@@ -4185,6 +4273,18 @@
         <v>310</v>
       </c>
       <c r="H7" s="13"/>
+      <c r="J7" s="4">
+        <v>4.3967280000000004</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>1186</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>1165</v>
+      </c>
       <c r="N7" s="4">
         <v>2</v>
       </c>
@@ -4270,8 +4370,12 @@
       <c r="K9" s="3" t="s">
         <v>982</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>1167</v>
+      </c>
       <c r="N9" s="3">
         <v>2</v>
       </c>
@@ -4393,8 +4497,12 @@
       <c r="K12" s="3" t="s">
         <v>983</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="L12" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>1168</v>
+      </c>
       <c r="N12" s="3">
         <v>2</v>
       </c>
@@ -4585,6 +4693,12 @@
       <c r="K17" s="3" t="s">
         <v>984</v>
       </c>
+      <c r="L17" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>1169</v>
+      </c>
       <c r="N17" s="3">
         <v>4</v>
       </c>
@@ -4639,8 +4753,12 @@
       <c r="K18" s="3" t="s">
         <v>985</v>
       </c>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>1170</v>
+      </c>
       <c r="N18" s="3">
         <v>2</v>
       </c>
@@ -4724,6 +4842,12 @@
       <c r="K20" s="4" t="s">
         <v>984</v>
       </c>
+      <c r="L20" s="4" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="N20" s="4">
         <v>2</v>
       </c>
@@ -4767,6 +4891,12 @@
         <v>462</v>
       </c>
       <c r="H21" s="7"/>
+      <c r="J21" s="3">
+        <v>0.28016000000000002</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>1063</v>
+      </c>
       <c r="L21" s="3" t="s">
         <v>845</v>
       </c>
@@ -4818,6 +4948,12 @@
       </c>
       <c r="K22" s="4" t="s">
         <v>986</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>1064</v>
       </c>
       <c r="N22" s="4">
         <v>2</v>
@@ -4884,8 +5020,12 @@
       <c r="K24" s="3" t="s">
         <v>987</v>
       </c>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="L24" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N24" s="3">
         <v>4</v>
       </c>
@@ -4931,8 +5071,12 @@
       <c r="G25" s="4"/>
       <c r="H25" s="13"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
+      <c r="J25" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>1187</v>
+      </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -5042,8 +5186,12 @@
       <c r="K28" s="3" t="s">
         <v>988</v>
       </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
+      <c r="L28" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>1064</v>
+      </c>
       <c r="N28" s="3">
         <v>2</v>
       </c>
@@ -5149,6 +5297,12 @@
       <c r="K32" s="4" t="s">
         <v>989</v>
       </c>
+      <c r="L32" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="M32" s="14" t="s">
+        <v>1171</v>
+      </c>
       <c r="N32" s="4">
         <v>2</v>
       </c>
@@ -5203,8 +5357,12 @@
       <c r="K33" s="3" t="s">
         <v>990</v>
       </c>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
+      <c r="L33" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>1172</v>
+      </c>
       <c r="N33" s="3">
         <v>2</v>
       </c>
@@ -5420,8 +5578,12 @@
       <c r="D40" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>1173</v>
+      </c>
       <c r="G40" s="3" t="s">
         <v>128</v>
       </c>
@@ -5433,8 +5595,12 @@
       <c r="K40" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
+      <c r="L40" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>1173</v>
+      </c>
       <c r="N40" s="3">
         <v>2</v>
       </c>
@@ -5598,6 +5764,12 @@
       <c r="K46" s="3" t="s">
         <v>993</v>
       </c>
+      <c r="L46" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>1174</v>
+      </c>
       <c r="N46" s="3">
         <v>4</v>
       </c>
@@ -5641,8 +5813,12 @@
       <c r="K47" s="3" t="s">
         <v>994</v>
       </c>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
+      <c r="L47" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N47" s="3">
         <v>4</v>
       </c>
@@ -5687,6 +5863,12 @@
       <c r="K48" s="4" t="s">
         <v>993</v>
       </c>
+      <c r="L48" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>1175</v>
+      </c>
       <c r="N48" s="4">
         <v>2</v>
       </c>
@@ -5735,8 +5917,12 @@
       <c r="K49" s="3" t="s">
         <v>995</v>
       </c>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
+      <c r="L49" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>1176</v>
+      </c>
       <c r="N49" s="3">
         <v>2</v>
       </c>
@@ -5803,8 +5989,12 @@
       <c r="K51" s="3" t="s">
         <v>996</v>
       </c>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
+      <c r="L51" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>1177</v>
+      </c>
       <c r="N51" s="3">
         <v>2</v>
       </c>
@@ -5877,6 +6067,12 @@
         <v>456</v>
       </c>
       <c r="H53" s="7"/>
+      <c r="L53" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M53" s="5" t="s">
+        <v>1178</v>
+      </c>
       <c r="N53" s="3">
         <v>2</v>
       </c>
@@ -5922,6 +6118,12 @@
       </c>
       <c r="K54" s="3" t="s">
         <v>997</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M54" s="3" t="s">
+        <v>1179</v>
       </c>
       <c r="N54" s="3">
         <v>2</v>
@@ -5970,8 +6172,12 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
+      <c r="L55" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>1180</v>
+      </c>
       <c r="N55" s="3">
         <v>6</v>
       </c>
@@ -6027,6 +6233,12 @@
       </c>
       <c r="K56" s="3" t="s">
         <v>998</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>1181</v>
       </c>
       <c r="N56" s="3">
         <v>2</v>
@@ -6081,8 +6293,12 @@
       <c r="K57" s="4" t="s">
         <v>999</v>
       </c>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
+      <c r="L57" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>1182</v>
+      </c>
       <c r="N57" s="4">
         <v>2</v>
       </c>
@@ -6126,10 +6342,18 @@
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
+      <c r="J58" s="3">
+        <v>0.107715799591002</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>1188</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>1183</v>
+      </c>
       <c r="N58" s="3">
         <v>2</v>
       </c>
@@ -6220,6 +6444,12 @@
       <c r="K61" s="3" t="s">
         <v>984</v>
       </c>
+      <c r="L61" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>1184</v>
+      </c>
       <c r="N61" s="3">
         <v>2</v>
       </c>
@@ -6297,8 +6527,12 @@
       <c r="K63" s="3" t="s">
         <v>1000</v>
       </c>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
+      <c r="L63" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M63" s="3" t="s">
+        <v>1185</v>
+      </c>
       <c r="N63" s="3">
         <v>2</v>
       </c>
@@ -6444,6 +6678,12 @@
       </c>
       <c r="H68" s="7" t="s">
         <v>911</v>
+      </c>
+      <c r="J68" s="3">
+        <v>0.78936605316973396</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>1189</v>
       </c>
       <c r="N68" s="3">
         <v>2</v>
@@ -6661,8 +6901,12 @@
       <c r="K76" s="3" t="s">
         <v>997</v>
       </c>
-      <c r="L76" s="3"/>
-      <c r="M76" s="3"/>
+      <c r="L76" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M76" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N76" s="3">
         <v>2</v>
       </c>
@@ -6739,8 +6983,12 @@
         <v>879</v>
       </c>
       <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
+      <c r="J78" s="3">
+        <v>0.43456032719836402</v>
+      </c>
+      <c r="K78" s="5" t="s">
+        <v>1190</v>
+      </c>
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
       <c r="N78" s="3">
@@ -6866,6 +7114,12 @@
       <c r="K82" s="3" t="s">
         <v>1002</v>
       </c>
+      <c r="L82" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M82" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N82" s="3">
         <v>4</v>
       </c>
@@ -6915,6 +7169,12 @@
       </c>
       <c r="K83" s="4" t="s">
         <v>1003</v>
+      </c>
+      <c r="L83" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="M83" s="4" t="s">
+        <v>1165</v>
       </c>
       <c r="N83" s="4">
         <v>2</v>
@@ -7870,6 +8130,12 @@
         <v>802</v>
       </c>
       <c r="H115" s="7"/>
+      <c r="J115" s="3">
+        <v>0.754601226993865</v>
+      </c>
+      <c r="K115" s="5" t="s">
+        <v>1191</v>
+      </c>
       <c r="N115" s="3">
         <v>2</v>
       </c>
@@ -7949,6 +8215,12 @@
       <c r="K117" s="3" t="s">
         <v>1010</v>
       </c>
+      <c r="L117" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M117" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N117" s="3">
         <v>2</v>
       </c>
@@ -7993,6 +8265,12 @@
       </c>
       <c r="K118" s="4" t="s">
         <v>997</v>
+      </c>
+      <c r="L118" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M118" s="4" t="s">
+        <v>1165</v>
       </c>
       <c r="N118" s="4">
         <v>4</v>
@@ -8293,6 +8571,12 @@
       <c r="K130" s="3" t="s">
         <v>1012</v>
       </c>
+      <c r="L130" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M130" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N130" s="3">
         <v>2</v>
       </c>
@@ -8436,8 +8720,12 @@
       <c r="K134" s="8" t="s">
         <v>1013</v>
       </c>
-      <c r="L134" s="8"/>
-      <c r="M134" s="8"/>
+      <c r="L134" s="8" t="s">
+        <v>845</v>
+      </c>
+      <c r="M134" s="8" t="s">
+        <v>1165</v>
+      </c>
       <c r="N134" s="8">
         <v>2</v>
       </c>
@@ -8762,8 +9050,12 @@
       <c r="K145" s="3" t="s">
         <v>1014</v>
       </c>
-      <c r="L145" s="3"/>
-      <c r="M145" s="3"/>
+      <c r="L145" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M145" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N145" s="3">
         <v>4</v>
       </c>
@@ -8990,8 +9282,12 @@
       <c r="K155" s="3" t="s">
         <v>1015</v>
       </c>
-      <c r="L155" s="3"/>
-      <c r="M155" s="3"/>
+      <c r="L155" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M155" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N155" s="3">
         <v>2</v>
       </c>
@@ -9116,6 +9412,12 @@
       </c>
       <c r="K159" s="4" t="s">
         <v>1016</v>
+      </c>
+      <c r="L159" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M159" s="4" t="s">
+        <v>1165</v>
       </c>
       <c r="N159" s="4">
         <v>2</v>
@@ -10045,8 +10347,12 @@
       <c r="K186" s="3" t="s">
         <v>1020</v>
       </c>
-      <c r="L186" s="3"/>
-      <c r="M186" s="3"/>
+      <c r="L186" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M186" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N186" s="3">
         <v>2</v>
       </c>
@@ -10477,8 +10783,12 @@
       <c r="K200" s="3" t="s">
         <v>1023</v>
       </c>
-      <c r="L200" s="3"/>
-      <c r="M200" s="3"/>
+      <c r="L200" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M200" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N200" s="3" t="s">
         <v>1116</v>
       </c>
@@ -10813,8 +11123,12 @@
       <c r="K211" s="3" t="s">
         <v>1025</v>
       </c>
-      <c r="L211" s="3"/>
-      <c r="M211" s="3"/>
+      <c r="L211" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M211" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N211" s="3">
         <v>2</v>
       </c>
@@ -11722,6 +12036,12 @@
       <c r="K239" s="3" t="s">
         <v>1032</v>
       </c>
+      <c r="L239" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M239" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N239" s="3">
         <v>2</v>
       </c>
@@ -11886,6 +12206,12 @@
       </c>
       <c r="K246" s="4" t="s">
         <v>997</v>
+      </c>
+      <c r="L246" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M246" s="4" t="s">
+        <v>1165</v>
       </c>
       <c r="N246" s="4">
         <v>2</v>
@@ -12804,6 +13130,12 @@
       </c>
       <c r="K279" s="4" t="s">
         <v>997</v>
+      </c>
+      <c r="L279" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="M279" s="4" t="s">
+        <v>1165</v>
       </c>
       <c r="N279" s="4">
         <v>2</v>
@@ -13431,6 +13763,12 @@
       <c r="K300" s="3" t="s">
         <v>1044</v>
       </c>
+      <c r="L300" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M300" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N300" s="3">
         <v>2</v>
       </c>
@@ -14001,8 +14339,12 @@
       <c r="K318" s="3" t="s">
         <v>997</v>
       </c>
-      <c r="L318" s="3"/>
-      <c r="M318" s="3"/>
+      <c r="L318" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M318" s="3" t="s">
+        <v>1165</v>
+      </c>
       <c r="N318" s="3">
         <v>6</v>
       </c>
@@ -14047,6 +14389,12 @@
       </c>
       <c r="K319" s="4" t="s">
         <v>1048</v>
+      </c>
+      <c r="L319" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M319" s="4" t="s">
+        <v>1165</v>
       </c>
       <c r="N319" s="4">
         <v>4</v>
@@ -14126,6 +14474,12 @@
       <c r="K321" s="4" t="s">
         <v>997</v>
       </c>
+      <c r="L321" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M321" s="4" t="s">
+        <v>1165</v>
+      </c>
       <c r="N321" s="4">
         <v>4</v>
       </c>
@@ -14426,8 +14780,12 @@
       <c r="K331" s="3" t="s">
         <v>1050</v>
       </c>
-      <c r="L331" s="3"/>
-      <c r="M331" s="3"/>
+      <c r="L331" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M331" s="5" t="s">
+        <v>1165</v>
+      </c>
       <c r="N331" s="3">
         <v>2</v>
       </c>
@@ -14509,6 +14867,12 @@
       </c>
       <c r="K335" s="3" t="s">
         <v>1051</v>
+      </c>
+      <c r="L335" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M335" s="3" t="s">
+        <v>1165</v>
       </c>
       <c r="N335" s="3">
         <v>2</v>
@@ -14624,6 +14988,12 @@
       </c>
       <c r="K339" s="4" t="s">
         <v>982</v>
+      </c>
+      <c r="L339" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="M339" s="4" t="s">
+        <v>1165</v>
       </c>
       <c r="N339" s="4">
         <v>2</v>
@@ -14952,9 +15322,20 @@
     <hyperlink ref="H92" r:id="rId7" xr:uid="{BA568409-981D-4049-9F64-BEB3B33169A6}"/>
     <hyperlink ref="H258" r:id="rId8" xr:uid="{9B248C90-96EE-4A81-A486-9C3F17AAAE42}"/>
     <hyperlink ref="H282" r:id="rId9" xr:uid="{70EA6D1D-5EF1-4BE0-BD29-78343D9AEAC7}"/>
+    <hyperlink ref="M3" r:id="rId10" xr:uid="{5922DE98-9199-4F4A-AE54-DBFA02169742}"/>
+    <hyperlink ref="M331" r:id="rId11" xr:uid="{5850B9E5-F8B1-4756-B6F6-C084E9A7ACB8}"/>
+    <hyperlink ref="M9" r:id="rId12" xr:uid="{C5CC1314-B295-41EB-8A30-DDE9B3698747}"/>
+    <hyperlink ref="M32" r:id="rId13" xr:uid="{789516B5-237E-4C88-ABEB-724A930FB826}"/>
+    <hyperlink ref="M46" r:id="rId14" xr:uid="{7A21E2CC-EA4F-4E48-825B-3AACEF9D94D5}"/>
+    <hyperlink ref="M53" r:id="rId15" xr:uid="{92037D06-531A-438F-BE22-DFFF28B1D6F4}"/>
+    <hyperlink ref="M56" r:id="rId16" display="https://doi.org/10.1371%2Fjournal.pone.0151424 - self-incompatible" xr:uid="{245CC1E6-BA31-4ED1-9380-877C58209AB7}"/>
+    <hyperlink ref="K58" r:id="rId17" xr:uid="{F2CB1712-C854-4F55-ADB5-742A740609A4}"/>
+    <hyperlink ref="K68" r:id="rId18" xr:uid="{9D2B65D5-B7E7-45EE-A766-9FD36328209A}"/>
+    <hyperlink ref="K78" r:id="rId19" xr:uid="{8F2F035D-A9A8-49CF-98F5-CBE57A513C42}"/>
+    <hyperlink ref="K115" r:id="rId20" xr:uid="{0027F09F-AF65-4BCE-8D72-5DD05532E32B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add genome size, mating system info
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/132102_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\723004_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="13_ncr:1_{BD57AC0C-C9C2-49CC-9A9B-865AD4069F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9584345-A0A4-48E7-86D0-C6014439D9DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B08120-9678-47FB-BE2A-BFE9D62118B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3483" uniqueCount="1192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3528" uniqueCount="1219">
   <si>
     <t>Species</t>
   </si>
@@ -3617,6 +3617,87 @@
   </si>
   <si>
     <t>https://doi.org/10.1038/ng.3972 - estimated from k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1534/g3.120.401326 - esetimate comes from k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/ng.654  - estimated from predicted coverage genome size = number of sequenced bp / coverage</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1534/g3.116.030411 - estimated from k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.15399 - based on k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/1755-0998.13362 - based on k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1534/g3.119.400529 - estimated from k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/nph.18305 - estimated from k-mers</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/1755-0998.13334 - might be estimated from assembly size</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/gigascience/giz071 - average of flow cytometry and k-mer estimates</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.15419 - average of flow cytometry estimates across 4 genotypes</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/f10050460 - average estimate across lots of cultivars, there seems to be a lot of genome size variation in this species</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s40415-016-0321-8 ; https://doi.org/10.21273/JASHS04634-18</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.indcrop.2005.04.002 ; https://doi.org/10.1016/S0378-4290(00)00117-9 ; https://doi.org/10.2478/s11756-007-0001-z</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.17660/ActaHortic.2000.510.7</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpls.2022.800768 ; https://doi.org/10.1007/s00606-003-0073-3</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/aob/mcp196 ; https://doi.org/10.1007/s10722-016-0422-z - not sure if I should label this as outcrossing or mixed</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.21273/HORTSCI.20.2.211 - &lt;10 % outcrossing = selfing, 10 - 90 % = mixed, &gt;90% = outcrossing</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3732/ajb.89.7.1156</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3732/ajb.92.1.107</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10722-017-0515-3</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371%2Fjournal.pone.0174150 - species is dioecious</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s12870-022-03673-y - species is dioecious</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/ng.3972 ; doi:10.1017/S0266467408005531</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10709-010-9442-3</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/ng.2987 - plant went through 18 generations of self-fertilization</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s00122-005-2063-z - species is at least self-compatible</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/nph.14722 ; https://doi.org/10.1093/sysbio/syp030 - there seems to be some migration at least</t>
   </si>
 </sst>
 </file>
@@ -4020,9 +4101,9 @@
   <dimension ref="A1:W356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A182" sqref="A182"/>
+      <selection pane="bottomLeft" activeCell="A165" sqref="A165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6685,6 +6766,12 @@
       <c r="K68" s="5" t="s">
         <v>1189</v>
       </c>
+      <c r="L68" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M68" s="5" t="s">
+        <v>1203</v>
+      </c>
       <c r="N68" s="3">
         <v>2</v>
       </c>
@@ -6814,6 +6901,12 @@
       </c>
       <c r="K73" s="3" t="s">
         <v>1001</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M73" s="3" t="s">
+        <v>1204</v>
       </c>
       <c r="N73" s="3">
         <v>4</v>
@@ -6989,8 +7082,12 @@
       <c r="K78" s="5" t="s">
         <v>1190</v>
       </c>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
+      <c r="L78" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M78" s="3" t="s">
+        <v>1205</v>
+      </c>
       <c r="N78" s="3">
         <v>2</v>
       </c>
@@ -7299,6 +7396,12 @@
       <c r="K88" s="3" t="s">
         <v>1004</v>
       </c>
+      <c r="L88" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M88" s="3" t="s">
+        <v>1206</v>
+      </c>
       <c r="N88" s="3">
         <v>2</v>
       </c>
@@ -7422,8 +7525,12 @@
       <c r="K92" s="3" t="s">
         <v>996</v>
       </c>
-      <c r="L92" s="3"/>
-      <c r="M92" s="3"/>
+      <c r="L92" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>1207</v>
+      </c>
       <c r="N92" s="3">
         <v>2</v>
       </c>
@@ -7470,6 +7577,12 @@
       <c r="K93" s="3" t="s">
         <v>1005</v>
       </c>
+      <c r="L93" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="M93" s="5" t="s">
+        <v>1208</v>
+      </c>
       <c r="N93" s="3">
         <v>2</v>
       </c>
@@ -7551,8 +7664,12 @@
       <c r="K96" s="3" t="s">
         <v>1006</v>
       </c>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
+      <c r="L96" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M96" s="3" t="s">
+        <v>1209</v>
+      </c>
       <c r="N96" s="3">
         <v>2</v>
       </c>
@@ -7651,8 +7768,12 @@
       <c r="K99" s="3" t="s">
         <v>983</v>
       </c>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
+      <c r="L99" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M99" s="3" t="s">
+        <v>1210</v>
+      </c>
       <c r="N99" s="3">
         <v>2</v>
       </c>
@@ -7907,8 +8028,12 @@
       <c r="K109" s="3" t="s">
         <v>1007</v>
       </c>
-      <c r="L109" s="3"/>
-      <c r="M109" s="3"/>
+      <c r="L109" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M109" s="3" t="s">
+        <v>1211</v>
+      </c>
       <c r="N109" s="3">
         <v>4</v>
       </c>
@@ -7962,8 +8087,12 @@
       <c r="K110" s="3" t="s">
         <v>1008</v>
       </c>
-      <c r="L110" s="3"/>
-      <c r="M110" s="3"/>
+      <c r="L110" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M110" s="5" t="s">
+        <v>1212</v>
+      </c>
       <c r="N110" s="3" t="s">
         <v>1085</v>
       </c>
@@ -8046,6 +8175,12 @@
       <c r="K112" s="3" t="s">
         <v>1009</v>
       </c>
+      <c r="L112" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M112" s="5" t="s">
+        <v>1213</v>
+      </c>
       <c r="N112" s="3">
         <v>2</v>
       </c>
@@ -8136,6 +8271,12 @@
       <c r="K115" s="5" t="s">
         <v>1191</v>
       </c>
+      <c r="L115" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M115" s="5" t="s">
+        <v>1214</v>
+      </c>
       <c r="N115" s="3">
         <v>2</v>
       </c>
@@ -8416,8 +8557,12 @@
       <c r="K125" s="4" t="s">
         <v>1011</v>
       </c>
-      <c r="L125" s="4"/>
-      <c r="M125" s="4"/>
+      <c r="L125" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="M125" s="4" t="s">
+        <v>1215</v>
+      </c>
       <c r="N125" s="4">
         <v>2</v>
       </c>
@@ -8808,8 +8953,12 @@
       <c r="K136" s="3" t="s">
         <v>1014</v>
       </c>
-      <c r="L136" s="3"/>
-      <c r="M136" s="3"/>
+      <c r="L136" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M136" s="5" t="s">
+        <v>1216</v>
+      </c>
       <c r="N136" s="3">
         <v>2</v>
       </c>
@@ -8923,6 +9072,12 @@
       </c>
       <c r="K139" s="3" t="s">
         <v>989</v>
+      </c>
+      <c r="L139" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M139" s="5" t="s">
+        <v>1217</v>
       </c>
       <c r="N139" s="3">
         <v>4</v>
@@ -9337,8 +9492,12 @@
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
-      <c r="L156" s="3"/>
-      <c r="M156" s="3"/>
+      <c r="L156" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="M156" s="5" t="s">
+        <v>1218</v>
+      </c>
       <c r="N156" s="3">
         <v>2</v>
       </c>
@@ -10135,6 +10294,12 @@
       <c r="H182" s="7" t="s">
         <v>932</v>
       </c>
+      <c r="J182" s="3">
+        <v>0.915848670756646</v>
+      </c>
+      <c r="K182" s="5" t="s">
+        <v>1192</v>
+      </c>
       <c r="N182" s="3">
         <v>2</v>
       </c>
@@ -10180,8 +10345,12 @@
         <v>817</v>
       </c>
       <c r="I183" s="3"/>
-      <c r="J183" s="3"/>
-      <c r="K183" s="3"/>
+      <c r="J183" s="3">
+        <v>0.75899795501022405</v>
+      </c>
+      <c r="K183" s="5" t="s">
+        <v>1193</v>
+      </c>
       <c r="L183" s="3"/>
       <c r="M183" s="3"/>
       <c r="N183" s="3">
@@ -11714,6 +11883,12 @@
         <v>133</v>
       </c>
       <c r="H227" s="13"/>
+      <c r="J227" s="4">
+        <v>0.54794381288343497</v>
+      </c>
+      <c r="K227" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="L227" s="4" t="s">
         <v>845</v>
       </c>
@@ -12677,8 +12852,12 @@
         <v>894</v>
       </c>
       <c r="I263" s="3"/>
-      <c r="J263" s="3"/>
-      <c r="K263" s="3"/>
+      <c r="J263" s="3">
+        <v>0.74130879345603196</v>
+      </c>
+      <c r="K263" s="5" t="s">
+        <v>1194</v>
+      </c>
       <c r="L263" s="3"/>
       <c r="M263" s="3"/>
       <c r="N263" s="3">
@@ -12888,8 +13067,12 @@
         <v>868</v>
       </c>
       <c r="I268" s="3"/>
-      <c r="J268" s="3"/>
-      <c r="K268" s="3"/>
+      <c r="J268" s="3">
+        <v>0.76687116564417102</v>
+      </c>
+      <c r="K268" s="5" t="s">
+        <v>1195</v>
+      </c>
       <c r="L268" s="3"/>
       <c r="M268" s="3"/>
       <c r="N268" s="3">
@@ -13000,8 +13183,12 @@
         <v>867</v>
       </c>
       <c r="I273" s="3"/>
-      <c r="J273" s="3"/>
-      <c r="K273" s="3"/>
+      <c r="J273" s="3">
+        <v>0.38445807770961099</v>
+      </c>
+      <c r="K273" s="5" t="s">
+        <v>1196</v>
+      </c>
       <c r="L273" s="3"/>
       <c r="M273" s="3"/>
       <c r="N273" s="3">
@@ -13374,6 +13561,12 @@
         <v>690</v>
       </c>
       <c r="H288" s="13"/>
+      <c r="J288" s="4">
+        <v>0.97137014314928405</v>
+      </c>
+      <c r="K288" s="14" t="s">
+        <v>1197</v>
+      </c>
       <c r="N288" s="4">
         <v>2</v>
       </c>
@@ -13621,8 +13814,12 @@
       <c r="G297" s="4"/>
       <c r="H297" s="13"/>
       <c r="I297" s="4"/>
-      <c r="J297" s="4"/>
-      <c r="K297" s="4"/>
+      <c r="J297" s="4">
+        <v>0.94376278118609402</v>
+      </c>
+      <c r="K297" s="4" t="s">
+        <v>1143</v>
+      </c>
       <c r="L297" s="4"/>
       <c r="M297" s="4"/>
       <c r="N297" s="4">
@@ -13979,6 +14176,12 @@
         <v>559</v>
       </c>
       <c r="H306" s="7"/>
+      <c r="J306" s="3">
+        <v>1.5081799591002001</v>
+      </c>
+      <c r="K306" s="5" t="s">
+        <v>1198</v>
+      </c>
       <c r="N306" s="3">
         <v>2</v>
       </c>
@@ -14054,6 +14257,12 @@
         <v>563</v>
       </c>
       <c r="H310" s="7"/>
+      <c r="J310" s="3">
+        <v>1.0084867075664601</v>
+      </c>
+      <c r="K310" s="5" t="s">
+        <v>1199</v>
+      </c>
       <c r="N310" s="3">
         <v>2</v>
       </c>
@@ -14933,8 +15142,12 @@
       <c r="G338" s="3"/>
       <c r="H338" s="7"/>
       <c r="I338" s="3"/>
-      <c r="J338" s="3"/>
-      <c r="K338" s="3"/>
+      <c r="J338" s="3">
+        <v>0.44780163599181999</v>
+      </c>
+      <c r="K338" s="5" t="s">
+        <v>1200</v>
+      </c>
       <c r="L338" s="3"/>
       <c r="M338" s="3"/>
       <c r="N338" s="3">
@@ -15097,8 +15310,12 @@
       </c>
       <c r="H344" s="7"/>
       <c r="I344" s="3"/>
-      <c r="J344" s="3"/>
-      <c r="K344" s="3"/>
+      <c r="J344" s="3">
+        <v>3.7749999999999999</v>
+      </c>
+      <c r="K344" s="5" t="s">
+        <v>1201</v>
+      </c>
       <c r="L344" s="3"/>
       <c r="M344" s="3"/>
       <c r="N344" s="3">
@@ -15146,8 +15363,12 @@
         <v>969</v>
       </c>
       <c r="I345" s="3"/>
-      <c r="J345" s="3"/>
-      <c r="K345" s="3"/>
+      <c r="J345" s="3">
+        <v>0.41773006134969298</v>
+      </c>
+      <c r="K345" s="5" t="s">
+        <v>1202</v>
+      </c>
       <c r="L345" s="3"/>
       <c r="M345" s="3"/>
       <c r="N345" s="3">
@@ -15333,9 +15554,28 @@
     <hyperlink ref="K68" r:id="rId18" xr:uid="{9D2B65D5-B7E7-45EE-A766-9FD36328209A}"/>
     <hyperlink ref="K78" r:id="rId19" xr:uid="{8F2F035D-A9A8-49CF-98F5-CBE57A513C42}"/>
     <hyperlink ref="K115" r:id="rId20" xr:uid="{0027F09F-AF65-4BCE-8D72-5DD05532E32B}"/>
+    <hyperlink ref="K182" r:id="rId21" xr:uid="{0FD52A34-0183-43CB-B12D-4BB58757036A}"/>
+    <hyperlink ref="K183" r:id="rId22" xr:uid="{ED61D3CE-A75D-4C39-B926-C7CEB8F5BF5A}"/>
+    <hyperlink ref="K263" r:id="rId23" xr:uid="{778C86D6-2C47-447A-878E-C7B0E2DAD726}"/>
+    <hyperlink ref="K268" r:id="rId24" xr:uid="{656F2AB6-9D9A-47F1-B5C2-14C6D4710724}"/>
+    <hyperlink ref="K273" r:id="rId25" xr:uid="{8DE370CC-077C-462F-B545-7CA8FC1ED96B}"/>
+    <hyperlink ref="K288" r:id="rId26" xr:uid="{383C9B8E-5355-4843-A1C8-0379DE47222A}"/>
+    <hyperlink ref="K306" r:id="rId27" xr:uid="{3CFA87C4-1C32-488A-9E2A-E6231146BC48}"/>
+    <hyperlink ref="K310" r:id="rId28" xr:uid="{9B80660E-7A51-4225-A0CB-A0E071987486}"/>
+    <hyperlink ref="K338" r:id="rId29" xr:uid="{F406D56D-637D-4C66-B430-1D883D151963}"/>
+    <hyperlink ref="K344" r:id="rId30" xr:uid="{3E912F3F-757A-4AD5-A327-C0E4D1A5A477}"/>
+    <hyperlink ref="K345" r:id="rId31" xr:uid="{7CCFE681-F814-4769-9E69-5519721432AC}"/>
+    <hyperlink ref="M68" r:id="rId32" display="https://doi.org/10.1007/s40415-016-0321-8 ;" xr:uid="{4332AC83-6431-42A1-93E8-CB004F527721}"/>
+    <hyperlink ref="M93" r:id="rId33" xr:uid="{00862E4F-DB42-4064-AF68-1C913BF66151}"/>
+    <hyperlink ref="M110" r:id="rId34" xr:uid="{497503E3-20B0-46F1-90E6-5F89CD6476AD}"/>
+    <hyperlink ref="M112" r:id="rId35" xr:uid="{051E3D06-D1AB-4CCE-B0D9-4254A947E292}"/>
+    <hyperlink ref="M115" r:id="rId36" xr:uid="{2E89C4D3-C8E6-4981-AC0C-905F3DB8E690}"/>
+    <hyperlink ref="M136" r:id="rId37" xr:uid="{998087A9-41C4-44BF-B21F-F44247ACBB2E}"/>
+    <hyperlink ref="M139" r:id="rId38" xr:uid="{218652C7-1F49-4CEE-B7B0-8CDCD3321A75}"/>
+    <hyperlink ref="M156" r:id="rId39" display="https://doi.org/10.1111/nph.14722 - there seems to be some migration at least" xr:uid="{B5CBFBDE-9DC5-4A51-9328-E2D4110493FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add rest of mating system labels
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\723004_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67250_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B08120-9678-47FB-BE2A-BFE9D62118B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A350FC0-AB16-4441-8F21-85C5463AF8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3528" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="1261">
   <si>
     <t>Species</t>
   </si>
@@ -2587,15 +2587,9 @@
     <t>https://doi.org/10.1534/genetics.107.072371; https://doi.org/10.1038/ng.2567</t>
   </si>
   <si>
-    <t>mixed (48 - 70 % selfing)</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1266/jjg.44.207</t>
   </si>
   <si>
-    <t xml:space="preserve">mixed (25-69 % selfing) </t>
-  </si>
-  <si>
     <t>Name has changed from Oryza perennis subsp. barthii to Oryza barthii</t>
   </si>
   <si>
@@ -3698,6 +3692,138 @@
   </si>
   <si>
     <t>https://doi.org/10.1111/nph.14722 ; https://doi.org/10.1093/sysbio/syp030 - there seems to be some migration at least</t>
+  </si>
+  <si>
+    <t>B. Fornari, F. Cannata, M. Spada &amp; M. E. Malvolti. 1999. Allozyme analysis of genetic diversity and differentiation in European and Asiatic walnut (Juglans regia L.) populations ; https://doi.org/10.1007/s11676-020-01254-z</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111%2Feva.12043</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41598-017-03463-9</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1023/A:1008640201896 ; https://doi.org/10.1016/j.bse.2014.12.002</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038%2Fhdy.2010.81</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2135/cropsci1971.0011183X001100060025x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11295-019-1336-7 ; https://doi.org/10.3390/plants9020228</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371%2Fjournal.pgen.1002703 ; https://doi.org/10.1007/s11032-004-5592-2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371%2Fjournal.pone.0096596</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0304-4238(97)00038-1 ; https://doi.org/10.1016/j.scienta.2016.10.034</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/1755-0998.13094 ; https://doi.org/10.2307/2445917</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3732/ajb.90.4.561 ; https://doi.org/10.1093/jxb/eru511</t>
+  </si>
+  <si>
+    <t>Bhardwaj, D. R., and Akhilesh K. Singh. "Heterosis and Inbreeding Depression Analysis in Bitter Gourd (Momordica Charantia L.)." The Journal of Plant Science Research, vol. 38, no. 2, 2022, pp. 791-800. ProQuest, https://ezproxy.msu.edu/login?url=https://www.proquest.com/scholarly-journals/heterosis-inbreeding-depression-analysis-bitter/docview/2777434860/se-2, doi:https://doi.org/10.32381/JPSR.2022.38.02.32. - I'm assuming outcrossing based on presence of inbreedign depression in this species</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s00606-008-0096-x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/j.1537-2197.1995.tb11569.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/molbev/msr104</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s12870-021-02903-z</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/BF00229486</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/mec.13126 - plants are dioecious</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.21273/HORTSCI.42.5.1077 - plants are dioecious</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpls.2012.00116</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.21273/HORTSCI.24.2.359</t>
+  </si>
+  <si>
+    <t>Sork, V. L., Davis, F. W., Dyer, R. J., &amp; Smouse, P. E. (2002). Mating patterns in a savanna population of valley oak (Quercus lobata Neé). USDA Forest Service, 427-439. ; https://doi.org/10.1038/s41467-022-29584-y</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1558-5646.1995.tb02243.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/tpj.15399 - described as being cross compatible with other species</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/1755-0998.13362 - described as dioecious</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389%2Ffpls.2016.01169</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/bf00232954</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/ajb2.1621</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/pbr.12600</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/4252492</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/genetics/161.1.333</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11540-006-9002-5</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1159/000093335 - dioecious</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/j.1469-8137.1984.tb03567.x</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186%2F1999-3110-54-50</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s00122-020-03666-1</t>
+  </si>
+  <si>
+    <t>Sasikumar, Bhas. "Vanilla breeding-a review." Agricultural reviews 31.2 (2010). ; https://doi.org/10.1007/s10722-007-9260-3</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpls.2016.00830</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1139/gen-2013-0118</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s00468-019-01879-6 ; https://doi.org/10.1371/journal.pone.0140507</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3732/ajb.92.6.990</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038%2Fs41598-021-89696-1</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s11295-020-01462-y#citeas</t>
   </si>
 </sst>
 </file>
@@ -4101,9 +4227,9 @@
   <dimension ref="A1:W356"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A165" sqref="A165"/>
+      <selection pane="bottomLeft" activeCell="A302" sqref="A302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4138,10 +4264,10 @@
         <v>447</v>
       </c>
       <c r="F1" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="G1" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>809</v>
@@ -4150,7 +4276,7 @@
         <v>811</v>
       </c>
       <c r="J1" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="K1" t="s">
         <v>768</v>
@@ -4162,10 +4288,10 @@
         <v>844</v>
       </c>
       <c r="N1" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="O1" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="P1" s="6" t="s">
         <v>66</v>
@@ -4247,22 +4373,22 @@
         <v>0.8</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="N3" s="3">
         <v>2</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="Q3" s="10">
         <v>5</v>
@@ -4358,19 +4484,19 @@
         <v>4.3967280000000004</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N7" s="4">
         <v>2</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="12">
@@ -4449,19 +4575,19 @@
         <v>0.5</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="N9" s="3">
         <v>2</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="P9" s="7" t="s">
         <v>761</v>
@@ -4576,19 +4702,19 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="N12" s="3">
         <v>2</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="P12" s="7"/>
       <c r="Q12" s="10">
@@ -4646,19 +4772,19 @@
         <v>0.24</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="N14" s="3">
         <v>2</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="P14" s="7"/>
       <c r="Q14" s="10">
@@ -4718,10 +4844,10 @@
         <v>0.25</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3">
@@ -4772,19 +4898,19 @@
         <v>0.35</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="N17" s="3">
         <v>4</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="P17" s="7"/>
       <c r="Q17" s="10">
@@ -4832,19 +4958,19 @@
         <v>0.16</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="N18" s="3">
         <v>2</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="P18" s="7"/>
       <c r="Q18" s="10">
@@ -4921,10 +5047,10 @@
         <v>0.38</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>162</v>
@@ -4933,7 +5059,7 @@
         <v>2</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="P20" s="13"/>
       <c r="Q20" s="12">
@@ -4976,7 +5102,7 @@
         <v>0.28016000000000002</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>845</v>
@@ -4988,7 +5114,7 @@
         <v>2</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="P21" s="7" t="s">
         <v>576</v>
@@ -5028,19 +5154,19 @@
         <v>1.27</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="N22" s="4">
         <v>2</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="P22" s="13" t="s">
         <v>618</v>
@@ -5099,19 +5225,19 @@
         <v>2.87</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="L24" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N24" s="3">
         <v>4</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="P24" s="7" t="s">
         <v>145</v>
@@ -5156,7 +5282,7 @@
         <v>2.8</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -5265,19 +5391,19 @@
         <v>2.8</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="L28" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="N28" s="3">
         <v>2</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="P28" s="7" t="s">
         <v>578</v>
@@ -5376,19 +5502,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M32" s="14" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="N32" s="4">
         <v>2</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="P32" s="13" t="s">
         <v>766</v>
@@ -5436,19 +5562,19 @@
         <v>0.92</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="N33" s="3">
         <v>2</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="P33" s="7" t="s">
         <v>239</v>
@@ -5570,19 +5696,19 @@
         <v>0.24</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="L37" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="N37" s="3">
         <v>2</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="P37" s="7" t="s">
         <v>723</v>
@@ -5660,10 +5786,10 @@
         <v>446</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>128</v>
@@ -5674,19 +5800,19 @@
         <v>0.32</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="L40" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="N40" s="3">
         <v>2</v>
       </c>
       <c r="O40" s="3" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="P40" s="7" t="s">
         <v>281</v>
@@ -5772,19 +5898,19 @@
         <v>0.43</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="L43" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="N43" s="4">
         <v>2</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="P43" s="13" t="s">
         <v>842</v>
@@ -5843,19 +5969,19 @@
         <v>1.5</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="N46" s="3">
         <v>4</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="P46" s="7"/>
       <c r="Q46" s="10">
@@ -5892,19 +6018,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K47" s="3" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="L47" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N47" s="3">
         <v>4</v>
       </c>
       <c r="O47" s="3" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="P47" s="7"/>
       <c r="Q47" s="10">
@@ -5942,19 +6068,19 @@
         <v>0.8</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="N48" s="4">
         <v>2</v>
       </c>
       <c r="O48" s="4" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="P48" s="13" t="s">
         <v>800</v>
@@ -5989,26 +6115,26 @@
         <v>687</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="I49" s="3"/>
       <c r="J49" s="3">
         <v>0.8</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="L49" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="N49" s="3">
         <v>2</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="P49" s="7" t="s">
         <v>159</v>
@@ -6058,29 +6184,29 @@
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3">
         <v>0.8</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="L51" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="N51" s="3">
         <v>2</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="P51" s="7" t="s">
         <v>159</v>
@@ -6149,10 +6275,10 @@
       </c>
       <c r="H53" s="7"/>
       <c r="L53" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="N53" s="3">
         <v>2</v>
@@ -6191,26 +6317,26 @@
         <v>456</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="H54" s="7"/>
       <c r="J54" s="3">
         <v>0.9</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="N54" s="3">
         <v>2</v>
       </c>
       <c r="O54" s="3" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="P54" s="7" t="s">
         <v>584</v>
@@ -6257,13 +6383,13 @@
         <v>845</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="N55" s="3">
         <v>6</v>
       </c>
       <c r="O55" s="3" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="P55" s="7" t="s">
         <v>325</v>
@@ -6304,28 +6430,28 @@
         <v>456</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="J56" s="3">
         <v>3.9</v>
       </c>
       <c r="K56" s="3" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="N56" s="3">
         <v>2</v>
       </c>
       <c r="O56" s="3" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="P56" s="7" t="s">
         <v>623</v>
@@ -6365,26 +6491,26 @@
         <v>326</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4">
         <v>0.84</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="N57" s="4">
         <v>2</v>
       </c>
       <c r="O57" s="4" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="P57" s="13" t="s">
         <v>329</v>
@@ -6427,19 +6553,19 @@
         <v>0.107715799591002</v>
       </c>
       <c r="K58" s="5" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="N58" s="3">
         <v>2</v>
       </c>
       <c r="O58" s="3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="P58" s="7" t="s">
         <v>159</v>
@@ -6523,19 +6649,19 @@
         <v>0.22</v>
       </c>
       <c r="K61" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="L61" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="N61" s="3">
         <v>2</v>
       </c>
       <c r="O61" s="3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="P61" s="7" t="s">
         <v>724</v>
@@ -6596,29 +6722,29 @@
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" s="3">
         <v>3.16</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="N63" s="3">
         <v>2</v>
       </c>
       <c r="O63" s="3" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="P63" s="7" t="s">
         <v>737</v>
@@ -6758,25 +6884,25 @@
         <v>473</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="J68" s="3">
         <v>0.78936605316973396</v>
       </c>
       <c r="K68" s="5" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M68" s="5" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="N68" s="3">
         <v>2</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="P68" s="7" t="s">
         <v>584</v>
@@ -6891,28 +7017,28 @@
         <v>446</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="J73" s="3">
         <v>1.48</v>
       </c>
       <c r="K73" s="3" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="L73" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="N73" s="3">
         <v>4</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="P73" s="7" t="s">
         <v>259</v>
@@ -6992,19 +7118,19 @@
         <v>1</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="L76" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N76" s="3">
         <v>2</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="P76" s="7" t="s">
         <v>260</v>
@@ -7070,29 +7196,29 @@
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="I78" s="3"/>
       <c r="J78" s="3">
         <v>0.43456032719836402</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="L78" s="3" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="N78" s="3">
         <v>2</v>
       </c>
       <c r="O78" s="3" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="P78" s="7" t="s">
         <v>300</v>
@@ -7209,19 +7335,19 @@
         <v>1.2</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N82" s="3">
         <v>4</v>
       </c>
       <c r="O82" s="3" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="P82" s="7" t="s">
         <v>584</v>
@@ -7256,28 +7382,28 @@
         <v>318</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="J83" s="4">
         <v>0.72</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="L83" s="4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M83" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N83" s="4">
         <v>2</v>
       </c>
       <c r="O83" s="4" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="P83" s="13" t="s">
         <v>342</v>
@@ -7385,28 +7511,28 @@
         <v>738</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="J88" s="3">
         <v>0.43</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="N88" s="3">
         <v>2</v>
       </c>
       <c r="O88" s="3" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="P88" s="7" t="s">
         <v>345</v>
@@ -7513,29 +7639,29 @@
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="H92" s="21" t="s">
         <v>914</v>
-      </c>
-      <c r="H92" s="21" t="s">
-        <v>916</v>
       </c>
       <c r="I92" s="3"/>
       <c r="J92" s="3">
         <v>1</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="L92" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="N92" s="3">
         <v>2</v>
       </c>
       <c r="O92" s="3" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="P92" s="7"/>
       <c r="Q92" s="10">
@@ -7566,28 +7692,28 @@
         <v>446</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="J93" s="3">
         <v>0.9</v>
       </c>
       <c r="K93" s="3" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="L93" s="3" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="M93" s="5" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="N93" s="3">
         <v>2</v>
       </c>
       <c r="O93" s="3" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="P93" s="7" t="s">
         <v>758</v>
@@ -7652,7 +7778,7 @@
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="H96" s="7" t="s">
         <v>746</v>
@@ -7662,13 +7788,13 @@
         <v>0.37</v>
       </c>
       <c r="K96" s="3" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="L96" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="N96" s="3">
         <v>2</v>
@@ -7766,13 +7892,13 @@
         <v>0.54</v>
       </c>
       <c r="K99" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="N99" s="3">
         <v>2</v>
@@ -8016,29 +8142,29 @@
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="I109" s="3"/>
       <c r="J109" s="3">
         <v>0.98</v>
       </c>
       <c r="K109" s="3" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="L109" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="N109" s="3">
         <v>4</v>
       </c>
       <c r="O109" s="3" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="P109" s="7"/>
       <c r="Q109" s="10">
@@ -8075,29 +8201,29 @@
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="3" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="I110" s="3"/>
       <c r="J110" s="3">
         <v>0.82</v>
       </c>
       <c r="K110" s="3" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="L110" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M110" s="5" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="N110" s="3" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="O110" s="3" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="P110" s="7" t="s">
         <v>145</v>
@@ -8173,19 +8299,19 @@
         <v>0.71</v>
       </c>
       <c r="K112" s="3" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="L112" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M112" s="5" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="N112" s="3">
         <v>2</v>
       </c>
       <c r="O112" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="P112" s="7" t="s">
         <v>636</v>
@@ -8269,19 +8395,19 @@
         <v>0.754601226993865</v>
       </c>
       <c r="K115" s="5" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="L115" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M115" s="5" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="N115" s="3">
         <v>2</v>
       </c>
       <c r="O115" s="3" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="P115" s="7" t="s">
         <v>591</v>
@@ -8354,19 +8480,19 @@
         <v>2.16</v>
       </c>
       <c r="K117" s="3" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="L117" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N117" s="3">
         <v>2</v>
       </c>
       <c r="O117" s="3" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="P117" s="7" t="s">
         <v>586</v>
@@ -8405,19 +8531,19 @@
         <v>1.6</v>
       </c>
       <c r="K118" s="4" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="L118" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M118" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N118" s="4">
         <v>4</v>
       </c>
       <c r="O118" s="4" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="P118" s="13" t="s">
         <v>586</v>
@@ -8555,19 +8681,19 @@
         <v>0.37</v>
       </c>
       <c r="K125" s="4" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="L125" s="4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M125" s="4" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="N125" s="4">
         <v>2</v>
       </c>
       <c r="O125" s="4" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="P125" s="13" t="s">
         <v>362</v>
@@ -8714,19 +8840,19 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="K130" s="3" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="L130" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M130" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N130" s="3">
         <v>2</v>
       </c>
       <c r="O130" s="3" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="P130" s="7" t="s">
         <v>290</v>
@@ -8786,10 +8912,10 @@
         <v>446</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="P132" s="7" t="s">
         <v>289</v>
@@ -8863,19 +8989,19 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K134" s="8" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="L134" s="8" t="s">
         <v>845</v>
       </c>
       <c r="M134" s="8" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N134" s="8">
         <v>2</v>
       </c>
       <c r="O134" s="8" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="P134" s="7"/>
       <c r="Q134" s="10">
@@ -8944,26 +9070,26 @@
         <v>497</v>
       </c>
       <c r="H136" s="7" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="I136" s="3"/>
       <c r="J136" s="3">
         <v>1.72</v>
       </c>
       <c r="K136" s="3" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="L136" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M136" s="5" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="N136" s="3">
         <v>2</v>
       </c>
       <c r="O136" s="3" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="P136" s="7" t="s">
         <v>584</v>
@@ -9065,25 +9191,25 @@
         <v>111</v>
       </c>
       <c r="H139" s="7" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="J139" s="3">
         <v>3</v>
       </c>
       <c r="K139" s="3" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="L139" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M139" s="5" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="N139" s="3">
         <v>4</v>
       </c>
       <c r="O139" s="3" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="P139" s="7"/>
       <c r="Q139" s="10">
@@ -9193,29 +9319,29 @@
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
       <c r="G145" s="3" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="H145" s="7" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="I145" s="3"/>
       <c r="J145" s="3">
         <v>2.4</v>
       </c>
       <c r="K145" s="3" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="L145" s="3" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="M145" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N145" s="3">
         <v>4</v>
       </c>
       <c r="O145" s="3" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="P145" s="7"/>
       <c r="Q145" s="10">
@@ -9435,19 +9561,19 @@
         <v>3.67</v>
       </c>
       <c r="K155" s="3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="L155" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M155" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N155" s="3">
         <v>2</v>
       </c>
       <c r="O155" s="3" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="P155" s="7" t="s">
         <v>145</v>
@@ -9493,16 +9619,16 @@
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
       <c r="L156" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M156" s="5" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="N156" s="3">
         <v>2</v>
       </c>
       <c r="O156" s="3" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="P156" s="7" t="s">
         <v>591</v>
@@ -9561,28 +9687,28 @@
         <v>446</v>
       </c>
       <c r="G159" s="4" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="H159" s="13" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="J159" s="4">
         <v>7.33</v>
       </c>
       <c r="K159" s="4" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="L159" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M159" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N159" s="4">
         <v>2</v>
       </c>
       <c r="O159" s="4" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="P159" s="13"/>
       <c r="Q159" s="12">
@@ -9596,7 +9722,7 @@
       </c>
       <c r="U159" s="16"/>
       <c r="W159" s="4" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="160" spans="1:23" x14ac:dyDescent="0.25">
@@ -9686,22 +9812,28 @@
         <v>318</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="H165" s="7" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="J165" s="3">
         <v>0.64</v>
       </c>
       <c r="K165" s="3" t="s">
-        <v>1004</v>
+        <v>1002</v>
+      </c>
+      <c r="L165" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M165" s="3" t="s">
+        <v>1217</v>
       </c>
       <c r="N165" s="3">
         <v>2</v>
       </c>
       <c r="O165" s="3" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="P165" s="7"/>
       <c r="Q165" s="10">
@@ -9770,22 +9902,28 @@
         <v>446</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="H168" s="7" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="J168" s="3">
         <v>3.31</v>
       </c>
       <c r="K168" s="3" t="s">
-        <v>990</v>
+        <v>988</v>
+      </c>
+      <c r="L168" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M168" s="3" t="s">
+        <v>1218</v>
       </c>
       <c r="N168" s="3">
         <v>2</v>
       </c>
       <c r="O168" s="3" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="P168" s="7" t="s">
         <v>263</v>
@@ -9882,29 +10020,29 @@
         <v>446</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="H171" s="13"/>
       <c r="J171" s="4">
         <v>4.21</v>
       </c>
       <c r="K171" s="4" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="L171" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M171" s="4" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="N171" s="4">
         <v>2</v>
       </c>
       <c r="O171" s="4" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="P171" s="13" t="s">
         <v>145</v>
@@ -9920,7 +10058,7 @@
       </c>
       <c r="U171" s="16"/>
       <c r="W171" s="4" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="172" spans="1:23" x14ac:dyDescent="0.25">
@@ -9943,15 +10081,23 @@
       </c>
       <c r="H172" s="7"/>
       <c r="I172" s="3"/>
-      <c r="J172" s="3"/>
-      <c r="K172" s="3"/>
-      <c r="L172" s="3"/>
-      <c r="M172" s="3"/>
+      <c r="J172" s="3">
+        <v>4.0899795501022398</v>
+      </c>
+      <c r="K172" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="L172" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M172" s="3" t="s">
+        <v>1220</v>
+      </c>
       <c r="N172" s="3">
         <v>2</v>
       </c>
       <c r="O172" s="3" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="P172" s="7" t="s">
         <v>145</v>
@@ -9991,25 +10137,31 @@
         <v>448</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="H173" s="7" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="J173" s="3">
         <v>0.7</v>
       </c>
       <c r="K173" s="3" t="s">
-        <v>1017</v>
+        <v>1015</v>
+      </c>
+      <c r="L173" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M173" s="3" t="s">
+        <v>1221</v>
       </c>
       <c r="N173" s="3">
         <v>2</v>
       </c>
       <c r="O173" s="3" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="P173" s="7" t="s">
         <v>304</v>
@@ -10141,34 +10293,34 @@
         <v>446</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="G179" s="3" t="s">
         <v>91</v>
       </c>
       <c r="H179" s="7" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="J179" s="3">
         <v>0.49</v>
       </c>
       <c r="K179" s="3" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="L179" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M179" s="3" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="N179" s="3">
         <v>2</v>
       </c>
       <c r="O179" s="3" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="P179" s="7" t="s">
         <v>264</v>
@@ -10246,15 +10398,19 @@
         <v>0.9</v>
       </c>
       <c r="K181" s="3" t="s">
-        <v>1019</v>
-      </c>
-      <c r="L181" s="3"/>
-      <c r="M181" s="3"/>
+        <v>1017</v>
+      </c>
+      <c r="L181" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M181" s="3" t="s">
+        <v>1222</v>
+      </c>
       <c r="N181" s="3">
         <v>2</v>
       </c>
       <c r="O181" s="3" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="P181" s="7"/>
       <c r="Q181" s="10">
@@ -10289,22 +10445,28 @@
         <v>456</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="H182" s="7" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="J182" s="3">
         <v>0.915848670756646</v>
       </c>
       <c r="K182" s="5" t="s">
-        <v>1192</v>
+        <v>1190</v>
+      </c>
+      <c r="L182" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M182" s="3" t="s">
+        <v>1223</v>
       </c>
       <c r="N182" s="3">
         <v>2</v>
       </c>
       <c r="O182" s="3" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="P182" s="7"/>
       <c r="Q182" s="10">
@@ -10349,15 +10511,19 @@
         <v>0.75899795501022405</v>
       </c>
       <c r="K183" s="5" t="s">
-        <v>1193</v>
-      </c>
-      <c r="L183" s="3"/>
-      <c r="M183" s="3"/>
+        <v>1191</v>
+      </c>
+      <c r="L183" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M183" s="3" t="s">
+        <v>1224</v>
+      </c>
       <c r="N183" s="3">
         <v>2</v>
       </c>
       <c r="O183" s="3" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="P183" s="7" t="s">
         <v>584</v>
@@ -10404,15 +10570,19 @@
         <v>0.78</v>
       </c>
       <c r="K184" s="3" t="s">
-        <v>1004</v>
-      </c>
-      <c r="L184" s="3"/>
-      <c r="M184" s="3"/>
+        <v>1002</v>
+      </c>
+      <c r="L184" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M184" s="3" t="s">
+        <v>1225</v>
+      </c>
       <c r="N184" s="3">
         <v>2</v>
       </c>
       <c r="O184" s="3" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="P184" s="7" t="s">
         <v>644</v>
@@ -10459,15 +10629,19 @@
         <v>0.46</v>
       </c>
       <c r="K185" s="3" t="s">
-        <v>983</v>
-      </c>
-      <c r="L185" s="3"/>
-      <c r="M185" s="3"/>
+        <v>981</v>
+      </c>
+      <c r="L185" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M185" s="3" t="s">
+        <v>1226</v>
+      </c>
       <c r="N185" s="3">
         <v>2</v>
       </c>
       <c r="O185" s="3" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="P185" s="7" t="s">
         <v>584</v>
@@ -10514,19 +10688,19 @@
         <v>0.8</v>
       </c>
       <c r="K186" s="3" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="L186" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M186" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N186" s="3">
         <v>2</v>
       </c>
       <c r="O186" s="3" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="P186" s="7" t="s">
         <v>265</v>
@@ -10659,19 +10833,19 @@
         <v>0.47</v>
       </c>
       <c r="K191" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="L191" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M191" s="3" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="N191" s="3">
         <v>2</v>
       </c>
       <c r="O191" s="3" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="P191" s="7" t="s">
         <v>159</v>
@@ -10772,13 +10946,19 @@
         <v>0.37</v>
       </c>
       <c r="K195" s="3" t="s">
-        <v>1021</v>
+        <v>1019</v>
+      </c>
+      <c r="L195" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M195" s="3" t="s">
+        <v>1227</v>
       </c>
       <c r="N195" s="3">
         <v>2</v>
       </c>
       <c r="O195" s="3" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="P195" s="7" t="s">
         <v>269</v>
@@ -10829,25 +11009,29 @@
       <c r="E197" s="3"/>
       <c r="F197" s="3"/>
       <c r="G197" s="3" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="H197" s="7" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="I197" s="3"/>
       <c r="J197" s="3">
         <v>2.61</v>
       </c>
       <c r="K197" s="3" t="s">
-        <v>1022</v>
-      </c>
-      <c r="L197" s="3"/>
-      <c r="M197" s="3"/>
+        <v>1020</v>
+      </c>
+      <c r="L197" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M197" s="3" t="s">
+        <v>1228</v>
+      </c>
       <c r="N197" s="3">
         <v>2</v>
       </c>
       <c r="O197" s="3" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="P197" s="7" t="s">
         <v>203</v>
@@ -10877,22 +11061,28 @@
         <v>456</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="H198" s="7" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="J198" s="3">
         <v>2.1</v>
       </c>
       <c r="K198" s="3" t="s">
-        <v>996</v>
+        <v>994</v>
+      </c>
+      <c r="L198" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M198" s="3" t="s">
+        <v>1229</v>
       </c>
       <c r="N198" s="3">
         <v>2</v>
       </c>
       <c r="O198" s="3" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="P198" s="7" t="s">
         <v>648</v>
@@ -10950,16 +11140,16 @@
         <v>0.6</v>
       </c>
       <c r="K200" s="3" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="L200" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M200" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N200" s="3" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="O200" s="3" t="s">
         <v>610</v>
@@ -11022,15 +11212,19 @@
         <v>0.24</v>
       </c>
       <c r="K202" s="3" t="s">
-        <v>998</v>
-      </c>
-      <c r="L202" s="3"/>
-      <c r="M202" s="3"/>
+        <v>996</v>
+      </c>
+      <c r="L202" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M202" s="3" t="s">
+        <v>1230</v>
+      </c>
       <c r="N202" s="3">
         <v>2</v>
       </c>
       <c r="O202" s="3" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="P202" s="7" t="s">
         <v>584</v>
@@ -11107,15 +11301,19 @@
         <v>5.18</v>
       </c>
       <c r="K206" s="4" t="s">
-        <v>1024</v>
-      </c>
-      <c r="L206" s="4"/>
-      <c r="M206" s="4"/>
+        <v>1022</v>
+      </c>
+      <c r="L206" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M206" s="4" t="s">
+        <v>1231</v>
+      </c>
       <c r="N206" s="4">
         <v>2</v>
       </c>
       <c r="O206" s="4" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="P206" s="13" t="s">
         <v>701</v>
@@ -11290,13 +11488,13 @@
         <v>1.95</v>
       </c>
       <c r="K211" s="3" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="L211" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M211" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N211" s="3">
         <v>2</v>
@@ -11407,22 +11605,22 @@
         <v>0.6</v>
       </c>
       <c r="K215" s="3" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="L215" s="3" t="s">
-        <v>850</v>
+        <v>1164</v>
       </c>
       <c r="M215" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="N215" s="3">
         <v>2</v>
       </c>
       <c r="O215" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="P215" s="7" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="Q215" s="10">
         <v>86</v>
@@ -11458,19 +11656,19 @@
         <v>0.4</v>
       </c>
       <c r="K216" s="3" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="L216" s="3" t="s">
         <v>136</v>
       </c>
       <c r="M216" s="3" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="N216" s="3">
         <v>2</v>
       </c>
       <c r="O216" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="P216" s="7" t="s">
         <v>381</v>
@@ -11505,13 +11703,13 @@
         <v>383</v>
       </c>
       <c r="H217" s="7" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="J217" s="3">
         <v>0.8</v>
       </c>
       <c r="K217" s="3" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="L217" s="3" t="s">
         <v>845</v>
@@ -11523,7 +11721,7 @@
         <v>2</v>
       </c>
       <c r="O217" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="P217" s="7"/>
       <c r="Q217" s="10">
@@ -11562,10 +11760,10 @@
         <v>388</v>
       </c>
       <c r="C219" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="P219" s="6" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="U219" s="18"/>
     </row>
@@ -11584,22 +11782,22 @@
         <v>0.8</v>
       </c>
       <c r="K220" s="3" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="L220" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="N220" s="3">
         <v>2</v>
       </c>
       <c r="O220" s="3" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="P220" s="7" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="Q220" s="10">
         <v>18</v>
@@ -11661,7 +11859,7 @@
         <v>845</v>
       </c>
       <c r="M222" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="P222" s="6" t="s">
         <v>393</v>
@@ -11685,19 +11883,19 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="K223" s="3" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="L223" s="3" t="s">
-        <v>136</v>
+        <v>850</v>
       </c>
       <c r="M223" s="3" t="s">
-        <v>855</v>
+        <v>1232</v>
       </c>
       <c r="N223" s="3">
         <v>2</v>
       </c>
       <c r="O223" s="3" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="P223" s="7" t="s">
         <v>396</v>
@@ -11745,10 +11943,10 @@
         <v>0.46</v>
       </c>
       <c r="K224" s="3" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="L224" s="3" t="s">
-        <v>848</v>
+        <v>1164</v>
       </c>
       <c r="M224" s="3" t="s">
         <v>847</v>
@@ -11757,7 +11955,7 @@
         <v>2</v>
       </c>
       <c r="O224" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="P224" s="7" t="s">
         <v>400</v>
@@ -11796,17 +11994,17 @@
       <c r="E225" s="3"/>
       <c r="F225" s="3"/>
       <c r="G225" s="3" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="H225" s="7" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="I225" s="3"/>
       <c r="J225" s="3">
         <v>0.5</v>
       </c>
       <c r="K225" s="3" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="L225" s="3" t="s">
         <v>845</v>
@@ -11818,7 +12016,7 @@
         <v>2</v>
       </c>
       <c r="O225" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="P225" s="7" t="s">
         <v>271</v>
@@ -11893,13 +12091,13 @@
         <v>845</v>
       </c>
       <c r="M227" s="4" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="N227" s="4">
         <v>2</v>
       </c>
       <c r="O227" s="4" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="P227" s="13" t="s">
         <v>291</v>
@@ -11939,25 +12137,29 @@
       <c r="E228" s="3"/>
       <c r="F228" s="3"/>
       <c r="G228" s="3" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="H228" s="7" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="I228" s="3"/>
       <c r="J228" s="3">
         <v>1.93</v>
       </c>
       <c r="K228" s="3" t="s">
-        <v>1030</v>
-      </c>
-      <c r="L228" s="3"/>
-      <c r="M228" s="3"/>
+        <v>1028</v>
+      </c>
+      <c r="L228" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M228" s="3" t="s">
+        <v>1233</v>
+      </c>
       <c r="N228" s="3">
         <v>4</v>
       </c>
       <c r="O228" s="3" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="P228" s="7" t="s">
         <v>272</v>
@@ -12061,7 +12263,13 @@
         <v>3.8</v>
       </c>
       <c r="K233" s="4" t="s">
-        <v>1031</v>
+        <v>1029</v>
+      </c>
+      <c r="L233" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M233" s="4" t="s">
+        <v>1234</v>
       </c>
       <c r="N233" s="4">
         <v>2</v>
@@ -12200,28 +12408,28 @@
         <v>446</v>
       </c>
       <c r="G239" s="3" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="H239" s="7" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="J239" s="3">
         <v>0.6</v>
       </c>
       <c r="K239" s="3" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="L239" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M239" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N239" s="3">
         <v>2</v>
       </c>
       <c r="O239" s="3" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="P239" s="7"/>
       <c r="Q239" s="10">
@@ -12250,25 +12458,29 @@
       <c r="E240" s="3"/>
       <c r="F240" s="3"/>
       <c r="G240" s="3" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="H240" s="7" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="I240" s="3"/>
       <c r="J240" s="3">
         <v>1</v>
       </c>
       <c r="K240" s="3" t="s">
-        <v>1033</v>
-      </c>
-      <c r="L240" s="3"/>
-      <c r="M240" s="3"/>
+        <v>1031</v>
+      </c>
+      <c r="L240" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M240" s="5" t="s">
+        <v>1236</v>
+      </c>
       <c r="N240" s="3">
         <v>2</v>
       </c>
       <c r="O240" s="3" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="P240" s="7"/>
       <c r="Q240" s="10">
@@ -12380,13 +12592,13 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="K246" s="4" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="L246" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M246" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N246" s="4">
         <v>2</v>
@@ -12436,10 +12648,10 @@
         <v>456</v>
       </c>
       <c r="E248" s="3" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="F248" s="3" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="G248" s="3" t="s">
         <v>537</v>
@@ -12450,15 +12662,19 @@
         <v>0.49</v>
       </c>
       <c r="K248" s="3" t="s">
-        <v>1034</v>
-      </c>
-      <c r="L248" s="3"/>
-      <c r="M248" s="3"/>
+        <v>1032</v>
+      </c>
+      <c r="L248" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M248" s="3" t="s">
+        <v>1124</v>
+      </c>
       <c r="N248" s="3">
         <v>2</v>
       </c>
       <c r="O248" s="3" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="P248" s="7" t="s">
         <v>584</v>
@@ -12529,15 +12745,19 @@
         <v>0.49</v>
       </c>
       <c r="K251" s="3" t="s">
-        <v>1035</v>
-      </c>
-      <c r="L251" s="3"/>
-      <c r="M251" s="3"/>
+        <v>1033</v>
+      </c>
+      <c r="L251" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M251" s="5" t="s">
+        <v>1235</v>
+      </c>
       <c r="N251" s="3">
         <v>2</v>
       </c>
       <c r="O251" s="3" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="P251" s="7" t="s">
         <v>252</v>
@@ -12645,25 +12865,29 @@
       <c r="E257" s="3"/>
       <c r="F257" s="3"/>
       <c r="G257" s="3" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="H257" s="7" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="I257" s="3"/>
       <c r="J257" s="3">
         <v>0.31</v>
       </c>
       <c r="K257" s="3" t="s">
-        <v>983</v>
-      </c>
-      <c r="L257" s="3"/>
-      <c r="M257" s="3"/>
+        <v>981</v>
+      </c>
+      <c r="L257" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M257" s="3" t="s">
+        <v>656</v>
+      </c>
       <c r="N257" s="3">
         <v>2</v>
       </c>
       <c r="O257" s="3" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="P257" s="7" t="s">
         <v>584</v>
@@ -12705,22 +12929,26 @@
         <v>410</v>
       </c>
       <c r="H258" s="21" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="I258" s="3"/>
       <c r="J258" s="3">
         <v>0.43</v>
       </c>
       <c r="K258" s="3" t="s">
-        <v>1004</v>
-      </c>
-      <c r="L258" s="3"/>
-      <c r="M258" s="3"/>
+        <v>1002</v>
+      </c>
+      <c r="L258" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M258" s="3" t="s">
+        <v>1237</v>
+      </c>
       <c r="N258" s="3">
         <v>2</v>
       </c>
       <c r="O258" s="3" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="P258" s="7" t="s">
         <v>413</v>
@@ -12770,25 +12998,29 @@
       <c r="E260" s="3"/>
       <c r="F260" s="3"/>
       <c r="G260" s="3" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="H260" s="7" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="I260" s="3"/>
       <c r="J260" s="3">
         <v>0.3</v>
       </c>
       <c r="K260" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="L260" s="3"/>
-      <c r="M260" s="3"/>
+        <v>1034</v>
+      </c>
+      <c r="L260" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M260" s="3" t="s">
+        <v>1238</v>
+      </c>
       <c r="N260" s="3">
         <v>2</v>
       </c>
       <c r="O260" s="3" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="P260" s="7" t="s">
         <v>273</v>
@@ -12849,22 +13081,26 @@
         <v>418</v>
       </c>
       <c r="H263" s="7" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="I263" s="3"/>
       <c r="J263" s="3">
         <v>0.74130879345603196</v>
       </c>
       <c r="K263" s="5" t="s">
-        <v>1194</v>
-      </c>
-      <c r="L263" s="3"/>
-      <c r="M263" s="3"/>
+        <v>1192</v>
+      </c>
+      <c r="L263" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M263" s="3" t="s">
+        <v>1239</v>
+      </c>
       <c r="N263" s="3">
         <v>2</v>
       </c>
       <c r="O263" s="3" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="P263" s="7" t="s">
         <v>419</v>
@@ -12901,26 +13137,26 @@
         <v>456</v>
       </c>
       <c r="G264" s="3" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H264" s="7"/>
       <c r="J264" s="3">
         <v>0.9</v>
       </c>
       <c r="K264" s="3" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="L264" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M264" s="3" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="N264" s="3">
         <v>2</v>
       </c>
       <c r="O264" s="3" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="P264" s="7" t="s">
         <v>584</v>
@@ -12977,23 +13213,35 @@
       <c r="D266" s="3" t="s">
         <v>456</v>
       </c>
+      <c r="E266" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F266" s="3" t="s">
+        <v>1240</v>
+      </c>
       <c r="G266" s="3" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="H266" s="7" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="J266" s="3">
         <v>1.05</v>
       </c>
       <c r="K266" s="3" t="s">
-        <v>1038</v>
+        <v>1036</v>
+      </c>
+      <c r="L266" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M266" s="3" t="s">
+        <v>1240</v>
       </c>
       <c r="N266" s="3">
         <v>2</v>
       </c>
       <c r="O266" s="3" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="P266" s="7" t="s">
         <v>718</v>
@@ -13064,17 +13312,21 @@
         <v>546</v>
       </c>
       <c r="H268" s="7" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="I268" s="3"/>
       <c r="J268" s="3">
         <v>0.76687116564417102</v>
       </c>
       <c r="K268" s="5" t="s">
-        <v>1195</v>
-      </c>
-      <c r="L268" s="3"/>
-      <c r="M268" s="3"/>
+        <v>1193</v>
+      </c>
+      <c r="L268" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M268" s="5" t="s">
+        <v>1241</v>
+      </c>
       <c r="N268" s="3">
         <v>2</v>
       </c>
@@ -13082,7 +13334,7 @@
         <v>660</v>
       </c>
       <c r="P268" s="7" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="Q268" s="10">
         <v>32</v>
@@ -13177,25 +13429,29 @@
       <c r="E273" s="3"/>
       <c r="F273" s="3"/>
       <c r="G273" s="3" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="H273" s="7" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="I273" s="3"/>
       <c r="J273" s="3">
         <v>0.38445807770961099</v>
       </c>
       <c r="K273" s="5" t="s">
-        <v>1196</v>
-      </c>
-      <c r="L273" s="3"/>
-      <c r="M273" s="3"/>
+        <v>1194</v>
+      </c>
+      <c r="L273" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M273" s="5" t="s">
+        <v>1242</v>
+      </c>
       <c r="N273" s="3">
         <v>2</v>
       </c>
       <c r="O273" s="3" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="P273" s="7" t="s">
         <v>596</v>
@@ -13307,28 +13563,28 @@
         <v>318</v>
       </c>
       <c r="G279" s="4" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="H279" s="4" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="J279" s="4">
         <v>8.8000000000000007</v>
       </c>
       <c r="K279" s="4" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="L279" s="4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M279" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N279" s="4">
         <v>2</v>
       </c>
       <c r="O279" s="4" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="P279" s="13" t="s">
         <v>323</v>
@@ -13378,25 +13634,29 @@
       <c r="E282" s="3"/>
       <c r="F282" s="3"/>
       <c r="G282" s="3" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="H282" s="21" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="I282" s="3"/>
       <c r="J282" s="3">
         <v>0.97</v>
       </c>
       <c r="K282" s="3" t="s">
-        <v>1039</v>
-      </c>
-      <c r="L282" s="3"/>
-      <c r="M282" s="3"/>
+        <v>1037</v>
+      </c>
+      <c r="L282" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M282" s="3" t="s">
+        <v>1243</v>
+      </c>
       <c r="N282" s="3">
         <v>2</v>
       </c>
       <c r="O282" s="3" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="P282" s="7" t="s">
         <v>429</v>
@@ -13431,7 +13691,7 @@
       <c r="E283" s="3"/>
       <c r="F283" s="3"/>
       <c r="G283" s="3" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="H283" s="7"/>
       <c r="I283" s="3"/>
@@ -13439,15 +13699,19 @@
         <v>0.5</v>
       </c>
       <c r="K283" s="3" t="s">
-        <v>1040</v>
-      </c>
-      <c r="L283" s="3"/>
-      <c r="M283" s="3"/>
+        <v>1038</v>
+      </c>
+      <c r="L283" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M283" s="3" t="s">
+        <v>1244</v>
+      </c>
       <c r="N283" s="3">
         <v>2</v>
       </c>
       <c r="O283" s="3" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="P283" s="7" t="s">
         <v>274</v>
@@ -13487,13 +13751,19 @@
         <v>0.8</v>
       </c>
       <c r="K284" s="3" t="s">
-        <v>1041</v>
+        <v>1039</v>
+      </c>
+      <c r="L284" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M284" s="3" t="s">
+        <v>1244</v>
       </c>
       <c r="N284" s="3">
         <v>2</v>
       </c>
       <c r="O284" s="3" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="P284" s="7" t="s">
         <v>275</v>
@@ -13565,13 +13835,19 @@
         <v>0.97137014314928405</v>
       </c>
       <c r="K288" s="14" t="s">
-        <v>1197</v>
+        <v>1195</v>
+      </c>
+      <c r="L288" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="M288" s="4" t="s">
+        <v>1245</v>
       </c>
       <c r="N288" s="4">
         <v>2</v>
       </c>
       <c r="O288" s="4" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="P288" s="13"/>
       <c r="Q288" s="12">
@@ -13636,13 +13912,19 @@
         <v>1.06</v>
       </c>
       <c r="K291" s="3" t="s">
-        <v>1042</v>
+        <v>1040</v>
+      </c>
+      <c r="L291" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M291" s="3" t="s">
+        <v>1246</v>
       </c>
       <c r="N291" s="3">
         <v>2</v>
       </c>
       <c r="O291" s="3" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="P291" s="7" t="s">
         <v>159</v>
@@ -13755,13 +14037,19 @@
         <v>1</v>
       </c>
       <c r="K295" s="4" t="s">
-        <v>982</v>
+        <v>980</v>
+      </c>
+      <c r="L295" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M295" s="4" t="s">
+        <v>1247</v>
       </c>
       <c r="N295" s="4">
         <v>2</v>
       </c>
       <c r="O295" s="4" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="P295" s="13" t="s">
         <v>692</v>
@@ -13818,15 +14106,19 @@
         <v>0.94376278118609402</v>
       </c>
       <c r="K297" s="4" t="s">
-        <v>1143</v>
-      </c>
-      <c r="L297" s="4"/>
-      <c r="M297" s="4"/>
+        <v>1141</v>
+      </c>
+      <c r="L297" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M297" s="4" t="s">
+        <v>1248</v>
+      </c>
       <c r="N297" s="4">
         <v>2</v>
       </c>
       <c r="O297" s="4" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="P297" s="13" t="s">
         <v>696</v>
@@ -13869,15 +14161,19 @@
         <v>1.2</v>
       </c>
       <c r="K298" s="3" t="s">
-        <v>1043</v>
-      </c>
-      <c r="L298" s="3"/>
-      <c r="M298" s="3"/>
+        <v>1041</v>
+      </c>
+      <c r="L298" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M298" s="3" t="s">
+        <v>1249</v>
+      </c>
       <c r="N298" s="3">
         <v>2</v>
       </c>
       <c r="O298" s="3" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="P298" s="7" t="s">
         <v>596</v>
@@ -13916,13 +14212,17 @@
       <c r="I299" s="4"/>
       <c r="J299" s="4"/>
       <c r="K299" s="4"/>
-      <c r="L299" s="4"/>
-      <c r="M299" s="4"/>
+      <c r="L299" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="M299" s="4" t="s">
+        <v>1249</v>
+      </c>
       <c r="N299" s="4" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="O299" s="4" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="P299" s="13" t="s">
         <v>222</v>
@@ -13949,28 +14249,28 @@
         <v>446</v>
       </c>
       <c r="G300" s="3" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="H300" s="7" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="J300" s="3">
         <v>1.2</v>
       </c>
       <c r="K300" s="3" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="L300" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M300" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N300" s="3">
         <v>2</v>
       </c>
       <c r="O300" s="3" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="P300" s="7" t="s">
         <v>159</v>
@@ -14030,20 +14330,24 @@
       <c r="E303" s="3"/>
       <c r="F303" s="3"/>
       <c r="G303" s="3" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="H303" s="7" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="I303" s="3"/>
       <c r="J303" s="3">
         <v>1</v>
       </c>
       <c r="K303" s="3" t="s">
-        <v>1019</v>
-      </c>
-      <c r="L303" s="3"/>
-      <c r="M303" s="3"/>
+        <v>1017</v>
+      </c>
+      <c r="L303" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M303" s="5" t="s">
+        <v>1250</v>
+      </c>
       <c r="N303" s="3">
         <v>2</v>
       </c>
@@ -14124,13 +14428,13 @@
         <v>0.3</v>
       </c>
       <c r="K305" s="3" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="L305" s="3" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="M305" s="3" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="N305" s="3">
         <v>2</v>
@@ -14180,13 +14484,19 @@
         <v>1.5081799591002001</v>
       </c>
       <c r="K306" s="5" t="s">
-        <v>1198</v>
+        <v>1196</v>
+      </c>
+      <c r="L306" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M306" s="3" t="s">
+        <v>1251</v>
       </c>
       <c r="N306" s="3">
         <v>2</v>
       </c>
       <c r="O306" s="3" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="P306" s="7" t="s">
         <v>595</v>
@@ -14261,7 +14571,13 @@
         <v>1.0084867075664601</v>
       </c>
       <c r="K310" s="5" t="s">
-        <v>1199</v>
+        <v>1197</v>
+      </c>
+      <c r="L310" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M310" s="3" t="s">
+        <v>1252</v>
       </c>
       <c r="N310" s="3">
         <v>2</v>
@@ -14358,22 +14674,28 @@
         <v>446</v>
       </c>
       <c r="G314" s="3" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="H314" s="7" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="J314" s="3">
         <v>13</v>
       </c>
       <c r="K314" s="3" t="s">
-        <v>1046</v>
+        <v>1044</v>
+      </c>
+      <c r="L314" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M314" s="3" t="s">
+        <v>1253</v>
       </c>
       <c r="N314" s="3">
         <v>6</v>
       </c>
       <c r="O314" s="3" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="P314" s="7" t="s">
         <v>142</v>
@@ -14409,7 +14731,7 @@
         <v>0.52</v>
       </c>
       <c r="K315" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="L315" s="3" t="s">
         <v>845</v>
@@ -14450,29 +14772,29 @@
       <c r="E316" s="3"/>
       <c r="F316" s="3"/>
       <c r="G316" s="3" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="H316" s="7" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="I316" s="3"/>
       <c r="J316" s="3">
         <v>0.43</v>
       </c>
       <c r="K316" s="3" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="L316" s="3" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M316" s="3" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="N316" s="3">
         <v>2</v>
       </c>
       <c r="O316" s="3" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="P316" s="7" t="s">
         <v>232</v>
@@ -14546,19 +14868,19 @@
         <v>17.3</v>
       </c>
       <c r="K318" s="3" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="L318" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M318" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N318" s="3">
         <v>6</v>
       </c>
       <c r="O318" s="3" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="P318" s="7" t="s">
         <v>233</v>
@@ -14591,28 +14913,28 @@
         <v>430</v>
       </c>
       <c r="H319" s="13" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="J319" s="4">
         <v>12.3</v>
       </c>
       <c r="K319" s="4" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="L319" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M319" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N319" s="4">
         <v>4</v>
       </c>
       <c r="O319" s="4" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="P319" s="13" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="Q319" s="12">
         <v>109</v>
@@ -14624,7 +14946,7 @@
         <v>257</v>
       </c>
       <c r="W319" s="4" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="320" spans="1:23" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -14672,28 +14994,28 @@
         <v>318</v>
       </c>
       <c r="G321" s="4" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H321" s="13" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="J321" s="4">
         <v>12.3</v>
       </c>
       <c r="K321" s="4" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="L321" s="4" t="s">
         <v>845</v>
       </c>
       <c r="M321" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N321" s="4">
         <v>4</v>
       </c>
       <c r="O321" s="4" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="P321" s="13" t="s">
         <v>301</v>
@@ -14708,7 +15030,7 @@
         <v>257</v>
       </c>
       <c r="W321" s="4" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="322" spans="1:23" x14ac:dyDescent="0.25">
@@ -14766,25 +15088,29 @@
       <c r="E324" s="3"/>
       <c r="F324" s="3"/>
       <c r="G324" s="3" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="H324" s="7" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="I324" s="3"/>
       <c r="J324" s="3">
         <v>3.76</v>
       </c>
       <c r="K324" s="3" t="s">
-        <v>1049</v>
-      </c>
-      <c r="L324" s="3"/>
-      <c r="M324" s="3"/>
+        <v>1047</v>
+      </c>
+      <c r="L324" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M324" s="3" t="s">
+        <v>1254</v>
+      </c>
       <c r="N324" s="3">
         <v>2</v>
       </c>
       <c r="O324" s="3" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="P324" s="7" t="s">
         <v>604</v>
@@ -14837,25 +15163,29 @@
       <c r="E327" s="3"/>
       <c r="F327" s="3"/>
       <c r="G327" s="3" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="H327" s="3" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="I327" s="3"/>
       <c r="J327" s="3">
         <v>0.5</v>
       </c>
       <c r="K327" s="3" t="s">
-        <v>989</v>
-      </c>
-      <c r="L327" s="3"/>
-      <c r="M327" s="3"/>
+        <v>987</v>
+      </c>
+      <c r="L327" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="M327" s="3" t="s">
+        <v>1255</v>
+      </c>
       <c r="N327" s="3">
         <v>2</v>
       </c>
       <c r="O327" s="3" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="P327" s="7"/>
       <c r="Q327" s="10">
@@ -14888,25 +15218,29 @@
       <c r="E328" s="3"/>
       <c r="F328" s="3"/>
       <c r="G328" s="3" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="H328" s="3" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="I328" s="3"/>
       <c r="J328" s="3">
         <v>0.6</v>
       </c>
       <c r="K328" s="3" t="s">
-        <v>1050</v>
-      </c>
-      <c r="L328" s="3"/>
-      <c r="M328" s="3"/>
+        <v>1048</v>
+      </c>
+      <c r="L328" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="M328" s="3" t="s">
+        <v>1256</v>
+      </c>
       <c r="N328" s="3">
         <v>2</v>
       </c>
       <c r="O328" s="3" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="P328" s="7" t="s">
         <v>595</v>
@@ -14977,29 +15311,29 @@
       <c r="E331" s="3"/>
       <c r="F331" s="3"/>
       <c r="G331" s="3" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="H331" s="7" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="I331" s="3"/>
       <c r="J331" s="3">
         <v>0.6</v>
       </c>
       <c r="K331" s="3" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="L331" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M331" s="5" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N331" s="3">
         <v>2</v>
       </c>
       <c r="O331" s="3" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="P331" s="7" t="s">
         <v>445</v>
@@ -15066,28 +15400,28 @@
         <v>446</v>
       </c>
       <c r="G335" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H335" s="7" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="J335" s="3">
         <v>0.4</v>
       </c>
       <c r="K335" s="3" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="L335" s="3" t="s">
         <v>845</v>
       </c>
       <c r="M335" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N335" s="3">
         <v>2</v>
       </c>
       <c r="O335" s="3" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="P335" s="7" t="s">
         <v>277</v>
@@ -15146,15 +15480,19 @@
         <v>0.44780163599181999</v>
       </c>
       <c r="K338" s="5" t="s">
-        <v>1200</v>
-      </c>
-      <c r="L338" s="3"/>
-      <c r="M338" s="3"/>
+        <v>1198</v>
+      </c>
+      <c r="L338" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M338" s="3" t="s">
+        <v>1257</v>
+      </c>
       <c r="N338" s="3">
         <v>2</v>
       </c>
       <c r="O338" s="3" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="P338" s="7" t="s">
         <v>584</v>
@@ -15191,28 +15529,28 @@
         <v>446</v>
       </c>
       <c r="G339" s="13" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="H339" s="13" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="J339" s="4">
         <v>2.7</v>
       </c>
       <c r="K339" s="4" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="L339" s="4" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="M339" s="4" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="N339" s="4">
         <v>2</v>
       </c>
       <c r="O339" s="4" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="P339" s="13" t="s">
         <v>798</v>
@@ -15300,10 +15638,10 @@
         <v>456</v>
       </c>
       <c r="E344" s="3" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="F344" s="3" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="G344" s="3" t="s">
         <v>571</v>
@@ -15314,15 +15652,19 @@
         <v>3.7749999999999999</v>
       </c>
       <c r="K344" s="5" t="s">
-        <v>1201</v>
-      </c>
-      <c r="L344" s="3"/>
-      <c r="M344" s="3"/>
+        <v>1199</v>
+      </c>
+      <c r="L344" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M344" s="3" t="s">
+        <v>1258</v>
+      </c>
       <c r="N344" s="3">
         <v>2</v>
       </c>
       <c r="O344" s="3" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="P344" s="7" t="s">
         <v>604</v>
@@ -15357,25 +15699,29 @@
       <c r="E345" s="3"/>
       <c r="F345" s="3"/>
       <c r="G345" s="3" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="H345" s="7" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="I345" s="3"/>
       <c r="J345" s="3">
         <v>0.41773006134969298</v>
       </c>
       <c r="K345" s="5" t="s">
-        <v>1202</v>
-      </c>
-      <c r="L345" s="3"/>
-      <c r="M345" s="3"/>
+        <v>1200</v>
+      </c>
+      <c r="L345" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M345" s="3" t="s">
+        <v>1259</v>
+      </c>
       <c r="N345" s="3">
         <v>2</v>
       </c>
       <c r="O345" s="3" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="P345" s="7" t="s">
         <v>584</v>
@@ -15432,7 +15778,7 @@
       </c>
       <c r="H347" s="13"/>
       <c r="P347" s="13" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="Q347" s="12"/>
     </row>
@@ -15445,7 +15791,7 @@
       </c>
       <c r="H348" s="13"/>
       <c r="P348" s="13" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="Q348" s="12"/>
     </row>
@@ -15458,19 +15804,19 @@
       </c>
       <c r="H349" s="13"/>
       <c r="P349" s="13" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="Q349" s="12"/>
     </row>
     <row r="350" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A350" s="3" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B350" s="3" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="C350" s="3" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="D350" s="3" t="s">
         <v>446</v>
@@ -15480,16 +15826,22 @@
         <v>0.49</v>
       </c>
       <c r="K350" s="3" t="s">
-        <v>1052</v>
+        <v>1050</v>
+      </c>
+      <c r="L350" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="M350" s="3" t="s">
+        <v>1260</v>
       </c>
       <c r="N350" s="3">
         <v>2</v>
       </c>
       <c r="O350" s="3" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="P350" s="7" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="Q350" s="10">
         <v>227</v>
@@ -15497,32 +15849,32 @@
     </row>
     <row r="351" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="352" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="D356" t="s">
         <v>456</v>
@@ -15573,9 +15925,14 @@
     <hyperlink ref="M136" r:id="rId37" xr:uid="{998087A9-41C4-44BF-B21F-F44247ACBB2E}"/>
     <hyperlink ref="M139" r:id="rId38" xr:uid="{218652C7-1F49-4CEE-B7B0-8CDCD3321A75}"/>
     <hyperlink ref="M156" r:id="rId39" display="https://doi.org/10.1111/nph.14722 - there seems to be some migration at least" xr:uid="{B5CBFBDE-9DC5-4A51-9328-E2D4110493FB}"/>
+    <hyperlink ref="M251" r:id="rId40" xr:uid="{CD3396E5-3303-439A-A3B4-9E88A411D59F}"/>
+    <hyperlink ref="M240" r:id="rId41" xr:uid="{96419FC8-54EF-4412-BCA7-A79FD02A9C3B}"/>
+    <hyperlink ref="M268" r:id="rId42" xr:uid="{F3119FD2-29B2-4484-991E-C95050A8D4E5}"/>
+    <hyperlink ref="M273" r:id="rId43" xr:uid="{D86490D2-53D7-4FCE-849D-687EA60A509E}"/>
+    <hyperlink ref="M303" r:id="rId44" xr:uid="{9ECEE33C-CD35-40D4-9ADA-DBD7FBB658AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
 
@@ -21060,7 +21417,7 @@
         <v>676</v>
       </c>
       <c r="C1" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finish adding height data
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\330276_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67226_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5FED73-ECF4-4BC2-9DCB-E9E26184FA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F3644E-3D0F-4E9C-B2E0-97D6FF269AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3862" uniqueCount="1259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3876" uniqueCount="1274">
   <si>
     <t>Species</t>
   </si>
@@ -3804,9 +3804,6 @@
     <t>https://doi.org/10.1111/j.1439-037X.2010.00429.x ; I got this value by taking the average height of the 15 white bars (i.e. non-salt-stress condition) in figure 1 a using image j, converting heights in pixels to heights in cm based on the scale of the y-axis</t>
   </si>
   <si>
-    <t>cannot find a published reference with a DOI for this. There are some research botanical garden websites with height values, but I don't know if I can trust that</t>
-  </si>
-  <si>
     <t>cultivation status</t>
   </si>
   <si>
@@ -3814,6 +3811,54 @@
   </si>
   <si>
     <t>can only find GBS data, actually I don't think this is GBS data, it's targeted sequencing of 400 SNPS</t>
+  </si>
+  <si>
+    <t>http://www.missouribotanicalgarden.org/gardens-gardening/your-garden/plant-finder/plant-details/kc/e454/cucurbita-argyrosperma.aspx ; average of height range reported on website for missouri botanical garden, then converted to meters; Retrieved 2023-10-25</t>
+  </si>
+  <si>
+    <t>DOI: 10.5897/JPBCS2016.0605 ; Animasaun, D. A., J. A. Morakinyo, and O. T. Mustapha. "Assessment of the effects of gamma irradiation on the growth and yield of Digitaria exilis [Haller]." Journal of Applied Biosciences 75 (2014): 6164-6172. ; average value for HP variable in Table 4</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5897/AJB11.1292 ; Mean value for 2008 and 2009 averages in Table 1</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2135/cropsci2005.07-0202 ; Average of 2000 Height H3 values in Table 1 ; according to this paper, evaluating height at maturity in soybean is difficult but these values come from 40 days after planting</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10722-005-2932-y ; Mean of averages reported in columns I and II for Lens ervoides</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1139/G07-040 ; mean of 2004 and 2005 values in Table 2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.biocon.2010.06.029 ; Gross, C. L., and Peter H. Weston. "Macadamia jansenii (Proteaceae), a new species from central Queensland." Australian Systematic Botany 5.6 (1992): 725-728. ; average value of range reported in text 6-18 m</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.scienta.2011.06.036</t>
+  </si>
+  <si>
+    <t>http://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=282778 ; average of height range reported by Missouri Botanical Garden (12 - 20 feet), then converted to meters</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.21273/HORTSCI.44.3.656 ; Mean of Ht column in Table 2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.2135/cropsci2011.05.0287 ; Control value in table 4</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/genetics/150.2.899 ; Most common value in Figure 3 histogram for plant height</t>
+  </si>
+  <si>
+    <t>https://owic.oregonstate.edu/black-cottonwood-populus-trichocarpa ; average of range given in text (125 - 150 ft), then converted to meters</t>
+  </si>
+  <si>
+    <t>https://www.rhododendron.org/descriptionS_taxon.asp?ID=259 ; description from American Rhododendron Society</t>
+  </si>
+  <si>
+    <t>https://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=283438 ; In its native habitat, it may grow to as much as 50-75' tall over time, but as an indoor plant it grows much shorter ; I took the average of this range then converted it to meters</t>
+  </si>
+  <si>
+    <t>https://www.rhs.org.uk/plants/19138/xanthoceras-sorbifolium/details ; retrieved on 2023-10-25 ; mean of ultimate height range 2.5-4 m ; might also consider looking at https://doi.org/10.1002/fes3.500 ; Mean from Table 1</t>
   </si>
 </sst>
 </file>
@@ -15945,9 +15990,9 @@
   <dimension ref="A1:Z132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16018,7 +16063,7 @@
         <v>1248</v>
       </c>
       <c r="R1" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="S1" s="6" t="s">
         <v>66</v>
@@ -16086,7 +16131,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>1038</v>
@@ -16216,7 +16261,7 @@
         <v>1250</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>750</v>
@@ -16284,7 +16329,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="10">
@@ -16768,7 +16813,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S13" s="7" t="s">
         <v>145</v>
@@ -16905,7 +16950,7 @@
         <v>1252</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S15" s="13" t="s">
         <v>754</v>
@@ -16970,7 +17015,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S16" s="7" t="s">
         <v>239</v>
@@ -17209,7 +17254,7 @@
         <v>1050</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S20" s="7"/>
       <c r="T20" s="10">
@@ -17269,7 +17314,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S21" s="7"/>
       <c r="T21" s="10">
@@ -17322,7 +17367,7 @@
         <v>1052</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S22" s="13" t="s">
         <v>783</v>
@@ -17381,7 +17426,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S23" s="7" t="s">
         <v>159</v>
@@ -17447,7 +17492,7 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S24" s="7" t="s">
         <v>159</v>
@@ -17497,7 +17542,7 @@
         <v>582</v>
       </c>
       <c r="R25" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S25" s="7"/>
       <c r="T25" s="10">
@@ -17552,7 +17597,7 @@
         <v>867</v>
       </c>
       <c r="R26" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S26" s="7" t="s">
         <v>583</v>
@@ -17614,7 +17659,7 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S27" s="7" t="s">
         <v>324</v>
@@ -17679,7 +17724,7 @@
         <v>1055</v>
       </c>
       <c r="R28" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S28" s="7" t="s">
         <v>622</v>
@@ -17743,7 +17788,7 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S29" s="13" t="s">
         <v>328</v>
@@ -17928,7 +17973,7 @@
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S32" s="7" t="s">
         <v>728</v>
@@ -17985,7 +18030,7 @@
         <v>1059</v>
       </c>
       <c r="R33" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S33" s="7" t="s">
         <v>583</v>
@@ -17998,6 +18043,12 @@
       </c>
       <c r="V33" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="X33" s="15">
+        <v>45222</v>
+      </c>
+      <c r="Y33" s="3">
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -18044,7 +18095,7 @@
         <v>1254</v>
       </c>
       <c r="R34" s="5" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S34" s="7" t="s">
         <v>259</v>
@@ -18104,7 +18155,7 @@
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S35" s="7" t="s">
         <v>260</v>
@@ -18166,7 +18217,7 @@
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S36" s="7" t="s">
         <v>299</v>
@@ -18227,7 +18278,7 @@
         <v>1061</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S37" s="7" t="s">
         <v>583</v>
@@ -18286,7 +18337,7 @@
         <v>1061</v>
       </c>
       <c r="R38" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S38" s="13" t="s">
         <v>341</v>
@@ -18334,7 +18385,7 @@
         <v>954</v>
       </c>
       <c r="R39" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S39" s="7" t="s">
         <v>953</v>
@@ -18384,7 +18435,7 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
       <c r="R40" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S40" s="7" t="s">
         <v>344</v>
@@ -18445,7 +18496,7 @@
         <v>1062</v>
       </c>
       <c r="R41" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S41" s="7"/>
       <c r="T41" s="10">
@@ -18501,7 +18552,7 @@
       <c r="P42" s="3"/>
       <c r="Q42" s="3"/>
       <c r="R42" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S42" s="7" t="s">
         <v>748</v>
@@ -18564,14 +18615,14 @@
       <c r="O43" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="P43" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q43" s="3" t="s">
-        <v>1255</v>
+      <c r="P43" s="3">
+        <v>0.34289999999999998</v>
+      </c>
+      <c r="Q43" s="5" t="s">
+        <v>1258</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S43" s="7" t="s">
         <v>607</v>
@@ -18635,7 +18686,7 @@
       <c r="P44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S44" s="7" t="s">
         <v>583</v>
@@ -18698,10 +18749,14 @@
       <c r="O45" s="3" t="s">
         <v>1064</v>
       </c>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
+      <c r="P45" s="3">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>1259</v>
+      </c>
       <c r="R45" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S45" s="7"/>
       <c r="T45" s="10">
@@ -18760,7 +18815,7 @@
         <v>1066</v>
       </c>
       <c r="R46" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S46" s="7" t="s">
         <v>145</v>
@@ -18813,8 +18868,14 @@
       <c r="O47" s="3" t="s">
         <v>1067</v>
       </c>
+      <c r="P47" s="3">
+        <v>1.9245000000000001</v>
+      </c>
+      <c r="Q47" s="5" t="s">
+        <v>1260</v>
+      </c>
       <c r="R47" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S47" s="7" t="s">
         <v>635</v>
@@ -18871,7 +18932,7 @@
         <v>1068</v>
       </c>
       <c r="R48" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S48" s="7" t="s">
         <v>590</v>
@@ -18933,7 +18994,7 @@
       <c r="P49" s="3"/>
       <c r="Q49" s="3"/>
       <c r="R49" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S49" s="7" t="s">
         <v>585</v>
@@ -18995,7 +19056,7 @@
       <c r="P50" s="4"/>
       <c r="Q50" s="4"/>
       <c r="R50" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S50" s="13" t="s">
         <v>585</v>
@@ -19059,7 +19120,7 @@
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
       <c r="R51" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S51" s="13" t="s">
         <v>361</v>
@@ -19119,7 +19180,7 @@
         <v>1072</v>
       </c>
       <c r="R52" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S52" s="7" t="s">
         <v>290</v>
@@ -19168,8 +19229,12 @@
       <c r="O53" s="8" t="s">
         <v>1073</v>
       </c>
-      <c r="P53" s="8"/>
-      <c r="Q53" s="8"/>
+      <c r="P53" s="8">
+        <v>1.12375</v>
+      </c>
+      <c r="Q53" s="5" t="s">
+        <v>1261</v>
+      </c>
       <c r="R53" s="8" t="s">
         <v>874</v>
       </c>
@@ -19230,7 +19295,7 @@
         <v>870</v>
       </c>
       <c r="R54" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S54" s="7" t="s">
         <v>583</v>
@@ -19294,7 +19359,7 @@
       <c r="P55" s="3"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S55" s="7"/>
       <c r="T55" s="10">
@@ -19358,7 +19423,7 @@
       <c r="P56" s="3"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S56" s="7"/>
       <c r="T56" s="10">
@@ -19416,7 +19481,7 @@
       <c r="P57" s="3"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S57" s="7" t="s">
         <v>145</v>
@@ -19542,7 +19607,7 @@
       <c r="P59" s="4"/>
       <c r="Q59" s="4"/>
       <c r="R59" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S59" s="13"/>
       <c r="T59" s="12">
@@ -19599,7 +19664,7 @@
         <v>1078</v>
       </c>
       <c r="R60" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S60" s="7"/>
       <c r="T60" s="10">
@@ -19610,6 +19675,12 @@
       </c>
       <c r="V60" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="X60" s="15">
+        <v>45222</v>
+      </c>
+      <c r="Y60" s="3">
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:26" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -19655,7 +19726,7 @@
       <c r="P61" s="3"/>
       <c r="Q61" s="3"/>
       <c r="R61" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S61" s="7" t="s">
         <v>263</v>
@@ -19721,7 +19792,7 @@
       <c r="P62" s="4"/>
       <c r="Q62" s="4"/>
       <c r="R62" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S62" s="13" t="s">
         <v>145</v>
@@ -19777,6 +19848,12 @@
       <c r="O63" s="3" t="s">
         <v>1083</v>
       </c>
+      <c r="P63" s="3">
+        <v>0.2495</v>
+      </c>
+      <c r="Q63" s="5" t="s">
+        <v>1262</v>
+      </c>
       <c r="R63" s="3" t="s">
         <v>874</v>
       </c>
@@ -19843,7 +19920,7 @@
         <v>1084</v>
       </c>
       <c r="R64" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S64" s="7" t="s">
         <v>303</v>
@@ -19908,8 +19985,12 @@
       <c r="O65" s="3" t="s">
         <v>1085</v>
       </c>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="3"/>
+      <c r="P65" s="3">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="Q65" s="5" t="s">
+        <v>1263</v>
+      </c>
       <c r="R65" s="3" t="s">
         <v>874</v>
       </c>
@@ -19972,7 +20053,7 @@
         <v>1086</v>
       </c>
       <c r="R66" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S66" s="7"/>
       <c r="T66" s="10">
@@ -20031,10 +20112,14 @@
       <c r="O67" s="3" t="s">
         <v>1087</v>
       </c>
-      <c r="P67" s="3"/>
-      <c r="Q67" s="3"/>
+      <c r="P67" s="3">
+        <v>12</v>
+      </c>
+      <c r="Q67" s="5" t="s">
+        <v>1264</v>
+      </c>
       <c r="R67" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S67" s="7"/>
       <c r="T67" s="10">
@@ -20095,10 +20180,14 @@
       <c r="O68" s="3" t="s">
         <v>1088</v>
       </c>
-      <c r="P68" s="3"/>
-      <c r="Q68" s="3"/>
+      <c r="P68" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="Q68" s="3" t="s">
+        <v>1265</v>
+      </c>
       <c r="R68" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S68" s="7" t="s">
         <v>583</v>
@@ -20226,7 +20315,7 @@
       <c r="P70" s="3"/>
       <c r="Q70" s="3"/>
       <c r="R70" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S70" s="7" t="s">
         <v>583</v>
@@ -20290,7 +20379,7 @@
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
       <c r="R71" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S71" s="7" t="s">
         <v>265</v>
@@ -20476,7 +20565,7 @@
         <v>1094</v>
       </c>
       <c r="R74" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S74" s="7" t="s">
         <v>203</v>
@@ -20532,7 +20621,7 @@
       <c r="P75" s="3"/>
       <c r="Q75" s="3"/>
       <c r="R75" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S75" s="7" t="s">
         <v>647</v>
@@ -20595,10 +20684,14 @@
       <c r="O76" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="P76" s="3"/>
-      <c r="Q76" s="3"/>
+      <c r="P76" s="3">
+        <v>4.8768000000000002</v>
+      </c>
+      <c r="Q76" s="5" t="s">
+        <v>1266</v>
+      </c>
       <c r="R76" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S76" s="7" t="s">
         <v>611</v>
@@ -20661,10 +20754,14 @@
       <c r="O77" s="3" t="s">
         <v>1097</v>
       </c>
-      <c r="P77" s="3"/>
-      <c r="Q77" s="3"/>
+      <c r="P77" s="3">
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="Q77" s="5" t="s">
+        <v>1267</v>
+      </c>
       <c r="R77" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S77" s="7" t="s">
         <v>583</v>
@@ -20728,7 +20825,7 @@
       <c r="P78" s="4"/>
       <c r="Q78" s="4"/>
       <c r="R78" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S78" s="13" t="s">
         <v>696</v>
@@ -20791,7 +20888,7 @@
         <v>206</v>
       </c>
       <c r="R79" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S79" s="7" t="s">
         <v>270</v>
@@ -20957,8 +21054,14 @@
       <c r="O82" s="3" t="s">
         <v>1099</v>
       </c>
+      <c r="P82" s="3">
+        <v>0.74390000000000001</v>
+      </c>
+      <c r="Q82" s="5" t="s">
+        <v>1268</v>
+      </c>
       <c r="R82" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S82" s="7"/>
       <c r="T82" s="10">
@@ -21130,8 +21233,12 @@
       <c r="O85" s="3" t="s">
         <v>1099</v>
       </c>
-      <c r="P85" s="3"/>
-      <c r="Q85" s="3"/>
+      <c r="P85" s="3">
+        <v>0.105</v>
+      </c>
+      <c r="Q85" s="5" t="s">
+        <v>1269</v>
+      </c>
       <c r="R85" s="3" t="s">
         <v>874</v>
       </c>
@@ -21199,7 +21306,7 @@
       <c r="P86" s="3"/>
       <c r="Q86" s="3"/>
       <c r="R86" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S86" s="7" t="s">
         <v>271</v>
@@ -21327,7 +21434,7 @@
       <c r="P88" s="3"/>
       <c r="Q88" s="3"/>
       <c r="R88" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S88" s="7" t="s">
         <v>272</v>
@@ -21387,7 +21494,7 @@
       <c r="P89" s="4"/>
       <c r="Q89" s="4"/>
       <c r="R89" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S89" s="13" t="s">
         <v>402</v>
@@ -21455,7 +21562,7 @@
       <c r="P90" s="3"/>
       <c r="Q90" s="3"/>
       <c r="R90" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S90" s="7"/>
       <c r="T90" s="10">
@@ -21515,7 +21622,7 @@
       <c r="P91" s="3"/>
       <c r="Q91" s="3"/>
       <c r="R91" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S91" s="7"/>
       <c r="T91" s="10">
@@ -21577,7 +21684,7 @@
       <c r="P92" s="4"/>
       <c r="Q92" s="4"/>
       <c r="R92" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S92" s="13" t="s">
         <v>408</v>
@@ -21706,10 +21813,14 @@
       <c r="O94" s="3" t="s">
         <v>1107</v>
       </c>
-      <c r="P94" s="3"/>
-      <c r="Q94" s="3"/>
+      <c r="P94" s="3">
+        <v>41.91</v>
+      </c>
+      <c r="Q94" s="5" t="s">
+        <v>1270</v>
+      </c>
       <c r="R94" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S94" s="7" t="s">
         <v>252</v>
@@ -21775,7 +21886,7 @@
       <c r="P95" s="3"/>
       <c r="Q95" s="3"/>
       <c r="R95" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S95" s="7" t="s">
         <v>583</v>
@@ -21841,7 +21952,7 @@
       <c r="P96" s="3"/>
       <c r="Q96" s="3"/>
       <c r="R96" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S96" s="7" t="s">
         <v>412</v>
@@ -21907,7 +22018,7 @@
       <c r="P97" s="3"/>
       <c r="Q97" s="3"/>
       <c r="R97" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S97" s="7" t="s">
         <v>273</v>
@@ -22022,7 +22133,7 @@
         <v>1113</v>
       </c>
       <c r="R99" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S99" s="7" t="s">
         <v>583</v>
@@ -22084,7 +22195,7 @@
       <c r="P100" s="3"/>
       <c r="Q100" s="3"/>
       <c r="R100" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S100" s="7" t="s">
         <v>712</v>
@@ -22147,8 +22258,12 @@
       <c r="O101" s="3" t="s">
         <v>659</v>
       </c>
-      <c r="P101" s="3"/>
-      <c r="Q101" s="3"/>
+      <c r="P101" s="3">
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="Q101" s="5" t="s">
+        <v>1271</v>
+      </c>
       <c r="R101" s="3" t="s">
         <v>874</v>
       </c>
@@ -22282,7 +22397,7 @@
       <c r="P103" s="4"/>
       <c r="Q103" s="4"/>
       <c r="R103" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S103" s="13" t="s">
         <v>322</v>
@@ -22344,7 +22459,7 @@
       <c r="P104" s="3"/>
       <c r="Q104" s="3"/>
       <c r="R104" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S104" s="7" t="s">
         <v>428</v>
@@ -22399,7 +22514,7 @@
         <v>1119</v>
       </c>
       <c r="R105" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S105" s="7" t="s">
         <v>274</v>
@@ -22581,7 +22696,7 @@
       <c r="P108" s="3"/>
       <c r="Q108" s="3"/>
       <c r="R108" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S108" s="7" t="s">
         <v>159</v>
@@ -22645,7 +22760,7 @@
       <c r="P109" s="4"/>
       <c r="Q109" s="4"/>
       <c r="R109" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S109" s="13" t="s">
         <v>687</v>
@@ -22823,7 +22938,7 @@
       <c r="P112" s="4"/>
       <c r="Q112" s="4"/>
       <c r="R112" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S112" s="13" t="s">
         <v>222</v>
@@ -22879,7 +22994,7 @@
       <c r="P113" s="3"/>
       <c r="Q113" s="3"/>
       <c r="R113" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S113" s="7" t="s">
         <v>159</v>
@@ -22941,7 +23056,7 @@
       <c r="P114" s="3"/>
       <c r="Q114" s="3"/>
       <c r="R114" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S114" s="7" t="s">
         <v>276</v>
@@ -22997,7 +23112,7 @@
         <v>231</v>
       </c>
       <c r="R115" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S115" s="7" t="s">
         <v>278</v>
@@ -23170,7 +23285,7 @@
         <v>1130</v>
       </c>
       <c r="R118" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S118" s="7" t="s">
         <v>142</v>
@@ -23226,7 +23341,7 @@
       <c r="P119" s="3"/>
       <c r="Q119" s="3"/>
       <c r="R119" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S119" s="7" t="s">
         <v>583</v>
@@ -23281,10 +23396,10 @@
         <v>1131</v>
       </c>
       <c r="R120" s="4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="S120" s="13" t="s">
         <v>1257</v>
-      </c>
-      <c r="S120" s="13" t="s">
-        <v>1258</v>
       </c>
       <c r="T120" s="12">
         <v>672</v>
@@ -23337,7 +23452,7 @@
       <c r="P121" s="3"/>
       <c r="Q121" s="3"/>
       <c r="R121" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S121" s="7" t="s">
         <v>233</v>
@@ -23452,7 +23567,7 @@
       <c r="P123" s="4"/>
       <c r="Q123" s="4"/>
       <c r="R123" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S123" s="13" t="s">
         <v>300</v>
@@ -23513,10 +23628,14 @@
       <c r="O124" s="3" t="s">
         <v>1135</v>
       </c>
-      <c r="P124" s="3"/>
-      <c r="Q124" s="3"/>
+      <c r="P124" s="3">
+        <v>19.05</v>
+      </c>
+      <c r="Q124" s="5" t="s">
+        <v>1272</v>
+      </c>
       <c r="R124" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S124" s="7" t="s">
         <v>603</v>
@@ -23580,7 +23699,7 @@
       <c r="P125" s="3"/>
       <c r="Q125" s="3"/>
       <c r="R125" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S125" s="7"/>
       <c r="T125" s="10">
@@ -23640,7 +23759,7 @@
       <c r="P126" s="3"/>
       <c r="Q126" s="3"/>
       <c r="R126" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S126" s="7" t="s">
         <v>594</v>
@@ -23695,7 +23814,7 @@
         <v>1138</v>
       </c>
       <c r="R127" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S127" s="7" t="s">
         <v>444</v>
@@ -23759,7 +23878,7 @@
       <c r="P128" s="3"/>
       <c r="Q128" s="3"/>
       <c r="R128" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S128" s="7" t="s">
         <v>277</v>
@@ -23818,10 +23937,14 @@
       <c r="O129" s="3" t="s">
         <v>1140</v>
       </c>
-      <c r="P129" s="3"/>
-      <c r="Q129" s="3"/>
+      <c r="P129" s="3">
+        <v>3.25</v>
+      </c>
+      <c r="Q129" s="5" t="s">
+        <v>1273</v>
+      </c>
       <c r="R129" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S129" s="7" t="s">
         <v>583</v>
@@ -23887,7 +24010,7 @@
       <c r="P130" s="4"/>
       <c r="Q130" s="4"/>
       <c r="R130" s="4" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S130" s="13" t="s">
         <v>781</v>
@@ -23948,7 +24071,7 @@
         <v>1142</v>
       </c>
       <c r="R131" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S131" s="7" t="s">
         <v>603</v>
@@ -24001,7 +24124,7 @@
         <v>1143</v>
       </c>
       <c r="R132" s="3" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="S132" s="7" t="s">
         <v>583</v>
@@ -24012,6 +24135,12 @@
       </c>
       <c r="V132" s="3" t="s">
         <v>257</v>
+      </c>
+      <c r="X132" s="15">
+        <v>45222</v>
+      </c>
+      <c r="Y132" s="3">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -24067,6 +24196,20 @@
     <hyperlink ref="Q30" r:id="rId46" xr:uid="{21076D40-9243-4168-B697-514BE758B3C7}"/>
     <hyperlink ref="Q34" r:id="rId47" display="https://doi.org/10.1111/j.1439-037X.2010.00429.x ; I got this value by taking the average height of the 15 white bars (i.e. non-salt-stress condition) in figure 1 a using image j, converting heights in pixels to heights in cm based on the scale of the y-axis" xr:uid="{3863F86F-3D00-4730-95EF-1A5BD52DCFDD}"/>
     <hyperlink ref="B94" r:id="rId48" xr:uid="{159829CC-A986-4B44-94EC-5057ABB2E9DB}"/>
+    <hyperlink ref="Q43" r:id="rId49" xr:uid="{015F3695-EFC5-4E34-8CFF-723E20AE597C}"/>
+    <hyperlink ref="Q47" r:id="rId50" xr:uid="{6270B348-F18A-471A-8C5C-05D7C6485070}"/>
+    <hyperlink ref="Q53" r:id="rId51" xr:uid="{71ECD90B-8D49-4F77-AE01-57307CAE0BB5}"/>
+    <hyperlink ref="Q63" r:id="rId52" xr:uid="{1F8F5272-884C-4567-8446-2E087E065EF1}"/>
+    <hyperlink ref="Q65" r:id="rId53" xr:uid="{EF670AE0-7FBB-40BB-BFC8-04BEF555DAF0}"/>
+    <hyperlink ref="Q67" r:id="rId54" xr:uid="{9F1AAC25-C8E9-4311-B97C-F460205DDA81}"/>
+    <hyperlink ref="Q76" r:id="rId55" xr:uid="{EE95F07B-2C68-4858-8728-1BC9B5A64399}"/>
+    <hyperlink ref="Q77" r:id="rId56" xr:uid="{62774BFE-6D2C-4DA5-8A58-148287B9075E}"/>
+    <hyperlink ref="Q82" r:id="rId57" xr:uid="{5318486D-287E-4E41-85DA-DED68BDC3523}"/>
+    <hyperlink ref="Q85" r:id="rId58" xr:uid="{1F22773A-8196-4D43-8217-BB3DD0E29E41}"/>
+    <hyperlink ref="Q94" r:id="rId59" xr:uid="{45F148EB-1C96-4891-9E9D-8AE8F70FEEB5}"/>
+    <hyperlink ref="Q101" r:id="rId60" xr:uid="{CD533664-41C6-4EA6-B220-C9D568EFF065}"/>
+    <hyperlink ref="Q124" r:id="rId61" display="https://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=283438 ; In its native habitat, it may grow to as much as 50-75' tall over time, but as an indoor plant it grows much shorter ; I took the average of this range then converted it to meters" xr:uid="{F382B955-CABD-4C97-A40A-74C06333904B}"/>
+    <hyperlink ref="Q129" r:id="rId62" display="https://doi.org/10.1002/fes3.500 ; Mean from Table 1" xr:uid="{8C79EE87-526F-46CA-A17F-5DCBEEC5C2AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update docs, refine metadata
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67030_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\67430_2_17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA9A11F-8137-4D75-A791-1BB7F4909E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C15D38-B0BA-416F-BE83-93F8266DE427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="3045" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3883" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3884" uniqueCount="1285">
   <si>
     <t>Species</t>
   </si>
@@ -3883,6 +3883,15 @@
   </si>
   <si>
     <t>scaffold04645 was removed from the analysis because the file was not created during the snakemake workflow</t>
+  </si>
+  <si>
+    <t>This species falls under the fort lauderdale accord, so I shouldn't use it</t>
+  </si>
+  <si>
+    <t>GUPTA S, KOZAK M, SAHAY G, et al. Genetic parameters of selection and stability and identification of divergent parents for hybridization in rice bean (Vigna umbellata Thunb. (Ohwi and Ohashi)) in India. The Journal of Agricultural Science. 2009;147(5):581-588. doi:10.1017/S0021859609008715 ; this value represents the mean of the average height values given in table 3</t>
+  </si>
+  <si>
+    <t>Madsen, JOHN D., et al. "Sensitivity of wild rice (Zizania palustris L.) to the aquatic herbicide triclopyr." J. Aquat. Plant Manage 46 (2008): 150-154.</t>
   </si>
 </sst>
 </file>
@@ -3926,7 +3935,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3945,6 +3954,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3959,7 +3974,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4002,6 +4017,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -16028,10 +16052,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9A1616-AAC6-4433-A869-98443D18E34E}">
   <dimension ref="A1:Z132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
+      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16754,60 +16778,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:26" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
         <v>462</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="22" t="s">
         <v>616</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="22" t="s">
         <v>615</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="22" t="s">
         <v>455</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="J12" s="4">
+      <c r="H12" s="23"/>
+      <c r="J12" s="22">
         <v>1.27</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="22" t="s">
         <v>966</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="22" t="s">
         <v>1044</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="22">
         <v>2</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="22" t="s">
         <v>1044</v>
       </c>
-      <c r="R12" s="4" t="s">
+      <c r="R12" s="22" t="s">
         <v>874</v>
       </c>
-      <c r="S12" s="13" t="s">
+      <c r="S12" s="23" t="s">
         <v>617</v>
       </c>
-      <c r="T12" s="12">
+      <c r="T12" s="24">
         <v>5</v>
       </c>
-      <c r="U12" s="4">
-        <v>1</v>
-      </c>
-      <c r="V12" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X12" s="16">
+      <c r="U12" s="22">
+        <v>1</v>
+      </c>
+      <c r="V12" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="X12" s="25">
         <v>45023</v>
       </c>
-      <c r="Y12" s="4">
+      <c r="Y12" s="22">
         <v>3</v>
       </c>
-      <c r="Z12" s="4" t="s">
+      <c r="Z12" s="22" t="s">
         <v>782</v>
       </c>
     </row>
@@ -17209,57 +17233,57 @@
       </c>
       <c r="Z18" s="3"/>
     </row>
-    <row r="19" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:26" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>761</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="22" t="s">
         <v>770</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="22" t="s">
         <v>771</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="22" t="s">
         <v>761</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="J19" s="4">
+      <c r="H19" s="23"/>
+      <c r="J19" s="22">
         <v>0.43</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="22" t="s">
         <v>972</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="22" t="s">
         <v>1049</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19" s="22">
         <v>2</v>
       </c>
-      <c r="O19" s="4" t="s">
+      <c r="O19" s="22" t="s">
         <v>1049</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="R19" s="22" t="s">
         <v>874</v>
       </c>
-      <c r="S19" s="13" t="s">
-        <v>825</v>
-      </c>
-      <c r="T19" s="12">
+      <c r="S19" s="23" t="s">
+        <v>1282</v>
+      </c>
+      <c r="T19" s="24">
         <v>178</v>
       </c>
-      <c r="U19" s="4">
-        <v>1</v>
-      </c>
-      <c r="V19" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X19" s="16"/>
+      <c r="U19" s="22">
+        <v>1</v>
+      </c>
+      <c r="V19" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="X19" s="25"/>
     </row>
     <row r="20" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -17380,57 +17404,57 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:26" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
         <v>702</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="22" t="s">
         <v>699</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="22" t="s">
         <v>757</v>
       </c>
-      <c r="H22" s="13"/>
-      <c r="J22" s="4">
+      <c r="H22" s="23"/>
+      <c r="J22" s="22">
         <v>0.8</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="22" t="s">
         <v>973</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="L22" s="22" t="s">
         <v>833</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="M22" s="22" t="s">
         <v>1155</v>
       </c>
-      <c r="N22" s="4">
+      <c r="N22" s="22">
         <v>2</v>
       </c>
-      <c r="O22" s="4" t="s">
+      <c r="O22" s="22" t="s">
         <v>1052</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="R22" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="S22" s="13" t="s">
+      <c r="S22" s="23" t="s">
         <v>783</v>
       </c>
-      <c r="T22" s="12">
+      <c r="T22" s="24">
         <v>7</v>
       </c>
-      <c r="U22" s="4">
-        <v>1</v>
-      </c>
-      <c r="V22" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X22" s="16"/>
+      <c r="U22" s="22">
+        <v>1</v>
+      </c>
+      <c r="V22" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="X22" s="25"/>
     </row>
     <row r="23" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -17667,7 +17691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>323</v>
       </c>
@@ -17680,13 +17704,10 @@
       <c r="D27" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
       <c r="G27" s="3" t="s">
         <v>756</v>
       </c>
       <c r="H27" s="7"/>
-      <c r="I27" s="3"/>
       <c r="J27" s="3">
         <v>0.76687116600000005</v>
       </c>
@@ -17705,8 +17726,6 @@
       <c r="O27" s="3" t="s">
         <v>1054</v>
       </c>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
       <c r="R27" s="3" t="s">
         <v>1256</v>
       </c>
@@ -17794,7 +17813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>325</v>
       </c>
@@ -17807,15 +17826,12 @@
       <c r="D29" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
       <c r="G29" s="4" t="s">
         <v>325</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>889</v>
       </c>
-      <c r="I29" s="4"/>
       <c r="J29" s="4">
         <v>0.84</v>
       </c>
@@ -17834,8 +17850,6 @@
       <c r="O29" s="4" t="s">
         <v>1056</v>
       </c>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="4"/>
       <c r="R29" s="4" t="s">
         <v>1256</v>
       </c>
@@ -17851,10 +17865,6 @@
       <c r="V29" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="W29" s="4"/>
-      <c r="X29" s="4"/>
-      <c r="Y29" s="4"/>
-      <c r="Z29" s="4"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -19018,7 +19028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>490</v>
       </c>
@@ -19031,13 +19041,10 @@
       <c r="D49" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
       <c r="G49" s="3" t="s">
         <v>786</v>
       </c>
       <c r="H49" s="7"/>
-      <c r="I49" s="3"/>
       <c r="J49" s="3">
         <v>2.16</v>
       </c>
@@ -19056,8 +19063,6 @@
       <c r="O49" s="3" t="s">
         <v>1069</v>
       </c>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
       <c r="R49" s="3" t="s">
         <v>1256</v>
       </c>
@@ -19073,142 +19078,127 @@
       <c r="V49" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W49" s="3"/>
       <c r="X49" s="15">
         <v>45036</v>
       </c>
       <c r="Y49" s="3">
         <v>4</v>
       </c>
-      <c r="Z49" s="3"/>
-    </row>
-    <row r="50" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    </row>
+    <row r="50" spans="1:26" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
         <v>491</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="22" t="s">
         <v>639</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="22" t="s">
         <v>455</v>
       </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4" t="s">
+      <c r="G50" s="22" t="s">
         <v>787</v>
       </c>
-      <c r="H50" s="13"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4">
+      <c r="H50" s="23"/>
+      <c r="J50" s="22">
         <v>1.6</v>
       </c>
-      <c r="K50" s="4" t="s">
+      <c r="K50" s="22" t="s">
         <v>977</v>
       </c>
-      <c r="L50" s="4" t="s">
+      <c r="L50" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="M50" s="4" t="s">
+      <c r="M50" s="22" t="s">
         <v>1145</v>
       </c>
-      <c r="N50" s="4">
+      <c r="N50" s="22">
         <v>4</v>
       </c>
-      <c r="O50" s="4" t="s">
+      <c r="O50" s="22" t="s">
         <v>1070</v>
       </c>
-      <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4" t="s">
+      <c r="R50" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="S50" s="13" t="s">
+      <c r="S50" s="23" t="s">
         <v>585</v>
       </c>
-      <c r="T50" s="12">
+      <c r="T50" s="24">
         <v>88</v>
       </c>
-      <c r="U50" s="4">
-        <v>1</v>
-      </c>
-      <c r="V50" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W50" s="4"/>
-      <c r="X50" s="16">
+      <c r="U50" s="22">
+        <v>1</v>
+      </c>
+      <c r="V50" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="X50" s="25">
         <v>45036</v>
       </c>
-      <c r="Y50" s="4">
+      <c r="Y50" s="22">
         <v>4</v>
       </c>
-      <c r="Z50" s="4" t="s">
+      <c r="Z50" s="22" t="s">
         <v>789</v>
       </c>
     </row>
     <row r="51" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4" t="s">
+      <c r="G51" s="3" t="s">
         <v>777</v>
       </c>
-      <c r="H51" s="13"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4">
+      <c r="H51" s="7"/>
+      <c r="J51" s="3">
         <v>0.37</v>
       </c>
-      <c r="K51" s="4" t="s">
+      <c r="K51" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="L51" s="4" t="s">
+      <c r="L51" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="M51" s="4" t="s">
+      <c r="M51" s="3" t="s">
         <v>1195</v>
       </c>
-      <c r="N51" s="4">
+      <c r="N51" s="3">
         <v>2</v>
       </c>
-      <c r="O51" s="4" t="s">
+      <c r="O51" s="3" t="s">
         <v>1071</v>
       </c>
-      <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4" t="s">
+      <c r="R51" s="3" t="s">
         <v>1256</v>
       </c>
-      <c r="S51" s="13" t="s">
+      <c r="S51" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="T51" s="12">
+      <c r="T51" s="10">
         <v>14</v>
       </c>
-      <c r="U51" s="4">
-        <v>1</v>
-      </c>
-      <c r="V51" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W51" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X51" s="16">
+      <c r="U51" s="3">
+        <v>1</v>
+      </c>
+      <c r="V51" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="W51" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="X51" s="15">
         <v>45009</v>
       </c>
-      <c r="Y51" s="4">
+      <c r="Y51" s="3">
         <v>0</v>
       </c>
-      <c r="Z51" s="4" t="s">
+      <c r="Z51" s="3" t="s">
         <v>765</v>
       </c>
     </row>
@@ -19254,7 +19244,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="53" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>88</v>
       </c>
@@ -19313,14 +19303,12 @@
       <c r="V53" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W53" s="3"/>
       <c r="X53" s="15">
         <v>45170</v>
       </c>
       <c r="Y53" s="3">
         <v>9</v>
       </c>
-      <c r="Z53" s="3"/>
     </row>
     <row r="54" spans="1:26" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
@@ -19505,7 +19493,7 @@
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
     </row>
-    <row r="57" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>25</v>
       </c>
@@ -19518,13 +19506,10 @@
       <c r="D57" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
       <c r="G57" s="3" t="s">
         <v>796</v>
       </c>
       <c r="H57" s="7"/>
-      <c r="I57" s="3"/>
       <c r="J57" s="3">
         <v>3.67</v>
       </c>
@@ -19543,8 +19528,6 @@
       <c r="O57" s="3" t="s">
         <v>1075</v>
       </c>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
       <c r="R57" s="3" t="s">
         <v>1256</v>
       </c>
@@ -19560,16 +19543,14 @@
       <c r="V57" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W57" s="3"/>
       <c r="X57" s="15">
         <v>45050</v>
       </c>
       <c r="Y57" s="3">
         <v>5</v>
       </c>
-      <c r="Z57" s="3"/>
-    </row>
-    <row r="58" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>508</v>
       </c>
@@ -19582,15 +19563,10 @@
       <c r="D58" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
       <c r="G58" s="3" t="s">
         <v>508</v>
       </c>
       <c r="H58" s="7"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
       <c r="L58" s="3" t="s">
         <v>833</v>
       </c>
@@ -19603,8 +19579,6 @@
       <c r="O58" s="3" t="s">
         <v>1076</v>
       </c>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
       <c r="R58" s="3" t="s">
         <v>874</v>
       </c>
@@ -19620,16 +19594,14 @@
       <c r="V58" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W58" s="3"/>
       <c r="X58" s="15">
         <v>45050</v>
       </c>
       <c r="Y58" s="3">
         <v>5</v>
       </c>
-      <c r="Z58" s="3"/>
-    </row>
-    <row r="59" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>24</v>
       </c>
@@ -19642,15 +19614,12 @@
       <c r="D59" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
       <c r="G59" s="4" t="s">
         <v>905</v>
       </c>
       <c r="H59" s="13" t="s">
         <v>906</v>
       </c>
-      <c r="I59" s="4"/>
       <c r="J59" s="4">
         <v>7.33</v>
       </c>
@@ -19669,8 +19638,6 @@
       <c r="O59" s="4" t="s">
         <v>1077</v>
       </c>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
       <c r="R59" s="4" t="s">
         <v>1256</v>
       </c>
@@ -19684,9 +19651,7 @@
       <c r="V59" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="W59" s="4"/>
       <c r="X59" s="16"/>
-      <c r="Y59" s="4"/>
       <c r="Z59" s="4" t="s">
         <v>886</v>
       </c>
@@ -19748,7 +19713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:26" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>77</v>
       </c>
@@ -19761,15 +19726,12 @@
       <c r="D61" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
       <c r="G61" s="3" t="s">
         <v>872</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>873</v>
       </c>
-      <c r="I61" s="3"/>
       <c r="J61" s="3">
         <v>3.31</v>
       </c>
@@ -19788,8 +19750,6 @@
       <c r="O61" s="3" t="s">
         <v>1079</v>
       </c>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
       <c r="R61" s="3" t="s">
         <v>1256</v>
       </c>
@@ -19805,14 +19765,12 @@
       <c r="V61" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W61" s="3"/>
       <c r="X61" s="15">
         <v>45170</v>
       </c>
       <c r="Y61" s="3">
         <v>9</v>
       </c>
-      <c r="Z61" s="3"/>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
@@ -20752,8 +20710,8 @@
       <c r="M76" s="3" t="s">
         <v>1145</v>
       </c>
-      <c r="N76" s="3" t="s">
-        <v>1096</v>
+      <c r="N76" s="3">
+        <v>2</v>
       </c>
       <c r="O76" s="3" t="s">
         <v>609</v>
@@ -20858,71 +20816,66 @@
       </c>
       <c r="Z77" s="3"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+    <row r="78" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C78" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="D78" s="4" t="s">
+      <c r="D78" s="3" t="s">
         <v>685</v>
       </c>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4" t="s">
+      <c r="G78" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="H78" s="13"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4">
+      <c r="H78" s="7"/>
+      <c r="J78" s="3">
         <v>5.18</v>
       </c>
-      <c r="K78" s="4" t="s">
+      <c r="K78" s="3" t="s">
         <v>1004</v>
       </c>
-      <c r="L78" s="4" t="s">
+      <c r="L78" s="3" t="s">
         <v>828</v>
       </c>
-      <c r="M78" s="4" t="s">
+      <c r="M78" s="3" t="s">
         <v>1213</v>
       </c>
-      <c r="N78" s="4">
+      <c r="N78" s="3">
         <v>2</v>
       </c>
-      <c r="O78" s="4" t="s">
+      <c r="O78" s="3" t="s">
         <v>1098</v>
       </c>
-      <c r="P78" s="4"/>
-      <c r="Q78" s="4"/>
-      <c r="R78" s="4" t="s">
+      <c r="R78" s="3" t="s">
         <v>1256</v>
       </c>
-      <c r="S78" s="13" t="s">
+      <c r="S78" s="7" t="s">
         <v>696</v>
       </c>
-      <c r="T78" s="12">
+      <c r="T78" s="10">
         <v>5</v>
       </c>
-      <c r="U78" s="4">
-        <v>1</v>
-      </c>
-      <c r="V78" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W78" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X78" s="16">
+      <c r="U78" s="3">
+        <v>1</v>
+      </c>
+      <c r="V78" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="W78" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="X78" s="15">
         <v>45009</v>
       </c>
-      <c r="Y78" s="4">
+      <c r="Y78" s="3">
         <v>0</v>
       </c>
-      <c r="Z78" s="4" t="s">
+      <c r="Z78" s="3" t="s">
         <v>765</v>
       </c>
     </row>
@@ -21337,7 +21290,7 @@
       </c>
       <c r="Z85" s="3"/>
     </row>
-    <row r="86" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>3</v>
       </c>
@@ -21350,15 +21303,12 @@
       <c r="D86" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
       <c r="G86" s="3" t="s">
         <v>915</v>
       </c>
       <c r="H86" s="7" t="s">
         <v>916</v>
       </c>
-      <c r="I86" s="3"/>
       <c r="J86" s="3">
         <v>0.5</v>
       </c>
@@ -21377,8 +21327,6 @@
       <c r="O86" s="3" t="s">
         <v>1099</v>
       </c>
-      <c r="P86" s="3"/>
-      <c r="Q86" s="3"/>
       <c r="R86" s="3" t="s">
         <v>1256</v>
       </c>
@@ -21394,10 +21342,6 @@
       <c r="V86" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W86" s="3"/>
-      <c r="X86" s="3"/>
-      <c r="Y86" s="3"/>
-      <c r="Z86" s="3"/>
     </row>
     <row r="87" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
@@ -21528,68 +21472,62 @@
       </c>
     </row>
     <row r="89" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C89" s="3" t="s">
         <v>731</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="D89" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E89" s="4"/>
-      <c r="F89" s="4"/>
-      <c r="G89" s="4" t="s">
+      <c r="G89" s="3" t="s">
         <v>815</v>
       </c>
-      <c r="H89" s="13"/>
-      <c r="I89" s="4"/>
-      <c r="J89" s="4">
+      <c r="H89" s="7"/>
+      <c r="J89" s="3">
         <v>3.8</v>
       </c>
-      <c r="K89" s="4" t="s">
+      <c r="K89" s="3" t="s">
         <v>1011</v>
       </c>
-      <c r="L89" s="4" t="s">
+      <c r="L89" s="3" t="s">
         <v>1146</v>
       </c>
-      <c r="M89" s="4" t="s">
+      <c r="M89" s="3" t="s">
         <v>1216</v>
       </c>
-      <c r="N89" s="4">
+      <c r="N89" s="3">
         <v>2</v>
       </c>
-      <c r="O89" s="4" t="s">
+      <c r="O89" s="3" t="s">
         <v>732</v>
       </c>
-      <c r="P89" s="4"/>
-      <c r="Q89" s="4"/>
-      <c r="R89" s="4" t="s">
+      <c r="R89" s="3" t="s">
         <v>1256</v>
       </c>
-      <c r="S89" s="13" t="s">
+      <c r="S89" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="T89" s="12">
+      <c r="T89" s="10">
         <v>91</v>
       </c>
-      <c r="U89" s="4">
-        <v>1</v>
-      </c>
-      <c r="V89" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W89" s="4"/>
-      <c r="X89" s="16">
+      <c r="U89" s="3">
+        <v>1</v>
+      </c>
+      <c r="V89" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="X89" s="15">
         <v>45065</v>
       </c>
-      <c r="Y89" s="4">
+      <c r="Y89" s="3">
         <v>6</v>
       </c>
-      <c r="Z89" s="4" t="s">
+      <c r="Z89" s="3" t="s">
         <v>821</v>
       </c>
     </row>
@@ -21657,7 +21595,7 @@
       </c>
       <c r="Z90" s="3"/>
     </row>
-    <row r="91" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>242</v>
       </c>
@@ -21670,15 +21608,12 @@
       <c r="D91" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
       <c r="G91" s="3" t="s">
         <v>878</v>
       </c>
       <c r="H91" s="7" t="s">
         <v>879</v>
       </c>
-      <c r="I91" s="3"/>
       <c r="J91" s="3">
         <v>1</v>
       </c>
@@ -21697,8 +21632,6 @@
       <c r="O91" s="3" t="s">
         <v>1105</v>
       </c>
-      <c r="P91" s="3"/>
-      <c r="Q91" s="3"/>
       <c r="R91" s="3" t="s">
         <v>1256</v>
       </c>
@@ -21712,14 +21645,12 @@
       <c r="V91" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W91" s="3"/>
       <c r="X91" s="15">
         <v>45170</v>
       </c>
       <c r="Y91" s="3">
         <v>9</v>
       </c>
-      <c r="Z91" s="3"/>
     </row>
     <row r="92" spans="1:26" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
@@ -22366,7 +22297,7 @@
       </c>
       <c r="Z101" s="3"/>
     </row>
-    <row r="102" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>547</v>
       </c>
@@ -22379,15 +22310,12 @@
       <c r="D102" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
       <c r="G102" s="3" t="s">
         <v>847</v>
       </c>
       <c r="H102" s="7" t="s">
         <v>848</v>
       </c>
-      <c r="I102" s="3"/>
       <c r="J102" s="3">
         <v>0.38445807770961099</v>
       </c>
@@ -22406,8 +22334,6 @@
       <c r="O102" s="3" t="s">
         <v>1116</v>
       </c>
-      <c r="P102" s="3"/>
-      <c r="Q102" s="3"/>
       <c r="R102" s="3" t="s">
         <v>874</v>
       </c>
@@ -22423,14 +22349,12 @@
       <c r="V102" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W102" s="3"/>
       <c r="X102" s="15">
         <v>45081</v>
       </c>
       <c r="Y102" s="3">
         <v>7</v>
       </c>
-      <c r="Z102" s="3"/>
     </row>
     <row r="103" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
@@ -22617,7 +22541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="106" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>132</v>
       </c>
@@ -22630,13 +22554,10 @@
       <c r="D106" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E106" s="3"/>
-      <c r="F106" s="3"/>
       <c r="G106" s="3" t="s">
         <v>132</v>
       </c>
       <c r="H106" s="7"/>
-      <c r="I106" s="3"/>
       <c r="J106" s="3">
         <v>0.8</v>
       </c>
@@ -22655,8 +22576,6 @@
       <c r="O106" s="3" t="s">
         <v>1119</v>
       </c>
-      <c r="P106" s="3"/>
-      <c r="Q106" s="3"/>
       <c r="R106" s="3" t="s">
         <v>874</v>
       </c>
@@ -22672,78 +22591,69 @@
       <c r="V106" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W106" s="3"/>
       <c r="X106" s="15">
         <v>45081</v>
       </c>
       <c r="Y106" s="3">
         <v>7</v>
       </c>
-      <c r="Z106" s="3"/>
-    </row>
-    <row r="107" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
+    </row>
+    <row r="107" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="22" t="s">
         <v>682</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="22" t="s">
         <v>698</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C107" s="22" t="s">
         <v>697</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="D107" s="22" t="s">
         <v>685</v>
       </c>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="4"/>
-      <c r="J107" s="4">
+      <c r="H107" s="23"/>
+      <c r="J107" s="22">
         <v>0.97137014314928405</v>
       </c>
-      <c r="K107" s="14" t="s">
+      <c r="K107" s="26" t="s">
         <v>1177</v>
       </c>
-      <c r="L107" s="4" t="s">
+      <c r="L107" s="22" t="s">
         <v>833</v>
       </c>
-      <c r="M107" s="4" t="s">
+      <c r="M107" s="22" t="s">
         <v>1227</v>
       </c>
-      <c r="N107" s="4">
+      <c r="N107" s="22">
         <v>2</v>
       </c>
-      <c r="O107" s="4" t="s">
+      <c r="O107" s="22" t="s">
         <v>1120</v>
       </c>
-      <c r="P107" s="4"/>
-      <c r="Q107" s="4"/>
-      <c r="R107" s="4" t="s">
+      <c r="R107" s="22" t="s">
         <v>874</v>
       </c>
-      <c r="S107" s="13"/>
-      <c r="T107" s="12">
+      <c r="S107" s="23"/>
+      <c r="T107" s="24">
         <v>30</v>
       </c>
-      <c r="U107" s="4">
-        <v>1</v>
-      </c>
-      <c r="V107" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W107" s="4"/>
-      <c r="X107" s="16">
+      <c r="U107" s="22">
+        <v>1</v>
+      </c>
+      <c r="V107" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="X107" s="25">
         <v>45081</v>
       </c>
-      <c r="Y107" s="4">
+      <c r="Y107" s="22">
         <v>7</v>
       </c>
-      <c r="Z107" s="4" t="s">
+      <c r="Z107" s="22" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="108" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>18</v>
       </c>
@@ -22756,13 +22666,10 @@
       <c r="D108" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
       <c r="G108" s="3" t="s">
         <v>555</v>
       </c>
       <c r="H108" s="7"/>
-      <c r="I108" s="3"/>
       <c r="J108" s="3">
         <v>1.06</v>
       </c>
@@ -22781,8 +22688,6 @@
       <c r="O108" s="3" t="s">
         <v>1121</v>
       </c>
-      <c r="P108" s="3"/>
-      <c r="Q108" s="3"/>
       <c r="R108" s="3" t="s">
         <v>1256</v>
       </c>
@@ -22798,78 +22703,70 @@
       <c r="V108" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W108" s="3"/>
       <c r="X108" s="15">
         <v>45202</v>
       </c>
       <c r="Y108" s="3">
         <v>12</v>
       </c>
-      <c r="Z108" s="3"/>
-    </row>
-    <row r="109" spans="1:26" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+    </row>
+    <row r="109" spans="1:26" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="22" t="s">
         <v>674</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="22" t="s">
         <v>686</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C109" s="22" t="s">
         <v>688</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="22" t="s">
         <v>685</v>
       </c>
-      <c r="E109" s="4"/>
-      <c r="F109" s="4"/>
-      <c r="G109" s="4" t="s">
+      <c r="G109" s="22" t="s">
         <v>823</v>
       </c>
-      <c r="H109" s="13"/>
-      <c r="I109" s="4"/>
-      <c r="J109" s="4">
-        <v>1</v>
-      </c>
-      <c r="K109" s="4" t="s">
+      <c r="H109" s="23"/>
+      <c r="J109" s="22">
+        <v>1</v>
+      </c>
+      <c r="K109" s="22" t="s">
         <v>962</v>
       </c>
-      <c r="L109" s="4" t="s">
+      <c r="L109" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="M109" s="4" t="s">
+      <c r="M109" s="22" t="s">
         <v>1229</v>
       </c>
-      <c r="N109" s="4">
+      <c r="N109" s="22">
         <v>2</v>
       </c>
-      <c r="O109" s="4" t="s">
+      <c r="O109" s="22" t="s">
         <v>1122</v>
       </c>
-      <c r="P109" s="4"/>
-      <c r="Q109" s="4"/>
-      <c r="R109" s="4" t="s">
+      <c r="R109" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="S109" s="13" t="s">
+      <c r="S109" s="23" t="s">
         <v>687</v>
       </c>
-      <c r="T109" s="12">
+      <c r="T109" s="24">
         <v>15</v>
       </c>
-      <c r="U109" s="4">
-        <v>1</v>
-      </c>
-      <c r="V109" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="W109" s="4"/>
-      <c r="X109" s="16">
+      <c r="U109" s="22">
+        <v>1</v>
+      </c>
+      <c r="V109" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="X109" s="25">
         <v>45081</v>
       </c>
-      <c r="Y109" s="4">
+      <c r="Y109" s="22">
         <v>7</v>
       </c>
-      <c r="Z109" s="4" t="s">
+      <c r="Z109" s="22" t="s">
         <v>824</v>
       </c>
     </row>
@@ -22995,49 +22892,33 @@
       </c>
       <c r="Z111" s="3"/>
     </row>
-    <row r="112" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+    <row r="112" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B112" s="4"/>
-      <c r="C112" s="4" t="s">
+      <c r="C112" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="D112" s="4"/>
-      <c r="E112" s="4"/>
-      <c r="F112" s="4"/>
-      <c r="G112" s="4"/>
-      <c r="H112" s="13"/>
-      <c r="I112" s="4"/>
-      <c r="J112" s="4"/>
-      <c r="K112" s="4"/>
-      <c r="L112" s="4" t="s">
+      <c r="H112" s="23"/>
+      <c r="L112" s="22" t="s">
         <v>833</v>
       </c>
-      <c r="M112" s="4" t="s">
+      <c r="M112" s="22" t="s">
         <v>1231</v>
       </c>
-      <c r="N112" s="4" t="s">
+      <c r="N112" s="22" t="s">
         <v>1126</v>
       </c>
-      <c r="O112" s="4" t="s">
+      <c r="O112" s="22" t="s">
         <v>1125</v>
       </c>
-      <c r="P112" s="4"/>
-      <c r="Q112" s="4"/>
-      <c r="R112" s="4" t="s">
+      <c r="R112" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="S112" s="13" t="s">
+      <c r="S112" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="T112" s="12"/>
-      <c r="U112" s="4"/>
-      <c r="V112" s="4"/>
-      <c r="W112" s="4"/>
-      <c r="X112" s="4"/>
-      <c r="Y112" s="4"/>
-      <c r="Z112" s="4"/>
+      <c r="T112" s="24"/>
     </row>
     <row r="113" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
@@ -23446,60 +23327,60 @@
       <c r="Y119" s="3"/>
       <c r="Z119" s="3"/>
     </row>
-    <row r="120" spans="1:26" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="4" t="s">
+    <row r="120" spans="1:26" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="22" t="s">
         <v>720</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C120" s="22" t="s">
         <v>719</v>
       </c>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="G120" s="4" t="s">
+      <c r="G120" s="22" t="s">
         <v>938</v>
       </c>
-      <c r="H120" s="13" t="s">
+      <c r="H120" s="23" t="s">
         <v>939</v>
       </c>
-      <c r="J120" s="4">
+      <c r="J120" s="22">
         <v>0.43</v>
       </c>
-      <c r="K120" s="4" t="s">
+      <c r="K120" s="22" t="s">
         <v>1027</v>
       </c>
-      <c r="L120" s="4" t="s">
+      <c r="L120" s="22" t="s">
         <v>833</v>
       </c>
-      <c r="M120" s="4" t="s">
+      <c r="M120" s="22" t="s">
         <v>1131</v>
       </c>
-      <c r="N120" s="4">
+      <c r="N120" s="22">
         <v>2</v>
       </c>
-      <c r="O120" s="4" t="s">
+      <c r="O120" s="22" t="s">
         <v>1131</v>
       </c>
-      <c r="R120" s="4" t="s">
+      <c r="R120" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="S120" s="13" t="s">
+      <c r="S120" s="23" t="s">
         <v>1257</v>
       </c>
-      <c r="T120" s="12">
+      <c r="T120" s="24">
         <v>672</v>
       </c>
-      <c r="U120" s="4">
-        <v>1</v>
-      </c>
-      <c r="V120" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="121" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U120" s="22">
+        <v>1</v>
+      </c>
+      <c r="V120" s="22" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="121" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>23</v>
       </c>
@@ -23512,13 +23393,10 @@
       <c r="D121" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
       <c r="G121" s="3" t="s">
         <v>433</v>
       </c>
       <c r="H121" s="7"/>
-      <c r="I121" s="3"/>
       <c r="J121" s="3">
         <v>17.3</v>
       </c>
@@ -23537,8 +23415,6 @@
       <c r="O121" s="3" t="s">
         <v>1132</v>
       </c>
-      <c r="P121" s="3"/>
-      <c r="Q121" s="3"/>
       <c r="R121" s="3" t="s">
         <v>1256</v>
       </c>
@@ -23554,61 +23430,57 @@
       <c r="V121" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W121" s="3"/>
-      <c r="X121" s="3"/>
-      <c r="Y121" s="3"/>
-      <c r="Z121" s="3"/>
-    </row>
-    <row r="122" spans="1:26" s="4" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
+    </row>
+    <row r="122" spans="1:26" s="22" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A122" s="22" t="s">
         <v>429</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="22" t="s">
         <v>734</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C122" s="22" t="s">
         <v>733</v>
       </c>
-      <c r="G122" s="4" t="s">
+      <c r="G122" s="22" t="s">
         <v>429</v>
       </c>
-      <c r="H122" s="13" t="s">
+      <c r="H122" s="23" t="s">
         <v>940</v>
       </c>
-      <c r="J122" s="4">
+      <c r="J122" s="22">
         <v>12.3</v>
       </c>
-      <c r="K122" s="4" t="s">
+      <c r="K122" s="22" t="s">
         <v>1028</v>
       </c>
-      <c r="L122" s="4" t="s">
+      <c r="L122" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="M122" s="4" t="s">
+      <c r="M122" s="22" t="s">
         <v>1145</v>
       </c>
-      <c r="N122" s="4">
+      <c r="N122" s="22">
         <v>4</v>
       </c>
-      <c r="O122" s="4" t="s">
+      <c r="O122" s="22" t="s">
         <v>1133</v>
       </c>
-      <c r="R122" s="4" t="s">
+      <c r="R122" s="22" t="s">
         <v>874</v>
       </c>
-      <c r="S122" s="13" t="s">
+      <c r="S122" s="23" t="s">
         <v>1134</v>
       </c>
-      <c r="T122" s="12">
+      <c r="T122" s="24">
         <v>109</v>
       </c>
-      <c r="U122" s="4">
-        <v>1</v>
-      </c>
-      <c r="V122" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="Z122" s="4" t="s">
+      <c r="U122" s="22">
+        <v>1</v>
+      </c>
+      <c r="V122" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z122" s="22" t="s">
         <v>886</v>
       </c>
     </row>
@@ -23676,7 +23548,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="124" spans="1:26" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>261</v>
       </c>
@@ -23689,15 +23561,12 @@
       <c r="D124" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
       <c r="G124" s="3" t="s">
         <v>882</v>
       </c>
       <c r="H124" s="7" t="s">
         <v>883</v>
       </c>
-      <c r="I124" s="3"/>
       <c r="J124" s="3">
         <v>3.76</v>
       </c>
@@ -23737,14 +23606,12 @@
       <c r="V124" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W124" s="3"/>
       <c r="X124" s="15">
         <v>45170</v>
       </c>
       <c r="Y124" s="3">
         <v>9</v>
       </c>
-      <c r="Z124" s="3"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
@@ -23850,8 +23717,12 @@
       <c r="O126" s="3" t="s">
         <v>1137</v>
       </c>
-      <c r="P126" s="3"/>
-      <c r="Q126" s="3"/>
+      <c r="P126" s="3">
+        <v>1.39</v>
+      </c>
+      <c r="Q126" s="3" t="s">
+        <v>1283</v>
+      </c>
       <c r="R126" s="3" t="s">
         <v>1256</v>
       </c>
@@ -23995,7 +23866,7 @@
       </c>
       <c r="Z128" s="3"/>
     </row>
-    <row r="129" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>568</v>
       </c>
@@ -24008,11 +23879,7 @@
       <c r="D129" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E129" s="3"/>
-      <c r="F129" s="3"/>
-      <c r="G129" s="3"/>
       <c r="H129" s="7"/>
-      <c r="I129" s="3"/>
       <c r="J129" s="3">
         <v>0.44780163599181999</v>
       </c>
@@ -24052,16 +23919,14 @@
       <c r="V129" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="W129" s="3"/>
       <c r="X129" s="15">
         <v>45170</v>
       </c>
       <c r="Y129" s="3">
         <v>9</v>
       </c>
-      <c r="Z129" s="3"/>
-    </row>
-    <row r="130" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:26" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>9</v>
       </c>
@@ -24074,15 +23939,12 @@
       <c r="D130" s="4" t="s">
         <v>445</v>
       </c>
-      <c r="E130" s="4"/>
-      <c r="F130" s="4"/>
       <c r="G130" s="13" t="s">
         <v>947</v>
       </c>
       <c r="H130" s="13" t="s">
         <v>948</v>
       </c>
-      <c r="I130" s="4"/>
       <c r="J130" s="4">
         <v>2.7</v>
       </c>
@@ -24101,8 +23963,6 @@
       <c r="O130" s="4" t="s">
         <v>1141</v>
       </c>
-      <c r="P130" s="4"/>
-      <c r="Q130" s="4"/>
       <c r="R130" s="4" t="s">
         <v>1256</v>
       </c>
@@ -24118,74 +23978,76 @@
       <c r="V130" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="W130" s="4"/>
-      <c r="X130" s="4"/>
-      <c r="Y130" s="4"/>
-      <c r="Z130" s="4"/>
-    </row>
-    <row r="131" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="4" t="s">
+    </row>
+    <row r="131" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C131" s="3" t="s">
         <v>745</v>
       </c>
-      <c r="D131" s="4" t="s">
+      <c r="D131" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E131" s="4" t="s">
+      <c r="E131" s="3" t="s">
         <v>1082</v>
       </c>
-      <c r="F131" s="4" t="s">
+      <c r="F131" s="3" t="s">
         <v>1142</v>
       </c>
-      <c r="G131" s="4" t="s">
+      <c r="G131" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="H131" s="13"/>
-      <c r="J131" s="4">
+      <c r="H131" s="7"/>
+      <c r="J131" s="3">
         <v>3.7749999999999999</v>
       </c>
-      <c r="K131" s="14" t="s">
+      <c r="K131" s="5" t="s">
         <v>1181</v>
       </c>
-      <c r="L131" s="4" t="s">
+      <c r="L131" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="M131" s="4" t="s">
+      <c r="M131" s="3" t="s">
         <v>1240</v>
       </c>
-      <c r="N131" s="4">
+      <c r="N131" s="3">
         <v>2</v>
       </c>
-      <c r="O131" s="4" t="s">
+      <c r="O131" s="3" t="s">
         <v>1142</v>
       </c>
-      <c r="R131" s="4" t="s">
+      <c r="P131" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q131" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="R131" s="3" t="s">
         <v>1256</v>
       </c>
-      <c r="S131" s="13" t="s">
+      <c r="S131" s="7" t="s">
         <v>603</v>
       </c>
-      <c r="T131" s="12">
+      <c r="T131" s="10">
         <v>821</v>
       </c>
-      <c r="U131" s="4">
-        <v>1</v>
-      </c>
-      <c r="V131" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X131" s="16">
+      <c r="U131" s="3">
+        <v>1</v>
+      </c>
+      <c r="V131" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="X131" s="15">
         <v>45230</v>
       </c>
-      <c r="Y131" s="4">
+      <c r="Y131" s="3">
         <v>17</v>
       </c>
-      <c r="Z131" s="4" t="s">
+      <c r="Z131" s="3" t="s">
         <v>1279</v>
       </c>
     </row>

</xml_diff>

<commit_message>
plot multiple regression models
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/131238_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\459640_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{19133C89-6566-42D6-AA5B-2444853423A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42EACBFA-2D2E-43A5-8C51-A3244A3D7801}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ED7326-FA56-4DFB-81E7-3157F44B7237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3894" uniqueCount="1300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3896" uniqueCount="1301">
   <si>
     <t>Species</t>
   </si>
@@ -3937,6 +3937,9 @@
   </si>
   <si>
     <t>I initially ran this species in batch 10, and once prior to that. I wanted to switch to using the GBS dataset, which had more individuals at lower coverage. However, this made it hard to identify SNPs and meaningfully compare k-mer spectra. Thus, I re-ran this species in batch 25 using the original WGS dataset</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/BF00126757</t>
   </si>
 </sst>
 </file>
@@ -16112,10 +16115,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9A1616-AAC6-4433-A869-98443D18E34E}">
   <dimension ref="A1:AA132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="S64" sqref="S64"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16881,6 +16884,12 @@
       <c r="P12" s="3" t="s">
         <v>1044</v>
       </c>
+      <c r="Q12" s="3">
+        <v>0.3861</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>1300</v>
+      </c>
       <c r="S12" s="3" t="s">
         <v>874</v>
       </c>
@@ -23212,6 +23221,9 @@
       </c>
       <c r="D115" s="3" t="s">
         <v>445</v>
+      </c>
+      <c r="H115" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="I115" s="7"/>
       <c r="K115" s="3">

</xml_diff>

<commit_message>
update docs, finish plots
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\459640_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/263374_2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ED7326-FA56-4DFB-81E7-3157F44B7237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{DCCF6899-72E0-4DD8-84E7-ADE619EF62B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49C62267-A199-4D50-ADB6-8AD9B48EF772}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3896" uniqueCount="1301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3900" uniqueCount="1304">
   <si>
     <t>Species</t>
   </si>
@@ -3930,9 +3930,6 @@
     <t>Yucca filamentosa C3 alt v2.1</t>
   </si>
   <si>
-    <t>Assembly and annotation publication</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1093/plcell/koab077</t>
   </si>
   <si>
@@ -3940,6 +3937,18 @@
   </si>
   <si>
     <t>https://doi.org/10.1007/BF00126757</t>
+  </si>
+  <si>
+    <t>DNA-seq publication</t>
+  </si>
+  <si>
+    <t>Assembly and annotation version</t>
+  </si>
+  <si>
+    <t>var. rush v1.1</t>
+  </si>
+  <si>
+    <t>GCA_911865555.2</t>
   </si>
 </sst>
 </file>
@@ -16116,9 +16125,9 @@
   <dimension ref="A1:AA132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16141,7 +16150,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>1300</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -16150,7 +16159,7 @@
         <v>316</v>
       </c>
       <c r="E1" t="s">
-        <v>1297</v>
+        <v>1301</v>
       </c>
       <c r="F1" t="s">
         <v>446</v>
@@ -16286,61 +16295,61 @@
       </c>
       <c r="AA2" s="3"/>
     </row>
-    <row r="3" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="K3" s="4">
+      <c r="I3" s="23"/>
+      <c r="K3" s="22">
         <v>4.3967280000000004</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="22" t="s">
         <v>1166</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="22" t="s">
         <v>1145</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="22">
         <v>2</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="22" t="s">
         <v>1039</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="22" t="s">
         <v>874</v>
       </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="12">
+      <c r="T3" s="23"/>
+      <c r="U3" s="24">
         <v>306</v>
       </c>
-      <c r="V3" s="4">
-        <v>1</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y3" s="16">
+      <c r="V3" s="22">
+        <v>1</v>
+      </c>
+      <c r="W3" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y3" s="25">
         <v>45012</v>
       </c>
-      <c r="Z3" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="4" t="s">
+      <c r="Z3" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="22" t="s">
         <v>772</v>
       </c>
     </row>
@@ -16888,7 +16897,7 @@
         <v>0.3861</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>874</v>
@@ -16981,7 +16990,7 @@
         <v>10</v>
       </c>
       <c r="AA13" s="3" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
@@ -18543,6 +18552,9 @@
       <c r="D39" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E39" s="3" t="s">
+        <v>1302</v>
+      </c>
       <c r="I39" s="7"/>
       <c r="K39" s="3">
         <v>0.49</v>
@@ -18570,6 +18582,12 @@
       </c>
       <c r="U39" s="10">
         <v>227</v>
+      </c>
+      <c r="Y39" s="15">
+        <v>45327</v>
+      </c>
+      <c r="Z39" s="3">
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="60" x14ac:dyDescent="0.25">
@@ -19730,61 +19748,61 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:27" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:27" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="E59" s="4" t="s">
-        <v>1298</v>
-      </c>
-      <c r="H59" s="4" t="s">
+      <c r="E59" s="22" t="s">
+        <v>1297</v>
+      </c>
+      <c r="H59" s="22" t="s">
         <v>905</v>
       </c>
-      <c r="I59" s="13" t="s">
+      <c r="I59" s="23" t="s">
         <v>906</v>
       </c>
-      <c r="K59" s="4">
+      <c r="K59" s="22">
         <v>7.33</v>
       </c>
-      <c r="L59" s="4" t="s">
+      <c r="L59" s="22" t="s">
         <v>996</v>
       </c>
-      <c r="M59" s="4" t="s">
+      <c r="M59" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="N59" s="4" t="s">
+      <c r="N59" s="22" t="s">
         <v>1145</v>
       </c>
-      <c r="O59" s="4">
+      <c r="O59" s="22">
         <v>2</v>
       </c>
-      <c r="P59" s="4" t="s">
+      <c r="P59" s="22" t="s">
         <v>1077</v>
       </c>
-      <c r="S59" s="4" t="s">
+      <c r="S59" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="T59" s="13"/>
-      <c r="U59" s="12">
+      <c r="T59" s="23"/>
+      <c r="U59" s="24">
         <v>300</v>
       </c>
-      <c r="V59" s="4">
-        <v>1</v>
-      </c>
-      <c r="W59" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="Y59" s="16"/>
-      <c r="AA59" s="4" t="s">
+      <c r="V59" s="22">
+        <v>1</v>
+      </c>
+      <c r="W59" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y59" s="25"/>
+      <c r="AA59" s="22" t="s">
         <v>886</v>
       </c>
     </row>
@@ -19904,68 +19922,61 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+    <row r="62" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="22" t="s">
         <v>1082</v>
       </c>
-      <c r="G62" s="4" t="s">
+      <c r="G62" s="22" t="s">
         <v>1080</v>
       </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="4"/>
-      <c r="K62" s="4">
+      <c r="I62" s="23"/>
+      <c r="K62" s="22">
         <v>4.21</v>
       </c>
-      <c r="L62" s="4" t="s">
+      <c r="L62" s="22" t="s">
         <v>963</v>
       </c>
-      <c r="M62" s="4" t="s">
+      <c r="M62" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="N62" s="4" t="s">
+      <c r="N62" s="22" t="s">
         <v>1080</v>
       </c>
-      <c r="O62" s="4">
+      <c r="O62" s="22">
         <v>2</v>
       </c>
-      <c r="P62" s="4" t="s">
+      <c r="P62" s="22" t="s">
         <v>1080</v>
       </c>
-      <c r="Q62" s="4"/>
-      <c r="R62" s="4"/>
-      <c r="S62" s="4" t="s">
+      <c r="S62" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="T62" s="13" t="s">
+      <c r="T62" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="U62" s="12">
+      <c r="U62" s="24">
         <v>176</v>
       </c>
-      <c r="V62" s="4">
-        <v>1</v>
-      </c>
-      <c r="W62" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X62" s="4"/>
-      <c r="Y62" s="16"/>
-      <c r="Z62" s="4"/>
-      <c r="AA62" s="4" t="s">
+      <c r="V62" s="22">
+        <v>1</v>
+      </c>
+      <c r="W62" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y62" s="25"/>
+      <c r="AA62" s="22" t="s">
         <v>886</v>
       </c>
     </row>
@@ -21799,66 +21810,57 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:27" ht="105" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
+    <row r="92" spans="1:27" s="22" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="22" t="s">
         <v>406</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4" t="s">
+      <c r="H92" s="22" t="s">
         <v>816</v>
       </c>
-      <c r="I92" s="13" t="s">
+      <c r="I92" s="23" t="s">
         <v>817</v>
       </c>
-      <c r="J92" s="4"/>
-      <c r="K92" s="4">
+      <c r="K92" s="22">
         <v>4.9000000000000004</v>
       </c>
-      <c r="L92" s="4" t="s">
+      <c r="L92" s="22" t="s">
         <v>977</v>
       </c>
-      <c r="M92" s="4" t="s">
+      <c r="M92" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="N92" s="4" t="s">
+      <c r="N92" s="22" t="s">
         <v>1145</v>
       </c>
-      <c r="O92" s="4">
+      <c r="O92" s="22">
         <v>2</v>
       </c>
-      <c r="P92" s="4" t="s">
+      <c r="P92" s="22" t="s">
         <v>407</v>
       </c>
-      <c r="Q92" s="4"/>
-      <c r="R92" s="4"/>
-      <c r="S92" s="4" t="s">
+      <c r="S92" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="T92" s="13" t="s">
+      <c r="T92" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="U92" s="12">
+      <c r="U92" s="24">
         <v>27</v>
       </c>
-      <c r="V92" s="4">
-        <v>1</v>
-      </c>
-      <c r="W92" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X92" s="4"/>
-      <c r="Y92" s="16"/>
-      <c r="Z92" s="4"/>
-      <c r="AA92" s="4" t="s">
+      <c r="V92" s="22">
+        <v>1</v>
+      </c>
+      <c r="W92" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y92" s="25"/>
+      <c r="AA92" s="22" t="s">
         <v>818</v>
       </c>
     </row>
@@ -23380,57 +23382,60 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:27" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A118" s="4" t="s">
+    <row r="118" spans="1:27" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A118" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C118" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D118" s="4" t="s">
+      <c r="D118" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="H118" s="4" t="s">
+      <c r="H118" s="22" t="s">
         <v>936</v>
       </c>
-      <c r="I118" s="13" t="s">
+      <c r="I118" s="23" t="s">
         <v>937</v>
       </c>
-      <c r="K118" s="4">
+      <c r="K118" s="22">
         <v>13</v>
       </c>
-      <c r="L118" s="4" t="s">
+      <c r="L118" s="22" t="s">
         <v>1026</v>
       </c>
-      <c r="M118" s="4" t="s">
+      <c r="M118" s="22" t="s">
         <v>833</v>
       </c>
-      <c r="N118" s="4" t="s">
+      <c r="N118" s="22" t="s">
         <v>1235</v>
       </c>
-      <c r="O118" s="4">
+      <c r="O118" s="22">
         <v>6</v>
       </c>
-      <c r="P118" s="4" t="s">
+      <c r="P118" s="22" t="s">
         <v>1130</v>
       </c>
-      <c r="S118" s="4" t="s">
+      <c r="S118" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="T118" s="13" t="s">
+      <c r="T118" s="23" t="s">
         <v>1276</v>
       </c>
-      <c r="U118" s="12">
+      <c r="U118" s="24">
         <v>768</v>
       </c>
-      <c r="V118" s="4">
-        <v>1</v>
-      </c>
-      <c r="W118" s="4" t="s">
-        <v>257</v>
+      <c r="V118" s="22">
+        <v>1</v>
+      </c>
+      <c r="W118" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA118" s="22" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="119" spans="1:27" x14ac:dyDescent="0.25">
@@ -23446,7 +23451,9 @@
       <c r="D119" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E119" s="3"/>
+      <c r="E119" s="3" t="s">
+        <v>1303</v>
+      </c>
       <c r="F119" s="3"/>
       <c r="G119" s="3"/>
       <c r="H119" s="3" t="s">
@@ -23488,8 +23495,12 @@
         <v>257</v>
       </c>
       <c r="X119" s="3"/>
-      <c r="Y119" s="3"/>
-      <c r="Z119" s="3"/>
+      <c r="Y119" s="15">
+        <v>45327</v>
+      </c>
+      <c r="Z119" s="3">
+        <v>26</v>
+      </c>
       <c r="AA119" s="3"/>
     </row>
     <row r="120" spans="1:27" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -23545,55 +23556,58 @@
         <v>257</v>
       </c>
     </row>
-    <row r="121" spans="1:27" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
+    <row r="121" spans="1:27" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="B121" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="C121" s="3" t="s">
+      <c r="C121" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="22" t="s">
         <v>445</v>
       </c>
-      <c r="H121" s="3" t="s">
+      <c r="H121" s="22" t="s">
         <v>433</v>
       </c>
-      <c r="I121" s="7"/>
-      <c r="K121" s="3">
+      <c r="I121" s="23"/>
+      <c r="K121" s="22">
         <v>17.3</v>
       </c>
-      <c r="L121" s="3" t="s">
+      <c r="L121" s="22" t="s">
         <v>977</v>
       </c>
-      <c r="M121" s="3" t="s">
+      <c r="M121" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="N121" s="3" t="s">
+      <c r="N121" s="22" t="s">
         <v>1145</v>
       </c>
-      <c r="O121" s="3">
+      <c r="O121" s="22">
         <v>6</v>
       </c>
-      <c r="P121" s="3" t="s">
+      <c r="P121" s="22" t="s">
         <v>1132</v>
       </c>
-      <c r="S121" s="3" t="s">
+      <c r="S121" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="T121" s="7" t="s">
+      <c r="T121" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="U121" s="10">
+      <c r="U121" s="24">
         <v>786</v>
       </c>
-      <c r="V121" s="3">
-        <v>1</v>
-      </c>
-      <c r="W121" s="3" t="s">
-        <v>257</v>
+      <c r="V121" s="22">
+        <v>1</v>
+      </c>
+      <c r="W121" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA121" s="22" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="122" spans="1:27" s="22" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -23649,68 +23663,59 @@
         <v>886</v>
       </c>
     </row>
-    <row r="123" spans="1:27" ht="45" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
+    <row r="123" spans="1:27" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="C123" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="D123" s="4" t="s">
+      <c r="D123" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="E123" s="4"/>
-      <c r="F123" s="4"/>
-      <c r="G123" s="4"/>
-      <c r="H123" s="4" t="s">
+      <c r="H123" s="22" t="s">
         <v>941</v>
       </c>
-      <c r="I123" s="13" t="s">
+      <c r="I123" s="23" t="s">
         <v>942</v>
       </c>
-      <c r="J123" s="4"/>
-      <c r="K123" s="4">
+      <c r="K123" s="22">
         <v>12.3</v>
       </c>
-      <c r="L123" s="4" t="s">
+      <c r="L123" s="22" t="s">
         <v>977</v>
       </c>
-      <c r="M123" s="4" t="s">
+      <c r="M123" s="22" t="s">
         <v>828</v>
       </c>
-      <c r="N123" s="4" t="s">
+      <c r="N123" s="22" t="s">
         <v>1145</v>
       </c>
-      <c r="O123" s="4">
+      <c r="O123" s="22">
         <v>4</v>
       </c>
-      <c r="P123" s="4" t="s">
+      <c r="P123" s="22" t="s">
         <v>1133</v>
       </c>
-      <c r="Q123" s="4"/>
-      <c r="R123" s="4"/>
-      <c r="S123" s="4" t="s">
+      <c r="S123" s="22" t="s">
         <v>1256</v>
       </c>
-      <c r="T123" s="13" t="s">
+      <c r="T123" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="U123" s="12">
+      <c r="U123" s="24">
         <v>114</v>
       </c>
-      <c r="V123" s="4">
-        <v>1</v>
-      </c>
-      <c r="W123" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="X123" s="4"/>
-      <c r="Y123" s="4"/>
-      <c r="Z123" s="4"/>
-      <c r="AA123" s="4" t="s">
+      <c r="V123" s="22">
+        <v>1</v>
+      </c>
+      <c r="W123" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="AA123" s="22" t="s">
         <v>886</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add invaded range to range size estimates
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/263374_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\6817706_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{DCCF6899-72E0-4DD8-84E7-ADE619EF62B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49C62267-A199-4D50-ADB6-8AD9B48EF772}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EDB065-C390-45AF-8A64-8A14EFAA3245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -16125,9 +16125,9 @@
   <dimension ref="A1:AA132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
+      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
finish life cycle habit covariate
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\788000_2_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/197332_2_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A9EE8E-2DD4-49D5-83E4-04A9A718AFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{B4A9EE8E-2DD4-49D5-83E4-04A9A718AFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAF4EDDC-247C-4304-979C-7E8428602819}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4017" uniqueCount="1374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4131" uniqueCount="1433">
   <si>
     <t>Species</t>
   </si>
@@ -4159,6 +4159,183 @@
   </si>
   <si>
     <t>https://eol.org/pages/487229</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/468144</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0107781</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/703664</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/486498</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3732/ajb.1400297</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/633316</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/582270</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1154718</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/703659</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s10682-006-0019-7</t>
+  </si>
+  <si>
+    <t>WGS; paper links to 38 genotypes in total, but only mentions 34 newly genotyped lines. I labeled it as a perennial, but it also has annual populations</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115038</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/584304</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1116073</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/596454</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/581050</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/579181</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115582</t>
+  </si>
+  <si>
+    <t>Rice Knowledge Bank, Wild Rice Taxonomy, http://www.knowledgebank.irri.org/images/docs/wild-rice-taxonomy.pdf, accessed 2024-02-20</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115583</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115584</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s00122-016-2745-8</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115470</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115098</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1114492</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1114474</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/594796</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/645324</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1135088</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1276830</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/301091</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/231737</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/631649</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1151479</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1151323</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1371/journal.pone.0177389</t>
+  </si>
+  <si>
+    <t>maybe works. Can't find a solid publication demonstrating ploidy, but the pop gen paper cited here seems to assume diploid genetics. Can't find source for life cycle habit, but it's probably perennial because most rhodendrons are perennial</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/2872067</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115159</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/484896</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1114673</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1114660</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/392557</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/47134785</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/47134908</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115166</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/582002</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1007/s11051-014-2774-7</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/483846</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/2886389</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/583698</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1127948</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/655074</t>
+  </si>
+  <si>
+    <t>Vikram, Nalabolu, and Narayan Chandra Sarkar. "Rice bean (Vigna umbellata)-A potential legume under adverse conditions." International Journal of Bio-resource and Stress Management 13.9 (2022): 928-934.</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/655178</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/582304</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpls.2021.730737</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/582338</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/52189015</t>
   </si>
 </sst>
 </file>
@@ -16334,10 +16511,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9A1616-AAC6-4433-A869-98443D18E34E}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20412,6 +20589,12 @@
       <c r="D61" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F61" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>1374</v>
+      </c>
       <c r="H61" s="3" t="s">
         <v>872</v>
       </c>
@@ -20529,6 +20712,12 @@
       <c r="D63" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F63" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>1375</v>
+      </c>
       <c r="H63" s="3" t="s">
         <v>90</v>
       </c>
@@ -20593,7 +20782,7 @@
         <v>445</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>447</v>
+        <v>1082</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>1084</v>
@@ -20733,6 +20922,12 @@
       <c r="D66" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="F66" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>1376</v>
+      </c>
       <c r="H66" s="3" t="s">
         <v>797</v>
       </c>
@@ -20791,8 +20986,12 @@
         <v>455</v>
       </c>
       <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
+      <c r="F67" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>1377</v>
+      </c>
       <c r="H67" s="3" t="s">
         <v>911</v>
       </c>
@@ -20861,8 +21060,12 @@
         <v>455</v>
       </c>
       <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
+      <c r="F68" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>1378</v>
+      </c>
       <c r="H68" s="3" t="s">
         <v>799</v>
       </c>
@@ -20933,8 +21136,12 @@
         <v>455</v>
       </c>
       <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
+      <c r="F69" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>1379</v>
+      </c>
       <c r="H69" s="3" t="s">
         <v>518</v>
       </c>
@@ -20999,8 +21206,12 @@
         <v>455</v>
       </c>
       <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
+      <c r="F70" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>1380</v>
+      </c>
       <c r="H70" s="3" t="s">
         <v>801</v>
       </c>
@@ -21065,8 +21276,12 @@
         <v>445</v>
       </c>
       <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
+      <c r="F71" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>1381</v>
+      </c>
       <c r="H71" s="3" t="s">
         <v>802</v>
       </c>
@@ -21130,6 +21345,12 @@
       <c r="D72" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F72" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>1382</v>
+      </c>
       <c r="H72" s="3" t="s">
         <v>803</v>
       </c>
@@ -21176,7 +21397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>19</v>
       </c>
@@ -21190,8 +21411,12 @@
         <v>445</v>
       </c>
       <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
+      <c r="F73" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>1383</v>
+      </c>
       <c r="H73" s="3" t="s">
         <v>805</v>
       </c>
@@ -21224,7 +21449,7 @@
       </c>
       <c r="T73" s="3"/>
       <c r="U73" s="7" t="s">
-        <v>269</v>
+        <v>1384</v>
       </c>
       <c r="V73" s="10">
         <v>38</v>
@@ -21257,6 +21482,12 @@
       <c r="D74" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F74" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>1385</v>
+      </c>
       <c r="H74" s="3" t="s">
         <v>913</v>
       </c>
@@ -21318,8 +21549,12 @@
         <v>455</v>
       </c>
       <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
+      <c r="F75" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>1386</v>
+      </c>
       <c r="H75" s="3" t="s">
         <v>875</v>
       </c>
@@ -21386,8 +21621,12 @@
         <v>445</v>
       </c>
       <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
+      <c r="F76" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>1387</v>
+      </c>
       <c r="H76" s="3" t="s">
         <v>809</v>
       </c>
@@ -21458,8 +21697,12 @@
         <v>455</v>
       </c>
       <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
+      <c r="F77" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>1388</v>
+      </c>
       <c r="H77" s="3" t="s">
         <v>811</v>
       </c>
@@ -21529,6 +21772,12 @@
       <c r="D78" s="3" t="s">
         <v>685</v>
       </c>
+      <c r="F78" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>1389</v>
+      </c>
       <c r="H78" s="3" t="s">
         <v>776</v>
       </c>
@@ -21592,6 +21841,12 @@
       <c r="D79" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F79" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>1390</v>
+      </c>
       <c r="H79" s="3" t="s">
         <v>813</v>
       </c>
@@ -21649,6 +21904,12 @@
       <c r="D80" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="F80" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>1391</v>
+      </c>
       <c r="H80" s="3" t="s">
         <v>375</v>
       </c>
@@ -21703,6 +21964,12 @@
       <c r="D81" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="F81" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>1392</v>
+      </c>
       <c r="H81" s="3" t="s">
         <v>379</v>
       </c>
@@ -21757,6 +22024,12 @@
       <c r="C82" s="3" t="s">
         <v>384</v>
       </c>
+      <c r="F82" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>1393</v>
+      </c>
       <c r="H82" s="3" t="s">
         <v>382</v>
       </c>
@@ -21817,6 +22090,12 @@
       <c r="D83" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="F83" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>1394</v>
+      </c>
       <c r="I83" s="7"/>
       <c r="K83" s="3">
         <v>0.8</v>
@@ -21870,8 +22149,12 @@
         <v>317</v>
       </c>
       <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
+      <c r="F84" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>1395</v>
+      </c>
       <c r="H84" s="3" t="s">
         <v>393</v>
       </c>
@@ -21938,8 +22221,12 @@
         <v>317</v>
       </c>
       <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
+      <c r="F85" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>1396</v>
+      </c>
       <c r="H85" s="3" t="s">
         <v>397</v>
       </c>
@@ -22007,6 +22294,12 @@
       <c r="D86" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F86" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>1397</v>
+      </c>
       <c r="H86" s="3" t="s">
         <v>915</v>
       </c>
@@ -22061,8 +22354,12 @@
         <v>445</v>
       </c>
       <c r="E87" s="4"/>
-      <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
+      <c r="F87" s="4" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>1398</v>
+      </c>
       <c r="H87" s="4" t="s">
         <v>133</v>
       </c>
@@ -22128,6 +22425,12 @@
       <c r="D88" s="4" t="s">
         <v>445</v>
       </c>
+      <c r="F88" s="4" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>1399</v>
+      </c>
       <c r="H88" s="4" t="s">
         <v>917</v>
       </c>
@@ -22190,6 +22493,12 @@
       <c r="D89" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="F89" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>1400</v>
+      </c>
       <c r="H89" s="3" t="s">
         <v>815</v>
       </c>
@@ -22251,8 +22560,12 @@
         <v>317</v>
       </c>
       <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
+      <c r="F90" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>1401</v>
+      </c>
       <c r="H90" s="3" t="s">
         <v>919</v>
       </c>
@@ -22316,6 +22629,12 @@
       <c r="D91" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="F91" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>1402</v>
+      </c>
       <c r="H91" s="3" t="s">
         <v>878</v>
       </c>
@@ -22429,7 +22748,7 @@
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3" t="s">
-        <v>1108</v>
+        <v>1319</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>1106</v>
@@ -22498,8 +22817,12 @@
         <v>445</v>
       </c>
       <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
+      <c r="F94" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>1403</v>
+      </c>
       <c r="H94" s="3" t="s">
         <v>51</v>
       </c>
@@ -22570,8 +22893,12 @@
         <v>455</v>
       </c>
       <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
+      <c r="F95" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>1404</v>
+      </c>
       <c r="H95" s="3" t="s">
         <v>921</v>
       </c>
@@ -22638,8 +22965,12 @@
         <v>317</v>
       </c>
       <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
+      <c r="F96" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>1405</v>
+      </c>
       <c r="H96" s="3" t="s">
         <v>409</v>
       </c>
@@ -22706,8 +23037,12 @@
         <v>445</v>
       </c>
       <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
+      <c r="F97" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>1406</v>
+      </c>
       <c r="H97" s="3" t="s">
         <v>925</v>
       </c>
@@ -22770,6 +23105,12 @@
       <c r="D98" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="F98" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>1407</v>
+      </c>
       <c r="H98" s="3" t="s">
         <v>417</v>
       </c>
@@ -22828,6 +23169,12 @@
       </c>
       <c r="D99" s="3" t="s">
         <v>455</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>1408</v>
       </c>
       <c r="H99" s="3" t="s">
         <v>926</v>
@@ -22939,7 +23286,7 @@
       </c>
       <c r="AB100" s="3"/>
     </row>
-    <row r="101" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:28" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>545</v>
       </c>
@@ -22953,8 +23300,12 @@
         <v>455</v>
       </c>
       <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
+      <c r="F101" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>1409</v>
+      </c>
       <c r="H101" s="3" t="s">
         <v>545</v>
       </c>
@@ -22991,7 +23342,7 @@
       </c>
       <c r="T101" s="3"/>
       <c r="U101" s="7" t="s">
-        <v>1115</v>
+        <v>1410</v>
       </c>
       <c r="V101" s="10">
         <v>32</v>
@@ -23024,6 +23375,12 @@
       <c r="D102" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="F102" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>1411</v>
+      </c>
       <c r="H102" s="3" t="s">
         <v>847</v>
       </c>
@@ -23084,8 +23441,12 @@
         <v>317</v>
       </c>
       <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
+      <c r="F103" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>1412</v>
+      </c>
       <c r="H103" s="4" t="s">
         <v>928</v>
       </c>
@@ -23148,8 +23509,12 @@
         <v>317</v>
       </c>
       <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
+      <c r="F104" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>1413</v>
+      </c>
       <c r="H104" s="3" t="s">
         <v>929</v>
       </c>
@@ -23215,6 +23580,12 @@
       <c r="D105" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F105" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>1414</v>
+      </c>
       <c r="H105" s="3" t="s">
         <v>931</v>
       </c>
@@ -23272,6 +23643,12 @@
       <c r="D106" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F106" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>1415</v>
+      </c>
       <c r="H106" s="3" t="s">
         <v>132</v>
       </c>
@@ -23384,6 +23761,12 @@
       <c r="D108" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F108" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>1416</v>
+      </c>
       <c r="H108" s="3" t="s">
         <v>555</v>
       </c>
@@ -23502,8 +23885,12 @@
         <v>685</v>
       </c>
       <c r="E110" s="4"/>
-      <c r="F110" s="4"/>
-      <c r="G110" s="4"/>
+      <c r="F110" s="4" t="s">
+        <v>1146</v>
+      </c>
+      <c r="G110" s="4" t="s">
+        <v>1417</v>
+      </c>
       <c r="H110" s="4"/>
       <c r="I110" s="13"/>
       <c r="J110" s="4"/>
@@ -23562,8 +23949,12 @@
         <v>455</v>
       </c>
       <c r="E111" s="3"/>
-      <c r="F111" s="3"/>
-      <c r="G111" s="3"/>
+      <c r="F111" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>1418</v>
+      </c>
       <c r="H111" s="3" t="s">
         <v>556</v>
       </c>
@@ -23656,8 +24047,12 @@
         <v>445</v>
       </c>
       <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
-      <c r="G113" s="3"/>
+      <c r="F113" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>1419</v>
+      </c>
       <c r="H113" s="3" t="s">
         <v>932</v>
       </c>
@@ -23720,8 +24115,12 @@
         <v>445</v>
       </c>
       <c r="E114" s="3"/>
-      <c r="F114" s="3"/>
-      <c r="G114" s="3"/>
+      <c r="F114" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>1420</v>
+      </c>
       <c r="H114" s="3" t="s">
         <v>934</v>
       </c>
@@ -23787,6 +24186,12 @@
       <c r="D115" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F115" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>1421</v>
+      </c>
       <c r="H115" s="3" t="s">
         <v>123</v>
       </c>
@@ -23844,6 +24249,12 @@
       <c r="D116" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="F116" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>1422</v>
+      </c>
       <c r="H116" s="3" t="s">
         <v>558</v>
       </c>
@@ -23901,6 +24312,12 @@
       <c r="D117" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="F117" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>1423</v>
+      </c>
       <c r="H117" s="3" t="s">
         <v>562</v>
       </c>
@@ -24017,8 +24434,12 @@
       <c r="E119" s="3" t="s">
         <v>1303</v>
       </c>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
+      <c r="F119" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>1424</v>
+      </c>
       <c r="H119" s="3" t="s">
         <v>564</v>
       </c>
@@ -24296,6 +24717,12 @@
       <c r="D124" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="F124" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>1425</v>
+      </c>
       <c r="H124" s="3" t="s">
         <v>882</v>
       </c>
@@ -24362,8 +24789,12 @@
         <v>317</v>
       </c>
       <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
-      <c r="G125" s="3"/>
+      <c r="F125" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>1426</v>
+      </c>
       <c r="H125" s="3" t="s">
         <v>944</v>
       </c>
@@ -24428,8 +24859,12 @@
         <v>455</v>
       </c>
       <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
-      <c r="G126" s="3"/>
+      <c r="F126" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>1427</v>
+      </c>
       <c r="H126" s="3" t="s">
         <v>946</v>
       </c>
@@ -24493,6 +24928,12 @@
       <c r="D127" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="F127" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G127" s="3" t="s">
+        <v>1428</v>
+      </c>
       <c r="H127" s="3" t="s">
         <v>853</v>
       </c>
@@ -24553,8 +24994,12 @@
         <v>445</v>
       </c>
       <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
-      <c r="G128" s="3"/>
+      <c r="F128" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>1429</v>
+      </c>
       <c r="H128" s="3" t="s">
         <v>884</v>
       </c>
@@ -24620,6 +25065,12 @@
       <c r="D129" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="F129" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>1430</v>
+      </c>
       <c r="I129" s="7"/>
       <c r="K129" s="3">
         <v>0.44780163599181999</v>
@@ -24680,6 +25131,12 @@
       <c r="D130" s="4" t="s">
         <v>445</v>
       </c>
+      <c r="F130" s="4" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G130" s="4" t="s">
+        <v>1432</v>
+      </c>
       <c r="H130" s="13" t="s">
         <v>947</v>
       </c>
@@ -24804,6 +25261,12 @@
       </c>
       <c r="D132" s="3" t="s">
         <v>455</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>1319</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>1431</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>950</v>

</xml_diff>

<commit_message>
clean up readme, update zea mays docs
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\1836112_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\722618_2_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A52863-35FD-4C21-AB36-82A08BAA317D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CC715A-58FD-40D2-9C5E-3DFBCE73474A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4148" uniqueCount="1453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="1455">
   <si>
     <t>Species</t>
   </si>
@@ -3774,9 +3774,6 @@
     <t>doi:10.1038/nbt.3096 ; https://doi.org/10.1016/j.molp.2020.01.014 ; https://doi.org/10.1101/2022.03.24.485586</t>
   </si>
   <si>
-    <t>PRJNA260788; PRJNA283986; PRJNA389800; PRJNA399729</t>
-  </si>
-  <si>
     <t>Brassica oleracea</t>
   </si>
   <si>
@@ -4396,6 +4393,15 @@
   </si>
   <si>
     <t>Encyclopedia of life: https://eol.org/pages/584172</t>
+  </si>
+  <si>
+    <t>PRJNA260788; PRJNA389800; PRJNA399729</t>
+  </si>
+  <si>
+    <t>APGv4; RefGen_V4</t>
+  </si>
+  <si>
+    <t>I removed the Mt and Pt assemblies from the pipeline</t>
   </si>
 </sst>
 </file>
@@ -16483,37 +16489,37 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
   </sheetData>
@@ -16576,10 +16582,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9A1616-AAC6-4433-A869-98443D18E34E}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="T26" sqref="T26"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16604,7 +16610,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -16613,7 +16619,7 @@
         <v>316</v>
       </c>
       <c r="E1" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="F1" t="s">
         <v>446</v>
@@ -16649,16 +16655,16 @@
         <v>866</v>
       </c>
       <c r="Q1" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="R1" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="S1" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="T1" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>66</v>
@@ -16700,10 +16706,10 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>773</v>
@@ -16731,10 +16737,10 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>1038</v>
@@ -16862,13 +16868,13 @@
         <v>1.026</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>750</v>
@@ -16908,10 +16914,10 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>1319</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>1320</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>751</v>
@@ -16939,13 +16945,13 @@
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>139</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="V5" s="10">
         <v>87</v>
@@ -16981,10 +16987,10 @@
         <v>445</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>26</v>
@@ -17000,7 +17006,7 @@
         <v>850</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="O6" s="3">
         <v>2</v>
@@ -17012,7 +17018,7 @@
         <v>874</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="U6" s="7"/>
       <c r="V6" s="10">
@@ -17047,10 +17053,10 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>16</v>
@@ -17079,7 +17085,7 @@
         <v>874</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="U7" s="7"/>
       <c r="V7" s="10">
@@ -17119,7 +17125,7 @@
         <v>1082</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>460</v>
@@ -17187,7 +17193,7 @@
         <v>1082</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>22</v>
@@ -17218,7 +17224,7 @@
         <v>874</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="10">
@@ -17255,10 +17261,10 @@
         <v>317</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>160</v>
@@ -17286,7 +17292,7 @@
         <v>874</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="U10" s="7"/>
       <c r="V10" s="10">
@@ -17308,7 +17314,7 @@
         <v>3</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -17325,10 +17331,10 @@
         <v>455</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>461</v>
@@ -17356,7 +17362,7 @@
         <v>874</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="U11" s="7" t="s">
         <v>575</v>
@@ -17395,7 +17401,7 @@
         <v>1082</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="I12" s="7"/>
       <c r="K12" s="3">
@@ -17420,13 +17426,13 @@
         <v>0.3861</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="U12" s="7" t="s">
         <v>617</v>
@@ -17447,7 +17453,7 @@
         <v>3</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.25">
@@ -17468,7 +17474,7 @@
         <v>1082</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>775</v>
@@ -17496,13 +17502,13 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="V13" s="10">
         <v>320</v>
@@ -17523,7 +17529,7 @@
         <v>10</v>
       </c>
       <c r="AB13" s="3" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="45" x14ac:dyDescent="0.25">
@@ -17544,7 +17550,7 @@
         <v>1082</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>774</v>
@@ -17573,16 +17579,16 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="S14" s="5" t="s">
         <v>874</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="V14" s="10">
         <v>3</v>
@@ -17621,7 +17627,7 @@
         <v>1082</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>753</v>
@@ -17649,13 +17655,13 @@
         <v>1.863</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="U15" s="7" t="s">
         <v>754</v>
@@ -17679,7 +17685,7 @@
         <v>3</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="30" x14ac:dyDescent="0.25">
@@ -17700,7 +17706,7 @@
         <v>1082</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>752</v>
@@ -17728,13 +17734,13 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="U16" s="7" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="V16" s="10">
         <v>597</v>
@@ -17769,10 +17775,10 @@
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="17" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>105</v>
@@ -17803,7 +17809,7 @@
         <v>874</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="U17" s="7" t="s">
         <v>715</v>
@@ -17875,7 +17881,7 @@
         <v>874</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="U18" s="7" t="s">
         <v>281</v>
@@ -17937,7 +17943,7 @@
         <v>874</v>
       </c>
       <c r="U19" s="23" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="V19" s="24">
         <v>178</v>
@@ -17967,7 +17973,7 @@
         <v>1082</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>807</v>
@@ -17992,10 +17998,10 @@
         <v>1050</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="U20" s="7"/>
       <c r="V20" s="10">
@@ -18032,7 +18038,7 @@
         <v>1082</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>808</v>
@@ -18060,13 +18066,13 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="V21" s="10">
         <v>1007</v>
@@ -18085,7 +18091,7 @@
         <v>19</v>
       </c>
       <c r="AB21" s="3" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="22" spans="1:28" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -18124,7 +18130,7 @@
         <v>1052</v>
       </c>
       <c r="S22" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U22" s="23" t="s">
         <v>783</v>
@@ -18142,7 +18148,7 @@
     </row>
     <row r="23" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>158</v>
@@ -18155,10 +18161,10 @@
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>684</v>
@@ -18188,13 +18194,13 @@
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="V23" s="10">
         <v>119</v>
@@ -18232,7 +18238,7 @@
         <v>1082</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>840</v>
@@ -18262,10 +18268,10 @@
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="U24" s="7" t="s">
         <v>159</v>
@@ -18302,17 +18308,17 @@
         <v>455</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="I25" s="7"/>
       <c r="K25" s="3">
         <v>0.87321063394682996</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>833</v>
@@ -18327,10 +18333,10 @@
         <v>582</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="U25" s="7"/>
       <c r="V25" s="10">
@@ -18363,10 +18369,10 @@
         <v>455</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>856</v>
@@ -18391,7 +18397,7 @@
         <v>867</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U26" s="7" t="s">
         <v>583</v>
@@ -18429,7 +18435,7 @@
         <v>1082</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>756</v>
@@ -18439,7 +18445,7 @@
         <v>0.76687116600000005</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>828</v>
@@ -18454,7 +18460,7 @@
         <v>1054</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>324</v>
@@ -18495,10 +18501,10 @@
         <v>455</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>842</v>
@@ -18525,7 +18531,7 @@
         <v>1055</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U28" s="7" t="s">
         <v>622</v>
@@ -18563,7 +18569,7 @@
         <v>1082</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>325</v>
@@ -18590,7 +18596,7 @@
         <v>1056</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U29" s="7" t="s">
         <v>328</v>
@@ -18629,7 +18635,7 @@
         <v>1082</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>59</v>
@@ -18658,7 +18664,7 @@
         <v>0.67</v>
       </c>
       <c r="R30" s="5" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="S30" s="5" t="s">
         <v>874</v>
@@ -18702,7 +18708,7 @@
         <v>1082</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>50</v>
@@ -18764,7 +18770,7 @@
         <v>1146</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>890</v>
@@ -18794,11 +18800,11 @@
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
       <c r="S32" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T32" s="3"/>
       <c r="U32" s="7" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="V32" s="10">
         <v>8028</v>
@@ -18832,7 +18838,7 @@
         <v>455</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>1059</v>
@@ -18862,7 +18868,7 @@
         <v>1059</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U33" s="7" t="s">
         <v>583</v>
@@ -18900,7 +18906,7 @@
         <v>1082</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>858</v>
@@ -18930,10 +18936,10 @@
         <v>0.80308799999999991</v>
       </c>
       <c r="R34" s="5" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="S34" s="5" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T34" s="5"/>
       <c r="U34" s="7" t="s">
@@ -18969,19 +18975,19 @@
         <v>445</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>1435</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>1436</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>1437</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3">
@@ -19005,7 +19011,7 @@
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
       <c r="S35" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T35" s="3"/>
       <c r="U35" s="7" t="s">
@@ -19043,7 +19049,7 @@
         <v>1082</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>859</v>
@@ -19073,7 +19079,7 @@
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T36" s="3"/>
       <c r="U36" s="7" t="s">
@@ -19111,10 +19117,10 @@
         <v>455</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>791</v>
@@ -19141,7 +19147,7 @@
         <v>1061</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U37" s="7" t="s">
         <v>583</v>
@@ -19176,10 +19182,10 @@
         <v>317</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>893</v>
@@ -19206,7 +19212,7 @@
         <v>1061</v>
       </c>
       <c r="S38" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U38" s="7" t="s">
         <v>341</v>
@@ -19241,26 +19247,26 @@
         <v>445</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="I39" s="7"/>
       <c r="K39" s="3">
         <v>0.49</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>833</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="O39" s="3">
         <v>2</v>
@@ -19269,7 +19275,7 @@
         <v>954</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U39" s="7" t="s">
         <v>953</v>
@@ -19297,10 +19303,10 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>861</v>
@@ -19330,7 +19336,7 @@
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T40" s="3"/>
       <c r="U40" s="7" t="s">
@@ -19371,7 +19377,7 @@
         <v>1082</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>894</v>
@@ -19398,7 +19404,7 @@
         <v>1062</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U41" s="7"/>
       <c r="V41" s="10">
@@ -19435,7 +19441,7 @@
         <v>1082</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>897</v>
@@ -19465,7 +19471,7 @@
       <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
       <c r="S42" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T42" s="3"/>
       <c r="U42" s="7" t="s">
@@ -19507,7 +19513,7 @@
         <v>1082</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>844</v>
@@ -19538,10 +19544,10 @@
         <v>0.34289999999999998</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T43" s="3"/>
       <c r="U43" s="7" t="s">
@@ -19583,7 +19589,7 @@
         <v>1082</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>788</v>
@@ -19611,7 +19617,7 @@
       <c r="Q44" s="3"/>
       <c r="R44" s="3"/>
       <c r="S44" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T44" s="3"/>
       <c r="U44" s="7" t="s">
@@ -19653,7 +19659,7 @@
         <v>1082</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>846</v>
@@ -19684,10 +19690,10 @@
         <v>0.97599999999999998</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T45" s="3"/>
       <c r="U45" s="7"/>
@@ -19723,10 +19729,10 @@
         <v>445</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>898</v>
@@ -19753,7 +19759,7 @@
         <v>1066</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U46" s="7" t="s">
         <v>145</v>
@@ -19788,10 +19794,10 @@
         <v>317</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>784</v>
@@ -19822,10 +19828,10 @@
         <v>1.9245000000000001</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="S47" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U47" s="7" t="s">
         <v>635</v>
@@ -19860,10 +19866,10 @@
         <v>455</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>785</v>
@@ -19888,7 +19894,7 @@
         <v>1068</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U48" s="7" t="s">
         <v>590</v>
@@ -19923,10 +19929,10 @@
         <v>455</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>786</v>
@@ -19951,7 +19957,7 @@
         <v>1069</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>585</v>
@@ -20005,7 +20011,7 @@
         <v>1070</v>
       </c>
       <c r="S50" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U50" s="23" t="s">
         <v>585</v>
@@ -20040,10 +20046,10 @@
         <v>317</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>777</v>
@@ -20068,7 +20074,7 @@
         <v>1071</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U51" s="7" t="s">
         <v>361</v>
@@ -20112,13 +20118,13 @@
         <v>1082</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="I52" s="7" t="s">
         <v>1438</v>
-      </c>
-      <c r="I52" s="7" t="s">
-        <v>1439</v>
       </c>
       <c r="K52" s="3">
         <v>1.1299999999999999</v>
@@ -20139,7 +20145,7 @@
         <v>1072</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U52" s="7" t="s">
         <v>290</v>
@@ -20172,7 +20178,7 @@
         <v>1082</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>88</v>
@@ -20201,7 +20207,7 @@
         <v>1.12375</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="S53" s="8" t="s">
         <v>874</v>
@@ -20238,10 +20244,10 @@
         <v>455</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>496</v>
@@ -20268,7 +20274,7 @@
         <v>870</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U54" s="7" t="s">
         <v>583</v>
@@ -20304,16 +20310,16 @@
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>111</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3">
@@ -20337,7 +20343,7 @@
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
       <c r="S55" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T55" s="3"/>
       <c r="U55" s="7"/>
@@ -20374,10 +20380,10 @@
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>903</v>
@@ -20407,7 +20413,7 @@
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
       <c r="S56" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T56" s="3"/>
       <c r="U56" s="7"/>
@@ -20446,7 +20452,7 @@
         <v>1082</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>796</v>
@@ -20471,7 +20477,7 @@
         <v>1075</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U57" s="7" t="s">
         <v>145</v>
@@ -20506,10 +20512,10 @@
         <v>455</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>508</v>
@@ -20519,7 +20525,7 @@
         <v>1.3</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="M58" s="3" t="s">
         <v>833</v>
@@ -20569,7 +20575,7 @@
         <v>445</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="H59" s="22" t="s">
         <v>905</v>
@@ -20596,7 +20602,7 @@
         <v>1077</v>
       </c>
       <c r="S59" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U59" s="23"/>
       <c r="V59" s="24">
@@ -20627,10 +20633,10 @@
         <v>317</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>907</v>
@@ -20657,7 +20663,7 @@
         <v>1078</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U60" s="7"/>
       <c r="V60" s="10">
@@ -20693,7 +20699,7 @@
         <v>1082</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>872</v>
@@ -20720,7 +20726,7 @@
         <v>1079</v>
       </c>
       <c r="S61" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>263</v>
@@ -20780,7 +20786,7 @@
         <v>1080</v>
       </c>
       <c r="S62" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U62" s="23" t="s">
         <v>145</v>
@@ -20816,7 +20822,7 @@
         <v>1082</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>90</v>
@@ -20844,7 +20850,7 @@
         <v>0.2495</v>
       </c>
       <c r="R63" s="5" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="S63" s="3" t="s">
         <v>874</v>
@@ -20912,7 +20918,7 @@
         <v>1084</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U64" s="7" t="s">
         <v>303</v>
@@ -20982,7 +20988,7 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="R65" s="5" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="S65" s="3" t="s">
         <v>874</v>
@@ -21026,7 +21032,7 @@
         <v>1082</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>797</v>
@@ -21053,7 +21059,7 @@
         <v>1086</v>
       </c>
       <c r="S66" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U66" s="7"/>
       <c r="V66" s="10">
@@ -21087,10 +21093,10 @@
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>911</v>
@@ -21121,10 +21127,10 @@
         <v>12</v>
       </c>
       <c r="R67" s="5" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T67" s="3"/>
       <c r="U67" s="7"/>
@@ -21161,10 +21167,10 @@
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>799</v>
@@ -21195,10 +21201,10 @@
         <v>3.6</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T68" s="3"/>
       <c r="U68" s="7" t="s">
@@ -21237,10 +21243,10 @@
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>518</v>
@@ -21307,10 +21313,10 @@
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>801</v>
@@ -21338,7 +21344,7 @@
       <c r="Q70" s="3"/>
       <c r="R70" s="3"/>
       <c r="S70" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T70" s="3"/>
       <c r="U70" s="7" t="s">
@@ -21377,10 +21383,10 @@
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>802</v>
@@ -21408,7 +21414,7 @@
       <c r="Q71" s="3"/>
       <c r="R71" s="3"/>
       <c r="S71" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T71" s="3"/>
       <c r="U71" s="7" t="s">
@@ -21449,7 +21455,7 @@
         <v>1082</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>803</v>
@@ -21515,7 +21521,7 @@
         <v>1146</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>805</v>
@@ -21549,7 +21555,7 @@
       </c>
       <c r="T73" s="3"/>
       <c r="U73" s="7" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="V73" s="10">
         <v>38</v>
@@ -21583,10 +21589,10 @@
         <v>445</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>913</v>
@@ -21613,7 +21619,7 @@
         <v>1094</v>
       </c>
       <c r="S74" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U74" s="7" t="s">
         <v>203</v>
@@ -21634,7 +21640,7 @@
         <v>22</v>
       </c>
       <c r="AB74" s="3" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="75" spans="1:28" ht="60" x14ac:dyDescent="0.25">
@@ -21653,7 +21659,7 @@
         <v>1082</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>875</v>
@@ -21683,7 +21689,7 @@
       <c r="Q75" s="3"/>
       <c r="R75" s="3"/>
       <c r="S75" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T75" s="3"/>
       <c r="U75" s="7" t="s">
@@ -21722,10 +21728,10 @@
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>809</v>
@@ -21756,10 +21762,10 @@
         <v>4.8768000000000002</v>
       </c>
       <c r="R76" s="5" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="S76" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T76" s="3"/>
       <c r="U76" s="7" t="s">
@@ -21798,10 +21804,10 @@
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>811</v>
@@ -21832,10 +21838,10 @@
         <v>0.91439999999999999</v>
       </c>
       <c r="R77" s="5" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="S77" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T77" s="3"/>
       <c r="U77" s="7" t="s">
@@ -21876,7 +21882,7 @@
         <v>1082</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>776</v>
@@ -21901,7 +21907,7 @@
         <v>1098</v>
       </c>
       <c r="S78" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U78" s="7" t="s">
         <v>696</v>
@@ -21942,10 +21948,10 @@
         <v>445</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>813</v>
@@ -21970,7 +21976,7 @@
         <v>206</v>
       </c>
       <c r="S79" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U79" s="7" t="s">
         <v>270</v>
@@ -22008,7 +22014,7 @@
         <v>1082</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>375</v>
@@ -22068,7 +22074,7 @@
         <v>1082</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>379</v>
@@ -22084,7 +22090,7 @@
         <v>833</v>
       </c>
       <c r="N81" s="3" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="O81" s="3">
         <v>2</v>
@@ -22128,7 +22134,7 @@
         <v>1082</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>382</v>
@@ -22158,10 +22164,10 @@
         <v>0.74390000000000001</v>
       </c>
       <c r="R82" s="5" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="S82" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U82" s="7"/>
       <c r="V82" s="10">
@@ -22191,10 +22197,10 @@
         <v>317</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="I83" s="7"/>
       <c r="K83" s="3">
@@ -22253,7 +22259,7 @@
         <v>1082</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>393</v>
@@ -22325,7 +22331,7 @@
         <v>1082</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>397</v>
@@ -22354,7 +22360,7 @@
         <v>0.105</v>
       </c>
       <c r="R85" s="5" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="S85" s="3" t="s">
         <v>874</v>
@@ -22392,16 +22398,16 @@
         <v>4</v>
       </c>
       <c r="D86" s="3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="E86" s="3" t="s">
         <v>1440</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>1441</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>915</v>
@@ -22428,7 +22434,7 @@
         <v>1099</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U86" s="7" t="s">
         <v>271</v>
@@ -22467,10 +22473,10 @@
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>133</v>
@@ -22538,10 +22544,10 @@
         <v>445</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>917</v>
@@ -22568,7 +22574,7 @@
         <v>1103</v>
       </c>
       <c r="S88" s="4" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U88" s="13" t="s">
         <v>272</v>
@@ -22589,7 +22595,7 @@
         <v>17</v>
       </c>
       <c r="AB88" s="4" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="89" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -22609,7 +22615,7 @@
         <v>1082</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>815</v>
@@ -22634,7 +22640,7 @@
         <v>732</v>
       </c>
       <c r="S89" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U89" s="7" t="s">
         <v>402</v>
@@ -22676,7 +22682,7 @@
         <v>1082</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>919</v>
@@ -22706,7 +22712,7 @@
       <c r="Q90" s="3"/>
       <c r="R90" s="3"/>
       <c r="S90" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T90" s="3"/>
       <c r="U90" s="7"/>
@@ -22742,10 +22748,10 @@
         <v>455</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>878</v>
@@ -22772,7 +22778,7 @@
         <v>1105</v>
       </c>
       <c r="S91" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U91" s="7"/>
       <c r="V91" s="10">
@@ -22826,7 +22832,7 @@
         <v>407</v>
       </c>
       <c r="S92" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U92" s="23" t="s">
         <v>408</v>
@@ -22860,7 +22866,7 @@
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>1106</v>
@@ -22930,10 +22936,10 @@
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>51</v>
@@ -22964,10 +22970,10 @@
         <v>41.91</v>
       </c>
       <c r="R94" s="5" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="S94" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T94" s="3"/>
       <c r="U94" s="7" t="s">
@@ -23006,10 +23012,10 @@
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>921</v>
@@ -23039,7 +23045,7 @@
       <c r="Q95" s="3"/>
       <c r="R95" s="3"/>
       <c r="S95" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T95" s="3"/>
       <c r="U95" s="7" t="s">
@@ -23078,10 +23084,10 @@
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>409</v>
@@ -23111,7 +23117,7 @@
       <c r="Q96" s="3"/>
       <c r="R96" s="3"/>
       <c r="S96" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T96" s="3"/>
       <c r="U96" s="7" t="s">
@@ -23150,10 +23156,10 @@
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>925</v>
@@ -23183,7 +23189,7 @@
       <c r="Q97" s="3"/>
       <c r="R97" s="3"/>
       <c r="S97" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T97" s="3"/>
       <c r="U97" s="7" t="s">
@@ -23218,10 +23224,10 @@
         <v>317</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>417</v>
@@ -23283,16 +23289,16 @@
         <v>455</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="I99" s="7"/>
       <c r="K99" s="3">
@@ -23314,10 +23320,10 @@
         <v>1113</v>
       </c>
       <c r="S99" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T99" s="3" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="U99" s="7" t="s">
         <v>583</v>
@@ -23386,7 +23392,7 @@
       <c r="Q100" s="3"/>
       <c r="R100" s="3"/>
       <c r="S100" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T100" s="3"/>
       <c r="U100" s="7" t="s">
@@ -23425,10 +23431,10 @@
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>545</v>
@@ -23459,14 +23465,14 @@
         <v>0.91439999999999999</v>
       </c>
       <c r="R101" s="5" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="S101" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T101" s="3"/>
       <c r="U101" s="7" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="V101" s="10">
         <v>32</v>
@@ -23500,10 +23506,10 @@
         <v>455</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>847</v>
@@ -23569,7 +23575,7 @@
         <v>1082</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="H103" s="4" t="s">
         <v>928</v>
@@ -23599,7 +23605,7 @@
       <c r="Q103" s="4"/>
       <c r="R103" s="4"/>
       <c r="S103" s="4" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T103" s="4"/>
       <c r="U103" s="13" t="s">
@@ -23637,7 +23643,7 @@
         <v>1082</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>929</v>
@@ -23667,7 +23673,7 @@
       <c r="Q104" s="3"/>
       <c r="R104" s="3"/>
       <c r="S104" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T104" s="3"/>
       <c r="U104" s="7" t="s">
@@ -23693,7 +23699,7 @@
     </row>
     <row r="105" spans="1:28" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>214</v>
@@ -23708,7 +23714,7 @@
         <v>1082</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>931</v>
@@ -23733,7 +23739,7 @@
         <v>1119</v>
       </c>
       <c r="S105" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U105" s="7" t="s">
         <v>274</v>
@@ -23771,7 +23777,7 @@
         <v>1082</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>132</v>
@@ -23889,7 +23895,7 @@
         <v>1082</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>555</v>
@@ -23914,7 +23920,7 @@
         <v>1121</v>
       </c>
       <c r="S108" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U108" s="7" t="s">
         <v>159</v>
@@ -23971,7 +23977,7 @@
         <v>1122</v>
       </c>
       <c r="S109" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U109" s="23" t="s">
         <v>687</v>
@@ -24013,7 +24019,7 @@
         <v>1146</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="H110" s="4"/>
       <c r="I110" s="13"/>
@@ -24074,10 +24080,10 @@
       </c>
       <c r="E111" s="3"/>
       <c r="F111" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>556</v>
@@ -24150,7 +24156,7 @@
         <v>1125</v>
       </c>
       <c r="S112" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U112" s="23" t="s">
         <v>222</v>
@@ -24171,13 +24177,13 @@
         <v>445</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>932</v>
@@ -24207,7 +24213,7 @@
       <c r="Q113" s="3"/>
       <c r="R113" s="3"/>
       <c r="S113" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T113" s="3"/>
       <c r="U113" s="7" t="s">
@@ -24233,7 +24239,7 @@
     </row>
     <row r="114" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>229</v>
@@ -24249,7 +24255,7 @@
         <v>1082</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>934</v>
@@ -24279,7 +24285,7 @@
       <c r="Q114" s="3"/>
       <c r="R114" s="3"/>
       <c r="S114" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T114" s="3"/>
       <c r="U114" s="7" t="s">
@@ -24317,10 +24323,10 @@
         <v>445</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>123</v>
@@ -24345,7 +24351,7 @@
         <v>231</v>
       </c>
       <c r="S115" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U115" s="7" t="s">
         <v>278</v>
@@ -24383,7 +24389,7 @@
         <v>1082</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>558</v>
@@ -24443,10 +24449,10 @@
         <v>455</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="H117" s="3" t="s">
         <v>562</v>
@@ -24530,10 +24536,10 @@
         <v>1130</v>
       </c>
       <c r="S118" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U118" s="23" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="V118" s="24">
         <v>768</v>
@@ -24562,13 +24568,13 @@
         <v>455</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>564</v>
@@ -24596,7 +24602,7 @@
       <c r="Q119" s="3"/>
       <c r="R119" s="3"/>
       <c r="S119" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T119" s="3"/>
       <c r="U119" s="7" t="s">
@@ -24656,10 +24662,10 @@
         <v>1131</v>
       </c>
       <c r="S120" s="22" t="s">
+        <v>1255</v>
+      </c>
+      <c r="U120" s="23" t="s">
         <v>1256</v>
-      </c>
-      <c r="U120" s="23" t="s">
-        <v>1257</v>
       </c>
       <c r="V120" s="24">
         <v>672</v>
@@ -24707,7 +24713,7 @@
         <v>1132</v>
       </c>
       <c r="S121" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U121" s="23" t="s">
         <v>233</v>
@@ -24816,7 +24822,7 @@
         <v>1133</v>
       </c>
       <c r="S123" s="22" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U123" s="23" t="s">
         <v>300</v>
@@ -24848,10 +24854,10 @@
         <v>455</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>882</v>
@@ -24881,10 +24887,10 @@
         <v>19.05</v>
       </c>
       <c r="R124" s="5" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="S124" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U124" s="7" t="s">
         <v>603</v>
@@ -24923,7 +24929,7 @@
         <v>1082</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>944</v>
@@ -24953,7 +24959,7 @@
       <c r="Q125" s="3"/>
       <c r="R125" s="3"/>
       <c r="S125" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T125" s="3"/>
       <c r="U125" s="7"/>
@@ -24993,7 +24999,7 @@
         <v>1082</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>946</v>
@@ -25024,10 +25030,10 @@
         <v>1.39</v>
       </c>
       <c r="R126" s="3" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="S126" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T126" s="3"/>
       <c r="U126" s="7" t="s">
@@ -25062,7 +25068,7 @@
         <v>1082</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>853</v>
@@ -25089,7 +25095,7 @@
         <v>1138</v>
       </c>
       <c r="S127" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U127" s="7" t="s">
         <v>444</v>
@@ -25125,10 +25131,10 @@
       </c>
       <c r="E128" s="3"/>
       <c r="F128" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>884</v>
@@ -25158,7 +25164,7 @@
       <c r="Q128" s="3"/>
       <c r="R128" s="3"/>
       <c r="S128" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T128" s="3"/>
       <c r="U128" s="7" t="s">
@@ -25196,10 +25202,10 @@
         <v>455</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="I129" s="7"/>
       <c r="K129" s="3">
@@ -25224,10 +25230,10 @@
         <v>3.25</v>
       </c>
       <c r="R129" s="5" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="S129" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U129" s="7" t="s">
         <v>583</v>
@@ -25248,63 +25254,75 @@
         <v>9</v>
       </c>
     </row>
-    <row r="130" spans="1:28" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A130" s="4" t="s">
+    <row r="130" spans="1:28" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="C130" s="4" t="s">
-        <v>1245</v>
-      </c>
-      <c r="D130" s="4" t="s">
+      <c r="C130" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D130" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="F130" s="4" t="s">
+      <c r="E130" s="3" t="s">
+        <v>1453</v>
+      </c>
+      <c r="F130" s="3" t="s">
         <v>1082</v>
       </c>
-      <c r="G130" s="4" t="s">
-        <v>1431</v>
-      </c>
-      <c r="H130" s="13" t="s">
+      <c r="G130" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="H130" s="7" t="s">
         <v>947</v>
       </c>
-      <c r="I130" s="13" t="s">
+      <c r="I130" s="7" t="s">
         <v>948</v>
       </c>
-      <c r="K130" s="4">
+      <c r="K130" s="3">
         <v>2.7</v>
       </c>
-      <c r="L130" s="4" t="s">
+      <c r="L130" s="3" t="s">
         <v>962</v>
       </c>
-      <c r="M130" s="4" t="s">
+      <c r="M130" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="N130" s="4" t="s">
+      <c r="N130" s="3" t="s">
         <v>1145</v>
       </c>
-      <c r="O130" s="4">
+      <c r="O130" s="3">
         <v>2</v>
       </c>
-      <c r="P130" s="4" t="s">
+      <c r="P130" s="3" t="s">
         <v>1141</v>
       </c>
-      <c r="S130" s="4" t="s">
-        <v>1256</v>
-      </c>
-      <c r="U130" s="13" t="s">
+      <c r="S130" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="U130" s="7" t="s">
         <v>781</v>
       </c>
-      <c r="V130" s="12">
+      <c r="V130" s="10">
         <v>33</v>
       </c>
-      <c r="W130" s="4">
-        <v>1</v>
-      </c>
-      <c r="X130" s="4" t="s">
-        <v>257</v>
+      <c r="W130" s="3">
+        <v>1</v>
+      </c>
+      <c r="X130" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z130" s="15">
+        <v>45376</v>
+      </c>
+      <c r="AA130" s="3">
+        <v>34</v>
+      </c>
+      <c r="AB130" s="3" t="s">
+        <v>1454</v>
       </c>
     </row>
     <row r="131" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -25352,10 +25370,10 @@
         <v>4</v>
       </c>
       <c r="R131" s="3" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="S131" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U131" s="7" t="s">
         <v>603</v>
@@ -25376,7 +25394,7 @@
         <v>17</v>
       </c>
       <c r="AB131" s="3" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="132" spans="1:28" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -25393,10 +25411,10 @@
         <v>455</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>950</v>
@@ -25423,7 +25441,7 @@
         <v>1143</v>
       </c>
       <c r="S132" s="3" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="U132" s="7" t="s">
         <v>583</v>

</xml_diff>

<commit_message>
update wild vs cultivated annotations
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/197128_2_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\723110_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:1_{F6CC715A-58FD-40D2-9C5E-3DFBCE73474A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B91D5BB7-E162-4454-8CAC-A51927BD0DC9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DBB1F4-C4EE-49DE-92AA-BFFC52C80BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4191" uniqueCount="1496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4224" uniqueCount="1529">
   <si>
     <t>Species</t>
   </si>
@@ -4525,6 +4525,105 @@
   </si>
   <si>
     <t>v1; v1.3; PRJNA41163</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/584706</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/584705</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/468106</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/52522464</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/487229</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/468144</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/703189</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/581568</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/47378562</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/703664</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/486498</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/629943</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/633316</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/582270</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1154718/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/703659/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/52199934/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115038/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/584304/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1116073/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/596454/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/581050/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/579181/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115582/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/5824504/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115583/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115584/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115872/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115470/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1115098/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/594796/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/645324/data</t>
+  </si>
+  <si>
+    <t>https://eol.org/pages/1135088/data</t>
   </si>
 </sst>
 </file>
@@ -16705,10 +16804,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9A1616-AAC6-4433-A869-98443D18E34E}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="S58" sqref="S58"/>
+      <selection pane="bottomLeft" activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20569,7 +20668,9 @@
       <c r="S55" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T55" s="3"/>
+      <c r="T55" s="5" t="s">
+        <v>1496</v>
+      </c>
       <c r="U55" s="7"/>
       <c r="V55" s="10">
         <v>336</v>
@@ -20639,7 +20740,9 @@
       <c r="S56" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T56" s="3"/>
+      <c r="T56" s="5" t="s">
+        <v>1497</v>
+      </c>
       <c r="U56" s="7"/>
       <c r="V56" s="10">
         <v>1081</v>
@@ -20703,6 +20806,9 @@
       <c r="S57" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T57" s="5" t="s">
+        <v>1498</v>
+      </c>
       <c r="U57" s="7" t="s">
         <v>145</v>
       </c>
@@ -20766,6 +20872,9 @@
       <c r="S58" s="3" t="s">
         <v>874</v>
       </c>
+      <c r="T58" s="5" t="s">
+        <v>1499</v>
+      </c>
       <c r="U58" s="7" t="s">
         <v>590</v>
       </c>
@@ -20889,6 +20998,9 @@
       <c r="S60" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T60" s="5" t="s">
+        <v>1500</v>
+      </c>
       <c r="U60" s="7"/>
       <c r="V60" s="10">
         <v>550</v>
@@ -20952,6 +21064,9 @@
       <c r="S61" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T61" s="5" t="s">
+        <v>1501</v>
+      </c>
       <c r="U61" s="7" t="s">
         <v>263</v>
       </c>
@@ -21079,6 +21194,9 @@
       <c r="S63" s="3" t="s">
         <v>874</v>
       </c>
+      <c r="T63" s="5" t="s">
+        <v>1502</v>
+      </c>
       <c r="U63" s="7" t="s">
         <v>145</v>
       </c>
@@ -21144,6 +21262,9 @@
       <c r="S64" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T64" s="5" t="s">
+        <v>1503</v>
+      </c>
       <c r="U64" s="7" t="s">
         <v>303</v>
       </c>
@@ -21217,7 +21338,9 @@
       <c r="S65" s="3" t="s">
         <v>874</v>
       </c>
-      <c r="T65" s="3"/>
+      <c r="T65" s="5" t="s">
+        <v>1504</v>
+      </c>
       <c r="U65" s="7" t="s">
         <v>264</v>
       </c>
@@ -21285,6 +21408,9 @@
       <c r="S66" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T66" s="5" t="s">
+        <v>1505</v>
+      </c>
       <c r="U66" s="7"/>
       <c r="V66" s="10">
         <v>55</v>
@@ -21356,7 +21482,9 @@
       <c r="S67" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T67" s="3"/>
+      <c r="T67" s="5" t="s">
+        <v>1506</v>
+      </c>
       <c r="U67" s="7"/>
       <c r="V67" s="10">
         <v>208</v>
@@ -21430,7 +21558,9 @@
       <c r="S68" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T68" s="3"/>
+      <c r="T68" s="5" t="s">
+        <v>1507</v>
+      </c>
       <c r="U68" s="7" t="s">
         <v>583</v>
       </c>
@@ -21498,9 +21628,11 @@
       <c r="Q69" s="3"/>
       <c r="R69" s="3"/>
       <c r="S69" s="3" t="s">
-        <v>874</v>
-      </c>
-      <c r="T69" s="3"/>
+        <v>1255</v>
+      </c>
+      <c r="T69" s="5" t="s">
+        <v>1508</v>
+      </c>
       <c r="U69" s="7" t="s">
         <v>643</v>
       </c>
@@ -21570,7 +21702,9 @@
       <c r="S70" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T70" s="3"/>
+      <c r="T70" s="5" t="s">
+        <v>1509</v>
+      </c>
       <c r="U70" s="7" t="s">
         <v>583</v>
       </c>
@@ -21640,7 +21774,9 @@
       <c r="S71" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T71" s="3"/>
+      <c r="T71" s="3" t="s">
+        <v>1510</v>
+      </c>
       <c r="U71" s="7" t="s">
         <v>265</v>
       </c>
@@ -21706,7 +21842,10 @@
         <v>1092</v>
       </c>
       <c r="S72" s="3" t="s">
-        <v>874</v>
+        <v>1255</v>
+      </c>
+      <c r="T72" s="3" t="s">
+        <v>1511</v>
       </c>
       <c r="U72" s="7" t="s">
         <v>159</v>
@@ -21777,7 +21916,9 @@
       <c r="S73" s="3" t="s">
         <v>874</v>
       </c>
-      <c r="T73" s="3"/>
+      <c r="T73" s="3" t="s">
+        <v>1512</v>
+      </c>
       <c r="U73" s="7" t="s">
         <v>1373</v>
       </c>
@@ -21844,6 +21985,9 @@
       </c>
       <c r="S74" s="3" t="s">
         <v>1255</v>
+      </c>
+      <c r="T74" s="3" t="s">
+        <v>1513</v>
       </c>
       <c r="U74" s="7" t="s">
         <v>203</v>
@@ -21915,7 +22059,9 @@
       <c r="S75" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T75" s="3"/>
+      <c r="T75" s="3" t="s">
+        <v>1514</v>
+      </c>
       <c r="U75" s="7" t="s">
         <v>647</v>
       </c>
@@ -21991,7 +22137,9 @@
       <c r="S76" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T76" s="3"/>
+      <c r="T76" s="3" t="s">
+        <v>1515</v>
+      </c>
       <c r="U76" s="7" t="s">
         <v>611</v>
       </c>
@@ -22067,7 +22215,9 @@
       <c r="S77" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T77" s="3"/>
+      <c r="T77" s="3" t="s">
+        <v>1516</v>
+      </c>
       <c r="U77" s="7" t="s">
         <v>583</v>
       </c>
@@ -22133,6 +22283,9 @@
       <c r="S78" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T78" s="3" t="s">
+        <v>1517</v>
+      </c>
       <c r="U78" s="7" t="s">
         <v>696</v>
       </c>
@@ -22202,6 +22355,9 @@
       <c r="S79" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T79" s="3" t="s">
+        <v>1518</v>
+      </c>
       <c r="U79" s="7" t="s">
         <v>270</v>
       </c>
@@ -22265,6 +22421,9 @@
       <c r="S80" s="3" t="s">
         <v>874</v>
       </c>
+      <c r="T80" s="3" t="s">
+        <v>1519</v>
+      </c>
       <c r="U80" s="7" t="s">
         <v>832</v>
       </c>
@@ -22325,6 +22484,9 @@
       <c r="S81" s="3" t="s">
         <v>874</v>
       </c>
+      <c r="T81" s="3" t="s">
+        <v>1520</v>
+      </c>
       <c r="U81" s="7" t="s">
         <v>380</v>
       </c>
@@ -22393,6 +22555,9 @@
       <c r="S82" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T82" s="3" t="s">
+        <v>1521</v>
+      </c>
       <c r="U82" s="7"/>
       <c r="V82" s="10">
         <v>163</v>
@@ -22447,6 +22612,9 @@
       </c>
       <c r="S83" s="3" t="s">
         <v>874</v>
+      </c>
+      <c r="T83" s="3" t="s">
+        <v>1522</v>
       </c>
       <c r="U83" s="7" t="s">
         <v>835</v>
@@ -22513,7 +22681,9 @@
       <c r="S84" s="3" t="s">
         <v>874</v>
       </c>
-      <c r="T84" s="3"/>
+      <c r="T84" s="3" t="s">
+        <v>1523</v>
+      </c>
       <c r="U84" s="7" t="s">
         <v>395</v>
       </c>
@@ -22589,7 +22759,9 @@
       <c r="S85" s="3" t="s">
         <v>874</v>
       </c>
-      <c r="T85" s="3"/>
+      <c r="T85" s="3" t="s">
+        <v>1524</v>
+      </c>
       <c r="U85" s="7" t="s">
         <v>399</v>
       </c>
@@ -22659,6 +22831,9 @@
       </c>
       <c r="S86" s="3" t="s">
         <v>1255</v>
+      </c>
+      <c r="T86" s="3" t="s">
+        <v>1525</v>
       </c>
       <c r="U86" s="7" t="s">
         <v>271</v>
@@ -22866,6 +23041,9 @@
       <c r="S89" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T89" s="3" t="s">
+        <v>1526</v>
+      </c>
       <c r="U89" s="7" t="s">
         <v>402</v>
       </c>
@@ -22938,7 +23116,9 @@
       <c r="S90" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T90" s="3"/>
+      <c r="T90" s="3" t="s">
+        <v>1527</v>
+      </c>
       <c r="U90" s="7"/>
       <c r="V90" s="10">
         <v>683</v>
@@ -23003,6 +23183,9 @@
       </c>
       <c r="S91" s="3" t="s">
         <v>1255</v>
+      </c>
+      <c r="T91" s="3" t="s">
+        <v>1528</v>
       </c>
       <c r="U91" s="7"/>
       <c r="V91" s="10">
@@ -25767,6 +25950,20 @@
     <hyperlink ref="T49" r:id="rId76" xr:uid="{B2D1EEF0-CC8D-475D-AC61-622A048780E4}"/>
     <hyperlink ref="T53" r:id="rId77" xr:uid="{BE903FE3-4E19-4999-8947-55BCF63B937F}"/>
     <hyperlink ref="T54" r:id="rId78" xr:uid="{65536FCC-016F-45C4-B2EA-E24087E6E0C7}"/>
+    <hyperlink ref="T55" r:id="rId79" xr:uid="{98541FF0-B643-4025-9B11-6D2A8B43BE81}"/>
+    <hyperlink ref="T56" r:id="rId80" xr:uid="{93128A70-2208-4835-8826-987F00D5CE49}"/>
+    <hyperlink ref="T57" r:id="rId81" xr:uid="{448324D5-4938-4640-87A8-B0123432A0A8}"/>
+    <hyperlink ref="T58" r:id="rId82" xr:uid="{6A6EA229-627C-4BEB-9EB1-FB2268BA41E2}"/>
+    <hyperlink ref="T60" r:id="rId83" xr:uid="{B94719F3-AA21-4F3C-B176-05A4537368DE}"/>
+    <hyperlink ref="T61" r:id="rId84" xr:uid="{E3AB83A7-B6F6-4DF7-A3A6-4C39A37C2CC0}"/>
+    <hyperlink ref="T63" r:id="rId85" xr:uid="{FD592E99-AFA7-4161-A05C-AD418B758346}"/>
+    <hyperlink ref="T64" r:id="rId86" xr:uid="{F0682AD9-CF2B-474A-BAB7-1BAB2F2F0A91}"/>
+    <hyperlink ref="T65" r:id="rId87" xr:uid="{AC5D57E4-F59D-4EA8-AD41-DE2BDE03AD7E}"/>
+    <hyperlink ref="T66" r:id="rId88" xr:uid="{617CAC3E-E004-4B31-A68F-04FC7A473E73}"/>
+    <hyperlink ref="T67" r:id="rId89" xr:uid="{87683EAD-DDAC-40A7-84BD-158C2D18B849}"/>
+    <hyperlink ref="T68" r:id="rId90" xr:uid="{7130DD20-18CA-4B99-BEB5-3D7B840E699C}"/>
+    <hyperlink ref="T69" r:id="rId91" xr:uid="{03103B16-DE8B-4156-8FE9-040B48617618}"/>
+    <hyperlink ref="T70" r:id="rId92" xr:uid="{C599F5BA-C1B1-4E37-80D1-1F478DE474FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update docs with final wild vs cultivated labels
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\723110_2_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/2689286_2_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DBB1F4-C4EE-49DE-92AA-BFFC52C80BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{59DBB1F4-C4EE-49DE-92AA-BFFC52C80BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B01E69A-1AF1-4F75-8502-12F425D9704D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2880" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4224" uniqueCount="1529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4253" uniqueCount="1504">
   <si>
     <t>Species</t>
   </si>
@@ -4464,30 +4464,6 @@
     <t>https://eol.org/pages/1114313</t>
   </si>
   <si>
-    <t>https://eol.org/pages/1121207</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/49023867</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/483665</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1095470</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/594632</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/641527</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/47114859</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/483664</t>
-  </si>
-  <si>
     <t>GCA_003024255; https://doi.org/10.1186/s12864-018-4656-3</t>
   </si>
   <si>
@@ -4527,103 +4503,52 @@
     <t>v1; v1.3; PRJNA41163</t>
   </si>
   <si>
-    <t>https://eol.org/pages/584706</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/584705</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/468106</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/52522464</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/487229</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/468144</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/703189</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/581568</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/47378562</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/703664</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/486498</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/629943</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/633316</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/582270</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1154718/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/703659/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/52199934/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1115038/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/584304/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1116073/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/596454/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/581050/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/579181/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1115582/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/5824504/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1115583/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1115584/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1115872/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1115470/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1115098/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/594796/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/645324/data</t>
-  </si>
-  <si>
-    <t>https://eol.org/pages/1135088/data</t>
+    <t>Encyclopedia of Life: https://eol.org/pages/47114859</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/703189</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/581568</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/47378562</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/629943</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/52199934</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/5824504</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/1115872</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/584296</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/51600284</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/2891295</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/5698451</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/51843988</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/655171</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/2885841</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/1115259</t>
   </si>
 </sst>
 </file>
@@ -16805,9 +16730,9 @@
   <dimension ref="A1:AB132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="D130" sqref="D130"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16927,7 +16852,7 @@
         <v>317</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1483</v>
+        <v>1475</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>1318</v>
@@ -17061,7 +16986,7 @@
         <v>445</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>1484</v>
+        <v>1476</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>1082</v>
@@ -17139,7 +17064,7 @@
         <v>445</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>1485</v>
+        <v>1477</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>1318</v>
@@ -17215,7 +17140,7 @@
         <v>445</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>1486</v>
+        <v>1478</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>1318</v>
@@ -17283,7 +17208,7 @@
         <v>445</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>1487</v>
+        <v>1479</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>1318</v>
@@ -17355,7 +17280,7 @@
         <v>455</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>1488</v>
+        <v>1480</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>1082</v>
@@ -17425,7 +17350,7 @@
         <v>445</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>1489</v>
+        <v>1481</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>1082</v>
@@ -17708,7 +17633,7 @@
         <v>445</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>1490</v>
+        <v>1482</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>1082</v>
@@ -17942,7 +17867,7 @@
         <v>445</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>1491</v>
+        <v>1483</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>1082</v>
@@ -18016,7 +17941,7 @@
         <v>445</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>1492</v>
+        <v>1484</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>1318</v>
@@ -18090,7 +18015,7 @@
         <v>445</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>1493</v>
+        <v>1485</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1082</v>
@@ -18406,7 +18331,7 @@
         <v>445</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>1494</v>
+        <v>1486</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>1318</v>
@@ -18482,7 +18407,7 @@
         <v>445</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1495</v>
+        <v>1487</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>1082</v>
@@ -20062,7 +19987,7 @@
         <v>1255</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>1475</v>
+        <v>1350</v>
       </c>
       <c r="U46" s="7" t="s">
         <v>145</v>
@@ -20137,7 +20062,7 @@
         <v>1255</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>1476</v>
+        <v>1356</v>
       </c>
       <c r="U47" s="7" t="s">
         <v>635</v>
@@ -20203,7 +20128,7 @@
         <v>1255</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>1477</v>
+        <v>1357</v>
       </c>
       <c r="U48" s="7" t="s">
         <v>590</v>
@@ -20269,7 +20194,7 @@
         <v>1255</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>1478</v>
+        <v>1358</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>585</v>
@@ -20389,7 +20314,7 @@
         <v>1255</v>
       </c>
       <c r="T51" s="3" t="s">
-        <v>1479</v>
+        <v>1359</v>
       </c>
       <c r="U51" s="7" t="s">
         <v>361</v>
@@ -20463,7 +20388,7 @@
         <v>1255</v>
       </c>
       <c r="T52" s="3" t="s">
-        <v>1480</v>
+        <v>1360</v>
       </c>
       <c r="U52" s="7" t="s">
         <v>290</v>
@@ -20531,7 +20456,7 @@
         <v>874</v>
       </c>
       <c r="T53" s="5" t="s">
-        <v>1481</v>
+        <v>1488</v>
       </c>
       <c r="U53" s="7"/>
       <c r="V53" s="10">
@@ -20597,7 +20522,7 @@
         <v>1255</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>1482</v>
+        <v>1378</v>
       </c>
       <c r="U54" s="7" t="s">
         <v>583</v>
@@ -20669,7 +20594,7 @@
         <v>1255</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>1496</v>
+        <v>1379</v>
       </c>
       <c r="U55" s="7"/>
       <c r="V55" s="10">
@@ -20741,7 +20666,7 @@
         <v>1255</v>
       </c>
       <c r="T56" s="5" t="s">
-        <v>1497</v>
+        <v>1380</v>
       </c>
       <c r="U56" s="7"/>
       <c r="V56" s="10">
@@ -20807,7 +20732,7 @@
         <v>1255</v>
       </c>
       <c r="T57" s="5" t="s">
-        <v>1498</v>
+        <v>1381</v>
       </c>
       <c r="U57" s="7" t="s">
         <v>145</v>
@@ -20873,7 +20798,7 @@
         <v>874</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>1499</v>
+        <v>1382</v>
       </c>
       <c r="U58" s="7" t="s">
         <v>590</v>
@@ -20999,7 +20924,7 @@
         <v>1255</v>
       </c>
       <c r="T60" s="5" t="s">
-        <v>1500</v>
+        <v>1383</v>
       </c>
       <c r="U60" s="7"/>
       <c r="V60" s="10">
@@ -21065,7 +20990,7 @@
         <v>1255</v>
       </c>
       <c r="T61" s="5" t="s">
-        <v>1501</v>
+        <v>1384</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>263</v>
@@ -21195,7 +21120,7 @@
         <v>874</v>
       </c>
       <c r="T63" s="5" t="s">
-        <v>1502</v>
+        <v>1489</v>
       </c>
       <c r="U63" s="7" t="s">
         <v>145</v>
@@ -21263,7 +21188,7 @@
         <v>1255</v>
       </c>
       <c r="T64" s="5" t="s">
-        <v>1503</v>
+        <v>1490</v>
       </c>
       <c r="U64" s="7" t="s">
         <v>303</v>
@@ -21339,7 +21264,7 @@
         <v>874</v>
       </c>
       <c r="T65" s="5" t="s">
-        <v>1504</v>
+        <v>1491</v>
       </c>
       <c r="U65" s="7" t="s">
         <v>264</v>
@@ -21409,7 +21334,7 @@
         <v>1255</v>
       </c>
       <c r="T66" s="5" t="s">
-        <v>1505</v>
+        <v>1385</v>
       </c>
       <c r="U66" s="7"/>
       <c r="V66" s="10">
@@ -21483,7 +21408,7 @@
         <v>1255</v>
       </c>
       <c r="T67" s="5" t="s">
-        <v>1506</v>
+        <v>1386</v>
       </c>
       <c r="U67" s="7"/>
       <c r="V67" s="10">
@@ -21559,7 +21484,7 @@
         <v>1255</v>
       </c>
       <c r="T68" s="5" t="s">
-        <v>1507</v>
+        <v>1492</v>
       </c>
       <c r="U68" s="7" t="s">
         <v>583</v>
@@ -21631,7 +21556,7 @@
         <v>1255</v>
       </c>
       <c r="T69" s="5" t="s">
-        <v>1508</v>
+        <v>1387</v>
       </c>
       <c r="U69" s="7" t="s">
         <v>643</v>
@@ -21703,7 +21628,7 @@
         <v>1255</v>
       </c>
       <c r="T70" s="5" t="s">
-        <v>1509</v>
+        <v>1388</v>
       </c>
       <c r="U70" s="7" t="s">
         <v>583</v>
@@ -21775,7 +21700,7 @@
         <v>1255</v>
       </c>
       <c r="T71" s="3" t="s">
-        <v>1510</v>
+        <v>1389</v>
       </c>
       <c r="U71" s="7" t="s">
         <v>265</v>
@@ -21845,7 +21770,7 @@
         <v>1255</v>
       </c>
       <c r="T72" s="3" t="s">
-        <v>1511</v>
+        <v>1390</v>
       </c>
       <c r="U72" s="7" t="s">
         <v>159</v>
@@ -21917,7 +21842,7 @@
         <v>874</v>
       </c>
       <c r="T73" s="3" t="s">
-        <v>1512</v>
+        <v>1493</v>
       </c>
       <c r="U73" s="7" t="s">
         <v>1373</v>
@@ -21987,7 +21912,7 @@
         <v>1255</v>
       </c>
       <c r="T74" s="3" t="s">
-        <v>1513</v>
+        <v>1391</v>
       </c>
       <c r="U74" s="7" t="s">
         <v>203</v>
@@ -22060,7 +21985,7 @@
         <v>1255</v>
       </c>
       <c r="T75" s="3" t="s">
-        <v>1514</v>
+        <v>1392</v>
       </c>
       <c r="U75" s="7" t="s">
         <v>647</v>
@@ -22138,7 +22063,7 @@
         <v>1255</v>
       </c>
       <c r="T76" s="3" t="s">
-        <v>1515</v>
+        <v>1393</v>
       </c>
       <c r="U76" s="7" t="s">
         <v>611</v>
@@ -22216,7 +22141,7 @@
         <v>1255</v>
       </c>
       <c r="T77" s="3" t="s">
-        <v>1516</v>
+        <v>1394</v>
       </c>
       <c r="U77" s="7" t="s">
         <v>583</v>
@@ -22284,7 +22209,7 @@
         <v>1255</v>
       </c>
       <c r="T78" s="3" t="s">
-        <v>1517</v>
+        <v>1395</v>
       </c>
       <c r="U78" s="7" t="s">
         <v>696</v>
@@ -22356,7 +22281,7 @@
         <v>1255</v>
       </c>
       <c r="T79" s="3" t="s">
-        <v>1518</v>
+        <v>1396</v>
       </c>
       <c r="U79" s="7" t="s">
         <v>270</v>
@@ -22422,7 +22347,7 @@
         <v>874</v>
       </c>
       <c r="T80" s="3" t="s">
-        <v>1519</v>
+        <v>1397</v>
       </c>
       <c r="U80" s="7" t="s">
         <v>832</v>
@@ -22485,7 +22410,7 @@
         <v>874</v>
       </c>
       <c r="T81" s="3" t="s">
-        <v>1520</v>
+        <v>1494</v>
       </c>
       <c r="U81" s="7" t="s">
         <v>380</v>
@@ -22556,7 +22481,7 @@
         <v>1255</v>
       </c>
       <c r="T82" s="3" t="s">
-        <v>1521</v>
+        <v>1398</v>
       </c>
       <c r="U82" s="7"/>
       <c r="V82" s="10">
@@ -22614,7 +22539,7 @@
         <v>874</v>
       </c>
       <c r="T83" s="3" t="s">
-        <v>1522</v>
+        <v>1399</v>
       </c>
       <c r="U83" s="7" t="s">
         <v>835</v>
@@ -22682,7 +22607,7 @@
         <v>874</v>
       </c>
       <c r="T84" s="3" t="s">
-        <v>1523</v>
+        <v>1495</v>
       </c>
       <c r="U84" s="7" t="s">
         <v>395</v>
@@ -22760,7 +22685,7 @@
         <v>874</v>
       </c>
       <c r="T85" s="3" t="s">
-        <v>1524</v>
+        <v>1400</v>
       </c>
       <c r="U85" s="7" t="s">
         <v>399</v>
@@ -22833,7 +22758,7 @@
         <v>1255</v>
       </c>
       <c r="T86" s="3" t="s">
-        <v>1525</v>
+        <v>1401</v>
       </c>
       <c r="U86" s="7" t="s">
         <v>271</v>
@@ -23042,7 +22967,7 @@
         <v>1255</v>
       </c>
       <c r="T89" s="3" t="s">
-        <v>1526</v>
+        <v>1404</v>
       </c>
       <c r="U89" s="7" t="s">
         <v>402</v>
@@ -23117,7 +23042,7 @@
         <v>1255</v>
       </c>
       <c r="T90" s="3" t="s">
-        <v>1527</v>
+        <v>1405</v>
       </c>
       <c r="U90" s="7"/>
       <c r="V90" s="10">
@@ -23185,7 +23110,7 @@
         <v>1255</v>
       </c>
       <c r="T91" s="3" t="s">
-        <v>1528</v>
+        <v>1406</v>
       </c>
       <c r="U91" s="7"/>
       <c r="V91" s="10">
@@ -23304,9 +23229,11 @@
       <c r="Q93" s="3"/>
       <c r="R93" s="3"/>
       <c r="S93" s="3" t="s">
-        <v>874</v>
-      </c>
-      <c r="T93" s="3"/>
+        <v>1255</v>
+      </c>
+      <c r="T93" s="3" t="s">
+        <v>1496</v>
+      </c>
       <c r="U93" s="7" t="s">
         <v>583</v>
       </c>
@@ -23380,9 +23307,11 @@
         <v>1269</v>
       </c>
       <c r="S94" s="3" t="s">
-        <v>1255</v>
-      </c>
-      <c r="T94" s="3"/>
+        <v>874</v>
+      </c>
+      <c r="T94" s="3" t="s">
+        <v>1407</v>
+      </c>
       <c r="U94" s="7" t="s">
         <v>252</v>
       </c>
@@ -23454,7 +23383,9 @@
       <c r="S95" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T95" s="3"/>
+      <c r="T95" s="3" t="s">
+        <v>1408</v>
+      </c>
       <c r="U95" s="7" t="s">
         <v>583</v>
       </c>
@@ -23526,7 +23457,9 @@
       <c r="S96" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T96" s="3"/>
+      <c r="T96" s="3" t="s">
+        <v>1409</v>
+      </c>
       <c r="U96" s="7" t="s">
         <v>412</v>
       </c>
@@ -23598,7 +23531,9 @@
       <c r="S97" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T97" s="3"/>
+      <c r="T97" s="3" t="s">
+        <v>1410</v>
+      </c>
       <c r="U97" s="7" t="s">
         <v>273</v>
       </c>
@@ -23662,6 +23597,9 @@
       </c>
       <c r="S98" s="3" t="s">
         <v>874</v>
+      </c>
+      <c r="T98" s="3" t="s">
+        <v>1411</v>
       </c>
       <c r="U98" s="7" t="s">
         <v>418</v>
@@ -23801,7 +23739,9 @@
       <c r="S100" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T100" s="3"/>
+      <c r="T100" s="3" t="s">
+        <v>1497</v>
+      </c>
       <c r="U100" s="7" t="s">
         <v>712</v>
       </c>
@@ -23877,7 +23817,9 @@
       <c r="S101" s="3" t="s">
         <v>874</v>
       </c>
-      <c r="T101" s="3"/>
+      <c r="T101" s="3" t="s">
+        <v>1498</v>
+      </c>
       <c r="U101" s="7" t="s">
         <v>1368</v>
       </c>
@@ -23944,6 +23886,9 @@
       </c>
       <c r="S102" s="3" t="s">
         <v>874</v>
+      </c>
+      <c r="T102" s="3" t="s">
+        <v>1413</v>
       </c>
       <c r="U102" s="7" t="s">
         <v>595</v>
@@ -24082,7 +24027,9 @@
       <c r="S104" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T104" s="3"/>
+      <c r="T104" s="3" t="s">
+        <v>1415</v>
+      </c>
       <c r="U104" s="7" t="s">
         <v>428</v>
       </c>
@@ -24148,6 +24095,9 @@
       <c r="S105" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T105" s="3" t="s">
+        <v>1416</v>
+      </c>
       <c r="U105" s="7" t="s">
         <v>274</v>
       </c>
@@ -24211,6 +24161,9 @@
       <c r="S106" s="3" t="s">
         <v>874</v>
       </c>
+      <c r="T106" s="3" t="s">
+        <v>1417</v>
+      </c>
       <c r="U106" s="7" t="s">
         <v>275</v>
       </c>
@@ -24328,6 +24281,9 @@
       </c>
       <c r="S108" s="3" t="s">
         <v>1255</v>
+      </c>
+      <c r="T108" s="3" t="s">
+        <v>1418</v>
       </c>
       <c r="U108" s="7" t="s">
         <v>159</v>
@@ -24520,7 +24476,9 @@
       <c r="S111" s="3" t="s">
         <v>874</v>
       </c>
-      <c r="T111" s="3"/>
+      <c r="T111" s="3" t="s">
+        <v>1499</v>
+      </c>
       <c r="U111" s="7" t="s">
         <v>595</v>
       </c>
@@ -24622,7 +24580,9 @@
       <c r="S113" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T113" s="3"/>
+      <c r="T113" s="3" t="s">
+        <v>1421</v>
+      </c>
       <c r="U113" s="7" t="s">
         <v>159</v>
       </c>
@@ -24694,7 +24654,9 @@
       <c r="S114" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T114" s="3"/>
+      <c r="T114" s="3" t="s">
+        <v>1422</v>
+      </c>
       <c r="U114" s="7" t="s">
         <v>276</v>
       </c>
@@ -24758,7 +24720,10 @@
         <v>231</v>
       </c>
       <c r="S115" s="3" t="s">
-        <v>1255</v>
+        <v>874</v>
+      </c>
+      <c r="T115" s="3" t="s">
+        <v>1500</v>
       </c>
       <c r="U115" s="7" t="s">
         <v>278</v>
@@ -24823,6 +24788,9 @@
       <c r="S116" s="3" t="s">
         <v>874</v>
       </c>
+      <c r="T116" s="3" t="s">
+        <v>1423</v>
+      </c>
       <c r="U116" s="7" t="s">
         <v>594</v>
       </c>
@@ -24885,6 +24853,9 @@
       </c>
       <c r="S117" s="3" t="s">
         <v>874</v>
+      </c>
+      <c r="T117" s="3" t="s">
+        <v>1424</v>
       </c>
       <c r="U117" s="7" t="s">
         <v>594</v>
@@ -25011,7 +24982,9 @@
       <c r="S119" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T119" s="3"/>
+      <c r="T119" s="3" t="s">
+        <v>1425</v>
+      </c>
       <c r="U119" s="7" t="s">
         <v>583</v>
       </c>
@@ -25298,6 +25271,9 @@
       </c>
       <c r="S124" s="3" t="s">
         <v>1255</v>
+      </c>
+      <c r="T124" s="3" t="s">
+        <v>1426</v>
       </c>
       <c r="U124" s="7" t="s">
         <v>603</v>
@@ -25368,7 +25344,9 @@
       <c r="S125" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T125" s="3"/>
+      <c r="T125" s="3" t="s">
+        <v>1427</v>
+      </c>
       <c r="U125" s="7"/>
       <c r="V125" s="10">
         <v>558</v>
@@ -25442,7 +25420,9 @@
       <c r="S126" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T126" s="3"/>
+      <c r="T126" s="3" t="s">
+        <v>1501</v>
+      </c>
       <c r="U126" s="7" t="s">
         <v>594</v>
       </c>
@@ -25504,6 +25484,9 @@
       <c r="S127" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T127" s="3" t="s">
+        <v>1428</v>
+      </c>
       <c r="U127" s="7" t="s">
         <v>444</v>
       </c>
@@ -25573,7 +25556,9 @@
       <c r="S128" s="3" t="s">
         <v>1255</v>
       </c>
-      <c r="T128" s="3"/>
+      <c r="T128" s="3" t="s">
+        <v>1429</v>
+      </c>
       <c r="U128" s="7" t="s">
         <v>277</v>
       </c>
@@ -25642,6 +25627,9 @@
       <c r="S129" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T129" s="3" t="s">
+        <v>1502</v>
+      </c>
       <c r="U129" s="7" t="s">
         <v>583</v>
       </c>
@@ -25710,6 +25698,9 @@
       <c r="S130" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T130" s="3" t="s">
+        <v>1503</v>
+      </c>
       <c r="U130" s="7" t="s">
         <v>781</v>
       </c>
@@ -25782,6 +25773,9 @@
       <c r="S131" s="3" t="s">
         <v>1255</v>
       </c>
+      <c r="T131" s="3" t="s">
+        <v>1142</v>
+      </c>
       <c r="U131" s="7" t="s">
         <v>603</v>
       </c>
@@ -25849,6 +25843,9 @@
       </c>
       <c r="S132" s="3" t="s">
         <v>1255</v>
+      </c>
+      <c r="T132" s="3" t="s">
+        <v>1431</v>
       </c>
       <c r="U132" s="7" t="s">
         <v>583</v>
@@ -25944,26 +25941,26 @@
     <hyperlink ref="N39" r:id="rId70" xr:uid="{F106909F-A437-4D92-8178-D29EE28CB1F4}"/>
     <hyperlink ref="P39" r:id="rId71" xr:uid="{73BC78FA-DA4F-4B3D-B5E3-FB774222D285}"/>
     <hyperlink ref="T45" r:id="rId72" xr:uid="{0C0C3D63-49F0-43FA-B438-03C544B159FB}"/>
-    <hyperlink ref="T46" r:id="rId73" xr:uid="{9D4AE2E3-6A00-4069-9AAF-194903D8E369}"/>
-    <hyperlink ref="T47" r:id="rId74" xr:uid="{BE4187D2-0384-49AA-AE6D-044AB3E282C4}"/>
-    <hyperlink ref="T48" r:id="rId75" xr:uid="{FDBC7D42-08D2-42C9-BF8E-6B4DBC5B085A}"/>
-    <hyperlink ref="T49" r:id="rId76" xr:uid="{B2D1EEF0-CC8D-475D-AC61-622A048780E4}"/>
-    <hyperlink ref="T53" r:id="rId77" xr:uid="{BE903FE3-4E19-4999-8947-55BCF63B937F}"/>
-    <hyperlink ref="T54" r:id="rId78" xr:uid="{65536FCC-016F-45C4-B2EA-E24087E6E0C7}"/>
-    <hyperlink ref="T55" r:id="rId79" xr:uid="{98541FF0-B643-4025-9B11-6D2A8B43BE81}"/>
-    <hyperlink ref="T56" r:id="rId80" xr:uid="{93128A70-2208-4835-8826-987F00D5CE49}"/>
-    <hyperlink ref="T57" r:id="rId81" xr:uid="{448324D5-4938-4640-87A8-B0123432A0A8}"/>
-    <hyperlink ref="T58" r:id="rId82" xr:uid="{6A6EA229-627C-4BEB-9EB1-FB2268BA41E2}"/>
-    <hyperlink ref="T60" r:id="rId83" xr:uid="{B94719F3-AA21-4F3C-B176-05A4537368DE}"/>
-    <hyperlink ref="T61" r:id="rId84" xr:uid="{E3AB83A7-B6F6-4DF7-A3A6-4C39A37C2CC0}"/>
-    <hyperlink ref="T63" r:id="rId85" xr:uid="{FD592E99-AFA7-4161-A05C-AD418B758346}"/>
-    <hyperlink ref="T64" r:id="rId86" xr:uid="{F0682AD9-CF2B-474A-BAB7-1BAB2F2F0A91}"/>
-    <hyperlink ref="T65" r:id="rId87" xr:uid="{AC5D57E4-F59D-4EA8-AD41-DE2BDE03AD7E}"/>
-    <hyperlink ref="T66" r:id="rId88" xr:uid="{617CAC3E-E004-4B31-A68F-04FC7A473E73}"/>
-    <hyperlink ref="T67" r:id="rId89" xr:uid="{87683EAD-DDAC-40A7-84BD-158C2D18B849}"/>
-    <hyperlink ref="T68" r:id="rId90" xr:uid="{7130DD20-18CA-4B99-BEB5-3D7B840E699C}"/>
-    <hyperlink ref="T69" r:id="rId91" xr:uid="{03103B16-DE8B-4156-8FE9-040B48617618}"/>
-    <hyperlink ref="T70" r:id="rId92" xr:uid="{C599F5BA-C1B1-4E37-80D1-1F478DE474FA}"/>
+    <hyperlink ref="T46" r:id="rId73" display="https://eol.org/pages/1121207" xr:uid="{9D4AE2E3-6A00-4069-9AAF-194903D8E369}"/>
+    <hyperlink ref="T47" r:id="rId74" display="https://eol.org/pages/49023867" xr:uid="{BE4187D2-0384-49AA-AE6D-044AB3E282C4}"/>
+    <hyperlink ref="T48" r:id="rId75" display="https://eol.org/pages/483665" xr:uid="{FDBC7D42-08D2-42C9-BF8E-6B4DBC5B085A}"/>
+    <hyperlink ref="T49" r:id="rId76" display="https://eol.org/pages/1095470" xr:uid="{B2D1EEF0-CC8D-475D-AC61-622A048780E4}"/>
+    <hyperlink ref="T53" r:id="rId77" display="https://eol.org/pages/47114859" xr:uid="{BE903FE3-4E19-4999-8947-55BCF63B937F}"/>
+    <hyperlink ref="T54" r:id="rId78" display="https://eol.org/pages/483664" xr:uid="{65536FCC-016F-45C4-B2EA-E24087E6E0C7}"/>
+    <hyperlink ref="T55" r:id="rId79" display="https://eol.org/pages/584706" xr:uid="{98541FF0-B643-4025-9B11-6D2A8B43BE81}"/>
+    <hyperlink ref="T56" r:id="rId80" display="https://eol.org/pages/584705" xr:uid="{93128A70-2208-4835-8826-987F00D5CE49}"/>
+    <hyperlink ref="T57" r:id="rId81" display="https://eol.org/pages/468106" xr:uid="{448324D5-4938-4640-87A8-B0123432A0A8}"/>
+    <hyperlink ref="T58" r:id="rId82" display="https://eol.org/pages/52522464" xr:uid="{6A6EA229-627C-4BEB-9EB1-FB2268BA41E2}"/>
+    <hyperlink ref="T60" r:id="rId83" display="https://eol.org/pages/487229" xr:uid="{B94719F3-AA21-4F3C-B176-05A4537368DE}"/>
+    <hyperlink ref="T61" r:id="rId84" display="https://eol.org/pages/468144" xr:uid="{E3AB83A7-B6F6-4DF7-A3A6-4C39A37C2CC0}"/>
+    <hyperlink ref="T63" r:id="rId85" display="https://eol.org/pages/703189" xr:uid="{FD592E99-AFA7-4161-A05C-AD418B758346}"/>
+    <hyperlink ref="T64" r:id="rId86" display="https://eol.org/pages/581568" xr:uid="{F0682AD9-CF2B-474A-BAB7-1BAB2F2F0A91}"/>
+    <hyperlink ref="T65" r:id="rId87" display="https://eol.org/pages/47378562" xr:uid="{AC5D57E4-F59D-4EA8-AD41-DE2BDE03AD7E}"/>
+    <hyperlink ref="T66" r:id="rId88" display="https://eol.org/pages/703664" xr:uid="{617CAC3E-E004-4B31-A68F-04FC7A473E73}"/>
+    <hyperlink ref="T67" r:id="rId89" display="https://eol.org/pages/486498" xr:uid="{87683EAD-DDAC-40A7-84BD-158C2D18B849}"/>
+    <hyperlink ref="T68" r:id="rId90" display="https://eol.org/pages/629943" xr:uid="{7130DD20-18CA-4B99-BEB5-3D7B840E699C}"/>
+    <hyperlink ref="T69" r:id="rId91" display="https://eol.org/pages/633316" xr:uid="{03103B16-DE8B-4156-8FE9-040B48617618}"/>
+    <hyperlink ref="T70" r:id="rId92" display="https://eol.org/pages/582270" xr:uid="{C599F5BA-C1B1-4E37-80D1-1F478DE474FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update height references, values
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/2689286_2_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198206_2_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{59DBB1F4-C4EE-49DE-92AA-BFFC52C80BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B01E69A-1AF1-4F75-8502-12F425D9704D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB90D3A-413C-4FE9-B146-2B8C6A84EEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2880" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -3810,9 +3810,6 @@
     <t>can only find GBS data, actually I don't think this is GBS data, it's targeted sequencing of 400 SNPS</t>
   </si>
   <si>
-    <t>http://www.missouribotanicalgarden.org/gardens-gardening/your-garden/plant-finder/plant-details/kc/e454/cucurbita-argyrosperma.aspx ; average of height range reported on website for missouri botanical garden, then converted to meters; Retrieved 2023-10-25</t>
-  </si>
-  <si>
     <t>DOI: 10.5897/JPBCS2016.0605 ; Animasaun, D. A., J. A. Morakinyo, and O. T. Mustapha. "Assessment of the effects of gamma irradiation on the growth and yield of Digitaria exilis [Haller]." Journal of Applied Biosciences 75 (2014): 6164-6172. ; average value for HP variable in Table 4</t>
   </si>
   <si>
@@ -3834,9 +3831,6 @@
     <t>https://doi.org/10.1016/j.scienta.2011.06.036</t>
   </si>
   <si>
-    <t>http://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=282778 ; average of height range reported by Missouri Botanical Garden (12 - 20 feet), then converted to meters</t>
-  </si>
-  <si>
     <t>https://doi.org/10.21273/HORTSCI.44.3.656 ; Mean of Ht column in Table 2</t>
   </si>
   <si>
@@ -3846,18 +3840,6 @@
     <t>https://doi.org/10.1093/genetics/150.2.899 ; Most common value in Figure 3 histogram for plant height</t>
   </si>
   <si>
-    <t>https://owic.oregonstate.edu/black-cottonwood-populus-trichocarpa ; average of range given in text (125 - 150 ft), then converted to meters</t>
-  </si>
-  <si>
-    <t>https://www.rhododendron.org/descriptionS_taxon.asp?ID=259 ; description from American Rhododendron Society</t>
-  </si>
-  <si>
-    <t>https://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=283438 ; In its native habitat, it may grow to as much as 50-75' tall over time, but as an indoor plant it grows much shorter ; I took the average of this range then converted it to meters</t>
-  </si>
-  <si>
-    <t>https://www.rhs.org.uk/plants/19138/xanthoceras-sorbifolium/details ; retrieved on 2023-10-25 ; mean of ultimate height range 2.5-4 m ; might also consider looking at https://doi.org/10.1002/fes3.500 ; Mean from Table 1</t>
-  </si>
-  <si>
     <t>Hydrocotyle leucocephala HAP1 v2.1</t>
   </si>
   <si>
@@ -4549,6 +4531,24 @@
   </si>
   <si>
     <t>Encyclopedia of Life: https://eol.org/pages/1115259</t>
+  </si>
+  <si>
+    <t>doi: 10.5154/r.rchsza.2017.09.004 - number comes from Table 1 under the FC condition; Missouri botanical garden website also gives a height of around 0.3429 m</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/S0304-4238(97)00137-4; number comes from table 3, mean of M. accuminata species. http://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=282778 ; average of height range reported by Missouri Botanical Garden (12 - 20 feet), then converted to meters, suggests a height of 4.8768 m</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1139/cjb-2013-0303; trees described as being up to 35 m tall; https://owic.oregonstate.edu/black-cottonwood-populus-trichocarpa ; average of range given in text (125 - 150 ft), then converted to meters, suggests average height of 41.91 m</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/fes3.500 ; Mean from Table 1 ; https://www.rhs.org.uk/plants/19138/xanthoceras-sorbifolium/details ; retrieved on 2023-10-25 ; mean of ultimate height range 2.5-4 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.kew.org/plants/vanilla ; retrieved 2024-04-01 ; also says that plants can grow up to 30 m tall ; https://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=283438 ; In its native habitat, it may grow to as much as 50-75' tall over time, but as an indoor plant it grows much shorter ; I took the average of this range then converted it to meters and it suggests a height of 19.05 m </t>
+  </si>
+  <si>
+    <t>https://www.rhododendron.org/descriptionS_taxon.asp?ID=259 ; description from American Rhododendron Society ; gave height as 3 ft, which I then converted to meters</t>
   </si>
 </sst>
 </file>
@@ -16636,37 +16636,37 @@
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>1434</v>
+        <v>1428</v>
       </c>
     </row>
   </sheetData>
@@ -16730,9 +16730,9 @@
   <dimension ref="A1:AB132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16757,7 +16757,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -16766,7 +16766,7 @@
         <v>316</v>
       </c>
       <c r="E1" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
       <c r="F1" t="s">
         <v>446</v>
@@ -16811,7 +16811,7 @@
         <v>1254</v>
       </c>
       <c r="T1" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>66</v>
@@ -16852,13 +16852,13 @@
         <v>317</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1475</v>
+        <v>1469</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>773</v>
@@ -16889,7 +16889,7 @@
         <v>1255</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>1038</v>
@@ -16986,7 +16986,7 @@
         <v>445</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>1476</v>
+        <v>1470</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>1082</v>
@@ -17025,7 +17025,7 @@
         <v>1255</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>750</v>
@@ -17064,13 +17064,13 @@
         <v>445</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>1477</v>
+        <v>1471</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>751</v>
@@ -17104,7 +17104,7 @@
         <v>139</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
       <c r="V5" s="10">
         <v>87</v>
@@ -17140,13 +17140,13 @@
         <v>445</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>1478</v>
+        <v>1472</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>26</v>
@@ -17162,7 +17162,7 @@
         <v>850</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="O6" s="3">
         <v>2</v>
@@ -17174,7 +17174,7 @@
         <v>874</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="U6" s="7"/>
       <c r="V6" s="10">
@@ -17208,13 +17208,13 @@
         <v>445</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>1479</v>
+        <v>1473</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>16</v>
@@ -17243,7 +17243,7 @@
         <v>874</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
       <c r="U7" s="7"/>
       <c r="V7" s="10">
@@ -17280,13 +17280,13 @@
         <v>455</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>1480</v>
+        <v>1474</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>460</v>
@@ -17350,13 +17350,13 @@
         <v>445</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>1481</v>
+        <v>1475</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>22</v>
@@ -17387,7 +17387,7 @@
         <v>874</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="10">
@@ -17424,10 +17424,10 @@
         <v>317</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>160</v>
@@ -17455,7 +17455,7 @@
         <v>874</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
       <c r="U10" s="7"/>
       <c r="V10" s="10">
@@ -17477,7 +17477,7 @@
         <v>3</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="11" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -17494,10 +17494,10 @@
         <v>455</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>461</v>
@@ -17525,7 +17525,7 @@
         <v>874</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="U11" s="7" t="s">
         <v>575</v>
@@ -17564,7 +17564,7 @@
         <v>1082</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
       <c r="I12" s="7"/>
       <c r="K12" s="3">
@@ -17589,13 +17589,13 @@
         <v>0.3861</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
       <c r="U12" s="7" t="s">
         <v>617</v>
@@ -17616,7 +17616,7 @@
         <v>3</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.25">
@@ -17633,13 +17633,13 @@
         <v>445</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>1482</v>
+        <v>1476</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>775</v>
@@ -17670,10 +17670,10 @@
         <v>1255</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="V13" s="10">
         <v>320</v>
@@ -17694,7 +17694,7 @@
         <v>10</v>
       </c>
       <c r="AB13" s="3" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="45" x14ac:dyDescent="0.25">
@@ -17715,7 +17715,7 @@
         <v>1082</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>774</v>
@@ -17750,10 +17750,10 @@
         <v>874</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="V14" s="10">
         <v>3</v>
@@ -17792,7 +17792,7 @@
         <v>1082</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>753</v>
@@ -17826,7 +17826,7 @@
         <v>1255</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="U15" s="7" t="s">
         <v>754</v>
@@ -17850,7 +17850,7 @@
         <v>3</v>
       </c>
       <c r="AB15" s="3" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="30" x14ac:dyDescent="0.25">
@@ -17867,13 +17867,13 @@
         <v>445</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>1483</v>
+        <v>1477</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>1374</v>
+        <v>1368</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>752</v>
@@ -17904,10 +17904,10 @@
         <v>1255</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
       <c r="U16" s="7" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
       <c r="V16" s="10">
         <v>597</v>
@@ -17941,13 +17941,13 @@
         <v>445</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>1484</v>
+        <v>1478</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>105</v>
@@ -17978,7 +17978,7 @@
         <v>874</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>1450</v>
+        <v>1444</v>
       </c>
       <c r="U17" s="7" t="s">
         <v>715</v>
@@ -18015,7 +18015,7 @@
         <v>445</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>1485</v>
+        <v>1479</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1082</v>
@@ -18052,7 +18052,7 @@
         <v>874</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>1449</v>
+        <v>1443</v>
       </c>
       <c r="U18" s="7" t="s">
         <v>281</v>
@@ -18114,7 +18114,7 @@
         <v>874</v>
       </c>
       <c r="U19" s="23" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
       <c r="V19" s="24">
         <v>178</v>
@@ -18144,7 +18144,7 @@
         <v>1082</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>807</v>
@@ -18172,7 +18172,7 @@
         <v>1255</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>1448</v>
+        <v>1442</v>
       </c>
       <c r="U20" s="7"/>
       <c r="V20" s="10">
@@ -18209,7 +18209,7 @@
         <v>1082</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>1375</v>
+        <v>1369</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>808</v>
@@ -18240,10 +18240,10 @@
         <v>1255</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>1445</v>
+        <v>1439</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>1333</v>
+        <v>1327</v>
       </c>
       <c r="V21" s="10">
         <v>1007</v>
@@ -18262,7 +18262,7 @@
         <v>19</v>
       </c>
       <c r="AB21" s="3" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="22" spans="1:28" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -18331,13 +18331,13 @@
         <v>445</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>1486</v>
+        <v>1480</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>1376</v>
+        <v>1370</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>684</v>
@@ -18370,10 +18370,10 @@
         <v>1255</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>1456</v>
+        <v>1450</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>1372</v>
+        <v>1366</v>
       </c>
       <c r="V23" s="10">
         <v>119</v>
@@ -18407,13 +18407,13 @@
         <v>445</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1487</v>
+        <v>1481</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>840</v>
@@ -18446,7 +18446,7 @@
         <v>1255</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>1447</v>
+        <v>1441</v>
       </c>
       <c r="U24" s="7" t="s">
         <v>159</v>
@@ -18483,17 +18483,17 @@
         <v>455</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
       <c r="I25" s="7"/>
       <c r="K25" s="3">
         <v>0.87321063394682996</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>833</v>
@@ -18511,7 +18511,7 @@
         <v>1255</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>1446</v>
+        <v>1440</v>
       </c>
       <c r="U25" s="7"/>
       <c r="V25" s="10">
@@ -18544,10 +18544,10 @@
         <v>455</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>856</v>
@@ -18575,7 +18575,7 @@
         <v>1255</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>1454</v>
+        <v>1448</v>
       </c>
       <c r="U26" s="7" t="s">
         <v>583</v>
@@ -18613,7 +18613,7 @@
         <v>1082</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>756</v>
@@ -18641,7 +18641,7 @@
         <v>1255</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>1455</v>
+        <v>1449</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>324</v>
@@ -18682,10 +18682,10 @@
         <v>455</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>1339</v>
+        <v>1333</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>842</v>
@@ -18715,7 +18715,7 @@
         <v>1255</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>1457</v>
+        <v>1451</v>
       </c>
       <c r="U28" s="7" t="s">
         <v>622</v>
@@ -18753,7 +18753,7 @@
         <v>1082</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>1340</v>
+        <v>1334</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>325</v>
@@ -18783,7 +18783,7 @@
         <v>1255</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>1458</v>
+        <v>1452</v>
       </c>
       <c r="U29" s="7" t="s">
         <v>328</v>
@@ -18822,7 +18822,7 @@
         <v>1082</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>59</v>
@@ -18857,7 +18857,7 @@
         <v>874</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>1459</v>
+        <v>1453</v>
       </c>
       <c r="U30" s="7" t="s">
         <v>159</v>
@@ -18897,7 +18897,7 @@
         <v>1082</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>50</v>
@@ -18925,7 +18925,7 @@
         <v>874</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>1460</v>
+        <v>1454</v>
       </c>
       <c r="U31" s="7" t="s">
         <v>716</v>
@@ -18962,7 +18962,7 @@
         <v>1146</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>1377</v>
+        <v>1371</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>890</v>
@@ -18995,10 +18995,10 @@
         <v>1255</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>1461</v>
+        <v>1455</v>
       </c>
       <c r="U32" s="7" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
       <c r="V32" s="10">
         <v>8028</v>
@@ -19032,7 +19032,7 @@
         <v>455</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>1059</v>
@@ -19065,7 +19065,7 @@
         <v>1255</v>
       </c>
       <c r="T33" s="3" t="s">
-        <v>1462</v>
+        <v>1456</v>
       </c>
       <c r="U33" s="7" t="s">
         <v>583</v>
@@ -19103,7 +19103,7 @@
         <v>1082</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>858</v>
@@ -19139,7 +19139,7 @@
         <v>1255</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>1463</v>
+        <v>1457</v>
       </c>
       <c r="U34" s="7" t="s">
         <v>259</v>
@@ -19174,19 +19174,19 @@
         <v>445</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>1345</v>
+        <v>1339</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>1435</v>
+        <v>1429</v>
       </c>
       <c r="I35" s="7" t="s">
-        <v>1436</v>
+        <v>1430</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3">
@@ -19213,7 +19213,7 @@
         <v>1255</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>1464</v>
+        <v>1458</v>
       </c>
       <c r="U35" s="7" t="s">
         <v>260</v>
@@ -19250,7 +19250,7 @@
         <v>1082</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>1346</v>
+        <v>1340</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>859</v>
@@ -19283,7 +19283,7 @@
         <v>1255</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>1465</v>
+        <v>1459</v>
       </c>
       <c r="U36" s="7" t="s">
         <v>299</v>
@@ -19320,10 +19320,10 @@
         <v>455</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>1347</v>
+        <v>1341</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>791</v>
@@ -19353,7 +19353,7 @@
         <v>1255</v>
       </c>
       <c r="T37" s="3" t="s">
-        <v>1466</v>
+        <v>1460</v>
       </c>
       <c r="U37" s="7" t="s">
         <v>583</v>
@@ -19388,10 +19388,10 @@
         <v>317</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>1348</v>
+        <v>1342</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>893</v>
@@ -19421,7 +19421,7 @@
         <v>1255</v>
       </c>
       <c r="T38" s="3" t="s">
-        <v>1467</v>
+        <v>1461</v>
       </c>
       <c r="U38" s="7" t="s">
         <v>341</v>
@@ -19456,26 +19456,26 @@
         <v>445</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="I39" s="7"/>
       <c r="K39" s="3">
         <v>0.49</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>1432</v>
+        <v>1426</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>833</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>1433</v>
+        <v>1427</v>
       </c>
       <c r="O39" s="3">
         <v>2</v>
@@ -19487,7 +19487,7 @@
         <v>1255</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>1468</v>
+        <v>1462</v>
       </c>
       <c r="U39" s="7" t="s">
         <v>953</v>
@@ -19515,10 +19515,10 @@
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>1349</v>
+        <v>1343</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>861</v>
@@ -19551,7 +19551,7 @@
         <v>1255</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>1469</v>
+        <v>1463</v>
       </c>
       <c r="U40" s="7" t="s">
         <v>344</v>
@@ -19591,7 +19591,7 @@
         <v>1082</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>1351</v>
+        <v>1345</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>894</v>
@@ -19621,7 +19621,7 @@
         <v>1255</v>
       </c>
       <c r="T41" s="3" t="s">
-        <v>1470</v>
+        <v>1464</v>
       </c>
       <c r="U41" s="7"/>
       <c r="V41" s="10">
@@ -19658,7 +19658,7 @@
         <v>1082</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>1352</v>
+        <v>1346</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>897</v>
@@ -19691,7 +19691,7 @@
         <v>1255</v>
       </c>
       <c r="T42" s="3" t="s">
-        <v>1471</v>
+        <v>1465</v>
       </c>
       <c r="U42" s="7" t="s">
         <v>748</v>
@@ -19732,7 +19732,7 @@
         <v>1082</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>1353</v>
+        <v>1347</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>844</v>
@@ -19760,16 +19760,16 @@
         <v>736</v>
       </c>
       <c r="Q43" s="3">
-        <v>0.34289999999999998</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>1257</v>
+        <v>1498</v>
       </c>
       <c r="S43" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T43" s="3" t="s">
-        <v>1472</v>
+        <v>1466</v>
       </c>
       <c r="U43" s="7" t="s">
         <v>607</v>
@@ -19810,7 +19810,7 @@
         <v>1082</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>1354</v>
+        <v>1348</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>788</v>
@@ -19841,7 +19841,7 @@
         <v>1255</v>
       </c>
       <c r="T44" s="3" t="s">
-        <v>1473</v>
+        <v>1467</v>
       </c>
       <c r="U44" s="7" t="s">
         <v>583</v>
@@ -19882,7 +19882,7 @@
         <v>1082</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>1355</v>
+        <v>1349</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>846</v>
@@ -19913,13 +19913,13 @@
         <v>0.97599999999999998</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="S45" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>1474</v>
+        <v>1468</v>
       </c>
       <c r="U45" s="7"/>
       <c r="V45" s="10">
@@ -19954,10 +19954,10 @@
         <v>445</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>1350</v>
+        <v>1344</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>898</v>
@@ -19987,7 +19987,7 @@
         <v>1255</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>1350</v>
+        <v>1344</v>
       </c>
       <c r="U46" s="7" t="s">
         <v>145</v>
@@ -20022,10 +20022,10 @@
         <v>317</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>1356</v>
+        <v>1350</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>784</v>
@@ -20056,13 +20056,13 @@
         <v>1.9245000000000001</v>
       </c>
       <c r="R47" s="5" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="S47" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>1356</v>
+        <v>1350</v>
       </c>
       <c r="U47" s="7" t="s">
         <v>635</v>
@@ -20097,10 +20097,10 @@
         <v>455</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>785</v>
@@ -20128,7 +20128,7 @@
         <v>1255</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>1357</v>
+        <v>1351</v>
       </c>
       <c r="U48" s="7" t="s">
         <v>590</v>
@@ -20163,10 +20163,10 @@
         <v>455</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>1358</v>
+        <v>1352</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>786</v>
@@ -20194,7 +20194,7 @@
         <v>1255</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>1358</v>
+        <v>1352</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>585</v>
@@ -20283,10 +20283,10 @@
         <v>317</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>1359</v>
+        <v>1353</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>777</v>
@@ -20314,7 +20314,7 @@
         <v>1255</v>
       </c>
       <c r="T51" s="3" t="s">
-        <v>1359</v>
+        <v>1353</v>
       </c>
       <c r="U51" s="7" t="s">
         <v>361</v>
@@ -20358,13 +20358,13 @@
         <v>1082</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>1437</v>
+        <v>1431</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>1438</v>
+        <v>1432</v>
       </c>
       <c r="K52" s="3">
         <v>1.1299999999999999</v>
@@ -20388,7 +20388,7 @@
         <v>1255</v>
       </c>
       <c r="T52" s="3" t="s">
-        <v>1360</v>
+        <v>1354</v>
       </c>
       <c r="U52" s="7" t="s">
         <v>290</v>
@@ -20421,7 +20421,7 @@
         <v>1082</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>1361</v>
+        <v>1355</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>88</v>
@@ -20450,13 +20450,13 @@
         <v>1.12375</v>
       </c>
       <c r="R53" s="5" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="S53" s="8" t="s">
         <v>874</v>
       </c>
       <c r="T53" s="5" t="s">
-        <v>1488</v>
+        <v>1482</v>
       </c>
       <c r="U53" s="7"/>
       <c r="V53" s="10">
@@ -20489,10 +20489,10 @@
         <v>455</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>496</v>
@@ -20522,7 +20522,7 @@
         <v>1255</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>1378</v>
+        <v>1372</v>
       </c>
       <c r="U54" s="7" t="s">
         <v>583</v>
@@ -20558,16 +20558,16 @@
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>111</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3">
@@ -20594,7 +20594,7 @@
         <v>1255</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>1379</v>
+        <v>1373</v>
       </c>
       <c r="U55" s="7"/>
       <c r="V55" s="10">
@@ -20630,10 +20630,10 @@
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>1380</v>
+        <v>1374</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>903</v>
@@ -20666,7 +20666,7 @@
         <v>1255</v>
       </c>
       <c r="T56" s="5" t="s">
-        <v>1380</v>
+        <v>1374</v>
       </c>
       <c r="U56" s="7"/>
       <c r="V56" s="10">
@@ -20704,7 +20704,7 @@
         <v>1082</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>1381</v>
+        <v>1375</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>796</v>
@@ -20732,7 +20732,7 @@
         <v>1255</v>
       </c>
       <c r="T57" s="5" t="s">
-        <v>1381</v>
+        <v>1375</v>
       </c>
       <c r="U57" s="7" t="s">
         <v>145</v>
@@ -20767,10 +20767,10 @@
         <v>455</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>1382</v>
+        <v>1376</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>508</v>
@@ -20780,7 +20780,7 @@
         <v>1.3</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="M58" s="3" t="s">
         <v>833</v>
@@ -20798,7 +20798,7 @@
         <v>874</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>1382</v>
+        <v>1376</v>
       </c>
       <c r="U58" s="7" t="s">
         <v>590</v>
@@ -20833,7 +20833,7 @@
         <v>445</v>
       </c>
       <c r="E59" s="22" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
       <c r="H59" s="22" t="s">
         <v>905</v>
@@ -20891,10 +20891,10 @@
         <v>317</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>1383</v>
+        <v>1377</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>907</v>
@@ -20924,7 +20924,7 @@
         <v>1255</v>
       </c>
       <c r="T60" s="5" t="s">
-        <v>1383</v>
+        <v>1377</v>
       </c>
       <c r="U60" s="7"/>
       <c r="V60" s="10">
@@ -20960,7 +20960,7 @@
         <v>1082</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>1384</v>
+        <v>1378</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>872</v>
@@ -20990,7 +20990,7 @@
         <v>1255</v>
       </c>
       <c r="T61" s="5" t="s">
-        <v>1384</v>
+        <v>1378</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>263</v>
@@ -21086,7 +21086,7 @@
         <v>1082</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>1362</v>
+        <v>1356</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>90</v>
@@ -21114,13 +21114,13 @@
         <v>0.2495</v>
       </c>
       <c r="R63" s="5" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="S63" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T63" s="5" t="s">
-        <v>1489</v>
+        <v>1483</v>
       </c>
       <c r="U63" s="7" t="s">
         <v>145</v>
@@ -21188,7 +21188,7 @@
         <v>1255</v>
       </c>
       <c r="T64" s="5" t="s">
-        <v>1490</v>
+        <v>1484</v>
       </c>
       <c r="U64" s="7" t="s">
         <v>303</v>
@@ -21258,13 +21258,13 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="R65" s="5" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="S65" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T65" s="5" t="s">
-        <v>1491</v>
+        <v>1485</v>
       </c>
       <c r="U65" s="7" t="s">
         <v>264</v>
@@ -21304,7 +21304,7 @@
         <v>1082</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>1385</v>
+        <v>1379</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>797</v>
@@ -21334,7 +21334,7 @@
         <v>1255</v>
       </c>
       <c r="T66" s="5" t="s">
-        <v>1385</v>
+        <v>1379</v>
       </c>
       <c r="U66" s="7"/>
       <c r="V66" s="10">
@@ -21368,10 +21368,10 @@
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>1386</v>
+        <v>1380</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>911</v>
@@ -21402,13 +21402,13 @@
         <v>12</v>
       </c>
       <c r="R67" s="5" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="S67" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T67" s="5" t="s">
-        <v>1386</v>
+        <v>1380</v>
       </c>
       <c r="U67" s="7"/>
       <c r="V67" s="10">
@@ -21444,10 +21444,10 @@
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>1363</v>
+        <v>1357</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>799</v>
@@ -21478,13 +21478,13 @@
         <v>3.6</v>
       </c>
       <c r="R68" s="3" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="S68" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T68" s="5" t="s">
-        <v>1492</v>
+        <v>1486</v>
       </c>
       <c r="U68" s="7" t="s">
         <v>583</v>
@@ -21522,10 +21522,10 @@
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>1387</v>
+        <v>1381</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>518</v>
@@ -21556,7 +21556,7 @@
         <v>1255</v>
       </c>
       <c r="T69" s="5" t="s">
-        <v>1387</v>
+        <v>1381</v>
       </c>
       <c r="U69" s="7" t="s">
         <v>643</v>
@@ -21594,10 +21594,10 @@
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>1388</v>
+        <v>1382</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>801</v>
@@ -21628,7 +21628,7 @@
         <v>1255</v>
       </c>
       <c r="T70" s="5" t="s">
-        <v>1388</v>
+        <v>1382</v>
       </c>
       <c r="U70" s="7" t="s">
         <v>583</v>
@@ -21666,10 +21666,10 @@
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>1389</v>
+        <v>1383</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>802</v>
@@ -21700,7 +21700,7 @@
         <v>1255</v>
       </c>
       <c r="T71" s="3" t="s">
-        <v>1389</v>
+        <v>1383</v>
       </c>
       <c r="U71" s="7" t="s">
         <v>265</v>
@@ -21740,7 +21740,7 @@
         <v>1082</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>1390</v>
+        <v>1384</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>803</v>
@@ -21770,7 +21770,7 @@
         <v>1255</v>
       </c>
       <c r="T72" s="3" t="s">
-        <v>1390</v>
+        <v>1384</v>
       </c>
       <c r="U72" s="7" t="s">
         <v>159</v>
@@ -21809,7 +21809,7 @@
         <v>1146</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>1364</v>
+        <v>1358</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>805</v>
@@ -21842,10 +21842,10 @@
         <v>874</v>
       </c>
       <c r="T73" s="3" t="s">
-        <v>1493</v>
+        <v>1487</v>
       </c>
       <c r="U73" s="7" t="s">
-        <v>1373</v>
+        <v>1367</v>
       </c>
       <c r="V73" s="10">
         <v>38</v>
@@ -21879,10 +21879,10 @@
         <v>445</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>1391</v>
+        <v>1385</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>913</v>
@@ -21912,7 +21912,7 @@
         <v>1255</v>
       </c>
       <c r="T74" s="3" t="s">
-        <v>1391</v>
+        <v>1385</v>
       </c>
       <c r="U74" s="7" t="s">
         <v>203</v>
@@ -21933,7 +21933,7 @@
         <v>22</v>
       </c>
       <c r="AB74" s="3" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="75" spans="1:28" ht="60" x14ac:dyDescent="0.25">
@@ -21952,7 +21952,7 @@
         <v>1082</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>1392</v>
+        <v>1386</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>875</v>
@@ -21985,7 +21985,7 @@
         <v>1255</v>
       </c>
       <c r="T75" s="3" t="s">
-        <v>1392</v>
+        <v>1386</v>
       </c>
       <c r="U75" s="7" t="s">
         <v>647</v>
@@ -22023,10 +22023,10 @@
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>1393</v>
+        <v>1387</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>809</v>
@@ -22054,16 +22054,16 @@
         <v>609</v>
       </c>
       <c r="Q76" s="3">
-        <v>4.8768000000000002</v>
+        <v>3.67</v>
       </c>
       <c r="R76" s="5" t="s">
-        <v>1265</v>
+        <v>1499</v>
       </c>
       <c r="S76" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T76" s="3" t="s">
-        <v>1393</v>
+        <v>1387</v>
       </c>
       <c r="U76" s="7" t="s">
         <v>611</v>
@@ -22101,10 +22101,10 @@
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>1394</v>
+        <v>1388</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>811</v>
@@ -22135,13 +22135,13 @@
         <v>0.91439999999999999</v>
       </c>
       <c r="R77" s="5" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="S77" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T77" s="3" t="s">
-        <v>1394</v>
+        <v>1388</v>
       </c>
       <c r="U77" s="7" t="s">
         <v>583</v>
@@ -22181,7 +22181,7 @@
         <v>1082</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>1395</v>
+        <v>1389</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>776</v>
@@ -22209,7 +22209,7 @@
         <v>1255</v>
       </c>
       <c r="T78" s="3" t="s">
-        <v>1395</v>
+        <v>1389</v>
       </c>
       <c r="U78" s="7" t="s">
         <v>696</v>
@@ -22250,10 +22250,10 @@
         <v>445</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>1396</v>
+        <v>1390</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>813</v>
@@ -22281,7 +22281,7 @@
         <v>1255</v>
       </c>
       <c r="T79" s="3" t="s">
-        <v>1396</v>
+        <v>1390</v>
       </c>
       <c r="U79" s="7" t="s">
         <v>270</v>
@@ -22319,7 +22319,7 @@
         <v>1082</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>1397</v>
+        <v>1391</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>375</v>
@@ -22347,7 +22347,7 @@
         <v>874</v>
       </c>
       <c r="T80" s="3" t="s">
-        <v>1397</v>
+        <v>1391</v>
       </c>
       <c r="U80" s="7" t="s">
         <v>832</v>
@@ -22382,7 +22382,7 @@
         <v>1082</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>1365</v>
+        <v>1359</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>379</v>
@@ -22398,7 +22398,7 @@
         <v>833</v>
       </c>
       <c r="N81" s="3" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="O81" s="3">
         <v>2</v>
@@ -22410,7 +22410,7 @@
         <v>874</v>
       </c>
       <c r="T81" s="3" t="s">
-        <v>1494</v>
+        <v>1488</v>
       </c>
       <c r="U81" s="7" t="s">
         <v>380</v>
@@ -22445,7 +22445,7 @@
         <v>1082</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>1398</v>
+        <v>1392</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>382</v>
@@ -22475,13 +22475,13 @@
         <v>0.74390000000000001</v>
       </c>
       <c r="R82" s="5" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="S82" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T82" s="3" t="s">
-        <v>1398</v>
+        <v>1392</v>
       </c>
       <c r="U82" s="7"/>
       <c r="V82" s="10">
@@ -22511,10 +22511,10 @@
         <v>317</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>1399</v>
+        <v>1393</v>
       </c>
       <c r="I83" s="7"/>
       <c r="K83" s="3">
@@ -22539,7 +22539,7 @@
         <v>874</v>
       </c>
       <c r="T83" s="3" t="s">
-        <v>1399</v>
+        <v>1393</v>
       </c>
       <c r="U83" s="7" t="s">
         <v>835</v>
@@ -22576,7 +22576,7 @@
         <v>1082</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>1366</v>
+        <v>1360</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>393</v>
@@ -22607,7 +22607,7 @@
         <v>874</v>
       </c>
       <c r="T84" s="3" t="s">
-        <v>1495</v>
+        <v>1489</v>
       </c>
       <c r="U84" s="7" t="s">
         <v>395</v>
@@ -22650,7 +22650,7 @@
         <v>1082</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>1400</v>
+        <v>1394</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>397</v>
@@ -22679,13 +22679,13 @@
         <v>0.105</v>
       </c>
       <c r="R85" s="5" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="S85" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T85" s="3" t="s">
-        <v>1400</v>
+        <v>1394</v>
       </c>
       <c r="U85" s="7" t="s">
         <v>399</v>
@@ -22719,16 +22719,16 @@
         <v>4</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>1439</v>
+        <v>1433</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>1440</v>
+        <v>1434</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>1401</v>
+        <v>1395</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>915</v>
@@ -22758,7 +22758,7 @@
         <v>1255</v>
       </c>
       <c r="T86" s="3" t="s">
-        <v>1401</v>
+        <v>1395</v>
       </c>
       <c r="U86" s="7" t="s">
         <v>271</v>
@@ -22797,10 +22797,10 @@
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>1402</v>
+        <v>1396</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>133</v>
@@ -22868,10 +22868,10 @@
         <v>445</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>1403</v>
+        <v>1397</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>917</v>
@@ -22919,7 +22919,7 @@
         <v>17</v>
       </c>
       <c r="AB88" s="4" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="89" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -22939,7 +22939,7 @@
         <v>1082</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>1404</v>
+        <v>1398</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>815</v>
@@ -22967,7 +22967,7 @@
         <v>1255</v>
       </c>
       <c r="T89" s="3" t="s">
-        <v>1404</v>
+        <v>1398</v>
       </c>
       <c r="U89" s="7" t="s">
         <v>402</v>
@@ -23009,7 +23009,7 @@
         <v>1082</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>1405</v>
+        <v>1399</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>919</v>
@@ -23042,7 +23042,7 @@
         <v>1255</v>
       </c>
       <c r="T90" s="3" t="s">
-        <v>1405</v>
+        <v>1399</v>
       </c>
       <c r="U90" s="7"/>
       <c r="V90" s="10">
@@ -23077,10 +23077,10 @@
         <v>455</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>1406</v>
+        <v>1400</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>878</v>
@@ -23110,7 +23110,7 @@
         <v>1255</v>
       </c>
       <c r="T91" s="3" t="s">
-        <v>1406</v>
+        <v>1400</v>
       </c>
       <c r="U91" s="7"/>
       <c r="V91" s="10">
@@ -23198,7 +23198,7 @@
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>1106</v>
@@ -23232,7 +23232,7 @@
         <v>1255</v>
       </c>
       <c r="T93" s="3" t="s">
-        <v>1496</v>
+        <v>1490</v>
       </c>
       <c r="U93" s="7" t="s">
         <v>583</v>
@@ -23270,10 +23270,10 @@
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>1407</v>
+        <v>1401</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>51</v>
@@ -23301,16 +23301,16 @@
         <v>1107</v>
       </c>
       <c r="Q94" s="3">
-        <v>41.91</v>
+        <v>35</v>
       </c>
       <c r="R94" s="5" t="s">
-        <v>1269</v>
+        <v>1500</v>
       </c>
       <c r="S94" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T94" s="3" t="s">
-        <v>1407</v>
+        <v>1401</v>
       </c>
       <c r="U94" s="7" t="s">
         <v>252</v>
@@ -23348,10 +23348,10 @@
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>1408</v>
+        <v>1402</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>921</v>
@@ -23384,7 +23384,7 @@
         <v>1255</v>
       </c>
       <c r="T95" s="3" t="s">
-        <v>1408</v>
+        <v>1402</v>
       </c>
       <c r="U95" s="7" t="s">
         <v>583</v>
@@ -23422,10 +23422,10 @@
       </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>1409</v>
+        <v>1403</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>409</v>
@@ -23458,7 +23458,7 @@
         <v>1255</v>
       </c>
       <c r="T96" s="3" t="s">
-        <v>1409</v>
+        <v>1403</v>
       </c>
       <c r="U96" s="7" t="s">
         <v>412</v>
@@ -23496,10 +23496,10 @@
       </c>
       <c r="E97" s="3"/>
       <c r="F97" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>1410</v>
+        <v>1404</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>925</v>
@@ -23532,7 +23532,7 @@
         <v>1255</v>
       </c>
       <c r="T97" s="3" t="s">
-        <v>1410</v>
+        <v>1404</v>
       </c>
       <c r="U97" s="7" t="s">
         <v>273</v>
@@ -23566,10 +23566,10 @@
         <v>317</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>1411</v>
+        <v>1405</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>417</v>
@@ -23599,7 +23599,7 @@
         <v>874</v>
       </c>
       <c r="T98" s="3" t="s">
-        <v>1411</v>
+        <v>1405</v>
       </c>
       <c r="U98" s="7" t="s">
         <v>418</v>
@@ -23634,16 +23634,16 @@
         <v>455</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>1441</v>
+        <v>1435</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>1412</v>
+        <v>1406</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>1444</v>
+        <v>1438</v>
       </c>
       <c r="I99" s="7"/>
       <c r="K99" s="3">
@@ -23668,7 +23668,7 @@
         <v>1255</v>
       </c>
       <c r="T99" s="3" t="s">
-        <v>1443</v>
+        <v>1437</v>
       </c>
       <c r="U99" s="7" t="s">
         <v>583</v>
@@ -23740,7 +23740,7 @@
         <v>1255</v>
       </c>
       <c r="T100" s="3" t="s">
-        <v>1497</v>
+        <v>1491</v>
       </c>
       <c r="U100" s="7" t="s">
         <v>712</v>
@@ -23778,10 +23778,10 @@
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>1367</v>
+        <v>1361</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>545</v>
@@ -23812,16 +23812,16 @@
         <v>0.91439999999999999</v>
       </c>
       <c r="R101" s="5" t="s">
-        <v>1270</v>
+        <v>1503</v>
       </c>
       <c r="S101" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T101" s="3" t="s">
-        <v>1498</v>
+        <v>1492</v>
       </c>
       <c r="U101" s="7" t="s">
-        <v>1368</v>
+        <v>1362</v>
       </c>
       <c r="V101" s="10">
         <v>32</v>
@@ -23855,10 +23855,10 @@
         <v>455</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>1413</v>
+        <v>1407</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>847</v>
@@ -23888,7 +23888,7 @@
         <v>874</v>
       </c>
       <c r="T102" s="3" t="s">
-        <v>1413</v>
+        <v>1407</v>
       </c>
       <c r="U102" s="7" t="s">
         <v>595</v>
@@ -23927,7 +23927,7 @@
         <v>1082</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>1414</v>
+        <v>1408</v>
       </c>
       <c r="H103" s="4" t="s">
         <v>928</v>
@@ -23995,7 +23995,7 @@
         <v>1082</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>1415</v>
+        <v>1409</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>929</v>
@@ -24028,7 +24028,7 @@
         <v>1255</v>
       </c>
       <c r="T104" s="3" t="s">
-        <v>1415</v>
+        <v>1409</v>
       </c>
       <c r="U104" s="7" t="s">
         <v>428</v>
@@ -24053,7 +24053,7 @@
     </row>
     <row r="105" spans="1:28" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
       <c r="B105" s="3" t="s">
         <v>214</v>
@@ -24068,7 +24068,7 @@
         <v>1082</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>1416</v>
+        <v>1410</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>931</v>
@@ -24096,7 +24096,7 @@
         <v>1255</v>
       </c>
       <c r="T105" s="3" t="s">
-        <v>1416</v>
+        <v>1410</v>
       </c>
       <c r="U105" s="7" t="s">
         <v>274</v>
@@ -24134,7 +24134,7 @@
         <v>1082</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>1417</v>
+        <v>1411</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>132</v>
@@ -24162,7 +24162,7 @@
         <v>874</v>
       </c>
       <c r="T106" s="3" t="s">
-        <v>1417</v>
+        <v>1411</v>
       </c>
       <c r="U106" s="7" t="s">
         <v>275</v>
@@ -24255,7 +24255,7 @@
         <v>1082</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>1418</v>
+        <v>1412</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>555</v>
@@ -24283,7 +24283,7 @@
         <v>1255</v>
       </c>
       <c r="T108" s="3" t="s">
-        <v>1418</v>
+        <v>1412</v>
       </c>
       <c r="U108" s="7" t="s">
         <v>159</v>
@@ -24382,7 +24382,7 @@
         <v>1146</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>1419</v>
+        <v>1413</v>
       </c>
       <c r="H110" s="4"/>
       <c r="I110" s="13"/>
@@ -24443,10 +24443,10 @@
       </c>
       <c r="E111" s="3"/>
       <c r="F111" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>1420</v>
+        <v>1414</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>556</v>
@@ -24477,7 +24477,7 @@
         <v>874</v>
       </c>
       <c r="T111" s="3" t="s">
-        <v>1499</v>
+        <v>1493</v>
       </c>
       <c r="U111" s="7" t="s">
         <v>595</v>
@@ -24542,13 +24542,13 @@
         <v>445</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>1442</v>
+        <v>1436</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>1421</v>
+        <v>1415</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>932</v>
@@ -24581,7 +24581,7 @@
         <v>1255</v>
       </c>
       <c r="T113" s="3" t="s">
-        <v>1421</v>
+        <v>1415</v>
       </c>
       <c r="U113" s="7" t="s">
         <v>159</v>
@@ -24606,7 +24606,7 @@
     </row>
     <row r="114" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>229</v>
@@ -24622,7 +24622,7 @@
         <v>1082</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>934</v>
@@ -24655,7 +24655,7 @@
         <v>1255</v>
       </c>
       <c r="T114" s="3" t="s">
-        <v>1422</v>
+        <v>1416</v>
       </c>
       <c r="U114" s="7" t="s">
         <v>276</v>
@@ -24692,10 +24692,10 @@
         <v>445</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>1369</v>
+        <v>1363</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>123</v>
@@ -24723,7 +24723,7 @@
         <v>874</v>
       </c>
       <c r="T115" s="3" t="s">
-        <v>1500</v>
+        <v>1494</v>
       </c>
       <c r="U115" s="7" t="s">
         <v>278</v>
@@ -24761,7 +24761,7 @@
         <v>1082</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>558</v>
@@ -24789,7 +24789,7 @@
         <v>874</v>
       </c>
       <c r="T116" s="3" t="s">
-        <v>1423</v>
+        <v>1417</v>
       </c>
       <c r="U116" s="7" t="s">
         <v>594</v>
@@ -24824,10 +24824,10 @@
         <v>455</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>1424</v>
+        <v>1418</v>
       </c>
       <c r="H117" s="3" t="s">
         <v>562</v>
@@ -24855,7 +24855,7 @@
         <v>874</v>
       </c>
       <c r="T117" s="3" t="s">
-        <v>1424</v>
+        <v>1418</v>
       </c>
       <c r="U117" s="7" t="s">
         <v>594</v>
@@ -24917,7 +24917,7 @@
         <v>1255</v>
       </c>
       <c r="U118" s="23" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
       <c r="V118" s="24">
         <v>768</v>
@@ -24946,13 +24946,13 @@
         <v>455</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>1425</v>
+        <v>1419</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>564</v>
@@ -24983,7 +24983,7 @@
         <v>1255</v>
       </c>
       <c r="T119" s="3" t="s">
-        <v>1425</v>
+        <v>1419</v>
       </c>
       <c r="U119" s="7" t="s">
         <v>583</v>
@@ -25234,10 +25234,10 @@
         <v>455</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>1426</v>
+        <v>1420</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>882</v>
@@ -25264,16 +25264,16 @@
         <v>1135</v>
       </c>
       <c r="Q124" s="3">
-        <v>19.05</v>
+        <v>15</v>
       </c>
       <c r="R124" s="5" t="s">
-        <v>1271</v>
+        <v>1502</v>
       </c>
       <c r="S124" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T124" s="3" t="s">
-        <v>1426</v>
+        <v>1420</v>
       </c>
       <c r="U124" s="7" t="s">
         <v>603</v>
@@ -25312,7 +25312,7 @@
         <v>1082</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>1427</v>
+        <v>1421</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>944</v>
@@ -25345,7 +25345,7 @@
         <v>1255</v>
       </c>
       <c r="T125" s="3" t="s">
-        <v>1427</v>
+        <v>1421</v>
       </c>
       <c r="U125" s="7"/>
       <c r="V125" s="10">
@@ -25384,7 +25384,7 @@
         <v>1082</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>1370</v>
+        <v>1364</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>946</v>
@@ -25415,13 +25415,13 @@
         <v>1.39</v>
       </c>
       <c r="R126" s="3" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
       <c r="S126" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T126" s="3" t="s">
-        <v>1501</v>
+        <v>1495</v>
       </c>
       <c r="U126" s="7" t="s">
         <v>594</v>
@@ -25455,7 +25455,7 @@
         <v>1082</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>853</v>
@@ -25485,7 +25485,7 @@
         <v>1255</v>
       </c>
       <c r="T127" s="3" t="s">
-        <v>1428</v>
+        <v>1422</v>
       </c>
       <c r="U127" s="7" t="s">
         <v>444</v>
@@ -25521,10 +25521,10 @@
       </c>
       <c r="E128" s="3"/>
       <c r="F128" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>1429</v>
+        <v>1423</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>884</v>
@@ -25557,7 +25557,7 @@
         <v>1255</v>
       </c>
       <c r="T128" s="3" t="s">
-        <v>1429</v>
+        <v>1423</v>
       </c>
       <c r="U128" s="7" t="s">
         <v>277</v>
@@ -25594,10 +25594,10 @@
         <v>455</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>1371</v>
+        <v>1365</v>
       </c>
       <c r="I129" s="7"/>
       <c r="K129" s="3">
@@ -25619,16 +25619,16 @@
         <v>1140</v>
       </c>
       <c r="Q129" s="3">
-        <v>3.25</v>
+        <v>2.11</v>
       </c>
       <c r="R129" s="5" t="s">
-        <v>1272</v>
+        <v>1501</v>
       </c>
       <c r="S129" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T129" s="3" t="s">
-        <v>1502</v>
+        <v>1496</v>
       </c>
       <c r="U129" s="7" t="s">
         <v>583</v>
@@ -25657,19 +25657,19 @@
         <v>292</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>1451</v>
+        <v>1445</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>445</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>1452</v>
+        <v>1446</v>
       </c>
       <c r="F130" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>1430</v>
+        <v>1424</v>
       </c>
       <c r="H130" s="7" t="s">
         <v>947</v>
@@ -25699,7 +25699,7 @@
         <v>1255</v>
       </c>
       <c r="T130" s="3" t="s">
-        <v>1503</v>
+        <v>1497</v>
       </c>
       <c r="U130" s="7" t="s">
         <v>781</v>
@@ -25720,7 +25720,7 @@
         <v>34</v>
       </c>
       <c r="AB130" s="3" t="s">
-        <v>1453</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="131" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -25768,7 +25768,7 @@
         <v>4</v>
       </c>
       <c r="R131" s="3" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="S131" s="3" t="s">
         <v>1255</v>
@@ -25795,7 +25795,7 @@
         <v>17</v>
       </c>
       <c r="AB131" s="3" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="132" spans="1:28" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -25812,10 +25812,10 @@
         <v>455</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>1431</v>
+        <v>1425</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>950</v>
@@ -25845,7 +25845,7 @@
         <v>1255</v>
       </c>
       <c r="T132" s="3" t="s">
-        <v>1431</v>
+        <v>1425</v>
       </c>
       <c r="U132" s="7" t="s">
         <v>583</v>
@@ -25917,19 +25917,19 @@
     <hyperlink ref="R30" r:id="rId46" xr:uid="{21076D40-9243-4168-B697-514BE758B3C7}"/>
     <hyperlink ref="R34" r:id="rId47" display="https://doi.org/10.1111/j.1439-037X.2010.00429.x ; I got this value by taking the average height of the 15 white bars (i.e. non-salt-stress condition) in figure 1 a using image j, converting heights in pixels to heights in cm based on the scale of the y-axis" xr:uid="{3863F86F-3D00-4730-95EF-1A5BD52DCFDD}"/>
     <hyperlink ref="B94" r:id="rId48" xr:uid="{159829CC-A986-4B44-94EC-5057ABB2E9DB}"/>
-    <hyperlink ref="R43" r:id="rId49" xr:uid="{015F3695-EFC5-4E34-8CFF-723E20AE597C}"/>
+    <hyperlink ref="R43" r:id="rId49" display="http://www.missouribotanicalgarden.org/gardens-gardening/your-garden/plant-finder/plant-details/kc/e454/cucurbita-argyrosperma.aspx ; average of height range reported on website for missouri botanical garden, then converted to meters; Retrieved 2023-10-25" xr:uid="{015F3695-EFC5-4E34-8CFF-723E20AE597C}"/>
     <hyperlink ref="R47" r:id="rId50" xr:uid="{6270B348-F18A-471A-8C5C-05D7C6485070}"/>
     <hyperlink ref="R53" r:id="rId51" xr:uid="{71ECD90B-8D49-4F77-AE01-57307CAE0BB5}"/>
     <hyperlink ref="R63" r:id="rId52" xr:uid="{1F8F5272-884C-4567-8446-2E087E065EF1}"/>
     <hyperlink ref="R65" r:id="rId53" xr:uid="{EF670AE0-7FBB-40BB-BFC8-04BEF555DAF0}"/>
     <hyperlink ref="R67" r:id="rId54" xr:uid="{9F1AAC25-C8E9-4311-B97C-F460205DDA81}"/>
-    <hyperlink ref="R76" r:id="rId55" xr:uid="{EE95F07B-2C68-4858-8728-1BC9B5A64399}"/>
+    <hyperlink ref="R76" r:id="rId55" display="http://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=282778 ; average of height range reported by Missouri Botanical Garden (12 - 20 feet), then converted to meters, suggests a height of 4.8768 m" xr:uid="{EE95F07B-2C68-4858-8728-1BC9B5A64399}"/>
     <hyperlink ref="R77" r:id="rId56" xr:uid="{62774BFE-6D2C-4DA5-8A58-148287B9075E}"/>
     <hyperlink ref="R82" r:id="rId57" xr:uid="{5318486D-287E-4E41-85DA-DED68BDC3523}"/>
     <hyperlink ref="R85" r:id="rId58" xr:uid="{1F22773A-8196-4D43-8217-BB3DD0E29E41}"/>
-    <hyperlink ref="R94" r:id="rId59" xr:uid="{45F148EB-1C96-4891-9E9D-8AE8F70FEEB5}"/>
+    <hyperlink ref="R94" r:id="rId59" display="https://owic.oregonstate.edu/black-cottonwood-populus-trichocarpa ; average of range given in text (125 - 150 ft), then converted to meters, suggests average height of 41.91 m" xr:uid="{45F148EB-1C96-4891-9E9D-8AE8F70FEEB5}"/>
     <hyperlink ref="R101" r:id="rId60" xr:uid="{CD533664-41C6-4EA6-B220-C9D568EFF065}"/>
-    <hyperlink ref="R124" r:id="rId61" display="https://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=283438 ; In its native habitat, it may grow to as much as 50-75' tall over time, but as an indoor plant it grows much shorter ; I took the average of this range then converted it to meters" xr:uid="{F382B955-CABD-4C97-A40A-74C06333904B}"/>
+    <hyperlink ref="R124" r:id="rId61" display="https://www.missouribotanicalgarden.org/PlantFinder/PlantFinderDetails.aspx?taxonid=283438 ; In its native habitat, it may grow to as much as 50-75' tall over time, but as an indoor plant it grows much shorter ; I took the average of this range then converted it to meters and it suggests a height of 19.05 m " xr:uid="{F382B955-CABD-4C97-A40A-74C06333904B}"/>
     <hyperlink ref="R129" r:id="rId62" display="https://doi.org/10.1002/fes3.500 ; Mean from Table 1" xr:uid="{8C79EE87-526F-46CA-A17F-5DCBEEC5C2AD}"/>
     <hyperlink ref="L25" r:id="rId63" xr:uid="{56E96306-5D5E-4586-B3CD-EEC9B7A62DF8}"/>
     <hyperlink ref="N6" r:id="rId64" xr:uid="{74A214C2-3BDE-42C5-B7EB-C5C079A5F2BC}"/>

</xml_diff>

<commit_message>
update references for genomes used
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198206_2_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198206_2_16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB90D3A-413C-4FE9-B146-2B8C6A84EEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49794B9D-5799-4E99-A9F0-5B167275067F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4253" uniqueCount="1504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4299" uniqueCount="1547">
   <si>
     <t>Species</t>
   </si>
@@ -4549,6 +4549,135 @@
   </si>
   <si>
     <t>https://www.rhododendron.org/descriptionS_taxon.asp?ID=259 ; description from American Rhododendron Society ; gave height as 3 ft, which I then converted to meters</t>
+  </si>
+  <si>
+    <t>A_alpina_V4; GCA_000733195.1; https://doi.org/10.1038/nplants.2014.23</t>
+  </si>
+  <si>
+    <t>GCA_902206195.3</t>
+  </si>
+  <si>
+    <t>GCA_000817695.3</t>
+  </si>
+  <si>
+    <t>GCA_000816755.2</t>
+  </si>
+  <si>
+    <t>GCA_009727055.1</t>
+  </si>
+  <si>
+    <t>ASM1870372v1; GCA_018703725.1; https://doi.org/10.1038/s41588-021-00922-y</t>
+  </si>
+  <si>
+    <t>AST_PRJEB5043_v1; GCA_000751015.1; https://doi.org/10.1126/science.1253435</t>
+  </si>
+  <si>
+    <t>GCA_019426215.1</t>
+  </si>
+  <si>
+    <t>GCA_000340665.2</t>
+  </si>
+  <si>
+    <t>Cs; GCA_000633955.1; https://doi.org/10.1038/ncomms4706</t>
+  </si>
+  <si>
+    <t>AHAU_CSS_1; GCA_004153795.1</t>
+  </si>
+  <si>
+    <t>cs10; GCA_900626175.1</t>
+  </si>
+  <si>
+    <t>v1; v1.1; https://doi.org/10.1038/ng.2669</t>
+  </si>
+  <si>
+    <t>CM334; GCA_000512255.2;  https://doi.org/10.1038/ng.2877</t>
+  </si>
+  <si>
+    <t>GCA_014183005.1</t>
+  </si>
+  <si>
+    <t>v1.0; v1.0; https://doi.org/10.1038/nature21370</t>
+  </si>
+  <si>
+    <t>Cla97_v1; GCA_000238415.2; https://doi.org/10.1038/ng.2470</t>
+  </si>
+  <si>
+    <t>GCA_003713225.1</t>
+  </si>
+  <si>
+    <t>AUK_PRJEB4211_v1; GCA_900059795.1; https://doi.org/10.1126/science.1255274</t>
+  </si>
+  <si>
+    <t>GCA_901000735.2</t>
+  </si>
+  <si>
+    <t>Melonv4; GCA_902497455.1; https://doi.org/10.3389/fpls.2019.01815</t>
+  </si>
+  <si>
+    <t>v1; v1.0</t>
+  </si>
+  <si>
+    <t>GCA_018691285.1</t>
+  </si>
+  <si>
+    <t>ASM280686v2; GCA_002806865.2</t>
+  </si>
+  <si>
+    <t>Fonio_CM05836; GCA_902859565.1; https://doi.org/10.1038/s41467-020-18329-4</t>
+  </si>
+  <si>
+    <t>v1.0; v1.1; https://doi.org/10.1007/s00122-019-03311-6</t>
+  </si>
+  <si>
+    <t>TDr96_F1_v2_PseudoChromosome; GCA_009730915.1; https://doi.org/10.1073/pnas.2015830117</t>
+  </si>
+  <si>
+    <t>Duzib1.0; GCA_002303985.1</t>
+  </si>
+  <si>
+    <t>EG5; GCA_000442705.1</t>
+  </si>
+  <si>
+    <t>UNIPI_FiCari_1.0; GCA_009761775.1; https://doi.org/10.1038/srep41124</t>
+  </si>
+  <si>
+    <t>Wm82.a4.v1; https://doi.org/10.1111/tpj.14500</t>
+  </si>
+  <si>
+    <t>v1.0; v1.1; https://doi.org/10.1111/tpj.14500</t>
+  </si>
+  <si>
+    <t>ASM2569848v2; GCA_025698485.2</t>
+  </si>
+  <si>
+    <t>v1.0; v1.1; https://doi.org/10.1038/s41588-020-0614-5</t>
+  </si>
+  <si>
+    <t>v2.0; v2.1; https://doi.org/10.1038/s41588-020-0614-5</t>
+  </si>
+  <si>
+    <t>r1.0; r1.2; https://doi.org/10.1038/nature22380</t>
+  </si>
+  <si>
+    <t>ASM2208547v1; GCA_022085475.1</t>
+  </si>
+  <si>
+    <t>Walnut_2.0; GCA_001411555.2; https://doi.org/10.1093/gigascience/giaa050</t>
+  </si>
+  <si>
+    <t>v8; v8; https://doi.org/10.1038/ncomms14953</t>
+  </si>
+  <si>
+    <t>v1; v1; https://doi.org/10.1101/2021.07.23.453237</t>
+  </si>
+  <si>
+    <t>v1.0; v1.0; https://doi.org/10.1111/j.1365-313x.2012.05093.x</t>
+  </si>
+  <si>
+    <t>Lj1.0v1; https://doi.org/10.3390/genes11050483</t>
+  </si>
+  <si>
+    <t>LupAngTanjil_v1.0; GCA_001865875.1; https://doi.org/10.1111/pbi.12615</t>
   </si>
 </sst>
 </file>
@@ -16730,9 +16859,9 @@
   <dimension ref="A1:AB132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17423,6 +17552,9 @@
       <c r="D10" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E10" s="3" t="s">
+        <v>1504</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>1312</v>
       </c>
@@ -17493,6 +17625,9 @@
       <c r="D11" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E11" s="3" t="s">
+        <v>1505</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>1317</v>
       </c>
@@ -17559,6 +17694,9 @@
       </c>
       <c r="D12" s="3" t="s">
         <v>455</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>1506</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>1082</v>
@@ -17710,7 +17848,9 @@
       <c r="D14" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>1507</v>
+      </c>
       <c r="F14" s="3" t="s">
         <v>1082</v>
       </c>
@@ -17788,6 +17928,9 @@
       <c r="D15" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E15" s="3" t="s">
+        <v>1508</v>
+      </c>
       <c r="F15" s="3" t="s">
         <v>1082</v>
       </c>
@@ -18140,6 +18283,9 @@
       <c r="D20" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E20" s="3" t="s">
+        <v>1509</v>
+      </c>
       <c r="F20" s="3" t="s">
         <v>1082</v>
       </c>
@@ -18204,7 +18350,9 @@
       <c r="D21" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>1510</v>
+      </c>
       <c r="F21" s="3" t="s">
         <v>1082</v>
       </c>
@@ -18482,6 +18630,9 @@
       <c r="D25" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E25" s="3" t="s">
+        <v>1511</v>
+      </c>
       <c r="F25" s="3" t="s">
         <v>1312</v>
       </c>
@@ -18543,6 +18694,9 @@
       <c r="D26" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E26" s="3" t="s">
+        <v>1512</v>
+      </c>
       <c r="F26" s="3" t="s">
         <v>1312</v>
       </c>
@@ -18609,6 +18763,9 @@
       <c r="D27" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E27" s="3" t="s">
+        <v>1513</v>
+      </c>
       <c r="F27" s="3" t="s">
         <v>1082</v>
       </c>
@@ -18681,6 +18838,9 @@
       <c r="D28" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E28" s="3" t="s">
+        <v>1514</v>
+      </c>
       <c r="F28" s="3" t="s">
         <v>1312</v>
       </c>
@@ -18749,6 +18909,9 @@
       <c r="D29" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E29" s="3" t="s">
+        <v>1515</v>
+      </c>
       <c r="F29" s="3" t="s">
         <v>1082</v>
       </c>
@@ -18817,7 +18980,9 @@
       <c r="D30" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3" t="s">
+        <v>1516</v>
+      </c>
       <c r="F30" s="3" t="s">
         <v>1082</v>
       </c>
@@ -18893,6 +19058,9 @@
       <c r="D31" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E31" s="3" t="s">
+        <v>1516</v>
+      </c>
       <c r="F31" s="3" t="s">
         <v>1082</v>
       </c>
@@ -18956,8 +19124,12 @@
       <c r="C32" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>1517</v>
+      </c>
       <c r="F32" s="3" t="s">
         <v>1146</v>
       </c>
@@ -19031,6 +19203,9 @@
       <c r="D33" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E33" s="3" t="s">
+        <v>1518</v>
+      </c>
       <c r="F33" s="3" t="s">
         <v>1312</v>
       </c>
@@ -19098,6 +19273,9 @@
       </c>
       <c r="D34" s="3" t="s">
         <v>445</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>1519</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>1082</v>
@@ -19243,9 +19421,11 @@
         <v>43</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="E36" s="3"/>
+        <v>317</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>1520</v>
+      </c>
       <c r="F36" s="3" t="s">
         <v>1082</v>
       </c>
@@ -19319,6 +19499,9 @@
       <c r="D37" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E37" s="3" t="s">
+        <v>1521</v>
+      </c>
       <c r="F37" s="3" t="s">
         <v>1312</v>
       </c>
@@ -19387,6 +19570,9 @@
       <c r="D38" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E38" s="3" t="s">
+        <v>1522</v>
+      </c>
       <c r="F38" s="3" t="s">
         <v>1312</v>
       </c>
@@ -19512,8 +19698,12 @@
       <c r="C40" s="3" t="s">
         <v>729</v>
       </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>1523</v>
+      </c>
       <c r="F40" s="3" t="s">
         <v>1312</v>
       </c>
@@ -19587,6 +19777,9 @@
       <c r="D41" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E41" s="3" t="s">
+        <v>1524</v>
+      </c>
       <c r="F41" s="3" t="s">
         <v>1082</v>
       </c>
@@ -19653,7 +19846,9 @@
       <c r="D42" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>1525</v>
+      </c>
       <c r="F42" s="3" t="s">
         <v>1082</v>
       </c>
@@ -19727,7 +19922,9 @@
       <c r="D43" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>1526</v>
+      </c>
       <c r="F43" s="3" t="s">
         <v>1082</v>
       </c>
@@ -19805,7 +20002,9 @@
       <c r="D44" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>1527</v>
+      </c>
       <c r="F44" s="3" t="s">
         <v>1082</v>
       </c>
@@ -19877,7 +20076,9 @@
       <c r="D45" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>1528</v>
+      </c>
       <c r="F45" s="3" t="s">
         <v>1082</v>
       </c>
@@ -19953,6 +20154,9 @@
       <c r="D46" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E46" s="3" t="s">
+        <v>1529</v>
+      </c>
       <c r="F46" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20021,6 +20225,9 @@
       <c r="D47" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E47" s="3" t="s">
+        <v>1530</v>
+      </c>
       <c r="F47" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20096,6 +20303,9 @@
       <c r="D48" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E48" s="3" t="s">
+        <v>1531</v>
+      </c>
       <c r="F48" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20162,6 +20372,9 @@
       <c r="D49" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E49" s="3" t="s">
+        <v>1532</v>
+      </c>
       <c r="F49" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20282,6 +20495,9 @@
       <c r="D51" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E51" s="3" t="s">
+        <v>1533</v>
+      </c>
       <c r="F51" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20354,6 +20570,9 @@
       <c r="D52" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E52" s="3" t="s">
+        <v>1534</v>
+      </c>
       <c r="F52" s="3" t="s">
         <v>1082</v>
       </c>
@@ -20416,7 +20635,9 @@
       <c r="D53" s="8" t="s">
         <v>445</v>
       </c>
-      <c r="E53" s="8"/>
+      <c r="E53" s="8" t="s">
+        <v>1535</v>
+      </c>
       <c r="F53" s="8" t="s">
         <v>1082</v>
       </c>
@@ -20488,6 +20709,9 @@
       <c r="D54" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E54" s="3" t="s">
+        <v>1536</v>
+      </c>
       <c r="F54" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20556,7 +20780,9 @@
       <c r="D55" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>1537</v>
+      </c>
       <c r="F55" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20628,7 +20854,9 @@
       <c r="D56" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E56" s="3"/>
+      <c r="E56" s="3" t="s">
+        <v>1538</v>
+      </c>
       <c r="F56" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20700,6 +20928,9 @@
       <c r="D57" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E57" s="3" t="s">
+        <v>1539</v>
+      </c>
       <c r="F57" s="3" t="s">
         <v>1082</v>
       </c>
@@ -20766,6 +20997,9 @@
       <c r="D58" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E58" s="3" t="s">
+        <v>1540</v>
+      </c>
       <c r="F58" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20890,6 +21124,9 @@
       <c r="D60" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E60" s="3" t="s">
+        <v>1541</v>
+      </c>
       <c r="F60" s="3" t="s">
         <v>1312</v>
       </c>
@@ -20956,6 +21193,9 @@
       <c r="D61" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E61" s="3" t="s">
+        <v>1542</v>
+      </c>
       <c r="F61" s="3" t="s">
         <v>1082</v>
       </c>
@@ -21082,6 +21322,9 @@
       <c r="D63" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E63" s="3" t="s">
+        <v>1543</v>
+      </c>
       <c r="F63" s="3" t="s">
         <v>1082</v>
       </c>
@@ -21154,6 +21397,9 @@
       <c r="D64" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E64" s="3" t="s">
+        <v>1544</v>
+      </c>
       <c r="F64" s="3" t="s">
         <v>1082</v>
       </c>
@@ -21222,7 +21468,9 @@
       <c r="D65" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>1545</v>
+      </c>
       <c r="F65" s="3" t="s">
         <v>1082</v>
       </c>
@@ -21299,6 +21547,9 @@
       </c>
       <c r="D66" s="3" t="s">
         <v>317</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>1546</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>1082</v>
@@ -25934,33 +26185,33 @@
     <hyperlink ref="L25" r:id="rId63" xr:uid="{56E96306-5D5E-4586-B3CD-EEC9B7A62DF8}"/>
     <hyperlink ref="N6" r:id="rId64" xr:uid="{74A214C2-3BDE-42C5-B7EB-C5C079A5F2BC}"/>
     <hyperlink ref="G15" r:id="rId65" xr:uid="{3525B91C-085E-441D-B9B4-D1B377598311}"/>
-    <hyperlink ref="G21" r:id="rId66" display="https://eol.org/pages/583918" xr:uid="{7A52173C-806A-4EBD-8572-02DB271FC174}"/>
-    <hyperlink ref="G16" r:id="rId67" display="https://eol.org/pages/585884" xr:uid="{AC7EA6E6-24B3-4ED7-9E54-7044C31F15BB}"/>
-    <hyperlink ref="G23" r:id="rId68" display="https://eol.org/pages/583899" xr:uid="{9CD27666-E5F9-43A0-A522-45F024E47341}"/>
-    <hyperlink ref="G32" r:id="rId69" display="https://eol.org/pages/581098" xr:uid="{742B6EBA-04FA-4066-B448-B6F23EEAE7C6}"/>
-    <hyperlink ref="N39" r:id="rId70" xr:uid="{F106909F-A437-4D92-8178-D29EE28CB1F4}"/>
-    <hyperlink ref="P39" r:id="rId71" xr:uid="{73BC78FA-DA4F-4B3D-B5E3-FB774222D285}"/>
-    <hyperlink ref="T45" r:id="rId72" xr:uid="{0C0C3D63-49F0-43FA-B438-03C544B159FB}"/>
-    <hyperlink ref="T46" r:id="rId73" display="https://eol.org/pages/1121207" xr:uid="{9D4AE2E3-6A00-4069-9AAF-194903D8E369}"/>
-    <hyperlink ref="T47" r:id="rId74" display="https://eol.org/pages/49023867" xr:uid="{BE4187D2-0384-49AA-AE6D-044AB3E282C4}"/>
-    <hyperlink ref="T48" r:id="rId75" display="https://eol.org/pages/483665" xr:uid="{FDBC7D42-08D2-42C9-BF8E-6B4DBC5B085A}"/>
-    <hyperlink ref="T49" r:id="rId76" display="https://eol.org/pages/1095470" xr:uid="{B2D1EEF0-CC8D-475D-AC61-622A048780E4}"/>
-    <hyperlink ref="T53" r:id="rId77" display="https://eol.org/pages/47114859" xr:uid="{BE903FE3-4E19-4999-8947-55BCF63B937F}"/>
-    <hyperlink ref="T54" r:id="rId78" display="https://eol.org/pages/483664" xr:uid="{65536FCC-016F-45C4-B2EA-E24087E6E0C7}"/>
-    <hyperlink ref="T55" r:id="rId79" display="https://eol.org/pages/584706" xr:uid="{98541FF0-B643-4025-9B11-6D2A8B43BE81}"/>
-    <hyperlink ref="T56" r:id="rId80" display="https://eol.org/pages/584705" xr:uid="{93128A70-2208-4835-8826-987F00D5CE49}"/>
-    <hyperlink ref="T57" r:id="rId81" display="https://eol.org/pages/468106" xr:uid="{448324D5-4938-4640-87A8-B0123432A0A8}"/>
-    <hyperlink ref="T58" r:id="rId82" display="https://eol.org/pages/52522464" xr:uid="{6A6EA229-627C-4BEB-9EB1-FB2268BA41E2}"/>
-    <hyperlink ref="T60" r:id="rId83" display="https://eol.org/pages/487229" xr:uid="{B94719F3-AA21-4F3C-B176-05A4537368DE}"/>
-    <hyperlink ref="T61" r:id="rId84" display="https://eol.org/pages/468144" xr:uid="{E3AB83A7-B6F6-4DF7-A3A6-4C39A37C2CC0}"/>
-    <hyperlink ref="T63" r:id="rId85" display="https://eol.org/pages/703189" xr:uid="{FD592E99-AFA7-4161-A05C-AD418B758346}"/>
-    <hyperlink ref="T64" r:id="rId86" display="https://eol.org/pages/581568" xr:uid="{F0682AD9-CF2B-474A-BAB7-1BAB2F2F0A91}"/>
-    <hyperlink ref="T65" r:id="rId87" display="https://eol.org/pages/47378562" xr:uid="{AC5D57E4-F59D-4EA8-AD41-DE2BDE03AD7E}"/>
-    <hyperlink ref="T66" r:id="rId88" display="https://eol.org/pages/703664" xr:uid="{617CAC3E-E004-4B31-A68F-04FC7A473E73}"/>
-    <hyperlink ref="T67" r:id="rId89" display="https://eol.org/pages/486498" xr:uid="{87683EAD-DDAC-40A7-84BD-158C2D18B849}"/>
-    <hyperlink ref="T68" r:id="rId90" display="https://eol.org/pages/629943" xr:uid="{7130DD20-18CA-4B99-BEB5-3D7B840E699C}"/>
-    <hyperlink ref="T69" r:id="rId91" display="https://eol.org/pages/633316" xr:uid="{03103B16-DE8B-4156-8FE9-040B48617618}"/>
-    <hyperlink ref="T70" r:id="rId92" display="https://eol.org/pages/582270" xr:uid="{C599F5BA-C1B1-4E37-80D1-1F478DE474FA}"/>
+    <hyperlink ref="G16" r:id="rId66" display="https://eol.org/pages/585884" xr:uid="{AC7EA6E6-24B3-4ED7-9E54-7044C31F15BB}"/>
+    <hyperlink ref="G23" r:id="rId67" display="https://eol.org/pages/583899" xr:uid="{9CD27666-E5F9-43A0-A522-45F024E47341}"/>
+    <hyperlink ref="G32" r:id="rId68" display="https://eol.org/pages/581098" xr:uid="{742B6EBA-04FA-4066-B448-B6F23EEAE7C6}"/>
+    <hyperlink ref="N39" r:id="rId69" xr:uid="{F106909F-A437-4D92-8178-D29EE28CB1F4}"/>
+    <hyperlink ref="P39" r:id="rId70" xr:uid="{73BC78FA-DA4F-4B3D-B5E3-FB774222D285}"/>
+    <hyperlink ref="T45" r:id="rId71" xr:uid="{0C0C3D63-49F0-43FA-B438-03C544B159FB}"/>
+    <hyperlink ref="T46" r:id="rId72" display="https://eol.org/pages/1121207" xr:uid="{9D4AE2E3-6A00-4069-9AAF-194903D8E369}"/>
+    <hyperlink ref="T47" r:id="rId73" display="https://eol.org/pages/49023867" xr:uid="{BE4187D2-0384-49AA-AE6D-044AB3E282C4}"/>
+    <hyperlink ref="T48" r:id="rId74" display="https://eol.org/pages/483665" xr:uid="{FDBC7D42-08D2-42C9-BF8E-6B4DBC5B085A}"/>
+    <hyperlink ref="T49" r:id="rId75" display="https://eol.org/pages/1095470" xr:uid="{B2D1EEF0-CC8D-475D-AC61-622A048780E4}"/>
+    <hyperlink ref="T53" r:id="rId76" display="https://eol.org/pages/47114859" xr:uid="{BE903FE3-4E19-4999-8947-55BCF63B937F}"/>
+    <hyperlink ref="T54" r:id="rId77" display="https://eol.org/pages/483664" xr:uid="{65536FCC-016F-45C4-B2EA-E24087E6E0C7}"/>
+    <hyperlink ref="T55" r:id="rId78" display="https://eol.org/pages/584706" xr:uid="{98541FF0-B643-4025-9B11-6D2A8B43BE81}"/>
+    <hyperlink ref="T56" r:id="rId79" display="https://eol.org/pages/584705" xr:uid="{93128A70-2208-4835-8826-987F00D5CE49}"/>
+    <hyperlink ref="T57" r:id="rId80" display="https://eol.org/pages/468106" xr:uid="{448324D5-4938-4640-87A8-B0123432A0A8}"/>
+    <hyperlink ref="T58" r:id="rId81" display="https://eol.org/pages/52522464" xr:uid="{6A6EA229-627C-4BEB-9EB1-FB2268BA41E2}"/>
+    <hyperlink ref="T60" r:id="rId82" display="https://eol.org/pages/487229" xr:uid="{B94719F3-AA21-4F3C-B176-05A4537368DE}"/>
+    <hyperlink ref="T61" r:id="rId83" display="https://eol.org/pages/468144" xr:uid="{E3AB83A7-B6F6-4DF7-A3A6-4C39A37C2CC0}"/>
+    <hyperlink ref="T63" r:id="rId84" display="https://eol.org/pages/703189" xr:uid="{FD592E99-AFA7-4161-A05C-AD418B758346}"/>
+    <hyperlink ref="T64" r:id="rId85" display="https://eol.org/pages/581568" xr:uid="{F0682AD9-CF2B-474A-BAB7-1BAB2F2F0A91}"/>
+    <hyperlink ref="T65" r:id="rId86" display="https://eol.org/pages/47378562" xr:uid="{AC5D57E4-F59D-4EA8-AD41-DE2BDE03AD7E}"/>
+    <hyperlink ref="T66" r:id="rId87" display="https://eol.org/pages/703664" xr:uid="{617CAC3E-E004-4B31-A68F-04FC7A473E73}"/>
+    <hyperlink ref="T67" r:id="rId88" display="https://eol.org/pages/486498" xr:uid="{87683EAD-DDAC-40A7-84BD-158C2D18B849}"/>
+    <hyperlink ref="T68" r:id="rId89" display="https://eol.org/pages/629943" xr:uid="{7130DD20-18CA-4B99-BEB5-3D7B840E699C}"/>
+    <hyperlink ref="T69" r:id="rId90" display="https://eol.org/pages/633316" xr:uid="{03103B16-DE8B-4156-8FE9-040B48617618}"/>
+    <hyperlink ref="T70" r:id="rId91" display="https://eol.org/pages/582270" xr:uid="{C599F5BA-C1B1-4E37-80D1-1F478DE474FA}"/>
+    <hyperlink ref="G21" r:id="rId92" display="https://eol.org/pages/583918" xr:uid="{7A52173C-806A-4EBD-8572-02DB271FC174}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
finish references for genome versions
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198206_2_16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/1180714_2_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49794B9D-5799-4E99-A9F0-5B167275067F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{49794B9D-5799-4E99-A9F0-5B167275067F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B954DD63-4344-4F75-B8B9-52A33904A548}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4299" uniqueCount="1547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4354" uniqueCount="1595">
   <si>
     <t>Species</t>
   </si>
@@ -3927,9 +3927,6 @@
     <t>var. rush v1.1</t>
   </si>
   <si>
-    <t>GCA_911865555.2</t>
-  </si>
-  <si>
     <t>cultivation status reference</t>
   </si>
   <si>
@@ -4338,18 +4335,6 @@
     <t>Glycine tabacina has more GBIF observations and a native range that overlaps the native range of G. max. However, when I try to measure the range of G. tabacina I get a memory error because the number of occurrences is so high</t>
   </si>
   <si>
-    <t>Phytozome; https://doi.org/10.1093/nar/gkl976</t>
-  </si>
-  <si>
-    <t>v7.0</t>
-  </si>
-  <si>
-    <t>GCF_932294415.1</t>
-  </si>
-  <si>
-    <t>v3.1.1</t>
-  </si>
-  <si>
     <t>Encylopedia of life: https://eol.org/pages/1151323</t>
   </si>
   <si>
@@ -4678,6 +4663,165 @@
   </si>
   <si>
     <t>LupAngTanjil_v1.0; GCA_001865875.1; https://doi.org/10.1111/pbi.12615</t>
+  </si>
+  <si>
+    <t>SCU_Mint_v3; GCA_013358625.1</t>
+  </si>
+  <si>
+    <t>ASM211411v1; GCA_002114115.1</t>
+  </si>
+  <si>
+    <t>drMalSylv7.3; GCA_916048215.3</t>
+  </si>
+  <si>
+    <t>CATAS_Mindica_2.1; GCA_011075055.1</t>
+  </si>
+  <si>
+    <t>v8.0; v8.1</t>
+  </si>
+  <si>
+    <t>Mt4.0v1</t>
+  </si>
+  <si>
+    <t>v2.0; v2.0; https://doi.org/10.1073/pnas.1319032110</t>
+  </si>
+  <si>
+    <t>v7.0; v7.1; https://doi.org/10.1038/s41467-020-18923-6</t>
+  </si>
+  <si>
+    <t>ASM199503v1; GCA_001995035.1</t>
+  </si>
+  <si>
+    <t>v1; v1; https://doi.org/10.1038/nature11241</t>
+  </si>
+  <si>
+    <t>Chinese Lotus 1.1; GCA_000365185.2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1186/s12864-017-3791-6</t>
+  </si>
+  <si>
+    <t>v1.0; v1.0; https://doi.org/10.1073/pnas.1708621114</t>
+  </si>
+  <si>
+    <t>O.barthii_v1; GCA_000182155.2; https://doi.org/10.1038/s41588-018-0040-0</t>
+  </si>
+  <si>
+    <t>Oryza_brachyantha.v1.4b; GCA_000231095.2; https://doi.org/10.1038/ncomms2596</t>
+  </si>
+  <si>
+    <t>Oryza_glaberrima_V1; GCA_000147395.1; https://doi.org/10.1038/s41588-018-0040-0</t>
+  </si>
+  <si>
+    <t>O_longistaminata_v1.0; GCA_000789195.1; https://doi.org/10.1038/s41588-018-0040-0</t>
+  </si>
+  <si>
+    <t>Oryza_punctata_v1.2; GCA_000573905.1; https://doi.org/10.1038/s41588-018-0040-0</t>
+  </si>
+  <si>
+    <t>OR_W1943; GCA_000817225.1; https://doi.org/10.1038/s41588-018-0040-0</t>
+  </si>
+  <si>
+    <t>v7.0; v7.0; https://doi.org/10.1093/nar/gkl976</t>
+  </si>
+  <si>
+    <t>ASM357369v1; GCA_003573695.1; https://doi.org/10.1126/science.aat4096</t>
+  </si>
+  <si>
+    <t>PhaVulg1_0; GCA_000499845.1; https://doi.org/10.1038/ng.3008</t>
+  </si>
+  <si>
+    <t>palm_55x_up_171113_PBpolish2nd_filt_p; GCA_009389715.1</t>
+  </si>
+  <si>
+    <t>ASM1585260v2; GCA_015852605.2</t>
+  </si>
+  <si>
+    <t>v4.0; v4.1; https://doi.org/10.1126/science.1128691</t>
+  </si>
+  <si>
+    <t>pruArmRojPasHapCUR; GCA_903112645.1</t>
+  </si>
+  <si>
+    <t>PAV_r1.0; GCA_002207925.1; https://doi.org/10.1093/dnares/dsx020</t>
+  </si>
+  <si>
+    <t>v2.0; v2.1; https://doi.org/10.1038/ng.2586</t>
+  </si>
+  <si>
+    <t>ValleyOak3.0; GCA_001633185.2; https://doi.org/10.1534/g3.116.030411</t>
+  </si>
+  <si>
+    <t>GCA_932294415.1</t>
+  </si>
+  <si>
+    <t>ASM80110v3; GCA_000801105.3</t>
+  </si>
+  <si>
+    <t>RGv1.1; GCA_018127125.1</t>
+  </si>
+  <si>
+    <t>SDv1.1; GCA_015731905.1</t>
+  </si>
+  <si>
+    <t>S_indicum_v1.0; GCA_000512975.1; https://doi.org/10.1186/gb-2014-15-2-r39</t>
+  </si>
+  <si>
+    <t>v2; v2.2; https://doi.org/10.1038/nbt.2196</t>
+  </si>
+  <si>
+    <t>v2; v2.1; https://doi.org/10.1038/s41587-020-0681-2</t>
+  </si>
+  <si>
+    <t>SL4.0; ITAG4.0; https://doi.org/10.1101/767764</t>
+  </si>
+  <si>
+    <t>ASM1918654v1; GCA_019186545.1</t>
+  </si>
+  <si>
+    <t>v3.0; v3.1.1; https://doi.org/10.1111/tpj.13781</t>
+  </si>
+  <si>
+    <t>Spov3; Spov3; https://doi.org/10.1002/tpg2.20101</t>
+  </si>
+  <si>
+    <t>v1; v2; https://doi.org/10.1038/ncomms4311</t>
+  </si>
+  <si>
+    <t>SHERM; GCA_902706635.1</t>
+  </si>
+  <si>
+    <t>ASM1514329v1; GCA_015143295.1</t>
+  </si>
+  <si>
+    <t>T_arvense_v2; GCA_911865555.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASM2384627v1; GCA_023846275.1	</t>
+  </si>
+  <si>
+    <t>Vradiata_ver6; GCA_000741045.2; https://doi.org/10.1038/ncomms6443</t>
+  </si>
+  <si>
+    <t>ASM1883591v1; GCA_018835915.1</t>
+  </si>
+  <si>
+    <t>v1.0; v1.2; https://doi.org/10.1002/tpg2.20319</t>
+  </si>
+  <si>
+    <t>Genoscope.12X; v2.1; https://doi.org/10.1038/nature06148</t>
+  </si>
+  <si>
+    <t>ASM343084v1; GCA_003430845.1</t>
+  </si>
+  <si>
+    <t>ASM1927943v1; GCA_019279435.1</t>
+  </si>
+  <si>
+    <t>ASM2079620v1; GCA_020796205.1</t>
+  </si>
+  <si>
+    <t>Encyclopedia of Life: https://eol.org/pages/585514</t>
   </si>
 </sst>
 </file>
@@ -16795,7 +16939,7 @@
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
     </row>
   </sheetData>
@@ -16858,10 +17002,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9A1616-AAC6-4433-A869-98443D18E34E}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
+      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16940,7 +17084,7 @@
         <v>1254</v>
       </c>
       <c r="T1" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>66</v>
@@ -16981,13 +17125,13 @@
         <v>317</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1469</v>
+        <v>1464</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>773</v>
@@ -17018,7 +17162,7 @@
         <v>1255</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>1038</v>
@@ -17115,12 +17259,14 @@
         <v>445</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>1470</v>
+        <v>1465</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>1082</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>1594</v>
+      </c>
       <c r="H4" s="3" t="s">
         <v>749</v>
       </c>
@@ -17154,7 +17300,7 @@
         <v>1255</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>750</v>
@@ -17193,13 +17339,13 @@
         <v>445</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>1312</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>1313</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>751</v>
@@ -17233,7 +17379,7 @@
         <v>139</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="V5" s="10">
         <v>87</v>
@@ -17269,13 +17415,13 @@
         <v>445</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>1472</v>
+        <v>1467</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>26</v>
@@ -17303,7 +17449,7 @@
         <v>874</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="U6" s="7"/>
       <c r="V6" s="10">
@@ -17337,13 +17483,13 @@
         <v>445</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>1473</v>
+        <v>1468</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>16</v>
@@ -17372,7 +17518,7 @@
         <v>874</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="U7" s="7"/>
       <c r="V7" s="10">
@@ -17409,13 +17555,13 @@
         <v>455</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>1474</v>
+        <v>1469</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>460</v>
@@ -17479,13 +17625,13 @@
         <v>445</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>1475</v>
+        <v>1470</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>22</v>
@@ -17516,7 +17662,7 @@
         <v>874</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="10">
@@ -17553,13 +17699,13 @@
         <v>317</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>160</v>
@@ -17587,7 +17733,7 @@
         <v>874</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="U10" s="7"/>
       <c r="V10" s="10">
@@ -17626,13 +17772,13 @@
         <v>455</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>1505</v>
+        <v>1500</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>461</v>
@@ -17660,7 +17806,7 @@
         <v>874</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="U11" s="7" t="s">
         <v>575</v>
@@ -17696,13 +17842,16 @@
         <v>455</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>1318</v>
+        <v>1317</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>462</v>
       </c>
       <c r="I12" s="7"/>
       <c r="K12" s="3">
@@ -17733,7 +17882,7 @@
         <v>874</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="U12" s="7" t="s">
         <v>617</v>
@@ -17771,13 +17920,13 @@
         <v>445</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>1476</v>
+        <v>1471</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>775</v>
@@ -17808,10 +17957,10 @@
         <v>1255</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="V13" s="10">
         <v>320</v>
@@ -17849,13 +17998,13 @@
         <v>455</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>1507</v>
+        <v>1502</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>774</v>
@@ -17890,10 +18039,10 @@
         <v>874</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="U14" s="7" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="V14" s="10">
         <v>3</v>
@@ -17929,13 +18078,13 @@
         <v>455</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>1508</v>
+        <v>1503</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>753</v>
@@ -17969,7 +18118,7 @@
         <v>1255</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="U15" s="7" t="s">
         <v>754</v>
@@ -18010,13 +18159,13 @@
         <v>445</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>1477</v>
+        <v>1472</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>752</v>
@@ -18047,10 +18196,10 @@
         <v>1255</v>
       </c>
       <c r="T16" s="3" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="U16" s="7" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="V16" s="10">
         <v>597</v>
@@ -18084,13 +18233,13 @@
         <v>445</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>1478</v>
+        <v>1473</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>105</v>
@@ -18121,7 +18270,7 @@
         <v>874</v>
       </c>
       <c r="T17" s="3" t="s">
-        <v>1444</v>
+        <v>1439</v>
       </c>
       <c r="U17" s="7" t="s">
         <v>715</v>
@@ -18158,7 +18307,7 @@
         <v>445</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>1479</v>
+        <v>1474</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>1082</v>
@@ -18195,7 +18344,7 @@
         <v>874</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>1443</v>
+        <v>1438</v>
       </c>
       <c r="U18" s="7" t="s">
         <v>281</v>
@@ -18284,13 +18433,13 @@
         <v>317</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>1509</v>
+        <v>1504</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>807</v>
@@ -18318,7 +18467,7 @@
         <v>1255</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>1442</v>
+        <v>1437</v>
       </c>
       <c r="U20" s="7"/>
       <c r="V20" s="10">
@@ -18351,13 +18500,13 @@
         <v>317</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>1510</v>
+        <v>1505</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>808</v>
@@ -18388,10 +18537,10 @@
         <v>1255</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
       <c r="U21" s="7" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="V21" s="10">
         <v>1007</v>
@@ -18479,13 +18628,13 @@
         <v>445</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>1480</v>
+        <v>1475</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>684</v>
@@ -18518,10 +18667,10 @@
         <v>1255</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>1450</v>
+        <v>1445</v>
       </c>
       <c r="U23" s="7" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="V23" s="10">
         <v>119</v>
@@ -18555,13 +18704,13 @@
         <v>445</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>840</v>
@@ -18594,7 +18743,7 @@
         <v>1255</v>
       </c>
       <c r="T24" s="3" t="s">
-        <v>1441</v>
+        <v>1436</v>
       </c>
       <c r="U24" s="7" t="s">
         <v>159</v>
@@ -18631,13 +18780,16 @@
         <v>455</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>1511</v>
+        <v>1506</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>1329</v>
+        <v>1328</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>468</v>
       </c>
       <c r="I25" s="7"/>
       <c r="K25" s="3">
@@ -18662,7 +18814,7 @@
         <v>1255</v>
       </c>
       <c r="T25" s="3" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="U25" s="7"/>
       <c r="V25" s="10">
@@ -18695,13 +18847,13 @@
         <v>455</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>1512</v>
+        <v>1507</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>856</v>
@@ -18729,7 +18881,7 @@
         <v>1255</v>
       </c>
       <c r="T26" s="3" t="s">
-        <v>1448</v>
+        <v>1443</v>
       </c>
       <c r="U26" s="7" t="s">
         <v>583</v>
@@ -18764,13 +18916,13 @@
         <v>317</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>1513</v>
+        <v>1508</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>756</v>
@@ -18798,7 +18950,7 @@
         <v>1255</v>
       </c>
       <c r="T27" s="3" t="s">
-        <v>1449</v>
+        <v>1444</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>324</v>
@@ -18839,13 +18991,13 @@
         <v>455</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>1514</v>
+        <v>1509</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>842</v>
@@ -18875,7 +19027,7 @@
         <v>1255</v>
       </c>
       <c r="T28" s="3" t="s">
-        <v>1451</v>
+        <v>1446</v>
       </c>
       <c r="U28" s="7" t="s">
         <v>622</v>
@@ -18910,13 +19062,13 @@
         <v>317</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>1515</v>
+        <v>1510</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>325</v>
@@ -18946,7 +19098,7 @@
         <v>1255</v>
       </c>
       <c r="T29" s="3" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
       <c r="U29" s="7" t="s">
         <v>328</v>
@@ -18981,13 +19133,13 @@
         <v>445</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>1516</v>
+        <v>1511</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>59</v>
@@ -19022,7 +19174,7 @@
         <v>874</v>
       </c>
       <c r="T30" s="5" t="s">
-        <v>1453</v>
+        <v>1448</v>
       </c>
       <c r="U30" s="7" t="s">
         <v>159</v>
@@ -19059,13 +19211,13 @@
         <v>445</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>1516</v>
+        <v>1511</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>50</v>
@@ -19093,7 +19245,7 @@
         <v>874</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="U31" s="7" t="s">
         <v>716</v>
@@ -19128,13 +19280,13 @@
         <v>455</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>1517</v>
+        <v>1512</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>1146</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>890</v>
@@ -19167,10 +19319,10 @@
         <v>1255</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="U32" s="7" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="V32" s="10">
         <v>8028</v>
@@ -19204,10 +19356,10 @@
         <v>455</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>1518</v>
+        <v>1513</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>1059</v>
@@ -19240,7 +19392,7 @@
         <v>1255</v>
       </c>
       <c r="T33" s="3" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="U33" s="7" t="s">
         <v>583</v>
@@ -19275,13 +19427,13 @@
         <v>445</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>1519</v>
+        <v>1514</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>858</v>
@@ -19317,7 +19469,7 @@
         <v>1255</v>
       </c>
       <c r="T34" s="5" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
       <c r="U34" s="7" t="s">
         <v>259</v>
@@ -19352,19 +19504,19 @@
         <v>445</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>1429</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>1430</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3">
@@ -19391,7 +19543,7 @@
         <v>1255</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="U35" s="7" t="s">
         <v>260</v>
@@ -19424,13 +19576,13 @@
         <v>317</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>1520</v>
+        <v>1515</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>859</v>
@@ -19463,7 +19615,7 @@
         <v>1255</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="U36" s="7" t="s">
         <v>299</v>
@@ -19500,13 +19652,13 @@
         <v>455</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>1521</v>
+        <v>1516</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>791</v>
@@ -19536,7 +19688,7 @@
         <v>1255</v>
       </c>
       <c r="T37" s="3" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="U37" s="7" t="s">
         <v>583</v>
@@ -19571,13 +19723,13 @@
         <v>317</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>1522</v>
+        <v>1517</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>893</v>
@@ -19607,7 +19759,7 @@
         <v>1255</v>
       </c>
       <c r="T38" s="3" t="s">
-        <v>1461</v>
+        <v>1456</v>
       </c>
       <c r="U38" s="7" t="s">
         <v>341</v>
@@ -19645,23 +19797,26 @@
         <v>1295</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>1343</v>
+        <v>1342</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>864</v>
       </c>
       <c r="I39" s="7"/>
       <c r="K39" s="3">
         <v>0.49</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="M39" s="3" t="s">
         <v>833</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="O39" s="3">
         <v>2</v>
@@ -19673,7 +19828,7 @@
         <v>1255</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
       <c r="U39" s="7" t="s">
         <v>953</v>
@@ -19702,13 +19857,13 @@
         <v>455</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>1523</v>
+        <v>1518</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>861</v>
@@ -19741,7 +19896,7 @@
         <v>1255</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>1463</v>
+        <v>1458</v>
       </c>
       <c r="U40" s="7" t="s">
         <v>344</v>
@@ -19778,13 +19933,13 @@
         <v>317</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>1524</v>
+        <v>1519</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>894</v>
@@ -19814,7 +19969,7 @@
         <v>1255</v>
       </c>
       <c r="T41" s="3" t="s">
-        <v>1464</v>
+        <v>1459</v>
       </c>
       <c r="U41" s="7"/>
       <c r="V41" s="10">
@@ -19847,13 +20002,13 @@
         <v>445</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>1525</v>
+        <v>1520</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>897</v>
@@ -19886,7 +20041,7 @@
         <v>1255</v>
       </c>
       <c r="T42" s="3" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
       <c r="U42" s="7" t="s">
         <v>748</v>
@@ -19923,13 +20078,13 @@
         <v>455</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>1526</v>
+        <v>1521</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>844</v>
@@ -19960,13 +20115,13 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="R43" s="5" t="s">
-        <v>1498</v>
+        <v>1493</v>
       </c>
       <c r="S43" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T43" s="3" t="s">
-        <v>1466</v>
+        <v>1461</v>
       </c>
       <c r="U43" s="7" t="s">
         <v>607</v>
@@ -20003,13 +20158,13 @@
         <v>455</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>1527</v>
+        <v>1522</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>788</v>
@@ -20040,7 +20195,7 @@
         <v>1255</v>
       </c>
       <c r="T44" s="3" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="U44" s="7" t="s">
         <v>583</v>
@@ -20077,13 +20232,13 @@
         <v>317</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>1528</v>
+        <v>1523</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="H45" s="3" t="s">
         <v>846</v>
@@ -20120,7 +20275,7 @@
         <v>1255</v>
       </c>
       <c r="T45" s="5" t="s">
-        <v>1468</v>
+        <v>1463</v>
       </c>
       <c r="U45" s="7"/>
       <c r="V45" s="10">
@@ -20155,13 +20310,13 @@
         <v>445</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>1529</v>
+        <v>1524</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>898</v>
@@ -20191,7 +20346,7 @@
         <v>1255</v>
       </c>
       <c r="T46" s="5" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="U46" s="7" t="s">
         <v>145</v>
@@ -20226,13 +20381,13 @@
         <v>317</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>1530</v>
+        <v>1525</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="H47" s="3" t="s">
         <v>784</v>
@@ -20269,7 +20424,7 @@
         <v>1255</v>
       </c>
       <c r="T47" s="5" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="U47" s="7" t="s">
         <v>635</v>
@@ -20304,13 +20459,13 @@
         <v>455</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>1531</v>
+        <v>1526</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>785</v>
@@ -20338,7 +20493,7 @@
         <v>1255</v>
       </c>
       <c r="T48" s="5" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="U48" s="7" t="s">
         <v>590</v>
@@ -20373,13 +20528,13 @@
         <v>455</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>1532</v>
+        <v>1527</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>786</v>
@@ -20407,7 +20562,7 @@
         <v>1255</v>
       </c>
       <c r="T49" s="5" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="U49" s="7" t="s">
         <v>585</v>
@@ -20496,13 +20651,13 @@
         <v>317</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>1533</v>
+        <v>1528</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>777</v>
@@ -20530,7 +20685,7 @@
         <v>1255</v>
       </c>
       <c r="T51" s="3" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="U51" s="7" t="s">
         <v>361</v>
@@ -20571,19 +20726,19 @@
         <v>445</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>1534</v>
+        <v>1529</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="H52" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="I52" s="7" t="s">
         <v>1431</v>
-      </c>
-      <c r="I52" s="7" t="s">
-        <v>1432</v>
       </c>
       <c r="K52" s="3">
         <v>1.1299999999999999</v>
@@ -20607,7 +20762,7 @@
         <v>1255</v>
       </c>
       <c r="T52" s="3" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="U52" s="7" t="s">
         <v>290</v>
@@ -20636,13 +20791,13 @@
         <v>445</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>1082</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>88</v>
@@ -20677,7 +20832,7 @@
         <v>874</v>
       </c>
       <c r="T53" s="5" t="s">
-        <v>1482</v>
+        <v>1477</v>
       </c>
       <c r="U53" s="7"/>
       <c r="V53" s="10">
@@ -20710,13 +20865,13 @@
         <v>455</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>1536</v>
+        <v>1531</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>496</v>
@@ -20746,7 +20901,7 @@
         <v>1255</v>
       </c>
       <c r="T54" s="5" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="U54" s="7" t="s">
         <v>583</v>
@@ -20781,19 +20936,19 @@
         <v>445</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>1537</v>
+        <v>1532</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>111</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="J55" s="3"/>
       <c r="K55" s="3">
@@ -20820,7 +20975,7 @@
         <v>1255</v>
       </c>
       <c r="T55" s="5" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="U55" s="7"/>
       <c r="V55" s="10">
@@ -20855,13 +21010,13 @@
         <v>445</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>903</v>
@@ -20894,7 +21049,7 @@
         <v>1255</v>
       </c>
       <c r="T56" s="5" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="U56" s="7"/>
       <c r="V56" s="10">
@@ -20929,13 +21084,13 @@
         <v>445</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>1539</v>
+        <v>1534</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>796</v>
@@ -20963,7 +21118,7 @@
         <v>1255</v>
       </c>
       <c r="T57" s="5" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="U57" s="7" t="s">
         <v>145</v>
@@ -20998,13 +21153,13 @@
         <v>455</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>508</v>
@@ -21032,7 +21187,7 @@
         <v>874</v>
       </c>
       <c r="T58" s="5" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="U58" s="7" t="s">
         <v>590</v>
@@ -21125,13 +21280,13 @@
         <v>317</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>1541</v>
+        <v>1536</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>907</v>
@@ -21161,7 +21316,7 @@
         <v>1255</v>
       </c>
       <c r="T60" s="5" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="U60" s="7"/>
       <c r="V60" s="10">
@@ -21194,13 +21349,13 @@
         <v>445</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>1542</v>
+        <v>1537</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>872</v>
@@ -21230,7 +21385,7 @@
         <v>1255</v>
       </c>
       <c r="T61" s="5" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="U61" s="7" t="s">
         <v>263</v>
@@ -21323,13 +21478,13 @@
         <v>445</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>1543</v>
+        <v>1538</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="H63" s="3" t="s">
         <v>90</v>
@@ -21363,7 +21518,7 @@
         <v>874</v>
       </c>
       <c r="T63" s="5" t="s">
-        <v>1483</v>
+        <v>1478</v>
       </c>
       <c r="U63" s="7" t="s">
         <v>145</v>
@@ -21398,7 +21553,7 @@
         <v>445</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>1544</v>
+        <v>1539</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>1082</v>
@@ -21434,7 +21589,7 @@
         <v>1255</v>
       </c>
       <c r="T64" s="5" t="s">
-        <v>1484</v>
+        <v>1479</v>
       </c>
       <c r="U64" s="7" t="s">
         <v>303</v>
@@ -21469,7 +21624,7 @@
         <v>445</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>1545</v>
+        <v>1540</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>1082</v>
@@ -21512,7 +21667,7 @@
         <v>874</v>
       </c>
       <c r="T65" s="5" t="s">
-        <v>1485</v>
+        <v>1480</v>
       </c>
       <c r="U65" s="7" t="s">
         <v>264</v>
@@ -21549,13 +21704,13 @@
         <v>317</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>1546</v>
+        <v>1541</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>797</v>
@@ -21585,7 +21740,7 @@
         <v>1255</v>
       </c>
       <c r="T66" s="5" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="U66" s="7"/>
       <c r="V66" s="10">
@@ -21617,12 +21772,14 @@
       <c r="D67" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>1542</v>
+      </c>
       <c r="F67" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>911</v>
@@ -21659,7 +21816,7 @@
         <v>1255</v>
       </c>
       <c r="T67" s="5" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="U67" s="7"/>
       <c r="V67" s="10">
@@ -21693,12 +21850,14 @@
       <c r="D68" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E68" s="3"/>
+      <c r="E68" s="3" t="s">
+        <v>1543</v>
+      </c>
       <c r="F68" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>799</v>
@@ -21735,7 +21894,7 @@
         <v>1255</v>
       </c>
       <c r="T68" s="5" t="s">
-        <v>1486</v>
+        <v>1481</v>
       </c>
       <c r="U68" s="7" t="s">
         <v>583</v>
@@ -21771,12 +21930,14 @@
       <c r="D69" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E69" s="3"/>
+      <c r="E69" s="3" t="s">
+        <v>1544</v>
+      </c>
       <c r="F69" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>518</v>
@@ -21807,7 +21968,7 @@
         <v>1255</v>
       </c>
       <c r="T69" s="5" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="U69" s="7" t="s">
         <v>643</v>
@@ -21843,12 +22004,14 @@
       <c r="D70" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E70" s="3"/>
+      <c r="E70" s="3" t="s">
+        <v>1545</v>
+      </c>
       <c r="F70" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>801</v>
@@ -21879,7 +22042,7 @@
         <v>1255</v>
       </c>
       <c r="T70" s="5" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="U70" s="7" t="s">
         <v>583</v>
@@ -21915,12 +22078,14 @@
       <c r="D71" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E71" s="3"/>
+      <c r="E71" s="3" t="s">
+        <v>1546</v>
+      </c>
       <c r="F71" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>802</v>
@@ -21951,7 +22116,7 @@
         <v>1255</v>
       </c>
       <c r="T71" s="3" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="U71" s="7" t="s">
         <v>265</v>
@@ -21987,11 +22152,14 @@
       <c r="D72" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E72" s="3" t="s">
+        <v>1547</v>
+      </c>
       <c r="F72" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>803</v>
@@ -22021,7 +22189,7 @@
         <v>1255</v>
       </c>
       <c r="T72" s="3" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="U72" s="7" t="s">
         <v>159</v>
@@ -22055,12 +22223,14 @@
       <c r="D73" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E73" s="3"/>
+      <c r="E73" s="3" t="s">
+        <v>1548</v>
+      </c>
       <c r="F73" s="3" t="s">
         <v>1146</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>805</v>
@@ -22093,10 +22263,10 @@
         <v>874</v>
       </c>
       <c r="T73" s="3" t="s">
-        <v>1487</v>
+        <v>1482</v>
       </c>
       <c r="U73" s="7" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="V73" s="10">
         <v>38</v>
@@ -22129,11 +22299,14 @@
       <c r="D74" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E74" s="3" t="s">
+        <v>1549</v>
+      </c>
       <c r="F74" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>913</v>
@@ -22163,7 +22336,7 @@
         <v>1255</v>
       </c>
       <c r="T74" s="3" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="U74" s="7" t="s">
         <v>203</v>
@@ -22198,12 +22371,14 @@
       <c r="D75" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E75" s="3"/>
+      <c r="E75" s="3" t="s">
+        <v>1550</v>
+      </c>
       <c r="F75" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>875</v>
@@ -22236,7 +22411,7 @@
         <v>1255</v>
       </c>
       <c r="T75" s="3" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="U75" s="7" t="s">
         <v>647</v>
@@ -22272,12 +22447,14 @@
       <c r="D76" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E76" s="3"/>
+      <c r="E76" s="3" t="s">
+        <v>1551</v>
+      </c>
       <c r="F76" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>809</v>
@@ -22308,13 +22485,13 @@
         <v>3.67</v>
       </c>
       <c r="R76" s="5" t="s">
-        <v>1499</v>
+        <v>1494</v>
       </c>
       <c r="S76" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T76" s="3" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="U76" s="7" t="s">
         <v>611</v>
@@ -22350,12 +22527,14 @@
       <c r="D77" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E77" s="3"/>
+      <c r="E77" s="3" t="s">
+        <v>1552</v>
+      </c>
       <c r="F77" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>811</v>
@@ -22392,7 +22571,7 @@
         <v>1255</v>
       </c>
       <c r="T77" s="3" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="U77" s="7" t="s">
         <v>583</v>
@@ -22428,11 +22607,14 @@
       <c r="D78" s="3" t="s">
         <v>685</v>
       </c>
+      <c r="E78" s="3" t="s">
+        <v>1553</v>
+      </c>
       <c r="F78" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>776</v>
@@ -22460,7 +22642,7 @@
         <v>1255</v>
       </c>
       <c r="T78" s="3" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="U78" s="7" t="s">
         <v>696</v>
@@ -22500,11 +22682,14 @@
       <c r="D79" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E79" s="3" t="s">
+        <v>1554</v>
+      </c>
       <c r="F79" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>813</v>
@@ -22532,7 +22717,7 @@
         <v>1255</v>
       </c>
       <c r="T79" s="3" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="U79" s="7" t="s">
         <v>270</v>
@@ -22566,11 +22751,14 @@
       <c r="D80" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E80" s="3" t="s">
+        <v>1555</v>
+      </c>
       <c r="F80" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>375</v>
@@ -22598,7 +22786,7 @@
         <v>874</v>
       </c>
       <c r="T80" s="3" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="U80" s="7" t="s">
         <v>832</v>
@@ -22629,11 +22817,14 @@
       <c r="D81" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E81" s="3" t="s">
+        <v>1556</v>
+      </c>
       <c r="F81" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>379</v>
@@ -22661,7 +22852,7 @@
         <v>874</v>
       </c>
       <c r="T81" s="3" t="s">
-        <v>1488</v>
+        <v>1483</v>
       </c>
       <c r="U81" s="7" t="s">
         <v>380</v>
@@ -22692,11 +22883,17 @@
       <c r="C82" s="3" t="s">
         <v>384</v>
       </c>
+      <c r="D82" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>1557</v>
+      </c>
       <c r="F82" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>382</v>
@@ -22732,7 +22929,7 @@
         <v>1255</v>
       </c>
       <c r="T82" s="3" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="U82" s="7"/>
       <c r="V82" s="10">
@@ -22761,11 +22958,17 @@
       <c r="D83" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E83" s="3" t="s">
+        <v>1558</v>
+      </c>
       <c r="F83" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>1393</v>
+        <v>1392</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>387</v>
       </c>
       <c r="I83" s="7"/>
       <c r="K83" s="3">
@@ -22790,7 +22993,7 @@
         <v>874</v>
       </c>
       <c r="T83" s="3" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="U83" s="7" t="s">
         <v>835</v>
@@ -22822,12 +23025,14 @@
       <c r="D84" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E84" s="3"/>
+      <c r="E84" s="3" t="s">
+        <v>1559</v>
+      </c>
       <c r="F84" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>393</v>
@@ -22858,7 +23063,7 @@
         <v>874</v>
       </c>
       <c r="T84" s="3" t="s">
-        <v>1489</v>
+        <v>1484</v>
       </c>
       <c r="U84" s="7" t="s">
         <v>395</v>
@@ -22896,12 +23101,14 @@
       <c r="D85" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E85" s="3"/>
+      <c r="E85" s="3" t="s">
+        <v>1560</v>
+      </c>
       <c r="F85" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>397</v>
@@ -22936,7 +23143,7 @@
         <v>874</v>
       </c>
       <c r="T85" s="3" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="U85" s="7" t="s">
         <v>399</v>
@@ -22970,16 +23177,16 @@
         <v>4</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>1433</v>
+        <v>445</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>1434</v>
+        <v>1561</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>915</v>
@@ -23009,7 +23216,7 @@
         <v>1255</v>
       </c>
       <c r="T86" s="3" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="U86" s="7" t="s">
         <v>271</v>
@@ -23048,10 +23255,10 @@
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>133</v>
@@ -23119,10 +23326,10 @@
         <v>445</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="H88" s="4" t="s">
         <v>917</v>
@@ -23186,11 +23393,14 @@
       <c r="D89" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E89" s="3" t="s">
+        <v>1562</v>
+      </c>
       <c r="F89" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="H89" s="3" t="s">
         <v>815</v>
@@ -23218,7 +23428,7 @@
         <v>1255</v>
       </c>
       <c r="T89" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="U89" s="7" t="s">
         <v>402</v>
@@ -23255,12 +23465,14 @@
       <c r="D90" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E90" s="3"/>
+      <c r="E90" s="3" t="s">
+        <v>1563</v>
+      </c>
       <c r="F90" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>919</v>
@@ -23293,7 +23505,7 @@
         <v>1255</v>
       </c>
       <c r="T90" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="U90" s="7"/>
       <c r="V90" s="10">
@@ -23327,11 +23539,14 @@
       <c r="D91" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E91" s="3" t="s">
+        <v>1564</v>
+      </c>
       <c r="F91" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>878</v>
@@ -23361,7 +23576,7 @@
         <v>1255</v>
       </c>
       <c r="T91" s="3" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="U91" s="7"/>
       <c r="V91" s="10">
@@ -23447,9 +23662,11 @@
       <c r="D93" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E93" s="3"/>
+      <c r="E93" s="3" t="s">
+        <v>1565</v>
+      </c>
       <c r="F93" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>1106</v>
@@ -23483,7 +23700,7 @@
         <v>1255</v>
       </c>
       <c r="T93" s="3" t="s">
-        <v>1490</v>
+        <v>1485</v>
       </c>
       <c r="U93" s="7" t="s">
         <v>583</v>
@@ -23519,12 +23736,14 @@
       <c r="D94" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E94" s="3"/>
+      <c r="E94" s="3" t="s">
+        <v>1566</v>
+      </c>
       <c r="F94" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>51</v>
@@ -23555,13 +23774,13 @@
         <v>35</v>
       </c>
       <c r="R94" s="5" t="s">
-        <v>1500</v>
+        <v>1495</v>
       </c>
       <c r="S94" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T94" s="3" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="U94" s="7" t="s">
         <v>252</v>
@@ -23597,12 +23816,14 @@
       <c r="D95" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E95" s="3"/>
+      <c r="E95" s="3" t="s">
+        <v>1567</v>
+      </c>
       <c r="F95" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>921</v>
@@ -23635,7 +23856,7 @@
         <v>1255</v>
       </c>
       <c r="T95" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="U95" s="7" t="s">
         <v>583</v>
@@ -23671,12 +23892,14 @@
       <c r="D96" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E96" s="3"/>
+      <c r="E96" s="3" t="s">
+        <v>1568</v>
+      </c>
       <c r="F96" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>409</v>
@@ -23709,7 +23932,7 @@
         <v>1255</v>
       </c>
       <c r="T96" s="3" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="U96" s="7" t="s">
         <v>412</v>
@@ -23745,12 +23968,14 @@
       <c r="D97" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E97" s="3"/>
+      <c r="E97" s="3" t="s">
+        <v>1569</v>
+      </c>
       <c r="F97" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>925</v>
@@ -23783,7 +24008,7 @@
         <v>1255</v>
       </c>
       <c r="T97" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="U97" s="7" t="s">
         <v>273</v>
@@ -23816,11 +24041,14 @@
       <c r="D98" s="3" t="s">
         <v>317</v>
       </c>
+      <c r="E98" s="3" t="s">
+        <v>1570</v>
+      </c>
       <c r="F98" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>417</v>
@@ -23850,7 +24078,7 @@
         <v>874</v>
       </c>
       <c r="T98" s="3" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="U98" s="7" t="s">
         <v>418</v>
@@ -23885,16 +24113,16 @@
         <v>455</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>1435</v>
+        <v>1571</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="I99" s="7"/>
       <c r="K99" s="3">
@@ -23919,7 +24147,7 @@
         <v>1255</v>
       </c>
       <c r="T99" s="3" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
       <c r="U99" s="7" t="s">
         <v>583</v>
@@ -23953,7 +24181,9 @@
       <c r="D100" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E100" s="3"/>
+      <c r="E100" s="3" t="s">
+        <v>1572</v>
+      </c>
       <c r="F100" s="3" t="s">
         <v>1082</v>
       </c>
@@ -23991,7 +24221,7 @@
         <v>1255</v>
       </c>
       <c r="T100" s="3" t="s">
-        <v>1491</v>
+        <v>1486</v>
       </c>
       <c r="U100" s="7" t="s">
         <v>712</v>
@@ -24027,12 +24257,14 @@
       <c r="D101" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E101" s="3"/>
+      <c r="E101" s="3" t="s">
+        <v>1573</v>
+      </c>
       <c r="F101" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>545</v>
@@ -24063,16 +24295,16 @@
         <v>0.91439999999999999</v>
       </c>
       <c r="R101" s="5" t="s">
-        <v>1503</v>
+        <v>1498</v>
       </c>
       <c r="S101" s="3" t="s">
         <v>874</v>
       </c>
       <c r="T101" s="3" t="s">
-        <v>1492</v>
+        <v>1487</v>
       </c>
       <c r="U101" s="7" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="V101" s="10">
         <v>32</v>
@@ -24105,11 +24337,14 @@
       <c r="D102" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E102" s="3" t="s">
+        <v>1574</v>
+      </c>
       <c r="F102" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>847</v>
@@ -24139,7 +24374,7 @@
         <v>874</v>
       </c>
       <c r="T102" s="3" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="U102" s="7" t="s">
         <v>595</v>
@@ -24178,7 +24413,7 @@
         <v>1082</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="H103" s="4" t="s">
         <v>928</v>
@@ -24241,12 +24476,14 @@
       <c r="D104" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E104" s="3"/>
+      <c r="E104" s="3" t="s">
+        <v>1575</v>
+      </c>
       <c r="F104" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>929</v>
@@ -24279,7 +24516,7 @@
         <v>1255</v>
       </c>
       <c r="T104" s="3" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="U104" s="7" t="s">
         <v>428</v>
@@ -24315,11 +24552,14 @@
       <c r="D105" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E105" s="3" t="s">
+        <v>1576</v>
+      </c>
       <c r="F105" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>931</v>
@@ -24347,7 +24587,7 @@
         <v>1255</v>
       </c>
       <c r="T105" s="3" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="U105" s="7" t="s">
         <v>274</v>
@@ -24381,11 +24621,14 @@
       <c r="D106" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E106" s="3" t="s">
+        <v>1577</v>
+      </c>
       <c r="F106" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>132</v>
@@ -24413,7 +24656,7 @@
         <v>874</v>
       </c>
       <c r="T106" s="3" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="U106" s="7" t="s">
         <v>275</v>
@@ -24502,11 +24745,14 @@
       <c r="D108" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E108" s="3" t="s">
+        <v>1578</v>
+      </c>
       <c r="F108" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>555</v>
@@ -24534,7 +24780,7 @@
         <v>1255</v>
       </c>
       <c r="T108" s="3" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="U108" s="7" t="s">
         <v>159</v>
@@ -24633,7 +24879,7 @@
         <v>1146</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="H110" s="4"/>
       <c r="I110" s="13"/>
@@ -24692,12 +24938,14 @@
       <c r="D111" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E111" s="3"/>
+      <c r="E111" s="3" t="s">
+        <v>1579</v>
+      </c>
       <c r="F111" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>556</v>
@@ -24728,7 +24976,7 @@
         <v>874</v>
       </c>
       <c r="T111" s="3" t="s">
-        <v>1493</v>
+        <v>1488</v>
       </c>
       <c r="U111" s="7" t="s">
         <v>595</v>
@@ -24793,13 +25041,13 @@
         <v>445</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>1436</v>
+        <v>1580</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="H113" s="3" t="s">
         <v>932</v>
@@ -24832,7 +25080,7 @@
         <v>1255</v>
       </c>
       <c r="T113" s="3" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="U113" s="7" t="s">
         <v>159</v>
@@ -24868,12 +25116,14 @@
       <c r="D114" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E114" s="3"/>
+      <c r="E114" s="3" t="s">
+        <v>1581</v>
+      </c>
       <c r="F114" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>934</v>
@@ -24906,7 +25156,7 @@
         <v>1255</v>
       </c>
       <c r="T114" s="3" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="U114" s="7" t="s">
         <v>276</v>
@@ -24942,11 +25192,14 @@
       <c r="D115" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E115" s="3" t="s">
+        <v>1582</v>
+      </c>
       <c r="F115" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="H115" s="3" t="s">
         <v>123</v>
@@ -24974,7 +25227,7 @@
         <v>874</v>
       </c>
       <c r="T115" s="3" t="s">
-        <v>1494</v>
+        <v>1489</v>
       </c>
       <c r="U115" s="7" t="s">
         <v>278</v>
@@ -25008,11 +25261,14 @@
       <c r="D116" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E116" s="3" t="s">
+        <v>1583</v>
+      </c>
       <c r="F116" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>558</v>
@@ -25040,7 +25296,7 @@
         <v>874</v>
       </c>
       <c r="T116" s="3" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="U116" s="7" t="s">
         <v>594</v>
@@ -25074,11 +25330,14 @@
       <c r="D117" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E117" s="3" t="s">
+        <v>1584</v>
+      </c>
       <c r="F117" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="H117" s="3" t="s">
         <v>562</v>
@@ -25106,7 +25365,7 @@
         <v>874</v>
       </c>
       <c r="T117" s="3" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="U117" s="7" t="s">
         <v>594</v>
@@ -25197,13 +25456,13 @@
         <v>455</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>1296</v>
+        <v>1585</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="H119" s="3" t="s">
         <v>564</v>
@@ -25234,7 +25493,7 @@
         <v>1255</v>
       </c>
       <c r="T119" s="3" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="U119" s="7" t="s">
         <v>583</v>
@@ -25484,11 +25743,14 @@
       <c r="D124" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E124" s="3" t="s">
+        <v>1586</v>
+      </c>
       <c r="F124" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>882</v>
@@ -25518,13 +25780,13 @@
         <v>15</v>
       </c>
       <c r="R124" s="5" t="s">
-        <v>1502</v>
+        <v>1497</v>
       </c>
       <c r="S124" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T124" s="3" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="U124" s="7" t="s">
         <v>603</v>
@@ -25558,12 +25820,14 @@
       <c r="D125" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E125" s="3"/>
+      <c r="E125" s="3" t="s">
+        <v>1587</v>
+      </c>
       <c r="F125" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>944</v>
@@ -25596,7 +25860,7 @@
         <v>1255</v>
       </c>
       <c r="T125" s="3" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="U125" s="7"/>
       <c r="V125" s="10">
@@ -25630,12 +25894,14 @@
       <c r="D126" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E126" s="3"/>
+      <c r="E126" s="3" t="s">
+        <v>1588</v>
+      </c>
       <c r="F126" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>946</v>
@@ -25672,7 +25938,7 @@
         <v>1255</v>
       </c>
       <c r="T126" s="3" t="s">
-        <v>1495</v>
+        <v>1490</v>
       </c>
       <c r="U126" s="7" t="s">
         <v>594</v>
@@ -25702,11 +25968,14 @@
       <c r="D127" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="E127" s="3" t="s">
+        <v>1589</v>
+      </c>
       <c r="F127" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>853</v>
@@ -25736,7 +26005,7 @@
         <v>1255</v>
       </c>
       <c r="T127" s="3" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="U127" s="7" t="s">
         <v>444</v>
@@ -25770,12 +26039,14 @@
       <c r="D128" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="E128" s="3"/>
+      <c r="E128" s="3" t="s">
+        <v>1590</v>
+      </c>
       <c r="F128" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>884</v>
@@ -25808,7 +26079,7 @@
         <v>1255</v>
       </c>
       <c r="T128" s="3" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="U128" s="7" t="s">
         <v>277</v>
@@ -25844,11 +26115,17 @@
       <c r="D129" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E129" s="3" t="s">
+        <v>1591</v>
+      </c>
       <c r="F129" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>1365</v>
+        <v>1364</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>568</v>
       </c>
       <c r="I129" s="7"/>
       <c r="K129" s="3">
@@ -25873,13 +26150,13 @@
         <v>2.11</v>
       </c>
       <c r="R129" s="5" t="s">
-        <v>1501</v>
+        <v>1496</v>
       </c>
       <c r="S129" s="3" t="s">
         <v>1255</v>
       </c>
       <c r="T129" s="3" t="s">
-        <v>1496</v>
+        <v>1491</v>
       </c>
       <c r="U129" s="7" t="s">
         <v>583</v>
@@ -25908,19 +26185,19 @@
         <v>292</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>445</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>1446</v>
+        <v>1441</v>
       </c>
       <c r="F130" s="3" t="s">
         <v>1082</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="H130" s="7" t="s">
         <v>947</v>
@@ -25950,7 +26227,7 @@
         <v>1255</v>
       </c>
       <c r="T130" s="3" t="s">
-        <v>1497</v>
+        <v>1492</v>
       </c>
       <c r="U130" s="7" t="s">
         <v>781</v>
@@ -25971,7 +26248,7 @@
         <v>34</v>
       </c>
       <c r="AB130" s="3" t="s">
-        <v>1447</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="131" spans="1:28" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -25987,6 +26264,9 @@
       <c r="D131" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E131" s="3" t="s">
+        <v>1592</v>
+      </c>
       <c r="F131" s="3" t="s">
         <v>1082</v>
       </c>
@@ -26062,11 +26342,14 @@
       <c r="D132" s="3" t="s">
         <v>455</v>
       </c>
+      <c r="E132" s="3" t="s">
+        <v>1593</v>
+      </c>
       <c r="F132" s="3" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>950</v>
@@ -26096,7 +26379,7 @@
         <v>1255</v>
       </c>
       <c r="T132" s="3" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="U132" s="7" t="s">
         <v>583</v>
@@ -26214,5 +26497,6 @@
     <hyperlink ref="G21" r:id="rId92" display="https://eol.org/pages/583918" xr:uid="{7A52173C-806A-4EBD-8572-02DB271FC174}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId93"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reorganize main figures, reduce down to just key result
</commit_message>
<xml_diff>
--- a/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
+++ b/doc/2022-10-04_allPlantPolymorphisms_bioprojects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d159467a54f2bd9d/DOCUME^F1/MobaXterm/slash/miles_desktoplihoagr/RemoteFiles/1180714_2_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MILESR~1\AppData\Local\Temp\Mxt213\RemoteFiles\198206_3_22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{49794B9D-5799-4E99-A9F0-5B167275067F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B954DD63-4344-4F75-B8B9-52A33904A548}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C20501F-D2E5-49C1-981D-D43E81AA96FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes on datasets" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4354" uniqueCount="1595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4354" uniqueCount="1596">
   <si>
     <t>Species</t>
   </si>
@@ -4797,9 +4797,6 @@
     <t>T_arvense_v2; GCA_911865555.2</t>
   </si>
   <si>
-    <t xml:space="preserve">ASM2384627v1; GCA_023846275.1	</t>
-  </si>
-  <si>
     <t>Vradiata_ver6; GCA_000741045.2; https://doi.org/10.1038/ncomms6443</t>
   </si>
   <si>
@@ -4822,6 +4819,12 @@
   </si>
   <si>
     <t>Encyclopedia of Life: https://eol.org/pages/585514</t>
+  </si>
+  <si>
+    <t>ASM2384627v1; GCA_023846275.1</t>
+  </si>
+  <si>
+    <t>Sorghum arundinaceum/Sorghum bicolor subsp. verticilliflorum</t>
   </si>
 </sst>
 </file>
@@ -17002,10 +17005,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9A1616-AAC6-4433-A869-98443D18E34E}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2"/>
+      <selection pane="bottomLeft" activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17265,7 +17268,7 @@
         <v>1082</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>749</v>
@@ -25050,7 +25053,7 @@
         <v>1414</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>932</v>
+        <v>1595</v>
       </c>
       <c r="I113" s="7" t="s">
         <v>933</v>
@@ -25744,7 +25747,7 @@
         <v>455</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>1586</v>
+        <v>1594</v>
       </c>
       <c r="F124" s="3" t="s">
         <v>1311</v>
@@ -25821,7 +25824,7 @@
         <v>317</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="F125" s="3" t="s">
         <v>1082</v>
@@ -25895,7 +25898,7 @@
         <v>455</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="F126" s="3" t="s">
         <v>1082</v>
@@ -25969,7 +25972,7 @@
         <v>445</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="F127" s="3" t="s">
         <v>1082</v>
@@ -26040,7 +26043,7 @@
         <v>445</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="F128" s="3" t="s">
         <v>1311</v>
@@ -26116,7 +26119,7 @@
         <v>455</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="F129" s="3" t="s">
         <v>1311</v>
@@ -26265,7 +26268,7 @@
         <v>455</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>1082</v>
@@ -26343,7 +26346,7 @@
         <v>455</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>1311</v>

</xml_diff>